<commit_message>
CI: Auto Update Data (#67)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -612,7 +612,7 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.1), maa://25390 (97.4), maa://36681 (91.94)</t>
+          <t>maa://24702 (94.1), maa://25390 (97.41), maa://36681 (91.94)</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
@@ -717,7 +717,7 @@
       </c>
       <c r="AE2" s="2" t="inlineStr">
         <is>
-          <t>***maa://21730 (17.46), maa://25251 (91.89), ***maa://39501 (25.0), *maa://36675 (60.0)</t>
+          <t>***maa://21730 (17.19), maa://25251 (92.0), ***maa://39501 (20.0), *maa://36675 (60.0)</t>
         </is>
       </c>
     </row>
@@ -734,7 +734,7 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>maa://36987 (95.56), maa://40192 (100.0), maa://39849 (100.0)</t>
+          <t>maa://36987 (95.65), maa://40192 (100.0), maa://39849 (100.0)</t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -749,7 +749,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.19), *maa://22748 (75.0)</t>
+          <t>maa://21247 (98.26), *maa://22748 (75.0)</t>
         </is>
       </c>
       <c r="I3" s="4" t="inlineStr">
@@ -764,7 +764,7 @@
       </c>
       <c r="K3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (70.67), maa://20276 (81.95), *maa://22749 (62.5)</t>
+          <t>*maa://22880 (70.2), maa://20276 (82.35), *maa://22749 (62.5)</t>
         </is>
       </c>
       <c r="M3" s="4" t="inlineStr">
@@ -779,7 +779,7 @@
       </c>
       <c r="O3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (95.45), maa://26254 (95.24)</t>
+          <t>maa://21249 (95.5), maa://26254 (95.24)</t>
         </is>
       </c>
       <c r="Q3" s="4" t="inlineStr">
@@ -856,7 +856,7 @@
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.08), **maa://24303 (36.36), maa://22499 (85.71), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.18), **maa://24303 (36.36), maa://22499 (85.71), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -916,7 +916,7 @@
       </c>
       <c r="S4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (98.7), maa://22754 (91.67), maa://27295 (80.39), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (98.72), maa://22754 (91.67), maa://27295 (80.39), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="4" t="inlineStr">
@@ -931,7 +931,7 @@
       </c>
       <c r="W4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.44), ***maa://31785 (15.74), ***maa://36683 (26.67)</t>
+          <t>**maa://32495 (47.9), ***maa://31785 (15.74), ***maa://36683 (26.67)</t>
         </is>
       </c>
       <c r="Y4" s="4" t="inlineStr">
@@ -978,7 +978,7 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (82.26), maa://22744 (81.82)</t>
+          <t>maa://21245 (82.54), maa://22744 (82.61)</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -1252,7 +1252,7 @@
       </c>
       <c r="K7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (91.18), maa://24957 (97.3)</t>
+          <t>maa://28624 (91.3), maa://24957 (97.3)</t>
         </is>
       </c>
       <c r="M7" s="4" t="inlineStr">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="W7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (94.53), *maa://22758 (70.83)</t>
+          <t>maa://22399 (94.62), *maa://22758 (71.43)</t>
         </is>
       </c>
       <c r="Y7" s="4" t="inlineStr">
@@ -1327,7 +1327,7 @@
       </c>
       <c r="AE7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (71.43), *maa://36671 (73.17)</t>
+          <t>*maa://26191 (70.42), *maa://36671 (73.17)</t>
         </is>
       </c>
     </row>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="W8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (96.21)</t>
+          <t>maa://21411 (96.25)</t>
         </is>
       </c>
       <c r="Y8" s="4" t="inlineStr">
@@ -1556,7 +1556,7 @@
       </c>
       <c r="AA9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (88.61), ***maa://22740 (5.88), **maa://27377 (46.15), ***maa://25174 (20.0), *maa://39938 (54.55), maa://40166 (100.0)</t>
+          <t>maa://28711 (87.65), ***maa://22740 (5.88), **maa://27377 (46.15), ***maa://25174 (20.0), **maa://39938 (50.0), maa://40166 (100.0)</t>
         </is>
       </c>
       <c r="AC9" s="4" t="inlineStr">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="AE9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (89.74), **maa://22865 (44.44)</t>
+          <t>maa://26206 (90.0), **maa://22865 (45.65)</t>
         </is>
       </c>
     </row>
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.41), **maa://32237 (40.0), ***maa://34206 (14.29), ***maa://39951 (17.65), ***maa://39243 (25.0)</t>
+          <t>***maa://25695 (19.41), **maa://32237 (38.89), ***maa://34206 (14.29), ***maa://39951 (15.79), ***maa://39243 (25.0)</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="S10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (97.22), maa://22755 (87.25), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (97.24), maa://22755 (87.5), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="4" t="inlineStr">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="W10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.31), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.33), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="4" t="inlineStr">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="AE10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (56.52), *maa://22733 (60.71), maa://22761 (100.0)</t>
+          <t>*maa://25021 (56.52), *maa://22733 (58.62), maa://22761 (100.0)</t>
         </is>
       </c>
     </row>
@@ -1710,7 +1710,7 @@
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.62)</t>
+          <t>maa://36707 (99.63)</t>
         </is>
       </c>
       <c r="E11" s="4" t="inlineStr">
@@ -1770,7 +1770,7 @@
       </c>
       <c r="S11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (94.93), maa://22501 (98.08)</t>
+          <t>maa://22747 (94.96), maa://22501 (98.08)</t>
         </is>
       </c>
       <c r="U11" s="4" t="inlineStr">
@@ -1785,7 +1785,7 @@
       </c>
       <c r="W11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.77)</t>
+          <t>maa://36713 (97.78)</t>
         </is>
       </c>
       <c r="Y11" s="4" t="inlineStr">
@@ -1847,7 +1847,7 @@
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (89.73)</t>
+          <t>maa://21867 (89.86)</t>
         </is>
       </c>
       <c r="I12" s="4" t="inlineStr">
@@ -1907,7 +1907,7 @@
       </c>
       <c r="W12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.67), *maa://21485 (76.56), *maa://37962 (80.0)</t>
+          <t>maa://22753 (91.67), *maa://21485 (76.56), maa://37962 (81.25)</t>
         </is>
       </c>
       <c r="Y12" s="4" t="inlineStr">
@@ -1922,7 +1922,7 @@
       </c>
       <c r="AA12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.8), maa://36677 (94.59), maa://39872 (81.82)</t>
+          <t>maa://23669 (95.82), maa://36677 (94.74), maa://39872 (81.82)</t>
         </is>
       </c>
       <c r="AC12" s="4" t="inlineStr">
@@ -1954,7 +1954,7 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.34), maa://36673 (91.67), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.36), maa://36673 (91.8), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr">
@@ -1969,7 +1969,7 @@
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (75.38), **maa://22728 (48.78)</t>
+          <t>*maa://21248 (75.5), **maa://22728 (47.62)</t>
         </is>
       </c>
       <c r="I13" s="4" t="inlineStr">
@@ -1999,7 +1999,7 @@
       </c>
       <c r="O13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (91.67), *maa://22583 (75.44), *maa://22500 (55.81)</t>
+          <t>maa://22676 (91.75), *maa://22583 (75.86), *maa://22500 (55.81)</t>
         </is>
       </c>
       <c r="Q13" s="4" t="inlineStr">
@@ -2029,7 +2029,7 @@
       </c>
       <c r="W13" s="2" t="inlineStr">
         <is>
-          <t>*maa://34957 (77.78), *maa://22768 (53.33)</t>
+          <t>*maa://34957 (79.49), *maa://22768 (53.33)</t>
         </is>
       </c>
       <c r="Y13" s="4" t="inlineStr">
@@ -2059,7 +2059,7 @@
       </c>
       <c r="AE13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (30.83), maa://39883 (89.47), *maa://39885 (77.78)</t>
+          <t>**maa://22737 (30.83), maa://39883 (90.48), *maa://39885 (73.68)</t>
         </is>
       </c>
     </row>
@@ -2106,7 +2106,7 @@
       </c>
       <c r="K14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.12), maa://21288 (96.21), maa://36682 (100.0), maa://39841 (91.43)</t>
+          <t>maa://26245 (96.12), maa://21288 (96.21), maa://36682 (100.0), maa://39841 (92.11)</t>
         </is>
       </c>
       <c r="M14" s="4" t="inlineStr">
@@ -2198,7 +2198,7 @@
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (76.05), maa://22734 (83.33), *maa://30808 (62.96), ***maa://36048 (13.33)</t>
+          <t>*maa://22743 (76.05), maa://22734 (83.33), *maa://30808 (63.64), ***maa://36048 (13.33)</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr">
@@ -2213,7 +2213,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.2), maa://21478 (91.18)</t>
+          <t>maa://24304 (88.27), maa://21478 (91.18)</t>
         </is>
       </c>
       <c r="I15" s="4" t="inlineStr">
@@ -2243,7 +2243,7 @@
       </c>
       <c r="O15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (89.36), *maa://22727 (70.0)</t>
+          <t>maa://24762 (89.51), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="4" t="inlineStr">
@@ -2303,7 +2303,7 @@
       </c>
       <c r="AE15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.55), *maa://22766 (73.0), *maa://36666 (76.27)</t>
+          <t>maa://21364 (80.55), *maa://22766 (73.0), *maa://36666 (76.67)</t>
         </is>
       </c>
     </row>
@@ -2320,7 +2320,7 @@
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.15), maa://36679 (93.33), maa://37650 (94.74)</t>
+          <t>maa://21441 (96.15), maa://36679 (93.33), maa://37650 (95.0)</t>
         </is>
       </c>
       <c r="E16" s="4" t="inlineStr">
@@ -2395,7 +2395,7 @@
       </c>
       <c r="W16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (97.33), maa://28051 (95.83)</t>
+          <t>maa://28501 (97.37), maa://28051 (95.83)</t>
         </is>
       </c>
       <c r="Y16" s="4" t="inlineStr">
@@ -2410,7 +2410,7 @@
       </c>
       <c r="AA16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.95)</t>
+          <t>maa://26228 (96.0)</t>
         </is>
       </c>
       <c r="AC16" s="4" t="inlineStr">
@@ -2425,7 +2425,7 @@
       </c>
       <c r="AE16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (61.54), maa://27755 (91.43)</t>
+          <t>*maa://23911 (61.54), maa://27755 (91.55)</t>
         </is>
       </c>
     </row>
@@ -2564,7 +2564,7 @@
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.39)</t>
+          <t>maa://24570 (96.43)</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="G18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (90.15)</t>
+          <t>maa://24421 (90.34)</t>
         </is>
       </c>
       <c r="I18" s="4" t="inlineStr">
@@ -2639,7 +2639,7 @@
       </c>
       <c r="W18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (97.4), *maa://22741 (80.0)</t>
+          <t>maa://21917 (97.4), maa://22741 (83.33)</t>
         </is>
       </c>
       <c r="Y18" s="4" t="inlineStr">
@@ -2853,7 +2853,7 @@
       </c>
       <c r="O20" s="2" t="inlineStr">
         <is>
-          <t>maa://37442 (96.15)</t>
+          <t>maa://37442 (96.3)</t>
         </is>
       </c>
       <c r="Q20" s="4" t="inlineStr">
@@ -2960,7 +2960,7 @@
       </c>
       <c r="K21" s="2" t="inlineStr">
         <is>
-          <t>maa://31731 (94.87)</t>
+          <t>maa://31731 (95.0)</t>
         </is>
       </c>
       <c r="M21" s="4" t="inlineStr">
@@ -3020,7 +3020,7 @@
       </c>
       <c r="AA21" s="2" t="inlineStr">
         <is>
-          <t>*maa://21443 (78.64), **maa://23820 (30.19)</t>
+          <t>*maa://21443 (78.64), ***maa://23820 (29.63)</t>
         </is>
       </c>
       <c r="AC21" s="4" t="inlineStr">
@@ -3035,7 +3035,7 @@
       </c>
       <c r="AE21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.15), *maa://22432 (75.47)</t>
+          <t>maa://22524 (94.22), *maa://22432 (75.47)</t>
         </is>
       </c>
     </row>
@@ -3082,7 +3082,7 @@
       </c>
       <c r="K22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (87.21), *maa://22751 (77.05)</t>
+          <t>maa://27127 (87.36), *maa://22751 (77.05)</t>
         </is>
       </c>
       <c r="M22" s="4" t="inlineStr">
@@ -3127,7 +3127,7 @@
       </c>
       <c r="W22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.8), *maa://37649 (62.5)</t>
+          <t>maa://21282 (98.8), *maa://37649 (64.71)</t>
         </is>
       </c>
       <c r="Y22" s="4" t="inlineStr">
@@ -3204,7 +3204,7 @@
       </c>
       <c r="K23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (91.67), maa://39875 (94.29)</t>
+          <t>maa://39756 (92.03), maa://39875 (94.74)</t>
         </is>
       </c>
       <c r="M23" s="4" t="inlineStr">
@@ -3219,7 +3219,7 @@
       </c>
       <c r="O23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.62), *maa://29748 (75.41), ***maa://29785 (15.15), *maa://37566 (76.47)</t>
+          <t>maa://30587 (91.62), *maa://29748 (74.8), ***maa://29785 (15.15), *maa://37566 (76.47)</t>
         </is>
       </c>
       <c r="Q23" s="4" t="inlineStr">
@@ -3371,7 +3371,7 @@
       </c>
       <c r="W24" s="2" t="inlineStr">
         <is>
-          <t>maa://23504 (93.02), maa://29988 (85.79), **maa://22892 (40.43), *maa://25141 (77.31), *maa://36663 (79.25), ***maa://22815 (23.08)</t>
+          <t>maa://23504 (93.02), maa://29988 (85.86), **maa://22892 (40.43), *maa://25141 (77.31), *maa://36663 (79.25), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="4" t="inlineStr">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="AE24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (84.86), *maa://36672 (75.61), maa://29910 (95.65), **maa://21440 (34.55)</t>
+          <t>maa://22523 (84.86), *maa://36672 (75.61), maa://29910 (95.74), **maa://21440 (34.55)</t>
         </is>
       </c>
     </row>
@@ -3433,7 +3433,7 @@
       </c>
       <c r="G25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (77.78), *maa://25311 (75.56), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (77.95), *maa://25311 (74.73), ***maa://22725 (4.84)</t>
         </is>
       </c>
       <c r="I25" s="4" t="inlineStr">
@@ -3448,7 +3448,7 @@
       </c>
       <c r="K25" s="2" t="inlineStr">
         <is>
-          <t>maa://24378 (87.88)</t>
+          <t>maa://24378 (88.24)</t>
         </is>
       </c>
       <c r="M25" s="4" t="inlineStr">
@@ -3508,7 +3508,7 @@
       </c>
       <c r="AA25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (86.84), *maa://24516 (80.0), maa://26001 (92.31)</t>
+          <t>maa://31215 (85.9), *maa://24516 (80.0), maa://26001 (88.89)</t>
         </is>
       </c>
       <c r="AC25" s="4" t="inlineStr">
@@ -3555,7 +3555,7 @@
       </c>
       <c r="G26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (92.19)</t>
+          <t>maa://24913 (90.91)</t>
         </is>
       </c>
       <c r="I26" s="4" t="inlineStr">
@@ -3645,7 +3645,7 @@
       </c>
       <c r="AE26" s="2" t="inlineStr">
         <is>
-          <t>maa://30511 (83.33), *maa://29760 (54.55)</t>
+          <t>maa://30511 (83.87), *maa://29760 (54.55)</t>
         </is>
       </c>
     </row>
@@ -3784,7 +3784,7 @@
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.29), maa://25725 (81.82)</t>
+          <t>maa://24465 (90.3), maa://25725 (81.82)</t>
         </is>
       </c>
       <c r="E28" s="4" t="inlineStr">
@@ -3859,7 +3859,7 @@
       </c>
       <c r="W28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (85.19), ***maa://39723 (15.62)</t>
+          <t>maa://39929 (85.21), ***maa://39723 (15.15)</t>
         </is>
       </c>
       <c r="Y28" s="4" t="inlineStr">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="AE28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (93.9), *maa://36701 (64.0)</t>
+          <t>maa://36660 (94.02), *maa://36701 (64.0)</t>
         </is>
       </c>
     </row>
@@ -3921,7 +3921,7 @@
       </c>
       <c r="G29" s="2" t="inlineStr">
         <is>
-          <t>*maa://25175 (73.81)</t>
+          <t>*maa://25175 (70.45)</t>
         </is>
       </c>
       <c r="I29" s="4" t="inlineStr">
@@ -3936,7 +3936,7 @@
       </c>
       <c r="K29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.31), *maa://28440 (72.5), maa://31400 (100.0), *maa://28650 (66.67)</t>
+          <t>maa://28432 (93.33), *maa://28440 (72.5), maa://31400 (100.0), *maa://28650 (66.67)</t>
         </is>
       </c>
       <c r="M29" s="4" t="inlineStr">
@@ -3951,7 +3951,7 @@
       </c>
       <c r="O29" s="2" t="inlineStr">
         <is>
-          <t>*maa://23168 (55.77), **maa://30050 (44.44)</t>
+          <t>*maa://23168 (55.77), **maa://30050 (42.11)</t>
         </is>
       </c>
       <c r="Q29" s="4" t="inlineStr">
@@ -4011,7 +4011,7 @@
       </c>
       <c r="AE29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.44), ***maa://34960 (9.09)</t>
+          <t>*maa://24080 (68.25), ***maa://34960 (9.09)</t>
         </is>
       </c>
     </row>
@@ -4058,7 +4058,7 @@
       </c>
       <c r="K30" s="2" t="inlineStr">
         <is>
-          <t>maa://30442 (94.0)</t>
+          <t>maa://30442 (94.12)</t>
         </is>
       </c>
       <c r="M30" s="4" t="inlineStr">
@@ -4180,7 +4180,7 @@
       </c>
       <c r="K31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.42), *maa://36258 (79.45)</t>
+          <t>maa://35926 (93.42), maa://36258 (80.26)</t>
         </is>
       </c>
       <c r="M31" s="4" t="inlineStr">
@@ -4332,7 +4332,7 @@
       </c>
       <c r="S32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (100.0), maa://41238 (90.91)</t>
+          <t>maa://41108 (88.89), maa://41238 (93.33)</t>
         </is>
       </c>
       <c r="U32" s="4" t="inlineStr">
@@ -4439,7 +4439,7 @@
       </c>
       <c r="O33" s="2" t="inlineStr">
         <is>
-          <t>*maa://21956 (78.74), maa://22730 (82.14)</t>
+          <t>*maa://21956 (78.91), maa://22730 (82.14)</t>
         </is>
       </c>
       <c r="Q33" s="4" t="inlineStr">
@@ -4623,7 +4623,7 @@
       </c>
       <c r="K35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (95.0)</t>
+          <t>maa://41296 (96.15)</t>
         </is>
       </c>
       <c r="M35" s="4" t="inlineStr">
@@ -4919,7 +4919,7 @@
       </c>
       <c r="AE38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.44)</t>
+          <t>maa://36697 (86.78)</t>
         </is>
       </c>
     </row>
@@ -4936,7 +4936,7 @@
       </c>
       <c r="G39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (86.92), maa://36670 (87.93), maa://30434 (88.89), ***maa://25036 (16.0)</t>
+          <t>maa://25199 (86.11), maa://36670 (88.33), maa://30434 (88.89), ***maa://25036 (16.0)</t>
         </is>
       </c>
       <c r="I39" s="4" t="inlineStr">
@@ -5048,7 +5048,7 @@
       </c>
       <c r="O40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (96.19), maa://21386 (95.63), maa://36664 (91.89)</t>
+          <t>maa://23278 (96.19), maa://21386 (95.63), maa://36664 (92.11)</t>
         </is>
       </c>
       <c r="Q40" s="4" t="inlineStr">
@@ -5179,7 +5179,7 @@
       </c>
       <c r="G43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (92.5), maa://21284 (82.93)</t>
+          <t>maa://22525 (92.56), maa://21284 (82.93)</t>
         </is>
       </c>
       <c r="M43" s="4" t="inlineStr">
@@ -5276,7 +5276,7 @@
       </c>
       <c r="G45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (85.88), maa://30807 (94.92), *maa://22767 (52.94), ***maa://20796 (13.79)</t>
+          <t>maa://21229 (85.47), maa://30807 (94.92), *maa://22767 (52.94), ***maa://20796 (13.79)</t>
         </is>
       </c>
       <c r="M45" s="4" t="inlineStr">
@@ -5326,7 +5326,7 @@
       </c>
       <c r="G46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.27)</t>
+          <t>maa://35931 (92.34)</t>
         </is>
       </c>
       <c r="M46" s="4" t="inlineStr">
@@ -5376,7 +5376,7 @@
       </c>
       <c r="G47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (95.79), maa://29661 (97.58), maa://28038 (84.62)</t>
+          <t>maa://27410 (95.79), maa://29661 (97.6), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="M47" s="4" t="inlineStr">
@@ -5607,7 +5607,7 @@
       </c>
       <c r="G53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.1), **maa://32434 (36.36)</t>
+          <t>maa://32534 (93.16), **maa://32434 (36.36)</t>
         </is>
       </c>
     </row>
@@ -5641,7 +5641,7 @@
       </c>
       <c r="G55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.06)</t>
+          <t>maa://32532 (92.13)</t>
         </is>
       </c>
     </row>
@@ -5675,7 +5675,7 @@
       </c>
       <c r="G57" s="2" t="inlineStr">
         <is>
-          <t>maa://25176 (97.67)</t>
+          <t>maa://25176 (97.73)</t>
         </is>
       </c>
     </row>
@@ -5692,7 +5692,7 @@
       </c>
       <c r="G58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (62.5)</t>
+          <t>*maa://37964 (58.82)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: Auto Update Data (#68)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -612,7 +612,7 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.1), maa://25390 (97.41), maa://36681 (91.94)</t>
+          <t>maa://24702 (94.1), maa://25390 (97.42), maa://36681 (92.06)</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
@@ -764,7 +764,7 @@
       </c>
       <c r="K3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (70.2), maa://20276 (82.35), *maa://22749 (62.5)</t>
+          <t>*maa://22880 (70.2), maa://20276 (82.48), *maa://22749 (62.5)</t>
         </is>
       </c>
       <c r="M3" s="4" t="inlineStr">
@@ -779,7 +779,7 @@
       </c>
       <c r="O3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (95.5), maa://26254 (95.24)</t>
+          <t>maa://21249 (95.57), maa://26254 (95.24)</t>
         </is>
       </c>
       <c r="Q3" s="4" t="inlineStr">
@@ -931,7 +931,7 @@
       </c>
       <c r="W4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.9), ***maa://31785 (15.74), ***maa://36683 (26.67)</t>
+          <t>**maa://32495 (48.12), ***maa://31785 (15.74), ***maa://36683 (26.67)</t>
         </is>
       </c>
       <c r="Y4" s="4" t="inlineStr">
@@ -1130,7 +1130,7 @@
       </c>
       <c r="K6" s="2" t="inlineStr">
         <is>
-          <t>maa://24839 (99.19)</t>
+          <t>maa://24839 (99.2)</t>
         </is>
       </c>
       <c r="M6" s="4" t="inlineStr">
@@ -1237,7 +1237,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>*maa://22763 (64.0)</t>
+          <t>*maa://22763 (65.38)</t>
         </is>
       </c>
       <c r="I7" s="4" t="inlineStr">
@@ -1327,7 +1327,7 @@
       </c>
       <c r="AE7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (70.42), *maa://36671 (73.17)</t>
+          <t>*maa://26191 (69.44), *maa://36671 (73.81)</t>
         </is>
       </c>
     </row>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="W8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (96.25)</t>
+          <t>maa://21411 (96.28)</t>
         </is>
       </c>
       <c r="Y8" s="4" t="inlineStr">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="W9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (96.84)</t>
+          <t>maa://26223 (96.88)</t>
         </is>
       </c>
       <c r="Y9" s="4" t="inlineStr">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.41), **maa://32237 (38.89), ***maa://34206 (14.29), ***maa://39951 (15.79), ***maa://39243 (25.0)</t>
+          <t>***maa://25695 (19.41), **maa://32237 (38.89), ***maa://34206 (14.29), ***maa://39951 (20.0), ***maa://39243 (25.0)</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="S10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (97.24), maa://22755 (87.5), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (97.26), maa://22755 (87.5), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="4" t="inlineStr">
@@ -1907,7 +1907,7 @@
       </c>
       <c r="W12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.67), *maa://21485 (76.56), maa://37962 (81.25)</t>
+          <t>maa://22753 (91.72), *maa://21485 (76.56), maa://37962 (81.25)</t>
         </is>
       </c>
       <c r="Y12" s="4" t="inlineStr">
@@ -1922,7 +1922,7 @@
       </c>
       <c r="AA12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.82), maa://36677 (94.74), maa://39872 (81.82)</t>
+          <t>maa://23669 (95.83), maa://36677 (94.74), maa://39872 (81.82)</t>
         </is>
       </c>
       <c r="AC12" s="4" t="inlineStr">
@@ -1999,7 +1999,7 @@
       </c>
       <c r="O13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (91.75), *maa://22583 (75.86), *maa://22500 (55.81)</t>
+          <t>maa://22676 (91.75), *maa://22583 (74.58), *maa://22500 (55.81)</t>
         </is>
       </c>
       <c r="Q13" s="4" t="inlineStr">
@@ -2029,7 +2029,7 @@
       </c>
       <c r="W13" s="2" t="inlineStr">
         <is>
-          <t>*maa://34957 (79.49), *maa://22768 (53.33)</t>
+          <t>*maa://34957 (77.5), *maa://22768 (53.33)</t>
         </is>
       </c>
       <c r="Y13" s="4" t="inlineStr">
@@ -2213,7 +2213,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.27), maa://21478 (91.18)</t>
+          <t>maa://24304 (88.33), maa://21478 (91.18)</t>
         </is>
       </c>
       <c r="I15" s="4" t="inlineStr">
@@ -2320,7 +2320,7 @@
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.15), maa://36679 (93.33), maa://37650 (95.0)</t>
+          <t>maa://21441 (96.15), maa://36679 (93.33), maa://37650 (95.24)</t>
         </is>
       </c>
       <c r="E16" s="4" t="inlineStr">
@@ -2410,7 +2410,7 @@
       </c>
       <c r="AA16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (96.0)</t>
+          <t>maa://26228 (96.05)</t>
         </is>
       </c>
       <c r="AC16" s="4" t="inlineStr">
@@ -2457,7 +2457,7 @@
       </c>
       <c r="G17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.57), *maa://39599 (78.57)</t>
+          <t>maa://22430 (88.57), *maa://39599 (80.0)</t>
         </is>
       </c>
       <c r="I17" s="4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="G18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (90.34)</t>
+          <t>maa://24421 (90.38)</t>
         </is>
       </c>
       <c r="I18" s="4" t="inlineStr">
@@ -2746,7 +2746,7 @@
       </c>
       <c r="S19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (98.7)</t>
+          <t>maa://24386 (98.72)</t>
         </is>
       </c>
       <c r="U19" s="4" t="inlineStr">
@@ -2838,7 +2838,7 @@
       </c>
       <c r="K20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.71)</t>
+          <t>maa://41331 (86.36)</t>
         </is>
       </c>
       <c r="M20" s="4" t="inlineStr">
@@ -3005,7 +3005,7 @@
       </c>
       <c r="W21" s="2" t="inlineStr">
         <is>
-          <t>maa://20110 (86.36), maa://34946 (90.32)</t>
+          <t>maa://20110 (86.57), maa://34946 (90.32)</t>
         </is>
       </c>
       <c r="Y21" s="4" t="inlineStr">
@@ -3020,7 +3020,7 @@
       </c>
       <c r="AA21" s="2" t="inlineStr">
         <is>
-          <t>*maa://21443 (78.64), ***maa://23820 (29.63)</t>
+          <t>*maa://21443 (78.7), ***maa://23820 (29.63)</t>
         </is>
       </c>
       <c r="AC21" s="4" t="inlineStr">
@@ -3035,7 +3035,7 @@
       </c>
       <c r="AE21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.22), *maa://22432 (75.47)</t>
+          <t>maa://22524 (94.25), *maa://22432 (75.47)</t>
         </is>
       </c>
     </row>
@@ -3169,12 +3169,12 @@
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.79)</t>
+          <t>***maa://28036 (28.79), maa://41753 (100.0)</t>
         </is>
       </c>
       <c r="E23" s="4" t="inlineStr">
@@ -3204,7 +3204,7 @@
       </c>
       <c r="K23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (92.03), maa://39875 (94.74)</t>
+          <t>maa://39756 (92.14), maa://39875 (95.0)</t>
         </is>
       </c>
       <c r="M23" s="4" t="inlineStr">
@@ -3249,7 +3249,7 @@
       </c>
       <c r="W23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (60.0)</t>
+          <t>*maa://28503 (60.71)</t>
         </is>
       </c>
       <c r="Y23" s="4" t="inlineStr">
@@ -3296,7 +3296,7 @@
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>maa://24368 (80.37)</t>
+          <t>maa://24368 (80.43)</t>
         </is>
       </c>
       <c r="E24" s="4" t="inlineStr">
@@ -3371,7 +3371,7 @@
       </c>
       <c r="W24" s="2" t="inlineStr">
         <is>
-          <t>maa://23504 (93.02), maa://29988 (85.86), **maa://22892 (40.43), *maa://25141 (77.31), *maa://36663 (79.25), ***maa://22815 (23.08)</t>
+          <t>maa://23504 (93.04), maa://29988 (85.86), **maa://22892 (40.43), *maa://25141 (76.86), *maa://36663 (79.25), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="4" t="inlineStr">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="AE24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (84.86), *maa://36672 (75.61), maa://29910 (95.74), **maa://21440 (34.55)</t>
+          <t>maa://22523 (84.86), *maa://36672 (75.61), maa://29910 (93.88), **maa://21440 (34.55)</t>
         </is>
       </c>
     </row>
@@ -3433,7 +3433,7 @@
       </c>
       <c r="G25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (77.95), *maa://25311 (74.73), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (77.34), *maa://25311 (74.73), ***maa://22725 (4.84)</t>
         </is>
       </c>
       <c r="I25" s="4" t="inlineStr">
@@ -3677,7 +3677,7 @@
       </c>
       <c r="G27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (49.32), maa://34494 (100.0), **maa://36665 (50.0), maa://39601 (100.0)</t>
+          <t>**maa://21283 (49.32), maa://34494 (100.0), **maa://36665 (44.44), maa://39601 (85.71)</t>
         </is>
       </c>
       <c r="I27" s="4" t="inlineStr">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="S27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (77.14)</t>
+          <t>*maa://30624 (77.78)</t>
         </is>
       </c>
       <c r="U27" s="4" t="inlineStr">
@@ -3854,12 +3854,12 @@
       </c>
       <c r="V28" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="W28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (85.21), ***maa://39723 (15.15)</t>
+          <t>maa://39929 (85.71), ***maa://39723 (15.15), maa://41749 (100.0)</t>
         </is>
       </c>
       <c r="Y28" s="4" t="inlineStr">
@@ -3906,7 +3906,7 @@
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>maa://31694 (97.73)</t>
+          <t>maa://31694 (97.78)</t>
         </is>
       </c>
       <c r="E29" s="4" t="inlineStr">
@@ -4011,7 +4011,7 @@
       </c>
       <c r="AE29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.25), ***maa://34960 (9.09)</t>
+          <t>*maa://24080 (68.33), ***maa://34960 (9.09)</t>
         </is>
       </c>
     </row>
@@ -4332,7 +4332,7 @@
       </c>
       <c r="S32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (88.89), maa://41238 (93.33)</t>
+          <t>maa://41108 (91.67), maa://41238 (93.94)</t>
         </is>
       </c>
       <c r="U32" s="4" t="inlineStr">
@@ -4623,7 +4623,7 @@
       </c>
       <c r="K35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.15)</t>
+          <t>maa://41296 (96.43)</t>
         </is>
       </c>
       <c r="M35" s="4" t="inlineStr">
@@ -4919,7 +4919,7 @@
       </c>
       <c r="AE38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.78)</t>
+          <t>maa://36697 (86.18)</t>
         </is>
       </c>
     </row>
@@ -5048,7 +5048,7 @@
       </c>
       <c r="O40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (96.19), maa://21386 (95.63), maa://36664 (92.11)</t>
+          <t>maa://23278 (96.19), maa://21386 (95.63), maa://36664 (92.31)</t>
         </is>
       </c>
       <c r="Q40" s="4" t="inlineStr">
@@ -5095,7 +5095,7 @@
       </c>
       <c r="O41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (34.78)</t>
+          <t>**maa://35616 (36.0)</t>
         </is>
       </c>
       <c r="Q41" s="4" t="inlineStr">
@@ -5226,7 +5226,7 @@
       </c>
       <c r="G44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.47), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.49), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="M44" s="4" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#69)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -946,7 +946,7 @@
       </c>
       <c r="AA4" s="2" t="inlineStr">
         <is>
-          <t>*maa://32658 (76.92)</t>
+          <t>*maa://32658 (71.43)</t>
         </is>
       </c>
       <c r="AC4" s="4" t="inlineStr">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="O5" s="2" t="inlineStr">
         <is>
-          <t>maa://21919 (95.56), maa://21281 (91.67)</t>
+          <t>maa://21919 (95.56), maa://21281 (92.31)</t>
         </is>
       </c>
       <c r="Q5" s="4" t="inlineStr">
@@ -1145,7 +1145,7 @@
       </c>
       <c r="O6" s="2" t="inlineStr">
         <is>
-          <t>maa://31836 (92.86), maa://30381 (100.0)</t>
+          <t>maa://31836 (93.33), maa://30381 (100.0)</t>
         </is>
       </c>
       <c r="Q6" s="4" t="inlineStr">
@@ -1267,7 +1267,7 @@
       </c>
       <c r="O7" s="2" t="inlineStr">
         <is>
-          <t>maa://22750 (96.88)</t>
+          <t>maa://22750 (96.97)</t>
         </is>
       </c>
       <c r="Q7" s="4" t="inlineStr">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="S10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (97.26), maa://22755 (87.5), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (97.28), maa://22755 (87.5), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="4" t="inlineStr">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="AE10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (56.52), *maa://22733 (58.62), maa://22761 (100.0)</t>
+          <t>*maa://25021 (55.71), *maa://22733 (58.62), maa://22761 (100.0)</t>
         </is>
       </c>
     </row>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (75.5), **maa://22728 (47.62)</t>
+          <t>*maa://21248 (75.62), **maa://22728 (47.62)</t>
         </is>
       </c>
       <c r="I13" s="4" t="inlineStr">
@@ -2166,7 +2166,7 @@
       </c>
       <c r="AA14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (96.36)</t>
+          <t>maa://22764 (96.43)</t>
         </is>
       </c>
       <c r="AC14" s="4" t="inlineStr">
@@ -2303,7 +2303,7 @@
       </c>
       <c r="AE15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.55), *maa://22766 (73.0), *maa://36666 (76.67)</t>
+          <t>maa://21364 (80.61), *maa://22766 (73.0), *maa://36666 (76.67)</t>
         </is>
       </c>
     </row>
@@ -2457,7 +2457,7 @@
       </c>
       <c r="G17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.57), *maa://39599 (80.0)</t>
+          <t>maa://22430 (88.57), maa://39599 (81.25)</t>
         </is>
       </c>
       <c r="I17" s="4" t="inlineStr">
@@ -2654,7 +2654,7 @@
       </c>
       <c r="AA18" s="2" t="inlineStr">
         <is>
-          <t>maa://24393 (100.0)</t>
+          <t>maa://24393 (97.14)</t>
         </is>
       </c>
       <c r="AC18" s="4" t="inlineStr">
@@ -2808,7 +2808,7 @@
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.7), maa://25198 (93.62), **maa://20795 (49.18), maa://36680 (100.0)</t>
+          <t>maa://21432 (90.7), maa://25198 (93.62), **maa://20795 (49.59), maa://36680 (100.0)</t>
         </is>
       </c>
       <c r="E20" s="4" t="inlineStr">
@@ -2838,7 +2838,7 @@
       </c>
       <c r="K20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (86.36)</t>
+          <t>maa://41331 (86.96)</t>
         </is>
       </c>
       <c r="M20" s="4" t="inlineStr">
@@ -3082,7 +3082,7 @@
       </c>
       <c r="K22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (87.36), *maa://22751 (77.05)</t>
+          <t>maa://27127 (86.36), *maa://22751 (77.05)</t>
         </is>
       </c>
       <c r="M22" s="4" t="inlineStr">
@@ -3204,7 +3204,7 @@
       </c>
       <c r="K23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (92.14), maa://39875 (95.0)</t>
+          <t>maa://39756 (92.2), maa://39875 (95.12)</t>
         </is>
       </c>
       <c r="M23" s="4" t="inlineStr">
@@ -3249,7 +3249,7 @@
       </c>
       <c r="W23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (60.71)</t>
+          <t>*maa://28503 (61.4)</t>
         </is>
       </c>
       <c r="Y23" s="4" t="inlineStr">
@@ -3478,7 +3478,7 @@
       </c>
       <c r="S25" s="2" t="inlineStr">
         <is>
-          <t>maa://20109 (92.64), maa://22545 (100.0)</t>
+          <t>maa://20109 (92.68), maa://22545 (100.0)</t>
         </is>
       </c>
       <c r="U25" s="4" t="inlineStr">
@@ -3538,11 +3538,7 @@
           <t>0</t>
         </is>
       </c>
-      <c r="C26" s="2" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="C26" s="2" t="inlineStr"/>
       <c r="E26" s="4" t="inlineStr">
         <is>
           <t>宴</t>
@@ -3859,7 +3855,7 @@
       </c>
       <c r="W28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (85.71), ***maa://39723 (15.15), maa://41749 (100.0)</t>
+          <t>maa://39929 (85.8), ***maa://39723 (15.15), **maa://41749 (50.0)</t>
         </is>
       </c>
       <c r="Y28" s="4" t="inlineStr">
@@ -3936,7 +3932,7 @@
       </c>
       <c r="K29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.33), *maa://28440 (72.5), maa://31400 (100.0), *maa://28650 (66.67)</t>
+          <t>maa://28432 (93.36), *maa://28440 (72.5), maa://31400 (100.0), *maa://28650 (66.67)</t>
         </is>
       </c>
       <c r="M29" s="4" t="inlineStr">
@@ -4332,7 +4328,7 @@
       </c>
       <c r="S32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (91.67), maa://41238 (93.94)</t>
+          <t>maa://41108 (85.71), maa://41238 (94.12)</t>
         </is>
       </c>
       <c r="U32" s="4" t="inlineStr">
@@ -4623,7 +4619,7 @@
       </c>
       <c r="K35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.43)</t>
+          <t>maa://41296 (96.55)</t>
         </is>
       </c>
       <c r="M35" s="4" t="inlineStr">
@@ -4936,7 +4932,7 @@
       </c>
       <c r="G39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (86.11), maa://36670 (88.33), maa://30434 (88.89), ***maa://25036 (16.0)</t>
+          <t>maa://25199 (86.11), maa://36670 (88.52), maa://30434 (88.89), ***maa://25036 (16.0)</t>
         </is>
       </c>
       <c r="I39" s="4" t="inlineStr">
@@ -5675,7 +5671,7 @@
       </c>
       <c r="G57" s="2" t="inlineStr">
         <is>
-          <t>maa://25176 (97.73)</t>
+          <t>maa://25176 (97.78)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: Auto Update Data (#70)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -642,7 +642,7 @@
       </c>
       <c r="K2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (54.97), *maa://30515 (69.7), ***maa://20792 (11.93), *maa://34787 (72.13), maa://39402 (84.0), ***maa://29083 (29.41)</t>
+          <t>*maa://24633 (54.97), *maa://30515 (69.7), ***maa://20792 (11.93), *maa://34787 (72.13), maa://39402 (85.19), ***maa://29083 (29.41)</t>
         </is>
       </c>
       <c r="M2" s="4" t="inlineStr">
@@ -717,7 +717,7 @@
       </c>
       <c r="AE2" s="2" t="inlineStr">
         <is>
-          <t>***maa://21730 (17.19), maa://25251 (92.0), ***maa://39501 (20.0), *maa://36675 (60.0)</t>
+          <t>***maa://21730 (17.19), maa://25251 (92.11), ***maa://39501 (20.0), *maa://36675 (60.0)</t>
         </is>
       </c>
     </row>
@@ -839,7 +839,7 @@
       </c>
       <c r="AE3" s="2" t="inlineStr">
         <is>
-          <t>*maa://21289 (72.22)</t>
+          <t>*maa://21289 (68.42)</t>
         </is>
       </c>
     </row>
@@ -961,7 +961,7 @@
       </c>
       <c r="AE4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (63.41), ***maa://26209 (13.04), *maa://39394 (70.0)</t>
+          <t>*maa://30062 (63.41), ***maa://26209 (13.04), *maa://39394 (75.0)</t>
         </is>
       </c>
     </row>
@@ -1556,7 +1556,7 @@
       </c>
       <c r="AA9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.65), ***maa://22740 (5.88), **maa://27377 (46.15), ***maa://25174 (20.0), **maa://39938 (50.0), maa://40166 (100.0)</t>
+          <t>maa://28711 (87.8), ***maa://22740 (5.88), **maa://27377 (46.15), ***maa://25174 (20.0), *maa://39938 (53.85), maa://40166 (100.0)</t>
         </is>
       </c>
       <c r="AC9" s="4" t="inlineStr">
@@ -1785,7 +1785,7 @@
       </c>
       <c r="W11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.78)</t>
+          <t>maa://36713 (97.79)</t>
         </is>
       </c>
       <c r="Y11" s="4" t="inlineStr">
@@ -2106,7 +2106,7 @@
       </c>
       <c r="K14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.12), maa://21288 (96.21), maa://36682 (100.0), maa://39841 (92.11)</t>
+          <t>maa://26245 (96.12), maa://21288 (96.21), maa://36682 (100.0), maa://39841 (92.5)</t>
         </is>
       </c>
       <c r="M14" s="4" t="inlineStr">
@@ -2121,7 +2121,7 @@
       </c>
       <c r="O14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.45), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.46), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="4" t="inlineStr">
@@ -2303,7 +2303,7 @@
       </c>
       <c r="AE15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.61), *maa://22766 (73.0), *maa://36666 (76.67)</t>
+          <t>maa://21364 (80.61), *maa://22766 (73.0), *maa://36666 (77.05)</t>
         </is>
       </c>
     </row>
@@ -2564,7 +2564,7 @@
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.43)</t>
+          <t>maa://24570 (96.45)</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
@@ -2776,7 +2776,7 @@
       </c>
       <c r="AA19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (60.16), *maa://36668 (52.17)</t>
+          <t>*maa://30709 (60.27), *maa://36668 (52.17)</t>
         </is>
       </c>
       <c r="AC19" s="4" t="inlineStr">
@@ -2838,7 +2838,7 @@
       </c>
       <c r="K20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (86.96)</t>
+          <t>maa://41331 (87.5)</t>
         </is>
       </c>
       <c r="M20" s="4" t="inlineStr">
@@ -3020,7 +3020,7 @@
       </c>
       <c r="AA21" s="2" t="inlineStr">
         <is>
-          <t>*maa://21443 (78.7), ***maa://23820 (29.63)</t>
+          <t>*maa://21443 (78.77), ***maa://23820 (29.63)</t>
         </is>
       </c>
       <c r="AC21" s="4" t="inlineStr">
@@ -3204,7 +3204,7 @@
       </c>
       <c r="K23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (92.2), maa://39875 (95.12)</t>
+          <t>maa://39756 (92.31), maa://39875 (95.24)</t>
         </is>
       </c>
       <c r="M23" s="4" t="inlineStr">
@@ -3219,7 +3219,7 @@
       </c>
       <c r="O23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.62), *maa://29748 (74.8), ***maa://29785 (15.15), *maa://37566 (76.47)</t>
+          <t>maa://30587 (91.62), *maa://29748 (75.2), ***maa://29785 (15.15), *maa://37566 (76.47)</t>
         </is>
       </c>
       <c r="Q23" s="4" t="inlineStr">
@@ -3371,7 +3371,7 @@
       </c>
       <c r="W24" s="2" t="inlineStr">
         <is>
-          <t>maa://23504 (93.04), maa://29988 (85.86), **maa://22892 (40.43), *maa://25141 (76.86), *maa://36663 (79.25), ***maa://22815 (23.08)</t>
+          <t>maa://23504 (93.04), maa://29988 (85.86), **maa://22892 (40.43), *maa://25141 (76.86), *maa://36663 (79.63), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="4" t="inlineStr">
@@ -3418,7 +3418,7 @@
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.07)</t>
+          <t>maa://29753 (95.11)</t>
         </is>
       </c>
       <c r="E25" s="4" t="inlineStr">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="G25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (77.34), *maa://25311 (74.73), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (76.74), *maa://25311 (74.73), ***maa://22725 (4.84)</t>
         </is>
       </c>
       <c r="I25" s="4" t="inlineStr">
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AE26" s="2" t="inlineStr">
         <is>
-          <t>maa://30511 (83.87), *maa://29760 (54.55)</t>
+          <t>maa://30511 (83.87), *maa://29760 (61.54)</t>
         </is>
       </c>
     </row>
@@ -3673,7 +3673,7 @@
       </c>
       <c r="G27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (49.32), maa://34494 (100.0), **maa://36665 (44.44), maa://39601 (85.71)</t>
+          <t>**maa://21283 (48.65), maa://34494 (100.0), **maa://36665 (44.44), maa://39601 (85.71)</t>
         </is>
       </c>
       <c r="I27" s="4" t="inlineStr">
@@ -3780,7 +3780,7 @@
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.3), maa://25725 (81.82)</t>
+          <t>maa://24465 (90.32), maa://25725 (81.82)</t>
         </is>
       </c>
       <c r="E28" s="4" t="inlineStr">
@@ -3855,7 +3855,7 @@
       </c>
       <c r="W28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (85.8), ***maa://39723 (15.15), **maa://41749 (50.0)</t>
+          <t>maa://39929 (85.8), ***maa://39723 (15.15), *maa://41749 (80.0)</t>
         </is>
       </c>
       <c r="Y28" s="4" t="inlineStr">
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AE28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (94.02), *maa://36701 (64.0)</t>
+          <t>maa://36660 (94.05), *maa://36701 (64.0)</t>
         </is>
       </c>
     </row>
@@ -3932,7 +3932,7 @@
       </c>
       <c r="K29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.36), *maa://28440 (72.5), maa://31400 (100.0), *maa://28650 (66.67)</t>
+          <t>maa://28432 (93.38), *maa://28440 (72.5), maa://31400 (100.0), *maa://28650 (66.67)</t>
         </is>
       </c>
       <c r="M29" s="4" t="inlineStr">
@@ -4176,7 +4176,7 @@
       </c>
       <c r="K31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.42), maa://36258 (80.26)</t>
+          <t>maa://35926 (93.45), maa://36258 (80.26)</t>
         </is>
       </c>
       <c r="M31" s="4" t="inlineStr">
@@ -4328,7 +4328,7 @@
       </c>
       <c r="S32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (85.71), maa://41238 (94.12)</t>
+          <t>maa://41108 (88.24), maa://41238 (94.12)</t>
         </is>
       </c>
       <c r="U32" s="4" t="inlineStr">
@@ -5322,7 +5322,7 @@
       </c>
       <c r="G46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.34)</t>
+          <t>maa://35931 (92.38)</t>
         </is>
       </c>
       <c r="M46" s="4" t="inlineStr">
@@ -5372,7 +5372,7 @@
       </c>
       <c r="G47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (95.79), maa://29661 (97.6), maa://28038 (84.62)</t>
+          <t>maa://27410 (95.79), maa://29661 (97.64), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="M47" s="4" t="inlineStr">
@@ -5637,7 +5637,7 @@
       </c>
       <c r="G55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.13)</t>
+          <t>maa://32532 (92.17)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: Auto Update Data (#71)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.41), **maa://32237 (38.89), ***maa://34206 (14.29), ***maa://39951 (20.0), ***maa://39243 (25.0)</t>
+          <t>***maa://25695 (19.41), **maa://32237 (38.89), ***maa://34206 (14.29), ***maa://39951 (19.05), ***maa://39243 (25.0)</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
@@ -1770,7 +1770,7 @@
       </c>
       <c r="S11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (94.96), maa://22501 (98.08)</t>
+          <t>maa://22747 (95.0), maa://22501 (98.08)</t>
         </is>
       </c>
       <c r="U11" s="4" t="inlineStr">
@@ -1785,7 +1785,7 @@
       </c>
       <c r="W11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.79)</t>
+          <t>maa://36713 (97.8)</t>
         </is>
       </c>
       <c r="Y11" s="4" t="inlineStr">
@@ -1832,7 +1832,7 @@
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>maa://30766 (88.46), **maa://36678 (50.0)</t>
+          <t>maa://30766 (88.89), **maa://36678 (50.0)</t>
         </is>
       </c>
       <c r="E12" s="4" t="inlineStr">
@@ -1922,7 +1922,7 @@
       </c>
       <c r="AA12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.83), maa://36677 (94.74), maa://39872 (81.82)</t>
+          <t>maa://23669 (95.83), maa://36677 (94.74), maa://39872 (83.33)</t>
         </is>
       </c>
       <c r="AC12" s="4" t="inlineStr">
@@ -1969,7 +1969,7 @@
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (75.62), **maa://22728 (47.62)</t>
+          <t>*maa://21248 (75.74), **maa://22728 (47.62)</t>
         </is>
       </c>
       <c r="I13" s="4" t="inlineStr">
@@ -2029,7 +2029,7 @@
       </c>
       <c r="W13" s="2" t="inlineStr">
         <is>
-          <t>*maa://34957 (77.5), *maa://22768 (53.33)</t>
+          <t>*maa://34957 (78.05), *maa://22768 (53.33)</t>
         </is>
       </c>
       <c r="Y13" s="4" t="inlineStr">
@@ -2076,7 +2076,7 @@
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>maa://30764 (85.0)</t>
+          <t>maa://30764 (85.37)</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr">
@@ -2380,7 +2380,7 @@
       </c>
       <c r="S16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (95.14), *maa://28648 (69.09), *maa://36674 (76.0)</t>
+          <t>maa://22729 (95.14), *maa://28648 (69.09), *maa://36674 (76.92)</t>
         </is>
       </c>
       <c r="U16" s="4" t="inlineStr">
@@ -2442,7 +2442,7 @@
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>*maa://21624 (80.0)</t>
+          <t>maa://21624 (80.65)</t>
         </is>
       </c>
       <c r="E17" s="4" t="inlineStr">
@@ -2457,7 +2457,7 @@
       </c>
       <c r="G17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.57), maa://39599 (81.25)</t>
+          <t>maa://22430 (88.57), maa://39599 (82.35)</t>
         </is>
       </c>
       <c r="I17" s="4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="G18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (90.38)</t>
+          <t>maa://24421 (90.43)</t>
         </is>
       </c>
       <c r="I18" s="4" t="inlineStr">
@@ -2776,7 +2776,7 @@
       </c>
       <c r="AA19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (60.27), *maa://36668 (52.17)</t>
+          <t>*maa://30709 (60.38), *maa://36668 (52.17)</t>
         </is>
       </c>
       <c r="AC19" s="4" t="inlineStr">
@@ -2838,7 +2838,7 @@
       </c>
       <c r="K20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (87.5)</t>
+          <t>maa://41331 (88.0)</t>
         </is>
       </c>
       <c r="M20" s="4" t="inlineStr">
@@ -2853,7 +2853,7 @@
       </c>
       <c r="O20" s="2" t="inlineStr">
         <is>
-          <t>maa://37442 (96.3)</t>
+          <t>maa://37442 (96.43)</t>
         </is>
       </c>
       <c r="Q20" s="4" t="inlineStr">
@@ -3020,7 +3020,7 @@
       </c>
       <c r="AA21" s="2" t="inlineStr">
         <is>
-          <t>*maa://21443 (78.77), ***maa://23820 (29.63)</t>
+          <t>*maa://21443 (78.83), ***maa://23820 (29.63)</t>
         </is>
       </c>
       <c r="AC21" s="4" t="inlineStr">
@@ -3035,7 +3035,7 @@
       </c>
       <c r="AE21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.25), *maa://22432 (75.47)</t>
+          <t>maa://22524 (94.25), *maa://22432 (74.07)</t>
         </is>
       </c>
     </row>
@@ -3204,7 +3204,7 @@
       </c>
       <c r="K23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (92.31), maa://39875 (95.24)</t>
+          <t>maa://39756 (91.67), maa://39875 (95.45)</t>
         </is>
       </c>
       <c r="M23" s="4" t="inlineStr">
@@ -3219,7 +3219,7 @@
       </c>
       <c r="O23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.62), *maa://29748 (75.2), ***maa://29785 (15.15), *maa://37566 (76.47)</t>
+          <t>maa://30587 (91.62), *maa://29748 (75.2), ***maa://29785 (15.15), *maa://37566 (77.78)</t>
         </is>
       </c>
       <c r="Q23" s="4" t="inlineStr">
@@ -3296,7 +3296,7 @@
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>maa://24368 (80.43)</t>
+          <t>maa://24368 (80.5)</t>
         </is>
       </c>
       <c r="E24" s="4" t="inlineStr">
@@ -3535,10 +3535,14 @@
       </c>
       <c r="B26" s="4" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C26" s="2" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="inlineStr">
+        <is>
+          <t>maa://41802 (100.0)</t>
+        </is>
+      </c>
       <c r="E26" s="4" t="inlineStr">
         <is>
           <t>宴</t>
@@ -3780,7 +3784,7 @@
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.32), maa://25725 (81.82)</t>
+          <t>maa://24465 (90.32), maa://25725 (82.05)</t>
         </is>
       </c>
       <c r="E28" s="4" t="inlineStr">
@@ -3810,7 +3814,7 @@
       </c>
       <c r="K28" s="2" t="inlineStr">
         <is>
-          <t>*maa://30770 (77.5)</t>
+          <t>*maa://30770 (78.05)</t>
         </is>
       </c>
       <c r="M28" s="4" t="inlineStr">
@@ -3855,7 +3859,7 @@
       </c>
       <c r="W28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (85.8), ***maa://39723 (15.15), *maa://41749 (80.0)</t>
+          <t>maa://39929 (85.96), ***maa://39723 (15.15), *maa://41749 (66.67)</t>
         </is>
       </c>
       <c r="Y28" s="4" t="inlineStr">
@@ -3885,7 +3889,7 @@
       </c>
       <c r="AE28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (94.05), *maa://36701 (64.0)</t>
+          <t>maa://36660 (94.07), *maa://36701 (64.0)</t>
         </is>
       </c>
     </row>
@@ -3902,7 +3906,7 @@
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>maa://31694 (97.78)</t>
+          <t>maa://31694 (97.87)</t>
         </is>
       </c>
       <c r="E29" s="4" t="inlineStr">
@@ -3932,7 +3936,7 @@
       </c>
       <c r="K29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.38), *maa://28440 (72.5), maa://31400 (100.0), *maa://28650 (66.67)</t>
+          <t>maa://28432 (93.4), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (66.67)</t>
         </is>
       </c>
       <c r="M29" s="4" t="inlineStr">
@@ -4054,7 +4058,7 @@
       </c>
       <c r="K30" s="2" t="inlineStr">
         <is>
-          <t>maa://30442 (94.12)</t>
+          <t>maa://30442 (94.23)</t>
         </is>
       </c>
       <c r="M30" s="4" t="inlineStr">
@@ -4176,7 +4180,7 @@
       </c>
       <c r="K31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.45), maa://36258 (80.26)</t>
+          <t>maa://35926 (93.48), maa://36258 (80.26)</t>
         </is>
       </c>
       <c r="M31" s="4" t="inlineStr">
@@ -4328,7 +4332,7 @@
       </c>
       <c r="S32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (88.24), maa://41238 (94.12)</t>
+          <t>maa://41108 (89.47), maa://41238 (94.12)</t>
         </is>
       </c>
       <c r="U32" s="4" t="inlineStr">
@@ -4619,7 +4623,7 @@
       </c>
       <c r="K35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.55)</t>
+          <t>maa://41296 (96.77)</t>
         </is>
       </c>
       <c r="M35" s="4" t="inlineStr">
@@ -4696,7 +4700,7 @@
       </c>
       <c r="G36" s="2" t="inlineStr">
         <is>
-          <t>maa://24375 (92.11)</t>
+          <t>maa://24375 (92.31)</t>
         </is>
       </c>
       <c r="I36" s="4" t="inlineStr">
@@ -4932,7 +4936,7 @@
       </c>
       <c r="G39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (86.11), maa://36670 (88.52), maa://30434 (88.89), ***maa://25036 (16.0)</t>
+          <t>maa://25199 (86.11), maa://36670 (88.71), maa://30434 (88.89), ***maa://25036 (16.0)</t>
         </is>
       </c>
       <c r="I39" s="4" t="inlineStr">
@@ -5076,7 +5080,7 @@
       </c>
       <c r="G41" s="2" t="inlineStr">
         <is>
-          <t>maa://24466 (94.74)</t>
+          <t>maa://24466 (94.87)</t>
         </is>
       </c>
       <c r="M41" s="4" t="inlineStr">
@@ -5287,7 +5291,7 @@
       </c>
       <c r="O45" s="2" t="inlineStr">
         <is>
-          <t>*maa://36237 (60.0)</t>
+          <t>*maa://36237 (54.55)</t>
         </is>
       </c>
       <c r="Q45" s="4" t="inlineStr">
@@ -5322,7 +5326,7 @@
       </c>
       <c r="G46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.38)</t>
+          <t>maa://35931 (92.41)</t>
         </is>
       </c>
       <c r="M46" s="4" t="inlineStr">
@@ -5539,7 +5543,7 @@
       </c>
       <c r="G51" s="2" t="inlineStr">
         <is>
-          <t>*maa://30769 (76.92)</t>
+          <t>*maa://30769 (78.57)</t>
         </is>
       </c>
       <c r="M51" s="4" t="inlineStr">
@@ -5603,7 +5607,7 @@
       </c>
       <c r="G53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.16), **maa://32434 (36.36)</t>
+          <t>maa://32534 (93.18), **maa://32434 (36.36)</t>
         </is>
       </c>
     </row>
@@ -5637,7 +5641,7 @@
       </c>
       <c r="G55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.17)</t>
+          <t>maa://32532 (92.24)</t>
         </is>
       </c>
     </row>
@@ -5688,7 +5692,7 @@
       </c>
       <c r="G58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (58.82)</t>
+          <t>*maa://37964 (61.11)</t>
         </is>
       </c>
     </row>
@@ -5722,7 +5726,7 @@
       </c>
       <c r="G60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (55.56)</t>
+          <t>**maa://40438 (45.45)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: Auto Update Data (#72)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -612,7 +612,7 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.1), maa://25390 (97.42), maa://36681 (92.06)</t>
+          <t>maa://24702 (94.1), maa://25390 (97.42), maa://36681 (92.19)</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
@@ -717,7 +717,7 @@
       </c>
       <c r="AE2" s="2" t="inlineStr">
         <is>
-          <t>***maa://21730 (17.19), maa://25251 (92.11), ***maa://39501 (20.0), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.21), ***maa://21730 (17.19), ***maa://39501 (18.18), *maa://36675 (60.0)</t>
         </is>
       </c>
     </row>
@@ -779,7 +779,7 @@
       </c>
       <c r="O3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (95.57), maa://26254 (95.24)</t>
+          <t>maa://21249 (95.1), maa://26254 (95.24)</t>
         </is>
       </c>
       <c r="Q3" s="4" t="inlineStr">
@@ -809,7 +809,7 @@
       </c>
       <c r="W3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.81), maa://27484 (95.6), maa://27480 (82.35)</t>
+          <t>maa://27396 (84.81), maa://27484 (95.65), maa://27480 (82.35)</t>
         </is>
       </c>
       <c r="Y3" s="4" t="inlineStr">
@@ -824,7 +824,7 @@
       </c>
       <c r="AA3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (95.83)</t>
+          <t>maa://24390 (96.0)</t>
         </is>
       </c>
       <c r="AC3" s="4" t="inlineStr">
@@ -916,7 +916,7 @@
       </c>
       <c r="S4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (98.72), maa://22754 (91.67), maa://27295 (80.39), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (98.73), maa://22754 (91.67), maa://27295 (80.39), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="4" t="inlineStr">
@@ -931,7 +931,7 @@
       </c>
       <c r="W4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.12), ***maa://31785 (15.74), ***maa://36683 (26.67)</t>
+          <t>**maa://32495 (48.13), ***maa://31785 (16.51), ***maa://36683 (26.67)</t>
         </is>
       </c>
       <c r="Y4" s="4" t="inlineStr">
@@ -961,7 +961,7 @@
       </c>
       <c r="AE4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (63.41), ***maa://26209 (13.04), *maa://39394 (75.0)</t>
+          <t>*maa://30062 (63.41), ***maa://26209 (13.04), *maa://39394 (76.92)</t>
         </is>
       </c>
     </row>
@@ -978,7 +978,7 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (82.54), maa://22744 (82.61)</t>
+          <t>maa://21245 (82.63), maa://22744 (83.33)</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -1068,7 +1068,7 @@
       </c>
       <c r="AA5" s="2" t="inlineStr">
         <is>
-          <t>*maa://29863 (73.08), ***maa://22752 (13.33), **maa://26013 (33.33)</t>
+          <t>*maa://29863 (74.07), ***maa://22752 (13.33), **maa://26013 (42.86)</t>
         </is>
       </c>
       <c r="AC5" s="4" t="inlineStr">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="AE6" s="2" t="inlineStr">
         <is>
-          <t>*maa://33152 (56.67), ***maa://22770 (28.57)</t>
+          <t>*maa://33152 (58.06), ***maa://22770 (28.57)</t>
         </is>
       </c>
     </row>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="W7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (94.62), *maa://22758 (71.43)</t>
+          <t>maa://22399 (94.62), *maa://22758 (72.0)</t>
         </is>
       </c>
       <c r="Y7" s="4" t="inlineStr">
@@ -1344,7 +1344,7 @@
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>*maa://21476 (68.29), ***maa://39431 (25.0), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (69.05), ***maa://39431 (25.0), *maa://37551 (57.14)</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.41), **maa://32237 (38.89), ***maa://34206 (14.29), ***maa://39951 (19.05), ***maa://39243 (25.0)</t>
+          <t>***maa://25695 (19.3), **maa://32237 (38.89), ***maa://34206 (14.29), ***maa://39951 (18.18), **maa://39243 (40.0)</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="S10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (97.28), maa://22755 (87.5), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.62), maa://22755 (87.5), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="4" t="inlineStr">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="W10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.33), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.35), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="4" t="inlineStr">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="AE10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (55.71), *maa://22733 (58.62), maa://22761 (100.0)</t>
+          <t>*maa://25021 (56.34), *maa://22733 (58.62), maa://22761 (100.0)</t>
         </is>
       </c>
     </row>
@@ -1770,7 +1770,7 @@
       </c>
       <c r="S11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (95.0), maa://22501 (98.08)</t>
+          <t>maa://22747 (94.33), maa://22501 (98.11)</t>
         </is>
       </c>
       <c r="U11" s="4" t="inlineStr">
@@ -1785,7 +1785,7 @@
       </c>
       <c r="W11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.8)</t>
+          <t>maa://36713 (97.81)</t>
         </is>
       </c>
       <c r="Y11" s="4" t="inlineStr">
@@ -1922,7 +1922,7 @@
       </c>
       <c r="AA12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.83), maa://36677 (94.74), maa://39872 (83.33)</t>
+          <t>maa://23669 (95.83), maa://36677 (94.87), maa://39872 (83.33)</t>
         </is>
       </c>
       <c r="AC12" s="4" t="inlineStr">
@@ -1937,7 +1937,7 @@
       </c>
       <c r="AE12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.26), *maa://20106 (63.64), *maa://22769 (62.96)</t>
+          <t>*maa://28932 (78.45), *maa://20106 (63.64), *maa://22769 (62.96)</t>
         </is>
       </c>
     </row>
@@ -1954,7 +1954,7 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.36), maa://36673 (91.8), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.37), maa://36673 (91.8), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr">
@@ -1969,7 +1969,7 @@
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (75.74), **maa://22728 (47.62)</t>
+          <t>*maa://21248 (75.49), **maa://22728 (47.62)</t>
         </is>
       </c>
       <c r="I13" s="4" t="inlineStr">
@@ -2029,7 +2029,7 @@
       </c>
       <c r="W13" s="2" t="inlineStr">
         <is>
-          <t>*maa://34957 (78.05), *maa://22768 (53.33)</t>
+          <t>*maa://34957 (78.57), *maa://22768 (53.33)</t>
         </is>
       </c>
       <c r="Y13" s="4" t="inlineStr">
@@ -2121,7 +2121,7 @@
       </c>
       <c r="O14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.46), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.47), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="4" t="inlineStr">
@@ -2136,7 +2136,7 @@
       </c>
       <c r="S14" s="2" t="inlineStr">
         <is>
-          <t>*maa://22471 (59.7), maa://22521 (95.4)</t>
+          <t>*maa://22471 (59.42), maa://22521 (94.38)</t>
         </is>
       </c>
       <c r="U14" s="4" t="inlineStr">
@@ -2213,7 +2213,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.33), maa://21478 (91.18)</t>
+          <t>maa://24304 (88.4), maa://21478 (91.18)</t>
         </is>
       </c>
       <c r="I15" s="4" t="inlineStr">
@@ -2258,7 +2258,7 @@
       </c>
       <c r="S15" s="2" t="inlineStr">
         <is>
-          <t>maa://23892 (98.61)</t>
+          <t>maa://23892 (98.63)</t>
         </is>
       </c>
       <c r="U15" s="4" t="inlineStr">
@@ -2320,7 +2320,7 @@
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.15), maa://36679 (93.33), maa://37650 (95.24)</t>
+          <t>maa://21441 (96.15), maa://36679 (93.55), maa://37650 (95.45)</t>
         </is>
       </c>
       <c r="E16" s="4" t="inlineStr">
@@ -2365,7 +2365,7 @@
       </c>
       <c r="O16" s="2" t="inlineStr">
         <is>
-          <t>maa://28504 (91.3)</t>
+          <t>maa://28504 (91.49)</t>
         </is>
       </c>
       <c r="Q16" s="4" t="inlineStr">
@@ -2395,7 +2395,7 @@
       </c>
       <c r="W16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (97.37), maa://28051 (95.83)</t>
+          <t>maa://28501 (97.4), maa://28051 (95.83)</t>
         </is>
       </c>
       <c r="Y16" s="4" t="inlineStr">
@@ -2410,7 +2410,7 @@
       </c>
       <c r="AA16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (96.05)</t>
+          <t>maa://26228 (96.15)</t>
         </is>
       </c>
       <c r="AC16" s="4" t="inlineStr">
@@ -2425,7 +2425,7 @@
       </c>
       <c r="AE16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (61.54), maa://27755 (91.55)</t>
+          <t>*maa://23911 (61.54), maa://27755 (91.67)</t>
         </is>
       </c>
     </row>
@@ -2442,7 +2442,7 @@
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>maa://21624 (80.65)</t>
+          <t>maa://21624 (81.25)</t>
         </is>
       </c>
       <c r="E17" s="4" t="inlineStr">
@@ -2457,7 +2457,7 @@
       </c>
       <c r="G17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.57), maa://39599 (82.35)</t>
+          <t>maa://22430 (88.57), maa://39599 (83.33)</t>
         </is>
       </c>
       <c r="I17" s="4" t="inlineStr">
@@ -2564,7 +2564,7 @@
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.45)</t>
+          <t>maa://24570 (96.47)</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="G18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (90.43)</t>
+          <t>maa://24421 (90.48)</t>
         </is>
       </c>
       <c r="I18" s="4" t="inlineStr">
@@ -2639,7 +2639,7 @@
       </c>
       <c r="W18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (97.4), maa://22741 (83.33)</t>
+          <t>maa://21917 (97.47), maa://22741 (83.33)</t>
         </is>
       </c>
       <c r="Y18" s="4" t="inlineStr">
@@ -2746,7 +2746,7 @@
       </c>
       <c r="S19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (98.72)</t>
+          <t>maa://24386 (98.73)</t>
         </is>
       </c>
       <c r="U19" s="4" t="inlineStr">
@@ -2776,7 +2776,7 @@
       </c>
       <c r="AA19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (60.38), *maa://36668 (52.17)</t>
+          <t>*maa://30709 (60.48), *maa://36668 (52.17)</t>
         </is>
       </c>
       <c r="AC19" s="4" t="inlineStr">
@@ -2823,7 +2823,7 @@
       </c>
       <c r="G20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (88.28)</t>
+          <t>maa://22864 (88.37)</t>
         </is>
       </c>
       <c r="I20" s="4" t="inlineStr">
@@ -2838,7 +2838,7 @@
       </c>
       <c r="K20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (88.0)</t>
+          <t>maa://41331 (89.29)</t>
         </is>
       </c>
       <c r="M20" s="4" t="inlineStr">
@@ -3020,7 +3020,7 @@
       </c>
       <c r="AA21" s="2" t="inlineStr">
         <is>
-          <t>*maa://21443 (78.83), ***maa://23820 (29.63)</t>
+          <t>*maa://21443 (78.9), **maa://23820 (30.91)</t>
         </is>
       </c>
       <c r="AC21" s="4" t="inlineStr">
@@ -3127,7 +3127,7 @@
       </c>
       <c r="W22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.8), *maa://37649 (64.71)</t>
+          <t>maa://21282 (98.81), *maa://37649 (64.71)</t>
         </is>
       </c>
       <c r="Y22" s="4" t="inlineStr">
@@ -3157,7 +3157,7 @@
       </c>
       <c r="AE22" s="2" t="inlineStr">
         <is>
-          <t>maa://29658 (94.44)</t>
+          <t>maa://29658 (94.59)</t>
         </is>
       </c>
     </row>
@@ -3204,7 +3204,7 @@
       </c>
       <c r="K23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (91.67), maa://39875 (95.45)</t>
+          <t>maa://39756 (91.95), maa://39875 (95.56)</t>
         </is>
       </c>
       <c r="M23" s="4" t="inlineStr">
@@ -3249,7 +3249,7 @@
       </c>
       <c r="W23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (61.4)</t>
+          <t>*maa://28503 (62.07)</t>
         </is>
       </c>
       <c r="Y23" s="4" t="inlineStr">
@@ -3264,7 +3264,7 @@
       </c>
       <c r="AA23" s="2" t="inlineStr">
         <is>
-          <t>maa://29652 (97.22)</t>
+          <t>maa://29652 (97.3)</t>
         </is>
       </c>
       <c r="AC23" s="4" t="inlineStr">
@@ -3296,7 +3296,7 @@
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>maa://24368 (80.5)</t>
+          <t>maa://24368 (80.56)</t>
         </is>
       </c>
       <c r="E24" s="4" t="inlineStr">
@@ -3371,7 +3371,7 @@
       </c>
       <c r="W24" s="2" t="inlineStr">
         <is>
-          <t>maa://23504 (93.04), maa://29988 (85.86), **maa://22892 (40.43), *maa://25141 (76.86), *maa://36663 (79.63), ***maa://22815 (23.08)</t>
+          <t>maa://23504 (93.08), maa://29988 (85.93), **maa://22892 (40.43), *maa://25141 (76.86), *maa://36663 (79.63), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="4" t="inlineStr">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="AE24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (84.86), *maa://36672 (75.61), maa://29910 (93.88), **maa://21440 (34.55)</t>
+          <t>maa://22523 (84.86), *maa://36672 (76.19), maa://29910 (93.88), **maa://21440 (34.55)</t>
         </is>
       </c>
     </row>
@@ -3433,7 +3433,7 @@
       </c>
       <c r="G25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (76.74), *maa://25311 (74.73), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (76.15), *maa://25311 (73.91), ***maa://22725 (4.84)</t>
         </is>
       </c>
       <c r="I25" s="4" t="inlineStr">
@@ -3448,7 +3448,7 @@
       </c>
       <c r="K25" s="2" t="inlineStr">
         <is>
-          <t>maa://24378 (88.24)</t>
+          <t>maa://24378 (88.57)</t>
         </is>
       </c>
       <c r="M25" s="4" t="inlineStr">
@@ -3508,7 +3508,7 @@
       </c>
       <c r="AA25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (85.9), *maa://24516 (80.0), maa://26001 (88.89)</t>
+          <t>maa://31215 (83.75), *maa://24516 (79.07), maa://26001 (88.89)</t>
         </is>
       </c>
       <c r="AC25" s="4" t="inlineStr">
@@ -3615,7 +3615,7 @@
       </c>
       <c r="W26" s="2" t="inlineStr">
         <is>
-          <t>maa://24389 (95.83)</t>
+          <t>maa://24389 (96.0)</t>
         </is>
       </c>
       <c r="Y26" s="4" t="inlineStr">
@@ -3677,7 +3677,7 @@
       </c>
       <c r="G27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (48.65), maa://34494 (100.0), **maa://36665 (44.44), maa://39601 (85.71)</t>
+          <t>**maa://21283 (48.65), maa://34494 (100.0), **maa://36665 (44.44), maa://39601 (87.5)</t>
         </is>
       </c>
       <c r="I27" s="4" t="inlineStr">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="S27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (77.78)</t>
+          <t>*maa://30624 (75.68)</t>
         </is>
       </c>
       <c r="U27" s="4" t="inlineStr">
@@ -3814,7 +3814,7 @@
       </c>
       <c r="K28" s="2" t="inlineStr">
         <is>
-          <t>*maa://30770 (78.05)</t>
+          <t>*maa://30770 (78.57)</t>
         </is>
       </c>
       <c r="M28" s="4" t="inlineStr">
@@ -3859,7 +3859,7 @@
       </c>
       <c r="W28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (85.96), ***maa://39723 (15.15), *maa://41749 (66.67)</t>
+          <t>maa://39929 (85.56), ***maa://39723 (15.15), maa://41749 (81.82)</t>
         </is>
       </c>
       <c r="Y28" s="4" t="inlineStr">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="AE28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (94.07), *maa://36701 (64.0)</t>
+          <t>maa://36660 (94.09), *maa://36701 (64.0)</t>
         </is>
       </c>
     </row>
@@ -3936,7 +3936,7 @@
       </c>
       <c r="K29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.4), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (66.67)</t>
+          <t>maa://28432 (93.43), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (66.67)</t>
         </is>
       </c>
       <c r="M29" s="4" t="inlineStr">
@@ -4011,7 +4011,7 @@
       </c>
       <c r="AE29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.33), ***maa://34960 (9.09)</t>
+          <t>*maa://24080 (68.78), ***maa://34960 (9.09)</t>
         </is>
       </c>
     </row>
@@ -4088,7 +4088,7 @@
       </c>
       <c r="S30" s="2" t="inlineStr">
         <is>
-          <t>*maa://32940 (75.0), maa://24388 (93.75)</t>
+          <t>*maa://32940 (66.67), maa://24388 (93.75)</t>
         </is>
       </c>
       <c r="U30" s="4" t="inlineStr">
@@ -4103,7 +4103,7 @@
       </c>
       <c r="W30" s="2" t="inlineStr">
         <is>
-          <t>*maa://39477 (60.0)</t>
+          <t>*maa://39477 (71.43)</t>
         </is>
       </c>
       <c r="Y30" s="4" t="inlineStr">
@@ -4287,7 +4287,7 @@
       </c>
       <c r="G32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.01), maa://36667 (97.92), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.01), maa://36667 (98.0), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="4" t="inlineStr">
@@ -4302,7 +4302,7 @@
       </c>
       <c r="K32" s="2" t="inlineStr">
         <is>
-          <t>maa://28065 (97.22)</t>
+          <t>maa://28065 (94.59)</t>
         </is>
       </c>
       <c r="M32" s="4" t="inlineStr">
@@ -4332,7 +4332,7 @@
       </c>
       <c r="S32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (89.47), maa://41238 (94.12)</t>
+          <t>maa://41108 (87.5), maa://41238 (94.12)</t>
         </is>
       </c>
       <c r="U32" s="4" t="inlineStr">
@@ -4561,7 +4561,7 @@
       </c>
       <c r="S34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (93.04)</t>
+          <t>maa://24526 (93.07)</t>
         </is>
       </c>
       <c r="Y34" s="4" t="inlineStr">
@@ -4591,7 +4591,7 @@
       </c>
       <c r="AE34" s="2" t="inlineStr">
         <is>
-          <t>*maa://32650 (66.67)</t>
+          <t>*maa://32650 (69.23)</t>
         </is>
       </c>
     </row>
@@ -4623,7 +4623,7 @@
       </c>
       <c r="K35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.77)</t>
+          <t>maa://41296 (97.3)</t>
         </is>
       </c>
       <c r="M35" s="4" t="inlineStr">
@@ -4653,7 +4653,7 @@
       </c>
       <c r="S35" s="2" t="inlineStr">
         <is>
-          <t>maa://24842 (93.75)</t>
+          <t>maa://24842 (93.88)</t>
         </is>
       </c>
       <c r="Y35" s="4" t="inlineStr">
@@ -4683,7 +4683,7 @@
       </c>
       <c r="AE35" s="2" t="inlineStr">
         <is>
-          <t>maa://39479 (85.71)</t>
+          <t>maa://39479 (88.89)</t>
         </is>
       </c>
     </row>
@@ -4745,7 +4745,7 @@
       </c>
       <c r="S36" s="2" t="inlineStr">
         <is>
-          <t>maa://27613 (98.94)</t>
+          <t>maa://27613 (98.96)</t>
         </is>
       </c>
       <c r="AC36" s="4" t="inlineStr">
@@ -4807,7 +4807,7 @@
       </c>
       <c r="O37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.62), *maa://21239 (72.73)</t>
+          <t>maa://21280 (89.13), *maa://21239 (72.73)</t>
         </is>
       </c>
       <c r="Q37" s="4" t="inlineStr">
@@ -4822,7 +4822,7 @@
       </c>
       <c r="S37" s="2" t="inlineStr">
         <is>
-          <t>***maa://39354 (25.0)</t>
+          <t>**maa://39354 (40.0)</t>
         </is>
       </c>
       <c r="AC37" s="4" t="inlineStr">
@@ -4919,7 +4919,7 @@
       </c>
       <c r="AE38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.18)</t>
+          <t>maa://36697 (85.6)</t>
         </is>
       </c>
     </row>
@@ -4936,7 +4936,7 @@
       </c>
       <c r="G39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (86.11), maa://36670 (88.71), maa://30434 (88.89), ***maa://25036 (16.0)</t>
+          <t>maa://25199 (86.11), maa://36670 (89.23), maa://30434 (88.89), ***maa://25036 (16.0)</t>
         </is>
       </c>
       <c r="I39" s="4" t="inlineStr">
@@ -4966,7 +4966,7 @@
       </c>
       <c r="O39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.84)</t>
+          <t>maa://24709 (91.92)</t>
         </is>
       </c>
       <c r="Q39" s="4" t="inlineStr">
@@ -5095,7 +5095,7 @@
       </c>
       <c r="O41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (36.0)</t>
+          <t>**maa://35616 (34.62)</t>
         </is>
       </c>
       <c r="Q41" s="4" t="inlineStr">
@@ -5256,7 +5256,7 @@
       </c>
       <c r="S44" s="2" t="inlineStr">
         <is>
-          <t>maa://39366 (89.47)</t>
+          <t>maa://39366 (90.48)</t>
         </is>
       </c>
     </row>
@@ -5306,7 +5306,7 @@
       </c>
       <c r="S45" s="2" t="inlineStr">
         <is>
-          <t>*maa://39364 (66.67)</t>
+          <t>*maa://39364 (57.14)</t>
         </is>
       </c>
     </row>
@@ -5326,7 +5326,7 @@
       </c>
       <c r="G46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.41)</t>
+          <t>maa://35931 (92.44)</t>
         </is>
       </c>
       <c r="M46" s="4" t="inlineStr">
@@ -5491,7 +5491,7 @@
       </c>
       <c r="O49" s="2" t="inlineStr">
         <is>
-          <t>maa://39643 (83.33)</t>
+          <t>*maa://39643 (71.43)</t>
         </is>
       </c>
     </row>
@@ -5641,7 +5641,7 @@
       </c>
       <c r="G55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.24)</t>
+          <t>maa://32532 (92.27)</t>
         </is>
       </c>
     </row>
@@ -5675,7 +5675,7 @@
       </c>
       <c r="G57" s="2" t="inlineStr">
         <is>
-          <t>maa://25176 (97.78)</t>
+          <t>maa://25176 (97.83)</t>
         </is>
       </c>
     </row>
@@ -5709,7 +5709,7 @@
       </c>
       <c r="G59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (84.0), maa://31270 (96.91)</t>
+          <t>maa://27746 (84.0), maa://31270 (96.94)</t>
         </is>
       </c>
     </row>
@@ -5726,7 +5726,7 @@
       </c>
       <c r="G60" s="2" t="inlineStr">
         <is>
-          <t>**maa://40438 (45.45)</t>
+          <t>**maa://40438 (42.86)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: Auto Update Data (#75)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF72"/>
+  <dimension ref="A1:AF73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
@@ -717,7 +717,7 @@
       </c>
       <c r="AE2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.21), ***maa://21730 (17.19), ***maa://39501 (18.18), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.41), ***maa://21730 (17.19), ***maa://39501 (18.18), *maa://36675 (60.0)</t>
         </is>
       </c>
     </row>
@@ -764,7 +764,7 @@
       </c>
       <c r="K3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (70.2), maa://20276 (82.48), *maa://22749 (62.5)</t>
+          <t>*maa://22880 (70.2), maa://20276 (82.73), *maa://22749 (62.5)</t>
         </is>
       </c>
       <c r="M3" s="4" t="inlineStr">
@@ -779,7 +779,7 @@
       </c>
       <c r="O3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (95.1), maa://26254 (95.24)</t>
+          <t>maa://21249 (95.12), maa://26254 (95.24)</t>
         </is>
       </c>
       <c r="Q3" s="4" t="inlineStr">
@@ -794,7 +794,7 @@
       </c>
       <c r="S3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (88.24), **maa://20790 (43.94), ***maa://37170 (20.0)</t>
+          <t>maa://24617 (88.35), **maa://20790 (43.94), ***maa://37170 (20.0)</t>
         </is>
       </c>
       <c r="U3" s="4" t="inlineStr">
@@ -809,7 +809,7 @@
       </c>
       <c r="W3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.81), maa://27484 (95.65), maa://27480 (82.35)</t>
+          <t>maa://27396 (84.81), maa://27484 (95.74), maa://27480 (82.35)</t>
         </is>
       </c>
       <c r="Y3" s="4" t="inlineStr">
@@ -931,7 +931,7 @@
       </c>
       <c r="W4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.13), ***maa://31785 (16.51), ***maa://36683 (26.67)</t>
+          <t>**maa://32495 (47.93), ***maa://31785 (16.51), ***maa://36683 (26.67)</t>
         </is>
       </c>
       <c r="Y4" s="4" t="inlineStr">
@@ -961,7 +961,7 @@
       </c>
       <c r="AE4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (63.41), ***maa://26209 (13.04), *maa://39394 (76.92)</t>
+          <t>*maa://30062 (61.9), ***maa://26209 (13.04), *maa://39394 (78.57)</t>
         </is>
       </c>
     </row>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="AA5" s="2" t="inlineStr">
         <is>
-          <t>*maa://29863 (74.07), ***maa://22752 (13.33), **maa://26013 (42.86)</t>
+          <t>*maa://29863 (75.0), ***maa://22752 (13.33), **maa://26013 (42.86)</t>
         </is>
       </c>
       <c r="AC5" s="4" t="inlineStr">
@@ -1115,7 +1115,7 @@
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>maa://24370 (96.08)</t>
+          <t>maa://24370 (96.15)</t>
         </is>
       </c>
       <c r="I6" s="4" t="inlineStr">
@@ -1237,7 +1237,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>*maa://22763 (65.38)</t>
+          <t>*maa://22763 (66.67)</t>
         </is>
       </c>
       <c r="I7" s="4" t="inlineStr">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="W7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (94.62), *maa://22758 (72.0)</t>
+          <t>maa://22399 (94.62), *maa://22758 (70.59)</t>
         </is>
       </c>
       <c r="Y7" s="4" t="inlineStr">
@@ -1327,7 +1327,7 @@
       </c>
       <c r="AE7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (69.44), *maa://36671 (73.81)</t>
+          <t>*maa://26191 (68.49), *maa://36671 (72.09)</t>
         </is>
       </c>
     </row>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>*maa://21476 (69.05), ***maa://39431 (25.0), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (69.77), ***maa://39431 (25.0), *maa://37551 (57.14)</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
@@ -1419,7 +1419,7 @@
       </c>
       <c r="W8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (96.28)</t>
+          <t>maa://21411 (96.31)</t>
         </is>
       </c>
       <c r="Y8" s="4" t="inlineStr">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="AE9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (90.0), **maa://22865 (45.65)</t>
+          <t>maa://26206 (88.89), **maa://22865 (45.65)</t>
         </is>
       </c>
     </row>
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.3), **maa://32237 (38.89), ***maa://34206 (14.29), ***maa://39951 (18.18), **maa://39243 (40.0)</t>
+          <t>***maa://25695 (19.3), **maa://32237 (37.84), ***maa://34206 (14.29), ***maa://39951 (21.74), **maa://39243 (40.0)</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="S10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.62), maa://22755 (87.5), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.64), maa://22755 (87.62), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="4" t="inlineStr">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="W10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.35), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.38), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="4" t="inlineStr">
@@ -1740,7 +1740,7 @@
       </c>
       <c r="K11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (87.21)</t>
+          <t>maa://21287 (87.36)</t>
         </is>
       </c>
       <c r="M11" s="4" t="inlineStr">
@@ -1785,7 +1785,7 @@
       </c>
       <c r="W11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.81)</t>
+          <t>maa://36713 (97.83)</t>
         </is>
       </c>
       <c r="Y11" s="4" t="inlineStr">
@@ -1847,7 +1847,7 @@
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (89.86)</t>
+          <t>maa://21867 (89.93)</t>
         </is>
       </c>
       <c r="I12" s="4" t="inlineStr">
@@ -1907,7 +1907,7 @@
       </c>
       <c r="W12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.72), *maa://21485 (76.56), maa://37962 (81.25)</t>
+          <t>maa://22753 (91.84), *maa://21485 (76.56), maa://37962 (81.25)</t>
         </is>
       </c>
       <c r="Y12" s="4" t="inlineStr">
@@ -1922,7 +1922,7 @@
       </c>
       <c r="AA12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.83), maa://36677 (94.87), maa://39872 (83.33)</t>
+          <t>maa://23669 (95.86), maa://36677 (94.87), maa://39872 (83.33)</t>
         </is>
       </c>
       <c r="AC12" s="4" t="inlineStr">
@@ -1954,7 +1954,7 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.37), maa://36673 (91.8), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.41), maa://36673 (91.8), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr">
@@ -2029,7 +2029,7 @@
       </c>
       <c r="W13" s="2" t="inlineStr">
         <is>
-          <t>*maa://34957 (78.57), *maa://22768 (53.33)</t>
+          <t>*maa://34957 (75.0), *maa://22768 (53.33)</t>
         </is>
       </c>
       <c r="Y13" s="4" t="inlineStr">
@@ -2076,7 +2076,7 @@
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>maa://30764 (85.37)</t>
+          <t>maa://30764 (85.71)</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr">
@@ -2136,7 +2136,7 @@
       </c>
       <c r="S14" s="2" t="inlineStr">
         <is>
-          <t>*maa://22471 (59.42), maa://22521 (94.38)</t>
+          <t>*maa://22471 (59.42), maa://22521 (94.44)</t>
         </is>
       </c>
       <c r="U14" s="4" t="inlineStr">
@@ -2198,7 +2198,7 @@
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (76.05), maa://22734 (83.33), *maa://30808 (63.64), ***maa://36048 (13.33)</t>
+          <t>*maa://22743 (76.19), maa://22734 (83.33), *maa://30808 (63.64), ***maa://36048 (13.33)</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr">
@@ -2320,7 +2320,7 @@
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.15), maa://36679 (93.55), maa://37650 (95.45)</t>
+          <t>maa://21441 (96.17), maa://36679 (93.55), maa://37650 (95.45)</t>
         </is>
       </c>
       <c r="E16" s="4" t="inlineStr">
@@ -2380,7 +2380,7 @@
       </c>
       <c r="S16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (95.14), *maa://28648 (69.09), *maa://36674 (76.92)</t>
+          <t>maa://22729 (95.17), *maa://28648 (69.09), *maa://36674 (78.57)</t>
         </is>
       </c>
       <c r="U16" s="4" t="inlineStr">
@@ -2425,7 +2425,7 @@
       </c>
       <c r="AE16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (61.54), maa://27755 (91.67)</t>
+          <t>*maa://23911 (61.54), maa://27755 (91.78)</t>
         </is>
       </c>
     </row>
@@ -2497,12 +2497,12 @@
       </c>
       <c r="R17" s="4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0</t>
         </is>
       </c>
       <c r="S17" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>None</t>
         </is>
       </c>
       <c r="U17" s="4" t="inlineStr">
@@ -2564,7 +2564,7 @@
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.47)</t>
+          <t>maa://24570 (96.49)</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
@@ -2594,7 +2594,7 @@
       </c>
       <c r="K18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (88.28), *maa://22732 (52.5)</t>
+          <t>maa://22466 (88.37), *maa://22732 (52.5)</t>
         </is>
       </c>
       <c r="M18" s="4" t="inlineStr">
@@ -2746,7 +2746,7 @@
       </c>
       <c r="S19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (98.73)</t>
+          <t>maa://24386 (98.75)</t>
         </is>
       </c>
       <c r="U19" s="4" t="inlineStr">
@@ -2838,7 +2838,7 @@
       </c>
       <c r="K20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (89.29)</t>
+          <t>maa://41331 (90.32)</t>
         </is>
       </c>
       <c r="M20" s="4" t="inlineStr">
@@ -3035,7 +3035,7 @@
       </c>
       <c r="AE21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.25), *maa://22432 (74.07)</t>
+          <t>maa://22524 (94.29), *maa://22432 (74.07)</t>
         </is>
       </c>
     </row>
@@ -3127,7 +3127,7 @@
       </c>
       <c r="W22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.81), *maa://37649 (64.71)</t>
+          <t>maa://21282 (98.82), *maa://37649 (64.71)</t>
         </is>
       </c>
       <c r="Y22" s="4" t="inlineStr">
@@ -3204,7 +3204,7 @@
       </c>
       <c r="K23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (91.95), maa://39875 (95.56)</t>
+          <t>maa://39756 (92.11), maa://39875 (95.56)</t>
         </is>
       </c>
       <c r="M23" s="4" t="inlineStr">
@@ -3371,7 +3371,7 @@
       </c>
       <c r="W24" s="2" t="inlineStr">
         <is>
-          <t>maa://23504 (93.08), maa://29988 (85.93), **maa://22892 (40.43), *maa://25141 (76.86), *maa://36663 (79.63), ***maa://22815 (23.08)</t>
+          <t>maa://23504 (92.86), maa://29988 (86.0), **maa://22892 (40.14), *maa://25141 (76.86), *maa://36663 (80.0), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="4" t="inlineStr">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="AE24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (84.86), *maa://36672 (76.19), maa://29910 (93.88), **maa://21440 (34.55)</t>
+          <t>maa://22523 (84.86), *maa://36672 (76.74), maa://29910 (93.88), **maa://21440 (34.55)</t>
         </is>
       </c>
     </row>
@@ -3448,7 +3448,7 @@
       </c>
       <c r="K25" s="2" t="inlineStr">
         <is>
-          <t>maa://24378 (88.57)</t>
+          <t>maa://24378 (88.89)</t>
         </is>
       </c>
       <c r="M25" s="4" t="inlineStr">
@@ -3463,7 +3463,7 @@
       </c>
       <c r="O25" s="2" t="inlineStr">
         <is>
-          <t>maa://24382 (91.67)</t>
+          <t>maa://24382 (92.0)</t>
         </is>
       </c>
       <c r="Q25" s="4" t="inlineStr">
@@ -3555,7 +3555,7 @@
       </c>
       <c r="G26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (90.91)</t>
+          <t>maa://24913 (91.04)</t>
         </is>
       </c>
       <c r="I26" s="4" t="inlineStr">
@@ -3625,12 +3625,12 @@
       </c>
       <c r="Z26" s="4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AA26" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>None</t>
         </is>
       </c>
       <c r="AC26" s="4" t="inlineStr">
@@ -3784,7 +3784,7 @@
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.32), maa://25725 (82.05)</t>
+          <t>maa://24465 (90.32), maa://25725 (82.28)</t>
         </is>
       </c>
       <c r="E28" s="4" t="inlineStr">
@@ -3844,7 +3844,7 @@
       </c>
       <c r="S28" s="2" t="inlineStr">
         <is>
-          <t>maa://23263 (94.19), *maa://29765 (62.12)</t>
+          <t>maa://23263 (94.25), *maa://29765 (62.12)</t>
         </is>
       </c>
       <c r="U28" s="4" t="inlineStr">
@@ -3859,7 +3859,7 @@
       </c>
       <c r="W28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (85.56), ***maa://39723 (15.15), maa://41749 (81.82)</t>
+          <t>maa://39929 (86.02), ***maa://39723 (14.71), maa://41749 (85.71)</t>
         </is>
       </c>
       <c r="Y28" s="4" t="inlineStr">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="AE28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (94.09), *maa://36701 (64.0)</t>
+          <t>maa://36660 (93.75), *maa://36701 (64.0)</t>
         </is>
       </c>
     </row>
@@ -3936,7 +3936,7 @@
       </c>
       <c r="K29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.43), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (66.67)</t>
+          <t>maa://28432 (93.47), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (66.67)</t>
         </is>
       </c>
       <c r="M29" s="4" t="inlineStr">
@@ -3951,7 +3951,7 @@
       </c>
       <c r="O29" s="2" t="inlineStr">
         <is>
-          <t>*maa://23168 (55.77), **maa://30050 (42.11)</t>
+          <t>*maa://23168 (55.77), **maa://30050 (40.0)</t>
         </is>
       </c>
       <c r="Q29" s="4" t="inlineStr">
@@ -4180,7 +4180,7 @@
       </c>
       <c r="K31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.48), maa://36258 (80.26)</t>
+          <t>maa://35926 (93.53), maa://36258 (80.52)</t>
         </is>
       </c>
       <c r="M31" s="4" t="inlineStr">
@@ -4287,7 +4287,7 @@
       </c>
       <c r="G32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.01), maa://36667 (98.0), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.01), maa://36667 (98.04), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="4" t="inlineStr">
@@ -4332,7 +4332,7 @@
       </c>
       <c r="S32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (87.5), maa://41238 (94.12)</t>
+          <t>maa://41108 (88.89), maa://41238 (94.12)</t>
         </is>
       </c>
       <c r="U32" s="4" t="inlineStr">
@@ -4623,7 +4623,7 @@
       </c>
       <c r="K35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (97.3)</t>
+          <t>maa://41296 (97.5)</t>
         </is>
       </c>
       <c r="M35" s="4" t="inlineStr">
@@ -4683,7 +4683,7 @@
       </c>
       <c r="AE35" s="2" t="inlineStr">
         <is>
-          <t>maa://39479 (88.89)</t>
+          <t>maa://39479 (90.0)</t>
         </is>
       </c>
     </row>
@@ -4710,12 +4710,12 @@
       </c>
       <c r="J36" s="4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K36" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>None</t>
         </is>
       </c>
       <c r="M36" s="4" t="inlineStr">
@@ -4746,6 +4746,21 @@
       <c r="S36" s="2" t="inlineStr">
         <is>
           <t>maa://27613 (98.96)</t>
+        </is>
+      </c>
+      <c r="Y36" t="inlineStr">
+        <is>
+          <t>凯瑟琳</t>
+        </is>
+      </c>
+      <c r="Z36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA36" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="AC36" s="4" t="inlineStr">
@@ -4825,6 +4840,21 @@
           <t>**maa://39354 (40.0)</t>
         </is>
       </c>
+      <c r="Y37" t="inlineStr">
+        <is>
+          <t>波卜</t>
+        </is>
+      </c>
+      <c r="Z37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="AC37" s="4" t="inlineStr">
         <is>
           <t>艾拉</t>
@@ -4919,7 +4949,7 @@
       </c>
       <c r="AE38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (85.6)</t>
+          <t>maa://36697 (85.71)</t>
         </is>
       </c>
     </row>
@@ -5048,7 +5078,7 @@
       </c>
       <c r="O40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (96.19), maa://21386 (95.63), maa://36664 (92.31)</t>
+          <t>maa://23278 (96.21), maa://21386 (95.63), maa://36664 (92.31)</t>
         </is>
       </c>
       <c r="Q40" s="4" t="inlineStr">
@@ -5226,7 +5256,7 @@
       </c>
       <c r="G44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.49), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.51), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="M44" s="4" t="inlineStr">
@@ -5256,7 +5286,7 @@
       </c>
       <c r="S44" s="2" t="inlineStr">
         <is>
-          <t>maa://39366 (90.48)</t>
+          <t>maa://39366 (86.36)</t>
         </is>
       </c>
     </row>
@@ -5306,7 +5336,7 @@
       </c>
       <c r="S45" s="2" t="inlineStr">
         <is>
-          <t>*maa://39364 (57.14)</t>
+          <t>*maa://39364 (62.5)</t>
         </is>
       </c>
     </row>
@@ -5726,7 +5756,7 @@
       </c>
       <c r="G60" s="2" t="inlineStr">
         <is>
-          <t>**maa://40438 (42.86)</t>
+          <t>**maa://40438 (37.5)</t>
         </is>
       </c>
     </row>
@@ -5929,6 +5959,23 @@
         </is>
       </c>
       <c r="G72" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>维娜·维多利亚</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
CI: Auto Update Data (#77)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -705,7 +705,7 @@
       </c>
       <c r="AA2" s="5" t="inlineStr">
         <is>
-          <t>maa://21246 (91.2), maa://36684 (100.0), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.2), maa://36684 (98.57), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="4" t="inlineStr">
@@ -720,7 +720,7 @@
       </c>
       <c r="AE2" s="5" t="inlineStr">
         <is>
-          <t>maa://25251 (92.41), ***maa://21730 (17.19), ***maa://39501 (18.18), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.41), ***maa://21730 (17.19), ***maa://39501 (25.0), *maa://36675 (60.0)</t>
         </is>
       </c>
     </row>
@@ -767,7 +767,7 @@
       </c>
       <c r="K3" s="5" t="inlineStr">
         <is>
-          <t>*maa://22880 (70.2), maa://20276 (82.73), *maa://22749 (62.5)</t>
+          <t>*maa://22880 (69.74), maa://20276 (82.73), *maa://22749 (62.5)</t>
         </is>
       </c>
       <c r="M3" s="4" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="W4" s="5" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.93), ***maa://31785 (16.51), ***maa://36683 (26.67)</t>
+          <t>**maa://32495 (47.93), ***maa://31785 (18.02), ***maa://36683 (26.67)</t>
         </is>
       </c>
       <c r="Y4" s="4" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="AA4" s="5" t="inlineStr">
         <is>
-          <t>*maa://32658 (71.43)</t>
+          <t>*maa://32658 (73.33)</t>
         </is>
       </c>
       <c r="AC4" s="4" t="inlineStr">
@@ -1098,12 +1098,12 @@
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>**maa://42407 (50.0)</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -1193,7 +1193,7 @@
       </c>
       <c r="AA6" s="5" t="inlineStr">
         <is>
-          <t>maa://22739 (91.11)</t>
+          <t>maa://22739 (91.3)</t>
         </is>
       </c>
       <c r="AC6" s="4" t="inlineStr">
@@ -1208,7 +1208,7 @@
       </c>
       <c r="AE6" s="5" t="inlineStr">
         <is>
-          <t>*maa://33152 (58.06), ***maa://22770 (28.57)</t>
+          <t>*maa://33152 (59.38), ***maa://22770 (28.57)</t>
         </is>
       </c>
     </row>
@@ -1255,7 +1255,7 @@
       </c>
       <c r="K7" s="5" t="inlineStr">
         <is>
-          <t>maa://28624 (91.3), maa://24957 (97.3)</t>
+          <t>maa://28624 (91.3), maa://24957 (97.37)</t>
         </is>
       </c>
       <c r="M7" s="4" t="inlineStr">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="S7" s="5" t="inlineStr">
         <is>
-          <t>maa://21291 (88.89)</t>
+          <t>maa://21291 (89.19)</t>
         </is>
       </c>
       <c r="U7" s="4" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>*maa://21476 (69.77), ***maa://39431 (25.0), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (69.77), **maa://39431 (40.0), *maa://37551 (57.14)</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
@@ -1392,7 +1392,7 @@
       </c>
       <c r="O8" s="5" t="inlineStr">
         <is>
-          <t>maa://32931 (88.31), *maa://21916 (60.34), maa://23252 (92.31), **maa://22759 (45.45), maa://37496 (100.0)</t>
+          <t>maa://32931 (88.46), *maa://21916 (60.34), maa://23252 (92.31), **maa://22759 (45.45), maa://37496 (100.0)</t>
         </is>
       </c>
       <c r="Q8" s="4" t="inlineStr">
@@ -1422,7 +1422,7 @@
       </c>
       <c r="W8" s="5" t="inlineStr">
         <is>
-          <t>maa://21411 (95.99)</t>
+          <t>maa://21411 (96.0)</t>
         </is>
       </c>
       <c r="Y8" s="4" t="inlineStr">
@@ -1452,7 +1452,7 @@
       </c>
       <c r="AE8" s="5" t="inlineStr">
         <is>
-          <t>*maa://24479 (76.06), *maa://21990 (53.85)</t>
+          <t>*maa://24479 (76.39), *maa://21990 (53.85)</t>
         </is>
       </c>
     </row>
@@ -1499,7 +1499,7 @@
       </c>
       <c r="K9" s="5" t="inlineStr">
         <is>
-          <t>maa://22762 (91.57), **maa://39552 (50.0)</t>
+          <t>maa://22762 (91.57), *maa://39552 (66.67)</t>
         </is>
       </c>
       <c r="M9" s="4" t="inlineStr">
@@ -1544,7 +1544,7 @@
       </c>
       <c r="W9" s="5" t="inlineStr">
         <is>
-          <t>maa://26223 (96.88)</t>
+          <t>maa://26223 (96.91)</t>
         </is>
       </c>
       <c r="Y9" s="4" t="inlineStr">
@@ -1559,7 +1559,7 @@
       </c>
       <c r="AA9" s="5" t="inlineStr">
         <is>
-          <t>maa://28711 (87.8), ***maa://22740 (5.88), **maa://27377 (46.15), ***maa://25174 (20.0), **maa://39938 (50.0), maa://40166 (100.0)</t>
+          <t>maa://28711 (87.95), ***maa://22740 (5.88), **maa://27377 (46.15), ***maa://25174 (20.0), **maa://39938 (50.0), maa://40166 (100.0)</t>
         </is>
       </c>
       <c r="AC9" s="4" t="inlineStr">
@@ -1636,7 +1636,7 @@
       </c>
       <c r="O10" s="5" t="inlineStr">
         <is>
-          <t>maa://28977 (94.67), *maa://23264 (62.96), maa://36669 (90.91)</t>
+          <t>maa://28977 (94.67), *maa://23264 (62.96), maa://36669 (91.3)</t>
         </is>
       </c>
       <c r="Q10" s="4" t="inlineStr">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="S10" s="5" t="inlineStr">
         <is>
-          <t>maa://27395 (96.64), maa://22755 (87.62), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.67), maa://22755 (87.62), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="4" t="inlineStr">
@@ -1666,7 +1666,7 @@
       </c>
       <c r="W10" s="5" t="inlineStr">
         <is>
-          <t>maa://22301 (97.38), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.4), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="4" t="inlineStr">
@@ -1773,7 +1773,7 @@
       </c>
       <c r="S11" s="5" t="inlineStr">
         <is>
-          <t>maa://22747 (94.33), maa://22501 (98.11)</t>
+          <t>maa://22747 (94.33), maa://22501 (98.15)</t>
         </is>
       </c>
       <c r="U11" s="4" t="inlineStr">
@@ -1925,7 +1925,7 @@
       </c>
       <c r="AA12" s="5" t="inlineStr">
         <is>
-          <t>maa://23669 (95.86), maa://36677 (94.87), maa://39872 (83.33)</t>
+          <t>maa://23669 (95.86), maa://36677 (94.87), maa://39872 (84.62)</t>
         </is>
       </c>
       <c r="AC12" s="4" t="inlineStr">
@@ -1940,7 +1940,7 @@
       </c>
       <c r="AE12" s="5" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.45), *maa://20106 (63.64), *maa://22769 (62.96)</t>
+          <t>*maa://28932 (78.63), *maa://20106 (63.64), *maa://22769 (62.96)</t>
         </is>
       </c>
     </row>
@@ -1957,7 +1957,7 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>maa://24999 (91.41), maa://36673 (91.8), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.42), maa://36673 (91.8), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr">
@@ -1972,7 +1972,7 @@
       </c>
       <c r="G13" s="5" t="inlineStr">
         <is>
-          <t>*maa://21248 (75.49), **maa://22728 (47.62)</t>
+          <t>*maa://21248 (75.61), **maa://22728 (47.62)</t>
         </is>
       </c>
       <c r="I13" s="4" t="inlineStr">
@@ -2002,7 +2002,7 @@
       </c>
       <c r="O13" s="5" t="inlineStr">
         <is>
-          <t>maa://22676 (91.75), *maa://22583 (74.58), *maa://22500 (55.81)</t>
+          <t>maa://22676 (91.84), *maa://22583 (75.0), *maa://22500 (55.81)</t>
         </is>
       </c>
       <c r="Q13" s="4" t="inlineStr">
@@ -2079,7 +2079,7 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>maa://30764 (85.71)</t>
+          <t>maa://30764 (86.05)</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr">
@@ -2306,7 +2306,7 @@
       </c>
       <c r="AE15" s="5" t="inlineStr">
         <is>
-          <t>maa://21364 (80.61), *maa://22766 (73.0), *maa://36666 (77.05)</t>
+          <t>maa://21364 (80.61), *maa://22766 (73.0), *maa://36666 (77.42)</t>
         </is>
       </c>
     </row>
@@ -2323,7 +2323,7 @@
       </c>
       <c r="C16" s="5" t="inlineStr">
         <is>
-          <t>maa://21441 (96.17), maa://36679 (93.55), maa://37650 (95.45)</t>
+          <t>maa://21441 (96.17), maa://36679 (93.75), maa://37650 (95.45)</t>
         </is>
       </c>
       <c r="E16" s="4" t="inlineStr">
@@ -2383,7 +2383,7 @@
       </c>
       <c r="S16" s="5" t="inlineStr">
         <is>
-          <t>maa://22729 (95.17), *maa://28648 (69.09), *maa://36674 (78.57)</t>
+          <t>maa://22729 (95.17), *maa://28648 (69.09), *maa://36674 (79.31)</t>
         </is>
       </c>
       <c r="U16" s="4" t="inlineStr">
@@ -2460,7 +2460,7 @@
       </c>
       <c r="G17" s="5" t="inlineStr">
         <is>
-          <t>maa://22430 (88.57), maa://39599 (83.33)</t>
+          <t>maa://22430 (88.57), maa://39599 (84.21)</t>
         </is>
       </c>
       <c r="I17" s="4" t="inlineStr">
@@ -2563,7 +2563,7 @@
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
-          <t>maa://24570 (96.49)</t>
+          <t>maa://24570 (96.51)</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
@@ -2593,7 +2593,7 @@
       </c>
       <c r="K18" s="5" t="inlineStr">
         <is>
-          <t>maa://22466 (88.37), *maa://22732 (52.5)</t>
+          <t>maa://22466 (88.46), *maa://22732 (51.85)</t>
         </is>
       </c>
       <c r="M18" s="4" t="inlineStr">
@@ -2775,7 +2775,7 @@
       </c>
       <c r="AA19" s="5" t="inlineStr">
         <is>
-          <t>*maa://30709 (60.48), *maa://36668 (52.17)</t>
+          <t>*maa://30709 (60.59), *maa://36668 (52.17)</t>
         </is>
       </c>
       <c r="AC19" s="4" t="inlineStr">
@@ -2822,7 +2822,7 @@
       </c>
       <c r="G20" s="5" t="inlineStr">
         <is>
-          <t>maa://22864 (88.37)</t>
+          <t>maa://22864 (88.46)</t>
         </is>
       </c>
       <c r="I20" s="4" t="inlineStr">
@@ -2837,7 +2837,7 @@
       </c>
       <c r="K20" s="5" t="inlineStr">
         <is>
-          <t>maa://41331 (90.62)</t>
+          <t>maa://41331 (90.91)</t>
         </is>
       </c>
       <c r="M20" s="4" t="inlineStr">
@@ -3004,7 +3004,7 @@
       </c>
       <c r="W21" s="5" t="inlineStr">
         <is>
-          <t>maa://20110 (86.57), maa://34946 (90.32)</t>
+          <t>maa://20110 (86.57), maa://34946 (90.62)</t>
         </is>
       </c>
       <c r="Y21" s="4" t="inlineStr">
@@ -3019,7 +3019,7 @@
       </c>
       <c r="AA21" s="5" t="inlineStr">
         <is>
-          <t>*maa://21443 (78.9), **maa://23820 (30.91)</t>
+          <t>*maa://21443 (78.96), **maa://23820 (30.91)</t>
         </is>
       </c>
       <c r="AC21" s="4" t="inlineStr">
@@ -3034,7 +3034,7 @@
       </c>
       <c r="AE21" s="5" t="inlineStr">
         <is>
-          <t>maa://22524 (94.29), *maa://22432 (74.07)</t>
+          <t>maa://22524 (94.29), *maa://22432 (74.55)</t>
         </is>
       </c>
     </row>
@@ -3066,7 +3066,7 @@
       </c>
       <c r="G22" s="5" t="inlineStr">
         <is>
-          <t>maa://25236 (95.77), **maa://21678 (48.94), **maa://22735 (50.0)</t>
+          <t>maa://25236 (95.83), **maa://21678 (48.94), **maa://22735 (50.0)</t>
         </is>
       </c>
       <c r="I22" s="4" t="inlineStr">
@@ -3081,7 +3081,7 @@
       </c>
       <c r="K22" s="5" t="inlineStr">
         <is>
-          <t>maa://27127 (86.36), *maa://22751 (77.05)</t>
+          <t>maa://27127 (86.52), *maa://22751 (77.05)</t>
         </is>
       </c>
       <c r="M22" s="4" t="inlineStr">
@@ -3126,7 +3126,7 @@
       </c>
       <c r="W22" s="5" t="inlineStr">
         <is>
-          <t>maa://21282 (98.82), *maa://37649 (64.71)</t>
+          <t>maa://21282 (98.82), *maa://37649 (66.67)</t>
         </is>
       </c>
       <c r="Y22" s="4" t="inlineStr">
@@ -3203,7 +3203,7 @@
       </c>
       <c r="K23" s="5" t="inlineStr">
         <is>
-          <t>maa://39756 (92.11), maa://39875 (95.56)</t>
+          <t>maa://39756 (92.21), maa://39875 (95.65)</t>
         </is>
       </c>
       <c r="M23" s="4" t="inlineStr">
@@ -3218,7 +3218,7 @@
       </c>
       <c r="O23" s="5" t="inlineStr">
         <is>
-          <t>maa://30587 (91.62), *maa://29748 (75.2), ***maa://29785 (15.15), *maa://37566 (77.78)</t>
+          <t>maa://30587 (91.62), *maa://29748 (75.2), ***maa://29785 (15.15), *maa://37566 (78.95)</t>
         </is>
       </c>
       <c r="Q23" s="4" t="inlineStr">
@@ -3295,7 +3295,7 @@
       </c>
       <c r="C24" s="5" t="inlineStr">
         <is>
-          <t>maa://24368 (80.67)</t>
+          <t>maa://24368 (80.73)</t>
         </is>
       </c>
       <c r="E24" s="4" t="inlineStr">
@@ -3370,7 +3370,7 @@
       </c>
       <c r="W24" s="5" t="inlineStr">
         <is>
-          <t>maa://23504 (92.86), maa://29988 (86.07), **maa://22892 (40.14), *maa://25141 (76.86), *maa://36663 (80.0), ***maa://22815 (23.08)</t>
+          <t>maa://23504 (92.88), maa://29988 (86.07), **maa://22892 (40.14), *maa://25141 (76.86), maa://36663 (80.36), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="4" t="inlineStr">
@@ -3400,7 +3400,7 @@
       </c>
       <c r="AE24" s="5" t="inlineStr">
         <is>
-          <t>maa://22523 (84.86), *maa://36672 (76.74), maa://29910 (93.88), **maa://21440 (34.55)</t>
+          <t>maa://22523 (84.86), *maa://36672 (76.74), maa://29910 (94.0), **maa://21440 (34.55)</t>
         </is>
       </c>
     </row>
@@ -3432,7 +3432,7 @@
       </c>
       <c r="G25" s="5" t="inlineStr">
         <is>
-          <t>*maa://29063 (76.15), *maa://25311 (73.91), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (76.15), *maa://25311 (74.19), ***maa://22725 (4.84)</t>
         </is>
       </c>
       <c r="I25" s="4" t="inlineStr">
@@ -3629,7 +3629,7 @@
       </c>
       <c r="AA26" s="5" t="inlineStr">
         <is>
-          <t>***maa://42235 (25.0)</t>
+          <t>*maa://42235 (66.67)</t>
         </is>
       </c>
       <c r="AC26" s="4" t="inlineStr">
@@ -3644,7 +3644,7 @@
       </c>
       <c r="AE26" s="5" t="inlineStr">
         <is>
-          <t>maa://30511 (83.87), *maa://29760 (61.54)</t>
+          <t>maa://30511 (84.38), *maa://29760 (61.54)</t>
         </is>
       </c>
     </row>
@@ -3676,7 +3676,7 @@
       </c>
       <c r="G27" s="5" t="inlineStr">
         <is>
-          <t>**maa://21283 (48.65), maa://34494 (100.0), **maa://36665 (44.44), maa://39601 (87.5)</t>
+          <t>**maa://21283 (48.65), maa://34494 (100.0), **maa://36665 (44.44), maa://39601 (88.89)</t>
         </is>
       </c>
       <c r="I27" s="4" t="inlineStr">
@@ -3783,7 +3783,7 @@
       </c>
       <c r="C28" s="5" t="inlineStr">
         <is>
-          <t>maa://24465 (90.32), maa://25725 (82.28)</t>
+          <t>maa://24465 (90.33), maa://25725 (82.28)</t>
         </is>
       </c>
       <c r="E28" s="4" t="inlineStr">
@@ -3843,7 +3843,7 @@
       </c>
       <c r="S28" s="5" t="inlineStr">
         <is>
-          <t>maa://23263 (94.25), *maa://29765 (61.19)</t>
+          <t>maa://23263 (94.32), *maa://29765 (61.19)</t>
         </is>
       </c>
       <c r="U28" s="4" t="inlineStr">
@@ -3858,7 +3858,7 @@
       </c>
       <c r="W28" s="5" t="inlineStr">
         <is>
-          <t>maa://39929 (85.64), ***maa://39723 (14.71), maa://41749 (85.71)</t>
+          <t>maa://39929 (85.79), ***maa://39723 (14.71), maa://41749 (86.67)</t>
         </is>
       </c>
       <c r="Y28" s="4" t="inlineStr">
@@ -4010,7 +4010,7 @@
       </c>
       <c r="AE29" s="5" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.78), ***maa://34960 (9.09)</t>
+          <t>*maa://24080 (68.87), ***maa://34960 (9.09)</t>
         </is>
       </c>
     </row>
@@ -4057,7 +4057,7 @@
       </c>
       <c r="K30" s="5" t="inlineStr">
         <is>
-          <t>maa://30442 (94.23)</t>
+          <t>maa://30442 (94.34)</t>
         </is>
       </c>
       <c r="M30" s="4" t="inlineStr">
@@ -4072,7 +4072,7 @@
       </c>
       <c r="O30" s="5" t="inlineStr">
         <is>
-          <t>maa://21442 (99.48)</t>
+          <t>maa://21442 (99.49)</t>
         </is>
       </c>
       <c r="Q30" s="4" t="inlineStr">
@@ -4179,7 +4179,7 @@
       </c>
       <c r="K31" s="5" t="inlineStr">
         <is>
-          <t>maa://35926 (93.53), maa://36258 (80.52)</t>
+          <t>maa://35926 (93.56), maa://36258 (80.52)</t>
         </is>
       </c>
       <c r="M31" s="4" t="inlineStr">
@@ -4331,7 +4331,7 @@
       </c>
       <c r="S32" s="5" t="inlineStr">
         <is>
-          <t>maa://41108 (89.66), maa://41238 (94.44)</t>
+          <t>maa://41108 (90.32), maa://41238 (94.44)</t>
         </is>
       </c>
       <c r="U32" s="4" t="inlineStr">
@@ -4374,11 +4374,7 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AE32" s="5" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="AE32" s="5" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="4" t="inlineStr">
@@ -4438,7 +4434,7 @@
       </c>
       <c r="O33" s="5" t="inlineStr">
         <is>
-          <t>*maa://21956 (78.91), maa://22730 (82.14)</t>
+          <t>*maa://21956 (79.07), maa://22730 (82.14)</t>
         </is>
       </c>
       <c r="Q33" s="4" t="inlineStr">
@@ -4622,7 +4618,7 @@
       </c>
       <c r="K35" s="5" t="inlineStr">
         <is>
-          <t>maa://41296 (97.62)</t>
+          <t>maa://41296 (97.73)</t>
         </is>
       </c>
       <c r="M35" s="4" t="inlineStr">
@@ -4918,7 +4914,7 @@
       </c>
       <c r="O38" s="5" t="inlineStr">
         <is>
-          <t>*maa://24383 (66.29)</t>
+          <t>*maa://24383 (66.67)</t>
         </is>
       </c>
       <c r="Q38" s="4" t="inlineStr">
@@ -4965,7 +4961,7 @@
       </c>
       <c r="G39" s="5" t="inlineStr">
         <is>
-          <t>maa://25199 (86.11), maa://36670 (89.23), maa://30434 (88.89), ***maa://25036 (16.0)</t>
+          <t>maa://25199 (86.11), maa://36670 (89.39), maa://30434 (87.27), ***maa://25036 (16.0)</t>
         </is>
       </c>
       <c r="I39" s="4" t="inlineStr">
@@ -5077,7 +5073,7 @@
       </c>
       <c r="O40" s="5" t="inlineStr">
         <is>
-          <t>maa://23278 (96.21), maa://21386 (95.63), maa://36664 (92.31)</t>
+          <t>maa://23278 (95.88), maa://21386 (95.63), maa://36664 (90.24)</t>
         </is>
       </c>
       <c r="Q40" s="4" t="inlineStr">
@@ -5124,7 +5120,7 @@
       </c>
       <c r="O41" s="5" t="inlineStr">
         <is>
-          <t>**maa://35616 (34.62)</t>
+          <t>**maa://35616 (37.04)</t>
         </is>
       </c>
       <c r="Q41" s="4" t="inlineStr">
@@ -5255,7 +5251,7 @@
       </c>
       <c r="G44" s="5" t="inlineStr">
         <is>
-          <t>maa://29768 (97.51), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.52), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="M44" s="4" t="inlineStr">
@@ -5305,7 +5301,7 @@
       </c>
       <c r="G45" s="5" t="inlineStr">
         <is>
-          <t>maa://21229 (85.47), maa://30807 (94.92), *maa://22767 (52.94), ***maa://20796 (13.79)</t>
+          <t>maa://21229 (85.47), maa://30807 (95.08), *maa://22767 (52.94), ***maa://20796 (13.79)</t>
         </is>
       </c>
       <c r="M45" s="4" t="inlineStr">
@@ -5355,7 +5351,7 @@
       </c>
       <c r="G46" s="5" t="inlineStr">
         <is>
-          <t>maa://35931 (92.44)</t>
+          <t>maa://35931 (92.48)</t>
         </is>
       </c>
       <c r="M46" s="4" t="inlineStr">
@@ -5405,7 +5401,7 @@
       </c>
       <c r="G47" s="5" t="inlineStr">
         <is>
-          <t>maa://27410 (95.79), maa://29661 (97.64), maa://28038 (84.62)</t>
+          <t>maa://27410 (95.81), maa://29661 (97.64), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="M47" s="4" t="inlineStr">
@@ -5636,7 +5632,7 @@
       </c>
       <c r="G53" s="5" t="inlineStr">
         <is>
-          <t>maa://32534 (93.18), **maa://32434 (36.36)</t>
+          <t>maa://32534 (93.21), **maa://32434 (36.36)</t>
         </is>
       </c>
     </row>
@@ -5670,7 +5666,7 @@
       </c>
       <c r="G55" s="5" t="inlineStr">
         <is>
-          <t>maa://32532 (92.27)</t>
+          <t>maa://32532 (92.31)</t>
         </is>
       </c>
     </row>
@@ -5738,7 +5734,7 @@
       </c>
       <c r="G59" s="5" t="inlineStr">
         <is>
-          <t>maa://27746 (84.0), maa://31270 (96.94)</t>
+          <t>maa://27746 (84.0), maa://31270 (96.97)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: Auto Update Data (#78)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -705,7 +705,7 @@
       </c>
       <c r="AA2" s="5" t="inlineStr">
         <is>
-          <t>maa://21246 (91.2), maa://36684 (98.57), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.2), maa://36684 (98.59), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="4" t="inlineStr">
@@ -720,7 +720,7 @@
       </c>
       <c r="AE2" s="5" t="inlineStr">
         <is>
-          <t>maa://25251 (92.41), ***maa://21730 (17.19), ***maa://39501 (25.0), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.5), ***maa://21730 (17.19), ***maa://39501 (25.0), *maa://36675 (60.0)</t>
         </is>
       </c>
     </row>
@@ -752,7 +752,7 @@
       </c>
       <c r="G3" s="5" t="inlineStr">
         <is>
-          <t>maa://21247 (98.26), *maa://22748 (75.0)</t>
+          <t>maa://21247 (98.28), *maa://22748 (75.0)</t>
         </is>
       </c>
       <c r="I3" s="4" t="inlineStr">
@@ -767,7 +767,7 @@
       </c>
       <c r="K3" s="5" t="inlineStr">
         <is>
-          <t>*maa://22880 (69.74), maa://20276 (82.73), *maa://22749 (62.5)</t>
+          <t>*maa://22880 (69.93), maa://20276 (82.86), *maa://22749 (62.5)</t>
         </is>
       </c>
       <c r="M3" s="4" t="inlineStr">
@@ -812,7 +812,7 @@
       </c>
       <c r="W3" s="5" t="inlineStr">
         <is>
-          <t>maa://27396 (84.81), maa://27484 (95.74), maa://27480 (82.35)</t>
+          <t>maa://27396 (84.91), maa://27484 (95.74), maa://27480 (82.35)</t>
         </is>
       </c>
       <c r="Y3" s="4" t="inlineStr">
@@ -842,7 +842,7 @@
       </c>
       <c r="AE3" s="5" t="inlineStr">
         <is>
-          <t>*maa://21289 (68.42)</t>
+          <t>*maa://21289 (70.0)</t>
         </is>
       </c>
     </row>
@@ -859,7 +859,7 @@
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>maa://24632 (93.18), **maa://24303 (36.36), maa://22499 (85.71), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.23), **maa://24303 (36.36), maa://22499 (85.71), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="W4" s="5" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.93), ***maa://31785 (18.02), ***maa://36683 (26.67)</t>
+          <t>**maa://32495 (47.54), ***maa://31785 (18.02), ***maa://36683 (26.67)</t>
         </is>
       </c>
       <c r="Y4" s="4" t="inlineStr">
@@ -981,7 +981,7 @@
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>maa://21245 (82.63), maa://22744 (83.33)</t>
+          <t>maa://21245 (82.29), maa://22744 (83.33)</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -1103,7 +1103,7 @@
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>**maa://42407 (50.0)</t>
+          <t>*maa://42407 (75.0)</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -1255,7 +1255,7 @@
       </c>
       <c r="K7" s="5" t="inlineStr">
         <is>
-          <t>maa://28624 (91.3), maa://24957 (97.37)</t>
+          <t>maa://28624 (91.55), maa://24957 (97.44)</t>
         </is>
       </c>
       <c r="M7" s="4" t="inlineStr">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="O7" s="5" t="inlineStr">
         <is>
-          <t>maa://22750 (96.97)</t>
+          <t>maa://22750 (97.06)</t>
         </is>
       </c>
       <c r="Q7" s="4" t="inlineStr">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="S7" s="5" t="inlineStr">
         <is>
-          <t>maa://21291 (89.19)</t>
+          <t>maa://21291 (89.47)</t>
         </is>
       </c>
       <c r="U7" s="4" t="inlineStr">
@@ -1300,7 +1300,7 @@
       </c>
       <c r="W7" s="5" t="inlineStr">
         <is>
-          <t>maa://22399 (94.62), *maa://22758 (70.59)</t>
+          <t>maa://22399 (94.62), *maa://22758 (71.15)</t>
         </is>
       </c>
       <c r="Y7" s="4" t="inlineStr">
@@ -1392,7 +1392,7 @@
       </c>
       <c r="O8" s="5" t="inlineStr">
         <is>
-          <t>maa://32931 (88.46), *maa://21916 (60.34), maa://23252 (92.31), **maa://22759 (45.45), maa://37496 (100.0)</t>
+          <t>maa://32931 (88.61), *maa://21916 (60.34), maa://23252 (92.31), **maa://22759 (45.45), maa://37496 (100.0)</t>
         </is>
       </c>
       <c r="Q8" s="4" t="inlineStr">
@@ -1422,7 +1422,7 @@
       </c>
       <c r="W8" s="5" t="inlineStr">
         <is>
-          <t>maa://21411 (96.0)</t>
+          <t>maa://21411 (96.01)</t>
         </is>
       </c>
       <c r="Y8" s="4" t="inlineStr">
@@ -1452,7 +1452,7 @@
       </c>
       <c r="AE8" s="5" t="inlineStr">
         <is>
-          <t>*maa://24479 (76.39), *maa://21990 (53.85)</t>
+          <t>*maa://24479 (76.71), *maa://21990 (53.85)</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="O9" s="5" t="inlineStr">
         <is>
-          <t>maa://22736 (81.25)</t>
+          <t>maa://22736 (80.25)</t>
         </is>
       </c>
       <c r="Q9" s="4" t="inlineStr">
@@ -1544,7 +1544,7 @@
       </c>
       <c r="W9" s="5" t="inlineStr">
         <is>
-          <t>maa://26223 (96.91)</t>
+          <t>maa://26223 (96.94)</t>
         </is>
       </c>
       <c r="Y9" s="4" t="inlineStr">
@@ -1574,7 +1574,7 @@
       </c>
       <c r="AE9" s="5" t="inlineStr">
         <is>
-          <t>maa://26206 (89.02), **maa://22865 (45.65)</t>
+          <t>maa://26206 (89.16), **maa://22865 (45.65)</t>
         </is>
       </c>
     </row>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.3), **maa://32237 (37.84), ***maa://34206 (14.29), ***maa://39951 (20.83), **maa://39243 (33.33)</t>
+          <t>***maa://25695 (19.19), **maa://32237 (37.84), ***maa://34206 (18.18), ***maa://39951 (19.23), **maa://39243 (33.33)</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
@@ -1636,7 +1636,7 @@
       </c>
       <c r="O10" s="5" t="inlineStr">
         <is>
-          <t>maa://28977 (94.67), *maa://23264 (62.96), maa://36669 (91.3)</t>
+          <t>maa://28977 (94.74), *maa://23264 (62.96), maa://36669 (87.5)</t>
         </is>
       </c>
       <c r="Q10" s="4" t="inlineStr">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="S10" s="5" t="inlineStr">
         <is>
-          <t>maa://27395 (96.67), maa://22755 (87.62), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.03), maa://22755 (87.62), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="4" t="inlineStr">
@@ -1666,7 +1666,7 @@
       </c>
       <c r="W10" s="5" t="inlineStr">
         <is>
-          <t>maa://22301 (97.4), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.41), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="4" t="inlineStr">
@@ -1696,7 +1696,7 @@
       </c>
       <c r="AE10" s="5" t="inlineStr">
         <is>
-          <t>*maa://25021 (56.34), *maa://22733 (58.62), maa://22761 (100.0)</t>
+          <t>*maa://25021 (56.94), *maa://22733 (58.62), maa://22761 (100.0)</t>
         </is>
       </c>
     </row>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C11" s="5" t="inlineStr">
         <is>
-          <t>maa://36707 (99.63)</t>
+          <t>maa://36707 (99.64)</t>
         </is>
       </c>
       <c r="E11" s="4" t="inlineStr">
@@ -1818,7 +1818,7 @@
       </c>
       <c r="AE11" s="5" t="inlineStr">
         <is>
-          <t>maa://31203 (94.44), ***maa://24394 (16.0)</t>
+          <t>maa://31203 (94.44), ***maa://24394 (19.23)</t>
         </is>
       </c>
     </row>
@@ -1850,7 +1850,7 @@
       </c>
       <c r="G12" s="5" t="inlineStr">
         <is>
-          <t>maa://21867 (89.93)</t>
+          <t>maa://21867 (90.0)</t>
         </is>
       </c>
       <c r="I12" s="4" t="inlineStr">
@@ -1910,7 +1910,7 @@
       </c>
       <c r="W12" s="5" t="inlineStr">
         <is>
-          <t>maa://22753 (91.84), *maa://21485 (76.56), maa://37962 (81.25)</t>
+          <t>maa://22753 (91.84), *maa://21485 (76.74), maa://37962 (81.25)</t>
         </is>
       </c>
       <c r="Y12" s="4" t="inlineStr">
@@ -1925,7 +1925,7 @@
       </c>
       <c r="AA12" s="5" t="inlineStr">
         <is>
-          <t>maa://23669 (95.86), maa://36677 (94.87), maa://39872 (84.62)</t>
+          <t>maa://23669 (95.51), maa://36677 (92.5), maa://39872 (84.62)</t>
         </is>
       </c>
       <c r="AC12" s="4" t="inlineStr">
@@ -1957,7 +1957,7 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>maa://24999 (91.42), maa://36673 (91.8), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.45), maa://36673 (91.8), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr">
@@ -1972,7 +1972,7 @@
       </c>
       <c r="G13" s="5" t="inlineStr">
         <is>
-          <t>*maa://21248 (75.61), **maa://22728 (47.62)</t>
+          <t>*maa://21248 (75.73), **maa://22728 (47.62)</t>
         </is>
       </c>
       <c r="I13" s="4" t="inlineStr">
@@ -2032,7 +2032,7 @@
       </c>
       <c r="W13" s="5" t="inlineStr">
         <is>
-          <t>*maa://34957 (75.0), *maa://22768 (53.33)</t>
+          <t>*maa://34957 (75.56), *maa://22768 (53.33)</t>
         </is>
       </c>
       <c r="Y13" s="4" t="inlineStr">
@@ -2062,7 +2062,7 @@
       </c>
       <c r="AE13" s="5" t="inlineStr">
         <is>
-          <t>**maa://22737 (30.83), maa://39883 (90.91), *maa://39885 (73.68)</t>
+          <t>**maa://22737 (30.6), maa://39883 (87.5), *maa://39885 (73.68)</t>
         </is>
       </c>
     </row>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>maa://30764 (86.05)</t>
+          <t>maa://30764 (86.36)</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr">
@@ -2109,7 +2109,7 @@
       </c>
       <c r="K14" s="5" t="inlineStr">
         <is>
-          <t>maa://26245 (96.12), maa://21288 (96.21), maa://36682 (100.0), maa://39841 (92.5)</t>
+          <t>maa://26245 (96.12), maa://21288 (96.21), maa://36682 (100.0), maa://39841 (93.02)</t>
         </is>
       </c>
       <c r="M14" s="4" t="inlineStr">
@@ -2124,7 +2124,7 @@
       </c>
       <c r="O14" s="5" t="inlineStr">
         <is>
-          <t>maa://23250 (98.47), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.48), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="4" t="inlineStr">
@@ -2134,12 +2134,12 @@
       </c>
       <c r="R14" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="S14" s="5" t="inlineStr">
         <is>
-          <t>*maa://22471 (59.42), maa://22521 (94.44)</t>
+          <t>maa://22521 (94.44)</t>
         </is>
       </c>
       <c r="U14" s="4" t="inlineStr">
@@ -2154,7 +2154,7 @@
       </c>
       <c r="W14" s="5" t="inlineStr">
         <is>
-          <t>maa://37468 (92.31)</t>
+          <t>maa://37468 (92.86)</t>
         </is>
       </c>
       <c r="Y14" s="4" t="inlineStr">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>*maa://22743 (76.19), maa://22734 (83.33), *maa://30808 (63.64), ***maa://36048 (13.33)</t>
+          <t>*maa://22743 (76.19), maa://22734 (83.33), *maa://30808 (64.29), ***maa://36048 (13.33)</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr">
@@ -2216,7 +2216,7 @@
       </c>
       <c r="G15" s="5" t="inlineStr">
         <is>
-          <t>maa://24304 (88.4), maa://21478 (91.18)</t>
+          <t>maa://24304 (88.46), maa://21478 (91.18)</t>
         </is>
       </c>
       <c r="I15" s="4" t="inlineStr">
@@ -2246,7 +2246,7 @@
       </c>
       <c r="O15" s="5" t="inlineStr">
         <is>
-          <t>maa://24762 (89.51), *maa://22727 (70.0)</t>
+          <t>maa://24762 (89.58), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="4" t="inlineStr">
@@ -2306,7 +2306,7 @@
       </c>
       <c r="AE15" s="5" t="inlineStr">
         <is>
-          <t>maa://21364 (80.61), *maa://22766 (73.0), *maa://36666 (77.42)</t>
+          <t>maa://21364 (80.61), *maa://22766 (73.0), *maa://36666 (78.46)</t>
         </is>
       </c>
     </row>
@@ -2323,7 +2323,7 @@
       </c>
       <c r="C16" s="5" t="inlineStr">
         <is>
-          <t>maa://21441 (96.17), maa://36679 (93.75), maa://37650 (95.45)</t>
+          <t>maa://21441 (96.17), maa://36679 (93.94), maa://37650 (95.45)</t>
         </is>
       </c>
       <c r="E16" s="4" t="inlineStr">
@@ -2398,7 +2398,7 @@
       </c>
       <c r="W16" s="5" t="inlineStr">
         <is>
-          <t>maa://28501 (97.4), maa://28051 (95.83)</t>
+          <t>maa://28501 (97.44), maa://28051 (95.83)</t>
         </is>
       </c>
       <c r="Y16" s="4" t="inlineStr">
@@ -2428,7 +2428,7 @@
       </c>
       <c r="AE16" s="5" t="inlineStr">
         <is>
-          <t>*maa://23911 (61.54), maa://27755 (91.78)</t>
+          <t>*maa://23911 (61.96), maa://27755 (91.78)</t>
         </is>
       </c>
     </row>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
-          <t>maa://24570 (96.51)</t>
+          <t>maa://24570 (96.55)</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
@@ -2578,7 +2578,7 @@
       </c>
       <c r="G18" s="5" t="inlineStr">
         <is>
-          <t>maa://24421 (90.48)</t>
+          <t>maa://24421 (90.57)</t>
         </is>
       </c>
       <c r="I18" s="4" t="inlineStr">
@@ -2593,7 +2593,7 @@
       </c>
       <c r="K18" s="5" t="inlineStr">
         <is>
-          <t>maa://22466 (88.46), *maa://22732 (51.85)</t>
+          <t>maa://22466 (88.55), *maa://22732 (51.85)</t>
         </is>
       </c>
       <c r="M18" s="4" t="inlineStr">
@@ -2638,7 +2638,7 @@
       </c>
       <c r="W18" s="5" t="inlineStr">
         <is>
-          <t>maa://21917 (97.47), maa://22741 (83.33)</t>
+          <t>maa://21917 (97.5), maa://22741 (83.33)</t>
         </is>
       </c>
       <c r="Y18" s="4" t="inlineStr">
@@ -2668,7 +2668,7 @@
       </c>
       <c r="AE18" s="5" t="inlineStr">
         <is>
-          <t>*maa://24313 (57.33), **maa://29784 (46.15)</t>
+          <t>*maa://24313 (57.62), **maa://29784 (46.15)</t>
         </is>
       </c>
     </row>
@@ -2745,7 +2745,7 @@
       </c>
       <c r="S19" s="5" t="inlineStr">
         <is>
-          <t>maa://24386 (98.77)</t>
+          <t>maa://24386 (98.8)</t>
         </is>
       </c>
       <c r="U19" s="4" t="inlineStr">
@@ -2775,7 +2775,7 @@
       </c>
       <c r="AA19" s="5" t="inlineStr">
         <is>
-          <t>*maa://30709 (60.59), *maa://36668 (52.17)</t>
+          <t>*maa://30709 (60.8), *maa://36668 (52.17)</t>
         </is>
       </c>
       <c r="AC19" s="4" t="inlineStr">
@@ -2837,7 +2837,7 @@
       </c>
       <c r="K20" s="5" t="inlineStr">
         <is>
-          <t>maa://41331 (90.91)</t>
+          <t>maa://41331 (88.89)</t>
         </is>
       </c>
       <c r="M20" s="4" t="inlineStr">
@@ -2867,7 +2867,7 @@
       </c>
       <c r="S20" s="5" t="inlineStr">
         <is>
-          <t>maa://29113 (95.24)</t>
+          <t>maa://29113 (95.45)</t>
         </is>
       </c>
       <c r="U20" s="4" t="inlineStr">
@@ -3019,7 +3019,7 @@
       </c>
       <c r="AA21" s="5" t="inlineStr">
         <is>
-          <t>*maa://21443 (78.96), **maa://23820 (30.91)</t>
+          <t>*maa://21443 (78.72), **maa://23820 (30.91)</t>
         </is>
       </c>
       <c r="AC21" s="4" t="inlineStr">
@@ -3126,7 +3126,7 @@
       </c>
       <c r="W22" s="5" t="inlineStr">
         <is>
-          <t>maa://21282 (98.82), *maa://37649 (66.67)</t>
+          <t>maa://21282 (98.83), *maa://37649 (66.67)</t>
         </is>
       </c>
       <c r="Y22" s="4" t="inlineStr">
@@ -3173,7 +3173,7 @@
       </c>
       <c r="C23" s="5" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.36), maa://41753 (100.0)</t>
+          <t>***maa://28036 (28.36), *maa://41753 (75.0)</t>
         </is>
       </c>
       <c r="E23" s="4" t="inlineStr">
@@ -3203,7 +3203,7 @@
       </c>
       <c r="K23" s="5" t="inlineStr">
         <is>
-          <t>maa://39756 (92.21), maa://39875 (95.65)</t>
+          <t>maa://39756 (92.36), maa://39875 (95.65)</t>
         </is>
       </c>
       <c r="M23" s="4" t="inlineStr">
@@ -3233,7 +3233,7 @@
       </c>
       <c r="S23" s="5" t="inlineStr">
         <is>
-          <t>maa://24387 (82.86), maa://31212 (95.65)</t>
+          <t>maa://24387 (82.86), maa://31212 (95.83)</t>
         </is>
       </c>
       <c r="U23" s="4" t="inlineStr">
@@ -3295,7 +3295,7 @@
       </c>
       <c r="C24" s="5" t="inlineStr">
         <is>
-          <t>maa://24368 (80.73)</t>
+          <t>maa://24368 (80.36)</t>
         </is>
       </c>
       <c r="E24" s="4" t="inlineStr">
@@ -3370,7 +3370,7 @@
       </c>
       <c r="W24" s="5" t="inlineStr">
         <is>
-          <t>maa://23504 (92.88), maa://29988 (86.07), **maa://22892 (40.14), *maa://25141 (76.86), maa://36663 (80.36), ***maa://22815 (23.08)</t>
+          <t>maa://23504 (92.9), maa://29988 (86.21), **maa://22892 (40.14), *maa://25141 (76.86), maa://36663 (80.36), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="4" t="inlineStr">
@@ -3400,7 +3400,7 @@
       </c>
       <c r="AE24" s="5" t="inlineStr">
         <is>
-          <t>maa://22523 (84.86), *maa://36672 (76.74), maa://29910 (94.0), **maa://21440 (34.55)</t>
+          <t>maa://22523 (85.03), *maa://36672 (76.74), maa://29910 (94.0), **maa://21440 (34.55)</t>
         </is>
       </c>
     </row>
@@ -3417,7 +3417,7 @@
       </c>
       <c r="C25" s="5" t="inlineStr">
         <is>
-          <t>maa://29753 (95.11)</t>
+          <t>maa://29753 (95.13)</t>
         </is>
       </c>
       <c r="E25" s="4" t="inlineStr">
@@ -3629,7 +3629,7 @@
       </c>
       <c r="AA26" s="5" t="inlineStr">
         <is>
-          <t>*maa://42235 (66.67)</t>
+          <t>*maa://42235 (64.29)</t>
         </is>
       </c>
       <c r="AC26" s="4" t="inlineStr">
@@ -3676,7 +3676,7 @@
       </c>
       <c r="G27" s="5" t="inlineStr">
         <is>
-          <t>**maa://21283 (48.65), maa://34494 (100.0), **maa://36665 (44.44), maa://39601 (88.89)</t>
+          <t>**maa://21283 (48.65), maa://34494 (100.0), **maa://36665 (44.44), *maa://39601 (80.0)</t>
         </is>
       </c>
       <c r="I27" s="4" t="inlineStr">
@@ -3783,7 +3783,7 @@
       </c>
       <c r="C28" s="5" t="inlineStr">
         <is>
-          <t>maa://24465 (90.33), maa://25725 (82.28)</t>
+          <t>maa://24465 (90.35), maa://25725 (82.28)</t>
         </is>
       </c>
       <c r="E28" s="4" t="inlineStr">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="K28" s="5" t="inlineStr">
         <is>
-          <t>*maa://30770 (78.57)</t>
+          <t>*maa://30770 (79.07)</t>
         </is>
       </c>
       <c r="M28" s="4" t="inlineStr">
@@ -3858,7 +3858,7 @@
       </c>
       <c r="W28" s="5" t="inlineStr">
         <is>
-          <t>maa://39929 (85.79), ***maa://39723 (14.71), maa://41749 (86.67)</t>
+          <t>maa://39929 (86.15), ***maa://39723 (14.71), maa://41749 (81.25)</t>
         </is>
       </c>
       <c r="Y28" s="4" t="inlineStr">
@@ -3888,7 +3888,7 @@
       </c>
       <c r="AE28" s="5" t="inlineStr">
         <is>
-          <t>maa://36660 (93.75), *maa://36701 (64.0)</t>
+          <t>maa://36660 (93.77), *maa://36701 (64.0)</t>
         </is>
       </c>
     </row>
@@ -4010,7 +4010,7 @@
       </c>
       <c r="AE29" s="5" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.87), ***maa://34960 (9.09)</t>
+          <t>*maa://24080 (68.96), ***maa://34960 (9.09)</t>
         </is>
       </c>
     </row>
@@ -4057,7 +4057,7 @@
       </c>
       <c r="K30" s="5" t="inlineStr">
         <is>
-          <t>maa://30442 (94.34)</t>
+          <t>maa://30442 (94.44)</t>
         </is>
       </c>
       <c r="M30" s="4" t="inlineStr">
@@ -4286,7 +4286,7 @@
       </c>
       <c r="G32" s="5" t="inlineStr">
         <is>
-          <t>maa://21895 (97.01), maa://36667 (98.04), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.01), maa://36667 (98.08), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="4" t="inlineStr">
@@ -4331,7 +4331,7 @@
       </c>
       <c r="S32" s="5" t="inlineStr">
         <is>
-          <t>maa://41108 (90.32), maa://41238 (94.44)</t>
+          <t>maa://41108 (90.91), maa://41238 (94.44)</t>
         </is>
       </c>
       <c r="U32" s="4" t="inlineStr">
@@ -4371,10 +4371,14 @@
       </c>
       <c r="AD32" s="4" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AE32" s="5" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE32" s="5" t="inlineStr">
+        <is>
+          <t>maa://42408 (100.0)</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="4" t="inlineStr">
@@ -4618,7 +4622,7 @@
       </c>
       <c r="K35" s="5" t="inlineStr">
         <is>
-          <t>maa://41296 (97.73)</t>
+          <t>maa://41296 (97.96)</t>
         </is>
       </c>
       <c r="M35" s="4" t="inlineStr">
@@ -4961,7 +4965,7 @@
       </c>
       <c r="G39" s="5" t="inlineStr">
         <is>
-          <t>maa://25199 (86.11), maa://36670 (89.39), maa://30434 (87.27), ***maa://25036 (16.0)</t>
+          <t>maa://25199 (86.11), maa://36670 (88.06), maa://30434 (87.27), ***maa://25036 (16.0)</t>
         </is>
       </c>
       <c r="I39" s="4" t="inlineStr">
@@ -4991,7 +4995,7 @@
       </c>
       <c r="O39" s="5" t="inlineStr">
         <is>
-          <t>maa://24709 (91.92)</t>
+          <t>maa://24709 (92.0)</t>
         </is>
       </c>
       <c r="Q39" s="4" t="inlineStr">
@@ -5105,7 +5109,7 @@
       </c>
       <c r="G41" s="5" t="inlineStr">
         <is>
-          <t>maa://24466 (94.87)</t>
+          <t>maa://24466 (95.0)</t>
         </is>
       </c>
       <c r="M41" s="4" t="inlineStr">
@@ -5120,7 +5124,7 @@
       </c>
       <c r="O41" s="5" t="inlineStr">
         <is>
-          <t>**maa://35616 (37.04)</t>
+          <t>**maa://35616 (37.93)</t>
         </is>
       </c>
       <c r="Q41" s="4" t="inlineStr">
@@ -5204,7 +5208,7 @@
       </c>
       <c r="G43" s="5" t="inlineStr">
         <is>
-          <t>maa://22525 (92.56), maa://21284 (82.93)</t>
+          <t>maa://22525 (92.62), maa://21284 (82.93)</t>
         </is>
       </c>
       <c r="M43" s="4" t="inlineStr">
@@ -5281,7 +5285,7 @@
       </c>
       <c r="S44" s="5" t="inlineStr">
         <is>
-          <t>maa://39366 (86.36)</t>
+          <t>maa://39366 (86.96)</t>
         </is>
       </c>
     </row>
@@ -5351,7 +5355,7 @@
       </c>
       <c r="G46" s="5" t="inlineStr">
         <is>
-          <t>maa://35931 (92.48)</t>
+          <t>maa://35931 (92.51)</t>
         </is>
       </c>
       <c r="M46" s="4" t="inlineStr">
@@ -5568,7 +5572,7 @@
       </c>
       <c r="G51" s="5" t="inlineStr">
         <is>
-          <t>*maa://30769 (78.57)</t>
+          <t>*maa://30769 (80.0)</t>
         </is>
       </c>
       <c r="M51" s="4" t="inlineStr">
@@ -5717,7 +5721,7 @@
       </c>
       <c r="G58" s="5" t="inlineStr">
         <is>
-          <t>*maa://37964 (61.11)</t>
+          <t>*maa://37964 (63.16)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: Auto Update Data (#79)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -615,7 +615,7 @@
       </c>
       <c r="C2" s="5" t="inlineStr">
         <is>
-          <t>maa://24702 (94.1), maa://25390 (97.42), maa://36681 (92.19)</t>
+          <t>maa://24702 (94.1), maa://25390 (97.42), maa://36681 (90.77)</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
@@ -705,7 +705,7 @@
       </c>
       <c r="AA2" s="5" t="inlineStr">
         <is>
-          <t>maa://21246 (91.2), maa://36684 (98.59), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.2), maa://36684 (98.61), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="4" t="inlineStr">
@@ -720,7 +720,7 @@
       </c>
       <c r="AE2" s="5" t="inlineStr">
         <is>
-          <t>maa://25251 (92.5), ***maa://21730 (17.19), ***maa://39501 (25.0), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.5), ***maa://21730 (17.19), ***maa://39501 (23.08), *maa://36675 (60.0)</t>
         </is>
       </c>
     </row>
@@ -812,7 +812,7 @@
       </c>
       <c r="W3" s="5" t="inlineStr">
         <is>
-          <t>maa://27396 (84.91), maa://27484 (95.74), maa://27480 (82.35)</t>
+          <t>maa://27396 (84.97), maa://27484 (95.74), maa://27480 (82.35)</t>
         </is>
       </c>
       <c r="Y3" s="4" t="inlineStr">
@@ -859,7 +859,7 @@
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>maa://24632 (93.23), **maa://24303 (36.36), maa://22499 (85.71), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.28), **maa://24303 (36.36), maa://22499 (85.71), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="S6" s="5" t="inlineStr">
         <is>
-          <t>*maa://37411 (71.43)</t>
+          <t>*maa://37411 (75.0)</t>
         </is>
       </c>
       <c r="U6" s="4" t="inlineStr">
@@ -1208,7 +1208,7 @@
       </c>
       <c r="AE6" s="5" t="inlineStr">
         <is>
-          <t>*maa://33152 (59.38), ***maa://22770 (28.57)</t>
+          <t>*maa://33152 (60.61), ***maa://22770 (28.57)</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="AA8" s="5" t="inlineStr">
         <is>
-          <t>maa://25389 (88.46)</t>
+          <t>maa://25389 (88.89)</t>
         </is>
       </c>
       <c r="AC8" s="4" t="inlineStr">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.19), **maa://32237 (37.84), ***maa://34206 (18.18), ***maa://39951 (19.23), **maa://39243 (33.33)</t>
+          <t>***maa://25695 (19.19), **maa://32237 (37.84), ***maa://34206 (18.18), ***maa://39951 (18.52), **maa://39243 (33.33)</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
@@ -1773,7 +1773,7 @@
       </c>
       <c r="S11" s="5" t="inlineStr">
         <is>
-          <t>maa://22747 (94.33), maa://22501 (98.15)</t>
+          <t>maa://22747 (94.37), maa://22501 (98.15)</t>
         </is>
       </c>
       <c r="U11" s="4" t="inlineStr">
@@ -1788,7 +1788,7 @@
       </c>
       <c r="W11" s="5" t="inlineStr">
         <is>
-          <t>maa://36713 (97.83)</t>
+          <t>maa://36713 (97.84)</t>
         </is>
       </c>
       <c r="Y11" s="4" t="inlineStr">
@@ -1957,7 +1957,7 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>maa://24999 (91.45), maa://36673 (91.8), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.46), maa://36673 (91.8), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr">
@@ -1972,7 +1972,7 @@
       </c>
       <c r="G13" s="5" t="inlineStr">
         <is>
-          <t>*maa://21248 (75.73), **maa://22728 (47.62)</t>
+          <t>*maa://21248 (75.36), **maa://22728 (47.62)</t>
         </is>
       </c>
       <c r="I13" s="4" t="inlineStr">
@@ -2231,7 +2231,7 @@
       </c>
       <c r="K15" s="5" t="inlineStr">
         <is>
-          <t>*maa://21334 (54.17)</t>
+          <t>*maa://21334 (52.0)</t>
         </is>
       </c>
       <c r="M15" s="4" t="inlineStr">
@@ -2578,7 +2578,7 @@
       </c>
       <c r="G18" s="5" t="inlineStr">
         <is>
-          <t>maa://24421 (90.57)</t>
+          <t>maa://24421 (90.14)</t>
         </is>
       </c>
       <c r="I18" s="4" t="inlineStr">
@@ -2837,7 +2837,7 @@
       </c>
       <c r="K20" s="5" t="inlineStr">
         <is>
-          <t>maa://41331 (88.89)</t>
+          <t>maa://41331 (89.19)</t>
         </is>
       </c>
       <c r="M20" s="4" t="inlineStr">
@@ -3203,7 +3203,7 @@
       </c>
       <c r="K23" s="5" t="inlineStr">
         <is>
-          <t>maa://39756 (92.36), maa://39875 (95.65)</t>
+          <t>maa://39756 (92.41), maa://39875 (95.74)</t>
         </is>
       </c>
       <c r="M23" s="4" t="inlineStr">
@@ -3218,7 +3218,7 @@
       </c>
       <c r="O23" s="5" t="inlineStr">
         <is>
-          <t>maa://30587 (91.62), *maa://29748 (75.2), ***maa://29785 (15.15), *maa://37566 (78.95)</t>
+          <t>maa://30587 (91.67), *maa://29748 (75.2), ***maa://29785 (15.15), *maa://37566 (78.95)</t>
         </is>
       </c>
       <c r="Q23" s="4" t="inlineStr">
@@ -3400,7 +3400,7 @@
       </c>
       <c r="AE24" s="5" t="inlineStr">
         <is>
-          <t>maa://22523 (85.03), *maa://36672 (76.74), maa://29910 (94.0), **maa://21440 (34.55)</t>
+          <t>maa://22523 (85.03), *maa://36672 (76.74), maa://29910 (94.12), **maa://21440 (34.55)</t>
         </is>
       </c>
     </row>
@@ -3522,7 +3522,7 @@
       </c>
       <c r="AE25" s="5" t="inlineStr">
         <is>
-          <t>maa://20108 (96.09), maa://24621 (96.4), maa://36676 (100.0), maa://22771 (84.62), maa://37772 (100.0)</t>
+          <t>maa://20108 (96.12), maa://24621 (96.4), maa://36676 (100.0), maa://22771 (84.62), maa://37772 (100.0)</t>
         </is>
       </c>
     </row>
@@ -3858,7 +3858,7 @@
       </c>
       <c r="W28" s="5" t="inlineStr">
         <is>
-          <t>maa://39929 (86.15), ***maa://39723 (14.71), maa://41749 (81.25)</t>
+          <t>maa://39929 (86.29), ***maa://39723 (14.71), maa://41749 (81.25)</t>
         </is>
       </c>
       <c r="Y28" s="4" t="inlineStr">
@@ -3888,7 +3888,7 @@
       </c>
       <c r="AE28" s="5" t="inlineStr">
         <is>
-          <t>maa://36660 (93.77), *maa://36701 (64.0)</t>
+          <t>maa://36660 (93.8), *maa://36701 (64.0)</t>
         </is>
       </c>
     </row>
@@ -4010,7 +4010,7 @@
       </c>
       <c r="AE29" s="5" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.96), ***maa://34960 (9.09)</t>
+          <t>*maa://24080 (69.04), ***maa://34960 (9.09)</t>
         </is>
       </c>
     </row>
@@ -4286,7 +4286,7 @@
       </c>
       <c r="G32" s="5" t="inlineStr">
         <is>
-          <t>maa://21895 (97.01), maa://36667 (98.08), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.01), maa://36667 (98.11), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="4" t="inlineStr">
@@ -4331,7 +4331,7 @@
       </c>
       <c r="S32" s="5" t="inlineStr">
         <is>
-          <t>maa://41108 (90.91), maa://41238 (94.44)</t>
+          <t>maa://41108 (91.18), maa://41238 (94.44)</t>
         </is>
       </c>
       <c r="U32" s="4" t="inlineStr">
@@ -4590,7 +4590,7 @@
       </c>
       <c r="AE34" s="5" t="inlineStr">
         <is>
-          <t>*maa://32650 (69.23)</t>
+          <t>*maa://32650 (64.29)</t>
         </is>
       </c>
     </row>
@@ -4622,7 +4622,7 @@
       </c>
       <c r="K35" s="5" t="inlineStr">
         <is>
-          <t>maa://41296 (97.96)</t>
+          <t>maa://41296 (98.0)</t>
         </is>
       </c>
       <c r="M35" s="4" t="inlineStr">
@@ -4948,7 +4948,7 @@
       </c>
       <c r="AE38" s="5" t="inlineStr">
         <is>
-          <t>maa://36697 (85.83)</t>
+          <t>maa://36697 (85.16)</t>
         </is>
       </c>
     </row>
@@ -5285,7 +5285,7 @@
       </c>
       <c r="S44" s="5" t="inlineStr">
         <is>
-          <t>maa://39366 (86.96)</t>
+          <t>maa://39366 (83.33)</t>
         </is>
       </c>
     </row>
@@ -5355,7 +5355,7 @@
       </c>
       <c r="G46" s="5" t="inlineStr">
         <is>
-          <t>maa://35931 (92.51)</t>
+          <t>maa://35931 (92.54)</t>
         </is>
       </c>
       <c r="M46" s="4" t="inlineStr">
@@ -5755,7 +5755,7 @@
       </c>
       <c r="G60" s="5" t="inlineStr">
         <is>
-          <t>**maa://40438 (37.5)</t>
+          <t>**maa://40438 (33.33)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: Auto Update Data (#80)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -782,7 +782,7 @@
       </c>
       <c r="O3" s="5" t="inlineStr">
         <is>
-          <t>maa://21249 (95.12), maa://26254 (95.24)</t>
+          <t>maa://21249 (95.15), maa://26254 (95.24)</t>
         </is>
       </c>
       <c r="Q3" s="4" t="inlineStr">
@@ -919,7 +919,7 @@
       </c>
       <c r="S4" s="5" t="inlineStr">
         <is>
-          <t>maa://32509 (98.73), maa://22754 (91.67), maa://27295 (80.39), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (98.75), maa://22754 (91.67), maa://27295 (80.39), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="4" t="inlineStr">
@@ -1103,7 +1103,7 @@
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>*maa://42407 (75.0)</t>
+          <t>*maa://42407 (80.0)</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -1544,7 +1544,7 @@
       </c>
       <c r="W9" s="5" t="inlineStr">
         <is>
-          <t>maa://26223 (96.94)</t>
+          <t>maa://26223 (96.97)</t>
         </is>
       </c>
       <c r="Y9" s="4" t="inlineStr">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="S10" s="5" t="inlineStr">
         <is>
-          <t>maa://27395 (96.03), maa://22755 (87.62), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.03), maa://22755 (87.74), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="4" t="inlineStr">
@@ -2032,7 +2032,7 @@
       </c>
       <c r="W13" s="5" t="inlineStr">
         <is>
-          <t>*maa://34957 (75.56), *maa://22768 (53.33)</t>
+          <t>*maa://34957 (76.09), *maa://22768 (53.33)</t>
         </is>
       </c>
       <c r="Y13" s="4" t="inlineStr">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>*maa://22743 (76.19), maa://22734 (83.33), *maa://30808 (64.29), ***maa://36048 (13.33)</t>
+          <t>*maa://22743 (76.47), maa://22734 (83.33), *maa://30808 (64.29), ***maa://36048 (13.33)</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr">
@@ -2460,7 +2460,7 @@
       </c>
       <c r="G17" s="5" t="inlineStr">
         <is>
-          <t>maa://22430 (88.57), maa://39599 (84.21)</t>
+          <t>maa://22430 (88.57), *maa://39599 (80.0)</t>
         </is>
       </c>
       <c r="I17" s="4" t="inlineStr">
@@ -2500,10 +2500,14 @@
       </c>
       <c r="R17" s="4" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S17" s="5" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="S17" s="5" t="inlineStr">
+        <is>
+          <t>**maa://42324 (33.33)</t>
+        </is>
+      </c>
       <c r="U17" s="4" t="inlineStr">
         <is>
           <t>亚叶</t>
@@ -2563,7 +2567,7 @@
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
-          <t>maa://24570 (96.55)</t>
+          <t>maa://24570 (96.57)</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
@@ -2959,7 +2963,7 @@
       </c>
       <c r="K21" s="5" t="inlineStr">
         <is>
-          <t>maa://31731 (95.0)</t>
+          <t>maa://31731 (95.12)</t>
         </is>
       </c>
       <c r="M21" s="4" t="inlineStr">
@@ -3126,7 +3130,7 @@
       </c>
       <c r="W22" s="5" t="inlineStr">
         <is>
-          <t>maa://21282 (98.83), *maa://37649 (66.67)</t>
+          <t>maa://21282 (98.84), *maa://37649 (66.67)</t>
         </is>
       </c>
       <c r="Y22" s="4" t="inlineStr">
@@ -3248,7 +3252,7 @@
       </c>
       <c r="W23" s="5" t="inlineStr">
         <is>
-          <t>*maa://28503 (62.71)</t>
+          <t>*maa://28503 (63.33)</t>
         </is>
       </c>
       <c r="Y23" s="4" t="inlineStr">
@@ -3432,7 +3436,7 @@
       </c>
       <c r="G25" s="5" t="inlineStr">
         <is>
-          <t>*maa://29063 (76.15), *maa://25311 (74.19), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (75.57), *maa://25311 (74.19), ***maa://22725 (4.84)</t>
         </is>
       </c>
       <c r="I25" s="4" t="inlineStr">
@@ -3629,7 +3633,7 @@
       </c>
       <c r="AA26" s="5" t="inlineStr">
         <is>
-          <t>*maa://42235 (64.29)</t>
+          <t>*maa://42235 (68.75)</t>
         </is>
       </c>
       <c r="AC26" s="4" t="inlineStr">
@@ -3858,7 +3862,7 @@
       </c>
       <c r="W28" s="5" t="inlineStr">
         <is>
-          <t>maa://39929 (86.29), ***maa://39723 (14.71), maa://41749 (81.25)</t>
+          <t>maa://39929 (86.36), ***maa://39723 (14.71), maa://41749 (81.25)</t>
         </is>
       </c>
       <c r="Y28" s="4" t="inlineStr">
@@ -3888,7 +3892,7 @@
       </c>
       <c r="AE28" s="5" t="inlineStr">
         <is>
-          <t>maa://36660 (93.8), *maa://36701 (64.0)</t>
+          <t>maa://36660 (93.82), *maa://36701 (64.0)</t>
         </is>
       </c>
     </row>
@@ -4209,7 +4213,7 @@
       </c>
       <c r="S31" s="5" t="inlineStr">
         <is>
-          <t>maa://30711 (96.23), maa://30768 (100.0)</t>
+          <t>maa://30711 (96.3), maa://30768 (100.0)</t>
         </is>
       </c>
       <c r="U31" s="4" t="inlineStr">
@@ -5335,7 +5339,7 @@
       </c>
       <c r="S45" s="5" t="inlineStr">
         <is>
-          <t>*maa://39364 (62.5)</t>
+          <t>*maa://39364 (55.56)</t>
         </is>
       </c>
     </row>
@@ -5755,7 +5759,7 @@
       </c>
       <c r="G60" s="5" t="inlineStr">
         <is>
-          <t>**maa://40438 (33.33)</t>
+          <t>**maa://40438 (31.58)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: Auto Update Data (#81)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -1103,7 +1103,7 @@
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>*maa://42407 (80.0)</t>
+          <t>maa://42407 (83.33)</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -1559,7 +1559,7 @@
       </c>
       <c r="AA9" s="5" t="inlineStr">
         <is>
-          <t>maa://28711 (87.95), ***maa://22740 (5.88), **maa://27377 (46.15), ***maa://25174 (20.0), **maa://39938 (50.0), maa://40166 (100.0)</t>
+          <t>maa://28711 (87.95), ***maa://22740 (5.88), **maa://27377 (46.15), ***maa://25174 (20.0), **maa://39938 (46.67), maa://40166 (100.0)</t>
         </is>
       </c>
       <c r="AC9" s="4" t="inlineStr">
@@ -1925,7 +1925,7 @@
       </c>
       <c r="AA12" s="5" t="inlineStr">
         <is>
-          <t>maa://23669 (95.51), maa://36677 (92.5), maa://39872 (84.62)</t>
+          <t>maa://23669 (95.51), maa://36677 (92.5), maa://39872 (85.71)</t>
         </is>
       </c>
       <c r="AC12" s="4" t="inlineStr">
@@ -2062,7 +2062,7 @@
       </c>
       <c r="AE13" s="5" t="inlineStr">
         <is>
-          <t>**maa://22737 (30.6), maa://39883 (87.5), *maa://39885 (73.68)</t>
+          <t>**maa://22737 (30.6), maa://39883 (88.0), *maa://39885 (73.68)</t>
         </is>
       </c>
     </row>
@@ -2841,7 +2841,7 @@
       </c>
       <c r="K20" s="5" t="inlineStr">
         <is>
-          <t>maa://41331 (89.19)</t>
+          <t>maa://41331 (86.84)</t>
         </is>
       </c>
       <c r="M20" s="4" t="inlineStr">
@@ -3374,7 +3374,7 @@
       </c>
       <c r="W24" s="5" t="inlineStr">
         <is>
-          <t>maa://23504 (92.9), maa://29988 (86.21), **maa://22892 (40.14), *maa://25141 (76.86), maa://36663 (80.36), ***maa://22815 (23.08)</t>
+          <t>maa://23504 (92.9), maa://29988 (86.21), **maa://22892 (40.14), *maa://25141 (77.05), maa://36663 (80.36), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="4" t="inlineStr">
@@ -3633,7 +3633,7 @@
       </c>
       <c r="AA26" s="5" t="inlineStr">
         <is>
-          <t>*maa://42235 (68.75)</t>
+          <t>*maa://42235 (70.59)</t>
         </is>
       </c>
       <c r="AC26" s="4" t="inlineStr">
@@ -3862,7 +3862,7 @@
       </c>
       <c r="W28" s="5" t="inlineStr">
         <is>
-          <t>maa://39929 (86.36), ***maa://39723 (14.71), maa://41749 (81.25)</t>
+          <t>maa://39929 (86.43), ***maa://39723 (14.71), maa://41749 (81.25)</t>
         </is>
       </c>
       <c r="Y28" s="4" t="inlineStr">
@@ -4014,7 +4014,7 @@
       </c>
       <c r="AE29" s="5" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.04), ***maa://34960 (9.09)</t>
+          <t>*maa://24080 (69.13), ***maa://34960 (8.7)</t>
         </is>
       </c>
     </row>
@@ -5339,7 +5339,7 @@
       </c>
       <c r="S45" s="5" t="inlineStr">
         <is>
-          <t>*maa://39364 (55.56)</t>
+          <t>**maa://39364 (50.0)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: Auto Update Data (#82)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -752,7 +752,7 @@
       </c>
       <c r="G3" s="5" t="inlineStr">
         <is>
-          <t>maa://21247 (98.28), *maa://22748 (75.0)</t>
+          <t>maa://21247 (98.29), *maa://22748 (75.0)</t>
         </is>
       </c>
       <c r="I3" s="4" t="inlineStr">
@@ -782,7 +782,7 @@
       </c>
       <c r="O3" s="5" t="inlineStr">
         <is>
-          <t>maa://21249 (95.15), maa://26254 (95.24)</t>
+          <t>maa://21249 (95.17), maa://26254 (95.24)</t>
         </is>
       </c>
       <c r="Q3" s="4" t="inlineStr">
@@ -919,7 +919,7 @@
       </c>
       <c r="S4" s="5" t="inlineStr">
         <is>
-          <t>maa://32509 (98.75), maa://22754 (91.67), maa://27295 (80.39), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (98.77), maa://22754 (91.67), maa://27295 (80.39), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="4" t="inlineStr">
@@ -1574,7 +1574,7 @@
       </c>
       <c r="AE9" s="5" t="inlineStr">
         <is>
-          <t>maa://26206 (89.16), **maa://22865 (45.65)</t>
+          <t>maa://26206 (89.29), **maa://22865 (45.65)</t>
         </is>
       </c>
     </row>
@@ -2216,7 +2216,7 @@
       </c>
       <c r="G15" s="5" t="inlineStr">
         <is>
-          <t>maa://24304 (88.46), maa://21478 (91.18)</t>
+          <t>maa://24304 (88.52), maa://21478 (91.18)</t>
         </is>
       </c>
       <c r="I15" s="4" t="inlineStr">
@@ -2368,7 +2368,7 @@
       </c>
       <c r="O16" s="5" t="inlineStr">
         <is>
-          <t>maa://28504 (91.49)</t>
+          <t>maa://28504 (91.67)</t>
         </is>
       </c>
       <c r="Q16" s="4" t="inlineStr">
@@ -2460,7 +2460,7 @@
       </c>
       <c r="G17" s="5" t="inlineStr">
         <is>
-          <t>maa://22430 (88.57), *maa://39599 (80.0)</t>
+          <t>maa://22430 (88.57), maa://39599 (80.95)</t>
         </is>
       </c>
       <c r="I17" s="4" t="inlineStr">
@@ -2505,7 +2505,7 @@
       </c>
       <c r="S17" s="5" t="inlineStr">
         <is>
-          <t>**maa://42324 (33.33)</t>
+          <t>**maa://42324 (50.0)</t>
         </is>
       </c>
       <c r="U17" s="4" t="inlineStr">
@@ -2567,7 +2567,7 @@
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
-          <t>maa://24570 (96.57)</t>
+          <t>maa://24570 (96.59)</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="G18" s="5" t="inlineStr">
         <is>
-          <t>maa://24421 (90.14)</t>
+          <t>maa://24421 (90.19)</t>
         </is>
       </c>
       <c r="I18" s="4" t="inlineStr">
@@ -3008,7 +3008,7 @@
       </c>
       <c r="W21" s="5" t="inlineStr">
         <is>
-          <t>maa://20110 (86.57), maa://34946 (90.62)</t>
+          <t>maa://20110 (86.76), maa://34946 (90.62)</t>
         </is>
       </c>
       <c r="Y21" s="4" t="inlineStr">
@@ -3207,7 +3207,7 @@
       </c>
       <c r="K23" s="5" t="inlineStr">
         <is>
-          <t>maa://39756 (92.41), maa://39875 (95.74)</t>
+          <t>maa://39756 (92.41), maa://39875 (95.83)</t>
         </is>
       </c>
       <c r="M23" s="4" t="inlineStr">
@@ -3436,7 +3436,7 @@
       </c>
       <c r="G25" s="5" t="inlineStr">
         <is>
-          <t>*maa://29063 (75.57), *maa://25311 (74.19), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (75.76), *maa://25311 (74.19), ***maa://22725 (4.84)</t>
         </is>
       </c>
       <c r="I25" s="4" t="inlineStr">
@@ -3526,7 +3526,7 @@
       </c>
       <c r="AE25" s="5" t="inlineStr">
         <is>
-          <t>maa://20108 (96.12), maa://24621 (96.4), maa://36676 (100.0), maa://22771 (84.62), maa://37772 (100.0)</t>
+          <t>maa://20108 (96.12), maa://24621 (96.43), maa://36676 (100.0), maa://22771 (84.62), maa://37772 (100.0)</t>
         </is>
       </c>
     </row>
@@ -3862,7 +3862,7 @@
       </c>
       <c r="W28" s="5" t="inlineStr">
         <is>
-          <t>maa://39929 (86.43), ***maa://39723 (14.71), maa://41749 (81.25)</t>
+          <t>maa://39929 (86.57), ***maa://39723 (14.71), maa://41749 (81.25)</t>
         </is>
       </c>
       <c r="Y28" s="4" t="inlineStr">
@@ -3954,7 +3954,7 @@
       </c>
       <c r="O29" s="5" t="inlineStr">
         <is>
-          <t>*maa://23168 (55.77), **maa://30050 (40.0)</t>
+          <t>*maa://23168 (55.77), **maa://30050 (38.1)</t>
         </is>
       </c>
       <c r="Q29" s="4" t="inlineStr">
@@ -4335,7 +4335,7 @@
       </c>
       <c r="S32" s="5" t="inlineStr">
         <is>
-          <t>maa://41108 (91.18), maa://41238 (94.44)</t>
+          <t>maa://41108 (91.18), maa://41238 (94.59)</t>
         </is>
       </c>
       <c r="U32" s="4" t="inlineStr">
@@ -4564,7 +4564,7 @@
       </c>
       <c r="S34" s="5" t="inlineStr">
         <is>
-          <t>maa://24526 (93.07)</t>
+          <t>maa://24526 (93.1)</t>
         </is>
       </c>
       <c r="Y34" s="4" t="inlineStr">
@@ -4626,7 +4626,7 @@
       </c>
       <c r="K35" s="5" t="inlineStr">
         <is>
-          <t>maa://41296 (98.0)</t>
+          <t>maa://41296 (98.08)</t>
         </is>
       </c>
       <c r="M35" s="4" t="inlineStr">
@@ -4952,7 +4952,7 @@
       </c>
       <c r="AE38" s="5" t="inlineStr">
         <is>
-          <t>maa://36697 (85.16)</t>
+          <t>maa://36697 (84.5)</t>
         </is>
       </c>
     </row>
@@ -5674,7 +5674,7 @@
       </c>
       <c r="G55" s="5" t="inlineStr">
         <is>
-          <t>maa://32532 (92.31)</t>
+          <t>maa://32532 (92.34)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: Auto Update Data (#83)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -615,7 +615,7 @@
       </c>
       <c r="C2" s="5" t="inlineStr">
         <is>
-          <t>maa://24702 (94.1), maa://25390 (97.42), maa://36681 (90.77)</t>
+          <t>maa://24702 (94.1), maa://25390 (97.01), maa://36681 (90.77)</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
@@ -705,7 +705,7 @@
       </c>
       <c r="AA2" s="5" t="inlineStr">
         <is>
-          <t>maa://21246 (91.2), maa://36684 (98.61), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.2), maa://36684 (98.63), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="4" t="inlineStr">
@@ -720,7 +720,7 @@
       </c>
       <c r="AE2" s="5" t="inlineStr">
         <is>
-          <t>maa://25251 (92.5), ***maa://21730 (17.19), ***maa://39501 (23.08), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.5), ***maa://21730 (17.19), ***maa://39501 (21.43), *maa://36675 (60.0)</t>
         </is>
       </c>
     </row>
@@ -827,7 +827,7 @@
       </c>
       <c r="AA3" s="5" t="inlineStr">
         <is>
-          <t>maa://24390 (96.0)</t>
+          <t>maa://24390 (96.08)</t>
         </is>
       </c>
       <c r="AC3" s="4" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="W4" s="5" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.54), ***maa://31785 (18.02), ***maa://36683 (26.67)</t>
+          <t>**maa://32495 (47.54), ***maa://31785 (18.75), ***maa://36683 (26.67)</t>
         </is>
       </c>
       <c r="Y4" s="4" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="AA4" s="5" t="inlineStr">
         <is>
-          <t>*maa://32658 (73.33)</t>
+          <t>*maa://32658 (68.75)</t>
         </is>
       </c>
       <c r="AC4" s="4" t="inlineStr">
@@ -1103,7 +1103,7 @@
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>maa://42407 (83.33)</t>
+          <t>maa://42407 (87.5)</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -1300,7 +1300,7 @@
       </c>
       <c r="W7" s="5" t="inlineStr">
         <is>
-          <t>maa://22399 (94.62), *maa://22758 (71.15)</t>
+          <t>maa://22399 (94.66), *maa://22758 (71.7)</t>
         </is>
       </c>
       <c r="Y7" s="4" t="inlineStr">
@@ -1325,12 +1325,12 @@
       </c>
       <c r="AD7" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AE7" s="5" t="inlineStr">
         <is>
-          <t>*maa://26191 (68.49), *maa://36671 (72.09)</t>
+          <t>*maa://26191 (68.49), *maa://36671 (72.09), maa://42530 (100.0)</t>
         </is>
       </c>
     </row>
@@ -1422,7 +1422,7 @@
       </c>
       <c r="W8" s="5" t="inlineStr">
         <is>
-          <t>maa://21411 (96.01)</t>
+          <t>maa://21411 (96.03)</t>
         </is>
       </c>
       <c r="Y8" s="4" t="inlineStr">
@@ -1696,7 +1696,7 @@
       </c>
       <c r="AE10" s="5" t="inlineStr">
         <is>
-          <t>*maa://25021 (56.94), *maa://22733 (58.62), maa://22761 (100.0)</t>
+          <t>*maa://25021 (56.16), *maa://22733 (58.62), maa://22761 (100.0)</t>
         </is>
       </c>
     </row>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="W11" s="5" t="inlineStr">
         <is>
-          <t>maa://36713 (97.84)</t>
+          <t>maa://36713 (97.85)</t>
         </is>
       </c>
       <c r="Y11" s="4" t="inlineStr">
@@ -1910,7 +1910,7 @@
       </c>
       <c r="W12" s="5" t="inlineStr">
         <is>
-          <t>maa://22753 (91.84), *maa://21485 (76.74), maa://37962 (81.25)</t>
+          <t>maa://22753 (91.22), *maa://21485 (76.74), maa://37962 (81.25)</t>
         </is>
       </c>
       <c r="Y12" s="4" t="inlineStr">
@@ -2032,7 +2032,7 @@
       </c>
       <c r="W13" s="5" t="inlineStr">
         <is>
-          <t>*maa://34957 (76.09), *maa://22768 (53.33)</t>
+          <t>*maa://34957 (76.6), *maa://22768 (53.33)</t>
         </is>
       </c>
       <c r="Y13" s="4" t="inlineStr">
@@ -2062,7 +2062,7 @@
       </c>
       <c r="AE13" s="5" t="inlineStr">
         <is>
-          <t>**maa://22737 (30.6), maa://39883 (88.0), *maa://39885 (73.68)</t>
+          <t>**maa://22737 (30.6), maa://39883 (88.46), *maa://39885 (73.68)</t>
         </is>
       </c>
     </row>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="K14" s="5" t="inlineStr">
         <is>
-          <t>maa://26245 (96.12), maa://21288 (96.21), maa://36682 (100.0), maa://39841 (93.02)</t>
+          <t>maa://26245 (96.12), maa://21288 (96.21), maa://36682 (100.0), maa://39841 (93.18)</t>
         </is>
       </c>
       <c r="M14" s="4" t="inlineStr">
@@ -2216,7 +2216,7 @@
       </c>
       <c r="G15" s="5" t="inlineStr">
         <is>
-          <t>maa://24304 (88.52), maa://21478 (91.18)</t>
+          <t>maa://24304 (88.59), maa://21478 (91.18)</t>
         </is>
       </c>
       <c r="I15" s="4" t="inlineStr">
@@ -2323,7 +2323,7 @@
       </c>
       <c r="C16" s="5" t="inlineStr">
         <is>
-          <t>maa://21441 (96.17), maa://36679 (93.94), maa://37650 (95.45)</t>
+          <t>maa://21441 (96.17), maa://36679 (94.12), maa://37650 (95.45)</t>
         </is>
       </c>
       <c r="E16" s="4" t="inlineStr">
@@ -2398,7 +2398,7 @@
       </c>
       <c r="W16" s="5" t="inlineStr">
         <is>
-          <t>maa://28501 (97.44), maa://28051 (95.83)</t>
+          <t>maa://28501 (97.47), maa://28051 (95.83)</t>
         </is>
       </c>
       <c r="Y16" s="4" t="inlineStr">
@@ -2567,7 +2567,7 @@
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
-          <t>maa://24570 (96.59)</t>
+          <t>maa://24570 (96.61)</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="G18" s="5" t="inlineStr">
         <is>
-          <t>maa://24421 (90.19)</t>
+          <t>maa://24421 (90.23)</t>
         </is>
       </c>
       <c r="I18" s="4" t="inlineStr">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="S19" s="5" t="inlineStr">
         <is>
-          <t>maa://24386 (98.8)</t>
+          <t>maa://24386 (98.81)</t>
         </is>
       </c>
       <c r="U19" s="4" t="inlineStr">
@@ -2841,7 +2841,7 @@
       </c>
       <c r="K20" s="5" t="inlineStr">
         <is>
-          <t>maa://41331 (86.84)</t>
+          <t>maa://41331 (82.93)</t>
         </is>
       </c>
       <c r="M20" s="4" t="inlineStr">
@@ -2856,7 +2856,7 @@
       </c>
       <c r="O20" s="5" t="inlineStr">
         <is>
-          <t>maa://37442 (96.43)</t>
+          <t>maa://37442 (96.55)</t>
         </is>
       </c>
       <c r="Q20" s="4" t="inlineStr">
@@ -3207,7 +3207,7 @@
       </c>
       <c r="K23" s="5" t="inlineStr">
         <is>
-          <t>maa://39756 (92.41), maa://39875 (95.83)</t>
+          <t>maa://39756 (92.5), maa://39875 (95.83)</t>
         </is>
       </c>
       <c r="M23" s="4" t="inlineStr">
@@ -3374,7 +3374,7 @@
       </c>
       <c r="W24" s="5" t="inlineStr">
         <is>
-          <t>maa://23504 (92.9), maa://29988 (86.21), **maa://22892 (40.14), *maa://25141 (77.05), maa://36663 (80.36), ***maa://22815 (23.08)</t>
+          <t>maa://23504 (92.9), maa://29988 (86.27), **maa://22892 (40.14), *maa://25141 (77.05), maa://36663 (80.7), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="4" t="inlineStr">
@@ -3421,7 +3421,7 @@
       </c>
       <c r="C25" s="5" t="inlineStr">
         <is>
-          <t>maa://29753 (95.13)</t>
+          <t>maa://29753 (95.15)</t>
         </is>
       </c>
       <c r="E25" s="4" t="inlineStr">
@@ -3511,7 +3511,7 @@
       </c>
       <c r="AA25" s="5" t="inlineStr">
         <is>
-          <t>maa://31215 (83.95), *maa://24516 (79.07), maa://26001 (88.89)</t>
+          <t>maa://31215 (84.15), *maa://24516 (79.07), maa://26001 (88.89)</t>
         </is>
       </c>
       <c r="AC25" s="4" t="inlineStr">
@@ -3633,7 +3633,7 @@
       </c>
       <c r="AA26" s="5" t="inlineStr">
         <is>
-          <t>*maa://42235 (70.59)</t>
+          <t>*maa://42235 (73.68)</t>
         </is>
       </c>
       <c r="AC26" s="4" t="inlineStr">
@@ -3725,7 +3725,7 @@
       </c>
       <c r="S27" s="5" t="inlineStr">
         <is>
-          <t>*maa://30624 (75.68)</t>
+          <t>*maa://30624 (76.32)</t>
         </is>
       </c>
       <c r="U27" s="4" t="inlineStr">
@@ -3787,7 +3787,7 @@
       </c>
       <c r="C28" s="5" t="inlineStr">
         <is>
-          <t>maa://24465 (90.35), maa://25725 (82.28)</t>
+          <t>maa://24465 (90.36), maa://25725 (82.28)</t>
         </is>
       </c>
       <c r="E28" s="4" t="inlineStr">
@@ -3862,7 +3862,7 @@
       </c>
       <c r="W28" s="5" t="inlineStr">
         <is>
-          <t>maa://39929 (86.57), ***maa://39723 (14.71), maa://41749 (81.25)</t>
+          <t>maa://39929 (86.7), ***maa://39723 (14.71), maa://41749 (81.25)</t>
         </is>
       </c>
       <c r="Y28" s="4" t="inlineStr">
@@ -3892,7 +3892,7 @@
       </c>
       <c r="AE28" s="5" t="inlineStr">
         <is>
-          <t>maa://36660 (93.82), *maa://36701 (64.0)</t>
+          <t>maa://36660 (93.85), *maa://36701 (64.0)</t>
         </is>
       </c>
     </row>
@@ -3909,7 +3909,7 @@
       </c>
       <c r="C29" s="5" t="inlineStr">
         <is>
-          <t>maa://31694 (97.87)</t>
+          <t>maa://31694 (97.92)</t>
         </is>
       </c>
       <c r="E29" s="4" t="inlineStr">
@@ -4061,7 +4061,7 @@
       </c>
       <c r="K30" s="5" t="inlineStr">
         <is>
-          <t>maa://30442 (94.44)</t>
+          <t>maa://30442 (94.55)</t>
         </is>
       </c>
       <c r="M30" s="4" t="inlineStr">
@@ -4106,7 +4106,7 @@
       </c>
       <c r="W30" s="5" t="inlineStr">
         <is>
-          <t>*maa://39477 (71.43)</t>
+          <t>*maa://39477 (75.0)</t>
         </is>
       </c>
       <c r="Y30" s="4" t="inlineStr">
@@ -4335,7 +4335,7 @@
       </c>
       <c r="S32" s="5" t="inlineStr">
         <is>
-          <t>maa://41108 (91.18), maa://41238 (94.59)</t>
+          <t>maa://41108 (91.43), maa://41238 (94.59)</t>
         </is>
       </c>
       <c r="U32" s="4" t="inlineStr">
@@ -4564,7 +4564,7 @@
       </c>
       <c r="S34" s="5" t="inlineStr">
         <is>
-          <t>maa://24526 (93.1)</t>
+          <t>maa://24526 (93.13)</t>
         </is>
       </c>
       <c r="Y34" s="4" t="inlineStr">
@@ -4626,7 +4626,7 @@
       </c>
       <c r="K35" s="5" t="inlineStr">
         <is>
-          <t>maa://41296 (98.08)</t>
+          <t>maa://41296 (98.11)</t>
         </is>
       </c>
       <c r="M35" s="4" t="inlineStr">
@@ -4952,7 +4952,7 @@
       </c>
       <c r="AE38" s="5" t="inlineStr">
         <is>
-          <t>maa://36697 (84.5)</t>
+          <t>maa://36697 (84.62)</t>
         </is>
       </c>
     </row>
@@ -4969,7 +4969,7 @@
       </c>
       <c r="G39" s="5" t="inlineStr">
         <is>
-          <t>maa://25199 (86.11), maa://36670 (88.06), maa://30434 (87.27), ***maa://25036 (16.0)</t>
+          <t>maa://25199 (86.11), maa://36670 (88.06), maa://30434 (87.5), ***maa://25036 (16.0)</t>
         </is>
       </c>
       <c r="I39" s="4" t="inlineStr">
@@ -4999,7 +4999,7 @@
       </c>
       <c r="O39" s="5" t="inlineStr">
         <is>
-          <t>maa://24709 (92.0)</t>
+          <t>maa://24709 (92.16)</t>
         </is>
       </c>
       <c r="Q39" s="4" t="inlineStr">
@@ -5212,7 +5212,7 @@
       </c>
       <c r="G43" s="5" t="inlineStr">
         <is>
-          <t>maa://22525 (92.62), maa://21284 (82.93)</t>
+          <t>maa://22525 (92.68), maa://21284 (82.93)</t>
         </is>
       </c>
       <c r="M43" s="4" t="inlineStr">
@@ -5359,7 +5359,7 @@
       </c>
       <c r="G46" s="5" t="inlineStr">
         <is>
-          <t>maa://35931 (92.54)</t>
+          <t>maa://35931 (92.58)</t>
         </is>
       </c>
       <c r="M46" s="4" t="inlineStr">
@@ -5674,7 +5674,7 @@
       </c>
       <c r="G55" s="5" t="inlineStr">
         <is>
-          <t>maa://32532 (92.34)</t>
+          <t>maa://32532 (91.93)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: Auto Update Data (#84)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -705,7 +705,7 @@
       </c>
       <c r="AA2" s="5" t="inlineStr">
         <is>
-          <t>maa://21246 (91.2), maa://36684 (98.63), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.23), maa://36684 (98.63), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="4" t="inlineStr">
@@ -767,7 +767,7 @@
       </c>
       <c r="K3" s="5" t="inlineStr">
         <is>
-          <t>*maa://22880 (69.93), maa://20276 (82.86), *maa://22749 (62.5)</t>
+          <t>*maa://22880 (69.68), maa://20276 (82.86), *maa://22749 (66.67)</t>
         </is>
       </c>
       <c r="M3" s="4" t="inlineStr">
@@ -812,7 +812,7 @@
       </c>
       <c r="W3" s="5" t="inlineStr">
         <is>
-          <t>maa://27396 (84.97), maa://27484 (95.74), maa://27480 (82.35)</t>
+          <t>maa://27396 (85.02), maa://27484 (95.74), maa://27480 (82.35)</t>
         </is>
       </c>
       <c r="Y3" s="4" t="inlineStr">
@@ -827,7 +827,7 @@
       </c>
       <c r="AA3" s="5" t="inlineStr">
         <is>
-          <t>maa://24390 (96.08)</t>
+          <t>maa://24390 (96.15)</t>
         </is>
       </c>
       <c r="AC3" s="4" t="inlineStr">
@@ -919,7 +919,7 @@
       </c>
       <c r="S4" s="5" t="inlineStr">
         <is>
-          <t>maa://32509 (98.77), maa://22754 (91.67), maa://27295 (80.39), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (98.78), maa://22754 (91.67), maa://27295 (80.39), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="4" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="W4" s="5" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.54), ***maa://31785 (18.75), ***maa://36683 (26.67)</t>
+          <t>**maa://32495 (47.54), ***maa://31785 (19.47), ***maa://36683 (26.67)</t>
         </is>
       </c>
       <c r="Y4" s="4" t="inlineStr">
@@ -1193,7 +1193,7 @@
       </c>
       <c r="AA6" s="5" t="inlineStr">
         <is>
-          <t>maa://22739 (91.3)</t>
+          <t>maa://22739 (91.67)</t>
         </is>
       </c>
       <c r="AC6" s="4" t="inlineStr">
@@ -1300,7 +1300,7 @@
       </c>
       <c r="W7" s="5" t="inlineStr">
         <is>
-          <t>maa://22399 (94.66), *maa://22758 (71.7)</t>
+          <t>maa://22399 (94.66), *maa://22758 (70.37)</t>
         </is>
       </c>
       <c r="Y7" s="4" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="AE7" s="5" t="inlineStr">
         <is>
-          <t>*maa://26191 (68.49), *maa://36671 (72.09), maa://42530 (100.0)</t>
+          <t>*maa://26191 (68.49), *maa://36671 (72.73), maa://42530 (100.0)</t>
         </is>
       </c>
     </row>
@@ -1392,7 +1392,7 @@
       </c>
       <c r="O8" s="5" t="inlineStr">
         <is>
-          <t>maa://32931 (88.61), *maa://21916 (60.34), maa://23252 (92.31), **maa://22759 (45.45), maa://37496 (100.0)</t>
+          <t>maa://32931 (88.89), *maa://21916 (60.34), maa://23252 (92.31), **maa://22759 (45.45), maa://37496 (100.0)</t>
         </is>
       </c>
       <c r="Q8" s="4" t="inlineStr">
@@ -1422,7 +1422,7 @@
       </c>
       <c r="W8" s="5" t="inlineStr">
         <is>
-          <t>maa://21411 (96.03)</t>
+          <t>maa://21411 (96.04)</t>
         </is>
       </c>
       <c r="Y8" s="4" t="inlineStr">
@@ -1544,7 +1544,7 @@
       </c>
       <c r="W9" s="5" t="inlineStr">
         <is>
-          <t>maa://26223 (96.97)</t>
+          <t>maa://26223 (97.0)</t>
         </is>
       </c>
       <c r="Y9" s="4" t="inlineStr">
@@ -1559,7 +1559,7 @@
       </c>
       <c r="AA9" s="5" t="inlineStr">
         <is>
-          <t>maa://28711 (87.95), ***maa://22740 (5.88), **maa://27377 (46.15), ***maa://25174 (20.0), **maa://39938 (46.67), maa://40166 (100.0)</t>
+          <t>maa://28711 (88.1), ***maa://22740 (5.88), **maa://27377 (46.15), ***maa://25174 (20.0), **maa://39938 (43.75), maa://40166 (100.0)</t>
         </is>
       </c>
       <c r="AC9" s="4" t="inlineStr">
@@ -1666,7 +1666,7 @@
       </c>
       <c r="W10" s="5" t="inlineStr">
         <is>
-          <t>maa://22301 (97.41), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.42), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="4" t="inlineStr">
@@ -1788,7 +1788,7 @@
       </c>
       <c r="W11" s="5" t="inlineStr">
         <is>
-          <t>maa://36713 (97.85)</t>
+          <t>maa://36713 (97.86)</t>
         </is>
       </c>
       <c r="Y11" s="4" t="inlineStr">
@@ -1850,7 +1850,7 @@
       </c>
       <c r="G12" s="5" t="inlineStr">
         <is>
-          <t>maa://21867 (90.0)</t>
+          <t>maa://21867 (90.07)</t>
         </is>
       </c>
       <c r="I12" s="4" t="inlineStr">
@@ -1972,7 +1972,7 @@
       </c>
       <c r="G13" s="5" t="inlineStr">
         <is>
-          <t>*maa://21248 (75.36), **maa://22728 (47.62)</t>
+          <t>*maa://21248 (75.48), **maa://22728 (47.62)</t>
         </is>
       </c>
       <c r="I13" s="4" t="inlineStr">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>*maa://22743 (76.47), maa://22734 (83.33), *maa://30808 (64.29), ***maa://36048 (13.33)</t>
+          <t>*maa://22743 (76.61), maa://22734 (83.33), *maa://30808 (64.29), ***maa://36048 (12.9)</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr">
@@ -2216,7 +2216,7 @@
       </c>
       <c r="G15" s="5" t="inlineStr">
         <is>
-          <t>maa://24304 (88.59), maa://21478 (91.18)</t>
+          <t>maa://24304 (88.11), maa://21478 (91.18)</t>
         </is>
       </c>
       <c r="I15" s="4" t="inlineStr">
@@ -2306,7 +2306,7 @@
       </c>
       <c r="AE15" s="5" t="inlineStr">
         <is>
-          <t>maa://21364 (80.61), *maa://22766 (73.0), *maa://36666 (78.46)</t>
+          <t>maa://21364 (80.68), *maa://22766 (73.0), *maa://36666 (78.46)</t>
         </is>
       </c>
     </row>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="AE16" s="5" t="inlineStr">
         <is>
-          <t>*maa://23911 (61.96), maa://27755 (91.78)</t>
+          <t>*maa://23911 (61.96), maa://27755 (91.89)</t>
         </is>
       </c>
     </row>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="G17" s="5" t="inlineStr">
         <is>
-          <t>maa://22430 (88.57), maa://39599 (80.95)</t>
+          <t>maa://22430 (88.14), maa://39599 (80.95)</t>
         </is>
       </c>
       <c r="I17" s="4" t="inlineStr">
@@ -2505,7 +2505,7 @@
       </c>
       <c r="S17" s="5" t="inlineStr">
         <is>
-          <t>**maa://42324 (50.0)</t>
+          <t>***maa://42324 (28.57)</t>
         </is>
       </c>
       <c r="U17" s="4" t="inlineStr">
@@ -2567,7 +2567,7 @@
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
-          <t>maa://24570 (96.61)</t>
+          <t>maa://24570 (96.65)</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
@@ -2779,7 +2779,7 @@
       </c>
       <c r="AA19" s="5" t="inlineStr">
         <is>
-          <t>*maa://30709 (60.8), *maa://36668 (52.17)</t>
+          <t>*maa://30709 (60.9), *maa://36668 (52.17)</t>
         </is>
       </c>
       <c r="AC19" s="4" t="inlineStr">
@@ -2826,7 +2826,7 @@
       </c>
       <c r="G20" s="5" t="inlineStr">
         <is>
-          <t>maa://22864 (88.46)</t>
+          <t>maa://22864 (88.55)</t>
         </is>
       </c>
       <c r="I20" s="4" t="inlineStr">
@@ -3207,7 +3207,7 @@
       </c>
       <c r="K23" s="5" t="inlineStr">
         <is>
-          <t>maa://39756 (92.5), maa://39875 (95.83)</t>
+          <t>maa://39756 (92.59), maa://39875 (95.83)</t>
         </is>
       </c>
       <c r="M23" s="4" t="inlineStr">
@@ -3252,7 +3252,7 @@
       </c>
       <c r="W23" s="5" t="inlineStr">
         <is>
-          <t>*maa://28503 (63.33)</t>
+          <t>*maa://28503 (63.93)</t>
         </is>
       </c>
       <c r="Y23" s="4" t="inlineStr">
@@ -3299,7 +3299,7 @@
       </c>
       <c r="C24" s="5" t="inlineStr">
         <is>
-          <t>maa://24368 (80.36)</t>
+          <t>maa://24368 (80.42)</t>
         </is>
       </c>
       <c r="E24" s="4" t="inlineStr">
@@ -3374,7 +3374,7 @@
       </c>
       <c r="W24" s="5" t="inlineStr">
         <is>
-          <t>maa://23504 (92.9), maa://29988 (86.27), **maa://22892 (40.14), *maa://25141 (77.05), maa://36663 (80.7), ***maa://22815 (23.08)</t>
+          <t>maa://23504 (92.92), maa://29988 (86.34), **maa://22892 (40.14), *maa://25141 (77.05), maa://36663 (80.7), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="4" t="inlineStr">
@@ -3421,7 +3421,7 @@
       </c>
       <c r="C25" s="5" t="inlineStr">
         <is>
-          <t>maa://29753 (95.15)</t>
+          <t>maa://29753 (95.18)</t>
         </is>
       </c>
       <c r="E25" s="4" t="inlineStr">
@@ -3436,7 +3436,7 @@
       </c>
       <c r="G25" s="5" t="inlineStr">
         <is>
-          <t>*maa://29063 (75.76), *maa://25311 (74.19), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (76.12), *maa://25311 (74.19), ***maa://22725 (4.84)</t>
         </is>
       </c>
       <c r="I25" s="4" t="inlineStr">
@@ -3633,7 +3633,7 @@
       </c>
       <c r="AA26" s="5" t="inlineStr">
         <is>
-          <t>*maa://42235 (73.68)</t>
+          <t>*maa://42235 (76.19)</t>
         </is>
       </c>
       <c r="AC26" s="4" t="inlineStr">
@@ -3770,7 +3770,7 @@
       </c>
       <c r="AE27" s="5" t="inlineStr">
         <is>
-          <t>maa://24023 (96.77)</t>
+          <t>maa://24023 (96.83)</t>
         </is>
       </c>
     </row>
@@ -3862,7 +3862,7 @@
       </c>
       <c r="W28" s="5" t="inlineStr">
         <is>
-          <t>maa://39929 (86.7), ***maa://39723 (14.71), maa://41749 (81.25)</t>
+          <t>maa://39929 (86.83), ***maa://39723 (14.71), maa://41749 (81.25)</t>
         </is>
       </c>
       <c r="Y28" s="4" t="inlineStr">
@@ -3892,7 +3892,7 @@
       </c>
       <c r="AE28" s="5" t="inlineStr">
         <is>
-          <t>maa://36660 (93.85), *maa://36701 (64.0)</t>
+          <t>maa://36660 (93.87), *maa://36701 (64.0)</t>
         </is>
       </c>
     </row>
@@ -3939,7 +3939,7 @@
       </c>
       <c r="K29" s="5" t="inlineStr">
         <is>
-          <t>maa://28432 (93.47), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (66.67)</t>
+          <t>maa://28432 (93.52), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (66.67)</t>
         </is>
       </c>
       <c r="M29" s="4" t="inlineStr">
@@ -4014,7 +4014,7 @@
       </c>
       <c r="AE29" s="5" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.13), ***maa://34960 (8.7)</t>
+          <t>*maa://24080 (69.02), ***maa://34960 (8.7)</t>
         </is>
       </c>
     </row>
@@ -4335,7 +4335,7 @@
       </c>
       <c r="S32" s="5" t="inlineStr">
         <is>
-          <t>maa://41108 (91.43), maa://41238 (94.59)</t>
+          <t>maa://41108 (89.47), maa://41238 (94.59)</t>
         </is>
       </c>
       <c r="U32" s="4" t="inlineStr">
@@ -4564,7 +4564,7 @@
       </c>
       <c r="S34" s="5" t="inlineStr">
         <is>
-          <t>maa://24526 (93.13)</t>
+          <t>maa://24526 (93.16)</t>
         </is>
       </c>
       <c r="Y34" s="4" t="inlineStr">
@@ -4626,7 +4626,7 @@
       </c>
       <c r="K35" s="5" t="inlineStr">
         <is>
-          <t>maa://41296 (98.11)</t>
+          <t>maa://41296 (98.15)</t>
         </is>
       </c>
       <c r="M35" s="4" t="inlineStr">
@@ -4952,7 +4952,7 @@
       </c>
       <c r="AE38" s="5" t="inlineStr">
         <is>
-          <t>maa://36697 (84.62)</t>
+          <t>maa://36697 (84.73)</t>
         </is>
       </c>
     </row>
@@ -4999,7 +4999,7 @@
       </c>
       <c r="O39" s="5" t="inlineStr">
         <is>
-          <t>maa://24709 (92.16)</t>
+          <t>maa://24709 (92.23)</t>
         </is>
       </c>
       <c r="Q39" s="4" t="inlineStr">
@@ -5081,7 +5081,7 @@
       </c>
       <c r="O40" s="5" t="inlineStr">
         <is>
-          <t>maa://23278 (95.88), maa://21386 (95.63), maa://36664 (90.24)</t>
+          <t>maa://23278 (95.89), maa://21386 (95.63), maa://36664 (90.24)</t>
         </is>
       </c>
       <c r="Q40" s="4" t="inlineStr">
@@ -5259,7 +5259,7 @@
       </c>
       <c r="G44" s="5" t="inlineStr">
         <is>
-          <t>maa://29768 (97.52), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.54), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="M44" s="4" t="inlineStr">
@@ -5359,7 +5359,7 @@
       </c>
       <c r="G46" s="5" t="inlineStr">
         <is>
-          <t>maa://35931 (92.58)</t>
+          <t>maa://35931 (92.61)</t>
         </is>
       </c>
       <c r="M46" s="4" t="inlineStr">
@@ -5409,7 +5409,7 @@
       </c>
       <c r="G47" s="5" t="inlineStr">
         <is>
-          <t>maa://27410 (95.81), maa://29661 (97.64), maa://28038 (84.62)</t>
+          <t>maa://27410 (95.82), maa://29661 (97.64), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="M47" s="4" t="inlineStr">
@@ -5640,7 +5640,7 @@
       </c>
       <c r="G53" s="5" t="inlineStr">
         <is>
-          <t>maa://32534 (93.21), **maa://32434 (36.36)</t>
+          <t>maa://32534 (93.26), **maa://32434 (36.36)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: Auto Update Data (#85)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -615,7 +615,7 @@
       </c>
       <c r="C2" s="5" t="inlineStr">
         <is>
-          <t>maa://24702 (94.1), maa://25390 (97.01), maa://36681 (90.77)</t>
+          <t>maa://24702 (94.1), maa://25390 (96.6), maa://36681 (90.77)</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
@@ -705,7 +705,7 @@
       </c>
       <c r="AA2" s="5" t="inlineStr">
         <is>
-          <t>maa://21246 (91.23), maa://36684 (98.63), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.26), maa://36684 (98.63), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="4" t="inlineStr">
@@ -767,7 +767,7 @@
       </c>
       <c r="K3" s="5" t="inlineStr">
         <is>
-          <t>*maa://22880 (69.68), maa://20276 (82.86), *maa://22749 (66.67)</t>
+          <t>*maa://22880 (69.23), maa://20276 (82.86), *maa://22749 (66.67)</t>
         </is>
       </c>
       <c r="M3" s="4" t="inlineStr">
@@ -919,7 +919,7 @@
       </c>
       <c r="S4" s="5" t="inlineStr">
         <is>
-          <t>maa://32509 (98.78), maa://22754 (91.67), maa://27295 (80.39), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (98.8), maa://22754 (91.67), maa://27295 (80.39), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="4" t="inlineStr">
@@ -1103,7 +1103,7 @@
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>maa://42407 (87.5)</t>
+          <t>maa://42407 (88.89)</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -1133,7 +1133,7 @@
       </c>
       <c r="K6" s="5" t="inlineStr">
         <is>
-          <t>maa://24839 (99.2)</t>
+          <t>maa://24839 (99.21)</t>
         </is>
       </c>
       <c r="M6" s="4" t="inlineStr">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="S6" s="5" t="inlineStr">
         <is>
-          <t>*maa://37411 (75.0)</t>
+          <t>*maa://37411 (77.78)</t>
         </is>
       </c>
       <c r="U6" s="4" t="inlineStr">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="O7" s="5" t="inlineStr">
         <is>
-          <t>maa://22750 (97.06)</t>
+          <t>maa://22750 (97.14)</t>
         </is>
       </c>
       <c r="Q7" s="4" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>*maa://21476 (69.77), **maa://39431 (40.0), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (69.77), **maa://39431 (50.0), *maa://37551 (57.14)</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
@@ -1392,7 +1392,7 @@
       </c>
       <c r="O8" s="5" t="inlineStr">
         <is>
-          <t>maa://32931 (88.89), *maa://21916 (60.34), maa://23252 (92.31), **maa://22759 (45.45), maa://37496 (100.0)</t>
+          <t>maa://32931 (87.8), *maa://21916 (60.34), maa://23252 (92.31), **maa://22759 (45.45), maa://37496 (100.0)</t>
         </is>
       </c>
       <c r="Q8" s="4" t="inlineStr">
@@ -1422,7 +1422,7 @@
       </c>
       <c r="W8" s="5" t="inlineStr">
         <is>
-          <t>maa://21411 (96.04)</t>
+          <t>maa://21411 (96.07)</t>
         </is>
       </c>
       <c r="Y8" s="4" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="S9" s="5" t="inlineStr">
         <is>
-          <t>**maa://22866 (30.77), maa://26222 (97.3)</t>
+          <t>**maa://22866 (30.77), maa://26222 (97.37)</t>
         </is>
       </c>
       <c r="U9" s="4" t="inlineStr">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="S10" s="5" t="inlineStr">
         <is>
-          <t>maa://27395 (96.03), maa://22755 (87.74), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.08), maa://22755 (87.74), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="4" t="inlineStr">
@@ -1773,7 +1773,7 @@
       </c>
       <c r="S11" s="5" t="inlineStr">
         <is>
-          <t>maa://22747 (94.37), maa://22501 (98.15)</t>
+          <t>maa://22747 (94.41), maa://22501 (98.15)</t>
         </is>
       </c>
       <c r="U11" s="4" t="inlineStr">
@@ -1803,7 +1803,7 @@
       </c>
       <c r="AA11" s="5" t="inlineStr">
         <is>
-          <t>maa://22516 (89.16), maa://29912 (100.0), *maa://20794 (52.24)</t>
+          <t>maa://22516 (89.29), maa://29912 (100.0), *maa://20794 (52.24)</t>
         </is>
       </c>
       <c r="AC11" s="4" t="inlineStr">
@@ -1972,7 +1972,7 @@
       </c>
       <c r="G13" s="5" t="inlineStr">
         <is>
-          <t>*maa://21248 (75.48), **maa://22728 (47.62)</t>
+          <t>*maa://21248 (75.12), **maa://22728 (47.62)</t>
         </is>
       </c>
       <c r="I13" s="4" t="inlineStr">
@@ -2002,7 +2002,7 @@
       </c>
       <c r="O13" s="5" t="inlineStr">
         <is>
-          <t>maa://22676 (91.84), *maa://22583 (75.0), *maa://22500 (55.81)</t>
+          <t>maa://22676 (91.84), *maa://22583 (75.41), *maa://22500 (55.81)</t>
         </is>
       </c>
       <c r="Q13" s="4" t="inlineStr">
@@ -2032,7 +2032,7 @@
       </c>
       <c r="W13" s="5" t="inlineStr">
         <is>
-          <t>*maa://34957 (76.6), *maa://22768 (53.33)</t>
+          <t>*maa://34957 (76.6), *maa://22768 (51.61)</t>
         </is>
       </c>
       <c r="Y13" s="4" t="inlineStr">
@@ -2062,7 +2062,7 @@
       </c>
       <c r="AE13" s="5" t="inlineStr">
         <is>
-          <t>**maa://22737 (30.6), maa://39883 (88.46), *maa://39885 (73.68)</t>
+          <t>**maa://22737 (30.6), maa://39883 (88.89), *maa://39885 (73.68)</t>
         </is>
       </c>
     </row>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="K14" s="5" t="inlineStr">
         <is>
-          <t>maa://26245 (96.12), maa://21288 (96.21), maa://36682 (100.0), maa://39841 (93.18)</t>
+          <t>maa://26245 (96.12), maa://21288 (96.21), maa://36682 (100.0), maa://39841 (93.33)</t>
         </is>
       </c>
       <c r="M14" s="4" t="inlineStr">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>*maa://22743 (76.61), maa://22734 (83.33), *maa://30808 (64.29), ***maa://36048 (12.9)</t>
+          <t>*maa://22743 (76.88), maa://22734 (83.33), *maa://30808 (64.29), ***maa://36048 (12.9)</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr">
@@ -2323,7 +2323,7 @@
       </c>
       <c r="C16" s="5" t="inlineStr">
         <is>
-          <t>maa://21441 (96.17), maa://36679 (94.12), maa://37650 (95.45)</t>
+          <t>maa://21441 (96.17), maa://36679 (91.43), maa://37650 (95.45)</t>
         </is>
       </c>
       <c r="E16" s="4" t="inlineStr">
@@ -2368,7 +2368,7 @@
       </c>
       <c r="O16" s="5" t="inlineStr">
         <is>
-          <t>maa://28504 (91.67)</t>
+          <t>maa://28504 (91.84)</t>
         </is>
       </c>
       <c r="Q16" s="4" t="inlineStr">
@@ -2383,7 +2383,7 @@
       </c>
       <c r="S16" s="5" t="inlineStr">
         <is>
-          <t>maa://22729 (95.17), *maa://28648 (69.09), *maa://36674 (79.31)</t>
+          <t>maa://22729 (95.17), *maa://28648 (69.09), *maa://36674 (80.0)</t>
         </is>
       </c>
       <c r="U16" s="4" t="inlineStr">
@@ -2428,7 +2428,7 @@
       </c>
       <c r="AE16" s="5" t="inlineStr">
         <is>
-          <t>*maa://23911 (61.96), maa://27755 (91.89)</t>
+          <t>*maa://23911 (62.37), maa://27755 (91.89)</t>
         </is>
       </c>
     </row>
@@ -2567,7 +2567,7 @@
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
-          <t>maa://24570 (96.65)</t>
+          <t>maa://24570 (96.67)</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
@@ -2963,7 +2963,7 @@
       </c>
       <c r="K21" s="5" t="inlineStr">
         <is>
-          <t>maa://31731 (95.12)</t>
+          <t>maa://31731 (95.24)</t>
         </is>
       </c>
       <c r="M21" s="4" t="inlineStr">
@@ -3023,7 +3023,7 @@
       </c>
       <c r="AA21" s="5" t="inlineStr">
         <is>
-          <t>*maa://21443 (78.72), **maa://23820 (30.91)</t>
+          <t>*maa://21443 (78.79), **maa://23820 (30.91)</t>
         </is>
       </c>
       <c r="AC21" s="4" t="inlineStr">
@@ -3038,7 +3038,7 @@
       </c>
       <c r="AE21" s="5" t="inlineStr">
         <is>
-          <t>maa://22524 (94.29), *maa://22432 (74.55)</t>
+          <t>maa://22524 (94.32), *maa://22432 (74.55)</t>
         </is>
       </c>
     </row>
@@ -3085,7 +3085,7 @@
       </c>
       <c r="K22" s="5" t="inlineStr">
         <is>
-          <t>maa://27127 (86.52), *maa://22751 (77.05)</t>
+          <t>maa://27127 (86.52), *maa://22751 (77.42)</t>
         </is>
       </c>
       <c r="M22" s="4" t="inlineStr">
@@ -3374,7 +3374,7 @@
       </c>
       <c r="W24" s="5" t="inlineStr">
         <is>
-          <t>maa://23504 (92.92), maa://29988 (86.34), **maa://22892 (40.14), *maa://25141 (77.05), maa://36663 (80.7), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.41), maa://23504 (92.92), **maa://22892 (40.14), *maa://25141 (77.05), maa://36663 (80.7), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="4" t="inlineStr">
@@ -3404,7 +3404,7 @@
       </c>
       <c r="AE24" s="5" t="inlineStr">
         <is>
-          <t>maa://22523 (85.03), *maa://36672 (76.74), maa://29910 (94.12), **maa://21440 (34.55)</t>
+          <t>maa://22523 (85.19), *maa://36672 (76.74), maa://29910 (94.12), **maa://21440 (34.55)</t>
         </is>
       </c>
     </row>
@@ -3436,7 +3436,7 @@
       </c>
       <c r="G25" s="5" t="inlineStr">
         <is>
-          <t>*maa://29063 (76.12), *maa://25311 (74.19), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (75.56), *maa://25311 (74.19), ***maa://22725 (4.84)</t>
         </is>
       </c>
       <c r="I25" s="4" t="inlineStr">
@@ -3558,7 +3558,7 @@
       </c>
       <c r="G26" s="5" t="inlineStr">
         <is>
-          <t>maa://24913 (91.04)</t>
+          <t>maa://24913 (91.18)</t>
         </is>
       </c>
       <c r="I26" s="4" t="inlineStr">
@@ -3633,7 +3633,7 @@
       </c>
       <c r="AA26" s="5" t="inlineStr">
         <is>
-          <t>*maa://42235 (76.19)</t>
+          <t>*maa://42235 (78.26)</t>
         </is>
       </c>
       <c r="AC26" s="4" t="inlineStr">
@@ -3787,7 +3787,7 @@
       </c>
       <c r="C28" s="5" t="inlineStr">
         <is>
-          <t>maa://24465 (90.36), maa://25725 (82.28)</t>
+          <t>maa://24465 (90.37), maa://25725 (82.28)</t>
         </is>
       </c>
       <c r="E28" s="4" t="inlineStr">
@@ -3862,7 +3862,7 @@
       </c>
       <c r="W28" s="5" t="inlineStr">
         <is>
-          <t>maa://39929 (86.83), ***maa://39723 (14.71), maa://41749 (81.25)</t>
+          <t>maa://39929 (86.89), ***maa://39723 (14.71), maa://41749 (82.35)</t>
         </is>
       </c>
       <c r="Y28" s="4" t="inlineStr">
@@ -3892,7 +3892,7 @@
       </c>
       <c r="AE28" s="5" t="inlineStr">
         <is>
-          <t>maa://36660 (93.87), *maa://36701 (64.0)</t>
+          <t>maa://36660 (93.89), *maa://36701 (64.0)</t>
         </is>
       </c>
     </row>
@@ -3909,7 +3909,7 @@
       </c>
       <c r="C29" s="5" t="inlineStr">
         <is>
-          <t>maa://31694 (97.92)</t>
+          <t>maa://31694 (97.96)</t>
         </is>
       </c>
       <c r="E29" s="4" t="inlineStr">
@@ -3939,7 +3939,7 @@
       </c>
       <c r="K29" s="5" t="inlineStr">
         <is>
-          <t>maa://28432 (93.52), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (66.67)</t>
+          <t>maa://28432 (93.54), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (66.67)</t>
         </is>
       </c>
       <c r="M29" s="4" t="inlineStr">
@@ -4290,7 +4290,7 @@
       </c>
       <c r="G32" s="5" t="inlineStr">
         <is>
-          <t>maa://21895 (97.01), maa://36667 (98.11), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.01), maa://36667 (98.18), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="4" t="inlineStr">
@@ -4442,7 +4442,7 @@
       </c>
       <c r="O33" s="5" t="inlineStr">
         <is>
-          <t>*maa://21956 (79.07), maa://22730 (82.14)</t>
+          <t>*maa://21956 (79.23), maa://22730 (82.14)</t>
         </is>
       </c>
       <c r="Q33" s="4" t="inlineStr">
@@ -4564,7 +4564,7 @@
       </c>
       <c r="S34" s="5" t="inlineStr">
         <is>
-          <t>maa://24526 (93.16)</t>
+          <t>maa://24526 (93.19)</t>
         </is>
       </c>
       <c r="Y34" s="4" t="inlineStr">
@@ -4626,7 +4626,7 @@
       </c>
       <c r="K35" s="5" t="inlineStr">
         <is>
-          <t>maa://41296 (98.15)</t>
+          <t>maa://41296 (98.18)</t>
         </is>
       </c>
       <c r="M35" s="4" t="inlineStr">
@@ -4825,7 +4825,7 @@
       </c>
       <c r="O37" s="5" t="inlineStr">
         <is>
-          <t>maa://21280 (89.13), *maa://21239 (72.73)</t>
+          <t>maa://21280 (89.19), *maa://21239 (72.73)</t>
         </is>
       </c>
       <c r="Q37" s="4" t="inlineStr">
@@ -4952,7 +4952,7 @@
       </c>
       <c r="AE38" s="5" t="inlineStr">
         <is>
-          <t>maa://36697 (84.73)</t>
+          <t>maa://36697 (84.21)</t>
         </is>
       </c>
     </row>
@@ -4969,7 +4969,7 @@
       </c>
       <c r="G39" s="5" t="inlineStr">
         <is>
-          <t>maa://25199 (86.11), maa://36670 (88.06), maa://30434 (87.5), ***maa://25036 (16.0)</t>
+          <t>maa://25199 (86.11), maa://36670 (88.24), maa://30434 (87.5), ***maa://25036 (16.0)</t>
         </is>
       </c>
       <c r="I39" s="4" t="inlineStr">
@@ -5081,7 +5081,7 @@
       </c>
       <c r="O40" s="5" t="inlineStr">
         <is>
-          <t>maa://23278 (95.89), maa://21386 (95.63), maa://36664 (90.24)</t>
+          <t>maa://23278 (95.89), maa://21386 (95.65), maa://36664 (90.48)</t>
         </is>
       </c>
       <c r="Q40" s="4" t="inlineStr">
@@ -5128,7 +5128,7 @@
       </c>
       <c r="O41" s="5" t="inlineStr">
         <is>
-          <t>**maa://35616 (37.93)</t>
+          <t>**maa://35616 (36.67)</t>
         </is>
       </c>
       <c r="Q41" s="4" t="inlineStr">
@@ -5259,7 +5259,7 @@
       </c>
       <c r="G44" s="5" t="inlineStr">
         <is>
-          <t>maa://29768 (97.54), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.55), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="M44" s="4" t="inlineStr">
@@ -5359,7 +5359,7 @@
       </c>
       <c r="G46" s="5" t="inlineStr">
         <is>
-          <t>maa://35931 (92.61)</t>
+          <t>maa://35931 (92.64)</t>
         </is>
       </c>
       <c r="M46" s="4" t="inlineStr">
@@ -5640,7 +5640,7 @@
       </c>
       <c r="G53" s="5" t="inlineStr">
         <is>
-          <t>maa://32534 (93.26), **maa://32434 (36.36)</t>
+          <t>maa://32534 (93.31), **maa://32434 (36.36)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: Auto Update Data (#86)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -720,7 +720,7 @@
       </c>
       <c r="AE2" s="5" t="inlineStr">
         <is>
-          <t>maa://25251 (92.5), ***maa://21730 (17.19), ***maa://39501 (21.43), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.5), ***maa://21730 (17.19), ***maa://39501 (20.0), *maa://36675 (60.0)</t>
         </is>
       </c>
     </row>
@@ -812,7 +812,7 @@
       </c>
       <c r="W3" s="5" t="inlineStr">
         <is>
-          <t>maa://27396 (85.02), maa://27484 (95.74), maa://27480 (82.35)</t>
+          <t>maa://27396 (85.07), maa://27484 (95.74), maa://27480 (82.35)</t>
         </is>
       </c>
       <c r="Y3" s="4" t="inlineStr">
@@ -1392,7 +1392,7 @@
       </c>
       <c r="O8" s="5" t="inlineStr">
         <is>
-          <t>maa://32931 (87.8), *maa://21916 (60.34), maa://23252 (92.31), **maa://22759 (45.45), maa://37496 (100.0)</t>
+          <t>maa://32931 (86.9), *maa://21916 (61.02), maa://23252 (92.31), **maa://22759 (45.45), maa://37496 (100.0)</t>
         </is>
       </c>
       <c r="Q8" s="4" t="inlineStr">
@@ -1499,7 +1499,7 @@
       </c>
       <c r="K9" s="5" t="inlineStr">
         <is>
-          <t>maa://22762 (91.57), *maa://39552 (66.67)</t>
+          <t>maa://22762 (91.57), *maa://39552 (75.0)</t>
         </is>
       </c>
       <c r="M9" s="4" t="inlineStr">
@@ -1514,7 +1514,7 @@
       </c>
       <c r="O9" s="5" t="inlineStr">
         <is>
-          <t>maa://22736 (80.25)</t>
+          <t>maa://22736 (80.49)</t>
         </is>
       </c>
       <c r="Q9" s="4" t="inlineStr">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.19), **maa://32237 (37.84), ***maa://34206 (18.18), ***maa://39951 (18.52), **maa://39243 (33.33)</t>
+          <t>***maa://25695 (19.08), **maa://32237 (37.84), ***maa://34206 (18.18), ***maa://39951 (17.86), **maa://39243 (33.33)</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="S10" s="5" t="inlineStr">
         <is>
-          <t>maa://27395 (96.08), maa://22755 (87.74), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.1), maa://22755 (87.74), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="4" t="inlineStr">
@@ -1788,7 +1788,7 @@
       </c>
       <c r="W11" s="5" t="inlineStr">
         <is>
-          <t>maa://36713 (97.86)</t>
+          <t>maa://36713 (97.87)</t>
         </is>
       </c>
       <c r="Y11" s="4" t="inlineStr">
@@ -1910,7 +1910,7 @@
       </c>
       <c r="W12" s="5" t="inlineStr">
         <is>
-          <t>maa://22753 (91.22), *maa://21485 (76.74), maa://37962 (81.25)</t>
+          <t>maa://22753 (91.33), *maa://21485 (76.74), maa://37962 (81.25)</t>
         </is>
       </c>
       <c r="Y12" s="4" t="inlineStr">
@@ -2062,7 +2062,7 @@
       </c>
       <c r="AE13" s="5" t="inlineStr">
         <is>
-          <t>**maa://22737 (30.6), maa://39883 (88.89), *maa://39885 (73.68)</t>
+          <t>**maa://22737 (30.6), maa://39883 (89.29), *maa://39885 (73.68)</t>
         </is>
       </c>
     </row>
@@ -2124,7 +2124,7 @@
       </c>
       <c r="O14" s="5" t="inlineStr">
         <is>
-          <t>maa://23250 (98.48), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.49), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="4" t="inlineStr">
@@ -2134,12 +2134,12 @@
       </c>
       <c r="R14" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="S14" s="5" t="inlineStr">
         <is>
-          <t>maa://22521 (94.44)</t>
+          <t>maa://22521 (94.44), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="4" t="inlineStr">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>*maa://22743 (76.88), maa://22734 (83.33), *maa://30808 (64.29), ***maa://36048 (12.9)</t>
+          <t>*maa://22743 (76.44), maa://22734 (83.33), *maa://30808 (64.29), ***maa://36048 (12.9)</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr">
@@ -2567,7 +2567,7 @@
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
-          <t>maa://24570 (96.67)</t>
+          <t>maa://24570 (96.69)</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
@@ -2779,7 +2779,7 @@
       </c>
       <c r="AA19" s="5" t="inlineStr">
         <is>
-          <t>*maa://30709 (60.9), *maa://36668 (52.17)</t>
+          <t>*maa://30709 (61.01), *maa://36668 (52.17)</t>
         </is>
       </c>
       <c r="AC19" s="4" t="inlineStr">
@@ -2841,7 +2841,7 @@
       </c>
       <c r="K20" s="5" t="inlineStr">
         <is>
-          <t>maa://41331 (82.93)</t>
+          <t>maa://41331 (84.09)</t>
         </is>
       </c>
       <c r="M20" s="4" t="inlineStr">
@@ -2856,7 +2856,7 @@
       </c>
       <c r="O20" s="5" t="inlineStr">
         <is>
-          <t>maa://37442 (96.55)</t>
+          <t>maa://37442 (96.77)</t>
         </is>
       </c>
       <c r="Q20" s="4" t="inlineStr">
@@ -3038,7 +3038,7 @@
       </c>
       <c r="AE21" s="5" t="inlineStr">
         <is>
-          <t>maa://22524 (94.32), *maa://22432 (74.55)</t>
+          <t>maa://22524 (94.35), *maa://22432 (74.55)</t>
         </is>
       </c>
     </row>
@@ -3070,7 +3070,7 @@
       </c>
       <c r="G22" s="5" t="inlineStr">
         <is>
-          <t>maa://25236 (95.83), **maa://21678 (48.94), **maa://22735 (50.0)</t>
+          <t>maa://25236 (95.89), **maa://21678 (48.94), **maa://22735 (50.0)</t>
         </is>
       </c>
       <c r="I22" s="4" t="inlineStr">
@@ -3207,7 +3207,7 @@
       </c>
       <c r="K23" s="5" t="inlineStr">
         <is>
-          <t>maa://39756 (92.59), maa://39875 (95.83)</t>
+          <t>maa://39756 (92.59), maa://39875 (95.92)</t>
         </is>
       </c>
       <c r="M23" s="4" t="inlineStr">
@@ -3374,7 +3374,7 @@
       </c>
       <c r="W24" s="5" t="inlineStr">
         <is>
-          <t>maa://29988 (86.41), maa://23504 (92.92), **maa://22892 (40.14), *maa://25141 (77.05), maa://36663 (80.7), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.41), maa://23504 (92.94), **maa://22892 (40.14), *maa://25141 (77.05), maa://36663 (80.7), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="4" t="inlineStr">
@@ -3436,7 +3436,7 @@
       </c>
       <c r="G25" s="5" t="inlineStr">
         <is>
-          <t>*maa://29063 (75.56), *maa://25311 (74.19), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (75.74), *maa://25311 (74.19), ***maa://22725 (4.84)</t>
         </is>
       </c>
       <c r="I25" s="4" t="inlineStr">
@@ -3511,7 +3511,7 @@
       </c>
       <c r="AA25" s="5" t="inlineStr">
         <is>
-          <t>maa://31215 (84.15), *maa://24516 (79.07), maa://26001 (88.89)</t>
+          <t>maa://31215 (84.34), *maa://24516 (79.07), maa://26001 (88.89)</t>
         </is>
       </c>
       <c r="AC25" s="4" t="inlineStr">
@@ -3526,7 +3526,7 @@
       </c>
       <c r="AE25" s="5" t="inlineStr">
         <is>
-          <t>maa://20108 (96.12), maa://24621 (96.43), maa://36676 (100.0), maa://22771 (84.62), maa://37772 (100.0)</t>
+          <t>maa://20108 (96.15), maa://24621 (96.43), maa://36676 (100.0), maa://22771 (84.62), maa://37772 (100.0)</t>
         </is>
       </c>
     </row>
@@ -3633,7 +3633,7 @@
       </c>
       <c r="AA26" s="5" t="inlineStr">
         <is>
-          <t>*maa://42235 (78.26)</t>
+          <t>*maa://42235 (80.0)</t>
         </is>
       </c>
       <c r="AC26" s="4" t="inlineStr">
@@ -3787,7 +3787,7 @@
       </c>
       <c r="C28" s="5" t="inlineStr">
         <is>
-          <t>maa://24465 (90.37), maa://25725 (82.28)</t>
+          <t>maa://24465 (90.39), maa://25725 (82.28)</t>
         </is>
       </c>
       <c r="E28" s="4" t="inlineStr">
@@ -3862,7 +3862,7 @@
       </c>
       <c r="W28" s="5" t="inlineStr">
         <is>
-          <t>maa://39929 (86.89), ***maa://39723 (14.71), maa://41749 (82.35)</t>
+          <t>maa://39929 (87.08), ***maa://39723 (14.71), maa://41749 (85.0)</t>
         </is>
       </c>
       <c r="Y28" s="4" t="inlineStr">
@@ -4014,7 +4014,7 @@
       </c>
       <c r="AE29" s="5" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.02), ***maa://34960 (8.7)</t>
+          <t>*maa://24080 (69.11), ***maa://34960 (8.7)</t>
         </is>
       </c>
     </row>
@@ -4106,7 +4106,7 @@
       </c>
       <c r="W30" s="5" t="inlineStr">
         <is>
-          <t>*maa://39477 (75.0)</t>
+          <t>*maa://39477 (77.78)</t>
         </is>
       </c>
       <c r="Y30" s="4" t="inlineStr">
@@ -4183,7 +4183,7 @@
       </c>
       <c r="K31" s="5" t="inlineStr">
         <is>
-          <t>maa://35926 (93.56), maa://36258 (80.52)</t>
+          <t>maa://35926 (93.19), maa://36258 (80.52)</t>
         </is>
       </c>
       <c r="M31" s="4" t="inlineStr">
@@ -4335,7 +4335,7 @@
       </c>
       <c r="S32" s="5" t="inlineStr">
         <is>
-          <t>maa://41108 (89.47), maa://41238 (94.59)</t>
+          <t>maa://41108 (87.5), maa://41238 (94.74)</t>
         </is>
       </c>
       <c r="U32" s="4" t="inlineStr">
@@ -4626,7 +4626,7 @@
       </c>
       <c r="K35" s="5" t="inlineStr">
         <is>
-          <t>maa://41296 (98.18)</t>
+          <t>maa://41296 (98.25)</t>
         </is>
       </c>
       <c r="M35" s="4" t="inlineStr">
@@ -4952,7 +4952,7 @@
       </c>
       <c r="AE38" s="5" t="inlineStr">
         <is>
-          <t>maa://36697 (84.21)</t>
+          <t>maa://36697 (83.7)</t>
         </is>
       </c>
     </row>
@@ -5289,7 +5289,7 @@
       </c>
       <c r="S44" s="5" t="inlineStr">
         <is>
-          <t>maa://39366 (83.33)</t>
+          <t>maa://39366 (84.0)</t>
         </is>
       </c>
     </row>
@@ -5359,7 +5359,7 @@
       </c>
       <c r="G46" s="5" t="inlineStr">
         <is>
-          <t>maa://35931 (92.64)</t>
+          <t>maa://35931 (92.67)</t>
         </is>
       </c>
       <c r="M46" s="4" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#87)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -645,7 +645,7 @@
       </c>
       <c r="K2" s="5" t="inlineStr">
         <is>
-          <t>*maa://24633 (54.97), *maa://30515 (69.7), ***maa://20792 (11.93), *maa://34787 (72.13), maa://39402 (85.19), ***maa://29083 (29.41)</t>
+          <t>*maa://24633 (54.97), *maa://30515 (69.7), *maa://34787 (72.13), ***maa://20792 (11.93), maa://39402 (85.19), ***maa://29083 (29.41)</t>
         </is>
       </c>
       <c r="M2" s="4" t="inlineStr">
@@ -859,7 +859,7 @@
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>maa://24632 (93.28), **maa://24303 (36.36), maa://22499 (85.71), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.33), **maa://24303 (36.36), maa://22499 (85.71), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -1788,7 +1788,7 @@
       </c>
       <c r="W11" s="5" t="inlineStr">
         <is>
-          <t>maa://36713 (97.87)</t>
+          <t>maa://36713 (97.88)</t>
         </is>
       </c>
       <c r="Y11" s="4" t="inlineStr">
@@ -1910,7 +1910,7 @@
       </c>
       <c r="W12" s="5" t="inlineStr">
         <is>
-          <t>maa://22753 (91.33), *maa://21485 (76.74), maa://37962 (81.25)</t>
+          <t>maa://22753 (91.33), *maa://21485 (76.74), maa://37962 (82.35)</t>
         </is>
       </c>
       <c r="Y12" s="4" t="inlineStr">
@@ -1957,7 +1957,7 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>maa://24999 (91.46), maa://36673 (91.8), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.48), maa://36673 (91.8), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr">
@@ -2079,7 +2079,7 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>maa://30764 (86.36)</t>
+          <t>maa://30764 (86.67)</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr">
@@ -2306,7 +2306,7 @@
       </c>
       <c r="AE15" s="5" t="inlineStr">
         <is>
-          <t>maa://21364 (80.68), *maa://22766 (73.0), *maa://36666 (78.46)</t>
+          <t>maa://21364 (80.68), *maa://22766 (73.0), *maa://36666 (77.27)</t>
         </is>
       </c>
     </row>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="G17" s="5" t="inlineStr">
         <is>
-          <t>maa://22430 (88.14), maa://39599 (80.95)</t>
+          <t>maa://22430 (88.14), maa://39599 (81.82)</t>
         </is>
       </c>
       <c r="I17" s="4" t="inlineStr">
@@ -2779,7 +2779,7 @@
       </c>
       <c r="AA19" s="5" t="inlineStr">
         <is>
-          <t>*maa://30709 (61.01), *maa://36668 (52.17)</t>
+          <t>*maa://30709 (61.11), *maa://36668 (52.17)</t>
         </is>
       </c>
       <c r="AC19" s="4" t="inlineStr">
@@ -2841,7 +2841,7 @@
       </c>
       <c r="K20" s="5" t="inlineStr">
         <is>
-          <t>maa://41331 (84.09)</t>
+          <t>maa://41331 (84.44)</t>
         </is>
       </c>
       <c r="M20" s="4" t="inlineStr">
@@ -3207,7 +3207,7 @@
       </c>
       <c r="K23" s="5" t="inlineStr">
         <is>
-          <t>maa://39756 (92.59), maa://39875 (95.92)</t>
+          <t>maa://39756 (92.64), maa://39875 (95.92)</t>
         </is>
       </c>
       <c r="M23" s="4" t="inlineStr">
@@ -3222,7 +3222,7 @@
       </c>
       <c r="O23" s="5" t="inlineStr">
         <is>
-          <t>maa://30587 (91.67), *maa://29748 (75.2), ***maa://29785 (15.15), *maa://37566 (78.95)</t>
+          <t>maa://30587 (91.72), *maa://29748 (75.2), ***maa://29785 (15.15), *maa://37566 (78.95)</t>
         </is>
       </c>
       <c r="Q23" s="4" t="inlineStr">
@@ -3374,7 +3374,7 @@
       </c>
       <c r="W24" s="5" t="inlineStr">
         <is>
-          <t>maa://29988 (86.41), maa://23504 (92.94), **maa://22892 (40.14), *maa://25141 (77.05), maa://36663 (80.7), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.47), maa://23504 (92.94), **maa://22892 (40.14), *maa://25141 (77.05), maa://36663 (80.7), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="4" t="inlineStr">
@@ -3511,7 +3511,7 @@
       </c>
       <c r="AA25" s="5" t="inlineStr">
         <is>
-          <t>maa://31215 (84.34), *maa://24516 (79.07), maa://26001 (88.89)</t>
+          <t>maa://31215 (84.34), *maa://24516 (79.07), maa://26001 (87.27)</t>
         </is>
       </c>
       <c r="AC25" s="4" t="inlineStr">
@@ -3633,7 +3633,7 @@
       </c>
       <c r="AA26" s="5" t="inlineStr">
         <is>
-          <t>*maa://42235 (80.0)</t>
+          <t>maa://42235 (80.77)</t>
         </is>
       </c>
       <c r="AC26" s="4" t="inlineStr">
@@ -3787,7 +3787,7 @@
       </c>
       <c r="C28" s="5" t="inlineStr">
         <is>
-          <t>maa://24465 (90.39), maa://25725 (82.28)</t>
+          <t>maa://24465 (90.4), maa://25725 (82.28)</t>
         </is>
       </c>
       <c r="E28" s="4" t="inlineStr">
@@ -3847,7 +3847,7 @@
       </c>
       <c r="S28" s="5" t="inlineStr">
         <is>
-          <t>maa://23263 (94.32), *maa://29765 (61.19)</t>
+          <t>maa://23263 (94.32), *maa://29765 (60.29)</t>
         </is>
       </c>
       <c r="U28" s="4" t="inlineStr">
@@ -3862,7 +3862,7 @@
       </c>
       <c r="W28" s="5" t="inlineStr">
         <is>
-          <t>maa://39929 (87.08), ***maa://39723 (14.71), maa://41749 (85.0)</t>
+          <t>maa://39929 (87.14), ***maa://39723 (14.71), maa://41749 (85.0)</t>
         </is>
       </c>
       <c r="Y28" s="4" t="inlineStr">
@@ -3892,7 +3892,7 @@
       </c>
       <c r="AE28" s="5" t="inlineStr">
         <is>
-          <t>maa://36660 (93.89), *maa://36701 (64.0)</t>
+          <t>maa://36660 (93.54), *maa://36701 (64.0)</t>
         </is>
       </c>
     </row>
@@ -4014,7 +4014,7 @@
       </c>
       <c r="AE29" s="5" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.11), ***maa://34960 (8.7)</t>
+          <t>*maa://24080 (68.92), ***maa://34960 (8.7)</t>
         </is>
       </c>
     </row>
@@ -4106,7 +4106,7 @@
       </c>
       <c r="W30" s="5" t="inlineStr">
         <is>
-          <t>*maa://39477 (77.78)</t>
+          <t>*maa://39477 (80.0)</t>
         </is>
       </c>
       <c r="Y30" s="4" t="inlineStr">
@@ -4335,7 +4335,7 @@
       </c>
       <c r="S32" s="5" t="inlineStr">
         <is>
-          <t>maa://41108 (87.5), maa://41238 (94.74)</t>
+          <t>maa://41108 (87.8), maa://41238 (94.74)</t>
         </is>
       </c>
       <c r="U32" s="4" t="inlineStr">
@@ -4626,7 +4626,7 @@
       </c>
       <c r="K35" s="5" t="inlineStr">
         <is>
-          <t>maa://41296 (98.25)</t>
+          <t>maa://41296 (98.28)</t>
         </is>
       </c>
       <c r="M35" s="4" t="inlineStr">
@@ -5081,7 +5081,7 @@
       </c>
       <c r="O40" s="5" t="inlineStr">
         <is>
-          <t>maa://23278 (95.89), maa://21386 (95.65), maa://36664 (90.48)</t>
+          <t>maa://23278 (95.89), maa://21386 (95.65), maa://36664 (90.7)</t>
         </is>
       </c>
       <c r="Q40" s="4" t="inlineStr">
@@ -5289,7 +5289,7 @@
       </c>
       <c r="S44" s="5" t="inlineStr">
         <is>
-          <t>maa://39366 (84.0)</t>
+          <t>maa://39366 (84.62)</t>
         </is>
       </c>
     </row>
@@ -5304,12 +5304,12 @@
       </c>
       <c r="F45" s="4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G45" s="5" t="inlineStr">
         <is>
-          <t>maa://21229 (85.47), maa://30807 (95.08), *maa://22767 (52.94), ***maa://20796 (13.79)</t>
+          <t>maa://21229 (85.47), maa://30807 (95.08), *maa://22767 (52.94), ***maa://20796 (13.79), maa://42459 (100.0)</t>
         </is>
       </c>
       <c r="M45" s="4" t="inlineStr">
@@ -5324,7 +5324,7 @@
       </c>
       <c r="O45" s="5" t="inlineStr">
         <is>
-          <t>*maa://36237 (54.55)</t>
+          <t>*maa://36237 (58.33)</t>
         </is>
       </c>
       <c r="Q45" s="4" t="inlineStr">
@@ -5339,7 +5339,7 @@
       </c>
       <c r="S45" s="5" t="inlineStr">
         <is>
-          <t>**maa://39364 (50.0)</t>
+          <t>**maa://39364 (45.45)</t>
         </is>
       </c>
     </row>
@@ -5359,7 +5359,7 @@
       </c>
       <c r="G46" s="5" t="inlineStr">
         <is>
-          <t>maa://35931 (92.67)</t>
+          <t>maa://35931 (92.27)</t>
         </is>
       </c>
       <c r="M46" s="4" t="inlineStr">
@@ -5674,7 +5674,7 @@
       </c>
       <c r="G55" s="5" t="inlineStr">
         <is>
-          <t>maa://32532 (91.93)</t>
+          <t>maa://32532 (91.96)</t>
         </is>
       </c>
     </row>
@@ -5725,7 +5725,7 @@
       </c>
       <c r="G58" s="5" t="inlineStr">
         <is>
-          <t>*maa://37964 (63.16)</t>
+          <t>*maa://37964 (60.0)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: Auto Update Data (#88)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -615,7 +615,7 @@
       </c>
       <c r="C2" s="5" t="inlineStr">
         <is>
-          <t>maa://24702 (94.1), maa://25390 (96.6), maa://36681 (90.77)</t>
+          <t>maa://24702 (94.12), maa://25390 (96.19), maa://36681 (88.24)</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
@@ -645,7 +645,7 @@
       </c>
       <c r="K2" s="5" t="inlineStr">
         <is>
-          <t>*maa://24633 (54.97), *maa://30515 (69.7), *maa://34787 (72.13), ***maa://20792 (11.93), maa://39402 (85.19), ***maa://29083 (29.41)</t>
+          <t>*maa://24633 (54.97), *maa://30515 (69.7), *maa://34787 (72.13), ***maa://20792 (11.93), maa://39402 (86.21), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="4" t="inlineStr">
@@ -675,7 +675,7 @@
       </c>
       <c r="S2" s="5" t="inlineStr">
         <is>
-          <t>maa://22742 (92.2), *maa://20791 (62.32)</t>
+          <t>maa://22742 (92.25), *maa://20791 (62.32)</t>
         </is>
       </c>
       <c r="U2" s="4" t="inlineStr">
@@ -705,7 +705,7 @@
       </c>
       <c r="AA2" s="5" t="inlineStr">
         <is>
-          <t>maa://21246 (91.26), maa://36684 (98.63), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.26), maa://36684 (98.68), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="4" t="inlineStr">
@@ -720,7 +720,7 @@
       </c>
       <c r="AE2" s="5" t="inlineStr">
         <is>
-          <t>maa://25251 (92.5), ***maa://21730 (17.19), ***maa://39501 (20.0), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.77), ***maa://21730 (17.19), ***maa://39501 (18.75), *maa://36675 (60.0)</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>maa://36987 (95.65), maa://40192 (100.0), maa://39849 (100.0)</t>
+          <t>maa://36987 (93.62), maa://40192 (95.65), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -752,7 +752,7 @@
       </c>
       <c r="G3" s="5" t="inlineStr">
         <is>
-          <t>maa://21247 (98.29), *maa://22748 (75.0)</t>
+          <t>maa://21247 (98.31), *maa://22748 (75.0)</t>
         </is>
       </c>
       <c r="I3" s="4" t="inlineStr">
@@ -767,7 +767,7 @@
       </c>
       <c r="K3" s="5" t="inlineStr">
         <is>
-          <t>*maa://22880 (69.23), maa://20276 (82.86), *maa://22749 (66.67)</t>
+          <t>*maa://22880 (70.0), maa://20276 (83.33), *maa://22749 (66.67)</t>
         </is>
       </c>
       <c r="M3" s="4" t="inlineStr">
@@ -782,7 +782,7 @@
       </c>
       <c r="O3" s="5" t="inlineStr">
         <is>
-          <t>maa://21249 (95.17), maa://26254 (95.24)</t>
+          <t>maa://21249 (95.22), maa://26254 (95.65)</t>
         </is>
       </c>
       <c r="Q3" s="4" t="inlineStr">
@@ -797,7 +797,7 @@
       </c>
       <c r="S3" s="5" t="inlineStr">
         <is>
-          <t>maa://24617 (88.35), **maa://20790 (43.94), ***maa://37170 (20.0)</t>
+          <t>maa://24617 (88.46), **maa://20790 (43.94), ***maa://37170 (20.0)</t>
         </is>
       </c>
       <c r="U3" s="4" t="inlineStr">
@@ -812,7 +812,7 @@
       </c>
       <c r="W3" s="5" t="inlineStr">
         <is>
-          <t>maa://27396 (85.07), maa://27484 (95.74), maa://27480 (82.35)</t>
+          <t>maa://27396 (85.37), maa://27484 (95.79), maa://27480 (82.35)</t>
         </is>
       </c>
       <c r="Y3" s="4" t="inlineStr">
@@ -842,7 +842,7 @@
       </c>
       <c r="AE3" s="5" t="inlineStr">
         <is>
-          <t>*maa://21289 (70.0)</t>
+          <t>*maa://21289 (71.43)</t>
         </is>
       </c>
     </row>
@@ -859,7 +859,7 @@
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>maa://24632 (93.33), **maa://24303 (36.36), maa://22499 (85.71), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.43), **maa://24303 (36.36), maa://22499 (85.71), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -919,7 +919,7 @@
       </c>
       <c r="S4" s="5" t="inlineStr">
         <is>
-          <t>maa://32509 (98.8), maa://22754 (91.67), maa://27295 (80.39), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (97.7), maa://22754 (91.67), maa://27295 (80.77), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="4" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="W4" s="5" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.54), ***maa://31785 (19.47), ***maa://36683 (26.67)</t>
+          <t>**maa://32495 (47.01), ***maa://31785 (20.87), ***maa://36683 (26.67)</t>
         </is>
       </c>
       <c r="Y4" s="4" t="inlineStr">
@@ -964,7 +964,7 @@
       </c>
       <c r="AE4" s="5" t="inlineStr">
         <is>
-          <t>*maa://30062 (61.9), ***maa://26209 (13.04), *maa://39394 (78.57)</t>
+          <t>*maa://30062 (61.36), ***maa://26209 (13.04), *maa://39394 (73.33)</t>
         </is>
       </c>
     </row>
@@ -981,7 +981,7 @@
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>maa://21245 (82.29), maa://22744 (83.33)</t>
+          <t>maa://21245 (82.05), maa://22744 (83.33)</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="K5" s="5" t="inlineStr">
         <is>
-          <t>maa://22757 (81.48)</t>
+          <t>*maa://22757 (78.57)</t>
         </is>
       </c>
       <c r="M5" s="4" t="inlineStr">
@@ -1026,7 +1026,7 @@
       </c>
       <c r="O5" s="5" t="inlineStr">
         <is>
-          <t>maa://21919 (95.56), maa://21281 (92.31)</t>
+          <t>maa://21919 (95.74), maa://21281 (92.31)</t>
         </is>
       </c>
       <c r="Q5" s="4" t="inlineStr">
@@ -1071,7 +1071,7 @@
       </c>
       <c r="AA5" s="5" t="inlineStr">
         <is>
-          <t>*maa://29863 (75.0), ***maa://22752 (13.33), **maa://26013 (42.86)</t>
+          <t>*maa://29863 (72.41), ***maa://22752 (13.33), **maa://26013 (42.86)</t>
         </is>
       </c>
       <c r="AC5" s="4" t="inlineStr">
@@ -1103,7 +1103,7 @@
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>maa://42407 (88.89)</t>
+          <t>maa://42407 (94.12)</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -1118,7 +1118,7 @@
       </c>
       <c r="G6" s="5" t="inlineStr">
         <is>
-          <t>maa://24370 (96.15)</t>
+          <t>maa://24370 (96.3)</t>
         </is>
       </c>
       <c r="I6" s="4" t="inlineStr">
@@ -1133,7 +1133,7 @@
       </c>
       <c r="K6" s="5" t="inlineStr">
         <is>
-          <t>maa://24839 (99.21)</t>
+          <t>maa://24839 (99.22)</t>
         </is>
       </c>
       <c r="M6" s="4" t="inlineStr">
@@ -1148,7 +1148,7 @@
       </c>
       <c r="O6" s="5" t="inlineStr">
         <is>
-          <t>maa://31836 (93.33), maa://30381 (100.0)</t>
+          <t>maa://31836 (88.24), maa://30381 (91.67)</t>
         </is>
       </c>
       <c r="Q6" s="4" t="inlineStr">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="S6" s="5" t="inlineStr">
         <is>
-          <t>*maa://37411 (77.78)</t>
+          <t>maa://37411 (81.82)</t>
         </is>
       </c>
       <c r="U6" s="4" t="inlineStr">
@@ -1193,7 +1193,7 @@
       </c>
       <c r="AA6" s="5" t="inlineStr">
         <is>
-          <t>maa://22739 (91.67)</t>
+          <t>maa://22739 (92.0)</t>
         </is>
       </c>
       <c r="AC6" s="4" t="inlineStr">
@@ -1208,7 +1208,7 @@
       </c>
       <c r="AE6" s="5" t="inlineStr">
         <is>
-          <t>*maa://33152 (60.61), ***maa://22770 (28.57)</t>
+          <t>*maa://33152 (61.76), ***maa://22770 (28.57)</t>
         </is>
       </c>
     </row>
@@ -1225,7 +1225,7 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>maa://21955 (92.86)</t>
+          <t>maa://21955 (93.33)</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -1255,7 +1255,7 @@
       </c>
       <c r="K7" s="5" t="inlineStr">
         <is>
-          <t>maa://28624 (91.55), maa://24957 (97.44)</t>
+          <t>maa://28624 (92.0), maa://24957 (97.56)</t>
         </is>
       </c>
       <c r="M7" s="4" t="inlineStr">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="O7" s="5" t="inlineStr">
         <is>
-          <t>maa://22750 (97.14)</t>
+          <t>maa://22750 (94.44)</t>
         </is>
       </c>
       <c r="Q7" s="4" t="inlineStr">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="S7" s="5" t="inlineStr">
         <is>
-          <t>maa://21291 (89.47)</t>
+          <t>maa://21291 (89.74)</t>
         </is>
       </c>
       <c r="U7" s="4" t="inlineStr">
@@ -1300,7 +1300,7 @@
       </c>
       <c r="W7" s="5" t="inlineStr">
         <is>
-          <t>maa://22399 (94.66), *maa://22758 (70.37)</t>
+          <t>maa://22399 (94.74), *maa://22758 (70.37)</t>
         </is>
       </c>
       <c r="Y7" s="4" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="AE7" s="5" t="inlineStr">
         <is>
-          <t>*maa://26191 (68.49), *maa://36671 (72.73), maa://42530 (100.0)</t>
+          <t>*maa://26191 (68.49), *maa://36671 (72.73), *maa://42530 (75.0)</t>
         </is>
       </c>
     </row>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>*maa://21476 (69.77), **maa://39431 (50.0), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (70.45), **maa://39431 (42.86), *maa://37551 (57.14)</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="G8" s="5" t="inlineStr">
         <is>
-          <t>*maa://24371 (53.03)</t>
+          <t>*maa://24371 (52.24)</t>
         </is>
       </c>
       <c r="I8" s="4" t="inlineStr">
@@ -1392,7 +1392,7 @@
       </c>
       <c r="O8" s="5" t="inlineStr">
         <is>
-          <t>maa://32931 (86.9), *maa://21916 (61.02), maa://23252 (92.31), **maa://22759 (45.45), maa://37496 (100.0)</t>
+          <t>maa://32931 (87.21), *maa://21916 (60.0), maa://23252 (92.31), **maa://22759 (45.45), maa://37496 (100.0)</t>
         </is>
       </c>
       <c r="Q8" s="4" t="inlineStr">
@@ -1422,7 +1422,7 @@
       </c>
       <c r="W8" s="5" t="inlineStr">
         <is>
-          <t>maa://21411 (96.07)</t>
+          <t>maa://21411 (95.79)</t>
         </is>
       </c>
       <c r="Y8" s="4" t="inlineStr">
@@ -1437,7 +1437,7 @@
       </c>
       <c r="AA8" s="5" t="inlineStr">
         <is>
-          <t>maa://25389 (88.89)</t>
+          <t>maa://25389 (89.66)</t>
         </is>
       </c>
       <c r="AC8" s="4" t="inlineStr">
@@ -1452,7 +1452,7 @@
       </c>
       <c r="AE8" s="5" t="inlineStr">
         <is>
-          <t>*maa://24479 (76.71), *maa://21990 (53.85)</t>
+          <t>*maa://24479 (77.33), *maa://21990 (53.85)</t>
         </is>
       </c>
     </row>
@@ -1499,7 +1499,7 @@
       </c>
       <c r="K9" s="5" t="inlineStr">
         <is>
-          <t>maa://22762 (91.57), *maa://39552 (75.0)</t>
+          <t>maa://22762 (91.57), maa://39552 (85.71)</t>
         </is>
       </c>
       <c r="M9" s="4" t="inlineStr">
@@ -1514,7 +1514,7 @@
       </c>
       <c r="O9" s="5" t="inlineStr">
         <is>
-          <t>maa://22736 (80.49)</t>
+          <t>maa://22736 (80.95)</t>
         </is>
       </c>
       <c r="Q9" s="4" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="S9" s="5" t="inlineStr">
         <is>
-          <t>**maa://22866 (30.77), maa://26222 (97.37)</t>
+          <t>**maa://22866 (30.77), maa://26222 (97.5)</t>
         </is>
       </c>
       <c r="U9" s="4" t="inlineStr">
@@ -1544,7 +1544,7 @@
       </c>
       <c r="W9" s="5" t="inlineStr">
         <is>
-          <t>maa://26223 (97.0)</t>
+          <t>maa://26223 (97.09)</t>
         </is>
       </c>
       <c r="Y9" s="4" t="inlineStr">
@@ -1559,7 +1559,7 @@
       </c>
       <c r="AA9" s="5" t="inlineStr">
         <is>
-          <t>maa://28711 (88.1), ***maa://22740 (5.88), **maa://27377 (46.15), ***maa://25174 (20.0), **maa://39938 (43.75), maa://40166 (100.0)</t>
+          <t>maa://28711 (88.37), ***maa://22740 (5.88), **maa://27377 (46.15), ***maa://25174 (20.0), **maa://39938 (41.18), maa://40166 (100.0)</t>
         </is>
       </c>
       <c r="AC9" s="4" t="inlineStr">
@@ -1574,7 +1574,7 @@
       </c>
       <c r="AE9" s="5" t="inlineStr">
         <is>
-          <t>maa://26206 (89.29), **maa://22865 (45.65)</t>
+          <t>maa://26206 (90.11), **maa://22865 (47.92)</t>
         </is>
       </c>
     </row>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.08), **maa://32237 (37.84), ***maa://34206 (18.18), ***maa://39951 (17.86), **maa://39243 (33.33)</t>
+          <t>***maa://25695 (18.97), **maa://32237 (37.84), ***maa://34206 (18.18), ***maa://39951 (16.13), **maa://39243 (33.33)</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="G10" s="5" t="inlineStr">
         <is>
-          <t>maa://32651 (100.0)</t>
+          <t>maa://32651 (92.86)</t>
         </is>
       </c>
       <c r="I10" s="4" t="inlineStr">
@@ -1636,7 +1636,7 @@
       </c>
       <c r="O10" s="5" t="inlineStr">
         <is>
-          <t>maa://28977 (94.74), *maa://23264 (62.96), maa://36669 (87.5)</t>
+          <t>maa://28977 (93.59), *maa://23264 (61.82), maa://36669 (84.62)</t>
         </is>
       </c>
       <c r="Q10" s="4" t="inlineStr">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="S10" s="5" t="inlineStr">
         <is>
-          <t>maa://27395 (96.1), maa://22755 (87.74), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.18), maa://22755 (86.92), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="4" t="inlineStr">
@@ -1666,7 +1666,7 @@
       </c>
       <c r="W10" s="5" t="inlineStr">
         <is>
-          <t>maa://22301 (97.42), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.45), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="4" t="inlineStr">
@@ -1696,7 +1696,7 @@
       </c>
       <c r="AE10" s="5" t="inlineStr">
         <is>
-          <t>*maa://25021 (56.16), *maa://22733 (58.62), maa://22761 (100.0)</t>
+          <t>*maa://25021 (56.0), *maa://22733 (60.0), maa://22761 (100.0)</t>
         </is>
       </c>
     </row>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C11" s="5" t="inlineStr">
         <is>
-          <t>maa://36707 (99.64)</t>
+          <t>maa://36707 (99.66)</t>
         </is>
       </c>
       <c r="E11" s="4" t="inlineStr">
@@ -1788,7 +1788,7 @@
       </c>
       <c r="W11" s="5" t="inlineStr">
         <is>
-          <t>maa://36713 (97.88)</t>
+          <t>maa://36713 (97.92)</t>
         </is>
       </c>
       <c r="Y11" s="4" t="inlineStr">
@@ -1818,7 +1818,7 @@
       </c>
       <c r="AE11" s="5" t="inlineStr">
         <is>
-          <t>maa://31203 (94.44), ***maa://24394 (19.23)</t>
+          <t>maa://31203 (94.74), ***maa://24394 (19.23)</t>
         </is>
       </c>
     </row>
@@ -1850,7 +1850,7 @@
       </c>
       <c r="G12" s="5" t="inlineStr">
         <is>
-          <t>maa://21867 (90.07)</t>
+          <t>maa://21867 (90.2)</t>
         </is>
       </c>
       <c r="I12" s="4" t="inlineStr">
@@ -1910,7 +1910,7 @@
       </c>
       <c r="W12" s="5" t="inlineStr">
         <is>
-          <t>maa://22753 (91.33), *maa://21485 (76.74), maa://37962 (82.35)</t>
+          <t>maa://22753 (91.5), *maa://21485 (76.92), maa://37962 (83.33)</t>
         </is>
       </c>
       <c r="Y12" s="4" t="inlineStr">
@@ -1925,7 +1925,7 @@
       </c>
       <c r="AA12" s="5" t="inlineStr">
         <is>
-          <t>maa://23669 (95.51), maa://36677 (92.5), maa://39872 (85.71)</t>
+          <t>maa://23669 (95.51), maa://36677 (92.5), maa://39872 (86.67)</t>
         </is>
       </c>
       <c r="AC12" s="4" t="inlineStr">
@@ -1940,7 +1940,7 @@
       </c>
       <c r="AE12" s="5" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.63), *maa://20106 (63.64), *maa://22769 (62.96)</t>
+          <t>*maa://28932 (78.15), *maa://20106 (63.64), *maa://22769 (62.96)</t>
         </is>
       </c>
     </row>
@@ -1957,7 +1957,7 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>maa://24999 (91.48), maa://36673 (91.8), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.43), maa://36673 (92.06), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr">
@@ -1972,7 +1972,7 @@
       </c>
       <c r="G13" s="5" t="inlineStr">
         <is>
-          <t>*maa://21248 (75.12), **maa://22728 (47.62)</t>
+          <t>*maa://21248 (74.88), **maa://22728 (46.51)</t>
         </is>
       </c>
       <c r="I13" s="4" t="inlineStr">
@@ -2002,7 +2002,7 @@
       </c>
       <c r="O13" s="5" t="inlineStr">
         <is>
-          <t>maa://22676 (91.84), *maa://22583 (75.41), *maa://22500 (55.81)</t>
+          <t>maa://22676 (92.08), *maa://22583 (75.41), *maa://22500 (55.81)</t>
         </is>
       </c>
       <c r="Q13" s="4" t="inlineStr">
@@ -2032,7 +2032,7 @@
       </c>
       <c r="W13" s="5" t="inlineStr">
         <is>
-          <t>*maa://34957 (76.6), *maa://22768 (51.61)</t>
+          <t>*maa://34957 (77.36), *maa://22768 (51.61)</t>
         </is>
       </c>
       <c r="Y13" s="4" t="inlineStr">
@@ -2062,7 +2062,7 @@
       </c>
       <c r="AE13" s="5" t="inlineStr">
         <is>
-          <t>**maa://22737 (30.6), maa://39883 (89.29), *maa://39885 (73.68)</t>
+          <t>**maa://22737 (30.6), maa://39883 (90.62), *maa://39885 (70.0)</t>
         </is>
       </c>
     </row>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>maa://30764 (86.67)</t>
+          <t>maa://30764 (87.23)</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr">
@@ -2109,7 +2109,7 @@
       </c>
       <c r="K14" s="5" t="inlineStr">
         <is>
-          <t>maa://26245 (96.12), maa://21288 (96.21), maa://36682 (100.0), maa://39841 (93.33)</t>
+          <t>maa://26245 (96.12), maa://21288 (96.21), maa://36682 (100.0), maa://39841 (93.62)</t>
         </is>
       </c>
       <c r="M14" s="4" t="inlineStr">
@@ -2124,7 +2124,7 @@
       </c>
       <c r="O14" s="5" t="inlineStr">
         <is>
-          <t>maa://23250 (98.49), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.52), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="4" t="inlineStr">
@@ -2139,7 +2139,7 @@
       </c>
       <c r="S14" s="5" t="inlineStr">
         <is>
-          <t>maa://22521 (94.44), maa://42751 (100.0)</t>
+          <t>maa://22521 (94.51), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="4" t="inlineStr">
@@ -2154,7 +2154,7 @@
       </c>
       <c r="W14" s="5" t="inlineStr">
         <is>
-          <t>maa://37468 (92.86)</t>
+          <t>maa://37468 (87.5)</t>
         </is>
       </c>
       <c r="Y14" s="4" t="inlineStr">
@@ -2169,7 +2169,7 @@
       </c>
       <c r="AA14" s="5" t="inlineStr">
         <is>
-          <t>maa://22764 (96.43)</t>
+          <t>maa://22764 (96.61)</t>
         </is>
       </c>
       <c r="AC14" s="4" t="inlineStr">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>*maa://22743 (76.44), maa://22734 (83.33), *maa://30808 (64.29), ***maa://36048 (12.9)</t>
+          <t>*maa://22743 (77.09), maa://22734 (83.48), *maa://30808 (64.41), ***maa://36048 (12.5)</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr">
@@ -2216,7 +2216,7 @@
       </c>
       <c r="G15" s="5" t="inlineStr">
         <is>
-          <t>maa://24304 (88.11), maa://21478 (91.18)</t>
+          <t>maa://24304 (88.24), maa://21478 (91.18)</t>
         </is>
       </c>
       <c r="I15" s="4" t="inlineStr">
@@ -2231,7 +2231,7 @@
       </c>
       <c r="K15" s="5" t="inlineStr">
         <is>
-          <t>*maa://21334 (52.0)</t>
+          <t>*maa://21334 (51.85)</t>
         </is>
       </c>
       <c r="M15" s="4" t="inlineStr">
@@ -2246,7 +2246,7 @@
       </c>
       <c r="O15" s="5" t="inlineStr">
         <is>
-          <t>maa://24762 (89.58), *maa://22727 (70.0)</t>
+          <t>maa://24762 (89.66), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="4" t="inlineStr">
@@ -2261,7 +2261,7 @@
       </c>
       <c r="S15" s="5" t="inlineStr">
         <is>
-          <t>maa://23892 (98.63)</t>
+          <t>maa://23892 (98.65)</t>
         </is>
       </c>
       <c r="U15" s="4" t="inlineStr">
@@ -2276,7 +2276,7 @@
       </c>
       <c r="W15" s="5" t="inlineStr">
         <is>
-          <t>*maa://38786 (75.0)</t>
+          <t>*maa://38786 (80.0)</t>
         </is>
       </c>
       <c r="Y15" s="4" t="inlineStr">
@@ -2306,7 +2306,7 @@
       </c>
       <c r="AE15" s="5" t="inlineStr">
         <is>
-          <t>maa://21364 (80.68), *maa://22766 (73.0), *maa://36666 (77.27)</t>
+          <t>maa://21364 (80.68), *maa://22766 (72.12), *maa://36666 (77.61)</t>
         </is>
       </c>
     </row>
@@ -2323,7 +2323,7 @@
       </c>
       <c r="C16" s="5" t="inlineStr">
         <is>
-          <t>maa://21441 (96.17), maa://36679 (91.43), maa://37650 (95.45)</t>
+          <t>maa://21441 (96.17), maa://36679 (91.43), maa://37650 (96.3)</t>
         </is>
       </c>
       <c r="E16" s="4" t="inlineStr">
@@ -2368,7 +2368,7 @@
       </c>
       <c r="O16" s="5" t="inlineStr">
         <is>
-          <t>maa://28504 (91.84)</t>
+          <t>maa://28504 (90.38)</t>
         </is>
       </c>
       <c r="Q16" s="4" t="inlineStr">
@@ -2383,7 +2383,7 @@
       </c>
       <c r="S16" s="5" t="inlineStr">
         <is>
-          <t>maa://22729 (95.17), *maa://28648 (69.09), *maa://36674 (80.0)</t>
+          <t>maa://22729 (95.17), *maa://28648 (69.64), maa://36674 (81.25)</t>
         </is>
       </c>
       <c r="U16" s="4" t="inlineStr">
@@ -2398,7 +2398,7 @@
       </c>
       <c r="W16" s="5" t="inlineStr">
         <is>
-          <t>maa://28501 (97.47), maa://28051 (95.83)</t>
+          <t>maa://28501 (97.62), maa://28051 (95.83)</t>
         </is>
       </c>
       <c r="Y16" s="4" t="inlineStr">
@@ -2413,7 +2413,7 @@
       </c>
       <c r="AA16" s="5" t="inlineStr">
         <is>
-          <t>maa://26228 (96.15)</t>
+          <t>maa://26228 (95.06)</t>
         </is>
       </c>
       <c r="AC16" s="4" t="inlineStr">
@@ -2428,7 +2428,7 @@
       </c>
       <c r="AE16" s="5" t="inlineStr">
         <is>
-          <t>*maa://23911 (62.37), maa://27755 (91.89)</t>
+          <t>*maa://23911 (63.16), maa://27755 (92.11)</t>
         </is>
       </c>
     </row>
@@ -2445,7 +2445,7 @@
       </c>
       <c r="C17" s="5" t="inlineStr">
         <is>
-          <t>maa://21624 (81.25)</t>
+          <t>maa://21624 (81.82)</t>
         </is>
       </c>
       <c r="E17" s="4" t="inlineStr">
@@ -2460,7 +2460,7 @@
       </c>
       <c r="G17" s="5" t="inlineStr">
         <is>
-          <t>maa://22430 (88.14), maa://39599 (81.82)</t>
+          <t>maa://22430 (88.14), maa://39599 (84.0)</t>
         </is>
       </c>
       <c r="I17" s="4" t="inlineStr">
@@ -2490,7 +2490,7 @@
       </c>
       <c r="O17" s="5" t="inlineStr">
         <is>
-          <t>maa://23890 (81.25), *maa://24940 (69.23)</t>
+          <t>maa://23890 (80.41), *maa://24940 (66.67)</t>
         </is>
       </c>
       <c r="Q17" s="4" t="inlineStr">
@@ -2505,7 +2505,7 @@
       </c>
       <c r="S17" s="5" t="inlineStr">
         <is>
-          <t>***maa://42324 (28.57)</t>
+          <t>**maa://42324 (30.77)</t>
         </is>
       </c>
       <c r="U17" s="4" t="inlineStr">
@@ -2567,7 +2567,7 @@
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
-          <t>maa://24570 (96.69)</t>
+          <t>maa://24570 (96.79)</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="G18" s="5" t="inlineStr">
         <is>
-          <t>maa://24421 (90.23)</t>
+          <t>maa://24421 (90.37)</t>
         </is>
       </c>
       <c r="I18" s="4" t="inlineStr">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="K18" s="5" t="inlineStr">
         <is>
-          <t>maa://22466 (88.55), *maa://22732 (51.85)</t>
+          <t>maa://22466 (88.72), *maa://22732 (51.22)</t>
         </is>
       </c>
       <c r="M18" s="4" t="inlineStr">
@@ -2642,7 +2642,7 @@
       </c>
       <c r="W18" s="5" t="inlineStr">
         <is>
-          <t>maa://21917 (97.5), maa://22741 (83.33)</t>
+          <t>maa://21917 (97.53), maa://22741 (83.33)</t>
         </is>
       </c>
       <c r="Y18" s="4" t="inlineStr">
@@ -2657,7 +2657,7 @@
       </c>
       <c r="AA18" s="5" t="inlineStr">
         <is>
-          <t>maa://24393 (97.14)</t>
+          <t>maa://24393 (97.3)</t>
         </is>
       </c>
       <c r="AC18" s="4" t="inlineStr">
@@ -2672,7 +2672,7 @@
       </c>
       <c r="AE18" s="5" t="inlineStr">
         <is>
-          <t>*maa://24313 (57.62), **maa://29784 (46.15)</t>
+          <t>*maa://24313 (57.89), **maa://29784 (44.44)</t>
         </is>
       </c>
     </row>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="S19" s="5" t="inlineStr">
         <is>
-          <t>maa://24386 (98.81)</t>
+          <t>maa://24386 (98.84)</t>
         </is>
       </c>
       <c r="U19" s="4" t="inlineStr">
@@ -2779,7 +2779,7 @@
       </c>
       <c r="AA19" s="5" t="inlineStr">
         <is>
-          <t>*maa://30709 (61.11), *maa://36668 (52.17)</t>
+          <t>*maa://30709 (61.72), *maa://36668 (52.17)</t>
         </is>
       </c>
       <c r="AC19" s="4" t="inlineStr">
@@ -2794,7 +2794,7 @@
       </c>
       <c r="AE19" s="5" t="inlineStr">
         <is>
-          <t>*maa://21663 (61.02)</t>
+          <t>*maa://21663 (61.67)</t>
         </is>
       </c>
     </row>
@@ -2811,7 +2811,7 @@
       </c>
       <c r="C20" s="5" t="inlineStr">
         <is>
-          <t>maa://21432 (90.7), maa://25198 (93.62), **maa://20795 (49.59), maa://36680 (100.0)</t>
+          <t>maa://21432 (90.91), maa://25198 (93.68), *maa://20795 (50.4), maa://36680 (100.0)</t>
         </is>
       </c>
       <c r="E20" s="4" t="inlineStr">
@@ -2826,7 +2826,7 @@
       </c>
       <c r="G20" s="5" t="inlineStr">
         <is>
-          <t>maa://22864 (88.55)</t>
+          <t>maa://22864 (88.81)</t>
         </is>
       </c>
       <c r="I20" s="4" t="inlineStr">
@@ -2841,7 +2841,7 @@
       </c>
       <c r="K20" s="5" t="inlineStr">
         <is>
-          <t>maa://41331 (84.44)</t>
+          <t>maa://41331 (81.82)</t>
         </is>
       </c>
       <c r="M20" s="4" t="inlineStr">
@@ -2856,7 +2856,7 @@
       </c>
       <c r="O20" s="5" t="inlineStr">
         <is>
-          <t>maa://37442 (96.77)</t>
+          <t>maa://37442 (96.88)</t>
         </is>
       </c>
       <c r="Q20" s="4" t="inlineStr">
@@ -2871,7 +2871,7 @@
       </c>
       <c r="S20" s="5" t="inlineStr">
         <is>
-          <t>maa://29113 (95.45)</t>
+          <t>maa://29113 (95.65)</t>
         </is>
       </c>
       <c r="U20" s="4" t="inlineStr">
@@ -2948,7 +2948,7 @@
       </c>
       <c r="G21" s="5" t="inlineStr">
         <is>
-          <t>maa://24372 (97.56)</t>
+          <t>maa://24372 (96.43)</t>
         </is>
       </c>
       <c r="I21" s="4" t="inlineStr">
@@ -2963,7 +2963,7 @@
       </c>
       <c r="K21" s="5" t="inlineStr">
         <is>
-          <t>maa://31731 (95.24)</t>
+          <t>maa://31731 (95.56)</t>
         </is>
       </c>
       <c r="M21" s="4" t="inlineStr">
@@ -3008,7 +3008,7 @@
       </c>
       <c r="W21" s="5" t="inlineStr">
         <is>
-          <t>maa://20110 (86.76), maa://34946 (90.62)</t>
+          <t>maa://20110 (86.76), maa://34946 (91.18)</t>
         </is>
       </c>
       <c r="Y21" s="4" t="inlineStr">
@@ -3023,7 +3023,7 @@
       </c>
       <c r="AA21" s="5" t="inlineStr">
         <is>
-          <t>*maa://21443 (78.79), **maa://23820 (30.91)</t>
+          <t>*maa://21443 (79.04), ***maa://23820 (29.82)</t>
         </is>
       </c>
       <c r="AC21" s="4" t="inlineStr">
@@ -3038,7 +3038,7 @@
       </c>
       <c r="AE21" s="5" t="inlineStr">
         <is>
-          <t>maa://22524 (94.35), *maa://22432 (74.55)</t>
+          <t>maa://22524 (93.99), *maa://22432 (75.44)</t>
         </is>
       </c>
     </row>
@@ -3070,7 +3070,7 @@
       </c>
       <c r="G22" s="5" t="inlineStr">
         <is>
-          <t>maa://25236 (95.89), **maa://21678 (48.94), **maa://22735 (50.0)</t>
+          <t>maa://25236 (96.05), **maa://21678 (48.94), **maa://22735 (50.0)</t>
         </is>
       </c>
       <c r="I22" s="4" t="inlineStr">
@@ -3085,7 +3085,7 @@
       </c>
       <c r="K22" s="5" t="inlineStr">
         <is>
-          <t>maa://27127 (86.52), *maa://22751 (77.42)</t>
+          <t>maa://27127 (85.56), *maa://22751 (76.19)</t>
         </is>
       </c>
       <c r="M22" s="4" t="inlineStr">
@@ -3115,7 +3115,7 @@
       </c>
       <c r="S22" s="5" t="inlineStr">
         <is>
-          <t>maa://38495 (100.0)</t>
+          <t>maa://38495 (87.5)</t>
         </is>
       </c>
       <c r="U22" s="4" t="inlineStr">
@@ -3130,7 +3130,7 @@
       </c>
       <c r="W22" s="5" t="inlineStr">
         <is>
-          <t>maa://21282 (98.84), *maa://37649 (66.67)</t>
+          <t>maa://21282 (98.86), *maa://37649 (70.0)</t>
         </is>
       </c>
       <c r="Y22" s="4" t="inlineStr">
@@ -3160,7 +3160,7 @@
       </c>
       <c r="AE22" s="5" t="inlineStr">
         <is>
-          <t>maa://29658 (94.59)</t>
+          <t>maa://29658 (94.74)</t>
         </is>
       </c>
     </row>
@@ -3177,7 +3177,7 @@
       </c>
       <c r="C23" s="5" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.36), *maa://41753 (75.0)</t>
+          <t>***maa://28036 (28.36), *maa://41753 (60.0)</t>
         </is>
       </c>
       <c r="E23" s="4" t="inlineStr">
@@ -3207,7 +3207,7 @@
       </c>
       <c r="K23" s="5" t="inlineStr">
         <is>
-          <t>maa://39756 (92.64), maa://39875 (95.92)</t>
+          <t>maa://39756 (93.06), maa://39875 (94.34)</t>
         </is>
       </c>
       <c r="M23" s="4" t="inlineStr">
@@ -3222,7 +3222,7 @@
       </c>
       <c r="O23" s="5" t="inlineStr">
         <is>
-          <t>maa://30587 (91.72), *maa://29748 (75.2), ***maa://29785 (15.15), *maa://37566 (78.95)</t>
+          <t>maa://30587 (91.86), *maa://29748 (75.2), ***maa://29785 (15.15), *maa://37566 (76.19)</t>
         </is>
       </c>
       <c r="Q23" s="4" t="inlineStr">
@@ -3237,7 +3237,7 @@
       </c>
       <c r="S23" s="5" t="inlineStr">
         <is>
-          <t>maa://24387 (82.86), maa://31212 (95.83)</t>
+          <t>maa://24387 (82.86), maa://31212 (96.0)</t>
         </is>
       </c>
       <c r="U23" s="4" t="inlineStr">
@@ -3252,7 +3252,7 @@
       </c>
       <c r="W23" s="5" t="inlineStr">
         <is>
-          <t>*maa://28503 (63.93)</t>
+          <t>*maa://28503 (65.08)</t>
         </is>
       </c>
       <c r="Y23" s="4" t="inlineStr">
@@ -3267,7 +3267,7 @@
       </c>
       <c r="AA23" s="5" t="inlineStr">
         <is>
-          <t>maa://29652 (97.3)</t>
+          <t>maa://29652 (97.37)</t>
         </is>
       </c>
       <c r="AC23" s="4" t="inlineStr">
@@ -3299,7 +3299,7 @@
       </c>
       <c r="C24" s="5" t="inlineStr">
         <is>
-          <t>maa://24368 (80.42)</t>
+          <t>maa://24368 (80.36)</t>
         </is>
       </c>
       <c r="E24" s="4" t="inlineStr">
@@ -3374,7 +3374,7 @@
       </c>
       <c r="W24" s="5" t="inlineStr">
         <is>
-          <t>maa://29988 (86.47), maa://23504 (92.94), **maa://22892 (40.14), *maa://25141 (77.05), maa://36663 (80.7), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (85.78), maa://23504 (92.76), **maa://22892 (40.14), *maa://25141 (77.24), *maa://36663 (79.31), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="4" t="inlineStr">
@@ -3404,7 +3404,7 @@
       </c>
       <c r="AE24" s="5" t="inlineStr">
         <is>
-          <t>maa://22523 (85.19), *maa://36672 (76.74), maa://29910 (94.12), **maa://21440 (34.55)</t>
+          <t>maa://22523 (85.34), *maa://36672 (77.27), maa://29910 (94.12), **maa://21440 (34.55)</t>
         </is>
       </c>
     </row>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="C25" s="5" t="inlineStr">
         <is>
-          <t>maa://29753 (95.18)</t>
+          <t>maa://29753 (95.28)</t>
         </is>
       </c>
       <c r="E25" s="4" t="inlineStr">
@@ -3436,7 +3436,7 @@
       </c>
       <c r="G25" s="5" t="inlineStr">
         <is>
-          <t>*maa://29063 (75.74), *maa://25311 (74.19), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (74.64), *maa://25311 (74.47), ***maa://22725 (4.84)</t>
         </is>
       </c>
       <c r="I25" s="4" t="inlineStr">
@@ -3466,7 +3466,7 @@
       </c>
       <c r="O25" s="5" t="inlineStr">
         <is>
-          <t>maa://24382 (92.0)</t>
+          <t>maa://24382 (92.31)</t>
         </is>
       </c>
       <c r="Q25" s="4" t="inlineStr">
@@ -3481,7 +3481,7 @@
       </c>
       <c r="S25" s="5" t="inlineStr">
         <is>
-          <t>maa://20109 (92.68), maa://22545 (100.0)</t>
+          <t>maa://20109 (92.12), maa://22545 (100.0)</t>
         </is>
       </c>
       <c r="U25" s="4" t="inlineStr">
@@ -3496,7 +3496,7 @@
       </c>
       <c r="W25" s="5" t="inlineStr">
         <is>
-          <t>*maa://29890 (73.68)</t>
+          <t>*maa://29890 (75.0)</t>
         </is>
       </c>
       <c r="Y25" s="4" t="inlineStr">
@@ -3511,7 +3511,7 @@
       </c>
       <c r="AA25" s="5" t="inlineStr">
         <is>
-          <t>maa://31215 (84.34), *maa://24516 (79.07), maa://26001 (87.27)</t>
+          <t>maa://31215 (84.88), *maa://24516 (79.07), maa://26001 (87.27)</t>
         </is>
       </c>
       <c r="AC25" s="4" t="inlineStr">
@@ -3526,7 +3526,7 @@
       </c>
       <c r="AE25" s="5" t="inlineStr">
         <is>
-          <t>maa://20108 (96.15), maa://24621 (96.43), maa://36676 (100.0), maa://22771 (84.62), maa://37772 (100.0)</t>
+          <t>maa://20108 (96.18), maa://24621 (96.46), maa://36676 (100.0), maa://22771 (84.62), maa://37772 (100.0)</t>
         </is>
       </c>
     </row>
@@ -3558,7 +3558,7 @@
       </c>
       <c r="G26" s="5" t="inlineStr">
         <is>
-          <t>maa://24913 (91.18)</t>
+          <t>maa://24913 (91.43)</t>
         </is>
       </c>
       <c r="I26" s="4" t="inlineStr">
@@ -3633,7 +3633,7 @@
       </c>
       <c r="AA26" s="5" t="inlineStr">
         <is>
-          <t>maa://42235 (80.77)</t>
+          <t>maa://42235 (86.49)</t>
         </is>
       </c>
       <c r="AC26" s="4" t="inlineStr">
@@ -3648,7 +3648,7 @@
       </c>
       <c r="AE26" s="5" t="inlineStr">
         <is>
-          <t>maa://30511 (84.38), *maa://29760 (61.54)</t>
+          <t>maa://30511 (84.85), *maa://29760 (61.54)</t>
         </is>
       </c>
     </row>
@@ -3680,7 +3680,7 @@
       </c>
       <c r="G27" s="5" t="inlineStr">
         <is>
-          <t>**maa://21283 (48.65), maa://34494 (100.0), **maa://36665 (44.44), *maa://39601 (80.0)</t>
+          <t>**maa://21283 (48.65), maa://34494 (100.0), *maa://39601 (72.73), **maa://36665 (44.44)</t>
         </is>
       </c>
       <c r="I27" s="4" t="inlineStr">
@@ -3695,7 +3695,7 @@
       </c>
       <c r="K27" s="5" t="inlineStr">
         <is>
-          <t>maa://28071 (86.67)</t>
+          <t>maa://28071 (88.24)</t>
         </is>
       </c>
       <c r="M27" s="4" t="inlineStr">
@@ -3725,7 +3725,7 @@
       </c>
       <c r="S27" s="5" t="inlineStr">
         <is>
-          <t>*maa://30624 (76.32)</t>
+          <t>*maa://30624 (75.0)</t>
         </is>
       </c>
       <c r="U27" s="4" t="inlineStr">
@@ -3787,7 +3787,7 @@
       </c>
       <c r="C28" s="5" t="inlineStr">
         <is>
-          <t>maa://24465 (90.4), maa://25725 (82.28)</t>
+          <t>maa://24465 (90.47), maa://25725 (82.72)</t>
         </is>
       </c>
       <c r="E28" s="4" t="inlineStr">
@@ -3847,7 +3847,7 @@
       </c>
       <c r="S28" s="5" t="inlineStr">
         <is>
-          <t>maa://23263 (94.32), *maa://29765 (60.29)</t>
+          <t>maa://23263 (94.57), *maa://29765 (60.0)</t>
         </is>
       </c>
       <c r="U28" s="4" t="inlineStr">
@@ -3862,7 +3862,7 @@
       </c>
       <c r="W28" s="5" t="inlineStr">
         <is>
-          <t>maa://39929 (87.14), ***maa://39723 (14.71), maa://41749 (85.0)</t>
+          <t>maa://39929 (87.34), ***maa://39723 (14.29), maa://41749 (83.33)</t>
         </is>
       </c>
       <c r="Y28" s="4" t="inlineStr">
@@ -3892,7 +3892,7 @@
       </c>
       <c r="AE28" s="5" t="inlineStr">
         <is>
-          <t>maa://36660 (93.54), *maa://36701 (64.0)</t>
+          <t>maa://36660 (92.67), *maa://36701 (62.96)</t>
         </is>
       </c>
     </row>
@@ -3909,7 +3909,7 @@
       </c>
       <c r="C29" s="5" t="inlineStr">
         <is>
-          <t>maa://31694 (97.96)</t>
+          <t>maa://31694 (98.0)</t>
         </is>
       </c>
       <c r="E29" s="4" t="inlineStr">
@@ -3939,7 +3939,7 @@
       </c>
       <c r="K29" s="5" t="inlineStr">
         <is>
-          <t>maa://28432 (93.54), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (66.67)</t>
+          <t>maa://28432 (93.58), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (66.67)</t>
         </is>
       </c>
       <c r="M29" s="4" t="inlineStr">
@@ -4009,12 +4009,12 @@
       </c>
       <c r="AD29" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AE29" s="5" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.92), ***maa://34960 (8.7)</t>
+          <t>*maa://24080 (69.17), ***maa://34960 (8.7), maa://42865 (100.0)</t>
         </is>
       </c>
     </row>
@@ -4061,7 +4061,7 @@
       </c>
       <c r="K30" s="5" t="inlineStr">
         <is>
-          <t>maa://30442 (94.55)</t>
+          <t>maa://30442 (94.64)</t>
         </is>
       </c>
       <c r="M30" s="4" t="inlineStr">
@@ -4116,12 +4116,12 @@
       </c>
       <c r="Z30" s="4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AA30" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>maa://42979 (100.0)</t>
         </is>
       </c>
       <c r="AC30" s="4" t="inlineStr">
@@ -4183,7 +4183,7 @@
       </c>
       <c r="K31" s="5" t="inlineStr">
         <is>
-          <t>maa://35926 (93.19), maa://36258 (80.52)</t>
+          <t>maa://35926 (93.36), *maa://36258 (79.49)</t>
         </is>
       </c>
       <c r="M31" s="4" t="inlineStr">
@@ -4213,7 +4213,7 @@
       </c>
       <c r="S31" s="5" t="inlineStr">
         <is>
-          <t>maa://30711 (96.3), maa://30768 (100.0)</t>
+          <t>maa://30711 (96.43), maa://30768 (100.0)</t>
         </is>
       </c>
       <c r="U31" s="4" t="inlineStr">
@@ -4290,7 +4290,7 @@
       </c>
       <c r="G32" s="5" t="inlineStr">
         <is>
-          <t>maa://21895 (97.01), maa://36667 (98.18), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.02), maa://36667 (98.21), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="4" t="inlineStr">
@@ -4330,12 +4330,12 @@
       </c>
       <c r="R32" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="S32" s="5" t="inlineStr">
         <is>
-          <t>maa://41108 (87.8), maa://41238 (94.74)</t>
+          <t>maa://41108 (88.64), maa://41238 (95.24), maa://42859 (92.31)</t>
         </is>
       </c>
       <c r="U32" s="4" t="inlineStr">
@@ -4442,7 +4442,7 @@
       </c>
       <c r="O33" s="5" t="inlineStr">
         <is>
-          <t>*maa://21956 (79.23), maa://22730 (82.14)</t>
+          <t>*maa://21956 (78.95), maa://22730 (82.14)</t>
         </is>
       </c>
       <c r="Q33" s="4" t="inlineStr">
@@ -4564,7 +4564,7 @@
       </c>
       <c r="S34" s="5" t="inlineStr">
         <is>
-          <t>maa://24526 (93.19)</t>
+          <t>maa://24526 (93.25)</t>
         </is>
       </c>
       <c r="Y34" s="4" t="inlineStr">
@@ -4599,6 +4599,21 @@
       </c>
     </row>
     <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>忍冬</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="E35" s="4" t="inlineStr">
         <is>
           <t>史尔特尔</t>
@@ -4626,7 +4641,7 @@
       </c>
       <c r="K35" s="5" t="inlineStr">
         <is>
-          <t>maa://41296 (98.28)</t>
+          <t>maa://41296 (98.55)</t>
         </is>
       </c>
       <c r="M35" s="4" t="inlineStr">
@@ -4686,7 +4701,7 @@
       </c>
       <c r="AE35" s="5" t="inlineStr">
         <is>
-          <t>maa://39479 (90.0)</t>
+          <t>maa://39479 (92.31)</t>
         </is>
       </c>
     </row>
@@ -4748,7 +4763,7 @@
       </c>
       <c r="S36" s="5" t="inlineStr">
         <is>
-          <t>maa://27613 (98.96)</t>
+          <t>maa://27613 (98.97)</t>
         </is>
       </c>
       <c r="Y36" s="4" t="inlineStr">
@@ -4795,7 +4810,7 @@
       </c>
       <c r="G37" s="5" t="inlineStr">
         <is>
-          <t>*maa://24374 (55.26)</t>
+          <t>*maa://24374 (57.5)</t>
         </is>
       </c>
       <c r="I37" s="4" t="inlineStr">
@@ -4825,7 +4840,7 @@
       </c>
       <c r="O37" s="5" t="inlineStr">
         <is>
-          <t>maa://21280 (89.19), *maa://21239 (72.73)</t>
+          <t>maa://21280 (88.83), *maa://21239 (72.73)</t>
         </is>
       </c>
       <c r="Q37" s="4" t="inlineStr">
@@ -4937,7 +4952,7 @@
       </c>
       <c r="S38" s="5" t="inlineStr">
         <is>
-          <t>maa://30713 (100.0)</t>
+          <t>maa://30713 (96.55)</t>
         </is>
       </c>
       <c r="AC38" s="4" t="inlineStr">
@@ -4952,7 +4967,7 @@
       </c>
       <c r="AE38" s="5" t="inlineStr">
         <is>
-          <t>maa://36697 (83.7)</t>
+          <t>maa://36697 (84.51)</t>
         </is>
       </c>
     </row>
@@ -4969,7 +4984,7 @@
       </c>
       <c r="G39" s="5" t="inlineStr">
         <is>
-          <t>maa://25199 (86.11), maa://36670 (88.24), maa://30434 (87.5), ***maa://25036 (16.0)</t>
+          <t>maa://25199 (85.32), maa://36670 (88.57), maa://30434 (87.5), ***maa://25036 (16.0)</t>
         </is>
       </c>
       <c r="I39" s="4" t="inlineStr">
@@ -4999,7 +5014,7 @@
       </c>
       <c r="O39" s="5" t="inlineStr">
         <is>
-          <t>maa://24709 (92.23)</t>
+          <t>maa://24709 (92.31)</t>
         </is>
       </c>
       <c r="Q39" s="4" t="inlineStr">
@@ -5081,7 +5096,7 @@
       </c>
       <c r="O40" s="5" t="inlineStr">
         <is>
-          <t>maa://23278 (95.89), maa://21386 (95.65), maa://36664 (90.7)</t>
+          <t>maa://23278 (95.92), maa://21386 (95.68), maa://36664 (90.91)</t>
         </is>
       </c>
       <c r="Q40" s="4" t="inlineStr">
@@ -5095,6 +5110,21 @@
         </is>
       </c>
       <c r="S40" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC40" t="inlineStr">
+        <is>
+          <t>云迹</t>
+        </is>
+      </c>
+      <c r="AD40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE40" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -5113,7 +5143,22 @@
       </c>
       <c r="G41" s="5" t="inlineStr">
         <is>
-          <t>maa://24466 (95.0)</t>
+          <t>maa://24466 (95.12)</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>菲莱</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="M41" s="4" t="inlineStr">
@@ -5128,7 +5173,7 @@
       </c>
       <c r="O41" s="5" t="inlineStr">
         <is>
-          <t>**maa://35616 (36.67)</t>
+          <t>**maa://35616 (39.39)</t>
         </is>
       </c>
       <c r="Q41" s="4" t="inlineStr">
@@ -5144,6 +5189,21 @@
       <c r="S41" s="5" t="inlineStr">
         <is>
           <t>None</t>
+        </is>
+      </c>
+      <c r="AC41" t="inlineStr">
+        <is>
+          <t>裁度</t>
+        </is>
+      </c>
+      <c r="AD41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE41" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -5198,6 +5258,21 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AC42" t="inlineStr">
+        <is>
+          <t>弑君者</t>
+        </is>
+      </c>
+      <c r="AD42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="E43" s="4" t="inlineStr">
@@ -5212,7 +5287,7 @@
       </c>
       <c r="G43" s="5" t="inlineStr">
         <is>
-          <t>maa://22525 (92.68), maa://21284 (82.93)</t>
+          <t>maa://22525 (92.74), maa://21284 (82.93)</t>
         </is>
       </c>
       <c r="M43" s="4" t="inlineStr">
@@ -5222,12 +5297,12 @@
       </c>
       <c r="N43" s="4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0</t>
         </is>
       </c>
       <c r="O43" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>None</t>
         </is>
       </c>
       <c r="Q43" s="4" t="inlineStr">
@@ -5237,12 +5312,12 @@
       </c>
       <c r="R43" s="4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0</t>
         </is>
       </c>
       <c r="S43" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5259,7 +5334,7 @@
       </c>
       <c r="G44" s="5" t="inlineStr">
         <is>
-          <t>maa://29768 (97.55), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.63), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="M44" s="4" t="inlineStr">
@@ -5289,7 +5364,7 @@
       </c>
       <c r="S44" s="5" t="inlineStr">
         <is>
-          <t>maa://39366 (84.62)</t>
+          <t>maa://39366 (85.71)</t>
         </is>
       </c>
     </row>
@@ -5309,7 +5384,7 @@
       </c>
       <c r="G45" s="5" t="inlineStr">
         <is>
-          <t>maa://21229 (85.47), maa://30807 (95.08), *maa://22767 (52.94), ***maa://20796 (13.79), maa://42459 (100.0)</t>
+          <t>maa://21229 (85.56), maa://30807 (95.08), *maa://22767 (55.56), ***maa://20796 (13.79), maa://42459 (100.0)</t>
         </is>
       </c>
       <c r="M45" s="4" t="inlineStr">
@@ -5339,7 +5414,7 @@
       </c>
       <c r="S45" s="5" t="inlineStr">
         <is>
-          <t>**maa://39364 (45.45)</t>
+          <t>**maa://39364 (46.15)</t>
         </is>
       </c>
     </row>
@@ -5359,7 +5434,7 @@
       </c>
       <c r="G46" s="5" t="inlineStr">
         <is>
-          <t>maa://35931 (92.27)</t>
+          <t>maa://35931 (92.5)</t>
         </is>
       </c>
       <c r="M46" s="4" t="inlineStr">
@@ -5409,7 +5484,7 @@
       </c>
       <c r="G47" s="5" t="inlineStr">
         <is>
-          <t>maa://27410 (95.82), maa://29661 (97.64), maa://28038 (84.62)</t>
+          <t>maa://27410 (95.86), maa://29661 (97.71), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="M47" s="4" t="inlineStr">
@@ -5524,7 +5599,22 @@
       </c>
       <c r="O49" s="5" t="inlineStr">
         <is>
-          <t>*maa://39643 (71.43)</t>
+          <t>*maa://39643 (66.67)</t>
+        </is>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>荒芜拉普兰德</t>
+        </is>
+      </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -5640,7 +5730,7 @@
       </c>
       <c r="G53" s="5" t="inlineStr">
         <is>
-          <t>maa://32534 (93.31), **maa://32434 (36.36)</t>
+          <t>maa://32534 (93.07), **maa://32434 (34.78)</t>
         </is>
       </c>
     </row>
@@ -5674,7 +5764,7 @@
       </c>
       <c r="G55" s="5" t="inlineStr">
         <is>
-          <t>maa://32532 (91.96)</t>
+          <t>maa://32532 (92.24)</t>
         </is>
       </c>
     </row>
@@ -5708,7 +5798,7 @@
       </c>
       <c r="G57" s="5" t="inlineStr">
         <is>
-          <t>maa://25176 (97.83)</t>
+          <t>maa://25176 (97.96)</t>
         </is>
       </c>
     </row>
@@ -5725,7 +5815,7 @@
       </c>
       <c r="G58" s="5" t="inlineStr">
         <is>
-          <t>*maa://37964 (60.0)</t>
+          <t>*maa://37964 (57.14)</t>
         </is>
       </c>
     </row>
@@ -5742,7 +5832,7 @@
       </c>
       <c r="G59" s="5" t="inlineStr">
         <is>
-          <t>maa://27746 (84.0), maa://31270 (96.97)</t>
+          <t>maa://27746 (83.17), maa://31270 (95.19)</t>
         </is>
       </c>
     </row>
@@ -5759,7 +5849,7 @@
       </c>
       <c r="G60" s="5" t="inlineStr">
         <is>
-          <t>**maa://40438 (31.58)</t>
+          <t>**maa://40438 (33.33)</t>
         </is>
       </c>
     </row>
@@ -5788,12 +5878,12 @@
       </c>
       <c r="F62" s="4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G62" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>maa://42981 (100.0)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: Auto Update Data (#89)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1260" yWindow="3000" windowWidth="23925" windowHeight="16665" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.12), maa://25390 (96.19), maa://36681 (88.24)</t>
+          <t>maa://24702 (94.12), maa://25390 (95.78), maa://36681 (88.24)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.26), maa://36684 (98.68), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.26), maa://36684 (98.7), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (70.0), maa://20276 (83.33), *maa://22749 (66.67)</t>
+          <t>*maa://22880 (69.57), maa://20276 (83.33), *maa://22749 (66.67)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (85.37), maa://27484 (95.79), maa://27480 (82.35)</t>
+          <t>maa://27396 (85.42), maa://27484 (95.79), maa://27480 (82.35)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (96.15)</t>
+          <t>maa://24390 (96.23)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.43), **maa://24303 (36.36), maa://22499 (85.71), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.48), **maa://24303 (36.36), maa://22499 (85.71), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.7), maa://22754 (91.67), maa://27295 (80.77), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (97.7), maa://22754 (91.67), maa://27295 (81.82), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (82.05), maa://22744 (83.33)</t>
+          <t>maa://21245 (82.14), maa://22744 (83.33)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (94.12)</t>
+          <t>maa://42407 (94.44)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="P6" s="2" t="inlineStr">
         <is>
-          <t>maa://31836 (88.24), maa://30381 (91.67)</t>
+          <t>maa://31836 (88.89), maa://30381 (91.67)</t>
         </is>
       </c>
       <c r="Q6" s="1" t="n"/>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>maa://21955 (93.33)</t>
+          <t>maa://21955 (93.55)</t>
         </is>
       </c>
       <c r="E7" s="1" t="n"/>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="P7" s="2" t="inlineStr">
         <is>
-          <t>maa://22750 (94.44)</t>
+          <t>maa://22750 (94.74)</t>
         </is>
       </c>
       <c r="Q7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (94.74), *maa://22758 (70.37)</t>
+          <t>maa://22399 (94.78), *maa://22758 (70.37)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (68.49), *maa://36671 (72.73), *maa://42530 (75.0)</t>
+          <t>*maa://26191 (68.92), *maa://36671 (73.33), *maa://42530 (75.0)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.02 22:43:40</t>
+          <t>更新日期：2024.11.02 22:47:19</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.09)</t>
+          <t>maa://26223 (97.12)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (88.37), ***maa://22740 (5.88), **maa://27377 (46.15), ***maa://25174 (20.0), **maa://39938 (41.18), maa://40166 (100.0)</t>
+          <t>maa://28711 (88.51), ***maa://22740 (5.88), **maa://27377 (46.15), ***maa://25174 (20.0), **maa://39938 (41.18), maa://40166 (100.0)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (90.11), **maa://22865 (47.92)</t>
+          <t>maa://26206 (90.22), **maa://22865 (47.92)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.5), *maa://21485 (76.92), maa://37962 (83.33)</t>
+          <t>maa://22753 (91.5), *maa://21485 (77.1), maa://37962 (83.33)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.51), maa://36677 (92.5), maa://39872 (86.67)</t>
+          <t>maa://23669 (95.51), maa://36677 (92.68), maa://39872 (86.67)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.15), *maa://20106 (63.64), *maa://22769 (62.96)</t>
+          <t>*maa://28932 (78.15), *maa://20106 (63.64), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.43), maa://36673 (92.06), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.45), maa://36673 (92.06), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (74.88), **maa://22728 (46.51)</t>
+          <t>*maa://21248 (74.53), **maa://22728 (46.51)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>*maa://34957 (77.36), *maa://22768 (51.61)</t>
+          <t>*maa://34957 (77.78), *maa://22768 (51.61)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (30.6), maa://39883 (90.62), *maa://39885 (70.0)</t>
+          <t>**maa://22737 (30.6), maa://39883 (91.43), *maa://39885 (70.0)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.12), maa://21288 (96.21), maa://36682 (100.0), maa://39841 (93.62)</t>
+          <t>maa://26245 (96.12), maa://21288 (96.21), maa://36682 (100.0), maa://39841 (93.75)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.09), maa://22734 (83.48), *maa://30808 (64.41), ***maa://36048 (12.5)</t>
+          <t>*maa://22743 (77.09), maa://22734 (83.48), *maa://30808 (64.41), ***maa://36048 (12.12)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.24), maa://21478 (91.18)</t>
+          <t>maa://24304 (88.3), maa://21478 (91.18)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (89.66), *maa://22727 (70.0)</t>
+          <t>maa://24762 (89.73), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.68), *maa://22766 (72.12), *maa://36666 (77.61)</t>
+          <t>maa://21364 (80.68), *maa://22766 (72.12), *maa://36666 (77.94)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (95.17), *maa://28648 (69.64), maa://36674 (81.25)</t>
+          <t>maa://22729 (95.21), *maa://28648 (69.64), maa://36674 (81.25)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (97.62), maa://28051 (95.83)</t>
+          <t>maa://28501 (97.67), maa://28051 (95.83)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>**maa://42324 (30.77)</t>
+          <t>***maa://42324 (28.57)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (98.84)</t>
+          <t>maa://24386 (98.85)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (61.72), *maa://36668 (52.17)</t>
+          <t>*maa://30709 (61.56), *maa://36668 (52.17)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (88.81)</t>
+          <t>maa://22864 (88.89)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (81.82)</t>
+          <t>maa://41331 (82.46)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3155,7 +3155,7 @@
       </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>maa://24372 (96.43)</t>
+          <t>maa://24372 (96.51)</t>
         </is>
       </c>
       <c r="I21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (93.99), *maa://22432 (75.44)</t>
+          <t>maa://22524 (94.02), *maa://22432 (75.44)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="T22" s="2" t="inlineStr">
         <is>
-          <t>maa://38495 (87.5)</t>
+          <t>maa://38495 (88.89)</t>
         </is>
       </c>
       <c r="U22" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.86), *maa://37649 (70.0)</t>
+          <t>maa://21282 (98.86), *maa://37649 (71.43)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (93.06), maa://39875 (94.34)</t>
+          <t>maa://39756 (93.1), maa://39875 (94.34)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.86), *maa://29748 (75.2), ***maa://29785 (15.15), *maa://37566 (76.19)</t>
+          <t>maa://30587 (91.33), *maa://29748 (75.2), ***maa://29785 (15.15), *maa://37566 (76.19)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.34), *maa://36672 (77.27), maa://29910 (94.12), **maa://21440 (34.55)</t>
+          <t>maa://22523 (85.34), *maa://36672 (77.78), maa://29910 (94.12), **maa://21440 (34.55)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.28)</t>
+          <t>maa://29753 (94.89)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (91.43)</t>
+          <t>maa://24913 (91.67)</t>
         </is>
       </c>
       <c r="I26" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (86.49)</t>
+          <t>maa://42235 (87.18)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.47), maa://25725 (82.72)</t>
+          <t>maa://24465 (90.48), maa://25725 (82.72)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (87.34), ***maa://39723 (14.29), maa://41749 (83.33)</t>
+          <t>maa://39929 (87.55), ***maa://39723 (14.29), maa://41749 (83.33)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.67), *maa://36701 (62.96)</t>
+          <t>maa://36660 (92.7), *maa://36701 (62.96)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.58), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (66.67)</t>
+          <t>maa://28432 (93.6), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (66.67)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4373,7 +4373,7 @@
       </c>
       <c r="T30" s="2" t="inlineStr">
         <is>
-          <t>*maa://32940 (66.67), maa://24388 (93.75)</t>
+          <t>*maa://32940 (66.67), maa://24388 (94.12)</t>
         </is>
       </c>
       <c r="U30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.36), *maa://36258 (79.49)</t>
+          <t>maa://35926 (93.36), *maa://36258 (79.75)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (88.64), maa://41238 (95.24), maa://42859 (92.31)</t>
+          <t>maa://41108 (88.64), maa://41238 (95.24), maa://42859 (92.86)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4959,7 +4959,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (98.55)</t>
+          <t>maa://41296 (98.59)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (84.51)</t>
+          <t>maa://36697 (84.72)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5442,7 +5442,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.92), maa://21386 (95.68), maa://36664 (90.91)</t>
+          <t>maa://23278 (95.92), maa://21386 (95.68), maa://36664 (91.11)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (92.74), maa://21284 (82.93)</t>
+          <t>maa://22525 (92.8), maa://21284 (82.93)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5702,7 +5702,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.63), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.65), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5808,7 +5808,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.5)</t>
+          <t>maa://35931 (92.15)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5861,7 +5861,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (95.86), maa://29661 (97.71), maa://28038 (84.62)</t>
+          <t>maa://27410 (95.86), maa://29661 (97.73), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6122,7 +6122,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.07), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.09), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6248,7 +6248,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>**maa://40438 (33.33)</t>
+          <t>**maa://40438 (36.36)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>
@@ -6489,9 +6489,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="A5:A7"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A5:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#90)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (69.57), maa://20276 (83.33), *maa://22749 (66.67)</t>
+          <t>*maa://22880 (69.57), maa://20276 (83.45), *maa://22749 (66.67)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (95.22), maa://26254 (95.65)</t>
+          <t>maa://21249 (95.24), maa://26254 (95.65)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (85.42), maa://27484 (95.79), maa://27480 (82.35)</t>
+          <t>maa://27396 (85.47), maa://27484 (95.79), maa://27480 (82.35)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.7), maa://22754 (91.67), maa://27295 (81.82), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (97.73), maa://22754 (91.67), maa://27295 (81.82), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.01), ***maa://31785 (20.87), ***maa://36683 (26.67)</t>
+          <t>**maa://32495 (47.01), ***maa://31785 (20.87), ***maa://36683 (28.26)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (61.36), ***maa://26209 (13.04), *maa://39394 (73.33)</t>
+          <t>*maa://30062 (61.36), ***maa://26209 (13.04), *maa://39394 (75.0)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (82.14), maa://22744 (83.33)</t>
+          <t>maa://21245 (82.23), maa://22744 (83.33)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="T6" s="2" t="inlineStr">
         <is>
-          <t>maa://37411 (81.82)</t>
+          <t>maa://37411 (83.33)</t>
         </is>
       </c>
       <c r="U6" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (94.78), *maa://22758 (70.37)</t>
+          <t>maa://22399 (94.78), *maa://22758 (70.91)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.02 22:47:19</t>
+          <t>更新日期：2024.11.03 01:13:15</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1611,7 +1611,7 @@
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>maa://22762 (91.57), maa://39552 (85.71)</t>
+          <t>maa://22762 (91.57), maa://39552 (87.5)</t>
         </is>
       </c>
       <c r="M9" s="1" t="n"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (93.59), *maa://23264 (61.82), maa://36669 (84.62)</t>
+          <t>maa://28977 (93.59), *maa://23264 (61.82), maa://36669 (85.19)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.92)</t>
+          <t>maa://36713 (97.93)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.12), maa://21288 (96.21), maa://36682 (100.0), maa://39841 (93.75)</t>
+          <t>maa://26245 (96.12), maa://21288 (96.21), maa://36682 (100.0), maa://39841 (93.88)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.52), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.53), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="T14" s="2" t="inlineStr">
         <is>
-          <t>maa://22521 (94.51), maa://42751 (100.0)</t>
+          <t>maa://22521 (94.57), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (95.21), *maa://28648 (69.64), maa://36674 (81.25)</t>
+          <t>maa://22729 (95.24), *maa://28648 (69.64), maa://36674 (81.25)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (90.37)</t>
+          <t>maa://24421 (90.41)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="X18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (97.53), maa://22741 (83.33)</t>
+          <t>maa://21917 (97.56), maa://22741 (83.33)</t>
         </is>
       </c>
       <c r="Y18" s="1" t="n"/>
@@ -3155,7 +3155,7 @@
       </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>maa://24372 (96.51)</t>
+          <t>maa://24372 (96.55)</t>
         </is>
       </c>
       <c r="I21" s="1" t="n"/>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="X21" s="2" t="inlineStr">
         <is>
-          <t>maa://20110 (86.76), maa://34946 (91.18)</t>
+          <t>maa://20110 (86.76), maa://34946 (91.43)</t>
         </is>
       </c>
       <c r="Y21" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (85.56), *maa://22751 (76.19)</t>
+          <t>maa://27127 (85.71), *maa://22751 (76.19)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>maa://24368 (80.36)</t>
+          <t>maa://24368 (80.42)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (91.67)</t>
+          <t>maa://24913 (91.78)</t>
         </is>
       </c>
       <c r="I26" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>maa://23263 (94.57), *maa://29765 (60.0)</t>
+          <t>maa://23263 (94.62), *maa://29765 (60.0)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4357,7 +4357,7 @@
       </c>
       <c r="P30" s="2" t="inlineStr">
         <is>
-          <t>maa://21442 (99.49)</t>
+          <t>maa://21442 (99.5)</t>
         </is>
       </c>
       <c r="Q30" s="1" t="n"/>
@@ -4747,7 +4747,7 @@
       </c>
       <c r="P33" s="2" t="inlineStr">
         <is>
-          <t>*maa://21956 (78.95), maa://22730 (82.14)</t>
+          <t>*maa://21956 (79.1), maa://22730 (82.14)</t>
         </is>
       </c>
       <c r="Q33" s="1" t="n"/>
@@ -5357,7 +5357,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (92.31)</t>
+          <t>maa://24709 (92.38)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5527,7 +5527,7 @@
       </c>
       <c r="P41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (39.39)</t>
+          <t>**maa://35616 (38.24)</t>
         </is>
       </c>
       <c r="Q41" s="1" t="n"/>
@@ -5702,7 +5702,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.65), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.66), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -6230,7 +6230,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (83.17), maa://31270 (95.19)</t>
+          <t>maa://27746 (83.33), maa://31270 (95.19)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#91)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.26), maa://36684 (98.7), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.26), maa://36684 (98.72), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.77), ***maa://21730 (17.19), ***maa://39501 (18.75), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.77), ***maa://21730 (16.92), ***maa://39501 (18.75), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://36987 (93.62), maa://40192 (95.65), maa://39849 (88.89)</t>
+          <t>maa://36987 (93.62), maa://40192 (96.0), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (69.57), maa://20276 (83.45), *maa://22749 (66.67)</t>
+          <t>*maa://22880 (69.57), maa://20276 (83.56), *maa://22749 (66.67)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (95.24), maa://26254 (95.65)</t>
+          <t>maa://21249 (94.79), maa://26254 (95.65)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (88.46), **maa://20790 (43.94), ***maa://37170 (20.0)</t>
+          <t>maa://24617 (88.46), **maa://20790 (43.94), ***maa://37170 (19.57)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (85.47), maa://27484 (95.79), maa://27480 (82.35)</t>
+          <t>maa://27396 (85.52), maa://27484 (95.79), maa://27480 (82.35)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.48), **maa://24303 (36.36), maa://22499 (85.71), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.53), **maa://24303 (36.36), maa://22499 (85.71), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.73), maa://22754 (91.67), maa://27295 (81.82), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (97.73), maa://22754 (91.67), maa://27295 (82.14), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.01), ***maa://31785 (20.87), ***maa://36683 (28.26)</t>
+          <t>**maa://32495 (47.01), ***maa://31785 (21.55), ***maa://36683 (28.26)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (61.36), ***maa://26209 (13.04), *maa://39394 (75.0)</t>
+          <t>*maa://30062 (61.36), ***maa://26209 (13.04), *maa://39394 (76.47)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (82.23), maa://22744 (83.33)</t>
+          <t>maa://21245 (82.32), maa://22744 (83.33)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>*maa://22757 (78.57)</t>
+          <t>*maa://22757 (75.86)</t>
         </is>
       </c>
       <c r="M5" s="1" t="n"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="P5" s="2" t="inlineStr">
         <is>
-          <t>maa://21919 (95.74), maa://21281 (92.31)</t>
+          <t>maa://21919 (95.83), maa://21281 (92.31)</t>
         </is>
       </c>
       <c r="Q5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (94.44)</t>
+          <t>maa://42407 (89.47)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (94.78), *maa://22758 (70.91)</t>
+          <t>maa://22399 (94.78), *maa://22758 (71.43)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.03 01:13:15</t>
+          <t>更新日期：2024.11.03 14:53:27</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1611,7 +1611,7 @@
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>maa://22762 (91.57), maa://39552 (87.5)</t>
+          <t>maa://22762 (91.57), maa://39552 (88.89)</t>
         </is>
       </c>
       <c r="M9" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.12)</t>
+          <t>maa://26223 (97.14)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (88.51), ***maa://22740 (5.88), **maa://27377 (46.15), ***maa://25174 (20.0), **maa://39938 (41.18), maa://40166 (100.0)</t>
+          <t>maa://28711 (88.51), ***maa://22740 (5.88), **maa://27377 (46.15), ***maa://25174 (20.0), **maa://39938 (42.11), maa://40166 (85.71)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (90.22), **maa://22865 (47.92)</t>
+          <t>maa://26206 (90.32), **maa://22865 (47.92)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.97), **maa://32237 (37.84), ***maa://34206 (18.18), ***maa://39951 (16.13), **maa://39243 (33.33)</t>
+          <t>***maa://25695 (18.86), **maa://32237 (37.84), ***maa://34206 (18.18), ***maa://39951 (16.13), **maa://39243 (33.33)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (93.59), *maa://23264 (61.82), maa://36669 (85.19)</t>
+          <t>maa://28977 (93.59), maa://36669 (85.19), *maa://23264 (61.82)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (94.41), maa://22501 (98.15)</t>
+          <t>maa://22747 (93.75), maa://22501 (98.15)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.5), *maa://21485 (77.1), maa://37962 (83.33)</t>
+          <t>maa://22753 (91.5), *maa://21485 (77.1), maa://37962 (84.21)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.15), *maa://20106 (63.64), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (77.69), *maa://20106 (63.64), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (92.08), *maa://22583 (75.41), *maa://22500 (55.81)</t>
+          <t>maa://22676 (92.08), *maa://22583 (75.41), *maa://22500 (56.82)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (30.6), maa://39883 (91.43), *maa://39885 (70.0)</t>
+          <t>**maa://22737 (30.6), maa://39883 (91.43), *maa://39885 (66.67)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.53), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.54), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.09), maa://22734 (83.48), *maa://30808 (64.41), ***maa://36048 (12.12)</t>
+          <t>*maa://22743 (77.35), maa://22734 (83.48), *maa://30808 (65.0), ***maa://36048 (12.12)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.3), maa://21478 (91.18)</t>
+          <t>maa://24304 (88.36), maa://21478 (91.18)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.68), *maa://22766 (72.12), *maa://36666 (77.94)</t>
+          <t>maa://21364 (80.68), *maa://22766 (71.43), *maa://36666 (78.26)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.17), maa://36679 (91.43), maa://37650 (96.3)</t>
+          <t>maa://21441 (96.17), maa://36679 (91.43), maa://37650 (96.43)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (63.16), maa://27755 (92.11)</t>
+          <t>*maa://23911 (63.16), maa://27755 (92.21)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.14), maa://39599 (84.0)</t>
+          <t>maa://22430 (88.2), maa://39599 (85.19)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2651,7 +2651,7 @@
       </c>
       <c r="L17" s="2" t="inlineStr">
         <is>
-          <t>*maa://21679 (75.0)</t>
+          <t>*maa://21679 (76.0)</t>
         </is>
       </c>
       <c r="M17" s="1" t="n"/>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>***maa://42324 (28.57)</t>
+          <t>***maa://42324 (26.67)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2813,7 +2813,7 @@
       </c>
       <c r="T18" s="2" t="inlineStr">
         <is>
-          <t>maa://24385 (96.88)</t>
+          <t>maa://24385 (96.97)</t>
         </is>
       </c>
       <c r="U18" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (82.46)</t>
+          <t>maa://41331 (83.61)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="T20" s="2" t="inlineStr">
         <is>
-          <t>maa://29113 (95.65)</t>
+          <t>maa://29113 (88.0)</t>
         </is>
       </c>
       <c r="U20" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>*maa://21443 (79.04), ***maa://23820 (29.82)</t>
+          <t>*maa://21443 (79.1), ***maa://23820 (29.82)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (85.71), *maa://22751 (76.19)</t>
+          <t>maa://27127 (85.87), *maa://22751 (76.19)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (93.1), maa://39875 (94.34)</t>
+          <t>maa://39756 (93.14), maa://39875 (94.34)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.33), *maa://29748 (75.2), ***maa://29785 (15.15), *maa://37566 (76.19)</t>
+          <t>maa://30587 (91.33), *maa://29748 (75.2), ***maa://29785 (15.15), *maa://37566 (77.27)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (85.78), maa://23504 (92.76), **maa://22892 (40.14), *maa://25141 (77.24), *maa://36663 (79.31), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (85.78), maa://23504 (92.76), **maa://22892 (40.14), *maa://25141 (77.24), *maa://36663 (79.66), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (94.89)</t>
+          <t>maa://29753 (94.92)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (74.64), *maa://25311 (74.47), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (74.64), *maa://25311 (74.74), ***maa://22725 (4.84)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.18), maa://24621 (96.46), maa://36676 (100.0), maa://22771 (84.62), maa://37772 (100.0)</t>
+          <t>maa://20108 (96.18), maa://24621 (96.46), maa://36676 (100.0), maa://22771 (85.71), maa://37772 (100.0)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (87.18)</t>
+          <t>maa://42235 (88.1)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.48), maa://25725 (82.72)</t>
+          <t>maa://24465 (90.5), maa://25725 (82.93)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (87.55), ***maa://39723 (14.29), maa://41749 (83.33)</t>
+          <t>maa://39929 (87.76), ***maa://39723 (14.29), maa://41749 (83.33)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.7), *maa://36701 (62.96)</t>
+          <t>maa://36660 (92.73), *maa://36701 (62.96)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.6), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (66.67)</t>
+          <t>maa://28432 (93.62), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.17), ***maa://34960 (8.7), maa://42865 (100.0)</t>
+          <t>*maa://24080 (69.17), ***maa://34960 (8.7), maa://42865 (90.0)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (100.0)</t>
+          <t>maa://42979 (92.86)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.36), *maa://36258 (79.75)</t>
+          <t>maa://35926 (93.39), *maa://36258 (79.75)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (88.64), maa://41238 (95.24), maa://42859 (92.86)</t>
+          <t>maa://41108 (88.89), maa://41238 (95.24), maa://42859 (94.12)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4959,7 +4959,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (98.59)</t>
+          <t>maa://41296 (98.63)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5495,7 +5495,7 @@
       </c>
       <c r="H41" s="2" t="inlineStr">
         <is>
-          <t>maa://24466 (95.12)</t>
+          <t>maa://24466 (92.86)</t>
         </is>
       </c>
       <c r="I41" s="1" t="n"/>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (92.8), maa://21284 (82.93)</t>
+          <t>maa://22525 (92.86), maa://21284 (82.93)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5808,7 +5808,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.15)</t>
+          <t>maa://35931 (92.18)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5861,7 +5861,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (95.86), maa://29661 (97.73), maa://28038 (84.62)</t>
+          <t>maa://27410 (95.89), maa://29661 (97.73), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6158,7 +6158,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.24)</t>
+          <t>maa://32532 (92.27)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6194,7 +6194,7 @@
       </c>
       <c r="H57" s="2" t="inlineStr">
         <is>
-          <t>maa://25176 (97.96)</t>
+          <t>maa://25176 (98.0)</t>
         </is>
       </c>
       <c r="I57" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#92)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.12), maa://25390 (95.78), maa://36681 (88.24)</t>
+          <t>maa://24702 (94.16), maa://25390 (95.8), maa://36681 (85.71)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (54.97), *maa://30515 (69.7), *maa://34787 (72.13), ***maa://20792 (11.93), maa://39402 (86.21), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (54.97), *maa://30515 (69.0), *maa://34787 (70.97), ***maa://20792 (11.93), maa://39402 (84.38), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (92.25), *maa://20791 (62.32)</t>
+          <t>maa://22742 (91.61), *maa://20791 (62.32)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.26), maa://36684 (98.72), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.26), maa://36684 (97.53), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.77), ***maa://21730 (16.92), ***maa://39501 (18.75), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.94), ***maa://21730 (16.92), ***maa://39501 (17.65), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://36987 (93.62), maa://40192 (96.0), maa://39849 (88.89)</t>
+          <t>maa://36987 (93.62), maa://40192 (96.15), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (69.57), maa://20276 (83.56), *maa://22749 (66.67)</t>
+          <t>*maa://22880 (68.67), maa://20276 (84.0), *maa://22749 (66.67)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.79), maa://26254 (95.65)</t>
+          <t>maa://21249 (94.84), maa://26254 (95.65)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (88.46), **maa://20790 (43.94), ***maa://37170 (19.57)</t>
+          <t>maa://24617 (88.46), **maa://20790 (43.94), ***maa://37170 (20.83)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (85.52), maa://27484 (95.79), maa://27480 (82.35)</t>
+          <t>maa://27396 (84.77), maa://27484 (95.83), maa://27480 (82.35)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (96.23)</t>
+          <t>maa://24390 (96.36)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.53), **maa://24303 (36.36), maa://22499 (85.71), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.57), **maa://24303 (33.33), maa://22499 (85.71), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.73), maa://22754 (91.67), maa://27295 (82.14), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (97.8), maa://27295 (82.46), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -994,12 +994,12 @@
       </c>
       <c r="W4" s="1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.01), ***maa://31785 (21.55), ***maa://36683 (28.26)</t>
+          <t>**maa://32495 (46.85), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (100.0)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1015,7 +1015,7 @@
       </c>
       <c r="AB4" s="2" t="inlineStr">
         <is>
-          <t>*maa://32658 (68.75)</t>
+          <t>*maa://32658 (66.67)</t>
         </is>
       </c>
       <c r="AC4" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (61.36), ***maa://26209 (13.04), *maa://39394 (76.47)</t>
+          <t>*maa://30062 (61.36), ***maa://26209 (13.04), *maa://39394 (72.22)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (82.32), maa://22744 (83.33)</t>
+          <t>maa://21245 (82.76), maa://22744 (83.33)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="P5" s="2" t="inlineStr">
         <is>
-          <t>maa://21919 (95.83), maa://21281 (92.31)</t>
+          <t>maa://21919 (95.92), maa://21281 (85.71)</t>
         </is>
       </c>
       <c r="Q5" s="1" t="n"/>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="AB5" s="2" t="inlineStr">
         <is>
-          <t>*maa://29863 (72.41), ***maa://22752 (13.33), **maa://26013 (42.86)</t>
+          <t>*maa://29863 (70.0), ***maa://22752 (13.33), **maa://26013 (42.86)</t>
         </is>
       </c>
       <c r="AC5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (89.47)</t>
+          <t>maa://42407 (92.59)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>maa://24370 (96.3)</t>
+          <t>maa://24370 (96.36)</t>
         </is>
       </c>
       <c r="I6" s="1" t="n"/>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>maa://24839 (99.22)</t>
+          <t>maa://24839 (99.24)</t>
         </is>
       </c>
       <c r="M6" s="1" t="n"/>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="P6" s="2" t="inlineStr">
         <is>
-          <t>maa://31836 (88.89), maa://30381 (91.67)</t>
+          <t>maa://31836 (89.47), maa://30381 (91.67)</t>
         </is>
       </c>
       <c r="Q6" s="1" t="n"/>
@@ -1280,7 +1280,7 @@
       </c>
       <c r="AB6" s="2" t="inlineStr">
         <is>
-          <t>maa://22739 (92.0)</t>
+          <t>maa://22739 (92.31)</t>
         </is>
       </c>
       <c r="AC6" s="1" t="n"/>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="AF6" s="2" t="inlineStr">
         <is>
-          <t>*maa://33152 (61.76), ***maa://22770 (28.57)</t>
+          <t>*maa://33152 (60.53), ***maa://22770 (28.57)</t>
         </is>
       </c>
       <c r="AG6" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (92.0), maa://24957 (97.56)</t>
+          <t>maa://28624 (92.21), maa://24957 (97.62)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="P7" s="2" t="inlineStr">
         <is>
-          <t>maa://22750 (94.74)</t>
+          <t>maa://22750 (94.87)</t>
         </is>
       </c>
       <c r="Q7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (94.78), *maa://22758 (71.43)</t>
+          <t>maa://22399 (94.85), *maa://22758 (71.93)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (68.92), *maa://36671 (73.33), *maa://42530 (75.0)</t>
+          <t>*maa://26191 (68.0), *maa://36671 (71.74), **maa://42530 (42.86)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.03 14:53:27</t>
+          <t>更新日期：2024.11.09 17:55:06</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>*maa://21476 (70.45), **maa://39431 (42.86), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (71.11), **maa://39431 (44.44), *maa://37551 (57.14)</t>
         </is>
       </c>
       <c r="E8" s="1" t="n"/>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24371 (52.24)</t>
+          <t>*maa://24371 (52.17)</t>
         </is>
       </c>
       <c r="I8" s="1" t="n"/>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (87.21), *maa://21916 (60.0), maa://23252 (92.31), **maa://22759 (45.45), maa://37496 (100.0)</t>
+          <t>maa://32931 (85.71), *maa://21916 (60.0), maa://23252 (92.31), **maa://22759 (45.45), maa://37496 (95.65)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.79)</t>
+          <t>maa://21411 (95.85)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="AB8" s="2" t="inlineStr">
         <is>
-          <t>maa://25389 (89.66)</t>
+          <t>maa://25389 (87.1)</t>
         </is>
       </c>
       <c r="AC8" s="1" t="n"/>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="AF8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24479 (77.33), *maa://21990 (53.85)</t>
+          <t>*maa://24479 (77.92), *maa://21990 (53.85)</t>
         </is>
       </c>
       <c r="AG8" s="1" t="n"/>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>maa://22765 (91.76), *maa://21915 (68.0)</t>
+          <t>maa://22765 (91.86), *maa://21915 (68.0)</t>
         </is>
       </c>
       <c r="E9" s="1" t="n"/>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>maa://22762 (91.57), maa://39552 (88.89)</t>
+          <t>maa://22762 (91.67), maa://39552 (90.0)</t>
         </is>
       </c>
       <c r="M9" s="1" t="n"/>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (80.95)</t>
+          <t>maa://22736 (80.46)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1643,7 +1643,7 @@
       </c>
       <c r="T9" s="2" t="inlineStr">
         <is>
-          <t>**maa://22866 (30.77), maa://26222 (97.5)</t>
+          <t>**maa://22866 (30.77), maa://26222 (97.56)</t>
         </is>
       </c>
       <c r="U9" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.14)</t>
+          <t>maa://26223 (97.2)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (88.51), ***maa://22740 (5.88), **maa://27377 (46.15), ***maa://25174 (20.0), **maa://39938 (42.11), maa://40166 (85.71)</t>
+          <t>maa://28711 (87.91), ***maa://22740 (5.88), **maa://27377 (46.15), ***maa://25174 (20.0), **maa://39938 (45.0), maa://40166 (87.5)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (90.32), **maa://22865 (47.92)</t>
+          <t>maa://26206 (89.58), **maa://22865 (48.98)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.86), **maa://32237 (37.84), ***maa://34206 (18.18), ***maa://39951 (16.13), **maa://39243 (33.33)</t>
+          <t>***maa://25695 (18.86), **maa://32237 (42.5), ***maa://34206 (18.18), ***maa://39951 (15.15), ***maa://39243 (28.57)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="H10" s="2" t="inlineStr">
         <is>
-          <t>maa://32651 (92.86)</t>
+          <t>maa://32651 (93.75)</t>
         </is>
       </c>
       <c r="I10" s="1" t="n"/>
@@ -1741,7 +1741,7 @@
       </c>
       <c r="L10" s="2" t="inlineStr">
         <is>
-          <t>**maa://24395 (43.48)</t>
+          <t>**maa://24395 (44.0)</t>
         </is>
       </c>
       <c r="M10" s="1" t="n"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (93.59), maa://36669 (85.19), *maa://23264 (61.82)</t>
+          <t>maa://28977 (92.41), maa://36669 (85.71), *maa://23264 (61.82)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.18), maa://22755 (86.92), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (95.6), maa://22755 (87.04), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.45), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.46), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (56.0), *maa://22733 (60.0), maa://22761 (100.0)</t>
+          <t>*maa://25021 (53.85), *maa://22733 (58.06), maa://22761 (100.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.66)</t>
+          <t>maa://36707 (99.34)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (87.5)</t>
+          <t>maa://21287 (87.78)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (93.75), maa://22501 (98.15)</t>
+          <t>maa://22747 (93.79), maa://22501 (98.18)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.93)</t>
+          <t>maa://36713 (98.01)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1951,7 +1951,7 @@
       </c>
       <c r="AF11" s="2" t="inlineStr">
         <is>
-          <t>maa://31203 (94.74), ***maa://24394 (19.23)</t>
+          <t>maa://31203 (95.45), ***maa://24394 (19.23)</t>
         </is>
       </c>
       <c r="AG11" s="1" t="n"/>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (90.2)</t>
+          <t>maa://21867 (89.74)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.5), *maa://21485 (77.1), maa://37962 (84.21)</t>
+          <t>maa://22753 (91.5), *maa://21485 (77.44), maa://37962 (85.71)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.51), maa://36677 (92.68), maa://39872 (86.67)</t>
+          <t>maa://23669 (95.19), maa://36677 (93.33), maa://39872 (88.89)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (77.69), *maa://20106 (63.64), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (77.6), *maa://20106 (63.64), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.45), maa://36673 (92.06), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.52), maa://36673 (92.42), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (74.53), **maa://22728 (46.51)</t>
+          <t>*maa://21248 (74.65), **maa://22728 (46.51)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (92.08), *maa://22583 (75.41), *maa://22500 (56.82)</t>
+          <t>maa://22676 (91.26), *maa://22583 (75.41), *maa://22500 (56.82)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>*maa://34957 (77.78), *maa://22768 (51.61)</t>
+          <t>*maa://34957 (77.19), *maa://22768 (51.61)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (30.6), maa://39883 (91.43), *maa://39885 (66.67)</t>
+          <t>**maa://22737 (30.37), maa://39883 (89.74), *maa://39885 (58.33)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>maa://30764 (87.23)</t>
+          <t>maa://30764 (87.76)</t>
         </is>
       </c>
       <c r="E14" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.12), maa://21288 (96.21), maa://36682 (100.0), maa://39841 (93.88)</t>
+          <t>maa://26245 (96.12), maa://21288 (96.21), maa://36682 (100.0), maa://39841 (92.98)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.54), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.56), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2309,7 +2309,7 @@
       </c>
       <c r="X14" s="2" t="inlineStr">
         <is>
-          <t>maa://37468 (87.5)</t>
+          <t>maa://37468 (88.24)</t>
         </is>
       </c>
       <c r="Y14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.35), maa://22734 (83.48), *maa://30808 (65.0), ***maa://36048 (12.12)</t>
+          <t>*maa://22743 (76.88), maa://22734 (83.76), *maa://30808 (63.93), ***maa://36048 (11.76)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.36), maa://21478 (91.18)</t>
+          <t>maa://24304 (88.54), maa://21478 (91.18)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (89.73), *maa://22727 (70.0)</t>
+          <t>maa://24762 (89.86), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.68), *maa://22766 (71.43), *maa://36666 (78.26)</t>
+          <t>maa://21364 (80.74), *maa://22766 (70.75), *maa://36666 (77.03)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.17), maa://36679 (91.43), maa://37650 (96.43)</t>
+          <t>maa://21441 (96.19), maa://36679 (91.89), maa://37650 (96.67)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2500,12 +2500,12 @@
       </c>
       <c r="G16" s="1" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H16" s="2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>maa://43216 (100.0)</t>
         </is>
       </c>
       <c r="I16" s="1" t="n"/>
@@ -2537,7 +2537,7 @@
       </c>
       <c r="P16" s="2" t="inlineStr">
         <is>
-          <t>maa://28504 (90.38)</t>
+          <t>maa://28504 (90.57)</t>
         </is>
       </c>
       <c r="Q16" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (95.24), *maa://28648 (69.64), maa://36674 (81.25)</t>
+          <t>maa://22729 (95.24), *maa://28648 (68.42), maa://36674 (82.86)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (97.67), maa://28051 (95.83)</t>
+          <t>maa://28501 (97.75), maa://28051 (95.83)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.06)</t>
+          <t>maa://26228 (95.18)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (63.16), maa://27755 (92.21)</t>
+          <t>*maa://23911 (63.54), maa://27755 (92.31)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.2), maa://39599 (85.19)</t>
+          <t>maa://22430 (88.2), maa://39599 (85.71)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>***maa://42324 (26.67)</t>
+          <t>**maa://42324 (31.25)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.79)</t>
+          <t>maa://24570 (96.86)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (90.41)</t>
+          <t>maa://24421 (90.13)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="X18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (97.56), maa://22741 (83.33)</t>
+          <t>maa://21917 (97.59), maa://22741 (83.33)</t>
         </is>
       </c>
       <c r="Y18" s="1" t="n"/>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (57.89), **maa://29784 (44.44)</t>
+          <t>*maa://24313 (57.14), **maa://29784 (44.44)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (98.85)</t>
+          <t>maa://24386 (98.89)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (61.56), *maa://36668 (52.17)</t>
+          <t>*maa://30709 (61.99), *maa://36668 (54.17)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -2991,7 +2991,7 @@
       </c>
       <c r="AF19" s="2" t="inlineStr">
         <is>
-          <t>*maa://21663 (61.67)</t>
+          <t>*maa://21663 (61.29)</t>
         </is>
       </c>
       <c r="AG19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.91), maa://25198 (93.68), *maa://20795 (50.4), maa://36680 (100.0)</t>
+          <t>maa://21432 (90.37), maa://25198 (93.81), *maa://20795 (50.4), maa://36680 (96.43)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (88.89)</t>
+          <t>maa://22864 (88.97)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (83.61)</t>
+          <t>maa://41331 (83.82)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="P20" s="2" t="inlineStr">
         <is>
-          <t>maa://37442 (96.88)</t>
+          <t>maa://37442 (96.97)</t>
         </is>
       </c>
       <c r="Q20" s="1" t="n"/>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="T20" s="2" t="inlineStr">
         <is>
-          <t>maa://29113 (88.0)</t>
+          <t>maa://29113 (85.19)</t>
         </is>
       </c>
       <c r="U20" s="1" t="n"/>
@@ -3155,7 +3155,7 @@
       </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>maa://24372 (96.55)</t>
+          <t>maa://24372 (96.63)</t>
         </is>
       </c>
       <c r="I21" s="1" t="n"/>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="X21" s="2" t="inlineStr">
         <is>
-          <t>maa://20110 (86.76), maa://34946 (91.43)</t>
+          <t>maa://20110 (86.76), maa://34946 (91.67)</t>
         </is>
       </c>
       <c r="Y21" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>*maa://21443 (79.1), ***maa://23820 (29.82)</t>
+          <t>*maa://21443 (79.23), ***maa://23820 (29.82)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.02), *maa://22432 (75.44)</t>
+          <t>maa://22524 (94.24), *maa://22432 (75.86)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>maa://25236 (96.05), **maa://21678 (48.94), **maa://22735 (50.0)</t>
+          <t>maa://25236 (96.15), **maa://21678 (48.94), **maa://22735 (50.0)</t>
         </is>
       </c>
       <c r="I22" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (85.87), *maa://22751 (76.19)</t>
+          <t>maa://27127 (86.02), *maa://22751 (75.0)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="T22" s="2" t="inlineStr">
         <is>
-          <t>maa://38495 (88.89)</t>
+          <t>*maa://38495 (80.0)</t>
         </is>
       </c>
       <c r="U22" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.86), *maa://37649 (71.43)</t>
+          <t>maa://21282 (98.32), *maa://37649 (68.18)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="AF22" s="2" t="inlineStr">
         <is>
-          <t>maa://29658 (94.74)</t>
+          <t>maa://29658 (92.68)</t>
         </is>
       </c>
       <c r="AG22" s="1" t="n"/>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.36), *maa://41753 (60.0)</t>
+          <t>***maa://28036 (28.36), *maa://41753 (55.56)</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (93.14), maa://39875 (94.34)</t>
+          <t>maa://39756 (93.12), maa://39875 (94.74)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.33), *maa://29748 (75.2), ***maa://29785 (15.15), *maa://37566 (77.27)</t>
+          <t>maa://30587 (91.53), *maa://29748 (75.4), ***maa://29785 (16.42), *maa://37566 (76.92)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="T23" s="2" t="inlineStr">
         <is>
-          <t>maa://24387 (82.86), maa://31212 (96.0)</t>
+          <t>maa://24387 (83.33), maa://31212 (96.0)</t>
         </is>
       </c>
       <c r="U23" s="1" t="n"/>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="X23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (65.08)</t>
+          <t>*maa://28503 (65.62)</t>
         </is>
       </c>
       <c r="Y23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>maa://24368 (80.42)</t>
+          <t>maa://24368 (80.47)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (85.78), maa://23504 (92.76), **maa://22892 (40.14), *maa://25141 (77.24), *maa://36663 (79.66), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (85.98), maa://23504 (92.88), **maa://22892 (39.86), *maa://25141 (77.42), maa://36663 (80.65), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.34), *maa://36672 (77.78), maa://29910 (94.12), **maa://21440 (34.55)</t>
+          <t>maa://22523 (85.42), *maa://36672 (79.17), maa://29910 (92.31), **maa://21440 (34.55)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (94.92)</t>
+          <t>maa://29753 (95.0)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3691,7 +3691,7 @@
       </c>
       <c r="L25" s="2" t="inlineStr">
         <is>
-          <t>maa://24378 (88.89)</t>
+          <t>maa://24378 (86.49)</t>
         </is>
       </c>
       <c r="M25" s="1" t="n"/>
@@ -3707,7 +3707,7 @@
       </c>
       <c r="P25" s="2" t="inlineStr">
         <is>
-          <t>maa://24382 (92.31)</t>
+          <t>maa://24382 (92.59)</t>
         </is>
       </c>
       <c r="Q25" s="1" t="n"/>
@@ -3718,12 +3718,12 @@
       </c>
       <c r="S25" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="T25" s="2" t="inlineStr">
         <is>
-          <t>maa://20109 (92.12), maa://22545 (100.0)</t>
+          <t>maa://20109 (92.12), maa://22545 (100.0), maa://42915 (100.0)</t>
         </is>
       </c>
       <c r="U25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (84.88), *maa://24516 (79.07), maa://26001 (87.27)</t>
+          <t>maa://31215 (85.06), *maa://24516 (79.07), maa://26001 (87.27)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.18), maa://24621 (96.46), maa://36676 (100.0), maa://22771 (85.71), maa://37772 (100.0)</t>
+          <t>maa://20108 (96.21), maa://24621 (96.49), maa://36676 (96.3), maa://22771 (85.71), maa://37772 (100.0)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (91.78)</t>
+          <t>maa://24913 (90.79)</t>
         </is>
       </c>
       <c r="I26" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (88.1)</t>
+          <t>maa://42235 (90.38)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3901,7 +3901,7 @@
       </c>
       <c r="AF26" s="2" t="inlineStr">
         <is>
-          <t>maa://30511 (84.85), *maa://29760 (61.54)</t>
+          <t>maa://30511 (82.35), *maa://29760 (61.54)</t>
         </is>
       </c>
       <c r="AG26" s="1" t="n"/>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (48.65), maa://34494 (100.0), *maa://39601 (72.73), **maa://36665 (44.44)</t>
+          <t>**maa://21283 (48.65), maa://34494 (96.15), *maa://39601 (69.23), **maa://36665 (44.44)</t>
         </is>
       </c>
       <c r="I27" s="1" t="n"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (75.0)</t>
+          <t>*maa://30624 (73.33)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4031,7 +4031,7 @@
       </c>
       <c r="AF27" s="2" t="inlineStr">
         <is>
-          <t>maa://24023 (96.83)</t>
+          <t>maa://24023 (96.88)</t>
         </is>
       </c>
       <c r="AG27" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.5), maa://25725 (82.93)</t>
+          <t>maa://24465 (90.58), maa://25725 (83.13)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>maa://23263 (94.62), *maa://29765 (60.0)</t>
+          <t>maa://23263 (94.74), *maa://29765 (59.72)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (87.76), ***maa://39723 (14.29), maa://41749 (83.33)</t>
+          <t>maa://39929 (88.48), ***maa://39723 (14.29), maa://41749 (82.14)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.73), *maa://36701 (62.96)</t>
+          <t>maa://36660 (92.93), *maa://36701 (62.96)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>*maa://25175 (70.45)</t>
+          <t>*maa://25175 (71.11)</t>
         </is>
       </c>
       <c r="I29" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.62), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.31), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4227,7 +4227,7 @@
       </c>
       <c r="P29" s="2" t="inlineStr">
         <is>
-          <t>*maa://23168 (55.77), **maa://30050 (38.1)</t>
+          <t>*maa://23168 (55.77), **maa://30050 (40.91)</t>
         </is>
       </c>
       <c r="Q29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.17), ***maa://34960 (8.7), maa://42865 (90.0)</t>
+          <t>*maa://24080 (69.17), ***maa://34960 (8.7), maa://42865 (89.47)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4341,7 +4341,7 @@
       </c>
       <c r="L30" s="2" t="inlineStr">
         <is>
-          <t>maa://30442 (94.64)</t>
+          <t>maa://30442 (94.83)</t>
         </is>
       </c>
       <c r="M30" s="1" t="n"/>
@@ -4389,7 +4389,7 @@
       </c>
       <c r="X30" s="2" t="inlineStr">
         <is>
-          <t>*maa://39477 (80.0)</t>
+          <t>maa://39477 (81.82)</t>
         </is>
       </c>
       <c r="Y30" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (92.86)</t>
+          <t>maa://42979 (95.35)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.39), *maa://36258 (79.75)</t>
+          <t>maa://35926 (93.6), *maa://36258 (80.0)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.02), maa://36667 (98.21), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.04), maa://36667 (98.25), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4601,7 +4601,7 @@
       </c>
       <c r="L32" s="2" t="inlineStr">
         <is>
-          <t>maa://28065 (94.59)</t>
+          <t>maa://28065 (94.74)</t>
         </is>
       </c>
       <c r="M32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (88.89), maa://41238 (95.24), maa://42859 (94.12)</t>
+          <t>maa://41108 (89.13), maa://42859 (91.43), maa://41238 (95.45)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4715,7 +4715,7 @@
       </c>
       <c r="H33" s="2" t="inlineStr">
         <is>
-          <t>**maa://39351 (50.0)</t>
+          <t>**maa://39351 (33.33)</t>
         </is>
       </c>
       <c r="I33" s="1" t="n"/>
@@ -4877,7 +4877,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (93.25)</t>
+          <t>maa://24526 (93.31)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4959,7 +4959,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (98.63)</t>
+          <t>maa://41296 (97.5)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5089,7 +5089,7 @@
       </c>
       <c r="T36" s="2" t="inlineStr">
         <is>
-          <t>maa://27613 (98.97)</t>
+          <t>maa://27613 (98.98)</t>
         </is>
       </c>
       <c r="U36" s="1" t="n"/>
@@ -5139,7 +5139,7 @@
       </c>
       <c r="H37" s="2" t="inlineStr">
         <is>
-          <t>*maa://24374 (57.5)</t>
+          <t>*maa://24374 (58.54)</t>
         </is>
       </c>
       <c r="I37" s="1" t="n"/>
@@ -5171,7 +5171,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (88.83), *maa://21239 (72.73)</t>
+          <t>maa://21280 (88.95), *maa://21239 (72.73)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5272,7 +5272,7 @@
       </c>
       <c r="P38" s="2" t="inlineStr">
         <is>
-          <t>*maa://24383 (66.67)</t>
+          <t>*maa://24383 (67.03)</t>
         </is>
       </c>
       <c r="Q38" s="1" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (84.72)</t>
+          <t>maa://36697 (84.56)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5325,7 +5325,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (85.32), maa://36670 (88.57), maa://30434 (87.5), ***maa://25036 (16.0)</t>
+          <t>maa://25199 (85.32), maa://36670 (88.73), maa://30434 (87.72), ***maa://25036 (16.0)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5357,7 +5357,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (92.38)</t>
+          <t>maa://24709 (91.07)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5442,7 +5442,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.92), maa://21386 (95.68), maa://36664 (91.11)</t>
+          <t>maa://23278 (95.92), maa://21386 (95.7), maa://36664 (91.49)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5495,7 +5495,7 @@
       </c>
       <c r="H41" s="2" t="inlineStr">
         <is>
-          <t>maa://24466 (92.86)</t>
+          <t>maa://24466 (93.02)</t>
         </is>
       </c>
       <c r="I41" s="1" t="n"/>
@@ -5522,12 +5522,12 @@
       </c>
       <c r="O41" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="P41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (38.24)</t>
+          <t>**maa://35616 (38.24), *maa://43177 (66.67)</t>
         </is>
       </c>
       <c r="Q41" s="1" t="n"/>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (92.86), maa://21284 (82.93)</t>
+          <t>maa://22525 (92.25), maa://21284 (82.93)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5679,11 +5679,7 @@
           <t>0</t>
         </is>
       </c>
-      <c r="T43" s="2" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="T43" s="2" t="inlineStr"/>
       <c r="U43" s="1" t="n"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -5702,7 +5698,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.66), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.71), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5755,7 +5751,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (85.56), maa://30807 (95.08), *maa://22767 (55.56), ***maa://20796 (13.79), maa://42459 (100.0)</t>
+          <t>maa://21229 (85.56), maa://30807 (95.08), *maa://22767 (57.89), ***maa://20796 (13.79), *maa://42459 (60.0)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5787,7 +5783,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (46.15)</t>
+          <t>**maa://39364 (50.0)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -5808,7 +5804,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.18)</t>
+          <t>maa://35931 (92.06)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5861,7 +5857,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (95.89), maa://29661 (97.73), maa://28038 (84.62)</t>
+          <t>maa://27410 (95.91), maa://29661 (97.76), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -5983,7 +5979,7 @@
       </c>
       <c r="P49" s="2" t="inlineStr">
         <is>
-          <t>*maa://39643 (66.67)</t>
+          <t>*maa://39643 (72.22)</t>
         </is>
       </c>
       <c r="Q49" s="1" t="n"/>
@@ -6122,7 +6118,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.09), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.17), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6158,7 +6154,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.27)</t>
+          <t>maa://32532 (92.02)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6194,7 +6190,7 @@
       </c>
       <c r="H57" s="2" t="inlineStr">
         <is>
-          <t>maa://25176 (98.0)</t>
+          <t>maa://25176 (98.08)</t>
         </is>
       </c>
       <c r="I57" s="1" t="n"/>
@@ -6212,7 +6208,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (57.14)</t>
+          <t>*maa://37964 (54.55)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>
@@ -6230,7 +6226,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (83.33), maa://31270 (95.19)</t>
+          <t>maa://27746 (83.5), maa://31270 (95.33)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6248,7 +6244,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>**maa://40438 (36.36)</t>
+          <t>**maa://40438 (48.39)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#93)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.94), ***maa://21730 (16.92), ***maa://39501 (17.65), *maa://36675 (60.0)</t>
+          <t>maa://25251 (93.02), ***maa://21730 (16.92), ***maa://39501 (17.65), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (92.59)</t>
+          <t>maa://42407 (92.86)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="P6" s="2" t="inlineStr">
         <is>
-          <t>maa://31836 (89.47), maa://30381 (91.67)</t>
+          <t>maa://31836 (89.47), maa://30381 (92.31)</t>
         </is>
       </c>
       <c r="Q6" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (94.85), *maa://22758 (71.93)</t>
+          <t>maa://22399 (94.89), *maa://22758 (71.93)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.09 17:55:06</t>
+          <t>更新日期：2024.11.10 13:16:41</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (89.58), **maa://22865 (48.98)</t>
+          <t>maa://26206 (89.69), **maa://22865 (48.98)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.86), **maa://32237 (42.5), ***maa://34206 (18.18), ***maa://39951 (15.15), ***maa://39243 (28.57)</t>
+          <t>***maa://25695 (19.32), **maa://32237 (42.5), ***maa://34206 (18.18), ***maa://39951 (17.65), ***maa://39243 (28.57)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (95.6), maa://22755 (87.04), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (95.62), maa://22755 (87.27), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.46), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.47), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.34)</t>
+          <t>maa://36707 (99.35)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (93.79), maa://22501 (98.18)</t>
+          <t>maa://22747 (93.84), maa://22501 (98.18)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (98.01)</t>
+          <t>maa://36713 (98.03)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.19), maa://36677 (93.33), maa://39872 (88.89)</t>
+          <t>maa://23669 (95.19), maa://36677 (93.33), maa://39872 (89.47)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (77.6), *maa://20106 (63.64), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (77.78), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.52), maa://36673 (92.42), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.53), maa://36673 (92.42), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (74.65), **maa://22728 (46.51)</t>
+          <t>*maa://21248 (74.3), **maa://22728 (47.73)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (89.86), *maa://22727 (70.0)</t>
+          <t>maa://24762 (89.93), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.74), *maa://22766 (70.75), *maa://36666 (77.03)</t>
+          <t>maa://21364 (80.74), *maa://22766 (70.75), *maa://36666 (77.33)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.19), maa://36679 (91.89), maa://37650 (96.67)</t>
+          <t>maa://21441 (96.19), maa://36679 (92.31), maa://37650 (96.67)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.86)</t>
+          <t>maa://24570 (96.88)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="X18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (97.59), maa://22741 (83.33)</t>
+          <t>maa://21917 (97.62), maa://22741 (83.33)</t>
         </is>
       </c>
       <c r="Y18" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (98.89)</t>
+          <t>maa://24386 (98.9)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (83.82)</t>
+          <t>maa://41331 (84.06)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="X21" s="2" t="inlineStr">
         <is>
-          <t>maa://20110 (86.76), maa://34946 (91.67)</t>
+          <t>maa://20110 (86.76), maa://34946 (91.89)</t>
         </is>
       </c>
       <c r="Y21" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>*maa://21443 (79.23), ***maa://23820 (29.82)</t>
+          <t>*maa://21443 (79.29), ***maa://23820 (29.82)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (93.12), maa://39875 (94.74)</t>
+          <t>maa://39756 (93.19), maa://39875 (94.74)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (85.98), maa://23504 (92.88), **maa://22892 (39.86), *maa://25141 (77.42), maa://36663 (80.65), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.11), maa://23504 (92.88), **maa://22892 (39.86), *maa://25141 (77.42), maa://36663 (80.65), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.21), maa://24621 (96.49), maa://36676 (96.3), maa://22771 (85.71), maa://37772 (100.0)</t>
+          <t>maa://20108 (96.21), maa://24621 (96.52), maa://36676 (96.3), maa://22771 (85.71), maa://37772 (100.0)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (90.38)</t>
+          <t>maa://42235 (90.57)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4031,7 +4031,7 @@
       </c>
       <c r="AF27" s="2" t="inlineStr">
         <is>
-          <t>maa://24023 (96.88)</t>
+          <t>maa://24023 (96.92)</t>
         </is>
       </c>
       <c r="AG27" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.58), maa://25725 (83.13)</t>
+          <t>maa://24465 (90.59), maa://25725 (83.13)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (88.48), ***maa://39723 (14.29), maa://41749 (82.14)</t>
+          <t>maa://39929 (88.64), ***maa://39723 (14.29), maa://41749 (82.14)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.93), *maa://36701 (62.96)</t>
+          <t>maa://36660 (93.01), *maa://36701 (62.96)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.17), ***maa://34960 (8.7), maa://42865 (89.47)</t>
+          <t>*maa://24080 (69.17), ***maa://34960 (8.7), maa://42865 (90.0)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (95.35)</t>
+          <t>maa://42979 (95.74)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.6), *maa://36258 (80.0)</t>
+          <t>maa://35926 (93.68), *maa://36258 (80.0)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4503,7 +4503,7 @@
       </c>
       <c r="T31" s="2" t="inlineStr">
         <is>
-          <t>maa://30711 (96.43), maa://30768 (100.0)</t>
+          <t>maa://30711 (96.49), maa://30768 (100.0)</t>
         </is>
       </c>
       <c r="U31" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (89.13), maa://42859 (91.43), maa://41238 (95.45)</t>
+          <t>maa://41108 (89.36), maa://42859 (92.5), maa://41238 (95.45)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4877,7 +4877,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (93.31)</t>
+          <t>maa://24526 (93.33)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (84.56)</t>
+          <t>maa://36697 (84.77)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5325,7 +5325,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (85.32), maa://36670 (88.73), maa://30434 (87.72), ***maa://25036 (16.0)</t>
+          <t>maa://25199 (85.32), maa://36670 (87.5), maa://30434 (87.72), ***maa://25036 (16.0)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5751,7 +5751,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (85.56), maa://30807 (95.08), *maa://22767 (57.89), ***maa://20796 (13.79), *maa://42459 (60.0)</t>
+          <t>maa://21229 (85.56), maa://30807 (95.16), *maa://22767 (57.89), ***maa://20796 (13.79), *maa://42459 (60.0)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5804,7 +5804,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.06)</t>
+          <t>maa://35931 (92.09)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5857,7 +5857,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (95.91), maa://29661 (97.76), maa://28038 (84.62)</t>
+          <t>maa://27410 (95.92), maa://29661 (97.76), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -5979,7 +5979,7 @@
       </c>
       <c r="P49" s="2" t="inlineStr">
         <is>
-          <t>*maa://39643 (72.22)</t>
+          <t>*maa://39643 (68.42)</t>
         </is>
       </c>
       <c r="Q49" s="1" t="n"/>
@@ -6154,7 +6154,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.02)</t>
+          <t>maa://32532 (92.05)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6226,7 +6226,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (83.5), maa://31270 (95.33)</t>
+          <t>maa://27746 (83.5), maa://31270 (95.37)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#94)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.16), maa://25390 (95.8), maa://36681 (85.71)</t>
+          <t>maa://24702 (94.16), maa://25390 (95.82), maa://36681 (85.71)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (54.97), *maa://30515 (69.0), *maa://34787 (70.97), ***maa://20792 (11.93), maa://39402 (84.38), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (54.97), *maa://30515 (69.0), *maa://34787 (71.43), ***maa://20792 (11.93), maa://39402 (84.38), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.26), maa://36684 (97.53), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.29), maa://36684 (97.56), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (93.02), ***maa://21730 (16.92), ***maa://39501 (17.65), *maa://36675 (60.0)</t>
+          <t>maa://25251 (91.95), ***maa://21730 (16.92), ***maa://39501 (16.67), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://36987 (93.62), maa://40192 (96.15), maa://39849 (88.89)</t>
+          <t>maa://36987 (93.62), maa://40192 (96.3), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.31), *maa://22748 (75.0)</t>
+          <t>maa://21247 (98.35), *maa://22748 (75.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (68.67), maa://20276 (84.0), *maa://22749 (66.67)</t>
+          <t>*maa://22880 (68.82), maa://20276 (84.11), *maa://22749 (66.67)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.84), maa://26254 (95.65)</t>
+          <t>maa://21249 (94.84), maa://26254 (95.83)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.77), maa://27484 (95.83), maa://27480 (82.35)</t>
+          <t>maa://27396 (84.77), maa://27484 (95.88), maa://27480 (82.35)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -901,7 +901,7 @@
       </c>
       <c r="AF3" s="2" t="inlineStr">
         <is>
-          <t>*maa://21289 (71.43)</t>
+          <t>*maa://21289 (72.73)</t>
         </is>
       </c>
       <c r="AG3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.57), **maa://24303 (33.33), maa://22499 (85.71), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.71), **maa://24303 (33.33), maa://22499 (85.71), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.8), maa://27295 (82.46), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (97.83), maa://27295 (82.46), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (46.85), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (100.0)</t>
+          <t>**maa://32495 (47.06), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (100.0)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (61.36), ***maa://26209 (13.04), *maa://39394 (72.22)</t>
+          <t>*maa://30062 (61.36), ***maa://26209 (13.04), *maa://39394 (73.68)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (82.76), maa://22744 (83.33)</t>
+          <t>maa://21245 (82.35), maa://22744 (83.33)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="P5" s="2" t="inlineStr">
         <is>
-          <t>maa://21919 (95.92), maa://21281 (85.71)</t>
+          <t>maa://21919 (96.0), maa://21281 (85.71)</t>
         </is>
       </c>
       <c r="Q5" s="1" t="n"/>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>maa://24839 (99.24)</t>
+          <t>maa://24839 (99.25)</t>
         </is>
       </c>
       <c r="M6" s="1" t="n"/>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="AF6" s="2" t="inlineStr">
         <is>
-          <t>*maa://33152 (60.53), ***maa://22770 (28.57)</t>
+          <t>*maa://33152 (60.0), ***maa://22770 (28.57)</t>
         </is>
       </c>
       <c r="AG6" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (94.89), *maa://22758 (71.93)</t>
+          <t>maa://22399 (94.93), *maa://22758 (71.93)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (68.0), *maa://36671 (71.74), **maa://42530 (42.86)</t>
+          <t>*maa://26191 (68.0), *maa://36671 (71.74), **maa://42530 (50.0)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.10 13:16:41</t>
+          <t>更新日期：2024.11.13 13:18:25</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (85.71), *maa://21916 (60.0), maa://23252 (92.31), **maa://22759 (45.45), maa://37496 (95.65)</t>
+          <t>maa://32931 (85.11), *maa://21916 (60.0), maa://23252 (92.42), **maa://22759 (45.45), maa://37496 (95.83)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.85)</t>
+          <t>maa://21411 (95.87)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (80.46)</t>
+          <t>maa://22736 (80.68)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.2)</t>
+          <t>maa://26223 (97.25)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.91), ***maa://22740 (5.88), **maa://27377 (46.15), ***maa://25174 (20.0), **maa://39938 (45.0), maa://40166 (87.5)</t>
+          <t>maa://28711 (88.04), ***maa://22740 (5.88), **maa://27377 (46.15), **maa://39938 (45.0), ***maa://25174 (20.0), maa://40166 (90.91)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.32), **maa://32237 (42.5), ***maa://34206 (18.18), ***maa://39951 (17.65), ***maa://39243 (28.57)</t>
+          <t>***maa://25695 (19.32), **maa://32237 (41.46), ***maa://34206 (18.18), ***maa://39951 (17.65), ***maa://39243 (28.57)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (95.62), maa://22755 (87.27), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (95.68), maa://22755 (87.27), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.47), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.51), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.35)</t>
+          <t>maa://36707 (99.36)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (87.78)</t>
+          <t>maa://21287 (87.91)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (93.84), maa://22501 (98.18)</t>
+          <t>maa://22747 (93.2), maa://22501 (98.18)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (98.03)</t>
+          <t>maa://36713 (98.05)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.5), *maa://21485 (77.44), maa://37962 (85.71)</t>
+          <t>maa://22753 (91.5), *maa://21485 (77.44), maa://37962 (86.36)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.19), maa://36677 (93.33), maa://39872 (89.47)</t>
+          <t>maa://23669 (95.26), maa://36677 (93.33), maa://39872 (89.47)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.53), maa://36673 (92.42), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.54), maa://36673 (92.42), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (74.3), **maa://22728 (47.73)</t>
+          <t>*maa://21248 (74.42), **maa://22728 (47.73)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (30.37), maa://39883 (89.74), *maa://39885 (58.33)</t>
+          <t>**maa://22737 (30.37), maa://39883 (90.48), *maa://39885 (58.33)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.12), maa://21288 (96.21), maa://36682 (100.0), maa://39841 (92.98)</t>
+          <t>maa://26245 (96.15), maa://21288 (96.21), maa://36682 (97.3), maa://39841 (93.33)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.56), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.59), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="T14" s="2" t="inlineStr">
         <is>
-          <t>maa://22521 (94.57), maa://42751 (100.0)</t>
+          <t>maa://22521 (94.68), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (76.88), maa://22734 (83.76), *maa://30808 (63.93), ***maa://36048 (11.76)</t>
+          <t>*maa://22743 (77.01), maa://22734 (83.76), *maa://30808 (63.93), ***maa://36048 (14.29)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.54), maa://21478 (91.18)</t>
+          <t>maa://24304 (88.6), maa://21478 (91.18)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (89.93), *maa://22727 (70.0)</t>
+          <t>maa://24762 (90.0), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.74), *maa://22766 (70.75), *maa://36666 (77.33)</t>
+          <t>maa://21364 (80.47), *maa://22766 (71.03), *maa://36666 (77.63)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.19), maa://36679 (92.31), maa://37650 (96.67)</t>
+          <t>maa://21441 (96.21), maa://36679 (92.5), maa://37650 (96.77)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (95.24), *maa://28648 (68.42), maa://36674 (82.86)</t>
+          <t>maa://22729 (95.27), *maa://28648 (68.42), maa://36674 (82.86)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (97.75), maa://28051 (95.83)</t>
+          <t>maa://28501 (97.75), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (63.54), maa://27755 (92.31)</t>
+          <t>*maa://23911 (63.92), maa://27755 (92.41)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.2), maa://39599 (85.71)</t>
+          <t>maa://22430 (88.2), maa://39599 (86.67)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>**maa://42324 (31.25)</t>
+          <t>***maa://42324 (27.78)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.88)</t>
+          <t>maa://24570 (96.89)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (90.13)</t>
+          <t>maa://24421 (90.22)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (88.72), *maa://22732 (51.22)</t>
+          <t>maa://22466 (88.81), *maa://22732 (50.6)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (57.14), **maa://29784 (44.44)</t>
+          <t>*maa://24313 (57.69), **maa://29784 (44.44)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (61.99), *maa://36668 (54.17)</t>
+          <t>*maa://30709 (62.18), *maa://36668 (54.17)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.37), maa://25198 (93.81), *maa://20795 (50.4), maa://36680 (96.43)</t>
+          <t>maa://21432 (90.44), maa://25198 (92.86), *maa://20795 (50.4), maa://36680 (96.43)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (88.97)</t>
+          <t>maa://22864 (88.32)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (84.06)</t>
+          <t>maa://41331 (84.72)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="P20" s="2" t="inlineStr">
         <is>
-          <t>maa://37442 (96.97)</t>
+          <t>maa://37442 (97.22)</t>
         </is>
       </c>
       <c r="Q20" s="1" t="n"/>
@@ -3155,7 +3155,7 @@
       </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>maa://24372 (96.63)</t>
+          <t>maa://24372 (96.67)</t>
         </is>
       </c>
       <c r="I21" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>*maa://21443 (79.29), ***maa://23820 (29.82)</t>
+          <t>*maa://21443 (79.47), ***maa://23820 (29.82)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.24), *maa://22432 (75.86)</t>
+          <t>maa://22524 (94.27), *maa://22432 (75.86)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>maa://25236 (96.15), **maa://21678 (48.94), **maa://22735 (50.0)</t>
+          <t>maa://25236 (96.15), **maa://21678 (48.94), **maa://22735 (42.86)</t>
         </is>
       </c>
       <c r="I22" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (86.02), *maa://22751 (75.0)</t>
+          <t>maa://27127 (86.17), *maa://22751 (75.0)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="T22" s="2" t="inlineStr">
         <is>
-          <t>*maa://38495 (80.0)</t>
+          <t>maa://38495 (81.82)</t>
         </is>
       </c>
       <c r="U22" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.32), *maa://37649 (68.18)</t>
+          <t>maa://21282 (98.34), *maa://37649 (68.18)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (93.19), maa://39875 (94.74)</t>
+          <t>maa://39756 (93.0), maa://39875 (94.74)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.53), *maa://29748 (75.4), ***maa://29785 (16.42), *maa://37566 (76.92)</t>
+          <t>maa://30587 (91.62), *maa://29748 (75.4), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="T23" s="2" t="inlineStr">
         <is>
-          <t>maa://24387 (83.33), maa://31212 (96.0)</t>
+          <t>maa://24387 (83.33), maa://31212 (96.15)</t>
         </is>
       </c>
       <c r="U23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>maa://24368 (80.47)</t>
+          <t>maa://24368 (80.17)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.11), maa://23504 (92.88), **maa://22892 (39.86), *maa://25141 (77.42), maa://36663 (80.65), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.24), maa://23504 (92.93), **maa://22892 (39.86), *maa://25141 (77.42), maa://36663 (80.65), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.0)</t>
+          <t>maa://29753 (95.02)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (74.64), *maa://25311 (74.74), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (74.47), *maa://25311 (75.0), ***maa://22725 (4.84)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3707,7 +3707,7 @@
       </c>
       <c r="P25" s="2" t="inlineStr">
         <is>
-          <t>maa://24382 (92.59)</t>
+          <t>maa://24382 (92.86)</t>
         </is>
       </c>
       <c r="Q25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (85.06), *maa://24516 (79.07), maa://26001 (87.27)</t>
+          <t>maa://31215 (85.56), *maa://24516 (79.07), maa://26001 (87.27)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.21), maa://24621 (96.52), maa://36676 (96.3), maa://22771 (85.71), maa://37772 (100.0)</t>
+          <t>maa://20108 (96.21), maa://24621 (96.52), maa://36676 (96.43), maa://22771 (85.71), maa://37772 (100.0)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (90.79)</t>
+          <t>maa://24913 (90.91)</t>
         </is>
       </c>
       <c r="I26" s="1" t="n"/>
@@ -3837,7 +3837,7 @@
       </c>
       <c r="P26" s="2" t="inlineStr">
         <is>
-          <t>*maa://30968 (58.82), maa://39870 (100.0)</t>
+          <t>*maa://30968 (61.11), maa://39870 (100.0)</t>
         </is>
       </c>
       <c r="Q26" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (90.57)</t>
+          <t>maa://42235 (91.07)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (48.65), maa://34494 (96.15), *maa://39601 (69.23), **maa://36665 (44.44)</t>
+          <t>**maa://21283 (48.65), maa://34494 (96.15), *maa://39601 (71.43), **maa://36665 (44.44)</t>
         </is>
       </c>
       <c r="I27" s="1" t="n"/>
@@ -4031,7 +4031,7 @@
       </c>
       <c r="AF27" s="2" t="inlineStr">
         <is>
-          <t>maa://24023 (96.92)</t>
+          <t>maa://24023 (96.97)</t>
         </is>
       </c>
       <c r="AG27" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.59), maa://25725 (83.13)</t>
+          <t>maa://24465 (90.63), maa://25725 (83.13)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (88.64), ***maa://39723 (14.29), maa://41749 (82.14)</t>
+          <t>maa://39929 (88.64), ***maa://39723 (14.29), maa://41749 (82.76)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.17), ***maa://34960 (8.7), maa://42865 (90.0)</t>
+          <t>*maa://24080 (69.25), ***maa://34960 (8.7), maa://42865 (86.36)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (95.74)</t>
+          <t>maa://42979 (96.08)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.68), *maa://36258 (80.0)</t>
+          <t>maa://35926 (93.75), maa://36258 (80.49)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (89.36), maa://42859 (92.5), maa://41238 (95.45)</t>
+          <t>maa://41108 (87.5), maa://42859 (92.5), maa://41238 (95.74)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4877,7 +4877,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (93.33)</t>
+          <t>maa://24526 (93.36)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4959,7 +4959,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (97.5)</t>
+          <t>maa://41296 (97.59)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5023,7 +5023,7 @@
       </c>
       <c r="AF35" s="2" t="inlineStr">
         <is>
-          <t>maa://39479 (92.31)</t>
+          <t>maa://39479 (92.86)</t>
         </is>
       </c>
       <c r="AG35" s="1" t="n"/>
@@ -5139,7 +5139,7 @@
       </c>
       <c r="H37" s="2" t="inlineStr">
         <is>
-          <t>*maa://24374 (58.54)</t>
+          <t>*maa://24374 (59.52)</t>
         </is>
       </c>
       <c r="I37" s="1" t="n"/>
@@ -5171,7 +5171,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (88.95), *maa://21239 (72.73)</t>
+          <t>maa://21280 (89.01), *maa://21239 (72.73)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5272,7 +5272,7 @@
       </c>
       <c r="P38" s="2" t="inlineStr">
         <is>
-          <t>*maa://24383 (67.03)</t>
+          <t>*maa://24383 (67.39)</t>
         </is>
       </c>
       <c r="Q38" s="1" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (84.77)</t>
+          <t>maa://36697 (85.06)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5325,7 +5325,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (85.32), maa://36670 (87.5), maa://30434 (87.72), ***maa://25036 (16.0)</t>
+          <t>maa://25199 (85.32), maa://36670 (88.0), maa://30434 (88.14), ***maa://25036 (16.0)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5357,7 +5357,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.07)</t>
+          <t>maa://24709 (91.15)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5442,7 +5442,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.92), maa://21386 (95.7), maa://36664 (91.49)</t>
+          <t>maa://23278 (95.92), maa://21386 (95.7), maa://36664 (91.84)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5676,10 +5676,14 @@
       </c>
       <c r="S43" s="1" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="T43" s="2" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T43" s="2" t="inlineStr">
+        <is>
+          <t>maa://43198 (100.0)</t>
+        </is>
+      </c>
       <c r="U43" s="1" t="n"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -5783,7 +5787,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (50.0)</t>
+          <t>**maa://39364 (46.67)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -5804,7 +5808,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.09)</t>
+          <t>maa://35931 (92.19)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5857,7 +5861,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (95.92), maa://29661 (97.76), maa://28038 (84.62)</t>
+          <t>maa://27410 (95.96), maa://29661 (97.76), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -5979,7 +5983,7 @@
       </c>
       <c r="P49" s="2" t="inlineStr">
         <is>
-          <t>*maa://39643 (68.42)</t>
+          <t>*maa://39643 (65.0)</t>
         </is>
       </c>
       <c r="Q49" s="1" t="n"/>
@@ -6118,7 +6122,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.17), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.21), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6208,7 +6212,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (54.55)</t>
+          <t>*maa://37964 (56.52)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>
@@ -6244,7 +6248,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>**maa://40438 (48.39)</t>
+          <t>*maa://40438 (51.52)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#95)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.16), maa://25390 (95.82), maa://36681 (85.71)</t>
+          <t>maa://24702 (94.16), maa://25390 (95.82), maa://36681 (85.92)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.29), maa://36684 (97.56), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.32), maa://36684 (97.56), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (91.95), ***maa://21730 (16.92), ***maa://39501 (16.67), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.05), ***maa://21730 (16.92), ***maa://39501 (16.67), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.83), maa://27295 (82.46), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (97.85), maa://27295 (82.46), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.06), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (100.0)</t>
+          <t>**maa://32495 (47.27), ***maa://31785 (22.22), ***maa://36683 (28.26), *maa://43217 (80.0)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (92.86)</t>
+          <t>maa://42407 (93.1)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="AF6" s="2" t="inlineStr">
         <is>
-          <t>*maa://33152 (60.0), ***maa://22770 (28.57)</t>
+          <t>*maa://33152 (60.0), ***maa://22770 (27.27)</t>
         </is>
       </c>
       <c r="AG6" s="1" t="n"/>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>*maa://22763 (66.67)</t>
+          <t>*maa://22763 (67.86)</t>
         </is>
       </c>
       <c r="I7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.13 13:18:25</t>
+          <t>更新日期：2024.11.14 13:18:07</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (85.11), *maa://21916 (60.0), maa://23252 (92.42), **maa://22759 (45.45), maa://37496 (95.83)</t>
+          <t>maa://32931 (84.21), *maa://21916 (60.0), maa://23252 (92.42), **maa://22759 (45.45), maa://37496 (95.83)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1643,7 +1643,7 @@
       </c>
       <c r="T9" s="2" t="inlineStr">
         <is>
-          <t>**maa://22866 (30.77), maa://26222 (97.56)</t>
+          <t>**maa://22866 (30.77), maa://26222 (97.62)</t>
         </is>
       </c>
       <c r="U9" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.25)</t>
+          <t>maa://26223 (97.27)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (89.69), **maa://22865 (48.98)</t>
+          <t>maa://26206 (89.8), **maa://22865 (48.98)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (92.41), maa://36669 (85.71), *maa://23264 (61.82)</t>
+          <t>maa://28977 (91.25), maa://36669 (86.21), *maa://23264 (61.82)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (95.68), maa://22755 (87.27), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (95.73), maa://22755 (87.39), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.51), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.54), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (53.85), *maa://22733 (58.06), maa://22761 (100.0)</t>
+          <t>*maa://25021 (54.43), *maa://22733 (59.38), maa://22761 (100.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (87.91)</t>
+          <t>maa://21287 (88.04)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (93.2), maa://22501 (98.18)</t>
+          <t>maa://22747 (93.2), maa://22501 (98.21)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (98.05)</t>
+          <t>maa://36713 (98.06)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1951,7 +1951,7 @@
       </c>
       <c r="AF11" s="2" t="inlineStr">
         <is>
-          <t>maa://31203 (95.45), ***maa://24394 (19.23)</t>
+          <t>maa://31203 (95.65), ***maa://24394 (19.23)</t>
         </is>
       </c>
       <c r="AG11" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.5), *maa://21485 (77.44), maa://37962 (86.36)</t>
+          <t>maa://22753 (91.5), *maa://21485 (76.87), maa://37962 (86.36)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.26), maa://36677 (93.33), maa://39872 (89.47)</t>
+          <t>maa://23669 (95.26), maa://36677 (93.33), maa://39872 (90.0)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (74.42), **maa://22728 (47.73)</t>
+          <t>*maa://21248 (74.54), **maa://22728 (47.73)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>*maa://34957 (77.19), *maa://22768 (51.61)</t>
+          <t>*maa://34957 (77.59), *maa://22768 (51.61)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (30.37), maa://39883 (90.48), *maa://39885 (58.33)</t>
+          <t>**maa://22737 (30.37), maa://39883 (90.91), *maa://39885 (58.33)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.15), maa://21288 (96.21), maa://36682 (97.3), maa://39841 (93.33)</t>
+          <t>maa://26245 (96.18), maa://21288 (96.21), maa://36682 (97.3), maa://39841 (93.55)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="AB14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (96.61)</t>
+          <t>maa://22764 (96.67)</t>
         </is>
       </c>
       <c r="AC14" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.6), maa://21478 (91.18)</t>
+          <t>maa://24304 (88.66), maa://21478 (91.18)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.21), maa://36679 (92.5), maa://37650 (96.77)</t>
+          <t>maa://21441 (96.21), maa://36679 (92.68), maa://37650 (96.77)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (95.27), *maa://28648 (68.42), maa://36674 (82.86)</t>
+          <t>maa://22729 (95.27), *maa://28648 (68.42), maa://36674 (83.78)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.89)</t>
+          <t>maa://24570 (96.92)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (90.22)</t>
+          <t>maa://24421 (89.87)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (88.81), *maa://22732 (50.6)</t>
+          <t>maa://22466 (88.89), *maa://22732 (50.6)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="X18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (97.62), maa://22741 (83.33)</t>
+          <t>maa://21917 (97.65), maa://22741 (83.33)</t>
         </is>
       </c>
       <c r="Y18" s="1" t="n"/>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (57.69), **maa://29784 (44.44)</t>
+          <t>*maa://24313 (57.32), **maa://29784 (44.44)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (62.18), *maa://36668 (54.17)</t>
+          <t>*maa://30709 (62.28), *maa://36668 (54.17)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.44), maa://25198 (92.86), *maa://20795 (50.4), maa://36680 (96.43)</t>
+          <t>maa://21432 (90.51), maa://25198 (92.86), *maa://20795 (50.4), maa://36680 (96.43)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (88.32)</t>
+          <t>maa://22864 (88.41)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (84.72)</t>
+          <t>maa://41331 (84.93)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3155,7 +3155,7 @@
       </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>maa://24372 (96.67)</t>
+          <t>maa://24372 (96.7)</t>
         </is>
       </c>
       <c r="I21" s="1" t="n"/>
@@ -3187,7 +3187,7 @@
       </c>
       <c r="P21" s="2" t="inlineStr">
         <is>
-          <t>maa://24381 (85.71)</t>
+          <t>maa://24381 (86.67)</t>
         </is>
       </c>
       <c r="Q21" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>*maa://21443 (79.47), ***maa://23820 (29.82)</t>
+          <t>*maa://21443 (79.59), ***maa://23820 (29.82)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.27), *maa://22432 (75.86)</t>
+          <t>maa://22524 (94.33), *maa://22432 (76.27)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>maa://25236 (96.15), **maa://21678 (48.94), **maa://22735 (42.86)</t>
+          <t>maa://25236 (96.2), **maa://21678 (48.94), **maa://22735 (42.86)</t>
         </is>
       </c>
       <c r="I22" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.34), *maa://37649 (68.18)</t>
+          <t>maa://21282 (98.36), *maa://37649 (68.18)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="AF22" s="2" t="inlineStr">
         <is>
-          <t>maa://29658 (92.68)</t>
+          <t>maa://29658 (92.86)</t>
         </is>
       </c>
       <c r="AG22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (93.0), maa://39875 (94.74)</t>
+          <t>maa://39756 (93.07), maa://39875 (94.74)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3495,7 +3495,7 @@
       </c>
       <c r="AB23" s="2" t="inlineStr">
         <is>
-          <t>maa://29652 (97.37)</t>
+          <t>maa://29652 (97.44)</t>
         </is>
       </c>
       <c r="AC23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>maa://24368 (80.17)</t>
+          <t>maa://24368 (80.23)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.24), maa://23504 (92.93), **maa://22892 (39.86), *maa://25141 (77.42), maa://36663 (80.65), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.3), maa://23504 (92.95), **maa://22892 (39.86), *maa://25141 (77.42), maa://36663 (80.65), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.42), *maa://36672 (79.17), maa://29910 (92.31), **maa://21440 (34.55)</t>
+          <t>maa://22523 (85.42), *maa://36672 (79.59), maa://29910 (92.31), **maa://21440 (34.55)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.02)</t>
+          <t>maa://29753 (95.04)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (74.47), *maa://25311 (75.0), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (74.47), *maa://25311 (75.26), ***maa://22725 (4.84)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3723,7 +3723,7 @@
       </c>
       <c r="T25" s="2" t="inlineStr">
         <is>
-          <t>maa://20109 (92.12), maa://22545 (100.0), maa://42915 (100.0)</t>
+          <t>maa://20109 (92.17), maa://22545 (100.0), maa://42915 (100.0)</t>
         </is>
       </c>
       <c r="U25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (85.56), *maa://24516 (79.07), maa://26001 (87.27)</t>
+          <t>maa://31215 (85.71), *maa://24516 (79.07), maa://26001 (87.27)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.21), maa://24621 (96.52), maa://36676 (96.43), maa://22771 (85.71), maa://37772 (100.0)</t>
+          <t>maa://20108 (96.21), maa://24621 (96.55), maa://36676 (96.43), maa://22771 (85.71), maa://37772 (100.0)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (91.07)</t>
+          <t>maa://42235 (91.38)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>maa://23263 (94.74), *maa://29765 (59.72)</t>
+          <t>maa://23263 (94.79), *maa://29765 (60.27)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (88.64), ***maa://39723 (14.29), maa://41749 (82.76)</t>
+          <t>maa://39929 (88.93), ***maa://39723 (14.29), maa://41749 (82.76)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (93.01), *maa://36701 (62.96)</t>
+          <t>maa://36660 (92.39), *maa://36701 (62.96)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.31), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.33), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.25), ***maa://34960 (8.7), maa://42865 (86.36)</t>
+          <t>*maa://24080 (69.25), ***maa://34960 (8.7), maa://42865 (86.96)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.08)</t>
+          <t>maa://42979 (96.49)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (87.5), maa://42859 (92.5), maa://41238 (95.74)</t>
+          <t>maa://41108 (87.5), maa://42859 (92.86), maa://41238 (95.83)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4877,7 +4877,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (93.36)</t>
+          <t>maa://24526 (93.39)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4959,7 +4959,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (97.59)</t>
+          <t>maa://41296 (95.29)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5089,7 +5089,7 @@
       </c>
       <c r="T36" s="2" t="inlineStr">
         <is>
-          <t>maa://27613 (98.98)</t>
+          <t>maa://27613 (98.99)</t>
         </is>
       </c>
       <c r="U36" s="1" t="n"/>
@@ -5272,7 +5272,7 @@
       </c>
       <c r="P38" s="2" t="inlineStr">
         <is>
-          <t>*maa://24383 (67.39)</t>
+          <t>*maa://24383 (67.74)</t>
         </is>
       </c>
       <c r="Q38" s="1" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (85.06)</t>
+          <t>maa://36697 (85.26)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5442,7 +5442,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.92), maa://21386 (95.7), maa://36664 (91.84)</t>
+          <t>maa://23278 (95.92), maa://21386 (95.7), maa://36664 (90.0)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (92.25), maa://21284 (82.93)</t>
+          <t>maa://22525 (92.25), maa://21284 (83.33)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5755,7 +5755,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (85.56), maa://30807 (95.16), *maa://22767 (57.89), ***maa://20796 (13.79), *maa://42459 (60.0)</t>
+          <t>maa://21229 (85.08), maa://30807 (95.24), *maa://22767 (57.89), ***maa://20796 (13.79), *maa://42459 (60.0)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5787,7 +5787,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (46.67)</t>
+          <t>**maa://39364 (41.18)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -5861,7 +5861,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (95.96), maa://29661 (97.76), maa://28038 (84.62)</t>
+          <t>maa://27410 (95.98), maa://29661 (97.76), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6158,7 +6158,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.05)</t>
+          <t>maa://32532 (92.08)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6194,7 +6194,7 @@
       </c>
       <c r="H57" s="2" t="inlineStr">
         <is>
-          <t>maa://25176 (98.08)</t>
+          <t>maa://25176 (98.11)</t>
         </is>
       </c>
       <c r="I57" s="1" t="n"/>
@@ -6230,7 +6230,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (83.5), maa://31270 (95.37)</t>
+          <t>maa://27746 (83.5), maa://31270 (95.41)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6248,7 +6248,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (51.52)</t>
+          <t>*maa://40438 (54.29)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#96)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.16), maa://25390 (95.82), maa://36681 (85.92)</t>
+          <t>maa://24702 (94.16), maa://25390 (95.82), maa://36681 (86.11)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.32), maa://36684 (97.56), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.32), maa://36684 (97.59), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.05), ***maa://21730 (16.92), ***maa://39501 (16.67), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.22), ***maa://21730 (16.92), ***maa://39501 (15.79), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://36987 (93.62), maa://40192 (96.3), maa://39849 (88.89)</t>
+          <t>maa://36987 (93.62), maa://40192 (96.43), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.35), *maa://22748 (75.0)</t>
+          <t>maa://21247 (98.36), *maa://22748 (75.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (88.46), **maa://20790 (43.94), ***maa://37170 (20.83)</t>
+          <t>maa://24617 (88.46), **maa://20790 (43.94), ***maa://37170 (20.41)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.77), maa://27484 (95.88), maa://27480 (82.35)</t>
+          <t>maa://27396 (84.54), maa://27484 (95.88), maa://27480 (82.35)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.71), **maa://24303 (33.33), maa://22499 (85.71), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.75), **maa://24303 (33.33), maa://22499 (85.71), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.85), maa://27295 (82.46), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (97.87), maa://27295 (82.46), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.27), ***maa://31785 (22.22), ***maa://36683 (28.26), *maa://43217 (80.0)</t>
+          <t>**maa://32495 (47.27), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (86.67)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1015,7 +1015,7 @@
       </c>
       <c r="AB4" s="2" t="inlineStr">
         <is>
-          <t>*maa://32658 (66.67)</t>
+          <t>*maa://32658 (68.42)</t>
         </is>
       </c>
       <c r="AC4" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (61.36), ***maa://26209 (13.04), *maa://39394 (73.68)</t>
+          <t>*maa://30062 (61.36), ***maa://26209 (13.04), *maa://39394 (66.67)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (82.35), maa://22744 (83.33)</t>
+          <t>maa://21245 (82.52), maa://22744 (83.33)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>*maa://22757 (75.86)</t>
+          <t>*maa://22757 (76.67)</t>
         </is>
       </c>
       <c r="M5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (93.1)</t>
+          <t>maa://42407 (93.33)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1280,7 +1280,7 @@
       </c>
       <c r="AB6" s="2" t="inlineStr">
         <is>
-          <t>maa://22739 (92.31)</t>
+          <t>maa://22739 (92.59)</t>
         </is>
       </c>
       <c r="AC6" s="1" t="n"/>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="AF6" s="2" t="inlineStr">
         <is>
-          <t>*maa://33152 (60.0), ***maa://22770 (27.27)</t>
+          <t>*maa://33152 (61.9), ***maa://22770 (27.27)</t>
         </is>
       </c>
       <c r="AG6" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (92.21), maa://24957 (97.62)</t>
+          <t>maa://28624 (92.31), maa://24957 (97.62)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="P7" s="2" t="inlineStr">
         <is>
-          <t>maa://22750 (94.87)</t>
+          <t>maa://22750 (90.24)</t>
         </is>
       </c>
       <c r="Q7" s="1" t="n"/>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="T7" s="2" t="inlineStr">
         <is>
-          <t>maa://21291 (89.74)</t>
+          <t>maa://21291 (87.5)</t>
         </is>
       </c>
       <c r="U7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (94.93), *maa://22758 (71.93)</t>
+          <t>maa://22399 (95.0), *maa://22758 (72.41)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.14 13:18:07</t>
+          <t>更新日期：2024.11.15 13:19:01</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>*maa://21476 (71.11), **maa://39431 (44.44), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (71.74), **maa://39431 (44.44), *maa://37551 (57.14)</t>
         </is>
       </c>
       <c r="E8" s="1" t="n"/>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (84.21), *maa://21916 (60.0), maa://23252 (92.42), **maa://22759 (45.45), maa://37496 (95.83)</t>
+          <t>maa://32931 (84.54), *maa://21916 (60.66), maa://23252 (92.42), maa://37496 (96.0), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.87)</t>
+          <t>maa://21411 (95.9)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>maa://22765 (91.86), *maa://21915 (68.0)</t>
+          <t>maa://22765 (91.95), *maa://21915 (68.0)</t>
         </is>
       </c>
       <c r="E9" s="1" t="n"/>
@@ -1643,7 +1643,7 @@
       </c>
       <c r="T9" s="2" t="inlineStr">
         <is>
-          <t>**maa://22866 (30.77), maa://26222 (97.62)</t>
+          <t>**maa://22866 (30.77), maa://26222 (97.67)</t>
         </is>
       </c>
       <c r="U9" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.27)</t>
+          <t>maa://26223 (97.35)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (88.04), ***maa://22740 (5.88), **maa://27377 (46.15), **maa://39938 (45.0), ***maa://25174 (20.0), maa://40166 (90.91)</t>
+          <t>maa://28711 (88.04), ***maa://22740 (5.88), **maa://39938 (47.62), **maa://27377 (46.15), ***maa://25174 (20.0), maa://40166 (90.91)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (89.8), **maa://22865 (48.98)</t>
+          <t>maa://26206 (89.9), **maa://22865 (48.98)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.32), **maa://32237 (41.46), ***maa://34206 (18.18), ***maa://39951 (17.65), ***maa://39243 (28.57)</t>
+          <t>***maa://25695 (19.32), **maa://32237 (41.46), ***maa://34206 (18.18), ***maa://39951 (20.0), ***maa://39243 (28.57)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1741,7 +1741,7 @@
       </c>
       <c r="L10" s="2" t="inlineStr">
         <is>
-          <t>**maa://24395 (44.0)</t>
+          <t>**maa://24395 (42.31)</t>
         </is>
       </c>
       <c r="M10" s="1" t="n"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (91.25), maa://36669 (86.21), *maa://23264 (61.82)</t>
+          <t>maa://28977 (91.25), maa://36669 (87.1), *maa://23264 (61.82)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.54), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.56), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.36)</t>
+          <t>maa://36707 (99.37)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (98.06)</t>
+          <t>maa://36713 (98.07)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1935,7 +1935,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://22516 (89.29), maa://29912 (100.0), *maa://20794 (52.24)</t>
+          <t>maa://29912 (100.0), maa://22516 (89.41), *maa://20794 (52.24)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>maa://30766 (88.89), **maa://36678 (50.0)</t>
+          <t>maa://30766 (89.29), **maa://36678 (50.0)</t>
         </is>
       </c>
       <c r="E12" s="1" t="n"/>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (89.74)</t>
+          <t>maa://21867 (89.81)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.26), maa://36677 (93.33), maa://39872 (90.0)</t>
+          <t>maa://23669 (95.27), maa://36677 (93.33), maa://39872 (90.0)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (77.78), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (78.12), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.54), maa://36673 (92.42), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.56), maa://36673 (92.42), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (74.54), **maa://22728 (47.73)</t>
+          <t>*maa://21248 (74.19), **maa://22728 (47.73)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (30.37), maa://39883 (90.91), *maa://39885 (58.33)</t>
+          <t>**maa://22737 (30.37), maa://39883 (90.91), *maa://39885 (56.0)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>maa://30764 (87.76)</t>
+          <t>maa://30764 (88.0)</t>
         </is>
       </c>
       <c r="E14" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.18), maa://21288 (96.21), maa://36682 (97.3), maa://39841 (93.55)</t>
+          <t>maa://26245 (96.21), maa://21288 (96.21), maa://36682 (97.3), maa://39841 (93.75)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2309,7 +2309,7 @@
       </c>
       <c r="X14" s="2" t="inlineStr">
         <is>
-          <t>maa://37468 (88.24)</t>
+          <t>maa://37468 (88.89)</t>
         </is>
       </c>
       <c r="Y14" s="1" t="n"/>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="T15" s="2" t="inlineStr">
         <is>
-          <t>maa://23892 (98.65)</t>
+          <t>maa://23892 (98.68)</t>
         </is>
       </c>
       <c r="U15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.47), *maa://22766 (71.03), *maa://36666 (77.63)</t>
+          <t>maa://21364 (80.47), *maa://22766 (71.03), *maa://36666 (78.21)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.21), maa://36679 (92.68), maa://37650 (96.77)</t>
+          <t>maa://21441 (96.23), maa://36679 (92.68), maa://37650 (96.77)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (97.75), maa://28051 (96.0)</t>
+          <t>maa://28501 (97.78), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.18)</t>
+          <t>maa://26228 (95.24)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (63.92), maa://27755 (92.41)</t>
+          <t>*maa://23911 (64.65), maa://27755 (92.41)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>maa://21624 (81.82)</t>
+          <t>maa://21624 (82.35)</t>
         </is>
       </c>
       <c r="E17" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.2), maa://39599 (86.67)</t>
+          <t>maa://22430 (88.33), maa://39599 (86.67)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2667,7 +2667,7 @@
       </c>
       <c r="P17" s="2" t="inlineStr">
         <is>
-          <t>maa://23890 (80.41), *maa://24940 (66.67)</t>
+          <t>maa://23890 (80.81), *maa://24940 (66.67)</t>
         </is>
       </c>
       <c r="Q17" s="1" t="n"/>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>***maa://42324 (27.78)</t>
+          <t>**maa://42324 (31.58)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.92)</t>
+          <t>maa://24570 (96.94)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (88.89), *maa://22732 (50.6)</t>
+          <t>maa://22466 (88.97), *maa://22732 (50.6)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="X18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (97.65), maa://22741 (83.33)</t>
+          <t>maa://21917 (97.67), maa://22741 (83.33)</t>
         </is>
       </c>
       <c r="Y18" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (98.9)</t>
+          <t>maa://24386 (98.91)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (62.28), *maa://36668 (54.17)</t>
+          <t>*maa://30709 (62.47), *maa://36668 (54.17)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.51), maa://25198 (92.86), *maa://20795 (50.4), maa://36680 (96.43)</t>
+          <t>maa://21432 (90.58), maa://25198 (92.86), *maa://20795 (50.4), maa://36680 (96.43)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (88.41)</t>
+          <t>maa://22864 (88.49)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (84.93)</t>
+          <t>maa://41331 (82.89)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="X21" s="2" t="inlineStr">
         <is>
-          <t>maa://20110 (86.76), maa://34946 (91.89)</t>
+          <t>maa://20110 (86.76), maa://34946 (92.11)</t>
         </is>
       </c>
       <c r="Y21" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>*maa://21443 (79.59), ***maa://23820 (29.82)</t>
+          <t>*maa://21443 (79.65), ***maa://23820 (29.82)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.33), *maa://22432 (76.27)</t>
+          <t>maa://22524 (94.36), *maa://22432 (76.27)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>maa://25236 (96.2), **maa://21678 (48.94), **maa://22735 (42.86)</t>
+          <t>maa://25236 (96.25), **maa://21678 (48.94), **maa://22735 (42.86)</t>
         </is>
       </c>
       <c r="I22" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (86.17), *maa://22751 (75.0)</t>
+          <t>maa://27127 (86.46), *maa://22751 (73.85)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.36), *maa://37649 (68.18)</t>
+          <t>maa://21282 (98.38), *maa://37649 (69.57)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="AF22" s="2" t="inlineStr">
         <is>
-          <t>maa://29658 (92.86)</t>
+          <t>maa://29658 (93.02)</t>
         </is>
       </c>
       <c r="AG22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (93.07), maa://39875 (94.74)</t>
+          <t>maa://39756 (92.72), maa://39875 (93.1)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.62), *maa://29748 (75.4), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
+          <t>maa://30587 (91.67), *maa://29748 (75.4), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="T23" s="2" t="inlineStr">
         <is>
-          <t>maa://24387 (83.33), maa://31212 (96.15)</t>
+          <t>maa://24387 (81.08), maa://31212 (96.15)</t>
         </is>
       </c>
       <c r="U23" s="1" t="n"/>
@@ -3511,7 +3511,7 @@
       </c>
       <c r="AF23" s="2" t="inlineStr">
         <is>
-          <t>maa://31489 (93.33)</t>
+          <t>maa://31489 (93.75)</t>
         </is>
       </c>
       <c r="AG23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.3), maa://23504 (92.95), **maa://22892 (39.86), *maa://25141 (77.42), maa://36663 (80.65), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.36), maa://23504 (92.95), **maa://22892 (39.86), *maa://25141 (77.42), maa://36663 (80.65), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (74.47), *maa://25311 (75.26), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (73.61), *maa://25311 (74.49), ***maa://22725 (4.84)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (85.71), *maa://24516 (79.07), maa://26001 (87.27)</t>
+          <t>maa://31215 (84.78), *maa://24516 (79.07), maa://26001 (87.27)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (90.91)</t>
+          <t>maa://24913 (91.14)</t>
         </is>
       </c>
       <c r="I26" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (91.38)</t>
+          <t>maa://42235 (91.53)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3901,7 +3901,7 @@
       </c>
       <c r="AF26" s="2" t="inlineStr">
         <is>
-          <t>maa://30511 (82.35), *maa://29760 (61.54)</t>
+          <t>maa://30511 (82.35), *maa://29760 (64.29)</t>
         </is>
       </c>
       <c r="AG26" s="1" t="n"/>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (48.65), maa://34494 (96.15), *maa://39601 (71.43), **maa://36665 (44.44)</t>
+          <t>**maa://21283 (48.65), maa://34494 (96.15), *maa://39601 (73.33), **maa://36665 (44.44)</t>
         </is>
       </c>
       <c r="I27" s="1" t="n"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (73.33)</t>
+          <t>*maa://30624 (73.91)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.63), maa://25725 (83.13)</t>
+          <t>maa://24465 (90.66), maa://25725 (83.33)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>maa://23263 (94.79), *maa://29765 (60.27)</t>
+          <t>maa://23263 (94.85), *maa://29765 (60.27)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (88.93), ***maa://39723 (14.29), maa://41749 (82.76)</t>
+          <t>maa://39929 (89.05), ***maa://39723 (14.29), maa://41749 (83.87)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4179,7 +4179,7 @@
       </c>
       <c r="D29" s="2" t="inlineStr">
         <is>
-          <t>maa://31694 (98.0)</t>
+          <t>maa://31694 (98.08)</t>
         </is>
       </c>
       <c r="E29" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.33), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.36), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.25), ***maa://34960 (8.7), maa://42865 (86.96)</t>
+          <t>*maa://24080 (69.33), ***maa://34960 (8.7), maa://42865 (87.5)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4341,7 +4341,7 @@
       </c>
       <c r="L30" s="2" t="inlineStr">
         <is>
-          <t>maa://30442 (94.83)</t>
+          <t>maa://30442 (94.92)</t>
         </is>
       </c>
       <c r="M30" s="1" t="n"/>
@@ -4357,7 +4357,7 @@
       </c>
       <c r="P30" s="2" t="inlineStr">
         <is>
-          <t>maa://21442 (99.5)</t>
+          <t>maa://21442 (99.51)</t>
         </is>
       </c>
       <c r="Q30" s="1" t="n"/>
@@ -4389,7 +4389,7 @@
       </c>
       <c r="X30" s="2" t="inlineStr">
         <is>
-          <t>maa://39477 (81.82)</t>
+          <t>maa://39477 (83.33)</t>
         </is>
       </c>
       <c r="Y30" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.49)</t>
+          <t>maa://42979 (96.77)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.75), maa://36258 (80.49)</t>
+          <t>maa://35926 (93.8), maa://36258 (80.72)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4503,7 +4503,7 @@
       </c>
       <c r="T31" s="2" t="inlineStr">
         <is>
-          <t>maa://30711 (96.49), maa://30768 (100.0)</t>
+          <t>maa://30711 (96.61), maa://30768 (100.0)</t>
         </is>
       </c>
       <c r="U31" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (87.5), maa://42859 (92.86), maa://41238 (95.83)</t>
+          <t>maa://41108 (87.5), maa://42859 (93.18), maa://41238 (96.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4747,7 +4747,7 @@
       </c>
       <c r="P33" s="2" t="inlineStr">
         <is>
-          <t>*maa://21956 (79.1), maa://22730 (82.14)</t>
+          <t>*maa://21956 (79.26), maa://22730 (82.14)</t>
         </is>
       </c>
       <c r="Q33" s="1" t="n"/>
@@ -4877,7 +4877,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (93.39)</t>
+          <t>maa://24526 (93.44)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4959,7 +4959,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (95.29)</t>
+          <t>maa://41296 (95.45)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5089,7 +5089,7 @@
       </c>
       <c r="T36" s="2" t="inlineStr">
         <is>
-          <t>maa://27613 (98.99)</t>
+          <t>maa://27613 (99.0)</t>
         </is>
       </c>
       <c r="U36" s="1" t="n"/>
@@ -5171,7 +5171,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.01), *maa://21239 (72.73)</t>
+          <t>maa://21280 (89.12), *maa://21239 (72.73)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5272,7 +5272,7 @@
       </c>
       <c r="P38" s="2" t="inlineStr">
         <is>
-          <t>*maa://24383 (67.74)</t>
+          <t>*maa://24383 (68.09)</t>
         </is>
       </c>
       <c r="Q38" s="1" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (85.26)</t>
+          <t>maa://36697 (85.35)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5325,7 +5325,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (85.32), maa://36670 (88.0), maa://30434 (88.14), ***maa://25036 (16.0)</t>
+          <t>maa://25199 (85.32), maa://36670 (88.16), maa://30434 (88.14), ***maa://25036 (16.0)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5357,7 +5357,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.15)</t>
+          <t>maa://24709 (91.23)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5442,7 +5442,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.92), maa://21386 (95.7), maa://36664 (90.0)</t>
+          <t>maa://23278 (95.92), maa://21386 (95.7), maa://36664 (90.2)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5702,7 +5702,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.71), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.73), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5808,7 +5808,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.19)</t>
+          <t>maa://35931 (92.28)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5861,7 +5861,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (95.98), maa://29661 (97.76), maa://28038 (84.62)</t>
+          <t>maa://27410 (95.99), maa://29661 (97.78), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -5983,7 +5983,7 @@
       </c>
       <c r="P49" s="2" t="inlineStr">
         <is>
-          <t>*maa://39643 (65.0)</t>
+          <t>*maa://39643 (66.67)</t>
         </is>
       </c>
       <c r="Q49" s="1" t="n"/>
@@ -6088,7 +6088,7 @@
       </c>
       <c r="H52" s="2" t="inlineStr">
         <is>
-          <t>maa://24376 (100.0)</t>
+          <t>maa://24376 (96.43)</t>
         </is>
       </c>
       <c r="I52" s="1" t="n"/>
@@ -6122,7 +6122,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.21), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.24), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6158,7 +6158,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.08)</t>
+          <t>maa://32532 (92.15)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6212,7 +6212,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (56.52)</t>
+          <t>*maa://37964 (58.33)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>
@@ -6230,7 +6230,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (83.5), maa://31270 (95.41)</t>
+          <t>maa://27746 (83.5), maa://31270 (95.5)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6248,7 +6248,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (54.29)</t>
+          <t>*maa://40438 (52.78)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>
@@ -6284,7 +6284,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (100.0)</t>
+          <t>maa://42981 (94.74)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#97)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (54.97), *maa://30515 (69.0), *maa://34787 (71.43), ***maa://20792 (11.93), maa://39402 (84.38), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (55.26), *maa://30515 (69.0), *maa://34787 (71.43), ***maa://20792 (11.93), maa://39402 (84.38), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>maa://24839 (99.25)</t>
+          <t>maa://24839 (99.26)</t>
         </is>
       </c>
       <c r="M6" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (68.0), *maa://36671 (71.74), **maa://42530 (50.0)</t>
+          <t>*maa://26191 (68.0), *maa://36671 (71.74), *maa://42530 (55.56)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.15 13:19:01</t>
+          <t>更新日期：2024.11.16 13:18:21</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (84.54), *maa://21916 (60.66), maa://23252 (92.42), maa://37496 (96.0), **maa://22759 (45.45)</t>
+          <t>maa://32931 (84.54), *maa://21916 (60.66), maa://23252 (92.42), maa://37496 (96.15), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.01), maa://22734 (83.76), *maa://30808 (63.93), ***maa://36048 (14.29)</t>
+          <t>*maa://22743 (77.01), maa://22734 (83.76), *maa://30808 (63.93), ***maa://36048 (16.67)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.33), maa://39599 (86.67)</t>
+          <t>maa://22430 (88.33), maa://39599 (83.87)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (98.91)</t>
+          <t>maa://24386 (98.92)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (82.89)</t>
+          <t>maa://41331 (83.12)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.36), *maa://22432 (76.27)</t>
+          <t>maa://22524 (94.39), *maa://22432 (76.27)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (92.72), maa://39875 (93.1)</t>
+          <t>maa://39756 (92.79), maa://39875 (93.1)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.67), *maa://29748 (75.4), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
+          <t>maa://30587 (91.67), *maa://29748 (75.59), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>maa://24368 (80.23)</t>
+          <t>maa://24368 (80.29)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.36), maa://23504 (92.95), **maa://22892 (39.86), *maa://25141 (77.42), maa://36663 (80.65), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.36), maa://23504 (92.95), **maa://22892 (39.86), *maa://25141 (77.42), maa://36663 (80.95), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.04)</t>
+          <t>maa://29753 (95.06)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (91.53)</t>
+          <t>maa://42235 (91.67)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>maa://23263 (94.85), *maa://29765 (60.27)</t>
+          <t>maa://23263 (94.85), *maa://29765 (60.81)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.05), ***maa://39723 (14.29), maa://41749 (83.87)</t>
+          <t>maa://39929 (89.08), ***maa://39723 (14.29), maa://41749 (83.87)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.33), ***maa://34960 (8.7), maa://42865 (87.5)</t>
+          <t>*maa://24080 (69.33), ***maa://34960 (8.7), maa://42865 (88.0)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.77)</t>
+          <t>maa://42979 (96.88)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.8), maa://36258 (80.72)</t>
+          <t>maa://35926 (93.82), maa://36258 (80.72)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.04), maa://36667 (98.25), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.06), maa://36667 (98.25), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (87.5), maa://42859 (93.18), maa://41238 (96.0)</t>
+          <t>maa://41108 (87.5), maa://42859 (93.33), maa://41238 (94.23)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4747,7 +4747,7 @@
       </c>
       <c r="P33" s="2" t="inlineStr">
         <is>
-          <t>*maa://21956 (79.26), maa://22730 (82.14)</t>
+          <t>*maa://21956 (79.41), maa://22730 (82.14)</t>
         </is>
       </c>
       <c r="Q33" s="1" t="n"/>
@@ -4959,7 +4959,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (95.45)</t>
+          <t>maa://41296 (95.56)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (85.35)</t>
+          <t>maa://36697 (85.44)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -6122,7 +6122,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.24), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.26), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6158,7 +6158,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.15)</t>
+          <t>maa://32532 (92.18)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6230,7 +6230,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (83.5), maa://31270 (95.5)</t>
+          <t>maa://27746 (83.5), maa://31270 (95.54)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6284,7 +6284,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (94.74)</t>
+          <t>maa://42981 (95.24)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#98)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (92.31), maa://24957 (97.62)</t>
+          <t>maa://28624 (92.5), maa://24957 (97.62)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (68.0), *maa://36671 (71.74), *maa://42530 (55.56)</t>
+          <t>*maa://26191 (68.0), *maa://36671 (71.74), *maa://42530 (63.64)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.16 13:18:21</t>
+          <t>更新日期：2024.11.17 00:06:00</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.32), **maa://32237 (41.46), ***maa://34206 (18.18), ***maa://39951 (20.0), ***maa://39243 (28.57)</t>
+          <t>***maa://25695 (19.32), **maa://32237 (41.46), ***maa://34206 (18.18), ***maa://39951 (19.44), ***maa://39243 (28.57)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.5), *maa://21485 (76.87), maa://37962 (86.36)</t>
+          <t>maa://22753 (91.5), *maa://21485 (76.87), maa://37962 (86.96)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (95.27), *maa://28648 (68.42), maa://36674 (83.78)</t>
+          <t>maa://22729 (95.27), *maa://28648 (67.24), maa://36674 (84.21)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (64.65), maa://27755 (92.41)</t>
+          <t>*maa://23911 (65.0), maa://27755 (92.41)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (62.47), *maa://36668 (54.17)</t>
+          <t>*maa://30709 (62.56), *maa://36668 (54.17)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (83.12)</t>
+          <t>maa://41331 (83.33)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.39), *maa://22432 (76.27)</t>
+          <t>maa://22524 (94.42), *maa://22432 (76.27)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.38), *maa://37649 (69.57)</t>
+          <t>maa://21282 (98.4), *maa://37649 (69.57)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.08), ***maa://39723 (14.29), maa://41749 (83.87)</t>
+          <t>maa://39929 (89.08), ***maa://39723 (14.29), maa://41749 (84.38)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.33), ***maa://34960 (8.7), maa://42865 (88.0)</t>
+          <t>*maa://24080 (69.33), ***maa://34960 (8.7), maa://42865 (84.62)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.82), maa://36258 (80.72)</t>
+          <t>maa://35926 (93.82), maa://36258 (80.95)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4959,7 +4959,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (95.56)</t>
+          <t>maa://41296 (95.6)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -6158,7 +6158,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.18)</t>
+          <t>maa://32532 (92.21)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#99)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.22), ***maa://21730 (16.92), ***maa://39501 (15.79), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.22), ***maa://21730 (18.18), ***maa://39501 (15.79), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>maa://24370 (96.36)</t>
+          <t>maa://24370 (96.43)</t>
         </is>
       </c>
       <c r="I6" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.17 00:06:00</t>
+          <t>更新日期：2024.11.17 13:18:12</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (84.54), *maa://21916 (60.66), maa://23252 (92.42), maa://37496 (96.15), **maa://22759 (45.45)</t>
+          <t>maa://32931 (84.69), *maa://21916 (60.66), maa://23252 (92.42), maa://37496 (96.15), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (95.73), maa://22755 (87.39), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (95.76), maa://22755 (87.39), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (30.37), maa://39883 (90.91), *maa://39885 (56.0)</t>
+          <t>**maa://22737 (30.37), maa://39883 (91.11), *maa://39885 (56.0)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.21), maa://21288 (96.21), maa://36682 (97.3), maa://39841 (93.75)</t>
+          <t>maa://26245 (96.21), maa://21288 (96.21), maa://36682 (97.3), maa://39841 (93.85)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.24)</t>
+          <t>maa://26228 (95.29)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>**maa://42324 (31.58)</t>
+          <t>**maa://42324 (35.0)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (57.32), **maa://29784 (44.44)</t>
+          <t>*maa://24313 (57.59), **maa://29784 (44.44)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -3901,7 +3901,7 @@
       </c>
       <c r="AF26" s="2" t="inlineStr">
         <is>
-          <t>maa://30511 (82.35), *maa://29760 (64.29)</t>
+          <t>maa://30511 (82.86), *maa://29760 (64.29)</t>
         </is>
       </c>
       <c r="AG26" s="1" t="n"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (73.91)</t>
+          <t>*maa://30624 (74.47)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4389,7 +4389,7 @@
       </c>
       <c r="X30" s="2" t="inlineStr">
         <is>
-          <t>maa://39477 (83.33)</t>
+          <t>maa://39477 (84.62)</t>
         </is>
       </c>
       <c r="Y30" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.88)</t>
+          <t>maa://42979 (96.92)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.06), maa://36667 (98.25), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.06), maa://36667 (98.28), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -5023,7 +5023,7 @@
       </c>
       <c r="AF35" s="2" t="inlineStr">
         <is>
-          <t>maa://39479 (92.86)</t>
+          <t>maa://39479 (93.33)</t>
         </is>
       </c>
       <c r="AG35" s="1" t="n"/>
@@ -5702,7 +5702,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.73), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.74), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -6248,7 +6248,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (52.78)</t>
+          <t>*maa://40438 (54.05)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#100)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.16), maa://25390 (95.82), maa://36681 (86.11)</t>
+          <t>maa://24702 (94.16), maa://25390 (95.82), maa://36681 (86.3)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.32), maa://36684 (97.59), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.32), maa://36684 (97.62), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.36), *maa://22748 (75.0)</t>
+          <t>maa://21247 (98.37), *maa://22748 (75.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (68.82), maa://20276 (84.11), *maa://22749 (66.67)</t>
+          <t>*maa://22880 (69.01), maa://20276 (84.11), *maa://22749 (66.67)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.84), maa://26254 (95.83)</t>
+          <t>maa://21249 (94.86), maa://26254 (95.83)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (82.52), maa://22744 (83.33)</t>
+          <t>maa://21245 (82.61), maa://22744 (83.33)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="AF6" s="2" t="inlineStr">
         <is>
-          <t>*maa://33152 (61.9), ***maa://22770 (27.27)</t>
+          <t>*maa://33152 (60.47), ***maa://22770 (27.27)</t>
         </is>
       </c>
       <c r="AG6" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.0), *maa://22758 (72.41)</t>
+          <t>maa://22399 (95.04), *maa://22758 (72.41)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (68.0), *maa://36671 (71.74), *maa://42530 (63.64)</t>
+          <t>*maa://26191 (68.42), *maa://36671 (70.21), *maa://42530 (63.64)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.17 13:18:12</t>
+          <t>更新日期：2024.11.19 13:18:32</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (84.69), *maa://21916 (60.66), maa://23252 (92.42), maa://37496 (96.15), **maa://22759 (45.45)</t>
+          <t>maa://32931 (84.85), *maa://21916 (60.66), maa://23252 (92.42), maa://37496 (96.15), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (88.04), ***maa://22740 (5.88), **maa://39938 (47.62), **maa://27377 (46.15), ***maa://25174 (20.0), maa://40166 (90.91)</t>
+          <t>maa://28711 (88.3), ***maa://22740 (5.88), **maa://39938 (47.62), **maa://27377 (46.15), ***maa://25174 (20.0), maa://40166 (90.91)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (95.76), maa://22755 (87.39), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (95.78), maa://22755 (87.39), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.56), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.57), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (88.04)</t>
+          <t>maa://21287 (88.17)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (93.2), maa://22501 (98.21)</t>
+          <t>maa://22747 (93.2), maa://22501 (98.28)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (98.07)</t>
+          <t>maa://36713 (98.08)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (89.81)</t>
+          <t>maa://21867 (89.94)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.5), *maa://21485 (76.87), maa://37962 (86.96)</t>
+          <t>maa://22753 (91.61), *maa://21485 (76.87), maa://37962 (86.96)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.56), maa://36673 (92.42), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.59), maa://36673 (92.42), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (91.26), *maa://22583 (75.41), *maa://22500 (56.82)</t>
+          <t>maa://22676 (91.43), *maa://22583 (75.41), *maa://22500 (56.82)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>*maa://34957 (77.59), *maa://22768 (51.61)</t>
+          <t>*maa://34957 (77.97), *maa://22768 (51.61)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (30.37), maa://39883 (91.11), *maa://39885 (56.0)</t>
+          <t>**maa://22737 (30.37), maa://39883 (91.3), *maa://39885 (56.0)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.21), maa://21288 (96.21), maa://36682 (97.3), maa://39841 (93.85)</t>
+          <t>maa://26245 (96.24), maa://21288 (96.21), maa://36682 (97.3), maa://39841 (93.94)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="AB14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (96.67)</t>
+          <t>maa://22764 (96.72)</t>
         </is>
       </c>
       <c r="AC14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.01), maa://22734 (83.76), *maa://30808 (63.93), ***maa://36048 (16.67)</t>
+          <t>*maa://22743 (77.13), maa://22734 (83.76), *maa://30808 (63.93), ***maa://36048 (23.08)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.66), maa://21478 (91.18)</t>
+          <t>maa://24304 (88.72), maa://21478 (91.18)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.23), maa://36679 (92.68), maa://37650 (96.77)</t>
+          <t>maa://21441 (96.24), maa://36679 (92.68), maa://37650 (96.77)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.33), maa://39599 (83.87)</t>
+          <t>maa://22430 (88.4), maa://39599 (84.38)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>**maa://42324 (35.0)</t>
+          <t>**maa://42324 (40.0)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (89.87)</t>
+          <t>maa://24421 (89.91)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (98.92)</t>
+          <t>maa://24386 (98.94)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.58), maa://25198 (92.86), *maa://20795 (50.4), maa://36680 (96.43)</t>
+          <t>maa://21432 (90.78), maa://25198 (92.86), *maa://20795 (50.4), maa://36680 (96.43)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (88.49)</t>
+          <t>maa://22864 (88.57)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (83.33)</t>
+          <t>maa://41331 (82.72)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3139,7 +3139,7 @@
       </c>
       <c r="D21" s="2" t="inlineStr">
         <is>
-          <t>maa://21261 (100.0)</t>
+          <t>maa://21261 (97.37)</t>
         </is>
       </c>
       <c r="E21" s="1" t="n"/>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>maa://25236 (96.25), **maa://21678 (48.94), **maa://22735 (42.86)</t>
+          <t>maa://25236 (96.34), **maa://21678 (48.94), **maa://22735 (42.86)</t>
         </is>
       </c>
       <c r="I22" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.4), *maa://37649 (69.57)</t>
+          <t>maa://21282 (98.41), *maa://37649 (69.57)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.36), *maa://41753 (55.56)</t>
+          <t>***maa://28036 (28.36), **maa://41753 (50.0)</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (92.79), maa://39875 (93.1)</t>
+          <t>maa://39756 (92.99), maa://39875 (93.22)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>maa://24368 (80.29)</t>
+          <t>maa://24368 (80.06)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.36), maa://23504 (92.95), **maa://22892 (39.86), *maa://25141 (77.42), maa://36663 (80.95), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.36), maa://23504 (92.97), **maa://22892 (39.86), *maa://25141 (77.42), maa://36663 (80.95), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.06)</t>
+          <t>maa://29753 (95.08)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (73.61), *maa://25311 (74.49), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (73.79), *maa://25311 (74.49), ***maa://22725 (4.84)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3691,7 +3691,7 @@
       </c>
       <c r="L25" s="2" t="inlineStr">
         <is>
-          <t>maa://24378 (86.49)</t>
+          <t>maa://24378 (86.84)</t>
         </is>
       </c>
       <c r="M25" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (91.67)</t>
+          <t>maa://42235 (91.8)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4081,7 +4081,7 @@
       </c>
       <c r="L28" s="2" t="inlineStr">
         <is>
-          <t>*maa://30770 (79.07)</t>
+          <t>*maa://30770 (79.55)</t>
         </is>
       </c>
       <c r="M28" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>maa://23263 (94.85), *maa://29765 (60.81)</t>
+          <t>maa://23263 (94.85), *maa://29765 (61.33)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.08), ***maa://39723 (14.29), maa://41749 (84.38)</t>
+          <t>maa://39929 (89.2), ***maa://39723 (14.29), maa://41749 (85.29)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.39), *maa://36701 (62.96)</t>
+          <t>maa://36660 (92.47), *maa://36701 (62.96)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.36), *maa://28440 (72.84), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.38), *maa://28440 (73.49), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.33), ***maa://34960 (8.7), maa://42865 (84.62)</t>
+          <t>*maa://24080 (69.41), ***maa://34960 (8.7), maa://42865 (85.19)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.92)</t>
+          <t>maa://42979 (96.97)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.82), maa://36258 (80.95)</t>
+          <t>maa://35926 (93.82), maa://36258 (81.4)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4601,7 +4601,7 @@
       </c>
       <c r="L32" s="2" t="inlineStr">
         <is>
-          <t>maa://28065 (94.74)</t>
+          <t>maa://28065 (94.87)</t>
         </is>
       </c>
       <c r="M32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (87.5), maa://42859 (93.33), maa://41238 (94.23)</t>
+          <t>maa://41108 (87.5), maa://42859 (93.62), maa://41238 (94.74)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4681,7 +4681,7 @@
       </c>
       <c r="AF32" s="2" t="inlineStr">
         <is>
-          <t>maa://42408 (100.0)</t>
+          <t>maa://42408 (85.71)</t>
         </is>
       </c>
       <c r="AG32" s="1" t="n"/>
@@ -4747,7 +4747,7 @@
       </c>
       <c r="P33" s="2" t="inlineStr">
         <is>
-          <t>*maa://21956 (79.41), maa://22730 (82.14)</t>
+          <t>*maa://21956 (79.41), *maa://22730 (79.31)</t>
         </is>
       </c>
       <c r="Q33" s="1" t="n"/>
@@ -4959,7 +4959,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (95.6)</t>
+          <t>maa://41296 (95.7)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5041,7 +5041,7 @@
       </c>
       <c r="H36" s="2" t="inlineStr">
         <is>
-          <t>maa://24375 (92.31)</t>
+          <t>maa://24375 (92.5)</t>
         </is>
       </c>
       <c r="I36" s="1" t="n"/>
@@ -5171,7 +5171,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.12), *maa://21239 (72.73)</t>
+          <t>maa://21280 (89.18), *maa://21239 (72.73)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5272,7 +5272,7 @@
       </c>
       <c r="P38" s="2" t="inlineStr">
         <is>
-          <t>*maa://24383 (68.09)</t>
+          <t>*maa://24383 (68.42)</t>
         </is>
       </c>
       <c r="Q38" s="1" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (85.44)</t>
+          <t>maa://36697 (85.53)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5325,7 +5325,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (85.32), maa://36670 (88.16), maa://30434 (88.14), ***maa://25036 (16.0)</t>
+          <t>maa://25199 (85.32), maa://36670 (88.16), maa://30434 (88.33), ***maa://25036 (16.0)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5357,7 +5357,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.23)</t>
+          <t>maa://24709 (91.3)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5442,7 +5442,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.92), maa://21386 (95.7), maa://36664 (90.2)</t>
+          <t>maa://23278 (95.93), maa://21386 (95.7), maa://36664 (90.2)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5495,7 +5495,7 @@
       </c>
       <c r="H41" s="2" t="inlineStr">
         <is>
-          <t>maa://24466 (93.02)</t>
+          <t>maa://24466 (93.18)</t>
         </is>
       </c>
       <c r="I41" s="1" t="n"/>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (92.25), maa://21284 (83.33)</t>
+          <t>maa://22525 (92.31), maa://21284 (83.33)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5702,7 +5702,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.74), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.75), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5755,7 +5755,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (85.08), maa://30807 (95.24), *maa://22767 (57.89), ***maa://20796 (13.79), *maa://42459 (60.0)</t>
+          <t>maa://21229 (85.08), maa://30807 (95.24), *maa://22767 (57.89), ***maa://20796 (13.79), *maa://42459 (66.67)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5771,7 +5771,7 @@
       </c>
       <c r="P45" s="2" t="inlineStr">
         <is>
-          <t>*maa://36237 (58.33)</t>
+          <t>*maa://36237 (61.54)</t>
         </is>
       </c>
       <c r="Q45" s="1" t="n"/>
@@ -5787,7 +5787,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (41.18)</t>
+          <t>**maa://39364 (38.89)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -5808,7 +5808,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.28)</t>
+          <t>maa://35931 (92.4)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5861,7 +5861,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (95.99), maa://29661 (97.78), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.0), maa://29661 (97.78), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -5983,7 +5983,7 @@
       </c>
       <c r="P49" s="2" t="inlineStr">
         <is>
-          <t>*maa://39643 (66.67)</t>
+          <t>*maa://39643 (68.18)</t>
         </is>
       </c>
       <c r="Q49" s="1" t="n"/>
@@ -6054,7 +6054,7 @@
       </c>
       <c r="H51" s="2" t="inlineStr">
         <is>
-          <t>*maa://30769 (80.0)</t>
+          <t>maa://30769 (81.25)</t>
         </is>
       </c>
       <c r="I51" s="1" t="n"/>
@@ -6122,7 +6122,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.26), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.29), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6158,7 +6158,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.21)</t>
+          <t>maa://32532 (92.28)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6230,7 +6230,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (83.5), maa://31270 (95.54)</t>
+          <t>maa://27746 (82.69), maa://31270 (95.54)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6248,7 +6248,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (54.05)</t>
+          <t>*maa://40438 (55.26)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#101)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.16), maa://25390 (95.82), maa://36681 (86.3)</t>
+          <t>maa://24702 (94.18), maa://25390 (95.83), maa://36681 (86.3)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (88.46), **maa://20790 (43.94), ***maa://37170 (20.41)</t>
+          <t>maa://24617 (88.46), **maa://20790 (43.94), ***maa://37170 (20.0)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (61.36), ***maa://26209 (13.04), *maa://39394 (66.67)</t>
+          <t>*maa://30062 (60.0), ***maa://26209 (13.04), *maa://39394 (66.67)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.19 13:18:32</t>
+          <t>更新日期：2024.11.20 13:18:41</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.9)</t>
+          <t>maa://21411 (95.92)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.59), maa://36673 (92.42), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.61), maa://36673 (92.42), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (91.43), *maa://22583 (75.41), *maa://22500 (56.82)</t>
+          <t>maa://22676 (91.59), *maa://22583 (75.41), *maa://22500 (56.82)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (30.37), maa://39883 (91.3), *maa://39885 (56.0)</t>
+          <t>**maa://22737 (30.37), maa://39883 (91.67), *maa://39885 (56.0)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.24), maa://21288 (96.21), maa://36682 (97.3), maa://39841 (93.94)</t>
+          <t>maa://26245 (96.27), maa://21288 (96.21), maa://36682 (97.3), maa://39841 (94.03)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.13), maa://22734 (83.76), *maa://30808 (63.93), ***maa://36048 (23.08)</t>
+          <t>*maa://22743 (77.13), maa://22734 (83.76), *maa://30808 (63.93), ***maa://36048 (25.0)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.47), *maa://22766 (71.03), *maa://36666 (78.21)</t>
+          <t>maa://21364 (80.54), *maa://22766 (70.37), *maa://36666 (78.21)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.24), maa://36679 (92.68), maa://37650 (96.77)</t>
+          <t>maa://21441 (96.26), maa://36679 (92.68), maa://37650 (96.77)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (95.27), *maa://28648 (67.24), maa://36674 (84.21)</t>
+          <t>maa://22729 (95.3), *maa://28648 (67.24), maa://36674 (84.21)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.4), maa://39599 (84.38)</t>
+          <t>maa://22430 (88.46), maa://39599 (84.38)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.94)</t>
+          <t>maa://24570 (96.95)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (62.56), *maa://36668 (54.17)</t>
+          <t>*maa://30709 (62.56), *maa://36668 (53.42)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (92.99), maa://39875 (93.22)</t>
+          <t>maa://39756 (93.02), maa://39875 (93.22)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.2), ***maa://39723 (14.29), maa://41749 (85.29)</t>
+          <t>maa://39929 (89.2), ***maa://39723 (14.29), maa://41749 (85.71)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.38), *maa://28440 (73.49), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.38), *maa://28440 (73.81), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.97)</t>
+          <t>maa://42979 (97.06)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.06), maa://36667 (98.28), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.09), maa://36667 (98.28), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (87.5), maa://42859 (93.62), maa://41238 (94.74)</t>
+          <t>maa://41108 (87.5), maa://42859 (93.62), maa://41238 (94.92)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (85.53)</t>
+          <t>maa://36697 (85.62)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5357,7 +5357,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.3)</t>
+          <t>maa://24709 (91.38)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5808,7 +5808,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.4)</t>
+          <t>maa://35931 (92.42)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6122,7 +6122,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.29), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.31), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6158,7 +6158,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.28)</t>
+          <t>maa://32532 (92.31)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#102)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.18), maa://25390 (95.83), maa://36681 (86.3)</t>
+          <t>maa://24702 (94.18), maa://25390 (95.85), maa://36681 (86.3)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (68.42), *maa://36671 (70.21), *maa://42530 (63.64)</t>
+          <t>*maa://26191 (67.53), *maa://36671 (70.21), *maa://42530 (63.64)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.20 13:18:41</t>
+          <t>更新日期：2024.11.21 13:18:54</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (84.85), *maa://21916 (60.66), maa://23252 (92.42), maa://37496 (96.15), **maa://22759 (45.45)</t>
+          <t>maa://32931 (85.0), *maa://21916 (60.66), maa://23252 (92.42), maa://37496 (96.15), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.92)</t>
+          <t>maa://21411 (95.94)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (95.78), maa://22755 (87.39), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (95.81), maa://22755 (87.39), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (89.94)</t>
+          <t>maa://21867 (90.0)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.27), maa://21288 (96.21), maa://36682 (97.3), maa://39841 (94.03)</t>
+          <t>maa://26245 (96.27), maa://21288 (96.21), maa://36682 (97.3), maa://39841 (94.12)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (62.56), *maa://36668 (53.42)</t>
+          <t>*maa://30709 (62.56), *maa://36668 (54.05)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (86.46), *maa://22751 (73.85)</t>
+          <t>maa://27127 (86.6), *maa://22751 (73.85)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.2), ***maa://39723 (14.29), maa://41749 (85.71)</t>
+          <t>maa://39929 (89.24), ***maa://39723 (14.29), maa://41749 (85.71)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.06)</t>
+          <t>maa://42979 (97.1)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -5089,7 +5089,7 @@
       </c>
       <c r="T36" s="2" t="inlineStr">
         <is>
-          <t>maa://27613 (99.0)</t>
+          <t>maa://27613 (99.01)</t>
         </is>
       </c>
       <c r="U36" s="1" t="n"/>
@@ -5808,7 +5808,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.42)</t>
+          <t>maa://35931 (92.48)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6158,7 +6158,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.31)</t>
+          <t>maa://32532 (92.34)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#103)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.18), maa://25390 (95.85), maa://36681 (86.3)</t>
+          <t>maa://24702 (94.2), maa://25390 (95.85), maa://36681 (86.3)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (55.26), *maa://30515 (69.0), *maa://34787 (71.43), ***maa://20792 (11.93), maa://39402 (84.38), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (55.26), *maa://30515 (69.0), *maa://34787 (71.88), ***maa://20792 (11.93), maa://39402 (84.38), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.61), *maa://20791 (62.32)</t>
+          <t>maa://22742 (91.67), *maa://20791 (62.32)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (88.46), **maa://20790 (43.94), ***maa://37170 (20.0)</t>
+          <t>maa://24617 (88.57), **maa://20790 (43.94), ***maa://37170 (20.0)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.27), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (86.67)</t>
+          <t>**maa://32495 (47.27), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (87.5)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.21 13:18:54</t>
+          <t>更新日期：2024.11.22 13:18:20</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1561,7 +1561,7 @@
       </c>
       <c r="AF8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24479 (77.92), *maa://21990 (53.85)</t>
+          <t>*maa://24479 (78.21), *maa://21990 (53.85)</t>
         </is>
       </c>
       <c r="AG8" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.35)</t>
+          <t>maa://26223 (97.37)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.37)</t>
+          <t>maa://36707 (99.38)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.27), maa://36677 (93.33), maa://39872 (90.0)</t>
+          <t>maa://23669 (95.27), maa://36677 (93.48), maa://39872 (90.0)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.27), maa://21288 (96.21), maa://36682 (97.3), maa://39841 (94.12)</t>
+          <t>maa://26245 (96.3), maa://21288 (96.21), maa://36682 (97.3), maa://39841 (94.12)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.13), maa://22734 (83.76), *maa://30808 (63.93), ***maa://36048 (25.0)</t>
+          <t>*maa://22743 (77.13), maa://22734 (83.76), *maa://30808 (63.93), ***maa://36048 (26.83)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.29)</t>
+          <t>maa://26228 (95.35)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="X18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (97.67), maa://22741 (83.33)</t>
+          <t>maa://21917 (97.7), maa://22741 (83.33)</t>
         </is>
       </c>
       <c r="Y18" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (88.57)</t>
+          <t>maa://22864 (88.65)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="X21" s="2" t="inlineStr">
         <is>
-          <t>maa://20110 (86.76), maa://34946 (92.11)</t>
+          <t>maa://20110 (86.76), maa://34946 (92.31)</t>
         </is>
       </c>
       <c r="Y21" s="1" t="n"/>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="AF22" s="2" t="inlineStr">
         <is>
-          <t>maa://29658 (93.02)</t>
+          <t>maa://29658 (93.18)</t>
         </is>
       </c>
       <c r="AG22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (93.02), maa://39875 (93.22)</t>
+          <t>maa://39756 (93.06), maa://39875 (93.22)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="T23" s="2" t="inlineStr">
         <is>
-          <t>maa://24387 (81.08), maa://31212 (96.15)</t>
+          <t>maa://24387 (81.08), maa://31212 (96.3)</t>
         </is>
       </c>
       <c r="U23" s="1" t="n"/>
@@ -3495,7 +3495,7 @@
       </c>
       <c r="AB23" s="2" t="inlineStr">
         <is>
-          <t>maa://29652 (97.44)</t>
+          <t>maa://29652 (97.5)</t>
         </is>
       </c>
       <c r="AC23" s="1" t="n"/>
@@ -3739,7 +3739,7 @@
       </c>
       <c r="X25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29890 (75.0)</t>
+          <t>*maa://29890 (75.61)</t>
         </is>
       </c>
       <c r="Y25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (84.78), *maa://24516 (79.07), maa://26001 (87.27)</t>
+          <t>maa://31215 (84.95), *maa://24516 (79.07), maa://26001 (87.27)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3869,7 +3869,7 @@
       </c>
       <c r="X26" s="2" t="inlineStr">
         <is>
-          <t>maa://24389 (96.0)</t>
+          <t>maa://24389 (96.15)</t>
         </is>
       </c>
       <c r="Y26" s="1" t="n"/>
@@ -4031,7 +4031,7 @@
       </c>
       <c r="AF27" s="2" t="inlineStr">
         <is>
-          <t>maa://24023 (96.97)</t>
+          <t>maa://24023 (97.01)</t>
         </is>
       </c>
       <c r="AG27" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.24), ***maa://39723 (14.29), maa://41749 (85.71)</t>
+          <t>maa://39929 (89.27), ***maa://39723 (14.29), maa://41749 (85.71)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.47), *maa://36701 (62.96)</t>
+          <t>maa://36660 (92.49), *maa://36701 (62.96)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4373,7 +4373,7 @@
       </c>
       <c r="T30" s="2" t="inlineStr">
         <is>
-          <t>*maa://32940 (66.67), maa://24388 (94.12)</t>
+          <t>*maa://32940 (66.67), maa://24388 (94.44)</t>
         </is>
       </c>
       <c r="U30" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (87.5), maa://42859 (93.62), maa://41238 (94.92)</t>
+          <t>maa://41108 (87.5), maa://42859 (93.62), maa://41238 (95.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4991,7 +4991,7 @@
       </c>
       <c r="T35" s="2" t="inlineStr">
         <is>
-          <t>maa://24842 (93.88)</t>
+          <t>maa://24842 (94.0)</t>
         </is>
       </c>
       <c r="U35" s="1" t="n"/>
@@ -5089,7 +5089,7 @@
       </c>
       <c r="T36" s="2" t="inlineStr">
         <is>
-          <t>maa://27613 (99.01)</t>
+          <t>maa://27613 (99.02)</t>
         </is>
       </c>
       <c r="U36" s="1" t="n"/>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="T38" s="2" t="inlineStr">
         <is>
-          <t>maa://30713 (96.55)</t>
+          <t>maa://30713 (96.67)</t>
         </is>
       </c>
       <c r="U38" s="1" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (85.62)</t>
+          <t>maa://36697 (85.71)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5357,7 +5357,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.38)</t>
+          <t>maa://24709 (91.45)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5861,7 +5861,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.0), maa://29661 (97.78), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.01), maa://29661 (97.78), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#104)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.86), maa://26254 (95.83)</t>
+          <t>maa://21249 (94.88), maa://26254 (95.83)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (96.36)</t>
+          <t>maa://24390 (96.43)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (82.61), maa://22744 (83.33)</t>
+          <t>maa://21245 (82.61), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="P5" s="2" t="inlineStr">
         <is>
-          <t>maa://21919 (96.0), maa://21281 (85.71)</t>
+          <t>maa://21919 (96.08), maa://21281 (85.71)</t>
         </is>
       </c>
       <c r="Q5" s="1" t="n"/>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="T6" s="2" t="inlineStr">
         <is>
-          <t>maa://37411 (83.33)</t>
+          <t>maa://37411 (84.62)</t>
         </is>
       </c>
       <c r="U6" s="1" t="n"/>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>maa://21955 (93.55)</t>
+          <t>maa://21955 (93.75)</t>
         </is>
       </c>
       <c r="E7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.04), *maa://22758 (72.41)</t>
+          <t>maa://22399 (95.07), *maa://22758 (72.41)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.22 13:18:20</t>
+          <t>更新日期：2024.11.23 13:18:17</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24371 (52.17)</t>
+          <t>*maa://24371 (52.86)</t>
         </is>
       </c>
       <c r="I8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.94)</t>
+          <t>maa://21411 (95.96)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="AF8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24479 (78.21), *maa://21990 (53.85)</t>
+          <t>*maa://24479 (77.22), *maa://21990 (53.85)</t>
         </is>
       </c>
       <c r="AG8" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (95.81), maa://22755 (87.39), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (95.86), maa://22755 (87.39), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (93.2), maa://22501 (98.28)</t>
+          <t>maa://22747 (93.2), maa://22501 (98.33)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (98.08)</t>
+          <t>maa://36713 (98.09)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.61), maa://36673 (92.42), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.62), maa://36673 (92.42), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (91.59), *maa://22583 (75.41), *maa://22500 (56.82)</t>
+          <t>maa://22676 (91.67), *maa://22583 (75.41), *maa://22500 (56.82)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>*maa://34957 (77.97), *maa://22768 (51.61)</t>
+          <t>*maa://34957 (78.33), *maa://22768 (51.61)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.13), maa://22734 (83.76), *maa://30808 (63.93), ***maa://36048 (26.83)</t>
+          <t>*maa://22743 (77.13), maa://22734 (83.76), *maa://30808 (63.93), ***maa://36048 (28.57)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.54), *maa://22766 (70.37), *maa://36666 (78.21)</t>
+          <t>maa://21364 (80.33), *maa://22766 (70.37), *maa://36666 (77.22)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.95)</t>
+          <t>maa://24570 (96.97)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2991,7 +2991,7 @@
       </c>
       <c r="AF19" s="2" t="inlineStr">
         <is>
-          <t>*maa://21663 (61.29)</t>
+          <t>*maa://21663 (61.9)</t>
         </is>
       </c>
       <c r="AG19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.78), maa://25198 (92.86), *maa://20795 (50.4), maa://36680 (96.43)</t>
+          <t>maa://21432 (90.85), maa://25198 (92.93), *maa://20795 (50.79), maa://36680 (96.43)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (82.72)</t>
+          <t>maa://41331 (81.71)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (86.6), *maa://22751 (73.85)</t>
+          <t>maa://27127 (86.73), *maa://22751 (73.85)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (93.06), maa://39875 (93.22)</t>
+          <t>maa://39756 (93.15), maa://39875 (93.22)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.36), maa://23504 (92.97), **maa://22892 (39.86), *maa://25141 (77.42), maa://36663 (80.95), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.36), maa://23504 (93.05), **maa://22892 (39.86), *maa://25141 (77.42), maa://36663 (80.95), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.08)</t>
+          <t>maa://29753 (95.1)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.66), maa://25725 (83.33)</t>
+          <t>maa://24465 (90.67), maa://25725 (83.33)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.27), ***maa://39723 (14.29), maa://41749 (85.71)</t>
+          <t>maa://39929 (89.27), ***maa://39723 (14.29), maa://41749 (86.84)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.49), *maa://36701 (62.96)</t>
+          <t>maa://36660 (92.54), *maa://36701 (62.96)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.1)</t>
+          <t>maa://42979 (97.14)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.82), maa://36258 (81.4)</t>
+          <t>maa://35926 (93.82), maa://36258 (81.61)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.09), maa://36667 (98.28), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.11), maa://36667 (98.28), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (87.5), maa://42859 (93.62), maa://41238 (95.0)</t>
+          <t>maa://41108 (87.5), maa://42859 (93.75), maa://41238 (95.31)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4909,7 +4909,7 @@
       </c>
       <c r="AF34" s="2" t="inlineStr">
         <is>
-          <t>*maa://32650 (64.29)</t>
+          <t>*maa://32650 (66.67)</t>
         </is>
       </c>
       <c r="AG34" s="1" t="n"/>
@@ -4959,7 +4959,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (95.7)</t>
+          <t>maa://41296 (95.88)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (85.71)</t>
+          <t>maa://36697 (85.98)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5325,7 +5325,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (85.32), maa://36670 (88.16), maa://30434 (88.33), ***maa://25036 (16.0)</t>
+          <t>maa://25199 (85.32), maa://36670 (88.16), maa://30434 (88.52), ***maa://25036 (16.0)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5527,7 +5527,7 @@
       </c>
       <c r="P41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (38.24), *maa://43177 (66.67)</t>
+          <t>**maa://35616 (38.24), *maa://43177 (75.0)</t>
         </is>
       </c>
       <c r="Q41" s="1" t="n"/>
@@ -5808,7 +5808,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.48)</t>
+          <t>maa://35931 (92.54)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5861,7 +5861,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.01), maa://29661 (97.78), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.02), maa://29661 (97.78), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6122,7 +6122,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.31), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.33), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#107)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.2), maa://25390 (95.85), maa://36681 (86.3)</t>
+          <t>maa://24702 (94.2), maa://25390 (95.85), maa://36681 (86.67)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (55.26), *maa://30515 (69.0), *maa://34787 (71.88), ***maa://20792 (11.93), maa://39402 (84.38), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (55.26), *maa://30515 (69.0), *maa://34787 (71.88), ***maa://20792 (11.93), maa://39402 (84.85), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.67), *maa://20791 (62.32)</t>
+          <t>maa://22742 (91.72), *maa://20791 (62.32)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.32), maa://36684 (97.62), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.32), maa://36684 (97.65), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.22), ***maa://21730 (18.18), ***maa://39501 (15.79), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.31), ***maa://21730 (18.18), ***maa://39501 (15.79), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.54), maa://27484 (95.88), maa://27480 (82.35)</t>
+          <t>maa://27396 (84.54), maa://27484 (95.92), maa://27480 (82.35)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.75), **maa://24303 (33.33), maa://22499 (85.71), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.79), **maa://24303 (33.33), maa://22499 (85.71), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.27), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (87.5)</t>
+          <t>**maa://32495 (47.27), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (88.24)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (82.61), maa://22744 (84.0)</t>
+          <t>maa://21245 (82.69), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>maa://24370 (96.43)</t>
+          <t>maa://24370 (96.49)</t>
         </is>
       </c>
       <c r="I6" s="1" t="n"/>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="P6" s="2" t="inlineStr">
         <is>
-          <t>maa://31836 (89.47), maa://30381 (92.31)</t>
+          <t>maa://31836 (90.0), maa://30381 (92.31)</t>
         </is>
       </c>
       <c r="Q6" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.23 13:18:17</t>
+          <t>更新日期：2024.11.24 12:07:34</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.37)</t>
+          <t>maa://26223 (97.39)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (95.86), maa://22755 (87.39), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (95.88), maa://22755 (87.39), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (93.2), maa://22501 (98.33)</t>
+          <t>maa://22747 (93.2), maa://22501 (98.36)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (98.09)</t>
+          <t>maa://36713 (98.1)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.62), maa://36673 (92.42), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.63), maa://36673 (92.42), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.3), maa://21288 (96.21), maa://36682 (97.3), maa://39841 (94.12)</t>
+          <t>maa://26245 (96.3), maa://21288 (96.21), maa://36682 (97.37), maa://39841 (94.12)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="AB14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (96.72)</t>
+          <t>maa://22764 (96.77)</t>
         </is>
       </c>
       <c r="AC14" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.26), maa://36679 (92.68), maa://37650 (96.77)</t>
+          <t>maa://21441 (96.28), maa://36679 (92.68), maa://37650 (96.77)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2537,7 +2537,7 @@
       </c>
       <c r="P16" s="2" t="inlineStr">
         <is>
-          <t>maa://28504 (90.57)</t>
+          <t>maa://28504 (90.74)</t>
         </is>
       </c>
       <c r="Q16" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (95.3), *maa://28648 (67.24), maa://36674 (84.21)</t>
+          <t>maa://22729 (95.3), *maa://28648 (67.24), maa://36674 (82.05)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (97.78), maa://28051 (96.0)</t>
+          <t>maa://28501 (97.8), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2813,7 +2813,7 @@
       </c>
       <c r="T18" s="2" t="inlineStr">
         <is>
-          <t>maa://24385 (96.97)</t>
+          <t>maa://24385 (97.06)</t>
         </is>
       </c>
       <c r="U18" s="1" t="n"/>
@@ -2845,7 +2845,7 @@
       </c>
       <c r="AB18" s="2" t="inlineStr">
         <is>
-          <t>maa://24393 (97.3)</t>
+          <t>maa://24393 (97.37)</t>
         </is>
       </c>
       <c r="AC18" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (98.94)</t>
+          <t>maa://24386 (98.95)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.85), maa://25198 (92.93), *maa://20795 (50.79), maa://36680 (96.43)</t>
+          <t>maa://21432 (90.21), maa://25198 (92.93), *maa://20795 (50.79), maa://36680 (96.43)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (81.71)</t>
+          <t>maa://41331 (81.93)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3187,7 +3187,7 @@
       </c>
       <c r="P21" s="2" t="inlineStr">
         <is>
-          <t>maa://24381 (86.67)</t>
+          <t>maa://24381 (87.5)</t>
         </is>
       </c>
       <c r="Q21" s="1" t="n"/>
@@ -3203,7 +3203,7 @@
       </c>
       <c r="T21" s="2" t="inlineStr">
         <is>
-          <t>maa://21993 (88.24)</t>
+          <t>maa://21993 (88.89)</t>
         </is>
       </c>
       <c r="U21" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (93.15), maa://39875 (93.22)</t>
+          <t>maa://39756 (93.21), maa://39875 (93.22)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.36), maa://23504 (93.05), **maa://22892 (39.86), *maa://25141 (77.42), maa://36663 (80.95), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.36), maa://23504 (93.07), **maa://22892 (39.86), *maa://25141 (77.6), maa://36663 (80.95), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.1)</t>
+          <t>maa://29753 (95.12)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3707,7 +3707,7 @@
       </c>
       <c r="P25" s="2" t="inlineStr">
         <is>
-          <t>maa://24382 (92.86)</t>
+          <t>maa://24382 (93.1)</t>
         </is>
       </c>
       <c r="Q25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (84.95), *maa://24516 (79.07), maa://26001 (87.27)</t>
+          <t>maa://31215 (85.11), *maa://24516 (79.07), maa://26001 (87.27)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (91.14)</t>
+          <t>maa://24913 (91.25)</t>
         </is>
       </c>
       <c r="I26" s="1" t="n"/>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (48.65), maa://34494 (96.15), *maa://39601 (73.33), **maa://36665 (44.44)</t>
+          <t>**maa://21283 (48.65), maa://34494 (96.3), *maa://39601 (73.33), **maa://36665 (44.44)</t>
         </is>
       </c>
       <c r="I27" s="1" t="n"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (74.47)</t>
+          <t>*maa://30624 (75.0)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.27), ***maa://39723 (14.29), maa://41749 (86.84)</t>
+          <t>maa://39929 (89.35), ***maa://39723 (14.29), maa://41749 (86.84)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.54), *maa://36701 (62.96)</t>
+          <t>maa://36660 (92.59), *maa://36701 (62.96)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>*maa://25175 (71.11)</t>
+          <t>*maa://25175 (69.57)</t>
         </is>
       </c>
       <c r="I29" s="1" t="n"/>
@@ -4227,7 +4227,7 @@
       </c>
       <c r="P29" s="2" t="inlineStr">
         <is>
-          <t>*maa://23168 (55.77), **maa://30050 (40.91)</t>
+          <t>*maa://23168 (54.72), **maa://30050 (43.48)</t>
         </is>
       </c>
       <c r="Q29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.41), ***maa://34960 (8.7), maa://42865 (85.19)</t>
+          <t>*maa://24080 (69.23), ***maa://34960 (8.33), maa://42865 (82.14)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.14)</t>
+          <t>maa://42979 (97.26)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.82), maa://36258 (81.61)</t>
+          <t>maa://35926 (93.82), maa://36258 (81.82)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (87.5), maa://42859 (93.75), maa://41238 (95.31)</t>
+          <t>maa://41108 (87.76), maa://42859 (93.88), maa://41238 (95.38)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4959,7 +4959,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (95.88)</t>
+          <t>maa://41296 (95.92)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5139,7 +5139,7 @@
       </c>
       <c r="H37" s="2" t="inlineStr">
         <is>
-          <t>*maa://24374 (59.52)</t>
+          <t>*maa://24374 (58.14)</t>
         </is>
       </c>
       <c r="I37" s="1" t="n"/>
@@ -5187,7 +5187,7 @@
       </c>
       <c r="T37" s="2" t="inlineStr">
         <is>
-          <t>**maa://39354 (40.0)</t>
+          <t>**maa://39354 (33.33)</t>
         </is>
       </c>
       <c r="U37" s="1" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (85.98)</t>
+          <t>maa://36697 (86.06)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5325,7 +5325,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (85.32), maa://36670 (88.16), maa://30434 (88.52), ***maa://25036 (16.0)</t>
+          <t>maa://25199 (85.32), maa://36670 (88.46), maa://30434 (88.52), ***maa://25036 (16.0)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5357,7 +5357,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.45)</t>
+          <t>maa://24709 (91.53)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5803,12 +5803,12 @@
       </c>
       <c r="G46" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.54)</t>
+          <t>maa://35931 (92.57), maa://43901 (100.0)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5861,7 +5861,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.02), maa://29661 (97.78), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.05), maa://29661 (97.78), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6088,7 +6088,7 @@
       </c>
       <c r="H52" s="2" t="inlineStr">
         <is>
-          <t>maa://24376 (96.43)</t>
+          <t>maa://24376 (96.55)</t>
         </is>
       </c>
       <c r="I52" s="1" t="n"/>
@@ -6158,7 +6158,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.34)</t>
+          <t>maa://32532 (92.37)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6194,7 +6194,7 @@
       </c>
       <c r="H57" s="2" t="inlineStr">
         <is>
-          <t>maa://25176 (98.11)</t>
+          <t>maa://25176 (98.15)</t>
         </is>
       </c>
       <c r="I57" s="1" t="n"/>
@@ -6248,7 +6248,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (55.26)</t>
+          <t>*maa://40438 (56.41)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>
@@ -6284,7 +6284,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (95.24)</t>
+          <t>maa://42981 (95.45)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#109)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.32), maa://36684 (97.65), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.32), maa://36684 (97.7), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (69.01), maa://20276 (84.11), *maa://22749 (66.67)</t>
+          <t>*maa://22880 (69.01), maa://20276 (84.21), *maa://22749 (66.67)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.88), maa://26254 (95.83)</t>
+          <t>maa://21249 (94.91), maa://26254 (95.83)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.54), maa://27484 (95.92), maa://27480 (82.35)</t>
+          <t>maa://27396 (84.59), maa://27484 (95.92), maa://27480 (82.35)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.87), maa://27295 (82.46), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (97.87), maa://27295 (82.76), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.27), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (88.24)</t>
+          <t>**maa://32495 (47.27), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (88.89)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (92.5), maa://24957 (97.62)</t>
+          <t>maa://28624 (92.59), maa://24957 (97.62)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.07), *maa://22758 (72.41)</t>
+          <t>maa://22399 (95.07), *maa://22758 (72.88)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.24 12:07:34</t>
+          <t>更新日期：2024.11.24 15:31:26</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.96)</t>
+          <t>maa://21411 (95.98)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (91.67), *maa://22583 (75.41), *maa://22500 (56.82)</t>
+          <t>maa://22676 (91.67), *maa://22583 (75.81), *maa://22500 (56.82)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.3), maa://21288 (96.21), maa://36682 (97.37), maa://39841 (94.12)</t>
+          <t>maa://26245 (96.3), maa://21288 (96.21), maa://36682 (97.37), maa://39841 (94.2)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.72), maa://21478 (91.18)</t>
+          <t>maa://24304 (88.78), maa://21478 (91.18)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>**maa://42324 (40.0)</t>
+          <t>**maa://42324 (38.1)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (89.91)</t>
+          <t>maa://24421 (89.96)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (91.8)</t>
+          <t>maa://42235 (91.94)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.35), ***maa://39723 (14.29), maa://41749 (86.84)</t>
+          <t>maa://39929 (89.38), ***maa://39723 (14.29), maa://41749 (86.84)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4681,7 +4681,7 @@
       </c>
       <c r="AF32" s="2" t="inlineStr">
         <is>
-          <t>maa://42408 (85.71)</t>
+          <t>*maa://42408 (75.0)</t>
         </is>
       </c>
       <c r="AG32" s="1" t="n"/>
@@ -5734,7 +5734,7 @@
       </c>
       <c r="T44" s="2" t="inlineStr">
         <is>
-          <t>maa://39366 (85.71)</t>
+          <t>maa://39366 (86.21)</t>
         </is>
       </c>
       <c r="U44" s="1" t="n"/>
@@ -5787,7 +5787,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (38.89)</t>
+          <t>**maa://39364 (36.84)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -5983,7 +5983,7 @@
       </c>
       <c r="P49" s="2" t="inlineStr">
         <is>
-          <t>*maa://39643 (68.18)</t>
+          <t>*maa://39643 (69.57)</t>
         </is>
       </c>
       <c r="Q49" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#110)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.2), maa://25390 (95.85), maa://36681 (86.67)</t>
+          <t>maa://24702 (94.22), maa://25390 (95.87), maa://36681 (86.84)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (55.26), *maa://30515 (69.0), *maa://34787 (71.88), ***maa://20792 (11.93), maa://39402 (84.85), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (55.84), *maa://30515 (69.0), *maa://34787 (72.31), ***maa://20792 (11.93), maa://39402 (85.71), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.72), *maa://20791 (62.32)</t>
+          <t>maa://22742 (91.28), *maa://20791 (62.32)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.32), maa://36684 (97.7), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.32), maa://36684 (96.63), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.31), ***maa://21730 (18.18), ***maa://39501 (15.79), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.39), ***maa://21730 (19.4), ***maa://39501 (15.79), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://36987 (93.62), maa://40192 (96.43), maa://39849 (88.89)</t>
+          <t>maa://36987 (93.62), maa://40192 (96.67), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.37), *maa://22748 (75.0)</t>
+          <t>maa://21247 (98.39), *maa://22748 (75.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (69.01), maa://20276 (84.21), *maa://22749 (66.67)</t>
+          <t>*maa://22880 (68.0), maa://20276 (84.62), *maa://22749 (66.67)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.91), maa://26254 (95.83)</t>
+          <t>maa://21249 (94.52), maa://26254 (95.83)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (88.57), **maa://20790 (43.94), ***maa://37170 (20.0)</t>
+          <t>maa://24617 (88.68), **maa://20790 (44.78), ***maa://37170 (19.61)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.59), maa://27484 (95.92), maa://27480 (82.35)</t>
+          <t>maa://27396 (84.59), maa://27484 (96.0), maa://27480 (82.86)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.79), **maa://24303 (33.33), maa://22499 (85.71), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.15), **maa://24303 (33.33), maa://22499 (85.71), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.87), maa://27295 (82.76), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (97.89), maa://27295 (82.76), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.27), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (88.89)</t>
+          <t>**maa://32495 (47.47), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (91.3)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (82.69), maa://22744 (84.0)</t>
+          <t>maa://21245 (82.94), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (93.33)</t>
+          <t>maa://42407 (93.75)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>maa://24839 (99.26)</t>
+          <t>maa://24839 (99.27)</t>
         </is>
       </c>
       <c r="M6" s="1" t="n"/>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="P6" s="2" t="inlineStr">
         <is>
-          <t>maa://31836 (90.0), maa://30381 (92.31)</t>
+          <t>maa://31836 (90.48), maa://30381 (92.31)</t>
         </is>
       </c>
       <c r="Q6" s="1" t="n"/>
@@ -1280,7 +1280,7 @@
       </c>
       <c r="AB6" s="2" t="inlineStr">
         <is>
-          <t>maa://22739 (92.59)</t>
+          <t>maa://22739 (92.73)</t>
         </is>
       </c>
       <c r="AC6" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (92.59), maa://24957 (97.62)</t>
+          <t>maa://28624 (92.68), maa://24957 (97.62)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="P7" s="2" t="inlineStr">
         <is>
-          <t>maa://22750 (90.24)</t>
+          <t>maa://22750 (90.7)</t>
         </is>
       </c>
       <c r="Q7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (67.53), *maa://36671 (70.21), *maa://42530 (63.64)</t>
+          <t>*maa://26191 (67.95), *maa://36671 (70.21), *maa://42530 (63.64)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.24 15:31:26</t>
+          <t>更新日期：2024.11.30 13:17:44</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (85.0), *maa://21916 (60.66), maa://23252 (92.42), maa://37496 (96.15), **maa://22759 (45.45)</t>
+          <t>maa://32931 (85.15), *maa://21916 (61.29), maa://23252 (92.42), maa://37496 (96.15), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.98)</t>
+          <t>maa://21411 (96.05)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.39)</t>
+          <t>maa://26223 (97.41)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (88.3), ***maa://22740 (5.88), **maa://39938 (47.62), **maa://27377 (46.15), ***maa://25174 (20.0), maa://40166 (90.91)</t>
+          <t>maa://28711 (87.5), ***maa://22740 (5.88), **maa://39938 (50.0), **maa://27377 (46.15), ***maa://25174 (20.0), maa://40166 (90.91)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.32), **maa://32237 (41.46), ***maa://34206 (18.18), ***maa://39951 (19.44), ***maa://39243 (28.57)</t>
+          <t>***maa://25695 (19.32), **maa://32237 (41.46), ***maa://34206 (18.18), ***maa://39951 (18.92), ***maa://39243 (28.57)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (95.88), maa://22755 (87.39), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (95.93), maa://22755 (87.39), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (54.43), *maa://22733 (59.38), maa://22761 (100.0)</t>
+          <t>*maa://25021 (53.75), *maa://22733 (59.38), maa://22761 (100.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (88.17)</t>
+          <t>maa://21287 (88.3)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (93.2), maa://22501 (98.36)</t>
+          <t>maa://22747 (93.24), maa://22501 (98.51)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (98.1)</t>
+          <t>maa://36713 (98.11)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (90.0)</t>
+          <t>maa://21867 (90.12)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.61), *maa://21485 (76.87), maa://37962 (86.96)</t>
+          <t>maa://22753 (91.67), *maa://21485 (76.87), maa://37962 (88.0)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.27), maa://36677 (93.48), maa://39872 (90.0)</t>
+          <t>maa://23669 (95.34), maa://36677 (93.48), maa://39872 (90.0)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.63), maa://36673 (92.42), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.67), maa://36673 (92.65), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (74.19), **maa://22728 (47.73)</t>
+          <t>*maa://21248 (74.55), **maa://22728 (47.73)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (91.67), *maa://22583 (75.81), *maa://22500 (56.82)</t>
+          <t>maa://22676 (91.74), *maa://22583 (75.81), *maa://22500 (56.82)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (30.37), maa://39883 (91.67), *maa://39885 (56.0)</t>
+          <t>**maa://22737 (30.88), maa://39883 (90.0), *maa://39885 (56.0)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.3), maa://21288 (96.21), maa://36682 (97.37), maa://39841 (94.2)</t>
+          <t>maa://26245 (96.32), maa://21288 (96.24), maa://36682 (97.37), maa://39841 (94.44)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.59), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.6), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="T14" s="2" t="inlineStr">
         <is>
-          <t>maa://22521 (94.68), maa://42751 (100.0)</t>
+          <t>maa://22521 (93.68), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="1" t="n"/>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="AB14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (96.77)</t>
+          <t>maa://22764 (96.83)</t>
         </is>
       </c>
       <c r="AC14" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.78), maa://21478 (91.18)</t>
+          <t>maa://24304 (88.78), maa://21478 (91.43)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (90.0), *maa://22727 (70.0)</t>
+          <t>maa://24762 (90.07), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.33), *maa://22766 (70.37), *maa://36666 (77.22)</t>
+          <t>maa://21364 (80.46), *maa://22766 (70.64), *maa://36666 (77.22)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.28), maa://36679 (92.68), maa://37650 (96.77)</t>
+          <t>maa://21441 (96.28), maa://36679 (92.68), maa://37650 (96.88)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (95.3), *maa://28648 (67.24), maa://36674 (82.05)</t>
+          <t>maa://22729 (95.3), *maa://28648 (68.33), maa://36674 (82.05)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (65.0), maa://27755 (92.41)</t>
+          <t>*maa://23911 (65.0), maa://27755 (92.5)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.46), maa://39599 (84.38)</t>
+          <t>maa://22430 (88.52), maa://39599 (84.85)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2667,7 +2667,7 @@
       </c>
       <c r="P17" s="2" t="inlineStr">
         <is>
-          <t>maa://23890 (80.81), *maa://24940 (66.67)</t>
+          <t>maa://23890 (80.81), *maa://24940 (67.86)</t>
         </is>
       </c>
       <c r="Q17" s="1" t="n"/>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>**maa://42324 (38.1)</t>
+          <t>**maa://42324 (43.48)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.97)</t>
+          <t>maa://24570 (97.0)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (89.96)</t>
+          <t>maa://24421 (90.17)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2813,7 +2813,7 @@
       </c>
       <c r="T18" s="2" t="inlineStr">
         <is>
-          <t>maa://24385 (97.06)</t>
+          <t>maa://24385 (97.14)</t>
         </is>
       </c>
       <c r="U18" s="1" t="n"/>
@@ -2845,7 +2845,7 @@
       </c>
       <c r="AB18" s="2" t="inlineStr">
         <is>
-          <t>maa://24393 (97.37)</t>
+          <t>maa://24393 (97.5)</t>
         </is>
       </c>
       <c r="AC18" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (98.95)</t>
+          <t>maa://24386 (98.98)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (62.56), *maa://36668 (54.05)</t>
+          <t>*maa://30709 (62.66), *maa://36668 (54.05)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.21), maa://25198 (92.93), *maa://20795 (50.79), maa://36680 (96.43)</t>
+          <t>maa://21432 (90.28), maa://25198 (92.93), *maa://20795 (50.79), maa://36680 (96.43)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (88.65)</t>
+          <t>maa://22864 (88.81)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (81.93)</t>
+          <t>maa://41331 (82.35)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3155,7 +3155,7 @@
       </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>maa://24372 (96.7)</t>
+          <t>maa://24372 (96.74)</t>
         </is>
       </c>
       <c r="I21" s="1" t="n"/>
@@ -3187,7 +3187,7 @@
       </c>
       <c r="P21" s="2" t="inlineStr">
         <is>
-          <t>maa://24381 (87.5)</t>
+          <t>maa://24381 (88.89)</t>
         </is>
       </c>
       <c r="Q21" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>*maa://21443 (79.65), ***maa://23820 (29.82)</t>
+          <t>*maa://21443 (79.77), ***maa://23820 (29.82)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.42), *maa://22432 (76.27)</t>
+          <t>maa://22524 (94.44), *maa://22432 (76.27)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.41), *maa://37649 (69.57)</t>
+          <t>maa://21282 (98.43), *maa://37649 (70.83)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="AF22" s="2" t="inlineStr">
         <is>
-          <t>maa://29658 (93.18)</t>
+          <t>maa://29658 (93.33)</t>
         </is>
       </c>
       <c r="AG22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (93.21), maa://39875 (93.22)</t>
+          <t>maa://39756 (93.39), maa://39875 (93.33)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.67), *maa://29748 (75.59), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
+          <t>maa://30587 (91.76), *maa://29748 (75.59), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="T23" s="2" t="inlineStr">
         <is>
-          <t>maa://24387 (81.08), maa://31212 (96.3)</t>
+          <t>maa://24387 (81.58), maa://31212 (92.86)</t>
         </is>
       </c>
       <c r="U23" s="1" t="n"/>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="X23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (65.62)</t>
+          <t>*maa://28503 (66.67)</t>
         </is>
       </c>
       <c r="Y23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.36), maa://23504 (93.07), **maa://22892 (39.86), *maa://25141 (77.6), maa://36663 (80.95), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.43), maa://23504 (93.12), **maa://22892 (39.58), *maa://25141 (77.6), maa://36663 (80.95), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3691,7 +3691,7 @@
       </c>
       <c r="L25" s="2" t="inlineStr">
         <is>
-          <t>maa://24378 (86.84)</t>
+          <t>maa://24378 (87.18)</t>
         </is>
       </c>
       <c r="M25" s="1" t="n"/>
@@ -3723,7 +3723,7 @@
       </c>
       <c r="T25" s="2" t="inlineStr">
         <is>
-          <t>maa://20109 (92.17), maa://22545 (100.0), maa://42915 (100.0)</t>
+          <t>maa://20109 (92.26), maa://22545 (100.0), maa://42915 (100.0)</t>
         </is>
       </c>
       <c r="U25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (85.11), *maa://24516 (79.07), maa://26001 (87.27)</t>
+          <t>maa://31215 (85.42), *maa://24516 (79.07), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (91.25)</t>
+          <t>maa://24913 (91.36)</t>
         </is>
       </c>
       <c r="I26" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (91.94)</t>
+          <t>maa://42235 (92.06)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (48.65), maa://34494 (96.3), *maa://39601 (73.33), **maa://36665 (44.44)</t>
+          <t>**maa://21283 (48.65), maa://34494 (96.3), *maa://39601 (75.0), **maa://36665 (44.44)</t>
         </is>
       </c>
       <c r="I27" s="1" t="n"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (75.0)</t>
+          <t>*maa://30624 (75.51)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.67), maa://25725 (83.33)</t>
+          <t>maa://24465 (90.68), maa://25725 (83.33)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.38), ***maa://39723 (14.29), maa://41749 (86.84)</t>
+          <t>maa://39929 (89.08), ***maa://39723 (14.29), maa://41749 (88.64)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.59), *maa://36701 (62.96)</t>
+          <t>maa://36660 (92.36), *maa://36701 (62.96)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.38), *maa://28440 (73.81), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.38), *maa://28440 (75.28), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4227,7 +4227,7 @@
       </c>
       <c r="P29" s="2" t="inlineStr">
         <is>
-          <t>*maa://23168 (54.72), **maa://30050 (43.48)</t>
+          <t>*maa://23168 (54.72), **maa://30050 (50.0)</t>
         </is>
       </c>
       <c r="Q29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.23), ***maa://34960 (8.33), maa://42865 (82.14)</t>
+          <t>*maa://24080 (69.23), ***maa://34960 (8.33), *maa://42865 (80.0)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.26)</t>
+          <t>maa://42979 (97.53)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4466,12 +4466,12 @@
       </c>
       <c r="K31" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.82), maa://36258 (81.82)</t>
+          <t>maa://35926 (93.85), maa://36258 (82.42), maa://43904 (100.0)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.11), maa://36667 (98.28), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.19), maa://36667 (98.28), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (87.76), maa://42859 (93.88), maa://41238 (95.38)</t>
+          <t>maa://41108 (87.76), maa://42859 (94.0), maa://41238 (95.83)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4877,7 +4877,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (93.44)</t>
+          <t>maa://24526 (93.47)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4959,7 +4959,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (95.92)</t>
+          <t>maa://41296 (96.08)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.06)</t>
+          <t>maa://36697 (86.47)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5325,7 +5325,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (85.32), maa://36670 (88.46), maa://30434 (88.52), ***maa://25036 (16.0)</t>
+          <t>maa://25199 (84.55), maa://36670 (87.5), maa://30434 (88.52), ***maa://25036 (16.0)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5357,7 +5357,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.53)</t>
+          <t>maa://24709 (91.67)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5442,7 +5442,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.93), maa://21386 (95.7), maa://36664 (90.2)</t>
+          <t>maa://23278 (95.95), maa://21386 (95.74), maa://36664 (90.2)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (92.31), maa://21284 (83.33)</t>
+          <t>maa://22525 (92.48), maa://21284 (83.72)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5702,7 +5702,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.75), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.77), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5755,7 +5755,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (85.08), maa://30807 (95.24), *maa://22767 (57.89), ***maa://20796 (13.79), *maa://42459 (66.67)</t>
+          <t>maa://21229 (84.78), maa://30807 (95.38), *maa://22767 (55.0), ***maa://20796 (13.79), *maa://42459 (66.67)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5861,7 +5861,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.05), maa://29661 (97.78), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.11), maa://29661 (97.78), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6122,7 +6122,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.33), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.43), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6158,7 +6158,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.37)</t>
+          <t>maa://32532 (92.43)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6212,7 +6212,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (58.33)</t>
+          <t>*maa://37964 (56.0)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>
@@ -6230,7 +6230,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (82.69), maa://31270 (95.54)</t>
+          <t>maa://27746 (82.86), maa://31270 (94.69)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6248,7 +6248,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (56.41)</t>
+          <t>*maa://40438 (55.0)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>
@@ -6284,7 +6284,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (95.45)</t>
+          <t>maa://42981 (95.83)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#111)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.30 13:17:44</t>
+          <t>更新日期：2024.11.30 17:56:43</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.5), ***maa://22740 (5.88), **maa://39938 (50.0), **maa://27377 (46.15), ***maa://25174 (20.0), maa://40166 (90.91)</t>
+          <t>maa://28711 (87.5), ***maa://22740 (5.88), *maa://39938 (52.17), **maa://27377 (46.15), ***maa://25174 (20.0), maa://40166 (91.67)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.32), maa://21288 (96.24), maa://36682 (97.37), maa://39841 (94.44)</t>
+          <t>maa://26245 (96.32), maa://21288 (96.24), maa://36682 (97.37), maa://39841 (94.52)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (95.3), *maa://28648 (68.33), maa://36674 (82.05)</t>
+          <t>maa://22729 (95.33), *maa://28648 (68.33), maa://36674 (82.05)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (97.8), maa://28051 (96.0)</t>
+          <t>maa://28501 (97.83), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (88.97), *maa://22732 (50.6)</t>
+          <t>maa://22466 (89.05), *maa://22732 (50.6)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (62.66), *maa://36668 (54.05)</t>
+          <t>*maa://30709 (62.75), *maa://36668 (54.05)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.44), *maa://22432 (76.27)</t>
+          <t>maa://22524 (94.44), *maa://22432 (76.67)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.43), *maa://37649 (70.83)</t>
+          <t>maa://21282 (98.44), *maa://37649 (70.83)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (93.39), maa://39875 (93.33)</t>
+          <t>maa://39756 (93.45), maa://39875 (93.33)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.08), ***maa://39723 (14.29), maa://41749 (88.64)</t>
+          <t>maa://39929 (89.12), ***maa://39723 (14.29), maa://41749 (88.64)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.53)</t>
+          <t>maa://42979 (97.56)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (87.76), maa://42859 (94.0), maa://41238 (95.83)</t>
+          <t>maa://41108 (87.76), maa://42859 (94.12), maa://41238 (95.83)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -5734,7 +5734,7 @@
       </c>
       <c r="T44" s="2" t="inlineStr">
         <is>
-          <t>maa://39366 (86.21)</t>
+          <t>maa://39366 (86.67)</t>
         </is>
       </c>
       <c r="U44" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#112)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.28), *maa://20791 (62.32)</t>
+          <t>maa://22742 (91.33), *maa://20791 (62.32)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.39), *maa://22748 (75.0)</t>
+          <t>maa://21247 (98.4), *maa://22748 (75.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.15), **maa://24303 (33.33), maa://22499 (85.71), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.2), **maa://24303 (33.33), maa://22499 (85.71), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.30 17:56:43</t>
+          <t>更新日期：2024.11.30 23:36:59</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#113)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.32), maa://36684 (96.63), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.32), maa://36684 (96.67), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.2), **maa://24303 (33.33), maa://22499 (85.71), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.24), **maa://24303 (33.33), maa://22499 (85.71), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.11.30 23:36:59</t>
+          <t>更新日期：2024.12.01 15:12:11</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.41)</t>
+          <t>maa://26223 (97.44)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (98.11)</t>
+          <t>maa://36713 (98.12)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.32), maa://21288 (96.24), maa://36682 (97.37), maa://39841 (94.52)</t>
+          <t>maa://26245 (96.32), maa://21288 (96.24), maa://36682 (97.37), maa://39841 (94.59)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.52), maa://39599 (84.85)</t>
+          <t>maa://22430 (88.52), maa://39599 (85.29)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (88.81)</t>
+          <t>maa://22864 (88.89)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (93.45), maa://39875 (93.33)</t>
+          <t>maa://39756 (93.48), maa://39875 (93.33)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.38), *maa://28440 (75.28), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.4), *maa://28440 (75.28), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://41108 (87.76), maa://42859 (94.12), maa://41238 (95.83)</t>
+          <t>maa://42859 (94.34), maa://41108 (87.76), maa://41238 (95.83)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4747,7 +4747,7 @@
       </c>
       <c r="P33" s="2" t="inlineStr">
         <is>
-          <t>*maa://21956 (79.41), *maa://22730 (79.31)</t>
+          <t>*maa://21956 (79.56), *maa://22730 (79.31)</t>
         </is>
       </c>
       <c r="Q33" s="1" t="n"/>
@@ -5325,7 +5325,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (84.55), maa://36670 (87.5), maa://30434 (88.52), ***maa://25036 (16.0)</t>
+          <t>maa://25199 (84.55), maa://36670 (87.5), maa://30434 (88.71), ***maa://25036 (16.0)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#115)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.22), maa://25390 (95.87), maa://36681 (86.84)</t>
+          <t>maa://24702 (94.22), maa://25390 (95.88), maa://36681 (86.84)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (55.84), *maa://30515 (69.0), *maa://34787 (72.31), ***maa://20792 (11.93), maa://39402 (85.71), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (55.84), *maa://30515 (69.0), *maa://34787 (72.31), ***maa://20792 (11.93), maa://39402 (86.49), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.33), *maa://20791 (62.32)</t>
+          <t>maa://22742 (91.39), *maa://20791 (62.32)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.32), maa://36684 (96.67), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.32), maa://36684 (95.6), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (68.0), maa://20276 (84.62), *maa://22749 (66.67)</t>
+          <t>*maa://22880 (67.42), maa://20276 (84.71), *maa://22749 (66.67)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.52), maa://26254 (95.83)</t>
+          <t>maa://21249 (94.55), maa://26254 (95.83)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (88.68), **maa://20790 (44.78), ***maa://37170 (19.61)</t>
+          <t>maa://24617 (88.79), **maa://20790 (44.78), ***maa://37170 (18.87)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.59), maa://27484 (96.0), maa://27480 (82.86)</t>
+          <t>maa://27396 (84.64), maa://27484 (96.0), maa://27480 (82.86)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.89), maa://27295 (82.76), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (97.89), maa://27295 (83.33), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.47), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (91.3)</t>
+          <t>**maa://32495 (47.67), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (88.89)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>maa://24839 (99.27)</t>
+          <t>maa://24839 (99.28)</t>
         </is>
       </c>
       <c r="M6" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (92.68), maa://24957 (97.62)</t>
+          <t>maa://28624 (92.94), maa://24957 (97.62)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.07), *maa://22758 (72.88)</t>
+          <t>maa://22399 (95.1), *maa://22758 (72.88)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (67.95), *maa://36671 (70.21), *maa://42530 (63.64)</t>
+          <t>*maa://26191 (67.95), *maa://36671 (70.21), *maa://42530 (66.67)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.12.01 15:16:43</t>
+          <t>更新日期：2024.12.07 13:18:04</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (96.05)</t>
+          <t>maa://21411 (95.83)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>maa://22762 (91.67), maa://39552 (90.0)</t>
+          <t>maa://22762 (91.76), maa://39552 (90.0)</t>
         </is>
       </c>
       <c r="M9" s="1" t="n"/>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (80.68)</t>
+          <t>maa://22736 (80.9)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.5), ***maa://22740 (5.88), *maa://39938 (52.17), **maa://27377 (46.15), ***maa://25174 (20.0), maa://40166 (91.67)</t>
+          <t>maa://28711 (86.73), ***maa://22740 (5.88), **maa://39938 (48.0), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (92.86)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (89.9), **maa://22865 (48.98)</t>
+          <t>maa://26206 (89.9), **maa://22865 (50.0)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.32), **maa://32237 (41.46), ***maa://34206 (18.18), ***maa://39951 (18.92), ***maa://39243 (28.57)</t>
+          <t>***maa://25695 (19.21), **maa://32237 (41.46), ***maa://34206 (18.18), ***maa://39951 (17.95), ***maa://39243 (28.57)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (91.25), maa://36669 (87.1), *maa://23264 (61.82)</t>
+          <t>maa://28977 (91.36), maa://36669 (87.88), *maa://23264 (61.82)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.57), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.58), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.38)</t>
+          <t>maa://36707 (99.39)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (98.12)</t>
+          <t>maa://36713 (98.14)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.67), *maa://21485 (76.87), maa://37962 (88.0)</t>
+          <t>maa://22753 (91.19), *maa://21485 (76.87), maa://37962 (88.89)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.34), maa://36677 (93.48), maa://39872 (90.0)</t>
+          <t>maa://23669 (95.34), maa://36677 (93.62), maa://39872 (90.0)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.12), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (78.29), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.67), maa://36673 (92.65), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.7), maa://36673 (92.65), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (91.74), *maa://22583 (75.81), *maa://22500 (56.82)</t>
+          <t>maa://22676 (91.74), *maa://22583 (75.81), *maa://22500 (57.78)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>*maa://34957 (78.33), *maa://22768 (51.61)</t>
+          <t>*maa://34957 (78.69), *maa://22768 (51.61)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (30.88), maa://39883 (90.0), *maa://39885 (56.0)</t>
+          <t>**maa://22737 (31.39), maa://39883 (90.57), *maa://39885 (56.0)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.32), maa://21288 (96.24), maa://36682 (97.37), maa://39841 (94.59)</t>
+          <t>maa://26245 (96.38), maa://21288 (96.24), maa://39841 (94.81), maa://36682 (97.37)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.6), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.61), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.13), maa://22734 (83.76), *maa://30808 (63.93), ***maa://36048 (28.57)</t>
+          <t>*maa://22743 (76.84), maa://22734 (83.76), *maa://30808 (63.93), ***maa://36048 (28.57)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.78), maa://21478 (91.43)</t>
+          <t>maa://24304 (88.5), maa://21478 (91.43)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.46), *maa://22766 (70.64), *maa://36666 (77.22)</t>
+          <t>maa://21364 (80.53), *maa://22766 (70.64), *maa://36666 (77.78)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (95.33), *maa://28648 (68.33), maa://36674 (82.05)</t>
+          <t>maa://22729 (95.33), *maa://28648 (68.33), maa://36674 (82.5)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.52), maa://39599 (85.29)</t>
+          <t>maa://22430 (88.52), maa://39599 (85.71)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>**maa://42324 (43.48)</t>
+          <t>**maa://42324 (45.83)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.0)</t>
+          <t>maa://24570 (97.03)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (89.05), *maa://22732 (50.6)</t>
+          <t>maa://22466 (89.29), *maa://22732 (50.6)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (98.98)</t>
+          <t>maa://24386 (98.99)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (62.75), *maa://36668 (54.05)</t>
+          <t>*maa://30709 (62.84), *maa://36668 (54.67)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -2991,7 +2991,7 @@
       </c>
       <c r="AF19" s="2" t="inlineStr">
         <is>
-          <t>*maa://21663 (61.9)</t>
+          <t>*maa://21663 (62.5)</t>
         </is>
       </c>
       <c r="AG19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.28), maa://25198 (92.93), *maa://20795 (50.79), maa://36680 (96.43)</t>
+          <t>maa://21432 (89.73), maa://25198 (92.93), *maa://20795 (51.18), maa://36680 (96.55)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (88.89)</t>
+          <t>maa://22864 (88.97)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (82.35)</t>
+          <t>maa://41331 (83.7)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>*maa://21443 (79.77), ***maa://23820 (29.82)</t>
+          <t>*maa://21443 (79.94), ***maa://23820 (29.82)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.44), *maa://22432 (76.67)</t>
+          <t>maa://22524 (94.53), *maa://22432 (76.67)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (86.73), *maa://22751 (73.85)</t>
+          <t>maa://27127 (86.0), *maa://22751 (73.85)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.44), *maa://37649 (70.83)</t>
+          <t>maa://21282 (98.45), *maa://37649 (68.0)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="AF22" s="2" t="inlineStr">
         <is>
-          <t>maa://29658 (93.33)</t>
+          <t>maa://29658 (93.48)</t>
         </is>
       </c>
       <c r="AG22" s="1" t="n"/>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.36), **maa://41753 (50.0)</t>
+          <t>***maa://28036 (28.36), *maa://41753 (54.55)</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (93.48), maa://39875 (93.33)</t>
+          <t>maa://39756 (93.72), maa://39875 (93.55)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.76), *maa://29748 (75.59), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
+          <t>maa://30587 (91.8), *maa://29748 (75.59), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.43), maa://23504 (93.12), **maa://22892 (39.58), *maa://25141 (77.6), maa://36663 (80.95), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.55), maa://23504 (93.18), **maa://22892 (39.58), *maa://25141 (77.6), maa://36663 (81.25), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.42), *maa://36672 (79.59), maa://29910 (92.31), **maa://21440 (34.55)</t>
+          <t>maa://22523 (85.42), maa://36672 (80.39), maa://29910 (92.31), **maa://21440 (34.55)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.12)</t>
+          <t>maa://29753 (95.18)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (73.79), *maa://25311 (74.49), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (73.97), *maa://25311 (73.74), ***maa://22725 (4.84)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3723,7 +3723,7 @@
       </c>
       <c r="T25" s="2" t="inlineStr">
         <is>
-          <t>maa://20109 (92.26), maa://22545 (100.0), maa://42915 (100.0)</t>
+          <t>maa://20109 (92.31), maa://22545 (100.0), maa://42915 (100.0)</t>
         </is>
       </c>
       <c r="U25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (85.42), *maa://24516 (79.07), maa://26001 (87.5)</t>
+          <t>maa://31215 (85.42), *maa://24516 (79.31), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.21), maa://24621 (96.55), maa://36676 (96.43), maa://22771 (85.71), maa://37772 (100.0)</t>
+          <t>maa://20108 (96.21), maa://24621 (96.55), maa://36676 (96.67), maa://22771 (85.71), maa://37772 (100.0)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (92.06)</t>
+          <t>maa://42235 (92.86)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3901,7 +3901,7 @@
       </c>
       <c r="AF26" s="2" t="inlineStr">
         <is>
-          <t>maa://30511 (82.86), *maa://29760 (64.29)</t>
+          <t>maa://30511 (83.33), *maa://29760 (64.29)</t>
         </is>
       </c>
       <c r="AG26" s="1" t="n"/>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (48.65), maa://34494 (96.3), *maa://39601 (75.0), **maa://36665 (44.44)</t>
+          <t>**maa://21283 (48.65), maa://34494 (96.43), *maa://39601 (75.0), **maa://36665 (44.44)</t>
         </is>
       </c>
       <c r="I27" s="1" t="n"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (75.51)</t>
+          <t>*maa://30624 (76.0)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.68), maa://25725 (83.33)</t>
+          <t>maa://24465 (90.72), maa://25725 (83.53)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.12), ***maa://39723 (14.29), maa://41749 (88.64)</t>
+          <t>maa://39929 (89.37), ***maa://39723 (14.29), maa://41749 (90.0)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.36), *maa://36701 (62.96)</t>
+          <t>maa://36660 (92.83), *maa://36701 (64.29)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>*maa://25175 (69.57)</t>
+          <t>*maa://25175 (70.21)</t>
         </is>
       </c>
       <c r="I29" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.4), *maa://28440 (75.28), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.09), *maa://28440 (76.6), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.23), ***maa://34960 (8.33), *maa://42865 (80.0)</t>
+          <t>*maa://24080 (69.23), ***maa://34960 (8.33), *maa://42865 (77.42)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4357,7 +4357,7 @@
       </c>
       <c r="P30" s="2" t="inlineStr">
         <is>
-          <t>maa://21442 (99.51)</t>
+          <t>maa://21442 (99.52)</t>
         </is>
       </c>
       <c r="Q30" s="1" t="n"/>
@@ -4389,7 +4389,7 @@
       </c>
       <c r="X30" s="2" t="inlineStr">
         <is>
-          <t>maa://39477 (84.62)</t>
+          <t>maa://39477 (85.71)</t>
         </is>
       </c>
       <c r="Y30" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.56)</t>
+          <t>maa://42979 (97.83)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.85), maa://36258 (82.42), maa://43904 (100.0)</t>
+          <t>maa://35926 (93.87), maa://36258 (82.42), maa://43904 (100.0)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.19), maa://36667 (98.28), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.21), maa://36667 (98.31), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (94.34), maa://41108 (87.76), maa://41238 (95.83)</t>
+          <t>maa://42859 (95.08), maa://41108 (87.76), maa://41238 (96.05)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4767,6 +4767,22 @@
         </is>
       </c>
       <c r="U33" s="1" t="n"/>
+      <c r="V33" s="1" t="inlineStr">
+        <is>
+          <t>瑰盐</t>
+        </is>
+      </c>
+      <c r="W33" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X33" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y33" s="1" t="n"/>
       <c r="Z33" s="1" t="inlineStr">
         <is>
           <t>魔王</t>
@@ -4877,7 +4893,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (93.47)</t>
+          <t>maa://24526 (93.52)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4959,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.08)</t>
+          <t>maa://41296 (96.23)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5171,7 +5187,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.18), *maa://21239 (72.73)</t>
+          <t>maa://21280 (89.29), *maa://21239 (72.73)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5187,7 +5203,7 @@
       </c>
       <c r="T37" s="2" t="inlineStr">
         <is>
-          <t>**maa://39354 (33.33)</t>
+          <t>***maa://39354 (25.0)</t>
         </is>
       </c>
       <c r="U37" s="1" t="n"/>
@@ -5304,7 +5320,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.47)</t>
+          <t>maa://36697 (86.13)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5325,7 +5341,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (84.55), maa://36670 (87.5), maa://30434 (88.71), ***maa://25036 (16.0)</t>
+          <t>maa://25199 (84.55), maa://36670 (87.95), maa://30434 (89.06), ***maa://25036 (16.0)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5357,7 +5373,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.67)</t>
+          <t>maa://24709 (91.8)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5442,7 +5458,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.95), maa://21386 (95.74), maa://36664 (90.2)</t>
+          <t>maa://23278 (95.95), maa://21386 (95.74), maa://36664 (90.74)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5527,7 +5543,7 @@
       </c>
       <c r="P41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (38.24), *maa://43177 (75.0)</t>
+          <t>**maa://35616 (38.24), *maa://43177 (80.0)</t>
         </is>
       </c>
       <c r="Q41" s="1" t="n"/>
@@ -5649,7 +5665,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (92.48), maa://21284 (83.72)</t>
+          <t>maa://22525 (92.54), maa://21284 (83.72)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5685,6 +5701,22 @@
         </is>
       </c>
       <c r="U43" s="1" t="n"/>
+      <c r="AD43" s="1" t="inlineStr">
+        <is>
+          <t>引星棘刺</t>
+        </is>
+      </c>
+      <c r="AE43" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF43" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG43" s="1" t="n"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="B44" s="7" t="n"/>
@@ -5755,7 +5787,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.78), maa://30807 (95.38), *maa://22767 (55.0), ***maa://20796 (13.79), *maa://42459 (66.67)</t>
+          <t>maa://21229 (84.78), maa://30807 (95.45), *maa://22767 (55.0), ***maa://20796 (13.79), *maa://42459 (66.67)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5808,7 +5840,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.57), maa://43901 (100.0)</t>
+          <t>maa://35931 (92.39), *maa://43901 (80.0)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5861,7 +5893,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.11), maa://29661 (97.78), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.14), maa://29661 (97.78), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -5983,7 +6015,7 @@
       </c>
       <c r="P49" s="2" t="inlineStr">
         <is>
-          <t>*maa://39643 (69.57)</t>
+          <t>*maa://39643 (66.67)</t>
         </is>
       </c>
       <c r="Q49" s="1" t="n"/>
@@ -6040,6 +6072,22 @@
         </is>
       </c>
       <c r="Q50" s="1" t="n"/>
+      <c r="R50" s="1" t="inlineStr">
+        <is>
+          <t>特克诺</t>
+        </is>
+      </c>
+      <c r="S50" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T50" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U50" s="1" t="n"/>
     </row>
     <row r="51">
       <c r="F51" s="1" t="inlineStr">
@@ -6122,7 +6170,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.43), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.47), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6158,7 +6206,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.43)</t>
+          <t>maa://32532 (92.55)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6212,7 +6260,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (56.0)</t>
+          <t>*maa://37964 (55.56)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>
@@ -6230,7 +6278,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (82.86), maa://31270 (94.69)</t>
+          <t>maa://27746 (82.86), maa://31270 (94.78)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6248,7 +6296,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (55.0)</t>
+          <t>*maa://40438 (57.14)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>
@@ -6279,12 +6327,12 @@
       </c>
       <c r="G62" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (95.83)</t>
+          <t>maa://42981 (96.0), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>
@@ -6315,12 +6363,12 @@
       </c>
       <c r="G64" s="1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>None</t>
         </is>
       </c>
       <c r="I64" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#116)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (55.84), *maa://30515 (69.0), *maa://34787 (72.31), ***maa://20792 (11.93), maa://39402 (86.49), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (55.48), *maa://30515 (69.0), *maa://34787 (71.21), ***maa://20792 (11.93), maa://39402 (86.49), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.64), maa://27484 (96.0), maa://27480 (82.86)</t>
+          <t>maa://27396 (84.69), maa://27484 (96.0), maa://27480 (82.86)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (60.0), ***maa://26209 (13.04), *maa://39394 (66.67)</t>
+          <t>*maa://30062 (60.0), ***maa://26209 (13.04), *maa://39394 (68.18)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="T7" s="2" t="inlineStr">
         <is>
-          <t>maa://21291 (87.5)</t>
+          <t>maa://21291 (85.37)</t>
         </is>
       </c>
       <c r="U7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.12.07 13:18:04</t>
+          <t>更新日期：2024.12.07 23:48:34</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.21), **maa://32237 (41.46), ***maa://34206 (18.18), ***maa://39951 (17.95), ***maa://39243 (28.57)</t>
+          <t>***maa://25695 (19.1), **maa://32237 (41.46), ***maa://34206 (18.18), ***maa://39951 (17.5), ***maa://39243 (28.57)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.39)</t>
+          <t>maa://36707 (99.4)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (93.24), maa://22501 (98.51)</t>
+          <t>maa://22747 (93.33), maa://22501 (98.51)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (31.39), maa://39883 (90.57), *maa://39885 (56.0)</t>
+          <t>**maa://22737 (31.88), maa://39883 (90.57), *maa://39885 (56.0)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (76.84), maa://22734 (83.76), *maa://30808 (63.93), ***maa://36048 (28.57)</t>
+          <t>*maa://22743 (76.84), maa://22734 (83.9), *maa://30808 (63.93), ***maa://36048 (28.57)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.52), maa://39599 (85.71)</t>
+          <t>maa://22430 (88.59), maa://39599 (85.71)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.03)</t>
+          <t>maa://24570 (97.04)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (89.29), *maa://22732 (50.6)</t>
+          <t>maa://22466 (88.65), *maa://22732 (50.6)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (62.84), *maa://36668 (54.67)</t>
+          <t>*maa://30709 (62.94), *maa://36668 (54.67)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.8), *maa://29748 (75.59), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
+          <t>maa://30587 (91.85), *maa://29748 (75.59), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3837,7 +3837,7 @@
       </c>
       <c r="P26" s="2" t="inlineStr">
         <is>
-          <t>*maa://30968 (61.11), maa://39870 (100.0)</t>
+          <t>*maa://30968 (63.16), maa://39870 (100.0)</t>
         </is>
       </c>
       <c r="Q26" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.37), ***maa://39723 (14.29), maa://41749 (90.0)</t>
+          <t>maa://39929 (89.4), ***maa://39723 (14.29), maa://41749 (90.0)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.83)</t>
+          <t>maa://42979 (97.87)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.87), maa://36258 (82.42), maa://43904 (100.0)</t>
+          <t>maa://35926 (93.89), maa://36258 (82.42), maa://43904 (100.0)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.21), maa://36667 (98.31), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.22), maa://36667 (98.31), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (95.08), maa://41108 (87.76), maa://41238 (96.05)</t>
+          <t>maa://42859 (95.24), maa://41108 (87.76), maa://41238 (96.05)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.23)</t>
+          <t>maa://41296 (96.3)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.8)</t>
+          <t>maa://24709 (91.87)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5511,7 +5511,7 @@
       </c>
       <c r="H41" s="2" t="inlineStr">
         <is>
-          <t>maa://24466 (93.18)</t>
+          <t>maa://24466 (93.33)</t>
         </is>
       </c>
       <c r="I41" s="1" t="n"/>
@@ -5840,7 +5840,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.39), *maa://43901 (80.0)</t>
+          <t>maa://35931 (92.42), *maa://43901 (80.0)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.14), maa://29661 (97.78), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.15), maa://29661 (97.78), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6170,7 +6170,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.47), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.49), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6206,7 +6206,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.55)</t>
+          <t>maa://32532 (92.58)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#117)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (55.48), *maa://30515 (69.0), *maa://34787 (71.21), ***maa://20792 (11.93), maa://39402 (86.49), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (55.48), *maa://30515 (69.0), *maa://34787 (71.21), ***maa://20792 (11.93), maa://39402 (86.84), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="P6" s="2" t="inlineStr">
         <is>
-          <t>maa://31836 (90.48), maa://30381 (92.31)</t>
+          <t>maa://31836 (90.91), maa://30381 (92.31)</t>
         </is>
       </c>
       <c r="Q6" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.1), *maa://22758 (72.88)</t>
+          <t>maa://22399 (95.14), *maa://22758 (72.88)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.12.07 23:48:34</t>
+          <t>更新日期：2024.12.08 13:18:47</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24371 (52.86)</t>
+          <t>*maa://24371 (53.52)</t>
         </is>
       </c>
       <c r="I8" s="1" t="n"/>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (85.15), *maa://21916 (61.29), maa://23252 (92.42), maa://37496 (96.15), **maa://22759 (45.45)</t>
+          <t>maa://32931 (85.15), *maa://21916 (61.29), maa://23252 (92.42), maa://37496 (96.3), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (89.9), **maa://22865 (50.0)</t>
+          <t>maa://26206 (89.0), **maa://22865 (50.0)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.1), **maa://32237 (41.46), ***maa://34206 (18.18), ***maa://39951 (17.5), ***maa://39243 (28.57)</t>
+          <t>***maa://25695 (19.55), **maa://32237 (40.48), ***maa://34206 (18.18), ***maa://39951 (17.5), ***maa://39243 (28.57)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (53.75), *maa://22733 (59.38), maa://22761 (100.0)</t>
+          <t>*maa://25021 (53.09), *maa://22733 (59.38), maa://22761 (100.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (93.33), maa://22501 (98.51)</t>
+          <t>maa://22747 (93.38), maa://22501 (98.51)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.38), maa://21288 (96.24), maa://39841 (94.81), maa://36682 (97.37)</t>
+          <t>maa://26245 (96.38), maa://21288 (96.24), maa://39841 (94.87), maa://36682 (97.37)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (90.07), *maa://22727 (70.0)</t>
+          <t>maa://24762 (90.13), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.53), *maa://22766 (70.64), *maa://36666 (77.78)</t>
+          <t>maa://21364 (80.59), *maa://22766 (70.64), *maa://36666 (78.05)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (95.33), *maa://28648 (68.33), maa://36674 (82.5)</t>
+          <t>maa://22729 (95.33), *maa://28648 (68.33), maa://36674 (82.93)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (83.7)</t>
+          <t>maa://41331 (83.87)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>maa://24368 (80.06)</t>
+          <t>*maa://24368 (79.83)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.55), maa://23504 (93.18), **maa://22892 (39.58), *maa://25141 (77.6), maa://36663 (81.25), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.55), maa://23504 (93.18), **maa://22892 (39.58), *maa://25141 (77.6), maa://36663 (81.54), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.23), ***maa://34960 (8.33), *maa://42865 (77.42)</t>
+          <t>*maa://24080 (69.05), ***maa://34960 (8.33), *maa://42865 (77.42)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.87)</t>
+          <t>maa://42979 (97.94)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.22), maa://36667 (98.31), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.22), maa://36667 (98.33), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -5734,7 +5734,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.77), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.78), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#118)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.12.08 13:18:47</t>
+          <t>更新日期：2024.12.08 15:46:46</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.04)</t>
+          <t>maa://24570 (97.06)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.21), maa://24621 (96.55), maa://36676 (96.67), maa://22771 (85.71), maa://37772 (100.0)</t>
+          <t>maa://20108 (96.24), maa://24621 (96.55), maa://36676 (96.67), maa://22771 (85.71), maa://37772 (100.0)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.13)</t>
+          <t>maa://36697 (86.21)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.15), maa://29661 (97.78), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.15), maa://29661 (97.79), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6363,12 +6363,12 @@
       </c>
       <c r="G64" s="1" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>maa://44405 (100.0)</t>
         </is>
       </c>
       <c r="I64" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#119)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.22), maa://25390 (95.88), maa://36681 (86.84)</t>
+          <t>maa://24702 (94.22), maa://25390 (95.9), maa://36681 (87.01)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (55.48), *maa://30515 (69.0), *maa://34787 (71.21), ***maa://20792 (11.93), maa://39402 (86.84), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (55.48), *maa://30515 (69.0), *maa://34787 (71.21), ***maa://20792 (11.93), maa://39402 (87.18), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.39), *maa://20791 (62.32)</t>
+          <t>maa://22742 (91.45), *maa://20791 (62.86)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.32), maa://36684 (95.6), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.32), maa://36684 (95.65), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.39), ***maa://21730 (19.4), ***maa://39501 (15.79), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.39), ***maa://21730 (19.4), ***maa://39501 (15.0), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://36987 (93.62), maa://40192 (96.67), maa://39849 (88.89)</t>
+          <t>maa://36987 (95.83), maa://40192 (100.0), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (67.42), maa://20276 (84.71), *maa://22749 (66.67)</t>
+          <t>*maa://22880 (67.04), maa://20276 (84.71), *maa://22749 (66.67)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.55), maa://26254 (95.83)</t>
+          <t>maa://21249 (94.57), maa://26254 (95.83)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (88.79), **maa://20790 (44.78), ***maa://37170 (18.87)</t>
+          <t>maa://24617 (88.79), **maa://20790 (44.78), ***maa://37170 (18.52)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.69), maa://27484 (96.0), maa://27480 (82.86)</t>
+          <t>maa://27396 (84.69), maa://27484 (96.04), maa://27480 (82.86)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.89), maa://27295 (83.33), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (97.92), maa://27295 (83.33), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.67), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (88.89)</t>
+          <t>**maa://32495 (47.88), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (89.29)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (60.0), ***maa://26209 (13.04), *maa://39394 (68.18)</t>
+          <t>*maa://30062 (61.36), ***maa://26209 (13.04), *maa://39394 (68.18)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>*maa://22757 (76.67)</t>
+          <t>*maa://22757 (77.42)</t>
         </is>
       </c>
       <c r="M5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (93.75)</t>
+          <t>maa://42407 (93.94)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>maa://21955 (93.75)</t>
+          <t>maa://21955 (93.94)</t>
         </is>
       </c>
       <c r="E7" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (92.94), maa://24957 (97.62)</t>
+          <t>maa://28624 (93.02), maa://24957 (97.62)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="T7" s="2" t="inlineStr">
         <is>
-          <t>maa://21291 (85.37)</t>
+          <t>maa://21291 (85.71)</t>
         </is>
       </c>
       <c r="U7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (67.95), *maa://36671 (70.21), *maa://42530 (66.67)</t>
+          <t>*maa://26191 (67.95), *maa://36671 (70.21), *maa://42530 (69.23)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.12.08 15:46:46</t>
+          <t>更新日期：2024.12.12 13:20:00</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>*maa://21476 (71.74), **maa://39431 (44.44), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (71.74), **maa://39431 (45.45), *maa://37551 (57.14)</t>
         </is>
       </c>
       <c r="E8" s="1" t="n"/>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24371 (53.52)</t>
+          <t>*maa://24371 (54.29)</t>
         </is>
       </c>
       <c r="I8" s="1" t="n"/>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>maa://22765 (91.95), *maa://21915 (68.0)</t>
+          <t>maa://22765 (92.05), *maa://21915 (68.0)</t>
         </is>
       </c>
       <c r="E9" s="1" t="n"/>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>maa://22762 (91.76), maa://39552 (90.0)</t>
+          <t>maa://22762 (91.86), maa://39552 (90.0)</t>
         </is>
       </c>
       <c r="M9" s="1" t="n"/>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (80.9)</t>
+          <t>maa://22736 (81.11)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1643,7 +1643,7 @@
       </c>
       <c r="T9" s="2" t="inlineStr">
         <is>
-          <t>**maa://22866 (30.77), maa://26222 (97.67)</t>
+          <t>**maa://22866 (30.19), maa://26222 (97.78)</t>
         </is>
       </c>
       <c r="U9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (86.73), ***maa://22740 (5.88), **maa://39938 (48.0), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (92.86)</t>
+          <t>maa://28711 (86.87), ***maa://22740 (5.88), **maa://39938 (48.0), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (93.33)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.55), **maa://32237 (40.48), ***maa://34206 (18.18), ***maa://39951 (17.5), ***maa://39243 (28.57)</t>
+          <t>***maa://25695 (19.44), **maa://32237 (40.48), ***maa://34206 (18.18), ***maa://39951 (17.5), ***maa://39243 (28.57)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (91.36), maa://36669 (87.88), *maa://23264 (61.82)</t>
+          <t>maa://28977 (91.36), maa://36669 (88.24), *maa://23264 (61.82)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (95.93), maa://22755 (87.39), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (95.93), maa://22755 (87.5), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (53.09), *maa://22733 (59.38), maa://22761 (100.0)</t>
+          <t>*maa://25021 (53.66), *maa://22733 (59.38), maa://22761 (100.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (93.38), maa://22501 (98.51)</t>
+          <t>maa://22747 (93.38), maa://22501 (98.53)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>maa://30766 (89.29), **maa://36678 (50.0)</t>
+          <t>maa://30766 (89.29), *maa://36678 (60.0)</t>
         </is>
       </c>
       <c r="E12" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.19), *maa://21485 (76.87), maa://37962 (88.89)</t>
+          <t>maa://22753 (91.25), *maa://21485 (76.87), maa://37962 (88.89)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.34), maa://36677 (93.62), maa://39872 (90.0)</t>
+          <t>maa://23669 (95.34), maa://36677 (93.75), maa://39872 (90.0)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.7), maa://36673 (92.65), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.73), maa://36673 (92.65), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>*maa://34957 (78.69), *maa://22768 (51.61)</t>
+          <t>*maa://34957 (79.03), *maa://22768 (51.61)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>maa://30764 (88.0)</t>
+          <t>maa://30764 (88.24)</t>
         </is>
       </c>
       <c r="E14" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.38), maa://21288 (96.24), maa://39841 (94.87), maa://36682 (97.37)</t>
+          <t>maa://26245 (96.43), maa://21288 (96.27), maa://39841 (94.87), maa://36682 (97.37)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.61), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.62), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="T14" s="2" t="inlineStr">
         <is>
-          <t>maa://22521 (93.68), maa://42751 (100.0)</t>
+          <t>maa://22521 (93.75), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="1" t="n"/>
@@ -2309,7 +2309,7 @@
       </c>
       <c r="X14" s="2" t="inlineStr">
         <is>
-          <t>maa://37468 (88.89)</t>
+          <t>maa://37468 (89.47)</t>
         </is>
       </c>
       <c r="Y14" s="1" t="n"/>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="AB14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (96.83)</t>
+          <t>maa://22764 (96.88)</t>
         </is>
       </c>
       <c r="AC14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (76.84), maa://22734 (83.9), *maa://30808 (63.93), ***maa://36048 (28.57)</t>
+          <t>*maa://22743 (76.84), maa://22734 (83.9), *maa://30808 (64.52), ***maa://36048 (28.57)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.5), maa://21478 (91.43)</t>
+          <t>maa://24304 (88.56), maa://21478 (91.43)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.59), *maa://22766 (70.64), *maa://36666 (78.05)</t>
+          <t>maa://21364 (80.59), *maa://22766 (70.64), *maa://36666 (78.31)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.28), maa://36679 (92.68), maa://37650 (96.88)</t>
+          <t>maa://21441 (96.28), maa://36679 (93.02), maa://37650 (96.88)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2537,7 +2537,7 @@
       </c>
       <c r="P16" s="2" t="inlineStr">
         <is>
-          <t>maa://28504 (90.74)</t>
+          <t>maa://28504 (90.91)</t>
         </is>
       </c>
       <c r="Q16" s="1" t="n"/>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>**maa://42324 (45.83)</t>
+          <t>**maa://42324 (48.0)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (90.17)</t>
+          <t>maa://24421 (90.25)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="X18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (97.7), maa://22741 (83.33)</t>
+          <t>maa://21917 (97.75), maa://22741 (83.33)</t>
         </is>
       </c>
       <c r="Y18" s="1" t="n"/>
@@ -2845,7 +2845,7 @@
       </c>
       <c r="AB18" s="2" t="inlineStr">
         <is>
-          <t>maa://24393 (97.5)</t>
+          <t>maa://24393 (97.56)</t>
         </is>
       </c>
       <c r="AC18" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (98.99)</t>
+          <t>maa://24386 (99.0)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (62.94), *maa://36668 (54.67)</t>
+          <t>*maa://30709 (62.78), *maa://36668 (54.67)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (89.73), maa://25198 (92.93), *maa://20795 (51.18), maa://36680 (96.55)</t>
+          <t>maa://21432 (89.73), maa://25198 (93.0), *maa://20795 (51.18), maa://36680 (96.55)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="X21" s="2" t="inlineStr">
         <is>
-          <t>maa://20110 (86.76), maa://34946 (92.31)</t>
+          <t>maa://20110 (86.76), maa://34946 (92.5)</t>
         </is>
       </c>
       <c r="Y21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.53), *maa://22432 (76.67)</t>
+          <t>maa://22524 (94.55), *maa://22432 (76.67)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (86.0), *maa://22751 (73.85)</t>
+          <t>maa://27127 (85.15), *maa://22751 (73.85)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.45), *maa://37649 (68.0)</t>
+          <t>maa://21282 (98.46), *maa://37649 (68.0)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.36), *maa://41753 (54.55)</t>
+          <t>***maa://28036 (28.36), *maa://41753 (58.33)</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (93.72), maa://39875 (93.55)</t>
+          <t>maa://39756 (93.78), maa://39875 (93.55)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.85), *maa://29748 (75.59), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
+          <t>maa://30587 (91.89), *maa://29748 (75.59), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3495,7 +3495,7 @@
       </c>
       <c r="AB23" s="2" t="inlineStr">
         <is>
-          <t>maa://29652 (97.5)</t>
+          <t>maa://29652 (97.56)</t>
         </is>
       </c>
       <c r="AC23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.55), maa://23504 (93.18), **maa://22892 (39.58), *maa://25141 (77.6), maa://36663 (81.54), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.61), maa://23504 (93.19), **maa://22892 (39.58), *maa://25141 (77.6), maa://36663 (81.82), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.42), maa://36672 (80.39), maa://29910 (92.31), **maa://21440 (34.55)</t>
+          <t>maa://22523 (85.42), maa://36672 (80.77), maa://29910 (92.31), **maa://21440 (34.55)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (73.97), *maa://25311 (73.74), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (73.97), *maa://25311 (74.0), ***maa://22725 (4.84)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (85.42), *maa://24516 (79.31), maa://26001 (87.5)</t>
+          <t>maa://31215 (85.42), *maa://24516 (79.55), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>maa://41802 (100.0)</t>
+          <t>maa://41802 (91.67)</t>
         </is>
       </c>
       <c r="E26" s="1" t="n"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (91.36)</t>
+          <t>maa://24913 (91.46)</t>
         </is>
       </c>
       <c r="I26" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (92.86)</t>
+          <t>maa://42235 (92.96)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3901,7 +3901,7 @@
       </c>
       <c r="AF26" s="2" t="inlineStr">
         <is>
-          <t>maa://30511 (83.33), *maa://29760 (64.29)</t>
+          <t>maa://30511 (83.78), *maa://29760 (64.29)</t>
         </is>
       </c>
       <c r="AG26" s="1" t="n"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (76.0)</t>
+          <t>*maa://30624 (76.47)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4031,7 +4031,7 @@
       </c>
       <c r="AF27" s="2" t="inlineStr">
         <is>
-          <t>maa://24023 (97.01)</t>
+          <t>maa://24023 (97.06)</t>
         </is>
       </c>
       <c r="AG27" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.72), maa://25725 (83.53)</t>
+          <t>maa://24465 (90.76), maa://25725 (83.53)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>maa://23263 (94.85), *maa://29765 (61.33)</t>
+          <t>maa://23263 (94.85), *maa://29765 (60.53)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.4), ***maa://39723 (14.29), maa://41749 (90.0)</t>
+          <t>maa://39929 (89.51), ***maa://39723 (14.29), maa://41749 (90.0)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.09), *maa://28440 (76.6), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.11), *maa://28440 (76.6), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4227,7 +4227,7 @@
       </c>
       <c r="P29" s="2" t="inlineStr">
         <is>
-          <t>*maa://23168 (54.72), **maa://30050 (50.0)</t>
+          <t>*maa://23168 (54.72), *maa://30050 (51.85)</t>
         </is>
       </c>
       <c r="Q29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.94)</t>
+          <t>maa://42979 (96.97)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.89), maa://36258 (82.42), maa://43904 (100.0)</t>
+          <t>maa://35926 (93.92), maa://36258 (82.98), *maa://43904 (80.0)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (95.24), maa://41108 (87.76), maa://41238 (96.05)</t>
+          <t>maa://42859 (95.52), maa://41108 (87.76), maa://41238 (96.1)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.3)</t>
+          <t>maa://41296 (96.4)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.21)</t>
+          <t>maa://36697 (85.88)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.87)</t>
+          <t>maa://24709 (92.0)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5543,7 +5543,7 @@
       </c>
       <c r="P41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (38.24), *maa://43177 (80.0)</t>
+          <t>**maa://35616 (38.24), maa://43177 (81.82)</t>
         </is>
       </c>
       <c r="Q41" s="1" t="n"/>
@@ -5665,7 +5665,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (92.54), maa://21284 (83.72)</t>
+          <t>maa://22525 (92.59), maa://21284 (83.72)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5734,7 +5734,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.78), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.79), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5840,7 +5840,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.42), *maa://43901 (80.0)</t>
+          <t>maa://35931 (92.42), maa://43901 (85.71)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6206,7 +6206,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.58)</t>
+          <t>maa://32532 (92.22)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6242,7 +6242,7 @@
       </c>
       <c r="H57" s="2" t="inlineStr">
         <is>
-          <t>maa://25176 (98.15)</t>
+          <t>maa://25176 (98.18)</t>
         </is>
       </c>
       <c r="I57" s="1" t="n"/>
@@ -6260,7 +6260,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (55.56)</t>
+          <t>*maa://37964 (57.14)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>
@@ -6368,7 +6368,7 @@
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>maa://44405 (100.0)</t>
+          <t>**maa://44405 (50.0)</t>
         </is>
       </c>
       <c r="I64" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#120)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.32), maa://36684 (95.65), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.32), maa://36684 (95.7), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (61.36), ***maa://26209 (13.04), *maa://39394 (68.18)</t>
+          <t>*maa://30062 (62.22), ***maa://26209 (13.04), *maa://39394 (68.18)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (82.94), maa://22744 (84.0)</t>
+          <t>maa://21245 (83.02), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.12.12 13:20:00</t>
+          <t>更新日期：2024.12.13 13:19:35</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1757,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (91.36), maa://36669 (88.24), *maa://23264 (61.82)</t>
+          <t>maa://28977 (91.36), maa://36669 (88.57), *maa://23264 (61.82)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.28), maa://36679 (93.02), maa://37650 (96.88)</t>
+          <t>maa://21441 (96.3), maa://36679 (93.02), maa://37650 (96.88)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="X18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (97.75), maa://22741 (83.33)</t>
+          <t>maa://21917 (97.78), maa://22741 (83.33)</t>
         </is>
       </c>
       <c r="Y18" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (83.87)</t>
+          <t>maa://41331 (84.04)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="T22" s="2" t="inlineStr">
         <is>
-          <t>maa://38495 (81.82)</t>
+          <t>maa://38495 (83.33)</t>
         </is>
       </c>
       <c r="U22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (93.78), maa://39875 (93.55)</t>
+          <t>maa://39756 (93.8), maa://39875 (93.55)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.18)</t>
+          <t>maa://29753 (95.2)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (48.65), maa://34494 (96.43), *maa://39601 (75.0), **maa://36665 (44.44)</t>
+          <t>**maa://21283 (48.65), maa://34494 (96.43), *maa://39601 (76.47), **maa://36665 (44.44)</t>
         </is>
       </c>
       <c r="I27" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.97)</t>
+          <t>maa://42979 (97.03)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (95.52), maa://41108 (87.76), maa://41238 (96.1)</t>
+          <t>maa://42859 (95.59), maa://41108 (87.76), maa://41238 (96.1)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -5057,7 +5057,7 @@
       </c>
       <c r="H36" s="2" t="inlineStr">
         <is>
-          <t>maa://24375 (92.5)</t>
+          <t>maa://24375 (92.68)</t>
         </is>
       </c>
       <c r="I36" s="1" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (85.88)</t>
+          <t>maa://36697 (85.96)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5766,7 +5766,7 @@
       </c>
       <c r="T44" s="2" t="inlineStr">
         <is>
-          <t>maa://39366 (86.67)</t>
+          <t>maa://39366 (87.1)</t>
         </is>
       </c>
       <c r="U44" s="1" t="n"/>
@@ -5840,7 +5840,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.42), maa://43901 (85.71)</t>
+          <t>maa://35931 (92.45), maa://43901 (85.71)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6368,7 +6368,7 @@
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>**maa://44405 (50.0)</t>
+          <t>maa://44405 (94.74)</t>
         </is>
       </c>
       <c r="I64" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#121)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.39), ***maa://21730 (19.4), ***maa://39501 (15.0), *maa://36675 (60.0)</t>
+          <t>maa://25251 (91.4), ***maa://21730 (19.4), ***maa://39501 (15.0), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (96.43)</t>
+          <t>maa://24390 (96.49)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.92), maa://27295 (83.33), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (97.94), maa://27295 (83.33), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.12.13 13:19:35</t>
+          <t>更新日期：2024.12.14 13:22:12</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.83)</t>
+          <t>maa://21411 (95.86)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (89.0), **maa://22865 (50.0)</t>
+          <t>maa://26206 (89.11), **maa://22865 (50.0)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.34), maa://36677 (93.75), maa://39872 (90.0)</t>
+          <t>maa://23669 (95.36), maa://36677 (93.75), maa://39872 (90.0)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2391,7 +2391,7 @@
       </c>
       <c r="L15" s="2" t="inlineStr">
         <is>
-          <t>*maa://21334 (51.85)</t>
+          <t>*maa://21334 (53.57)</t>
         </is>
       </c>
       <c r="M15" s="1" t="n"/>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="X23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (66.67)</t>
+          <t>*maa://28503 (67.16)</t>
         </is>
       </c>
       <c r="Y23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.61), maa://23504 (93.19), **maa://22892 (39.58), *maa://25141 (77.6), maa://36663 (81.82), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.61), maa://23504 (93.21), **maa://22892 (39.58), *maa://25141 (77.6), maa://36663 (81.82), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (95.59), maa://41108 (87.76), maa://41238 (96.1)</t>
+          <t>maa://42859 (95.65), maa://41108 (87.76), maa://41238 (96.1)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.4)</t>
+          <t>maa://41296 (96.43)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5187,7 +5187,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.29), *maa://21239 (72.73)</t>
+          <t>maa://21280 (88.83), *maa://21239 (72.73)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5336,12 +5336,12 @@
       </c>
       <c r="G39" s="1" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (84.55), maa://36670 (87.95), maa://30434 (89.06), ***maa://25036 (16.0)</t>
+          <t>maa://25199 (84.68), maa://36670 (87.95), maa://30434 (89.06), ***maa://25036 (16.0), **maa://44165 (50.0)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5543,7 +5543,7 @@
       </c>
       <c r="P41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (38.24), maa://43177 (81.82)</t>
+          <t>**maa://35616 (38.24), maa://43177 (83.33)</t>
         </is>
       </c>
       <c r="Q41" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#122)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (67.04), maa://20276 (84.71), *maa://22749 (66.67)</t>
+          <t>*maa://22880 (66.67), maa://20276 (84.71), *maa://22749 (66.67)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.69), maa://27484 (96.04), maa://27480 (82.86)</t>
+          <t>maa://27396 (84.69), maa://27484 (96.08), maa://27480 (82.86)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="AB5" s="2" t="inlineStr">
         <is>
-          <t>*maa://29863 (70.0), ***maa://22752 (13.33), **maa://26013 (42.86)</t>
+          <t>*maa://29863 (70.97), ***maa://22752 (13.33), **maa://26013 (42.86)</t>
         </is>
       </c>
       <c r="AC5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (93.94)</t>
+          <t>maa://42407 (94.12)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.12.14 13:22:12</t>
+          <t>更新日期：2024.12.15 13:19:36</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (85.15), *maa://21916 (61.29), maa://23252 (92.42), maa://37496 (96.3), **maa://22759 (45.45)</t>
+          <t>maa://32931 (85.29), *maa://21916 (61.29), maa://23252 (92.42), maa://37496 (96.3), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.86)</t>
+          <t>maa://21411 (95.87)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (91.36), maa://36669 (88.57), *maa://23264 (61.82)</t>
+          <t>maa://28977 (91.36), maa://36669 (88.89), *maa://23264 (61.82)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (93.38), maa://22501 (98.53)</t>
+          <t>maa://22747 (93.38), maa://22501 (98.55)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (90.12)</t>
+          <t>maa://21867 (90.18)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.25), *maa://21485 (76.87), maa://37962 (88.89)</t>
+          <t>maa://22753 (91.3), *maa://21485 (76.87), maa://37962 (88.89)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.73), maa://36673 (92.65), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.74), maa://36673 (92.65), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>maa://30764 (88.24)</t>
+          <t>maa://30764 (88.46)</t>
         </is>
       </c>
       <c r="E14" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.59), *maa://22766 (70.64), *maa://36666 (78.31)</t>
+          <t>maa://21364 (80.66), *maa://22766 (70.64), *maa://36666 (78.31)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.59), maa://39599 (85.71)</t>
+          <t>maa://22430 (88.59), maa://39599 (86.11)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2991,7 +2991,7 @@
       </c>
       <c r="AF19" s="2" t="inlineStr">
         <is>
-          <t>*maa://21663 (62.5)</t>
+          <t>*maa://21663 (61.54)</t>
         </is>
       </c>
       <c r="AG19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (89.73), maa://25198 (93.0), *maa://20795 (51.18), maa://36680 (96.55)</t>
+          <t>maa://21432 (89.8), maa://25198 (93.0), *maa://20795 (51.18), maa://36680 (96.55)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (88.97)</t>
+          <t>maa://22864 (89.04)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="P20" s="2" t="inlineStr">
         <is>
-          <t>maa://37442 (97.22)</t>
+          <t>maa://37442 (94.59)</t>
         </is>
       </c>
       <c r="Q20" s="1" t="n"/>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.36), *maa://41753 (58.33)</t>
+          <t>***maa://28036 (27.94), *maa://41753 (58.33)</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (79.83)</t>
+          <t>*maa://24368 (79.6)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.61), maa://23504 (93.21), **maa://22892 (39.58), *maa://25141 (77.6), maa://36663 (81.82), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.61), maa://23504 (93.23), **maa://22892 (39.58), *maa://25141 (77.6), maa://36663 (81.82), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.2)</t>
+          <t>maa://29753 (95.22)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3951,7 +3951,7 @@
       </c>
       <c r="L27" s="2" t="inlineStr">
         <is>
-          <t>maa://28071 (88.24)</t>
+          <t>maa://28071 (88.89)</t>
         </is>
       </c>
       <c r="M27" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.76), maa://25725 (83.53)</t>
+          <t>maa://24465 (90.77), maa://25725 (83.53)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.51), ***maa://39723 (14.29), maa://41749 (90.0)</t>
+          <t>maa://39929 (89.58), ***maa://39723 (14.29), maa://41749 (90.0)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.22), maa://36667 (98.33), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.24), maa://36667 (98.33), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (95.65), maa://41108 (87.76), maa://41238 (96.1)</t>
+          <t>maa://42859 (95.77), maa://41108 (87.76), maa://41238 (96.1)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -5187,7 +5187,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (88.83), *maa://21239 (72.73)</t>
+          <t>maa://21280 (88.89), *maa://21239 (72.73)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.15), maa://29661 (97.79), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.17), maa://29661 (97.81), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#123)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.45), *maa://20791 (62.86)</t>
+          <t>maa://22742 (91.5), *maa://20791 (62.86)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (91.4), ***maa://21730 (19.4), ***maa://39501 (15.0), *maa://36675 (60.0)</t>
+          <t>maa://25251 (91.49), ***maa://21730 (19.4), ***maa://39501 (19.05), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.4), *maa://22748 (75.0)</t>
+          <t>maa://21247 (98.4), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (66.67), maa://20276 (84.71), *maa://22749 (66.67)</t>
+          <t>*maa://22880 (65.93), maa://20276 (84.71), *maa://22749 (72.73)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (96.49)</t>
+          <t>maa://24390 (96.55)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.94), maa://27295 (83.33), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (97.94), maa://27295 (83.61), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.88), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (89.29)</t>
+          <t>**maa://32495 (47.69), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (89.66)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (83.02), maa://22744 (84.0)</t>
+          <t>maa://21245 (83.1), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="AB5" s="2" t="inlineStr">
         <is>
-          <t>*maa://29863 (70.97), ***maa://22752 (13.33), **maa://26013 (42.86)</t>
+          <t>*maa://29863 (71.88), ***maa://22752 (13.33), **maa://26013 (42.86)</t>
         </is>
       </c>
       <c r="AC5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (94.12)</t>
+          <t>maa://42407 (94.44)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (67.95), *maa://36671 (70.21), *maa://42530 (69.23)</t>
+          <t>*maa://26191 (67.95), *maa://36671 (70.83), *maa://42530 (69.23)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.12.15 13:19:36</t>
+          <t>更新日期：2024.12.18 13:18:43</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.87)</t>
+          <t>maa://21411 (95.89)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="AF8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24479 (77.22), *maa://21990 (53.85)</t>
+          <t>*maa://24479 (77.78), *maa://21990 (53.85)</t>
         </is>
       </c>
       <c r="AG8" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (89.11), **maa://22865 (50.0)</t>
+          <t>maa://26206 (89.32), **maa://22865 (50.0)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.44), **maa://32237 (40.48), ***maa://34206 (18.18), ***maa://39951 (17.5), ***maa://39243 (28.57)</t>
+          <t>***maa://25695 (19.44), **maa://32237 (40.48), ***maa://34206 (18.18), ***maa://39951 (17.07), ***maa://39243 (28.57)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (93.38), maa://22501 (98.55)</t>
+          <t>maa://22747 (93.42), maa://22501 (98.55)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (98.14)</t>
+          <t>maa://36713 (98.15)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.36), maa://36677 (93.75), maa://39872 (90.0)</t>
+          <t>maa://23669 (95.36), maa://36677 (93.88), maa://39872 (90.0)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.29), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (78.46), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.74), maa://36673 (92.65), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.75), maa://36673 (92.65), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.43), maa://21288 (96.27), maa://39841 (94.87), maa://36682 (97.37)</t>
+          <t>maa://26245 (96.43), maa://21288 (96.27), maa://39841 (94.94), maa://36682 (97.37)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2309,7 +2309,7 @@
       </c>
       <c r="X14" s="2" t="inlineStr">
         <is>
-          <t>maa://37468 (89.47)</t>
+          <t>maa://37468 (90.0)</t>
         </is>
       </c>
       <c r="Y14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (76.84), maa://22734 (83.9), *maa://30808 (64.52), ***maa://36048 (28.57)</t>
+          <t>*maa://22743 (76.96), maa://22734 (83.9), *maa://30808 (64.52), ***maa://36048 (28.57)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.66), *maa://22766 (70.64), *maa://36666 (78.31)</t>
+          <t>maa://21364 (80.72), *maa://22766 (70.91), *maa://36666 (78.57)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.3), maa://36679 (93.02), maa://37650 (96.88)</t>
+          <t>maa://21441 (96.31), maa://36679 (93.02), maa://37650 (96.88)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.35)</t>
+          <t>maa://26228 (95.4)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>**maa://42324 (48.0)</t>
+          <t>**maa://42324 (46.15)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.06)</t>
+          <t>maa://24570 (97.07)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (90.25)</t>
+          <t>maa://24421 (90.3)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (88.65), *maa://22732 (50.6)</t>
+          <t>maa://22466 (88.73), *maa://22732 (50.6)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="X18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (97.78), maa://22741 (83.33)</t>
+          <t>maa://21917 (97.8), maa://22741 (83.33)</t>
         </is>
       </c>
       <c r="Y18" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (62.78), *maa://36668 (54.67)</t>
+          <t>*maa://30709 (62.96), *maa://36668 (55.84)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (89.8), maa://25198 (93.0), *maa://20795 (51.18), maa://36680 (96.55)</t>
+          <t>maa://21432 (89.86), maa://25198 (93.0), *maa://20795 (51.18), maa://36680 (96.55)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (89.04)</t>
+          <t>maa://22864 (89.12)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (84.04)</t>
+          <t>maa://41331 (84.21)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>*maa://21443 (79.94), ***maa://23820 (29.82)</t>
+          <t>*maa://21443 (80.0), ***maa://23820 (29.82)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.55), *maa://22432 (76.67)</t>
+          <t>maa://22524 (94.58), *maa://22432 (76.67)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (93.8), maa://39875 (93.55)</t>
+          <t>maa://39756 (93.95), maa://39875 (93.65)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.89), *maa://29748 (75.59), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
+          <t>maa://30587 (91.94), *maa://29748 (75.59), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (79.6)</t>
+          <t>*maa://24368 (79.66)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.61), maa://23504 (93.23), **maa://22892 (39.58), *maa://25141 (77.6), maa://36663 (81.82), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.67), maa://23504 (93.23), **maa://22892 (39.58), *maa://25141 (77.6), maa://36663 (80.6), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.42), maa://36672 (80.77), maa://29910 (92.31), **maa://21440 (34.55)</t>
+          <t>maa://22523 (85.42), maa://36672 (80.77), maa://29910 (92.45), **maa://21440 (34.55)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3723,7 +3723,7 @@
       </c>
       <c r="T25" s="2" t="inlineStr">
         <is>
-          <t>maa://20109 (92.31), maa://22545 (100.0), maa://42915 (100.0)</t>
+          <t>maa://20109 (92.35), maa://22545 (100.0), maa://42915 (100.0)</t>
         </is>
       </c>
       <c r="U25" s="1" t="n"/>
@@ -3739,7 +3739,7 @@
       </c>
       <c r="X25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29890 (75.61)</t>
+          <t>*maa://29890 (76.19)</t>
         </is>
       </c>
       <c r="Y25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (85.42), *maa://24516 (79.55), maa://26001 (87.5)</t>
+          <t>maa://31215 (85.57), *maa://24516 (79.78), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>maa://41802 (91.67)</t>
+          <t>maa://41802 (92.31)</t>
         </is>
       </c>
       <c r="E26" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (92.96)</t>
+          <t>maa://42235 (93.15)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (48.65), maa://34494 (96.43), *maa://39601 (76.47), **maa://36665 (44.44)</t>
+          <t>**maa://21283 (48.0), maa://34494 (96.43), *maa://39601 (76.47), **maa://36665 (44.44)</t>
         </is>
       </c>
       <c r="I27" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>maa://23263 (94.85), *maa://29765 (60.53)</t>
+          <t>maa://23263 (94.9), *maa://29765 (60.53)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.58), ***maa://39723 (14.29), maa://41749 (90.0)</t>
+          <t>maa://39929 (89.68), ***maa://39723 (14.29), maa://41749 (90.2)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.83), *maa://36701 (64.29)</t>
+          <t>maa://36660 (92.88), *maa://36701 (64.29)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.11), *maa://28440 (76.6), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (92.81), *maa://28440 (76.6), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.03)</t>
+          <t>maa://42979 (96.23)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.92), maa://36258 (82.98), *maa://43904 (80.0)</t>
+          <t>maa://35926 (93.94), maa://36258 (83.16), *maa://43904 (71.43)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (95.77), maa://41108 (87.76), maa://41238 (96.1)</t>
+          <t>maa://42859 (96.1), maa://41108 (87.76), maa://41238 (96.1)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (93.52)</t>
+          <t>maa://24526 (93.55)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.43)</t>
+          <t>maa://41296 (96.49)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (85.96)</t>
+          <t>maa://36697 (86.19)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (84.68), maa://36670 (87.95), maa://30434 (89.06), ***maa://25036 (16.0), **maa://44165 (50.0)</t>
+          <t>maa://25199 (84.82), maa://36670 (86.9), maa://30434 (89.06), ***maa://25036 (16.0), **maa://44165 (50.0)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (92.0)</t>
+          <t>maa://24709 (92.06)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5543,7 +5543,7 @@
       </c>
       <c r="P41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (38.24), maa://43177 (83.33)</t>
+          <t>**maa://35616 (38.24), maa://43177 (84.62)</t>
         </is>
       </c>
       <c r="Q41" s="1" t="n"/>
@@ -5840,7 +5840,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.45), maa://43901 (85.71)</t>
+          <t>maa://35931 (92.47), maa://43901 (87.5)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.17), maa://29661 (97.81), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.17), maa://29661 (97.83), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (82.86), maa://31270 (94.78)</t>
+          <t>maa://27746 (83.02), maa://31270 (94.78)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6296,7 +6296,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (57.14)</t>
+          <t>*maa://40438 (58.14)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>
@@ -6332,7 +6332,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (96.0), maa://43903 (100.0)</t>
+          <t>maa://42981 (96.15), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>
@@ -6368,7 +6368,7 @@
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>maa://44405 (94.74)</t>
+          <t>maa://44405 (95.0)</t>
         </is>
       </c>
       <c r="I64" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#124)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.5), *maa://20791 (62.86)</t>
+          <t>maa://22742 (91.56), *maa://20791 (62.86)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.4), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.41), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.93), maa://20276 (84.71), *maa://22749 (72.73)</t>
+          <t>*maa://22880 (65.93), maa://20276 (84.81), *maa://22749 (72.73)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.94), maa://27295 (83.61), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (97.96), maa://27295 (83.61), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (83.1), maa://22744 (84.0)</t>
+          <t>maa://21245 (83.18), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (93.02), maa://24957 (97.62)</t>
+          <t>maa://28624 (93.1), maa://24957 (97.62)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.12.18 13:18:43</t>
+          <t>更新日期：2024.12.19 13:19:06</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (86.87), ***maa://22740 (5.88), **maa://39938 (48.0), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (93.33)</t>
+          <t>maa://28711 (87.0), ***maa://22740 (5.88), **maa://39938 (48.0), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (93.33)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (95.93), maa://22755 (87.5), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (95.95), maa://22755 (87.5), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (93.42), maa://22501 (98.55)</t>
+          <t>maa://22747 (93.42), maa://22501 (98.57)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.3), *maa://21485 (76.87), maa://37962 (88.89)</t>
+          <t>maa://22753 (91.36), *maa://21485 (76.87), maa://37962 (88.89)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.46), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (78.63), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (31.88), maa://39883 (90.57), *maa://39885 (56.0)</t>
+          <t>**maa://22737 (32.37), maa://39883 (90.74), *maa://39885 (56.0)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.43), maa://21288 (96.27), maa://39841 (94.94), maa://36682 (97.37)</t>
+          <t>maa://26245 (96.43), maa://21288 (96.27), maa://39841 (95.0), maa://36682 (97.37)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="T14" s="2" t="inlineStr">
         <is>
-          <t>maa://22521 (93.75), maa://42751 (100.0)</t>
+          <t>maa://22521 (93.81), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (76.96), maa://22734 (83.9), *maa://30808 (64.52), ***maa://36048 (28.57)</t>
+          <t>*maa://22743 (76.96), maa://22734 (83.9), *maa://30808 (64.52), **maa://36048 (31.82)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (90.13), *maa://22727 (70.0)</t>
+          <t>maa://24762 (90.2), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.72), *maa://22766 (70.91), *maa://36666 (78.57)</t>
+          <t>maa://21364 (80.84), *maa://22766 (70.91), *maa://36666 (78.57)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (65.0), maa://27755 (92.5)</t>
+          <t>*maa://23911 (65.35), maa://27755 (92.5)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>maa://21624 (82.35)</t>
+          <t>maa://21624 (82.86)</t>
         </is>
       </c>
       <c r="E17" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.59), maa://39599 (86.11)</t>
+          <t>maa://22430 (88.65), maa://39599 (86.11)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>**maa://42324 (46.15)</t>
+          <t>**maa://42324 (48.15)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.07)</t>
+          <t>maa://24570 (97.09)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (88.73), *maa://22732 (50.6)</t>
+          <t>maa://22466 (88.81), *maa://22732 (50.6)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (62.96), *maa://36668 (55.84)</t>
+          <t>*maa://30709 (63.05), *maa://36668 (55.84)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>*maa://21443 (80.0), ***maa://23820 (29.82)</t>
+          <t>maa://21443 (80.06), ***maa://23820 (29.82)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="T22" s="2" t="inlineStr">
         <is>
-          <t>maa://38495 (83.33)</t>
+          <t>maa://38495 (84.62)</t>
         </is>
       </c>
       <c r="U22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (93.95), maa://39875 (93.65)</t>
+          <t>maa://39756 (93.98), maa://39875 (93.65)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.94), *maa://29748 (75.59), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
+          <t>maa://30587 (91.98), *maa://29748 (75.59), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="T23" s="2" t="inlineStr">
         <is>
-          <t>maa://24387 (81.58), maa://31212 (92.86)</t>
+          <t>maa://24387 (81.58), maa://31212 (93.1)</t>
         </is>
       </c>
       <c r="U23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.67), maa://23504 (93.23), **maa://22892 (39.58), *maa://25141 (77.6), maa://36663 (80.6), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.67), maa://23504 (93.26), **maa://22892 (39.58), *maa://25141 (77.6), maa://36663 (80.6), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.42), maa://36672 (80.77), maa://29910 (92.45), **maa://21440 (34.55)</t>
+          <t>maa://22523 (85.49), maa://36672 (80.77), maa://29910 (92.45), **maa://21440 (34.55)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3723,7 +3723,7 @@
       </c>
       <c r="T25" s="2" t="inlineStr">
         <is>
-          <t>maa://20109 (92.35), maa://22545 (100.0), maa://42915 (100.0)</t>
+          <t>maa://20109 (92.4), maa://22545 (100.0), maa://42915 (100.0)</t>
         </is>
       </c>
       <c r="U25" s="1" t="n"/>
@@ -3869,7 +3869,7 @@
       </c>
       <c r="X26" s="2" t="inlineStr">
         <is>
-          <t>maa://24389 (96.15)</t>
+          <t>maa://24389 (96.3)</t>
         </is>
       </c>
       <c r="Y26" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.68), ***maa://39723 (14.29), maa://41749 (90.2)</t>
+          <t>maa://39929 (89.68), ***maa://39723 (14.29), maa://41749 (90.57)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.94), maa://36258 (83.16), *maa://43904 (71.43)</t>
+          <t>maa://35926 (93.96), maa://36258 (83.16), *maa://43904 (71.43)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.24), maa://36667 (98.33), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.25), maa://36667 (98.33), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.1), maa://41108 (87.76), maa://41238 (96.1)</t>
+          <t>maa://42859 (96.1), maa://41108 (87.76), maa://41238 (96.15)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.49)</t>
+          <t>maa://41296 (96.55)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5187,7 +5187,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (88.89), *maa://21239 (72.73)</t>
+          <t>maa://21280 (89.0), *maa://21239 (66.67)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="P38" s="2" t="inlineStr">
         <is>
-          <t>*maa://24383 (68.42)</t>
+          <t>*maa://24383 (67.71)</t>
         </is>
       </c>
       <c r="Q38" s="1" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="T38" s="2" t="inlineStr">
         <is>
-          <t>maa://30713 (96.67)</t>
+          <t>maa://30713 (96.77)</t>
         </is>
       </c>
       <c r="U38" s="1" t="n"/>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (92.06)</t>
+          <t>maa://24709 (92.13)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5458,7 +5458,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.95), maa://21386 (95.74), maa://36664 (90.74)</t>
+          <t>maa://23278 (95.96), maa://21386 (95.74), maa://36664 (90.74)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5665,7 +5665,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (92.59), maa://21284 (83.72)</t>
+          <t>maa://22525 (92.65), maa://21284 (83.72)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5787,7 +5787,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.78), maa://30807 (95.45), *maa://22767 (55.0), ***maa://20796 (13.79), *maa://42459 (66.67)</t>
+          <t>maa://21229 (84.78), maa://30807 (95.45), *maa://22767 (55.0), ***maa://20796 (13.79), *maa://42459 (71.43)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5803,7 +5803,7 @@
       </c>
       <c r="P45" s="2" t="inlineStr">
         <is>
-          <t>*maa://36237 (61.54)</t>
+          <t>*maa://36237 (64.29)</t>
         </is>
       </c>
       <c r="Q45" s="1" t="n"/>
@@ -5819,7 +5819,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (36.84)</t>
+          <t>**maa://39364 (35.0)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.17), maa://29661 (97.83), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.18), maa://29661 (97.83), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6260,7 +6260,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (57.14)</t>
+          <t>*maa://37964 (55.17)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>
@@ -6296,7 +6296,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (58.14)</t>
+          <t>*maa://40438 (59.09)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#126)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.22), maa://25390 (95.9), maa://36681 (87.01)</t>
+          <t>maa://24702 (94.24), maa://25390 (95.9), maa://36681 (87.01)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (55.48), *maa://30515 (69.0), *maa://34787 (71.21), ***maa://20792 (11.93), maa://39402 (87.18), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (55.48), *maa://30515 (69.0), *maa://34787 (72.06), ***maa://20792 (11.93), maa://39402 (87.18), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.56), *maa://20791 (62.86)</t>
+          <t>maa://22742 (91.61), *maa://20791 (62.86)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.57), maa://26254 (95.83)</t>
+          <t>maa://21249 (94.59), maa://26254 (95.83)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (88.79), **maa://20790 (44.78), ***maa://37170 (18.52)</t>
+          <t>maa://24617 (88.89), **maa://20790 (44.78), ***maa://37170 (18.52)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.69), maa://27484 (96.08), maa://27480 (82.86)</t>
+          <t>maa://27396 (84.42), maa://27484 (96.08), maa://27480 (82.86)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.96), maa://27295 (83.61), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (97.98), maa://27295 (83.61), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.69), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (89.66)</t>
+          <t>**maa://32495 (47.89), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (89.66)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (62.22), ***maa://26209 (13.04), *maa://39394 (68.18)</t>
+          <t>*maa://30062 (63.04), ***maa://26209 (13.04), *maa://39394 (68.18)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>maa://24370 (96.49)</t>
+          <t>maa://24370 (96.55)</t>
         </is>
       </c>
       <c r="I6" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.14), *maa://22758 (72.88)</t>
+          <t>maa://22399 (95.17), *maa://22758 (73.33)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.12.19 13:19:06</t>
+          <t>更新日期：2024.12.20 08:32:28</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (95.95), maa://22755 (87.5), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (95.98), maa://22755 (87.5), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.58), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.6), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (93.42), maa://22501 (98.57)</t>
+          <t>maa://22747 (93.42), maa://22501 (98.59)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (91.74), *maa://22583 (75.81), *maa://22500 (57.78)</t>
+          <t>maa://22676 (91.82), *maa://22583 (75.81), *maa://22500 (57.78)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (76.96), maa://22734 (83.9), *maa://30808 (64.52), **maa://36048 (31.82)</t>
+          <t>*maa://22743 (76.96), maa://22734 (83.9), *maa://30808 (64.52), **maa://36048 (33.33)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.65), maa://39599 (86.11)</t>
+          <t>maa://22430 (88.65), maa://39599 (86.49)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2991,7 +2991,7 @@
       </c>
       <c r="AF19" s="2" t="inlineStr">
         <is>
-          <t>*maa://21663 (61.54)</t>
+          <t>*maa://21663 (62.12)</t>
         </is>
       </c>
       <c r="AG19" s="1" t="n"/>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="X21" s="2" t="inlineStr">
         <is>
-          <t>maa://20110 (86.76), maa://34946 (92.5)</t>
+          <t>maa://20110 (86.76), maa://34946 (92.68)</t>
         </is>
       </c>
       <c r="Y21" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (80.06), ***maa://23820 (29.82)</t>
+          <t>maa://21443 (80.11), ***maa://23820 (29.82)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (93.98), maa://39875 (93.65)</t>
+          <t>maa://39756 (94.0), maa://39875 (93.75)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.67), maa://23504 (93.26), **maa://22892 (39.58), *maa://25141 (77.6), maa://36663 (80.6), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.67), maa://23504 (93.28), **maa://22892 (39.58), *maa://25141 (77.6), maa://36663 (80.6), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (73.97), *maa://25311 (74.0), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (73.47), *maa://25311 (74.0), ***maa://22725 (4.84)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.24), maa://24621 (96.55), maa://36676 (96.67), maa://22771 (85.71), maa://37772 (100.0)</t>
+          <t>maa://20108 (96.24), maa://24621 (96.58), maa://36676 (96.67), maa://22771 (85.71), maa://37772 (100.0)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.68), ***maa://39723 (14.29), maa://41749 (90.57)</t>
+          <t>maa://39929 (89.68), ***maa://39723 (14.29), maa://41749 (90.74)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.05), ***maa://34960 (8.33), *maa://42865 (77.42)</t>
+          <t>*maa://24080 (69.05), ***maa://34960 (8.33), *maa://42865 (78.12)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.25), maa://36667 (98.33), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.27), maa://36667 (98.33), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -5187,7 +5187,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.0), *maa://21239 (66.67)</t>
+          <t>maa://21280 (89.05), *maa://21239 (66.67)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (84.82), maa://36670 (86.9), maa://30434 (89.06), ***maa://25036 (16.0), **maa://44165 (50.0)</t>
+          <t>maa://25199 (84.82), maa://36670 (87.06), maa://30434 (89.23), ***maa://25036 (16.0), **maa://44165 (50.0)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5787,7 +5787,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.78), maa://30807 (95.45), *maa://22767 (55.0), ***maa://20796 (13.79), *maa://42459 (71.43)</t>
+          <t>maa://21229 (84.78), maa://30807 (95.45), *maa://22767 (55.0), ***maa://20796 (13.79), *maa://42459 (75.0)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5840,7 +5840,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.47), maa://43901 (87.5)</t>
+          <t>maa://35931 (92.5), maa://43901 (87.5)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6170,7 +6170,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.49), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.52), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#127)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (91.49), ***maa://21730 (19.4), ***maa://39501 (19.05), *maa://36675 (60.0)</t>
+          <t>maa://25251 (91.58), ***maa://21730 (20.59), ***maa://39501 (19.05), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.59), maa://26254 (95.83)</t>
+          <t>maa://21249 (94.62), maa://26254 (95.83)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (96.55)</t>
+          <t>maa://24390 (96.61)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.98), maa://27295 (83.61), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (98.0), maa://27295 (83.61), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.89), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (89.66)</t>
+          <t>**maa://32495 (48.09), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (90.0)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (83.18), maa://22744 (84.0)</t>
+          <t>maa://21245 (83.41), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>*maa://22757 (77.42)</t>
+          <t>*maa://22757 (78.12)</t>
         </is>
       </c>
       <c r="M5" s="1" t="n"/>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="P6" s="2" t="inlineStr">
         <is>
-          <t>maa://31836 (90.91), maa://30381 (92.31)</t>
+          <t>maa://31836 (91.3), maa://30381 (92.31)</t>
         </is>
       </c>
       <c r="Q6" s="1" t="n"/>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="T7" s="2" t="inlineStr">
         <is>
-          <t>maa://21291 (85.71)</t>
+          <t>maa://21291 (86.05)</t>
         </is>
       </c>
       <c r="U7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.12.20 08:32:28</t>
+          <t>更新日期：2024.12.21 13:17:14</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (85.29), *maa://21916 (61.29), maa://23252 (92.42), maa://37496 (96.3), **maa://22759 (45.45)</t>
+          <t>maa://32931 (85.44), *maa://21916 (61.29), maa://23252 (92.42), maa://37496 (96.3), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (91.36), maa://36669 (88.89), *maa://23264 (61.82)</t>
+          <t>maa://28977 (91.36), maa://36669 (89.19), *maa://23264 (61.82)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.6), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.61), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (88.3)</t>
+          <t>maa://21287 (88.42)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (98.15)</t>
+          <t>maa://36713 (98.16)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (90.18)</t>
+          <t>maa://21867 (89.63)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.36), *maa://21485 (76.87), maa://37962 (88.89)</t>
+          <t>maa://22753 (91.41), *maa://21485 (76.87), maa://37962 (88.89)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.36), maa://36677 (93.88), maa://39872 (90.0)</t>
+          <t>maa://23669 (95.37), maa://36677 (93.88), maa://39872 (90.0)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.75), maa://36673 (92.65), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.77), maa://36673 (92.65), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.43), maa://21288 (96.27), maa://39841 (95.0), maa://36682 (97.37)</t>
+          <t>maa://26245 (96.48), maa://21288 (96.3), maa://39841 (95.0), maa://36682 (97.37)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2309,7 +2309,7 @@
       </c>
       <c r="X14" s="2" t="inlineStr">
         <is>
-          <t>maa://37468 (90.0)</t>
+          <t>maa://37468 (90.48)</t>
         </is>
       </c>
       <c r="Y14" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.31), maa://36679 (93.02), maa://37650 (96.88)</t>
+          <t>maa://21441 (96.33), maa://36679 (93.02), maa://37650 (96.88)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (95.33), *maa://28648 (68.33), maa://36674 (82.93)</t>
+          <t>maa://22729 (95.36), *maa://28648 (68.33), maa://36674 (82.93)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.09)</t>
+          <t>maa://24570 (97.1)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (99.0)</t>
+          <t>maa://24386 (99.02)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (89.86), maa://25198 (93.0), *maa://20795 (51.18), maa://36680 (96.55)</t>
+          <t>maa://21432 (89.86), maa://25198 (93.07), *maa://20795 (51.18), maa://36680 (96.55)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (89.12)</t>
+          <t>maa://22864 (89.19)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (84.21)</t>
+          <t>maa://41331 (84.54)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.58), *maa://22432 (76.67)</t>
+          <t>maa://22524 (94.61), *maa://22432 (76.67)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (94.0), maa://39875 (93.75)</t>
+          <t>maa://39756 (94.02), maa://39875 (93.75)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (79.66)</t>
+          <t>*maa://24368 (79.72)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.49), maa://36672 (80.77), maa://29910 (92.45), **maa://21440 (34.55)</t>
+          <t>maa://22523 (85.57), maa://36672 (80.77), maa://29910 (92.45), **maa://21440 (34.55)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.22)</t>
+          <t>maa://29753 (94.86)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (85.57), *maa://24516 (79.78), maa://26001 (87.5)</t>
+          <t>maa://31215 (85.71), *maa://24516 (79.78), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.68), ***maa://39723 (14.29), maa://41749 (90.74)</t>
+          <t>maa://39929 (89.71), ***maa://39723 (14.29), maa://41749 (90.74)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.88), *maa://36701 (64.29)</t>
+          <t>maa://36660 (92.9), *maa://36701 (64.29)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (92.81), *maa://28440 (76.6), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (92.83), *maa://28440 (76.6), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.23)</t>
+          <t>maa://42979 (96.26)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.55)</t>
+          <t>maa://41296 (96.61)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5105,7 +5105,7 @@
       </c>
       <c r="T36" s="2" t="inlineStr">
         <is>
-          <t>maa://27613 (99.02)</t>
+          <t>maa://27613 (99.03)</t>
         </is>
       </c>
       <c r="U36" s="1" t="n"/>
@@ -5458,7 +5458,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.96), maa://21386 (95.74), maa://36664 (90.74)</t>
+          <t>maa://23278 (95.97), maa://21386 (95.74), maa://36664 (90.74)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -6242,7 +6242,7 @@
       </c>
       <c r="H57" s="2" t="inlineStr">
         <is>
-          <t>maa://25176 (98.18)</t>
+          <t>maa://25176 (98.21)</t>
         </is>
       </c>
       <c r="I57" s="1" t="n"/>
@@ -6296,7 +6296,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (59.09)</t>
+          <t>*maa://40438 (60.0)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>
@@ -6332,7 +6332,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (96.15), maa://43903 (100.0)</t>
+          <t>maa://42981 (96.3), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>
@@ -6368,7 +6368,7 @@
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>maa://44405 (95.0)</t>
+          <t>maa://44405 (95.24)</t>
         </is>
       </c>
       <c r="I64" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#128)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.24), maa://25390 (95.9), maa://36681 (87.01)</t>
+          <t>maa://24702 (94.24), maa://25390 (95.92), maa://36681 (87.01)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (55.48), *maa://30515 (69.0), *maa://34787 (72.06), ***maa://20792 (11.93), maa://39402 (87.18), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (55.48), *maa://30515 (69.0), *maa://34787 (72.06), ***maa://20792 (11.93), maa://39402 (87.5), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.93), maa://20276 (84.81), *maa://22749 (72.73)</t>
+          <t>*maa://22880 (66.12), maa://20276 (84.81), *maa://22749 (72.73)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (88.89), **maa://20790 (44.78), ***maa://37170 (18.52)</t>
+          <t>maa://24617 (88.89), **maa://20790 (44.78), ***maa://37170 (20.0)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.42), maa://27484 (96.08), maa://27480 (82.86)</t>
+          <t>maa://27396 (84.42), maa://27484 (96.12), maa://27480 (82.86)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.24), **maa://24303 (33.33), maa://22499 (85.71), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.24), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>maa://21955 (93.94)</t>
+          <t>maa://21955 (94.12)</t>
         </is>
       </c>
       <c r="E7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.12.21 13:17:14</t>
+          <t>更新日期：2024.12.22 13:16:54</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>*maa://21476 (71.74), **maa://39431 (45.45), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (72.34), **maa://39431 (45.45), *maa://37551 (57.14)</t>
         </is>
       </c>
       <c r="E8" s="1" t="n"/>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (85.44), *maa://21916 (61.29), maa://23252 (92.42), maa://37496 (96.3), **maa://22759 (45.45)</t>
+          <t>maa://32931 (84.62), *maa://21916 (61.29), maa://23252 (92.42), maa://37496 (96.3), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.89)</t>
+          <t>maa://21411 (95.91)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (81.11)</t>
+          <t>maa://22736 (81.32)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.44)</t>
+          <t>maa://26223 (97.46)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (89.32), **maa://22865 (50.0)</t>
+          <t>maa://26206 (89.32), *maa://22865 (50.98)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.44), **maa://32237 (40.48), ***maa://34206 (18.18), ***maa://39951 (17.07), ***maa://39243 (28.57)</t>
+          <t>***maa://25695 (19.44), **maa://32237 (40.48), ***maa://34206 (21.74), ***maa://39951 (17.07), ***maa://39243 (28.57)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.37), maa://36677 (93.88), maa://39872 (90.0)</t>
+          <t>maa://23669 (95.39), maa://36677 (93.88), maa://39872 (90.0)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.63), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (78.79), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>*maa://34957 (79.03), *maa://22768 (51.61)</t>
+          <t>*maa://34957 (79.37), *maa://22768 (51.61)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.48), maa://21288 (96.3), maa://39841 (95.0), maa://36682 (97.37)</t>
+          <t>maa://26245 (96.5), maa://21288 (96.3), maa://39841 (95.06), maa://36682 (97.37)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (76.96), maa://22734 (83.9), *maa://30808 (64.52), **maa://36048 (33.33)</t>
+          <t>*maa://22743 (76.96), maa://22734 (84.03), *maa://30808 (64.52), **maa://36048 (33.33)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (90.2), *maa://22727 (70.0)</t>
+          <t>maa://24762 (90.26), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.84), *maa://22766 (70.91), *maa://36666 (78.57)</t>
+          <t>maa://21364 (80.91), *maa://22766 (70.91), *maa://36666 (78.57)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (90.3)</t>
+          <t>maa://24421 (90.34)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (99.02)</t>
+          <t>maa://24386 (99.04)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (63.05), *maa://36668 (55.84)</t>
+          <t>*maa://30709 (63.14), *maa://36668 (55.84)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (89.19)</t>
+          <t>maa://22864 (89.26)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.61), *maa://22432 (76.67)</t>
+          <t>maa://22524 (94.63), *maa://22432 (76.67)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (85.15), *maa://22751 (73.85)</t>
+          <t>maa://27127 (85.29), *maa://22751 (73.85)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.46), *maa://37649 (68.0)</t>
+          <t>maa://21282 (98.46), *maa://37649 (69.23)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (94.02), maa://39875 (93.75)</t>
+          <t>maa://39756 (94.05), maa://39875 (93.75)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.98), *maa://29748 (75.59), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
+          <t>maa://30587 (91.98), *maa://29748 (75.78), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.67), maa://23504 (93.28), **maa://22892 (39.58), *maa://25141 (77.6), maa://36663 (80.6), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.73), maa://23504 (93.28), **maa://22892 (39.58), *maa://25141 (77.6), maa://36663 (80.6), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (73.47), *maa://25311 (74.0), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (73.65), *maa://25311 (74.0), ***maa://22725 (4.84)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.24), maa://24621 (96.58), maa://36676 (96.67), maa://22771 (85.71), maa://37772 (100.0)</t>
+          <t>maa://20108 (96.27), maa://24621 (96.58), maa://36676 (96.67), maa://22771 (85.71), maa://37772 (100.0)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (93.15)</t>
+          <t>maa://42235 (93.24)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>maa://23263 (94.9), *maa://29765 (60.53)</t>
+          <t>maa://23263 (94.95), *maa://29765 (60.53)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.71), ***maa://39723 (14.29), maa://41749 (90.74)</t>
+          <t>maa://39929 (89.74), ***maa://39723 (14.29), maa://41749 (90.74)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (92.83), *maa://28440 (76.6), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (92.86), *maa://28440 (76.6), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.05), ***maa://34960 (8.33), *maa://42865 (78.12)</t>
+          <t>*maa://24080 (69.05), ***maa://34960 (8.33), *maa://42865 (78.79)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.96), maa://36258 (83.16), *maa://43904 (71.43)</t>
+          <t>maa://35926 (93.98), maa://36258 (83.16), *maa://43904 (71.43)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (84.82), maa://36670 (87.06), maa://30434 (89.23), ***maa://25036 (16.0), **maa://44165 (50.0)</t>
+          <t>maa://25199 (84.82), maa://36670 (87.21), maa://30434 (89.23), ***maa://25036 (16.0), **maa://44165 (50.0)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5543,7 +5543,7 @@
       </c>
       <c r="P41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (38.24), maa://43177 (84.62)</t>
+          <t>**maa://35616 (38.24), maa://43177 (85.71)</t>
         </is>
       </c>
       <c r="Q41" s="1" t="n"/>
@@ -5787,7 +5787,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.78), maa://30807 (95.45), *maa://22767 (55.0), ***maa://20796 (13.79), *maa://42459 (75.0)</t>
+          <t>maa://21229 (84.86), maa://30807 (95.45), *maa://22767 (55.0), ***maa://20796 (13.79), *maa://42459 (75.0)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.18), maa://29661 (97.83), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.18), maa://29661 (97.84), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#129)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (55.48), *maa://30515 (69.0), *maa://34787 (72.06), ***maa://20792 (11.93), maa://39402 (87.5), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (55.48), *maa://30515 (69.0), *maa://34787 (72.06), ***maa://20792 (11.93), maa://39402 (87.8), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.12.22 13:16:54</t>
+          <t>更新日期：2024.12.23 13:18:33</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.4)</t>
+          <t>maa://36707 (99.41)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (91.82), *maa://22583 (75.81), *maa://22500 (57.78)</t>
+          <t>maa://22676 (91.82), *maa://22583 (76.19), *maa://22500 (57.78)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (65.35), maa://27755 (92.5)</t>
+          <t>*maa://23911 (65.35), maa://27755 (92.59)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (63.14), *maa://36668 (55.84)</t>
+          <t>*maa://30709 (63.24), *maa://36668 (55.84)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (89.26)</t>
+          <t>maa://22864 (89.33)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (94.05), maa://39875 (93.75)</t>
+          <t>maa://39756 (94.07), maa://39875 (93.75)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.74), ***maa://39723 (14.29), maa://41749 (90.74)</t>
+          <t>maa://39929 (89.74), ***maa://39723 (14.29), maa://41749 (90.91)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (92.86), *maa://28440 (76.6), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (92.88), *maa://28440 (76.6), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.61)</t>
+          <t>maa://41296 (96.64)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5458,7 +5458,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.97), maa://21386 (95.74), maa://36664 (90.74)</t>
+          <t>maa://23278 (95.99), maa://21386 (95.74), maa://36664 (90.74)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5734,7 +5734,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.79), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.8), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.18), maa://29661 (97.84), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.19), maa://29661 (97.84), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6170,7 +6170,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.52), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.54), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6368,7 +6368,7 @@
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>maa://44405 (95.24)</t>
+          <t>maa://44405 (95.45)</t>
         </is>
       </c>
       <c r="I64" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#130)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.24), maa://25390 (95.92), maa://36681 (87.01)</t>
+          <t>maa://24702 (94.27), maa://25390 (95.92), maa://36681 (87.01)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (91.58), ***maa://21730 (20.59), ***maa://39501 (19.05), *maa://36675 (60.0)</t>
+          <t>maa://25251 (91.67), ***maa://21730 (20.59), ***maa://39501 (18.18), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (66.12), maa://20276 (84.81), *maa://22749 (72.73)</t>
+          <t>*maa://22880 (65.76), maa://20276 (84.91), *maa://22749 (72.73)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (88.89), **maa://20790 (44.78), ***maa://37170 (20.0)</t>
+          <t>maa://24617 (88.99), **maa://20790 (44.78), ***maa://37170 (19.3)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.42), maa://27484 (96.12), maa://27480 (82.86)</t>
+          <t>maa://27396 (84.42), maa://27484 (96.15), maa://27480 (82.86)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.24), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.29), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="AB5" s="2" t="inlineStr">
         <is>
-          <t>*maa://29863 (71.88), ***maa://22752 (13.33), **maa://26013 (42.86)</t>
+          <t>*maa://29863 (69.7), ***maa://22752 (13.33), **maa://26013 (42.86)</t>
         </is>
       </c>
       <c r="AC5" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.12.23 13:18:33</t>
+          <t>更新日期：2024.12.24 13:17:51</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.91)</t>
+          <t>maa://21411 (95.92)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.46)</t>
+          <t>maa://26223 (97.48)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (91.36), maa://36669 (89.19), *maa://23264 (61.82)</t>
+          <t>maa://28977 (91.36), maa://36669 (89.47), *maa://23264 (61.82)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (95.98), maa://22755 (87.5), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.0), maa://22755 (87.61), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.61), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.62), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (76.96), maa://22734 (84.03), *maa://30808 (64.52), **maa://36048 (33.33)</t>
+          <t>*maa://22743 (76.96), maa://22734 (84.03), *maa://30808 (65.08), **maa://36048 (33.33)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (95.36), *maa://28648 (68.33), maa://36674 (82.93)</t>
+          <t>maa://22729 (95.39), *maa://28648 (68.33), maa://36674 (82.93)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.65), maa://39599 (86.49)</t>
+          <t>maa://22430 (88.65), maa://39599 (86.84)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (90.34)</t>
+          <t>maa://24421 (90.38)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (99.04)</t>
+          <t>maa://24386 (99.05)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (89.86), maa://25198 (93.07), *maa://20795 (51.18), maa://36680 (96.55)</t>
+          <t>maa://21432 (89.86), maa://25198 (93.07), *maa://20795 (51.18), maa://36680 (96.67)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (94.07), maa://39875 (93.75)</t>
+          <t>maa://39756 (94.12), maa://39875 (93.75)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.98), *maa://29748 (75.78), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
+          <t>maa://30587 (92.02), *maa://29748 (75.78), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.73), maa://23504 (93.28), **maa://22892 (39.58), *maa://25141 (77.6), maa://36663 (80.6), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.73), maa://23504 (93.28), **maa://22892 (39.58), *maa://25141 (76.98), maa://36663 (80.6), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.57), maa://36672 (80.77), maa://29910 (92.45), **maa://21440 (34.55)</t>
+          <t>maa://22523 (85.64), maa://36672 (80.77), maa://29910 (92.45), **maa://21440 (34.55)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.74), ***maa://39723 (14.29), maa://41749 (90.91)</t>
+          <t>maa://39929 (89.84), ***maa://39723 (14.29), maa://41749 (90.91)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.9), *maa://36701 (64.29)</t>
+          <t>maa://36660 (92.93), *maa://36701 (64.29)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.26)</t>
+          <t>maa://42979 (96.3)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.98), maa://36258 (83.16), *maa://43904 (71.43)</t>
+          <t>maa://35926 (93.98), maa://36258 (83.16), *maa://43904 (75.0)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.1), maa://41108 (87.76), maa://41238 (96.15)</t>
+          <t>maa://42859 (96.2), maa://41108 (87.76), maa://41238 (96.15)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (84.82), maa://36670 (87.21), maa://30434 (89.23), ***maa://25036 (16.0), **maa://44165 (50.0)</t>
+          <t>maa://25199 (84.82), maa://36670 (87.21), maa://30434 (89.23), ***maa://25036 (16.0), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5840,7 +5840,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.5), maa://43901 (87.5)</t>
+          <t>maa://35931 (92.5), maa://43901 (88.89)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#131)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (55.48), *maa://30515 (69.0), *maa://34787 (72.06), ***maa://20792 (11.93), maa://39402 (87.8), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.05), *maa://30515 (69.31), *maa://34787 (72.46), ***maa://20792 (11.93), maa://39402 (88.37), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.61), *maa://20791 (62.86)</t>
+          <t>maa://22742 (91.67), *maa://20791 (63.38)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.32), maa://36684 (95.7), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.32), maa://36684 (95.74), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (91.67), ***maa://21730 (20.59), ***maa://39501 (18.18), *maa://36675 (60.0)</t>
+          <t>maa://25251 (91.75), ***maa://21730 (21.74), ***maa://39501 (18.18), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.41), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.44), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.76), maa://20276 (84.91), *maa://22749 (72.73)</t>
+          <t>*maa://22880 (65.95), maa://20276 (85.0), *maa://22749 (72.73)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.62), maa://26254 (95.83)</t>
+          <t>maa://21249 (94.22), maa://26254 (95.83)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.42), maa://27484 (96.15), maa://27480 (82.86)</t>
+          <t>maa://27396 (84.52), maa://27484 (96.15), maa://27480 (82.86)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (96.61)</t>
+          <t>maa://24390 (93.55)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.29), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.33), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (98.0), maa://27295 (83.61), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (98.04), maa://27295 (83.87), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.09), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (90.0)</t>
+          <t>**maa://32495 (47.91), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (90.32)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (83.41), maa://22744 (84.0)</t>
+          <t>maa://21245 (83.49), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>*maa://22757 (78.12)</t>
+          <t>*maa://22757 (78.79)</t>
         </is>
       </c>
       <c r="M5" s="1" t="n"/>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="AB5" s="2" t="inlineStr">
         <is>
-          <t>*maa://29863 (69.7), ***maa://22752 (13.33), **maa://26013 (42.86)</t>
+          <t>*maa://29863 (67.65), ***maa://22752 (12.5), **maa://26013 (37.5)</t>
         </is>
       </c>
       <c r="AC5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (94.44)</t>
+          <t>maa://42407 (94.59)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>maa://24839 (99.28)</t>
+          <t>maa://24839 (99.29)</t>
         </is>
       </c>
       <c r="M6" s="1" t="n"/>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>*maa://22763 (67.86)</t>
+          <t>*maa://22763 (68.97)</t>
         </is>
       </c>
       <c r="I7" s="1" t="n"/>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="T7" s="2" t="inlineStr">
         <is>
-          <t>maa://21291 (86.05)</t>
+          <t>maa://21291 (84.09)</t>
         </is>
       </c>
       <c r="U7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (67.95), *maa://36671 (70.83), *maa://42530 (69.23)</t>
+          <t>*maa://26191 (67.95), *maa://36671 (69.39), *maa://42530 (64.29)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.12.24 13:17:51</t>
+          <t>更新日期：2024.12.29 14:56:16</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (84.62), *maa://21916 (61.29), maa://23252 (92.42), maa://37496 (96.3), **maa://22759 (45.45)</t>
+          <t>maa://32931 (84.62), *maa://21916 (61.29), maa://23252 (92.42), maa://37496 (96.43), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (81.32)</t>
+          <t>maa://22736 (81.52)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.0), ***maa://22740 (5.88), **maa://39938 (48.0), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (93.33)</t>
+          <t>maa://28711 (87.25), ***maa://22740 (5.77), **maa://39938 (48.0), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (93.33)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (89.32), *maa://22865 (50.98)</t>
+          <t>maa://26206 (89.32), *maa://22865 (51.92)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1741,7 +1741,7 @@
       </c>
       <c r="L10" s="2" t="inlineStr">
         <is>
-          <t>**maa://24395 (42.31)</t>
+          <t>**maa://24395 (40.74)</t>
         </is>
       </c>
       <c r="M10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.0), maa://22755 (87.61), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.07), maa://22755 (87.61), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.62), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.63), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (53.66), *maa://22733 (59.38), maa://22761 (100.0)</t>
+          <t>*maa://25021 (54.22), *maa://22733 (59.38), maa://22761 (100.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (93.42), maa://22501 (98.59)</t>
+          <t>maa://22747 (92.81), maa://22501 (98.59)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (98.16)</t>
+          <t>maa://36713 (98.17)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1935,7 +1935,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://29912 (100.0), maa://22516 (89.41), *maa://20794 (52.24)</t>
+          <t>maa://29912 (100.0), maa://22516 (88.37), *maa://20794 (52.24)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (89.63)</t>
+          <t>maa://21867 (89.7)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.41), *maa://21485 (76.87), maa://37962 (88.89)</t>
+          <t>maa://22753 (91.46), *maa://21485 (76.87), maa://37962 (89.66)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.39), maa://36677 (93.88), maa://39872 (90.0)</t>
+          <t>maa://23669 (95.41), maa://36677 (92.16), maa://39872 (90.0)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.77), maa://36673 (92.65), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.79), maa://36673 (92.65), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (91.82), *maa://22583 (76.19), *maa://22500 (57.78)</t>
+          <t>maa://22676 (91.82), *maa://22583 (75.0), *maa://22500 (57.78)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.5), maa://21288 (96.3), maa://39841 (95.06), maa://36682 (97.37)</t>
+          <t>maa://26245 (96.53), maa://21288 (96.3), maa://39841 (95.12), maa://36682 (97.37)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (76.96), maa://22734 (84.03), *maa://30808 (65.08), **maa://36048 (33.33)</t>
+          <t>*maa://22743 (77.32), maa://22734 (84.03), *maa://30808 (65.08), **maa://36048 (33.33)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.56), maa://21478 (91.43)</t>
+          <t>maa://24304 (88.18), maa://21478 (91.43)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (90.26), *maa://22727 (70.0)</t>
+          <t>maa://24762 (90.32), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.33), maa://36679 (93.02), maa://37650 (96.88)</t>
+          <t>maa://21441 (96.35), maa://36679 (93.02), maa://37650 (96.97)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (65.35), maa://27755 (92.59)</t>
+          <t>*maa://23911 (65.69), maa://27755 (92.68)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.65), maa://39599 (86.84)</t>
+          <t>maa://22430 (88.71), maa://39599 (86.84)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2667,7 +2667,7 @@
       </c>
       <c r="P17" s="2" t="inlineStr">
         <is>
-          <t>maa://23890 (80.81), *maa://24940 (67.86)</t>
+          <t>maa://23890 (81.0), *maa://24940 (67.86)</t>
         </is>
       </c>
       <c r="Q17" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (90.38)</t>
+          <t>maa://24421 (90.46)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (88.81), *maa://22732 (50.6)</t>
+          <t>maa://22466 (88.89), *maa://22732 (50.6)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (57.59), **maa://29784 (44.44)</t>
+          <t>*maa://24313 (57.86), **maa://29784 (44.44)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (63.24), *maa://36668 (55.84)</t>
+          <t>*maa://30709 (63.5), *maa://36668 (55.84)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -2991,7 +2991,7 @@
       </c>
       <c r="AF19" s="2" t="inlineStr">
         <is>
-          <t>*maa://21663 (62.12)</t>
+          <t>*maa://21663 (61.19)</t>
         </is>
       </c>
       <c r="AG19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (89.86), maa://25198 (93.07), *maa://20795 (51.18), maa://36680 (96.67)</t>
+          <t>maa://21432 (89.86), maa://25198 (93.14), *maa://20795 (51.18), maa://36680 (96.67)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (84.54)</t>
+          <t>maa://41331 (84.69)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3155,7 +3155,7 @@
       </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>maa://24372 (96.74)</t>
+          <t>maa://24372 (96.77)</t>
         </is>
       </c>
       <c r="I21" s="1" t="n"/>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (27.94), *maa://41753 (58.33)</t>
+          <t>***maa://28036 (27.54), *maa://41753 (53.85)</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (94.12), maa://39875 (93.75)</t>
+          <t>maa://39756 (94.21), maa://39875 (93.75)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="X23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (67.16)</t>
+          <t>*maa://28503 (66.18)</t>
         </is>
       </c>
       <c r="Y23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (79.72)</t>
+          <t>*maa://24368 (79.55)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.73), maa://23504 (93.28), **maa://22892 (39.58), *maa://25141 (76.98), maa://36663 (80.6), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.84), maa://23504 (93.33), **maa://22892 (39.58), *maa://25141 (76.98), *maa://36663 (79.41), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.64), maa://36672 (80.77), maa://29910 (92.45), **maa://21440 (34.55)</t>
+          <t>maa://22523 (85.64), maa://36672 (80.77), maa://29910 (92.59), **maa://21440 (34.55)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (94.86)</t>
+          <t>maa://29753 (94.88)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (73.65), *maa://25311 (74.0), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (73.65), *maa://25311 (73.27), ***maa://22725 (4.84)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.84), ***maa://39723 (14.29), maa://41749 (90.91)</t>
+          <t>maa://39929 (89.91), ***maa://39723 (14.29), maa://41749 (91.07)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.93), *maa://36701 (64.29)</t>
+          <t>maa://36660 (92.97), *maa://36701 (64.29)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (92.88), *maa://28440 (76.6), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (92.9), *maa://28440 (76.6), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4227,7 +4227,7 @@
       </c>
       <c r="P29" s="2" t="inlineStr">
         <is>
-          <t>*maa://23168 (54.72), *maa://30050 (51.85)</t>
+          <t>*maa://23168 (54.72), *maa://30050 (51.72)</t>
         </is>
       </c>
       <c r="Q29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.05), ***maa://34960 (8.33), *maa://42865 (78.79)</t>
+          <t>*maa://24080 (69.05), ***maa://34960 (8.33), *maa://42865 (76.47)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4400,12 +4400,12 @@
       </c>
       <c r="AA30" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.3)</t>
+          <t>maa://42979 (96.36), maa://45045 (100.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.98), maa://36258 (83.16), *maa://43904 (75.0)</t>
+          <t>maa://35926 (93.63), maa://36258 (83.33), *maa://43904 (77.78)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.27), maa://36667 (98.33), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.28), maa://36667 (98.39), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.2), maa://41108 (87.76), maa://41238 (96.15)</t>
+          <t>maa://42859 (96.34), maa://41108 (87.76), maa://41238 (96.2)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (93.55)</t>
+          <t>maa://24526 (93.57)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.64)</t>
+          <t>maa://41296 (96.67)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5187,7 +5187,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.05), *maa://21239 (66.67)</t>
+          <t>maa://21280 (89.11), *maa://21239 (66.67)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="P38" s="2" t="inlineStr">
         <is>
-          <t>*maa://24383 (67.71)</t>
+          <t>*maa://24383 (68.04)</t>
         </is>
       </c>
       <c r="Q38" s="1" t="n"/>
@@ -5336,12 +5336,12 @@
       </c>
       <c r="G39" s="1" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (84.82), maa://36670 (87.21), maa://30434 (89.23), ***maa://25036 (16.0), *maa://44165 (66.67)</t>
+          <t>maa://25199 (84.82), maa://36670 (87.5), maa://30434 (89.39), ***maa://25036 (16.0), *maa://44165 (66.67), maa://45059 (100.0)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (92.13)</t>
+          <t>maa://24709 (91.41)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5734,7 +5734,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.8), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.83), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5787,7 +5787,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.86), maa://30807 (95.45), *maa://22767 (55.0), ***maa://20796 (13.79), *maa://42459 (75.0)</t>
+          <t>maa://21229 (84.86), maa://30807 (95.45), *maa://22767 (55.0), ***maa://20796 (13.79), *maa://42459 (77.78)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5819,7 +5819,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (35.0)</t>
+          <t>**maa://39364 (38.1)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -6206,7 +6206,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.22)</t>
+          <t>maa://32532 (92.25)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (83.02), maa://31270 (94.78)</t>
+          <t>maa://27746 (83.02), maa://31270 (94.83)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6296,7 +6296,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (60.0)</t>
+          <t>*maa://40438 (60.87)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>
@@ -6332,7 +6332,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (96.3), maa://43903 (100.0)</t>
+          <t>maa://42981 (96.43), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>
@@ -6368,7 +6368,7 @@
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>maa://44405 (95.45)</t>
+          <t>maa://44405 (91.3)</t>
         </is>
       </c>
       <c r="I64" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#132)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.27), maa://25390 (95.92), maa://36681 (87.01)</t>
+          <t>maa://24702 (94.27), maa://25390 (95.93), maa://36681 (87.01)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.05), *maa://30515 (69.31), *maa://34787 (72.46), ***maa://20792 (11.93), maa://39402 (88.37), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.05), *maa://30515 (69.31), *maa://34787 (72.86), ***maa://20792 (11.93), maa://39402 (88.37), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (91.75), ***maa://21730 (21.74), ***maa://39501 (18.18), *maa://36675 (60.0)</t>
+          <t>maa://25251 (91.75), ***maa://21730 (22.86), ***maa://39501 (18.18), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.44), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.45), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.22), maa://26254 (95.83)</t>
+          <t>maa://21249 (94.22), maa://26254 (96.0)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.33), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.38), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (93.1), maa://24957 (97.62)</t>
+          <t>maa://28624 (93.18), maa://24957 (97.62)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (67.95), *maa://36671 (69.39), *maa://42530 (64.29)</t>
+          <t>*maa://26191 (68.35), *maa://36671 (69.39), *maa://42530 (64.29)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.12.29 14:56:16</t>
+          <t>更新日期：2024.12.31 13:17:57</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.92)</t>
+          <t>maa://21411 (95.93)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.44), **maa://32237 (40.48), ***maa://34206 (21.74), ***maa://39951 (17.07), ***maa://39243 (28.57)</t>
+          <t>***maa://25695 (19.44), **maa://32237 (40.48), ***maa://34206 (21.74), ***maa://39951 (16.67), ***maa://39243 (28.57)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (89.7)</t>
+          <t>maa://21867 (89.76)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.41), maa://36677 (92.16), maa://39872 (90.0)</t>
+          <t>maa://23669 (95.41), maa://36677 (92.31), maa://39872 (90.0)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (91.82), *maa://22583 (75.0), *maa://22500 (57.78)</t>
+          <t>maa://22676 (91.96), *maa://22583 (75.0), *maa://22500 (57.78)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>*maa://34957 (79.37), *maa://22768 (51.61)</t>
+          <t>*maa://34957 (79.69), *maa://22768 (51.61)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="T15" s="2" t="inlineStr">
         <is>
-          <t>maa://23892 (98.68)</t>
+          <t>maa://23892 (97.4)</t>
         </is>
       </c>
       <c r="U15" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (95.39), *maa://28648 (68.33), maa://36674 (82.93)</t>
+          <t>maa://22729 (95.39), *maa://28648 (68.85), maa://36674 (82.93)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (90.46)</t>
+          <t>maa://24421 (90.5)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (88.89), *maa://22732 (50.6)</t>
+          <t>maa://22466 (88.97), *maa://22732 (50.6)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (89.86), maa://25198 (93.14), *maa://20795 (51.18), maa://36680 (96.67)</t>
+          <t>maa://21432 (89.86), maa://25198 (93.14), *maa://20795 (51.18), maa://36680 (93.55)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (84.69)</t>
+          <t>maa://41331 (85.15)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (80.11), ***maa://23820 (29.82)</t>
+          <t>maa://21443 (80.17), ***maa://23820 (29.82)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (85.29), *maa://22751 (73.85)</t>
+          <t>maa://27127 (85.44), *maa://22751 (73.85)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.46), *maa://37649 (69.23)</t>
+          <t>maa://21282 (98.47), *maa://37649 (66.67)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (94.21), maa://39875 (93.75)</t>
+          <t>maa://39756 (94.3), maa://39875 (93.75)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.84), maa://23504 (93.33), **maa://22892 (39.58), *maa://25141 (76.98), *maa://36663 (79.41), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.84), maa://23504 (93.15), **maa://22892 (39.58), *maa://25141 (76.98), *maa://36663 (78.26), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.64), maa://36672 (80.77), maa://29910 (92.59), **maa://21440 (34.55)</t>
+          <t>maa://22523 (85.71), maa://36672 (80.77), maa://29910 (92.59), **maa://21440 (34.55)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3739,7 +3739,7 @@
       </c>
       <c r="X25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29890 (76.19)</t>
+          <t>*maa://29890 (76.74)</t>
         </is>
       </c>
       <c r="Y25" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.27), maa://24621 (96.58), maa://36676 (96.67), maa://22771 (85.71), maa://37772 (100.0)</t>
+          <t>maa://20108 (96.27), maa://24621 (96.58), maa://36676 (96.77), maa://22771 (85.71), maa://37772 (100.0)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.91), ***maa://39723 (14.29), maa://41749 (91.07)</t>
+          <t>maa://39929 (89.97), ***maa://39723 (14.29), maa://41749 (91.38)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.97), *maa://36701 (64.29)</t>
+          <t>maa://36660 (92.99), *maa://36701 (64.29)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (92.9), *maa://28440 (76.6), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (92.9), *maa://28440 (76.84), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.36), maa://45045 (100.0)</t>
+          <t>maa://42979 (96.4), maa://45045 (100.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.63), maa://36258 (83.33), *maa://43904 (77.78)</t>
+          <t>maa://35926 (93.66), maa://36258 (83.67), *maa://43904 (77.78)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.28), maa://36667 (98.39), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.3), maa://36667 (98.39), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.34), maa://41108 (87.76), maa://41238 (96.2)</t>
+          <t>maa://42859 (96.34), maa://41108 (87.76), maa://41238 (96.3)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.67)</t>
+          <t>maa://41296 (96.69)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5007,7 +5007,7 @@
       </c>
       <c r="T35" s="2" t="inlineStr">
         <is>
-          <t>maa://24842 (94.0)</t>
+          <t>maa://24842 (94.12)</t>
         </is>
       </c>
       <c r="U35" s="1" t="n"/>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (84.82), maa://36670 (87.5), maa://30434 (89.39), ***maa://25036 (16.0), *maa://44165 (66.67), maa://45059 (100.0)</t>
+          <t>maa://25199 (84.82), maa://36670 (87.64), maa://30434 (89.39), ***maa://25036 (16.0), *maa://44165 (66.67), maa://45059 (100.0)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5734,7 +5734,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.83), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.84), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5840,7 +5840,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.5), maa://43901 (88.89)</t>
+          <t>maa://35931 (92.61), maa://43901 (88.89)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.19), maa://29661 (97.84), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.2), maa://29661 (97.86), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6170,7 +6170,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.54), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.56), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6206,7 +6206,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.25)</t>
+          <t>maa://32532 (91.92)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6242,7 +6242,7 @@
       </c>
       <c r="H57" s="2" t="inlineStr">
         <is>
-          <t>maa://25176 (98.21)</t>
+          <t>maa://25176 (98.25)</t>
         </is>
       </c>
       <c r="I57" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#133)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.05), *maa://30515 (69.31), *maa://34787 (72.86), ***maa://20792 (11.93), maa://39402 (88.37), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.05), *maa://30515 (69.31), *maa://34787 (72.86), ***maa://20792 (11.93), maa://39402 (88.64), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (91.75), ***maa://21730 (22.86), ***maa://39501 (18.18), *maa://36675 (60.0)</t>
+          <t>maa://25251 (91.84), ***maa://21730 (22.86), ***maa://39501 (18.18), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.95), maa://20276 (85.0), *maa://22749 (72.73)</t>
+          <t>*maa://22880 (65.95), maa://20276 (85.09), *maa://22749 (72.73)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>maa://21955 (94.12)</t>
+          <t>maa://21955 (94.29)</t>
         </is>
       </c>
       <c r="E7" s="1" t="n"/>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>*maa://22763 (68.97)</t>
+          <t>*maa://22763 (66.67)</t>
         </is>
       </c>
       <c r="I7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.12.31 13:17:57</t>
+          <t>更新日期：2025.01.01 13:19:57</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>*maa://21476 (72.34), **maa://39431 (45.45), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (72.92), **maa://39431 (45.45), *maa://37551 (57.14)</t>
         </is>
       </c>
       <c r="E8" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.25), ***maa://22740 (5.77), **maa://39938 (48.0), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (93.33)</t>
+          <t>maa://28711 (87.38), ***maa://22740 (5.77), **maa://39938 (48.0), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (93.33)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.07), maa://22755 (87.61), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.09), maa://22755 (87.61), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.63), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.64), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.53), maa://21288 (96.3), maa://39841 (95.12), maa://36682 (97.37)</t>
+          <t>maa://26245 (96.53), maa://21288 (96.3), maa://39841 (95.18), maa://36682 (97.37)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.32), maa://22734 (84.03), *maa://30808 (65.08), **maa://36048 (33.33)</t>
+          <t>*maa://22743 (77.44), maa://22734 (84.03), *maa://30808 (65.08), **maa://36048 (32.61)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.91), *maa://22766 (70.91), *maa://36666 (78.57)</t>
+          <t>maa://21364 (80.91), *maa://22766 (70.91), *maa://36666 (78.82)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (95.39), *maa://28648 (68.85), maa://36674 (82.93)</t>
+          <t>maa://22729 (94.77), *maa://28648 (68.85), maa://36674 (82.93)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (90.5)</t>
+          <t>maa://24421 (90.12)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (63.5), *maa://36668 (55.84)</t>
+          <t>*maa://30709 (63.59), *maa://36668 (55.84)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (94.3), maa://39875 (93.75)</t>
+          <t>maa://39756 (94.32), maa://39875 (93.75)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (79.55)</t>
+          <t>*maa://24368 (78.89)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.84), maa://23504 (93.15), **maa://22892 (39.58), *maa://25141 (76.98), *maa://36663 (78.26), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.84), maa://23504 (93.15), **maa://22892 (39.31), *maa://25141 (76.38), *maa://36663 (78.26), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3739,7 +3739,7 @@
       </c>
       <c r="X25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29890 (76.74)</t>
+          <t>*maa://29890 (77.27)</t>
         </is>
       </c>
       <c r="Y25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (85.71), *maa://24516 (79.78), maa://26001 (87.5)</t>
+          <t>maa://31215 (85.86), *maa://24516 (79.78), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3869,7 +3869,7 @@
       </c>
       <c r="X26" s="2" t="inlineStr">
         <is>
-          <t>maa://24389 (96.3)</t>
+          <t>maa://24389 (96.43)</t>
         </is>
       </c>
       <c r="Y26" s="1" t="n"/>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (48.0), maa://34494 (96.43), *maa://39601 (76.47), **maa://36665 (44.44)</t>
+          <t>**maa://21283 (48.0), maa://34494 (96.55), *maa://39601 (76.47), **maa://36665 (44.44)</t>
         </is>
       </c>
       <c r="I27" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.97), ***maa://39723 (14.29), maa://41749 (91.38)</t>
+          <t>maa://39929 (89.72), ***maa://39723 (14.29), maa://41749 (91.53)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.99), *maa://36701 (64.29)</t>
+          <t>maa://36660 (93.02), *maa://36701 (64.29)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (92.9), *maa://28440 (76.84), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (92.93), *maa://28440 (76.84), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4227,7 +4227,7 @@
       </c>
       <c r="P29" s="2" t="inlineStr">
         <is>
-          <t>*maa://23168 (54.72), *maa://30050 (51.72)</t>
+          <t>*maa://23168 (55.56), *maa://30050 (51.72)</t>
         </is>
       </c>
       <c r="Q29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.05), ***maa://34960 (8.33), *maa://42865 (76.47)</t>
+          <t>*maa://24080 (69.05), ***maa://34960 (8.33), *maa://42865 (77.14)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.4), maa://45045 (100.0)</t>
+          <t>maa://42979 (96.43), maa://45045 (100.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.19)</t>
+          <t>maa://36697 (86.26)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -6332,7 +6332,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (96.43), maa://43903 (100.0)</t>
+          <t>maa://42981 (96.55), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#134)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.27), maa://25390 (95.93), maa://36681 (87.01)</t>
+          <t>maa://24702 (94.29), maa://25390 (95.95), maa://36681 (87.01)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.05), *maa://30515 (69.31), *maa://34787 (72.86), ***maa://20792 (11.93), maa://39402 (88.64), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.05), *maa://30515 (69.31), *maa://34787 (72.86), ***maa://20792 (11.93), maa://39402 (88.89), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.67), *maa://20791 (63.38)</t>
+          <t>maa://22742 (91.08), *maa://20791 (63.38)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.32), maa://36684 (95.74), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.32), maa://36684 (95.79), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.22), maa://26254 (96.0)</t>
+          <t>maa://21249 (94.22), maa://26254 (96.15)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (88.99), **maa://20790 (44.78), ***maa://37170 (19.3)</t>
+          <t>maa://24617 (88.99), **maa://20790 (44.78), ***maa://37170 (18.97)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.38), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.42), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (98.04), maa://27295 (83.87), maa://22754 (91.67), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (98.04), maa://27295 (83.87), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.05)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="T6" s="2" t="inlineStr">
         <is>
-          <t>maa://37411 (84.62)</t>
+          <t>maa://37411 (85.71)</t>
         </is>
       </c>
       <c r="U6" s="1" t="n"/>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="AF6" s="2" t="inlineStr">
         <is>
-          <t>*maa://33152 (60.47), ***maa://22770 (27.27)</t>
+          <t>*maa://33152 (61.36), ***maa://22770 (27.27)</t>
         </is>
       </c>
       <c r="AG6" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.17), *maa://22758 (73.33)</t>
+          <t>maa://22399 (95.17), *maa://22758 (73.77)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (68.35), *maa://36671 (69.39), *maa://42530 (64.29)</t>
+          <t>*maa://26191 (68.75), *maa://36671 (69.39), *maa://42530 (64.29)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.01.01 13:19:57</t>
+          <t>更新日期：2025.01.03 13:17:45</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.93)</t>
+          <t>maa://21411 (95.94)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.48)</t>
+          <t>maa://26223 (97.5)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.38), ***maa://22740 (5.77), **maa://39938 (48.0), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (93.33)</t>
+          <t>maa://28711 (87.38), ***maa://22740 (5.77), **maa://39938 (46.15), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (94.12)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.44), **maa://32237 (40.48), ***maa://34206 (21.74), ***maa://39951 (16.67), ***maa://39243 (28.57)</t>
+          <t>***maa://25695 (19.34), **maa://32237 (40.48), ***maa://34206 (21.74), ***maa://39951 (16.28), ***maa://39243 (28.57)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.41)</t>
+          <t>maa://36707 (99.42)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (74.55), **maa://22728 (47.73)</t>
+          <t>*maa://21248 (74.89), **maa://22728 (47.73)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (91.96), *maa://22583 (75.0), *maa://22500 (57.78)</t>
+          <t>maa://22676 (91.96), *maa://22583 (75.38), *maa://22500 (57.78)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.53), maa://21288 (96.3), maa://39841 (95.18), maa://36682 (97.37)</t>
+          <t>maa://26245 (96.55), maa://21288 (96.3), maa://39841 (95.18), maa://36682 (97.37)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2354,12 +2354,12 @@
       </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.44), maa://22734 (84.03), *maa://30808 (65.08), **maa://36048 (32.61)</t>
+          <t>*maa://22743 (77.44), maa://22734 (84.03), *maa://30808 (65.08), **maa://36048 (32.61), maa://45058 (100.0)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (90.32), *maa://22727 (70.0)</t>
+          <t>maa://24762 (90.38), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.91), *maa://22766 (70.91), *maa://36666 (78.82)</t>
+          <t>maa://21364 (80.97), *maa://22766 (70.27), *maa://36666 (78.82)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.35), maa://36679 (93.02), maa://37650 (96.97)</t>
+          <t>maa://21441 (96.35), maa://36679 (93.18), maa://37650 (96.97)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.4)</t>
+          <t>maa://26228 (95.45)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (65.69), maa://27755 (92.68)</t>
+          <t>*maa://23911 (65.69), maa://27755 (92.77)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>maa://21624 (82.86)</t>
+          <t>maa://21624 (83.33)</t>
         </is>
       </c>
       <c r="E17" s="1" t="n"/>
@@ -2651,7 +2651,7 @@
       </c>
       <c r="L17" s="2" t="inlineStr">
         <is>
-          <t>*maa://21679 (76.0)</t>
+          <t>*maa://21679 (76.92)</t>
         </is>
       </c>
       <c r="M17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.1)</t>
+          <t>maa://24570 (97.13)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2991,7 +2991,7 @@
       </c>
       <c r="AF19" s="2" t="inlineStr">
         <is>
-          <t>*maa://21663 (61.19)</t>
+          <t>*maa://21663 (61.76)</t>
         </is>
       </c>
       <c r="AG19" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (89.33)</t>
+          <t>maa://22864 (89.4)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.15)</t>
+          <t>maa://41331 (85.29)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (94.32), maa://39875 (93.75)</t>
+          <t>maa://39756 (94.34), maa://39875 (93.85)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (92.02), *maa://29748 (75.78), ***maa://29785 (16.42), *maa://37566 (71.43)</t>
+          <t>maa://30587 (92.02), *maa://29748 (75.78), ***maa://29785 (16.42), *maa://37566 (68.97)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.71), maa://36672 (80.77), maa://29910 (92.59), **maa://21440 (34.55)</t>
+          <t>maa://22523 (85.71), maa://36672 (80.77), maa://29910 (92.73), **maa://21440 (34.55)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (94.88)</t>
+          <t>maa://29753 (94.9)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3670,12 +3670,12 @@
       </c>
       <c r="G25" s="1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (73.65), *maa://25311 (73.27), ***maa://22725 (4.84)</t>
+          <t>*maa://29063 (73.83), *maa://25311 (73.53), ***maa://22725 (4.84), maa://45047 (100.0)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3707,7 +3707,7 @@
       </c>
       <c r="P25" s="2" t="inlineStr">
         <is>
-          <t>maa://24382 (93.1)</t>
+          <t>maa://24382 (93.33)</t>
         </is>
       </c>
       <c r="Q25" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (93.24)</t>
+          <t>maa://42235 (93.33)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (48.0), maa://34494 (96.55), *maa://39601 (76.47), **maa://36665 (44.44)</t>
+          <t>**maa://21283 (48.0), maa://34494 (96.67), *maa://39601 (76.47), **maa://36665 (44.44)</t>
         </is>
       </c>
       <c r="I27" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.77), maa://25725 (83.53)</t>
+          <t>maa://24465 (90.78), maa://25725 (83.53)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>maa://23263 (94.95), *maa://29765 (60.53)</t>
+          <t>maa://23263 (95.0), *maa://29765 (60.53)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.72), ***maa://39723 (14.29), maa://41749 (91.53)</t>
+          <t>maa://39929 (89.75), ***maa://39723 (14.29), maa://41749 (91.53)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.05), ***maa://34960 (8.33), *maa://42865 (77.14)</t>
+          <t>*maa://24080 (69.05), ***maa://34960 (8.33), *maa://42865 (78.95)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4389,7 +4389,7 @@
       </c>
       <c r="X30" s="2" t="inlineStr">
         <is>
-          <t>maa://39477 (85.71)</t>
+          <t>maa://39477 (86.67)</t>
         </is>
       </c>
       <c r="Y30" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.43), maa://45045 (100.0)</t>
+          <t>maa://42979 (96.46), maa://45045 (100.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.66), maa://36258 (83.67), *maa://43904 (77.78)</t>
+          <t>maa://35926 (93.7), maa://36258 (83.67), *maa://43904 (80.0)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.3), maa://36667 (98.39), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.33), maa://36667 (98.41), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4747,7 +4747,7 @@
       </c>
       <c r="P33" s="2" t="inlineStr">
         <is>
-          <t>*maa://21956 (79.56), *maa://22730 (79.31)</t>
+          <t>*maa://21956 (79.71), *maa://22730 (79.31)</t>
         </is>
       </c>
       <c r="Q33" s="1" t="n"/>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (93.57)</t>
+          <t>maa://24526 (93.6)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.69)</t>
+          <t>maa://41296 (96.72)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.26)</t>
+          <t>maa://36697 (86.34)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (84.82), maa://36670 (87.64), maa://30434 (89.39), ***maa://25036 (16.0), *maa://44165 (66.67), maa://45059 (100.0)</t>
+          <t>maa://25199 (84.82), maa://36670 (87.78), maa://30434 (89.39), ***maa://25036 (16.0), *maa://44165 (66.67), maa://45059 (100.0)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.41)</t>
+          <t>maa://24709 (91.47)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5458,7 +5458,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.99), maa://21386 (95.74), maa://36664 (90.74)</t>
+          <t>maa://23278 (96.0), maa://21386 (95.74), maa://36664 (90.74)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5543,7 +5543,7 @@
       </c>
       <c r="P41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (38.24), maa://43177 (85.71)</t>
+          <t>**maa://35616 (38.24), maa://43177 (86.67)</t>
         </is>
       </c>
       <c r="Q41" s="1" t="n"/>
@@ -5665,7 +5665,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (92.65), maa://21284 (83.72)</t>
+          <t>maa://22525 (92.7), maa://21284 (83.72)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5734,7 +5734,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.84), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.85), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5787,7 +5787,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.86), maa://30807 (95.45), *maa://22767 (55.0), ***maa://20796 (13.79), *maa://42459 (77.78)</t>
+          <t>maa://21229 (84.86), maa://30807 (95.52), *maa://22767 (55.0), ***maa://20796 (13.79), *maa://42459 (77.78)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -6170,7 +6170,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.56), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.58), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6206,7 +6206,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (91.92)</t>
+          <t>maa://32532 (91.95)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (83.02), maa://31270 (94.83)</t>
+          <t>maa://27746 (83.02), maa://31270 (94.87)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6332,7 +6332,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (96.55), maa://43903 (100.0)</t>
+          <t>maa://42981 (96.67), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#135)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.29), maa://25390 (95.95), maa://36681 (87.01)</t>
+          <t>maa://24702 (94.29), maa://25390 (95.98), maa://36681 (87.01)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.05), *maa://30515 (69.31), *maa://34787 (72.86), ***maa://20792 (11.93), maa://39402 (88.89), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.05), *maa://30515 (69.31), *maa://34787 (72.86), ***maa://20792 (11.93), maa://39402 (89.13), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.52), maa://27484 (96.15), maa://27480 (82.86)</t>
+          <t>maa://27396 (84.57), maa://27484 (96.15), maa://27480 (82.86)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.91), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (90.32)</t>
+          <t>**maa://32495 (47.91), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (90.62)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (83.49), maa://22744 (84.0)</t>
+          <t>maa://21245 (83.56), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="AF6" s="2" t="inlineStr">
         <is>
-          <t>*maa://33152 (61.36), ***maa://22770 (27.27)</t>
+          <t>*maa://33152 (60.0), ***maa://22770 (26.09)</t>
         </is>
       </c>
       <c r="AG6" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (93.18), maa://24957 (97.62)</t>
+          <t>maa://28624 (93.55), maa://24957 (97.62)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.17), *maa://22758 (73.77)</t>
+          <t>maa://22399 (95.17), *maa://22758 (74.19)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.01.03 13:17:45</t>
+          <t>更新日期：2025.01.04 13:16:59</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>*maa://21476 (72.92), **maa://39431 (45.45), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (72.92), **maa://39431 (50.0), *maa://37551 (57.14)</t>
         </is>
       </c>
       <c r="E8" s="1" t="n"/>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="AF8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24479 (77.78), *maa://21990 (53.85)</t>
+          <t>*maa://24479 (76.83), *maa://21990 (51.85)</t>
         </is>
       </c>
       <c r="AG8" s="1" t="n"/>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>maa://22762 (91.86), maa://39552 (90.0)</t>
+          <t>maa://22762 (91.95), maa://39552 (90.0)</t>
         </is>
       </c>
       <c r="M9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (89.32), *maa://22865 (51.92)</t>
+          <t>maa://26206 (89.42), *maa://22865 (51.92)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.09), maa://22755 (87.61), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.11), maa://22755 (87.61), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1946,12 +1946,12 @@
       </c>
       <c r="AE11" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF11" s="2" t="inlineStr">
         <is>
-          <t>maa://31203 (95.65), ***maa://24394 (19.23)</t>
+          <t>maa://31203 (95.65)</t>
         </is>
       </c>
       <c r="AG11" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.46), *maa://21485 (76.87), maa://37962 (89.66)</t>
+          <t>maa://22753 (91.46), *maa://21485 (77.04), maa://37962 (89.66)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.79), maa://36673 (92.65), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.8), maa://36673 (92.65), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>*maa://34957 (79.69), *maa://22768 (51.61)</t>
+          <t>*maa://34957 (80.0), *maa://22768 (51.61)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.55), maa://21288 (96.3), maa://39841 (95.18), maa://36682 (97.37)</t>
+          <t>maa://26245 (96.55), maa://21288 (96.3), maa://39841 (95.29), maa://36682 (97.37)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.44), maa://22734 (84.03), *maa://30808 (65.08), **maa://36048 (32.61), maa://45058 (100.0)</t>
+          <t>*maa://22743 (77.44), maa://22734 (84.03), *maa://30808 (65.08), **maa://36048 (34.04), maa://45058 (100.0)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.77), *maa://28648 (68.85), maa://36674 (82.93)</t>
+          <t>maa://22729 (94.77), *maa://28648 (68.85), maa://36674 (83.33)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.13)</t>
+          <t>maa://24570 (97.14)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (63.59), *maa://36668 (55.84)</t>
+          <t>*maa://30709 (63.59), *maa://36668 (56.41)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (89.86), maa://25198 (93.14), *maa://20795 (51.18), maa://36680 (93.55)</t>
+          <t>maa://21432 (89.93), maa://25198 (93.14), *maa://20795 (51.18), maa://36680 (93.55)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.29)</t>
+          <t>maa://41331 (84.62)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (80.17), ***maa://23820 (29.82)</t>
+          <t>maa://21443 (80.23), ***maa://23820 (29.82)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.63), *maa://22432 (76.67)</t>
+          <t>maa://22524 (94.63), *maa://22432 (77.05)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (85.44), *maa://22751 (73.85)</t>
+          <t>maa://27127 (85.58), *maa://22751 (73.85)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (94.34), maa://39875 (93.85)</t>
+          <t>maa://39756 (94.36), maa://39875 (93.85)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.89)</t>
+          <t>*maa://24368 (78.3)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.84), maa://23504 (93.15), **maa://22892 (39.31), *maa://25141 (76.38), *maa://36663 (78.26), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.46), maa://23504 (93.18), **maa://22892 (39.31), *maa://25141 (76.38), *maa://36663 (78.26), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (73.83), *maa://25311 (73.53), ***maa://22725 (4.84), maa://45047 (100.0)</t>
+          <t>*maa://29063 (74.0), *maa://25311 (73.53), ***maa://22725 (4.84), maa://45047 (100.0)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (85.86), *maa://24516 (79.78), maa://26001 (87.5)</t>
+          <t>maa://31215 (86.0), *maa://24516 (79.78), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (93.33)</t>
+          <t>maa://42235 (93.51)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.75), ***maa://39723 (14.29), maa://41749 (91.53)</t>
+          <t>maa://39929 (89.85), ***maa://39723 (14.29), maa://41749 (91.67)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (93.02), *maa://36701 (64.29)</t>
+          <t>maa://36660 (93.04), *maa://36701 (64.29)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>*maa://25175 (70.21)</t>
+          <t>*maa://25175 (68.75)</t>
         </is>
       </c>
       <c r="I29" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (92.93), *maa://28440 (76.84), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (92.95), *maa://28440 (76.84), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.05), ***maa://34960 (8.33), *maa://42865 (78.95)</t>
+          <t>*maa://24080 (69.05), *maa://42865 (78.95), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.46), maa://45045 (100.0)</t>
+          <t>maa://42979 (96.52), maa://45045 (100.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.7), maa://36258 (83.67), *maa://43904 (80.0)</t>
+          <t>maa://35926 (93.73), maa://36258 (83.67), *maa://43904 (80.0)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.33), maa://36667 (98.41), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.37), maa://36667 (98.41), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.34), maa://41108 (87.76), maa://41238 (96.3)</t>
+          <t>maa://42859 (96.47), maa://41108 (87.76), maa://41238 (96.3)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.72)</t>
+          <t>maa://41296 (96.75)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.34)</t>
+          <t>maa://36697 (86.41)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (84.82), maa://36670 (87.78), maa://30434 (89.39), ***maa://25036 (16.0), *maa://44165 (66.67), maa://45059 (100.0)</t>
+          <t>maa://25199 (84.82), maa://36670 (87.78), maa://30434 (89.39), ***maa://25036 (16.0), *maa://44165 (66.67), *maa://45059 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5819,7 +5819,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (38.1)</t>
+          <t>**maa://39364 (36.36)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -5840,7 +5840,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.61), maa://43901 (88.89)</t>
+          <t>maa://35931 (92.63), maa://43901 (88.89)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6170,7 +6170,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.58), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.6), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6206,7 +6206,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (91.95)</t>
+          <t>maa://32532 (91.98)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (83.02), maa://31270 (94.87)</t>
+          <t>maa://27746 (83.18), maa://31270 (94.92)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6332,7 +6332,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (96.67), maa://43903 (100.0)</t>
+          <t>maa://42981 (96.77), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#136)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (91.84), ***maa://21730 (22.86), ***maa://39501 (18.18), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.0), ***maa://21730 (22.86), ***maa://39501 (18.18), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.45), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.46), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.57), maa://27484 (96.15), maa://27480 (82.86)</t>
+          <t>maa://27396 (84.62), maa://27484 (96.15), maa://27480 (82.86)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (94.59)</t>
+          <t>maa://42407 (94.74)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (93.55), maa://24957 (97.62)</t>
+          <t>maa://28624 (93.55), maa://24957 (97.67)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1421,12 +1421,12 @@
       </c>
       <c r="AE7" s="1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (68.75), *maa://36671 (69.39), *maa://42530 (64.29)</t>
+          <t>*maa://26191 (67.9), *maa://36671 (68.0), *maa://42530 (60.0), maa://45272 (100.0)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.01.04 13:16:59</t>
+          <t>更新日期：2025.01.05 13:20:09</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>*maa://21476 (72.92), **maa://39431 (50.0), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (73.47), **maa://39431 (50.0), *maa://37551 (57.14)</t>
         </is>
       </c>
       <c r="E8" s="1" t="n"/>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (84.62), *maa://21916 (61.29), maa://23252 (92.42), maa://37496 (96.43), **maa://22759 (45.45)</t>
+          <t>maa://32931 (83.96), *maa://21916 (61.29), maa://23252 (92.42), maa://37496 (96.43), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.94)</t>
+          <t>maa://21411 (95.95)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (89.42), *maa://22865 (51.92)</t>
+          <t>maa://26206 (89.52), *maa://22865 (51.92)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1704,12 +1704,12 @@
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.34), **maa://32237 (40.48), ***maa://34206 (21.74), ***maa://39951 (16.28), ***maa://39243 (28.57)</t>
+          <t>***maa://25695 (19.34), **maa://32237 (40.48), ***maa://34206 (21.74), ***maa://39951 (16.28), ***maa://39243 (28.57), maa://45271 (100.0)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1741,7 +1741,7 @@
       </c>
       <c r="L10" s="2" t="inlineStr">
         <is>
-          <t>**maa://24395 (40.74)</t>
+          <t>**maa://24395 (39.29)</t>
         </is>
       </c>
       <c r="M10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.64), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.66), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.81), maa://22501 (98.59)</t>
+          <t>maa://22747 (92.81), maa://22501 (98.61)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.46), *maa://21485 (77.04), maa://37962 (89.66)</t>
+          <t>maa://22753 (91.46), *maa://21485 (77.04), maa://37962 (86.67)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.79), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (78.2), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.8), maa://36673 (92.65), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.82), maa://36673 (92.65), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (91.96), *maa://22583 (75.38), *maa://22500 (57.78)</t>
+          <t>maa://22676 (91.96), *maa://22583 (74.24), *maa://22500 (57.78)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (32.37), maa://39883 (90.74), *maa://39885 (56.0)</t>
+          <t>**maa://22737 (32.37), maa://39883 (90.91), *maa://39885 (56.0)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.97), *maa://22766 (70.27), *maa://36666 (78.82)</t>
+          <t>maa://21364 (81.03), *maa://22766 (70.27), *maa://36666 (79.07)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (63.59), *maa://36668 (56.41)</t>
+          <t>*maa://30709 (63.68), *maa://36668 (56.41)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (84.62)</t>
+          <t>maa://41331 (84.91)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (80.23), ***maa://23820 (29.82)</t>
+          <t>*maa://21443 (80.0), ***maa://23820 (29.82)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.63), *maa://22432 (77.05)</t>
+          <t>maa://22524 (94.63), *maa://22432 (77.42)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.47), *maa://37649 (66.67)</t>
+          <t>maa://21282 (98.48), *maa://37649 (66.67)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (94.36), maa://39875 (93.85)</t>
+          <t>maa://39756 (94.38), maa://39875 (93.85)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (92.02), *maa://29748 (75.78), ***maa://29785 (16.42), *maa://37566 (68.97)</t>
+          <t>maa://30587 (92.06), *maa://29748 (75.78), ***maa://29785 (16.42), *maa://37566 (70.0)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.46), maa://23504 (93.18), **maa://22892 (39.31), *maa://25141 (76.38), *maa://36663 (78.26), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.46), maa://23504 (93.18), **maa://22892 (39.31), *maa://25141 (76.56), *maa://36663 (78.26), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.71), maa://36672 (80.77), maa://29910 (92.73), **maa://21440 (34.55)</t>
+          <t>maa://22523 (85.71), maa://36672 (80.77), maa://29910 (92.86), **maa://21440 (34.55)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (94.9)</t>
+          <t>maa://29753 (94.92)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (93.51)</t>
+          <t>maa://42235 (93.59)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (76.47)</t>
+          <t>*maa://30624 (77.36)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>maa://23263 (95.0), *maa://29765 (60.53)</t>
+          <t>maa://23263 (95.0), *maa://29765 (61.54)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.85), ***maa://39723 (14.29), maa://41749 (91.67)</t>
+          <t>maa://39929 (89.88), ***maa://39723 (14.29), maa://41749 (91.67)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4227,7 +4227,7 @@
       </c>
       <c r="P29" s="2" t="inlineStr">
         <is>
-          <t>*maa://23168 (55.56), *maa://30050 (51.72)</t>
+          <t>*maa://23168 (55.56), *maa://30050 (53.33)</t>
         </is>
       </c>
       <c r="Q29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.05), *maa://42865 (78.95), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.87), *maa://42865 (78.95), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.52), maa://45045 (100.0)</t>
+          <t>maa://42979 (96.61), maa://45045 (100.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.73), maa://36258 (83.67), *maa://43904 (80.0)</t>
+          <t>maa://35926 (93.38), maa://36258 (83.84), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.47), maa://41108 (87.76), maa://41238 (96.3)</t>
+          <t>maa://42859 (96.63), maa://41108 (87.76), maa://41238 (96.3)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4747,7 +4747,7 @@
       </c>
       <c r="P33" s="2" t="inlineStr">
         <is>
-          <t>*maa://21956 (79.71), *maa://22730 (79.31)</t>
+          <t>*maa://21956 (79.86), *maa://22730 (79.31)</t>
         </is>
       </c>
       <c r="Q33" s="1" t="n"/>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (93.6)</t>
+          <t>maa://24526 (93.63)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -5187,7 +5187,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.11), *maa://21239 (66.67)</t>
+          <t>maa://21280 (89.22), *maa://21239 (66.67)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.41)</t>
+          <t>maa://36697 (86.49)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (84.82), maa://36670 (87.78), maa://30434 (89.39), ***maa://25036 (16.0), *maa://44165 (66.67), *maa://45059 (66.67)</t>
+          <t>maa://25199 (84.82), maa://36670 (87.91), maa://30434 (89.39), ***maa://25036 (16.0), *maa://44165 (66.67), *maa://45059 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5734,7 +5734,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.85), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.86), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5840,7 +5840,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.63), maa://43901 (88.89)</t>
+          <t>maa://35931 (92.68), maa://43901 (90.0)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.2), maa://29661 (97.86), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.21), maa://29661 (97.86), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (83.18), maa://31270 (94.92)</t>
+          <t>maa://27746 (83.18), maa://31270 (94.96)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6332,7 +6332,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (96.77), maa://43903 (100.0)</t>
+          <t>maa://42981 (96.88), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#137)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.32), maa://36684 (95.79), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.32), maa://36684 (94.79), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (83.56), maa://22744 (84.0)</t>
+          <t>maa://21245 (83.64), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.01.05 13:20:09</t>
+          <t>更新日期：2025.01.06 13:18:43</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1821,7 +1821,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (54.22), *maa://22733 (59.38), maa://22761 (100.0)</t>
+          <t>*maa://25021 (54.76), *maa://22733 (59.38), maa://22761 (100.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (98.17)</t>
+          <t>maa://36713 (97.95)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>*maa://34957 (80.0), *maa://22768 (51.61)</t>
+          <t>maa://34957 (80.3), *maa://22768 (51.61)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (89.4)</t>
+          <t>maa://22864 (89.47)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (84.91)</t>
+          <t>maa://41331 (85.19)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>*maa://21443 (80.0), ***maa://23820 (29.82)</t>
+          <t>*maa://21443 (80.0), ***maa://23820 (29.31)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (85.58), *maa://22751 (73.85)</t>
+          <t>maa://27127 (84.76), *maa://22751 (73.85)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (94.38), maa://39875 (93.85)</t>
+          <t>maa://39756 (94.42), maa://39875 (93.85)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (93.59)</t>
+          <t>maa://42235 (93.67)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.78), maa://25725 (83.53)</t>
+          <t>maa://24465 (90.81), maa://25725 (83.53)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.88), ***maa://39723 (14.29), maa://41749 (91.67)</t>
+          <t>maa://39929 (89.88), maa://41749 (91.8), ***maa://39723 (14.29)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (92.95), *maa://28440 (76.84), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (92.95), *maa://28440 (77.08), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.61), maa://45045 (100.0)</t>
+          <t>maa://42979 (96.64), maa://45045 (100.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.75)</t>
+          <t>maa://41296 (96.8)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.21), maa://29661 (97.86), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.22), maa://29661 (97.86), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6170,7 +6170,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.6), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.62), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#138)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.32), maa://36684 (94.79), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.35), maa://36684 (94.79), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (93.55)</t>
+          <t>maa://24390 (93.65)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.01.06 13:18:43</t>
+          <t>更新日期：2025.01.07 13:17:31</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (83.96), *maa://21916 (61.29), maa://23252 (92.42), maa://37496 (96.43), **maa://22759 (45.45)</t>
+          <t>maa://32931 (83.96), *maa://21916 (61.29), maa://23252 (92.42), maa://37496 (96.55), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>maa://22765 (92.05), *maa://21915 (68.0)</t>
+          <t>maa://22765 (92.13), *maa://21915 (68.0)</t>
         </is>
       </c>
       <c r="E9" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.5)</t>
+          <t>maa://26223 (97.52)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.46), *maa://21485 (77.04), maa://37962 (86.67)</t>
+          <t>maa://22753 (91.46), *maa://21485 (77.21), maa://37962 (86.67)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.82), maa://36673 (92.65), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.82), maa://36673 (92.75), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (74.89), **maa://22728 (47.73)</t>
+          <t>*maa://21248 (75.11), **maa://22728 (47.73)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="T14" s="2" t="inlineStr">
         <is>
-          <t>maa://22521 (93.81), maa://42751 (100.0)</t>
+          <t>maa://22521 (93.88), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.77), *maa://28648 (68.85), maa://36674 (83.33)</t>
+          <t>maa://22729 (94.77), *maa://28648 (69.35), maa://36674 (83.33)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.45)</t>
+          <t>maa://26228 (95.51)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (77.36)</t>
+          <t>*maa://30624 (77.78)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.88), maa://41749 (91.8), ***maa://39723 (14.29)</t>
+          <t>maa://39929 (89.88), maa://41749 (91.94), ***maa://39723 (14.29)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.63), maa://41108 (87.76), maa://41238 (96.3)</t>
+          <t>maa://42859 (96.63), maa://41108 (87.76), maa://41238 (96.39)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (84.82), maa://36670 (87.91), maa://30434 (89.39), ***maa://25036 (16.0), *maa://44165 (66.67), *maa://45059 (66.67)</t>
+          <t>maa://25199 (84.82), maa://36670 (87.91), maa://30434 (89.55), ***maa://25036 (16.0), *maa://44165 (66.67), *maa://45059 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5840,7 +5840,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.68), maa://43901 (90.0)</t>
+          <t>maa://35931 (92.71), maa://43901 (90.0)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.22), maa://29661 (97.86), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.23), maa://29661 (97.86), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6170,7 +6170,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.62), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.65), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (83.18), maa://31270 (94.96)</t>
+          <t>maa://27746 (83.18), maa://31270 (95.0)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#139)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.29), maa://25390 (95.98), maa://36681 (87.01)</t>
+          <t>maa://24702 (94.31), maa://25390 (95.98), maa://36681 (87.01)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.05), *maa://30515 (69.31), *maa://34787 (72.86), ***maa://20792 (11.93), maa://39402 (89.13), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.05), *maa://30515 (69.31), *maa://34787 (73.61), ***maa://20792 (11.93), maa://39402 (89.36), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.08), *maa://20791 (63.38)</t>
+          <t>maa://22742 (91.08), *maa://20791 (63.89)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.35), maa://36684 (94.79), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.38), maa://36684 (94.79), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.0), ***maa://21730 (22.86), ***maa://39501 (18.18), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.08), ***maa://21730 (22.86), ***maa://39501 (18.18), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.46), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.47), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.95), maa://20276 (85.09), *maa://22749 (72.73)</t>
+          <t>*maa://22880 (66.13), maa://20276 (85.19), *maa://22749 (72.73)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.22), maa://26254 (96.15)</t>
+          <t>maa://21249 (94.22), maa://26254 (96.3)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (88.99), **maa://20790 (44.78), ***maa://37170 (18.97)</t>
+          <t>maa://24617 (89.09), **maa://20790 (44.12), ***maa://37170 (18.97)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (98.04), maa://27295 (83.87), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.05)</t>
+          <t>maa://32509 (98.04), maa://27295 (84.13), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.91), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (90.62)</t>
+          <t>**maa://32495 (47.91), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (90.91)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.01.07 13:17:31</t>
+          <t>更新日期：2025.01.09 13:18:22</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.95)</t>
+          <t>maa://21411 (95.97)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (54.76), *maa://22733 (59.38), maa://22761 (100.0)</t>
+          <t>*maa://25021 (55.29), *maa://22733 (59.38), maa://22761 (100.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.95)</t>
+          <t>maa://36713 (97.96)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.82), maa://36673 (92.75), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.83), maa://36673 (92.75), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>maa://34957 (80.3), *maa://22768 (51.61)</t>
+          <t>maa://34957 (80.88), *maa://22768 (51.61)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (32.37), maa://39883 (90.91), *maa://39885 (56.0)</t>
+          <t>**maa://22737 (32.37), maa://39883 (91.23), *maa://39885 (56.0)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.55), maa://21288 (96.3), maa://39841 (95.29), maa://36682 (97.37)</t>
+          <t>maa://26245 (96.55), maa://21288 (96.3), maa://39841 (95.35), maa://36682 (97.37)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.62), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.63), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.44), maa://22734 (84.03), *maa://30808 (65.08), **maa://36048 (34.04), maa://45058 (100.0)</t>
+          <t>*maa://22743 (77.55), maa://22734 (84.03), *maa://30808 (65.08), **maa://36048 (34.04), maa://45058 (100.0)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.18), maa://21478 (91.43)</t>
+          <t>maa://24304 (88.24), maa://21478 (91.43)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.03), *maa://22766 (70.27), *maa://36666 (79.07)</t>
+          <t>maa://21364 (81.09), *maa://22766 (70.27), *maa://36666 (78.16)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.77), *maa://28648 (69.35), maa://36674 (83.33)</t>
+          <t>maa://22729 (94.77), *maa://28648 (68.25), maa://36674 (83.33)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (97.83), maa://28051 (96.0)</t>
+          <t>maa://28501 (97.85), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.71), maa://39599 (86.84)</t>
+          <t>maa://22430 (88.77), maa://39599 (86.84)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.14)</t>
+          <t>maa://24570 (97.16)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (90.12)</t>
+          <t>maa://24421 (90.16)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (99.05)</t>
+          <t>maa://24386 (99.06)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (89.93), maa://25198 (93.14), *maa://20795 (51.18), maa://36680 (93.55)</t>
+          <t>maa://21432 (90.07), maa://25198 (93.14), *maa://20795 (51.18), maa://36680 (93.55)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>*maa://21443 (80.0), ***maa://23820 (29.31)</t>
+          <t>maa://21443 (80.06), ***maa://23820 (29.31)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>maa://25236 (96.34), **maa://21678 (48.94), **maa://22735 (42.86)</t>
+          <t>maa://25236 (96.39), **maa://21678 (48.94), **maa://22735 (42.86)</t>
         </is>
       </c>
       <c r="I22" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (84.76), *maa://22751 (73.85)</t>
+          <t>maa://27127 (84.91), *maa://22751 (73.85)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (94.42), maa://39875 (93.85)</t>
+          <t>maa://39756 (94.53), maa://39875 (93.85)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.46), maa://23504 (93.18), **maa://22892 (39.31), *maa://25141 (76.56), *maa://36663 (78.26), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.46), maa://23504 (93.18), **maa://22892 (39.31), *maa://25141 (76.56), *maa://36663 (78.57), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.27), maa://24621 (96.58), maa://36676 (96.77), maa://22771 (85.71), maa://37772 (100.0)</t>
+          <t>maa://20108 (96.27), maa://24621 (96.58), maa://36676 (96.88), maa://22771 (85.71), **maa://37772 (50.0)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.88), maa://41749 (91.94), ***maa://39723 (14.29)</t>
+          <t>maa://39929 (89.97), maa://41749 (91.94), ***maa://39723 (14.29)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.64), maa://45045 (100.0)</t>
+          <t>maa://42979 (96.67), maa://45045 (100.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.38), maa://36258 (83.84), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.38), maa://36258 (84.0), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.37), maa://36667 (98.41), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.38), maa://36667 (98.41), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.63), maa://41108 (87.76), maa://41238 (96.39)</t>
+          <t>maa://42859 (96.63), maa://41108 (87.76), maa://41238 (96.43)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.8)</t>
+          <t>maa://41296 (96.83)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (84.82), maa://36670 (87.91), maa://30434 (89.55), ***maa://25036 (16.0), *maa://44165 (66.67), *maa://45059 (66.67)</t>
+          <t>maa://25199 (84.82), maa://36670 (87.91), maa://30434 (89.55), ***maa://25036 (16.0), *maa://44165 (66.67), *maa://45059 (75.0)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5787,7 +5787,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.86), maa://30807 (95.52), *maa://22767 (55.0), ***maa://20796 (13.79), *maa://42459 (77.78)</t>
+          <t>maa://21229 (84.86), maa://30807 (95.52), *maa://22767 (55.0), ***maa://20796 (13.79), *maa://42459 (80.0)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5819,7 +5819,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (36.36)</t>
+          <t>**maa://39364 (39.13)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -5840,7 +5840,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.71), maa://43901 (90.0)</t>
+          <t>maa://35931 (92.41), maa://43901 (90.0)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.23), maa://29661 (97.86), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.24), maa://29661 (97.86), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6206,7 +6206,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (91.98)</t>
+          <t>maa://32532 (92.02)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6296,7 +6296,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (60.87)</t>
+          <t>*maa://40438 (61.7)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>
@@ -6332,7 +6332,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (96.88), maa://43903 (100.0)</t>
+          <t>maa://42981 (96.97), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#140)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.08), *maa://20791 (63.89)</t>
+          <t>maa://22742 (91.14), *maa://20791 (63.89)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.08), ***maa://21730 (22.86), ***maa://39501 (18.18), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.16), ***maa://21730 (22.86), ***maa://39501 (18.18), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.62), maa://27484 (96.15), maa://27480 (82.86)</t>
+          <t>maa://27396 (84.35), maa://27484 (96.15), maa://27480 (82.86)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (93.65)</t>
+          <t>maa://24390 (93.75)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.91), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (90.91)</t>
+          <t>**maa://32495 (47.91), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (91.18)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>*maa://22757 (78.79)</t>
+          <t>*maa://22757 (79.41)</t>
         </is>
       </c>
       <c r="M5" s="1" t="n"/>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>maa://21955 (94.29)</t>
+          <t>maa://21955 (94.44)</t>
         </is>
       </c>
       <c r="E7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.01.09 13:18:22</t>
+          <t>更新日期：2025.01.11 13:17:38</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>*maa://21476 (73.47), **maa://39431 (50.0), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (74.0), **maa://39431 (50.0), *maa://37551 (57.14)</t>
         </is>
       </c>
       <c r="E8" s="1" t="n"/>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="AB8" s="2" t="inlineStr">
         <is>
-          <t>maa://25389 (87.1)</t>
+          <t>maa://25389 (87.5)</t>
         </is>
       </c>
       <c r="AC8" s="1" t="n"/>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="AF8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24479 (76.83), *maa://21990 (51.85)</t>
+          <t>*maa://24479 (77.11), *maa://21990 (51.85)</t>
         </is>
       </c>
       <c r="AG8" s="1" t="n"/>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>maa://22765 (92.13), *maa://21915 (68.0)</t>
+          <t>maa://22765 (92.22), *maa://21915 (68.0)</t>
         </is>
       </c>
       <c r="E9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (89.52), *maa://22865 (51.92)</t>
+          <t>maa://26206 (89.62), *maa://22865 (51.92)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.34), **maa://32237 (40.48), ***maa://34206 (21.74), ***maa://39951 (16.28), ***maa://39243 (28.57), maa://45271 (100.0)</t>
+          <t>***maa://25695 (19.34), **maa://32237 (41.86), ***maa://34206 (20.83), ***maa://39951 (16.28), ***maa://39243 (28.57), *maa://45271 (60.0)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.42)</t>
+          <t>maa://36707 (99.43)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.81), maa://22501 (98.61)</t>
+          <t>maa://22747 (92.86), maa://22501 (97.3)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.96)</t>
+          <t>maa://36713 (97.97)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.46), *maa://21485 (77.21), maa://37962 (86.67)</t>
+          <t>maa://22753 (90.91), *maa://21485 (77.21), maa://37962 (86.67)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (91.96), *maa://22583 (74.24), *maa://22500 (57.78)</t>
+          <t>maa://22676 (92.04), *maa://22583 (74.24), *maa://22500 (57.78)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.55), maa://21288 (96.3), maa://39841 (95.35), maa://36682 (97.37)</t>
+          <t>maa://26245 (96.55), maa://21288 (96.3), maa://39841 (95.4), maa://36682 (97.37)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="AB14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (96.88)</t>
+          <t>maa://22764 (96.92)</t>
         </is>
       </c>
       <c r="AC14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.55), maa://22734 (84.03), *maa://30808 (65.08), **maa://36048 (34.04), maa://45058 (100.0)</t>
+          <t>*maa://22743 (77.55), maa://22734 (84.03), *maa://30808 (65.08), **maa://36048 (35.42), maa://45058 (100.0)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.77), maa://39599 (86.84)</t>
+          <t>maa://22430 (88.83), maa://39599 (86.84)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.16)</t>
+          <t>maa://24570 (97.18)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (90.16)</t>
+          <t>maa://24421 (89.8)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2845,7 +2845,7 @@
       </c>
       <c r="AB18" s="2" t="inlineStr">
         <is>
-          <t>maa://24393 (97.56)</t>
+          <t>maa://24393 (97.62)</t>
         </is>
       </c>
       <c r="AC18" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (99.06)</t>
+          <t>maa://24386 (99.07)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (63.68), *maa://36668 (56.41)</t>
+          <t>*maa://30709 (63.86), *maa://36668 (56.41)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (89.47)</t>
+          <t>maa://22864 (89.54)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.19)</t>
+          <t>maa://41331 (85.32)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (94.53), maa://39875 (93.85)</t>
+          <t>maa://39756 (94.57), maa://39875 (93.85)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="X23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (66.18)</t>
+          <t>*maa://28503 (65.71)</t>
         </is>
       </c>
       <c r="Y23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.46), maa://23504 (93.18), **maa://22892 (39.31), *maa://25141 (76.56), *maa://36663 (78.57), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (86.52), maa://23504 (93.18), **maa://22892 (39.73), *maa://25141 (76.56), *maa://36663 (78.57), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.71), maa://36672 (80.77), maa://29910 (92.86), **maa://21440 (34.55)</t>
+          <t>maa://22523 (85.71), maa://36672 (81.13), maa://29910 (92.86), **maa://21440 (34.55)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (94.92)</t>
+          <t>maa://29753 (94.94)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (86.0), *maa://24516 (79.78), maa://26001 (87.5)</t>
+          <t>maa://31215 (86.14), *maa://24516 (79.78), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (93.67)</t>
+          <t>maa://42235 (93.75)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3951,7 +3951,7 @@
       </c>
       <c r="L27" s="2" t="inlineStr">
         <is>
-          <t>maa://28071 (88.89)</t>
+          <t>maa://28071 (89.47)</t>
         </is>
       </c>
       <c r="M27" s="1" t="n"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (77.78)</t>
+          <t>*maa://30624 (78.18)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.97), maa://41749 (91.94), ***maa://39723 (14.29)</t>
+          <t>maa://39929 (89.97), maa://41749 (92.06), ***maa://39723 (14.29)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (92.95), *maa://28440 (77.08), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (92.97), *maa://28440 (77.08), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.38), maa://36667 (98.41), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.41), maa://36667 (98.41), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.63), maa://41108 (87.76), maa://41238 (96.43)</t>
+          <t>maa://42859 (96.67), maa://41108 (88.0), maa://41238 (96.43)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -5187,7 +5187,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.22), *maa://21239 (66.67)</t>
+          <t>maa://21280 (88.78), *maa://21239 (66.67)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.49)</t>
+          <t>maa://36697 (86.56)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (84.82), maa://36670 (87.91), maa://30434 (89.55), ***maa://25036 (16.0), *maa://44165 (66.67), *maa://45059 (75.0)</t>
+          <t>maa://25199 (84.82), maa://36670 (87.91), maa://30434 (89.86), ***maa://25036 (16.0), *maa://44165 (66.67), *maa://45059 (75.0)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.47)</t>
+          <t>maa://24709 (91.6)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5458,7 +5458,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (96.0), maa://21386 (95.74), maa://36664 (90.74)</t>
+          <t>maa://23278 (95.68), maa://21386 (95.74), maa://36664 (90.74)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5734,7 +5734,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.86), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.87), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5840,7 +5840,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.41), maa://43901 (90.0)</t>
+          <t>maa://35931 (92.41), maa://43901 (90.91)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.24), maa://29661 (97.86), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.25), maa://29661 (97.86), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6015,7 +6015,7 @@
       </c>
       <c r="P49" s="2" t="inlineStr">
         <is>
-          <t>*maa://39643 (66.67)</t>
+          <t>*maa://39643 (68.0)</t>
         </is>
       </c>
       <c r="Q49" s="1" t="n"/>
@@ -6170,7 +6170,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.65), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.67), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6206,7 +6206,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.02)</t>
+          <t>maa://32532 (92.05)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6242,7 +6242,7 @@
       </c>
       <c r="H57" s="2" t="inlineStr">
         <is>
-          <t>maa://25176 (98.25)</t>
+          <t>maa://25176 (98.28)</t>
         </is>
       </c>
       <c r="I57" s="1" t="n"/>
@@ -6296,7 +6296,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (61.7)</t>
+          <t>*maa://40438 (63.27)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#141)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.31), maa://25390 (95.98), maa://36681 (87.01)</t>
+          <t>maa://24702 (94.33), maa://25390 (95.98), maa://36681 (87.01)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="P5" s="2" t="inlineStr">
         <is>
-          <t>maa://21919 (96.08), maa://21281 (85.71)</t>
+          <t>maa://21919 (96.15), maa://21281 (85.71)</t>
         </is>
       </c>
       <c r="Q5" s="1" t="n"/>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="P6" s="2" t="inlineStr">
         <is>
-          <t>maa://31836 (91.3), maa://30381 (92.31)</t>
+          <t>maa://31836 (91.67), maa://30381 (92.31)</t>
         </is>
       </c>
       <c r="Q6" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.01.11 13:17:38</t>
+          <t>更新日期：2025.01.12 13:18:28</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24371 (54.29)</t>
+          <t>*maa://24371 (54.93)</t>
         </is>
       </c>
       <c r="I8" s="1" t="n"/>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (83.96), *maa://21916 (61.29), maa://23252 (92.42), maa://37496 (96.55), **maa://22759 (45.45)</t>
+          <t>maa://32931 (84.11), *maa://21916 (61.29), maa://23252 (92.42), maa://37496 (96.55), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="AF8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24479 (77.11), *maa://21990 (51.85)</t>
+          <t>*maa://24479 (77.38), *maa://21990 (51.85)</t>
         </is>
       </c>
       <c r="AG8" s="1" t="n"/>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>maa://22765 (92.22), *maa://21915 (68.0)</t>
+          <t>maa://22765 (92.31), *maa://21915 (68.0)</t>
         </is>
       </c>
       <c r="E9" s="1" t="n"/>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (81.52)</t>
+          <t>maa://22736 (81.72)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1643,7 +1643,7 @@
       </c>
       <c r="T9" s="2" t="inlineStr">
         <is>
-          <t>**maa://22866 (30.19), maa://26222 (97.78)</t>
+          <t>**maa://22866 (30.19), maa://26222 (97.83)</t>
         </is>
       </c>
       <c r="U9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.34), **maa://32237 (41.86), ***maa://34206 (20.83), ***maa://39951 (16.28), ***maa://39243 (28.57), *maa://45271 (60.0)</t>
+          <t>***maa://25695 (19.34), **maa://32237 (41.86), ***maa://34206 (20.83), ***maa://39951 (16.28), ***maa://39243 (28.57), **maa://45271 (50.0)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (91.36), maa://36669 (89.47), *maa://23264 (61.82)</t>
+          <t>maa://28977 (91.36), maa://36669 (89.74), *maa://23264 (61.82)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.66), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.67), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (88.42)</t>
+          <t>maa://21287 (88.54)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.83), maa://36673 (92.75), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.83), maa://36673 (92.86), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (92.04), *maa://22583 (74.24), *maa://22500 (57.78)</t>
+          <t>maa://22676 (92.11), *maa://22583 (74.24), *maa://22500 (57.78)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.55), maa://22734 (84.03), *maa://30808 (65.08), **maa://36048 (35.42), maa://45058 (100.0)</t>
+          <t>*maa://22743 (77.66), maa://22734 (84.03), *maa://30808 (65.08), **maa://36048 (35.42), maa://45058 (100.0)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.09), *maa://22766 (70.27), *maa://36666 (78.16)</t>
+          <t>maa://21364 (81.15), *maa://22766 (70.27), *maa://36666 (78.16)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.35), maa://36679 (93.18), maa://37650 (96.97)</t>
+          <t>maa://21441 (96.35), maa://36679 (93.48), maa://37650 (96.97)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.83), maa://39599 (86.84)</t>
+          <t>maa://22430 (88.83), maa://39599 (87.18)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (57.86), **maa://29784 (44.44)</t>
+          <t>*maa://24313 (58.13), **maa://29784 (44.44)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.07), maa://25198 (93.14), *maa://20795 (51.18), maa://36680 (93.55)</t>
+          <t>maa://21432 (90.07), maa://25198 (93.14), *maa://20795 (51.56), maa://36680 (93.55)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.32)</t>
+          <t>maa://41331 (85.59)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3139,7 +3139,7 @@
       </c>
       <c r="D21" s="2" t="inlineStr">
         <is>
-          <t>maa://21261 (97.37)</t>
+          <t>maa://21261 (97.44)</t>
         </is>
       </c>
       <c r="E21" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (84.91), *maa://22751 (73.85)</t>
+          <t>maa://27127 (84.26), *maa://22751 (73.85)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (27.54), *maa://41753 (53.85)</t>
+          <t>***maa://28036 (28.57), *maa://41753 (53.85)</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (94.57), maa://39875 (93.85)</t>
+          <t>maa://39756 (94.58), maa://39875 (93.85)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.3)</t>
+          <t>*maa://24368 (78.36)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (94.94)</t>
+          <t>maa://29753 (94.96)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (74.0), *maa://25311 (73.53), ***maa://22725 (4.84), maa://45047 (100.0)</t>
+          <t>*maa://29063 (74.17), *maa://25311 (73.53), ***maa://22725 (4.84), maa://45047 (100.0)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (86.14), *maa://24516 (79.78), maa://26001 (87.5)</t>
+          <t>maa://31215 (86.27), *maa://24516 (79.78), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.27), maa://24621 (96.58), maa://36676 (96.88), maa://22771 (85.71), **maa://37772 (50.0)</t>
+          <t>maa://20108 (96.27), maa://24621 (96.61), maa://36676 (96.88), maa://22771 (85.71), **maa://37772 (50.0)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.81), maa://25725 (83.53)</t>
+          <t>maa://24465 (90.81), maa://25725 (83.72)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (93.04), *maa://36701 (64.29)</t>
+          <t>maa://36660 (93.06), *maa://36701 (64.29)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.67), maa://45045 (100.0)</t>
+          <t>maa://42979 (96.69), maa://45045 (100.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.41), maa://36667 (98.41), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.41), maa://36667 (98.44), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.67), maa://41108 (88.0), maa://41238 (96.43)</t>
+          <t>maa://42859 (95.6), maa://41108 (88.0), maa://41238 (96.43)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.83)</t>
+          <t>maa://41296 (96.85)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5039,7 +5039,7 @@
       </c>
       <c r="AF35" s="2" t="inlineStr">
         <is>
-          <t>maa://39479 (93.33)</t>
+          <t>maa://39479 (93.75)</t>
         </is>
       </c>
       <c r="AG35" s="1" t="n"/>
@@ -5187,7 +5187,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (88.78), *maa://21239 (66.67)</t>
+          <t>maa://21280 (88.83), *maa://21239 (66.67)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (84.82), maa://36670 (87.91), maa://30434 (89.86), ***maa://25036 (16.0), *maa://44165 (66.67), *maa://45059 (75.0)</t>
+          <t>maa://25199 (84.82), maa://36670 (87.91), maa://30434 (89.86), ***maa://25036 (16.0), *maa://44165 (66.67), *maa://45059 (80.0)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.6)</t>
+          <t>maa://24709 (91.67)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5458,7 +5458,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.68), maa://21386 (95.74), maa://36664 (90.74)</t>
+          <t>maa://23278 (95.68), maa://21386 (95.74), maa://36664 (90.91)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5787,7 +5787,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.86), maa://30807 (95.52), *maa://22767 (55.0), ***maa://20796 (13.79), *maa://42459 (80.0)</t>
+          <t>maa://21229 (84.86), maa://30807 (95.52), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (81.82)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5840,7 +5840,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.41), maa://43901 (90.91)</t>
+          <t>maa://35931 (92.41), maa://43901 (91.67)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6206,7 +6206,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.05)</t>
+          <t>maa://32532 (92.08)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#142)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.33), maa://25390 (95.98), maa://36681 (87.01)</t>
+          <t>maa://24702 (94.35), maa://25390 (95.98), maa://36681 (87.01)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.05), *maa://30515 (69.31), *maa://34787 (73.61), ***maa://20792 (11.93), maa://39402 (89.36), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.05), *maa://30515 (69.31), *maa://34787 (73.61), ***maa://20792 (11.93), maa://39402 (89.58), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.14), *maa://20791 (63.89)</t>
+          <t>maa://22742 (91.19), *maa://20791 (63.89)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.38), maa://36684 (94.79), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.38), maa://36684 (94.95), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.16), ***maa://21730 (22.86), ***maa://39501 (18.18), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.31), ***maa://21730 (22.86), ***maa://39501 (18.18), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.47), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.48), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (66.13), maa://20276 (85.19), *maa://22749 (72.73)</t>
+          <t>*maa://22880 (66.31), maa://20276 (85.37), *maa://22749 (72.73)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.22), maa://26254 (96.3)</t>
+          <t>maa://21249 (94.25), maa://26254 (96.3)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.09), **maa://20790 (44.12), ***maa://37170 (18.97)</t>
+          <t>maa://24617 (89.29), **maa://20790 (44.12), ***maa://37170 (18.64)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.35), maa://27484 (96.15), maa://27480 (82.86)</t>
+          <t>maa://27396 (84.35), maa://27484 (96.23), maa://27480 (82.86)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.42), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.46), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (98.04), maa://27295 (84.13), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
+          <t>maa://32509 (98.08), maa://27295 (84.62), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.91), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (91.18)</t>
+          <t>**maa://32495 (47.91), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (91.67)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (83.64), maa://22744 (84.0)</t>
+          <t>maa://21245 (83.71), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="P5" s="2" t="inlineStr">
         <is>
-          <t>maa://21919 (96.15), maa://21281 (85.71)</t>
+          <t>maa://21919 (96.23), maa://21281 (85.71)</t>
         </is>
       </c>
       <c r="Q5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (94.74)</t>
+          <t>maa://42407 (94.87)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="P6" s="2" t="inlineStr">
         <is>
-          <t>maa://31836 (91.67), maa://30381 (92.31)</t>
+          <t>maa://31836 (92.0), maa://30381 (92.31)</t>
         </is>
       </c>
       <c r="Q6" s="1" t="n"/>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="T6" s="2" t="inlineStr">
         <is>
-          <t>maa://37411 (85.71)</t>
+          <t>maa://37411 (86.67)</t>
         </is>
       </c>
       <c r="U6" s="1" t="n"/>
@@ -1280,7 +1280,7 @@
       </c>
       <c r="AB6" s="2" t="inlineStr">
         <is>
-          <t>maa://22739 (92.73)</t>
+          <t>maa://22739 (92.86)</t>
         </is>
       </c>
       <c r="AC6" s="1" t="n"/>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="AF6" s="2" t="inlineStr">
         <is>
-          <t>*maa://33152 (60.0), ***maa://22770 (26.09)</t>
+          <t>*maa://33152 (60.87), ***maa://22770 (26.09)</t>
         </is>
       </c>
       <c r="AG6" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (93.55), maa://24957 (97.67)</t>
+          <t>maa://28624 (93.55), maa://24957 (97.73)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="T7" s="2" t="inlineStr">
         <is>
-          <t>maa://21291 (84.09)</t>
+          <t>maa://21291 (84.44)</t>
         </is>
       </c>
       <c r="U7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.17), *maa://22758 (74.19)</t>
+          <t>maa://22399 (95.24), *maa://22758 (74.6)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.01.12 13:18:28</t>
+          <t>更新日期：2025.01.17 13:17:18</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>*maa://21476 (74.0), **maa://39431 (50.0), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (74.51), **maa://39431 (50.0), *maa://37551 (57.14)</t>
         </is>
       </c>
       <c r="E8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.97)</t>
+          <t>maa://21411 (95.99)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="AF8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24479 (77.38), *maa://21990 (51.85)</t>
+          <t>*maa://24479 (77.65), *maa://21990 (51.85)</t>
         </is>
       </c>
       <c r="AG8" s="1" t="n"/>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (81.72)</t>
+          <t>maa://22736 (81.91)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1643,7 +1643,7 @@
       </c>
       <c r="T9" s="2" t="inlineStr">
         <is>
-          <t>**maa://22866 (30.19), maa://26222 (97.83)</t>
+          <t>**maa://22866 (30.19), maa://26222 (97.87)</t>
         </is>
       </c>
       <c r="U9" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.52)</t>
+          <t>maa://26223 (97.58)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.38), ***maa://22740 (5.77), **maa://39938 (46.15), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (94.12)</t>
+          <t>maa://28711 (87.38), ***maa://22740 (5.77), **maa://39938 (46.15), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (94.44)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (89.62), *maa://22865 (51.92)</t>
+          <t>maa://26206 (89.81), *maa://22865 (51.92)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.34), **maa://32237 (41.86), ***maa://34206 (20.83), ***maa://39951 (16.28), ***maa://39243 (28.57), **maa://45271 (50.0)</t>
+          <t>***maa://25695 (19.13), **maa://32237 (40.91), ***maa://34206 (20.83), ***maa://39951 (16.28), ***maa://39243 (28.57), **maa://45271 (50.0)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1741,7 +1741,7 @@
       </c>
       <c r="L10" s="2" t="inlineStr">
         <is>
-          <t>**maa://24395 (39.29)</t>
+          <t>**maa://24395 (41.38)</t>
         </is>
       </c>
       <c r="M10" s="1" t="n"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (91.36), maa://36669 (89.74), *maa://23264 (61.82)</t>
+          <t>maa://28977 (91.46), maa://36669 (90.0), *maa://23264 (61.82)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.11), maa://22755 (87.61), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.17), maa://22755 (87.61), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (55.29), *maa://22733 (59.38), maa://22761 (100.0)</t>
+          <t>*maa://25021 (55.29), *maa://22733 (60.61), maa://22761 (100.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (88.54)</t>
+          <t>maa://21287 (88.66)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.86), maa://22501 (97.3)</t>
+          <t>maa://22747 (92.86), maa://22501 (97.33)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.97)</t>
+          <t>maa://36713 (97.98)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (89.76)</t>
+          <t>maa://21867 (89.82)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (90.91), *maa://21485 (77.21), maa://37962 (86.67)</t>
+          <t>maa://22753 (90.96), *maa://21485 (77.37), maa://37962 (87.1)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.41), maa://36677 (92.31), maa://39872 (90.0)</t>
+          <t>maa://23669 (95.41), maa://36677 (92.45), maa://39872 (90.0)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.2), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (78.52), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.83), maa://36673 (92.86), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.85), maa://36673 (92.86), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (75.11), **maa://22728 (47.73)</t>
+          <t>*maa://21248 (75.22), **maa://22728 (47.73)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (92.11), *maa://22583 (74.24), *maa://22500 (57.78)</t>
+          <t>maa://22676 (92.17), *maa://22583 (74.24), *maa://22500 (57.78)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (32.37), maa://39883 (91.23), *maa://39885 (56.0)</t>
+          <t>**maa://22737 (32.14), maa://39883 (91.23), *maa://39885 (57.69)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.55), maa://21288 (96.3), maa://39841 (95.4), maa://36682 (97.37)</t>
+          <t>maa://26245 (96.55), maa://21288 (96.3), maa://39841 (95.45), maa://36682 (97.44)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.63), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.65), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="T14" s="2" t="inlineStr">
         <is>
-          <t>maa://22521 (93.88), maa://42751 (100.0)</t>
+          <t>maa://22521 (93.94), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="1" t="n"/>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="AB14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (96.92)</t>
+          <t>maa://22764 (96.97)</t>
         </is>
       </c>
       <c r="AC14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.66), maa://22734 (84.03), *maa://30808 (65.08), **maa://36048 (35.42), maa://45058 (100.0)</t>
+          <t>*maa://22743 (77.66), maa://22734 (84.03), *maa://30808 (65.62), **maa://36048 (36.0), maa://45058 (100.0)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.24), maa://21478 (91.43)</t>
+          <t>maa://24304 (88.24), maa://21478 (91.67)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.15), *maa://22766 (70.27), *maa://36666 (78.16)</t>
+          <t>maa://21364 (81.27), *maa://22766 (70.54), *maa://36666 (78.16)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (97.85), maa://28051 (96.0)</t>
+          <t>maa://28501 (97.87), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.51)</t>
+          <t>maa://26228 (95.56)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (65.69), maa://27755 (92.77)</t>
+          <t>*maa://23911 (65.38), maa://27755 (92.77)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.83), maa://39599 (87.18)</t>
+          <t>maa://22430 (88.95), maa://39599 (87.18)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (89.8)</t>
+          <t>maa://24421 (89.47)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (88.97), *maa://22732 (50.6)</t>
+          <t>maa://22466 (89.12), **maa://22732 (50.0)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="X18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (97.8), maa://22741 (83.33)</t>
+          <t>maa://21917 (97.8), maa://22741 (85.71)</t>
         </is>
       </c>
       <c r="Y18" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (99.07)</t>
+          <t>maa://24386 (99.08)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (89.54)</t>
+          <t>maa://22864 (89.61)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.59)</t>
+          <t>maa://41331 (84.82)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="P20" s="2" t="inlineStr">
         <is>
-          <t>maa://37442 (94.59)</t>
+          <t>maa://37442 (94.74)</t>
         </is>
       </c>
       <c r="Q20" s="1" t="n"/>
@@ -3171,7 +3171,7 @@
       </c>
       <c r="L21" s="2" t="inlineStr">
         <is>
-          <t>maa://31731 (95.56)</t>
+          <t>maa://31731 (95.74)</t>
         </is>
       </c>
       <c r="M21" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (80.06), ***maa://23820 (29.31)</t>
+          <t>maa://21443 (80.11), ***maa://23820 (29.31)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.63), *maa://22432 (77.42)</t>
+          <t>maa://22524 (94.69), *maa://22432 (77.78)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>maa://25236 (96.39), **maa://21678 (48.94), **maa://22735 (42.86)</t>
+          <t>maa://25236 (96.43), **maa://21678 (48.94), **maa://22735 (42.86)</t>
         </is>
       </c>
       <c r="I22" s="1" t="n"/>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="T22" s="2" t="inlineStr">
         <is>
-          <t>maa://38495 (84.62)</t>
+          <t>maa://38495 (85.71)</t>
         </is>
       </c>
       <c r="U22" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.48), *maa://37649 (66.67)</t>
+          <t>maa://21282 (98.51), *maa://37649 (66.67)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (94.58), maa://39875 (93.85)</t>
+          <t>maa://39756 (94.66), maa://39875 (93.85)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (92.06), *maa://29748 (75.78), ***maa://29785 (16.42), *maa://37566 (70.0)</t>
+          <t>maa://30587 (92.11), *maa://29748 (75.78), ***maa://29785 (16.42), *maa://37566 (70.0)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.36)</t>
+          <t>*maa://24368 (78.2)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (86.52), maa://23504 (93.18), **maa://22892 (39.73), *maa://25141 (76.56), *maa://36663 (78.57), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (85.9), maa://23504 (93.22), **maa://22892 (39.73), *maa://25141 (76.74), *maa://36663 (78.57), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.71), maa://36672 (81.13), maa://29910 (92.86), **maa://21440 (34.55)</t>
+          <t>maa://22523 (85.71), maa://36672 (81.48), maa://29910 (92.86), **maa://21440 (34.55)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (74.17), *maa://25311 (73.53), ***maa://22725 (4.84), maa://45047 (100.0)</t>
+          <t>*maa://29063 (74.34), *maa://25311 (73.53), ***maa://22725 (4.84), maa://45047 (100.0)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3723,7 +3723,7 @@
       </c>
       <c r="T25" s="2" t="inlineStr">
         <is>
-          <t>maa://20109 (92.4), maa://22545 (100.0), maa://42915 (100.0)</t>
+          <t>maa://20109 (92.44), maa://22545 (100.0), maa://42915 (100.0)</t>
         </is>
       </c>
       <c r="U25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (86.27), *maa://24516 (79.78), maa://26001 (87.5)</t>
+          <t>maa://31215 (86.41), *maa://24516 (79.78), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.27), maa://24621 (96.61), maa://36676 (96.88), maa://22771 (85.71), **maa://37772 (50.0)</t>
+          <t>maa://20108 (96.27), maa://24621 (96.64), maa://36676 (96.88), maa://22771 (85.71), **maa://37772 (50.0)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>maa://41802 (92.31)</t>
+          <t>maa://41802 (92.86)</t>
         </is>
       </c>
       <c r="E26" s="1" t="n"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (91.46)</t>
+          <t>maa://24913 (91.57)</t>
         </is>
       </c>
       <c r="I26" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (93.75)</t>
+          <t>maa://42235 (93.83)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3901,7 +3901,7 @@
       </c>
       <c r="AF26" s="2" t="inlineStr">
         <is>
-          <t>maa://30511 (83.78), *maa://29760 (64.29)</t>
+          <t>maa://30511 (84.21), *maa://29760 (64.29)</t>
         </is>
       </c>
       <c r="AG26" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.81), maa://25725 (83.72)</t>
+          <t>maa://24465 (90.83), maa://25725 (83.72)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4081,7 +4081,7 @@
       </c>
       <c r="L28" s="2" t="inlineStr">
         <is>
-          <t>*maa://30770 (79.55)</t>
+          <t>*maa://30770 (80.0)</t>
         </is>
       </c>
       <c r="M28" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>maa://23263 (95.0), *maa://29765 (61.54)</t>
+          <t>maa://23263 (95.05), *maa://29765 (61.54)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (89.97), maa://41749 (92.06), ***maa://39723 (14.29)</t>
+          <t>maa://39929 (90.12), maa://41749 (92.19), ***maa://39723 (14.29)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (93.06), *maa://36701 (64.29)</t>
+          <t>maa://36660 (93.12), *maa://36701 (64.29)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (92.97), *maa://28440 (77.08), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.02), *maa://28440 (77.08), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4227,7 +4227,7 @@
       </c>
       <c r="P29" s="2" t="inlineStr">
         <is>
-          <t>*maa://23168 (55.56), *maa://30050 (53.33)</t>
+          <t>*maa://23168 (56.36), *maa://30050 (51.61)</t>
         </is>
       </c>
       <c r="Q29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.87), *maa://42865 (78.95), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.87), maa://42865 (80.95), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4357,7 +4357,7 @@
       </c>
       <c r="P30" s="2" t="inlineStr">
         <is>
-          <t>maa://21442 (99.52)</t>
+          <t>maa://21442 (99.53)</t>
         </is>
       </c>
       <c r="Q30" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.69), maa://45045 (100.0)</t>
+          <t>maa://42979 (96.0), maa://45045 (100.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.38), maa://36258 (84.0), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.41), maa://36258 (84.16), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.41), maa://36667 (98.44), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.44), maa://36667 (98.46), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (95.6), maa://41108 (88.0), maa://41238 (96.43)</t>
+          <t>maa://42859 (95.7), maa://41108 (88.0), maa://41238 (96.55)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4681,7 +4681,7 @@
       </c>
       <c r="AF32" s="2" t="inlineStr">
         <is>
-          <t>*maa://42408 (75.0)</t>
+          <t>*maa://42408 (77.78)</t>
         </is>
       </c>
       <c r="AG32" s="1" t="n"/>
@@ -4747,7 +4747,7 @@
       </c>
       <c r="P33" s="2" t="inlineStr">
         <is>
-          <t>*maa://21956 (79.86), *maa://22730 (79.31)</t>
+          <t>maa://21956 (80.14), *maa://22730 (79.31)</t>
         </is>
       </c>
       <c r="Q33" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.85)</t>
+          <t>maa://41296 (96.88)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5105,7 +5105,7 @@
       </c>
       <c r="T36" s="2" t="inlineStr">
         <is>
-          <t>maa://27613 (99.03)</t>
+          <t>maa://27613 (99.04)</t>
         </is>
       </c>
       <c r="U36" s="1" t="n"/>
@@ -5187,7 +5187,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (88.83), *maa://21239 (66.67)</t>
+          <t>maa://21280 (88.89), *maa://21239 (66.67)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="P38" s="2" t="inlineStr">
         <is>
-          <t>*maa://24383 (68.04)</t>
+          <t>*maa://24383 (68.69)</t>
         </is>
       </c>
       <c r="Q38" s="1" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.56)</t>
+          <t>maa://36697 (86.84)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (84.82), maa://36670 (87.91), maa://30434 (89.86), ***maa://25036 (16.0), *maa://44165 (66.67), *maa://45059 (80.0)</t>
+          <t>maa://25199 (84.82), maa://36670 (87.91), maa://30434 (90.0), ***maa://25036 (16.0), *maa://44165 (66.67), *maa://45059 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.67)</t>
+          <t>maa://24709 (91.73)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5458,7 +5458,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.68), maa://21386 (95.74), maa://36664 (90.91)</t>
+          <t>maa://23278 (95.7), maa://21386 (95.74), maa://36664 (90.91)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5665,7 +5665,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (92.7), maa://21284 (83.72)</t>
+          <t>maa://22525 (92.7), maa://21284 (84.09)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5734,7 +5734,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.87), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.88), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5787,7 +5787,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.86), maa://30807 (95.52), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (81.82)</t>
+          <t>maa://21229 (84.86), maa://30807 (95.52), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (85.71)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5819,7 +5819,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (39.13)</t>
+          <t>**maa://39364 (36.0)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -5840,7 +5840,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.41), maa://43901 (91.67)</t>
+          <t>maa://35931 (92.44), maa://43901 (92.31)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.25), maa://29661 (97.86), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.26), maa://29661 (97.18), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6136,7 +6136,7 @@
       </c>
       <c r="H52" s="2" t="inlineStr">
         <is>
-          <t>maa://24376 (96.55)</t>
+          <t>maa://24376 (96.67)</t>
         </is>
       </c>
       <c r="I52" s="1" t="n"/>
@@ -6170,7 +6170,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.67), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.69), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6206,7 +6206,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.08)</t>
+          <t>maa://32532 (92.11)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (83.18), maa://31270 (95.0)</t>
+          <t>maa://27746 (82.41), maa://31270 (95.04)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6296,7 +6296,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (63.27)</t>
+          <t>*maa://40438 (64.0)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>
@@ -6332,7 +6332,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (96.97), maa://43903 (100.0)</t>
+          <t>maa://42981 (97.06), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>
@@ -6368,7 +6368,7 @@
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>maa://44405 (91.3)</t>
+          <t>maa://44405 (91.67)</t>
         </is>
       </c>
       <c r="I64" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#143)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (66.31), maa://20276 (85.37), *maa://22749 (72.73)</t>
+          <t>*maa://22880 (66.31), maa://20276 (85.45), *maa://22749 (72.73)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.35), maa://27484 (96.23), maa://27480 (82.86)</t>
+          <t>maa://27396 (84.35), maa://27484 (96.26), maa://27480 (82.86)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (98.08), maa://27295 (84.62), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
+          <t>maa://32509 (97.17), maa://27295 (84.62), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>*maa://22757 (79.41)</t>
+          <t>*maa://22757 (77.14)</t>
         </is>
       </c>
       <c r="M5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (94.87)</t>
+          <t>maa://42407 (95.0)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="T7" s="2" t="inlineStr">
         <is>
-          <t>maa://21291 (84.44)</t>
+          <t>maa://21291 (84.78)</t>
         </is>
       </c>
       <c r="U7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.01.17 13:17:18</t>
+          <t>更新日期：2025.01.18 13:16:09</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.38), ***maa://22740 (5.77), **maa://39938 (46.15), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (94.44)</t>
+          <t>maa://28711 (87.38), ***maa://22740 (5.77), **maa://39938 (46.15), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (95.0)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.56)</t>
+          <t>maa://26228 (95.6)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>maa://21624 (83.33)</t>
+          <t>maa://21624 (83.78)</t>
         </is>
       </c>
       <c r="E17" s="1" t="n"/>
@@ -2845,7 +2845,7 @@
       </c>
       <c r="AB18" s="2" t="inlineStr">
         <is>
-          <t>maa://24393 (97.62)</t>
+          <t>maa://24393 (97.67)</t>
         </is>
       </c>
       <c r="AC18" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (63.86), *maa://36668 (56.41)</t>
+          <t>*maa://30709 (63.94), *maa://36668 (56.41)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (84.82)</t>
+          <t>maa://41331 (84.96)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.69), *maa://22432 (77.78)</t>
+          <t>maa://22524 (94.71), *maa://22432 (77.78)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.51), *maa://37649 (66.67)</t>
+          <t>maa://21282 (98.51), *maa://37649 (67.86)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (94.66), maa://39875 (93.85)</t>
+          <t>maa://39756 (94.7), maa://39875 (93.85)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (93.83)</t>
+          <t>maa://42235 (93.9)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.12), maa://41749 (92.19), ***maa://39723 (14.29)</t>
+          <t>maa://39929 (90.15), maa://41749 (90.77), ***maa://39723 (14.29)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4227,7 +4227,7 @@
       </c>
       <c r="P29" s="2" t="inlineStr">
         <is>
-          <t>*maa://23168 (56.36), *maa://30050 (51.61)</t>
+          <t>*maa://23168 (57.14), *maa://30050 (51.61)</t>
         </is>
       </c>
       <c r="Q29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.0), maa://45045 (100.0)</t>
+          <t>maa://42979 (96.03), maa://45045 (100.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (95.7), maa://41108 (88.0), maa://41238 (96.55)</t>
+          <t>maa://42859 (95.74), maa://41108 (88.0), maa://41238 (96.55)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4681,7 +4681,7 @@
       </c>
       <c r="AF32" s="2" t="inlineStr">
         <is>
-          <t>*maa://42408 (77.78)</t>
+          <t>*maa://42408 (80.0)</t>
         </is>
       </c>
       <c r="AG32" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.88)</t>
+          <t>maa://41296 (96.9)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5105,7 +5105,7 @@
       </c>
       <c r="T36" s="2" t="inlineStr">
         <is>
-          <t>maa://27613 (99.04)</t>
+          <t>maa://27613 (99.05)</t>
         </is>
       </c>
       <c r="U36" s="1" t="n"/>
@@ -5203,7 +5203,7 @@
       </c>
       <c r="T37" s="2" t="inlineStr">
         <is>
-          <t>***maa://39354 (25.0)</t>
+          <t>**maa://39354 (33.33)</t>
         </is>
       </c>
       <c r="U37" s="1" t="n"/>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (84.82), maa://36670 (87.91), maa://30434 (90.0), ***maa://25036 (16.0), *maa://44165 (66.67), *maa://45059 (66.67)</t>
+          <t>maa://25199 (84.82), maa://36670 (87.91), maa://30434 (90.14), ***maa://25036 (16.0), *maa://44165 (66.67), *maa://45059 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5453,12 +5453,12 @@
       </c>
       <c r="O40" s="1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.7), maa://21386 (95.74), maa://36664 (90.91)</t>
+          <t>maa://23278 (95.7), maa://21386 (95.74), maa://36664 (90.91), maa://45550 (100.0)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5543,7 +5543,7 @@
       </c>
       <c r="P41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (38.24), maa://43177 (86.67)</t>
+          <t>**maa://35616 (38.24), maa://43177 (87.5)</t>
         </is>
       </c>
       <c r="Q41" s="1" t="n"/>
@@ -5766,7 +5766,7 @@
       </c>
       <c r="T44" s="2" t="inlineStr">
         <is>
-          <t>maa://39366 (87.1)</t>
+          <t>maa://39366 (87.5)</t>
         </is>
       </c>
       <c r="U44" s="1" t="n"/>
@@ -5819,7 +5819,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (36.0)</t>
+          <t>**maa://39364 (38.46)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -6296,7 +6296,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (64.0)</t>
+          <t>*maa://40438 (64.71)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#144)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.01.18 13:16:09</t>
+          <t>更新日期：2025.01.18 14:49:21</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (74.34), *maa://25311 (73.53), ***maa://22725 (4.84), maa://45047 (100.0)</t>
+          <t>*maa://29063 (74.51), *maa://25311 (73.53), ***maa://22725 (4.84), maa://45047 (100.0)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#145)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.35), maa://25390 (95.98), maa://36681 (87.01)</t>
+          <t>maa://24702 (94.39), maa://25390 (96.06), maa://36681 (87.34)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.05), *maa://30515 (69.31), *maa://34787 (73.61), ***maa://20792 (11.93), maa://39402 (89.58), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.33), *maa://30515 (69.61), *maa://34787 (72.97), ***maa://20792 (11.93), maa://39402 (90.2), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.19), *maa://20791 (63.89)</t>
+          <t>maa://22742 (91.3), *maa://20791 (63.01)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.38), maa://36684 (94.95), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.41), maa://36684 (95.0), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.31), ***maa://21730 (22.86), ***maa://39501 (18.18), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.45), ***maa://21730 (23.94), ***maa://39501 (21.74), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.48), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.5), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (66.31), maa://20276 (85.45), *maa://22749 (72.73)</t>
+          <t>*maa://22880 (65.26), maa://20276 (85.71), *maa://22749 (72.73)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.25), maa://26254 (96.3)</t>
+          <t>maa://21249 (94.27), maa://26254 (96.3)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.29), **maa://20790 (44.12), ***maa://37170 (18.64)</t>
+          <t>maa://24617 (89.38), **maa://20790 (44.12), ***maa://37170 (17.46)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.35), maa://27484 (96.26), maa://27480 (82.86)</t>
+          <t>maa://27396 (84.54), maa://27484 (96.36), maa://27480 (82.86)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (93.75)</t>
+          <t>maa://24390 (93.85)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.46), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.59), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.17), maa://27295 (84.62), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
+          <t>maa://32509 (97.3), maa://27295 (84.62), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (47.91), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (91.67)</t>
+          <t>**maa://32495 (48.31), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (87.18)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (63.04), ***maa://26209 (13.04), *maa://39394 (68.18)</t>
+          <t>*maa://30062 (63.83), ***maa://26209 (13.04), *maa://39394 (69.57)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (83.71), maa://22744 (84.0)</t>
+          <t>maa://21245 (83.93), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="P5" s="2" t="inlineStr">
         <is>
-          <t>maa://21919 (96.23), maa://21281 (85.71)</t>
+          <t>maa://21919 (96.3), *maa://21281 (80.0)</t>
         </is>
       </c>
       <c r="Q5" s="1" t="n"/>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="AB5" s="2" t="inlineStr">
         <is>
-          <t>*maa://29863 (67.65), ***maa://22752 (12.5), **maa://26013 (37.5)</t>
+          <t>*maa://29863 (68.57), ***maa://22752 (12.5), **maa://26013 (37.5)</t>
         </is>
       </c>
       <c r="AC5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (95.0)</t>
+          <t>maa://42407 (95.12)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>maa://24839 (99.29)</t>
+          <t>maa://24839 (98.95)</t>
         </is>
       </c>
       <c r="M6" s="1" t="n"/>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="T6" s="2" t="inlineStr">
         <is>
-          <t>maa://37411 (86.67)</t>
+          <t>maa://37411 (87.5)</t>
         </is>
       </c>
       <c r="U6" s="1" t="n"/>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>*maa://22763 (66.67)</t>
+          <t>*maa://22763 (64.52)</t>
         </is>
       </c>
       <c r="I7" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (93.55), maa://24957 (97.73)</t>
+          <t>maa://28624 (91.67), maa://24957 (97.73)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="P7" s="2" t="inlineStr">
         <is>
-          <t>maa://22750 (90.7)</t>
+          <t>maa://22750 (91.11)</t>
         </is>
       </c>
       <c r="Q7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.24), *maa://22758 (74.6)</t>
+          <t>maa://22399 (95.3), *maa://22758 (75.0)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (67.9), *maa://36671 (68.0), *maa://42530 (60.0), maa://45272 (100.0)</t>
+          <t>*maa://26191 (68.29), *maa://36671 (68.0), *maa://42530 (60.0), maa://45272 (100.0)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.01.18 14:49:21</t>
+          <t>更新日期：2025.01.25 08:45:24</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>*maa://21476 (74.51), **maa://39431 (50.0), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (73.08), **maa://39431 (50.0), *maa://37551 (57.14)</t>
         </is>
       </c>
       <c r="E8" s="1" t="n"/>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (84.11), *maa://21916 (61.29), maa://23252 (92.42), maa://37496 (96.55), **maa://22759 (45.45)</t>
+          <t>maa://32931 (83.49), *maa://21916 (61.9), maa://23252 (92.54), maa://37496 (96.67), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.99)</t>
+          <t>maa://21411 (96.03)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>maa://22762 (91.95), maa://39552 (90.0)</t>
+          <t>maa://22762 (92.05), maa://39552 (90.0)</t>
         </is>
       </c>
       <c r="M9" s="1" t="n"/>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (81.91)</t>
+          <t>maa://22736 (82.11)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.58)</t>
+          <t>maa://26223 (97.62)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.38), ***maa://22740 (5.77), **maa://39938 (46.15), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (95.0)</t>
+          <t>maa://28711 (86.36), ***maa://22740 (5.77), **maa://39938 (44.44), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (95.24)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (89.81), *maa://22865 (51.92)</t>
+          <t>maa://26206 (90.09), *maa://22865 (51.92)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.13), **maa://32237 (40.91), ***maa://34206 (20.83), ***maa://39951 (16.28), ***maa://39243 (28.57), **maa://45271 (50.0)</t>
+          <t>***maa://25695 (19.02), **maa://32237 (40.91), ***maa://34206 (20.83), ***maa://39951 (15.91), ***maa://39243 (28.57), **maa://45271 (50.0)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (91.46), maa://36669 (90.0), *maa://23264 (61.82)</t>
+          <t>maa://28977 (90.36), maa://36669 (87.8), *maa://23264 (61.82)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.17), maa://22755 (87.61), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.22), maa://22755 (87.72), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.67), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.7), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.43)</t>
+          <t>maa://36707 (99.45)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -1882,12 +1882,12 @@
       </c>
       <c r="O11" s="1" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P11" s="2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>maa://45557 (100.0)</t>
         </is>
       </c>
       <c r="Q11" s="1" t="n"/>
@@ -1898,12 +1898,12 @@
       </c>
       <c r="S11" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.86), maa://22501 (97.33)</t>
+          <t>maa://22747 (92.86), maa://22501 (97.47), *maa://45521 (60.0)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.98)</t>
+          <t>maa://36713 (97.84)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (89.82)</t>
+          <t>maa://21867 (89.88)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (90.96), *maa://21485 (77.37), maa://37962 (87.1)</t>
+          <t>maa://22753 (91.12), *maa://21485 (76.81), maa://37962 (87.88)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.41), maa://36677 (92.45), maa://39872 (90.0)</t>
+          <t>maa://23669 (95.44), maa://36677 (92.59), maa://39872 (90.48)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.52), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (77.94), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.85), maa://36673 (92.86), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.94), maa://36673 (92.96), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (75.22), **maa://22728 (47.73)</t>
+          <t>*maa://21248 (75.0), **maa://22728 (47.73)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (92.17), *maa://22583 (74.24), *maa://22500 (57.78)</t>
+          <t>maa://22676 (92.31), *maa://22583 (74.24), *maa://22500 (57.78)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>maa://34957 (80.88), *maa://22768 (51.61)</t>
+          <t>maa://34957 (81.16), *maa://22768 (51.61)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (32.14), maa://39883 (91.23), *maa://39885 (57.69)</t>
+          <t>**maa://22737 (32.62), maa://39883 (91.94), *maa://39885 (55.56)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.55), maa://21288 (96.3), maa://39841 (95.45), maa://36682 (97.44)</t>
+          <t>maa://26245 (96.58), maa://21288 (96.3), maa://39841 (95.65), maa://36682 (97.44)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.65), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.67), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="AB14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (96.97)</t>
+          <t>maa://22764 (97.01)</t>
         </is>
       </c>
       <c r="AC14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.66), maa://22734 (84.03), *maa://30808 (65.62), **maa://36048 (36.0), maa://45058 (100.0)</t>
+          <t>*maa://22743 (77.39), maa://22734 (84.03), *maa://30808 (63.64), **maa://36048 (39.62), maa://45058 (100.0)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.24), maa://21478 (91.67)</t>
+          <t>maa://24304 (87.86), maa://21478 (91.67)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (90.38), *maa://22727 (70.0)</t>
+          <t>maa://24762 (90.51), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.27), *maa://22766 (70.54), *maa://36666 (78.16)</t>
+          <t>maa://21364 (81.39), *maa://36666 (78.89), *maa://22766 (69.91)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.77), *maa://28648 (68.25), maa://36674 (83.33)</t>
+          <t>maa://22729 (94.77), *maa://28648 (68.75), maa://36674 (82.22)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (97.87), maa://28051 (96.0)</t>
+          <t>maa://28501 (97.89), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.6)</t>
+          <t>maa://26228 (95.65)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (65.38), maa://27755 (92.77)</t>
+          <t>*maa://23911 (65.38), maa://27755 (92.94)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.95), maa://39599 (87.18)</t>
+          <t>maa://22430 (88.54), maa://39599 (85.71)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.18)</t>
+          <t>maa://24570 (97.2)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (89.12), **maa://22732 (50.0)</t>
+          <t>maa://22466 (89.33), *maa://22732 (51.16)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="X18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (97.8), maa://22741 (85.71)</t>
+          <t>maa://21917 (96.77), maa://22741 (85.71)</t>
         </is>
       </c>
       <c r="Y18" s="1" t="n"/>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (58.13), **maa://29784 (44.44)</t>
+          <t>*maa://24313 (58.39), **maa://29784 (44.44)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (99.08)</t>
+          <t>maa://24386 (99.1)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (63.94), *maa://36668 (56.41)</t>
+          <t>*maa://30709 (64.37), *maa://36668 (57.5)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -2991,7 +2991,7 @@
       </c>
       <c r="AF19" s="2" t="inlineStr">
         <is>
-          <t>*maa://21663 (61.76)</t>
+          <t>*maa://21663 (62.32)</t>
         </is>
       </c>
       <c r="AG19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.07), maa://25198 (93.14), *maa://20795 (51.56), maa://36680 (93.55)</t>
+          <t>maa://21432 (89.68), maa://25198 (93.4), *maa://20795 (51.56), maa://36680 (93.75)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (84.96)</t>
+          <t>maa://41331 (86.07)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="P20" s="2" t="inlineStr">
         <is>
-          <t>maa://37442 (94.74)</t>
+          <t>maa://37442 (94.87)</t>
         </is>
       </c>
       <c r="Q20" s="1" t="n"/>
@@ -3155,7 +3155,7 @@
       </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>maa://24372 (96.77)</t>
+          <t>maa://24372 (96.84)</t>
         </is>
       </c>
       <c r="I21" s="1" t="n"/>
@@ -3171,7 +3171,7 @@
       </c>
       <c r="L21" s="2" t="inlineStr">
         <is>
-          <t>maa://31731 (95.74)</t>
+          <t>maa://31731 (95.92)</t>
         </is>
       </c>
       <c r="M21" s="1" t="n"/>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="X21" s="2" t="inlineStr">
         <is>
-          <t>maa://20110 (86.76), maa://34946 (92.68)</t>
+          <t>maa://20110 (86.76), maa://34946 (92.86)</t>
         </is>
       </c>
       <c r="Y21" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (80.11), ***maa://23820 (29.31)</t>
+          <t>maa://21443 (80.39), ***maa://23820 (29.31)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.71), *maa://22432 (77.78)</t>
+          <t>maa://22524 (94.29), *maa://22432 (77.78)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>maa://25236 (96.43), **maa://21678 (48.94), **maa://22735 (42.86)</t>
+          <t>maa://25236 (96.47), **maa://21678 (48.94), **maa://22735 (42.86)</t>
         </is>
       </c>
       <c r="I22" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (84.26), *maa://22751 (73.85)</t>
+          <t>maa://27127 (83.64), *maa://22751 (71.64)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.51), *maa://37649 (67.86)</t>
+          <t>maa://21282 (98.53), *maa://37649 (67.86)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (94.7), maa://39875 (93.85)</t>
+          <t>maa://39756 (94.97), maa://39875 (93.94)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (92.11), *maa://29748 (75.78), ***maa://29785 (16.42), *maa://37566 (70.0)</t>
+          <t>maa://30587 (91.71), *maa://29748 (75.78), ***maa://29785 (16.42), *maa://37566 (71.88)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="T23" s="2" t="inlineStr">
         <is>
-          <t>maa://24387 (81.58), maa://31212 (93.1)</t>
+          <t>maa://24387 (81.58), maa://31212 (93.33)</t>
         </is>
       </c>
       <c r="U23" s="1" t="n"/>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="X23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (65.71)</t>
+          <t>*maa://28503 (64.79)</t>
         </is>
       </c>
       <c r="Y23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.2)</t>
+          <t>*maa://24368 (78.05)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (85.9), maa://23504 (93.22), **maa://22892 (39.73), *maa://25141 (76.74), *maa://36663 (78.57), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (85.54), maa://23504 (93.3), **maa://22892 (40.14), *maa://25141 (76.74), *maa://36663 (77.46), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.71), maa://36672 (81.48), maa://29910 (92.86), **maa://21440 (34.55)</t>
+          <t>maa://22523 (85.71), maa://36672 (81.82), maa://29910 (92.86), **maa://21440 (34.55)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (94.96)</t>
+          <t>maa://29753 (95.0)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (74.51), *maa://25311 (73.53), ***maa://22725 (4.84), maa://45047 (100.0)</t>
+          <t>*maa://29063 (74.19), *maa://25311 (73.53), ***maa://22725 (4.84), **maa://45047 (50.0)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3739,7 +3739,7 @@
       </c>
       <c r="X25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29890 (77.27)</t>
+          <t>*maa://29890 (77.78)</t>
         </is>
       </c>
       <c r="Y25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (86.41), *maa://24516 (79.78), maa://26001 (87.5)</t>
+          <t>maa://31215 (86.79), *maa://24516 (79.78), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.27), maa://24621 (96.64), maa://36676 (96.88), maa://22771 (85.71), **maa://37772 (50.0)</t>
+          <t>maa://20108 (96.27), maa://24621 (96.69), maa://36676 (96.88), maa://22771 (85.71), **maa://37772 (50.0)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (91.57)</t>
+          <t>maa://24913 (91.67)</t>
         </is>
       </c>
       <c r="I26" s="1" t="n"/>
@@ -3837,7 +3837,7 @@
       </c>
       <c r="P26" s="2" t="inlineStr">
         <is>
-          <t>*maa://30968 (63.16), maa://39870 (100.0)</t>
+          <t>*maa://30968 (65.0), maa://39870 (90.91)</t>
         </is>
       </c>
       <c r="Q26" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (93.9)</t>
+          <t>maa://42235 (94.19)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3901,7 +3901,7 @@
       </c>
       <c r="AF26" s="2" t="inlineStr">
         <is>
-          <t>maa://30511 (84.21), *maa://29760 (64.29)</t>
+          <t>maa://30511 (82.5), *maa://29760 (64.29)</t>
         </is>
       </c>
       <c r="AG26" s="1" t="n"/>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (48.0), maa://34494 (96.67), *maa://39601 (76.47), **maa://36665 (44.44)</t>
+          <t>**maa://21283 (48.0), *maa://39601 (76.47), maa://34494 (96.97), **maa://36665 (44.44)</t>
         </is>
       </c>
       <c r="I27" s="1" t="n"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (78.18)</t>
+          <t>*maa://30624 (78.57)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4031,7 +4031,7 @@
       </c>
       <c r="AF27" s="2" t="inlineStr">
         <is>
-          <t>maa://24023 (97.06)</t>
+          <t>maa://24023 (97.1)</t>
         </is>
       </c>
       <c r="AG27" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.83), maa://25725 (83.72)</t>
+          <t>maa://24465 (90.91), maa://25725 (83.72)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>maa://23263 (95.05), *maa://29765 (61.54)</t>
+          <t>maa://23263 (95.1), *maa://29765 (62.96)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.15), maa://41749 (90.77), ***maa://39723 (14.29)</t>
+          <t>maa://39929 (90.6), maa://41749 (91.3), ***maa://39723 (14.29)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (93.12), *maa://36701 (64.29)</t>
+          <t>maa://36660 (92.66), *maa://36701 (65.52)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>*maa://25175 (68.75)</t>
+          <t>*maa://25175 (67.35)</t>
         </is>
       </c>
       <c r="I29" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.02), *maa://28440 (77.08), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.15), *maa://28440 (78.64), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4227,7 +4227,7 @@
       </c>
       <c r="P29" s="2" t="inlineStr">
         <is>
-          <t>*maa://23168 (57.14), *maa://30050 (51.61)</t>
+          <t>*maa://23168 (56.9), *maa://30050 (51.61)</t>
         </is>
       </c>
       <c r="Q29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.87), maa://42865 (80.95), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.95), maa://42865 (80.95), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4304,12 +4304,12 @@
       </c>
       <c r="C30" s="1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>maa://45792 (100.0)</t>
         </is>
       </c>
       <c r="E30" s="1" t="n"/>
@@ -4341,7 +4341,7 @@
       </c>
       <c r="L30" s="2" t="inlineStr">
         <is>
-          <t>maa://30442 (94.92)</t>
+          <t>maa://30442 (95.0)</t>
         </is>
       </c>
       <c r="M30" s="1" t="n"/>
@@ -4357,7 +4357,7 @@
       </c>
       <c r="P30" s="2" t="inlineStr">
         <is>
-          <t>maa://21442 (99.53)</t>
+          <t>maa://21442 (99.54)</t>
         </is>
       </c>
       <c r="Q30" s="1" t="n"/>
@@ -4389,7 +4389,7 @@
       </c>
       <c r="X30" s="2" t="inlineStr">
         <is>
-          <t>maa://39477 (86.67)</t>
+          <t>maa://39477 (87.5)</t>
         </is>
       </c>
       <c r="Y30" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.03), maa://45045 (100.0)</t>
+          <t>maa://42979 (96.15), maa://45045 (100.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.41), maa://36258 (84.16), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.45), maa://36258 (84.76), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4530,12 +4530,12 @@
       </c>
       <c r="AA31" s="1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AB31" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>None</t>
         </is>
       </c>
       <c r="AC31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.44), maa://36667 (98.46), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.45), maa://36667 (98.55), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4601,7 +4601,7 @@
       </c>
       <c r="L32" s="2" t="inlineStr">
         <is>
-          <t>maa://28065 (94.87)</t>
+          <t>maa://28065 (95.0)</t>
         </is>
       </c>
       <c r="M32" s="1" t="n"/>
@@ -4628,12 +4628,12 @@
       </c>
       <c r="S32" s="1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (95.74), maa://41108 (88.0), maa://41238 (96.55)</t>
+          <t>maa://42859 (95.96), maa://41108 (88.0), maa://41238 (96.81), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4758,12 +4758,12 @@
       </c>
       <c r="S33" s="1" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="T33" s="2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>maa://45558 (100.0)</t>
         </is>
       </c>
       <c r="U33" s="1" t="n"/>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (93.63)</t>
+          <t>maa://24526 (93.65)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4925,7 +4925,7 @@
       </c>
       <c r="AF34" s="2" t="inlineStr">
         <is>
-          <t>*maa://32650 (66.67)</t>
+          <t>*maa://32650 (68.75)</t>
         </is>
       </c>
       <c r="AG34" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.9)</t>
+          <t>maa://41296 (97.12)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5045,6 +5045,22 @@
       <c r="AG35" s="1" t="n"/>
     </row>
     <row r="36">
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>寻澜</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D36" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E36" s="1" t="n"/>
       <c r="F36" s="1" t="inlineStr">
         <is>
           <t>鞭刃</t>
@@ -5105,7 +5121,7 @@
       </c>
       <c r="T36" s="2" t="inlineStr">
         <is>
-          <t>maa://27613 (99.05)</t>
+          <t>maa://27613 (99.07)</t>
         </is>
       </c>
       <c r="U36" s="1" t="n"/>
@@ -5155,7 +5171,7 @@
       </c>
       <c r="H37" s="2" t="inlineStr">
         <is>
-          <t>*maa://24374 (58.14)</t>
+          <t>*maa://24374 (56.82)</t>
         </is>
       </c>
       <c r="I37" s="1" t="n"/>
@@ -5166,12 +5182,12 @@
       </c>
       <c r="K37" s="1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2</t>
         </is>
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>maa://45718 (100.0), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5187,7 +5203,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (88.89), *maa://21239 (66.67)</t>
+          <t>maa://21280 (88.94), *maa://21239 (66.67)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5308,6 +5324,22 @@
         </is>
       </c>
       <c r="U38" s="1" t="n"/>
+      <c r="Z38" s="1" t="inlineStr">
+        <is>
+          <t>行箸</t>
+        </is>
+      </c>
+      <c r="AA38" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB38" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC38" s="1" t="n"/>
       <c r="AD38" s="1" t="inlineStr">
         <is>
           <t>阿斯卡纶</t>
@@ -5320,7 +5352,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.84)</t>
+          <t>maa://36697 (86.93)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5341,7 +5373,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://25199 (84.82), maa://36670 (87.91), maa://30434 (90.14), ***maa://25036 (16.0), *maa://44165 (66.67), *maa://45059 (66.67)</t>
+          <t>maa://36670 (88.04), maa://25199 (84.82), maa://30434 (90.28), ***maa://25036 (16.0), *maa://45059 (57.14), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5373,7 +5405,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.73)</t>
+          <t>maa://24709 (91.97)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5384,12 +5416,12 @@
       </c>
       <c r="S39" s="1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1</t>
         </is>
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>*maa://45788 (70.0)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5458,7 +5490,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.7), maa://21386 (95.74), maa://36664 (90.91), maa://45550 (100.0)</t>
+          <t>maa://23278 (95.71), maa://21386 (95.74), maa://36664 (90.91), maa://45550 (100.0)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5600,6 +5632,22 @@
         </is>
       </c>
       <c r="I42" s="1" t="n"/>
+      <c r="J42" s="1" t="inlineStr">
+        <is>
+          <t>余</t>
+        </is>
+      </c>
+      <c r="K42" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L42" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M42" s="1" t="n"/>
       <c r="N42" s="1" t="inlineStr">
         <is>
           <t>子月</t>
@@ -5665,7 +5713,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (92.7), maa://21284 (84.09)</t>
+          <t>maa://22525 (92.81), maa://21284 (84.78)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5734,7 +5782,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.88), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.91), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5766,7 +5814,7 @@
       </c>
       <c r="T44" s="2" t="inlineStr">
         <is>
-          <t>maa://39366 (87.5)</t>
+          <t>maa://39366 (87.88)</t>
         </is>
       </c>
       <c r="U44" s="1" t="n"/>
@@ -5787,7 +5835,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.86), maa://30807 (95.52), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (85.71)</t>
+          <t>maa://21229 (84.95), maa://30807 (95.52), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (86.67)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5840,7 +5888,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.44), maa://43901 (92.31)</t>
+          <t>maa://35931 (92.64), maa://43901 (92.86)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5893,7 +5941,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.26), maa://29661 (97.18), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.34), maa://29661 (97.24), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6122,6 +6170,22 @@
         </is>
       </c>
       <c r="Q51" s="1" t="n"/>
+      <c r="R51" s="1" t="inlineStr">
+        <is>
+          <t>烛煌</t>
+        </is>
+      </c>
+      <c r="S51" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T51" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U51" s="1" t="n"/>
     </row>
     <row r="52">
       <c r="F52" s="1" t="inlineStr">
@@ -6170,7 +6234,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.69), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.97), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6206,7 +6270,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.11)</t>
+          <t>maa://32532 (92.31)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6260,7 +6324,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (55.17)</t>
+          <t>*maa://37964 (56.67)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>
@@ -6278,7 +6342,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (82.41), maa://31270 (95.04)</t>
+          <t>maa://27746 (82.57), maa://31270 (95.16)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6296,7 +6360,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (64.71)</t>
+          <t>*maa://40438 (65.38)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>
@@ -6332,7 +6396,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (97.06), maa://43903 (100.0)</t>
+          <t>maa://42981 (97.14), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>
@@ -6368,7 +6432,7 @@
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>maa://44405 (91.67)</t>
+          <t>maa://44405 (88.0)</t>
         </is>
       </c>
       <c r="I64" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#146)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.39), maa://25390 (96.06), maa://36681 (87.34)</t>
+          <t>maa://24702 (94.39), maa://25390 (96.09), maa://36681 (87.34)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.33), *maa://30515 (69.61), *maa://34787 (72.97), ***maa://20792 (11.93), maa://39402 (90.2), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.33), *maa://30515 (69.61), *maa://34787 (72.97), ***maa://20792 (11.93), maa://39402 (90.38), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.27), maa://26254 (96.3)</t>
+          <t>maa://21249 (94.3), maa://26254 (96.3)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -848,12 +848,12 @@
       </c>
       <c r="S3" s="1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.38), **maa://20790 (44.12), ***maa://37170 (17.46)</t>
+          <t>maa://24617 (89.38), **maa://20790 (44.12), ***maa://37170 (17.19), maa://45854 (100.0)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (93.85)</t>
+          <t>maa://24390 (94.03)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.59), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.63), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.3), maa://27295 (84.62), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
+          <t>maa://32509 (97.3), maa://27295 (84.85), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.31), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (87.18)</t>
+          <t>**maa://32495 (48.31), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (85.37)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (83.93), maa://22744 (84.0)</t>
+          <t>maa://21245 (84.0), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="P6" s="2" t="inlineStr">
         <is>
-          <t>maa://31836 (92.0), maa://30381 (92.31)</t>
+          <t>maa://31836 (92.31), maa://30381 (92.31)</t>
         </is>
       </c>
       <c r="Q6" s="1" t="n"/>
@@ -1280,7 +1280,7 @@
       </c>
       <c r="AB6" s="2" t="inlineStr">
         <is>
-          <t>maa://22739 (92.86)</t>
+          <t>maa://22739 (92.98)</t>
         </is>
       </c>
       <c r="AC6" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.01.25 08:45:24</t>
+          <t>更新日期：2025.01.26 08:43:45</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (96.03)</t>
+          <t>maa://21411 (96.06)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="AB8" s="2" t="inlineStr">
         <is>
-          <t>maa://25389 (87.5)</t>
+          <t>maa://25389 (87.88)</t>
         </is>
       </c>
       <c r="AC8" s="1" t="n"/>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="AF8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24479 (77.65), *maa://21990 (51.85)</t>
+          <t>*maa://24479 (77.91), *maa://21990 (51.85)</t>
         </is>
       </c>
       <c r="AG8" s="1" t="n"/>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>maa://22765 (92.31), *maa://21915 (68.0)</t>
+          <t>maa://22765 (92.31), *maa://21915 (69.23)</t>
         </is>
       </c>
       <c r="E9" s="1" t="n"/>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (82.11)</t>
+          <t>maa://22736 (82.29)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1643,7 +1643,7 @@
       </c>
       <c r="T9" s="2" t="inlineStr">
         <is>
-          <t>**maa://22866 (30.19), maa://26222 (97.87)</t>
+          <t>**maa://22866 (30.19), maa://26222 (97.92)</t>
         </is>
       </c>
       <c r="U9" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.62)</t>
+          <t>maa://26223 (97.67)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (90.09), *maa://22865 (51.92)</t>
+          <t>maa://26206 (90.18), *maa://22865 (51.92)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.02), **maa://32237 (40.91), ***maa://34206 (20.83), ***maa://39951 (15.91), ***maa://39243 (28.57), **maa://45271 (50.0)</t>
+          <t>***maa://25695 (19.02), **maa://32237 (40.91), ***maa://34206 (20.83), ***maa://39951 (15.56), ***maa://39243 (28.57), *maa://45271 (53.33)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.22), maa://22755 (87.72), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.24), maa://22755 (87.72), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1784,12 +1784,12 @@
       </c>
       <c r="W10" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.7), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.7), maa://22726 (100.0), maa://45828 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (55.29), *maa://22733 (60.61), maa://22761 (100.0)</t>
+          <t>*maa://25021 (54.65), *maa://22733 (60.61), maa://22761 (100.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1951,7 +1951,7 @@
       </c>
       <c r="AF11" s="2" t="inlineStr">
         <is>
-          <t>maa://31203 (95.65)</t>
+          <t>maa://31203 (95.83)</t>
         </is>
       </c>
       <c r="AG11" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.12), *maa://21485 (76.81), maa://37962 (87.88)</t>
+          <t>maa://22753 (91.18), *maa://21485 (76.81), maa://37962 (87.88)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.44), maa://36677 (92.59), maa://39872 (90.48)</t>
+          <t>maa://23669 (95.44), maa://36677 (92.59), maa://39872 (90.91)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (77.94), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (78.1), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.94), maa://36673 (92.96), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.82), maa://36673 (92.96), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (92.31), *maa://22583 (74.24), *maa://22500 (57.78)</t>
+          <t>maa://22676 (92.37), *maa://22583 (74.24), *maa://22500 (57.78)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>maa://34957 (81.16), *maa://22768 (51.61)</t>
+          <t>maa://34957 (81.43), *maa://22768 (51.61)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>maa://30764 (88.46)</t>
+          <t>maa://30764 (88.68)</t>
         </is>
       </c>
       <c r="E14" s="1" t="n"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.67), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.68), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.39), maa://22734 (84.03), *maa://30808 (63.64), **maa://36048 (39.62), maa://45058 (100.0)</t>
+          <t>*maa://22743 (77.39), maa://22734 (84.03), *maa://30808 (64.18), **maa://36048 (40.74), maa://45058 (100.0)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.39), *maa://36666 (78.89), *maa://22766 (69.91)</t>
+          <t>maa://21364 (81.45), *maa://36666 (78.89), *maa://22766 (69.91)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.35), maa://36679 (93.48), maa://37650 (96.97)</t>
+          <t>maa://21441 (96.35), maa://36679 (93.62), maa://37650 (96.97)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (97.89), maa://28051 (96.0)</t>
+          <t>maa://28501 (97.92), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.65)</t>
+          <t>maa://26228 (95.7)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.54), maa://39599 (85.71)</t>
+          <t>maa://22430 (88.6), maa://39599 (84.44)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.2)</t>
+          <t>maa://24570 (97.21)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (64.37), *maa://36668 (57.5)</t>
+          <t>*maa://30709 (64.54), *maa://36668 (57.5)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (86.07)</t>
+          <t>maa://41331 (86.29)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="T20" s="2" t="inlineStr">
         <is>
-          <t>maa://29113 (85.19)</t>
+          <t>maa://29113 (85.71)</t>
         </is>
       </c>
       <c r="U20" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.29), *maa://22432 (77.78)</t>
+          <t>maa://22524 (94.29), *maa://22432 (78.46)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (83.64), *maa://22751 (71.64)</t>
+          <t>maa://27127 (82.14), *maa://22751 (71.64)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.53), *maa://37649 (67.86)</t>
+          <t>maa://21282 (98.54), *maa://37649 (67.86)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (94.97), maa://39875 (93.94)</t>
+          <t>maa://39756 (95.0), maa://39875 (93.94)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3495,7 +3495,7 @@
       </c>
       <c r="AB23" s="2" t="inlineStr">
         <is>
-          <t>maa://29652 (97.56)</t>
+          <t>maa://29652 (97.62)</t>
         </is>
       </c>
       <c r="AC23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.05)</t>
+          <t>*maa://24368 (78.11)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (85.54), maa://23504 (93.3), **maa://22892 (40.14), *maa://25141 (76.74), *maa://36663 (77.46), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (85.19), maa://23504 (93.09), **maa://22892 (40.14), *maa://25141 (76.74), *maa://36663 (77.78), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3636,12 +3636,12 @@
       </c>
       <c r="AE24" s="1" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.71), maa://36672 (81.82), maa://29910 (92.86), **maa://21440 (34.55)</t>
+          <t>maa://22523 (85.71), maa://36672 (80.36), maa://29910 (92.86), **maa://21440 (34.55), maa://45831 (100.0)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3691,7 +3691,7 @@
       </c>
       <c r="L25" s="2" t="inlineStr">
         <is>
-          <t>maa://24378 (87.18)</t>
+          <t>maa://24378 (87.8)</t>
         </is>
       </c>
       <c r="M25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (86.79), *maa://24516 (79.78), maa://26001 (87.5)</t>
+          <t>maa://31215 (86.92), *maa://24516 (80.0), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (94.19)</t>
+          <t>maa://42235 (94.25)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (48.0), *maa://39601 (76.47), maa://34494 (96.97), **maa://36665 (44.44)</t>
+          <t>**maa://21283 (48.0), *maa://39601 (76.47), maa://34494 (97.06), **maa://36665 (44.44)</t>
         </is>
       </c>
       <c r="I27" s="1" t="n"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (78.57)</t>
+          <t>*maa://30624 (77.19)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.91), maa://25725 (83.72)</t>
+          <t>maa://24465 (90.93), maa://25725 (83.72)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4081,7 +4081,7 @@
       </c>
       <c r="L28" s="2" t="inlineStr">
         <is>
-          <t>*maa://30770 (80.0)</t>
+          <t>maa://30770 (80.43)</t>
         </is>
       </c>
       <c r="M28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.6), maa://41749 (91.3), ***maa://39723 (14.29)</t>
+          <t>maa://39929 (90.68), maa://41749 (91.3), ***maa://39723 (14.29)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.66), *maa://36701 (65.52)</t>
+          <t>maa://36660 (92.38), *maa://36701 (65.52)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>*maa://25175 (67.35)</t>
+          <t>*maa://25175 (66.0)</t>
         </is>
       </c>
       <c r="I29" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.15), *maa://28440 (78.64), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.17), *maa://28440 (78.85), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.95), maa://42865 (80.95), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.95), maa://42865 (82.22), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4400,12 +4400,12 @@
       </c>
       <c r="AA30" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.15), maa://45045 (100.0)</t>
+          <t>maa://42979 (96.21), maa://45045 (100.0), maa://45822 (100.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.45), maa://36258 (84.76), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.48), maa://36258 (84.76), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.45), maa://36667 (98.55), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.45), maa://36667 (98.57), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (95.96), maa://41108 (88.0), maa://41238 (96.81), maa://45523 (100.0)</t>
+          <t>maa://42859 (96.0), maa://41108 (88.0), maa://41238 (96.88), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4747,7 +4747,7 @@
       </c>
       <c r="P33" s="2" t="inlineStr">
         <is>
-          <t>maa://21956 (80.14), *maa://22730 (79.31)</t>
+          <t>maa://21956 (80.28), *maa://22730 (79.31)</t>
         </is>
       </c>
       <c r="Q33" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (97.12)</t>
+          <t>maa://41296 (95.77)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5203,7 +5203,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (88.94), *maa://21239 (66.67)</t>
+          <t>maa://21280 (89.0), *maa://21239 (66.67)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="P38" s="2" t="inlineStr">
         <is>
-          <t>*maa://24383 (68.69)</t>
+          <t>*maa://24383 (69.0)</t>
         </is>
       </c>
       <c r="Q38" s="1" t="n"/>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (88.04), maa://25199 (84.82), maa://30434 (90.28), ***maa://25036 (16.0), *maa://45059 (57.14), *maa://44165 (66.67)</t>
+          <t>maa://36670 (88.04), maa://25199 (84.82), maa://30434 (90.41), ***maa://25036 (16.0), *maa://45059 (66.67), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5405,7 +5405,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.97)</t>
+          <t>maa://24709 (92.09)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5416,12 +5416,12 @@
       </c>
       <c r="S39" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>*maa://45788 (70.0)</t>
+          <t>*maa://45788 (76.0), *maa://45790 (80.0)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5713,7 +5713,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (92.81), maa://21284 (84.78)</t>
+          <t>maa://22525 (92.81), maa://21284 (85.11)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5782,7 +5782,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.91), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.92), maa://27728 (96.0)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5941,7 +5941,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.34), maa://29661 (97.24), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.35), maa://29661 (97.24), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6234,7 +6234,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.97), **maa://32434 (34.78)</t>
+          <t>maa://32534 (94.01), **maa://32434 (34.78)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6306,7 +6306,7 @@
       </c>
       <c r="H57" s="2" t="inlineStr">
         <is>
-          <t>maa://25176 (98.28)</t>
+          <t>maa://25176 (98.31)</t>
         </is>
       </c>
       <c r="I57" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#147)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.39), maa://25390 (96.09), maa://36681 (87.34)</t>
+          <t>maa://24702 (94.43), maa://25390 (96.09), maa://36681 (87.34)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.33), *maa://30515 (69.61), *maa://34787 (72.97), ***maa://20792 (11.93), maa://39402 (90.38), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.6), *maa://30515 (69.9), *maa://34787 (72.97), ***maa://20792 (11.93), maa://39402 (90.57), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.3), *maa://20791 (63.01)</t>
+          <t>maa://22742 (91.36), *maa://20791 (63.01)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.41), maa://36684 (95.0), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.41), maa://36684 (95.05), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.45), ***maa://21730 (23.94), ***maa://39501 (21.74), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.52), ***maa://21730 (23.94), ***maa://39501 (21.74), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://36987 (95.83), maa://40192 (100.0), maa://39849 (88.89)</t>
+          <t>maa://36987 (95.92), maa://40192 (100.0), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.26), maa://20276 (85.71), *maa://22749 (72.73)</t>
+          <t>*maa://22880 (65.26), maa://20276 (85.8), *maa://22749 (72.73)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.63), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.67), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.3), maa://27295 (84.85), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
+          <t>maa://32509 (97.3), maa://27295 (85.07), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.31), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (85.37)</t>
+          <t>**maa://32495 (48.31), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (85.71)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (63.83), ***maa://26209 (13.04), *maa://39394 (69.57)</t>
+          <t>*maa://30062 (62.5), ***maa://26209 (13.04), *maa://39394 (69.57)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.0), maa://22744 (84.0)</t>
+          <t>maa://21245 (84.07), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="AB5" s="2" t="inlineStr">
         <is>
-          <t>*maa://29863 (68.57), ***maa://22752 (12.5), **maa://26013 (37.5)</t>
+          <t>*maa://29863 (66.67), ***maa://22752 (12.5), **maa://26013 (37.5)</t>
         </is>
       </c>
       <c r="AC5" s="1" t="n"/>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>maa://24839 (98.95)</t>
+          <t>maa://24839 (98.96)</t>
         </is>
       </c>
       <c r="M6" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (91.67), maa://24957 (97.73)</t>
+          <t>maa://28624 (91.75), maa://24957 (97.73)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="P7" s="2" t="inlineStr">
         <is>
-          <t>maa://22750 (91.11)</t>
+          <t>maa://22750 (91.3)</t>
         </is>
       </c>
       <c r="Q7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.3), *maa://22758 (75.0)</t>
+          <t>maa://22399 (95.3), *maa://22758 (75.38)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (68.29), *maa://36671 (68.0), *maa://42530 (60.0), maa://45272 (100.0)</t>
+          <t>*maa://26191 (68.67), *maa://36671 (68.0), *maa://42530 (60.0), maa://45272 (100.0)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.01.26 08:43:45</t>
+          <t>更新日期：2025.01.27 13:17:55</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (86.36), ***maa://22740 (5.77), **maa://39938 (44.44), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (95.24)</t>
+          <t>maa://28711 (86.49), ***maa://22740 (5.77), **maa://39938 (44.44), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (95.24)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.02), **maa://32237 (40.91), ***maa://34206 (20.83), ***maa://39951 (15.56), ***maa://39243 (28.57), *maa://45271 (53.33)</t>
+          <t>***maa://25695 (19.02), **maa://32237 (40.91), ***maa://34206 (20.83), ***maa://39951 (15.56), ***maa://39243 (28.57), *maa://45271 (56.25)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (88.66)</t>
+          <t>maa://21287 (88.78)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.86), maa://22501 (97.47), *maa://45521 (60.0)</t>
+          <t>maa://22747 (92.86), maa://22501 (97.5), *maa://45521 (60.0)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.84)</t>
+          <t>maa://36713 (97.85)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.18), *maa://21485 (76.81), maa://37962 (87.88)</t>
+          <t>maa://22753 (91.23), *maa://21485 (76.81), maa://37962 (87.88)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (92.37), *maa://22583 (74.24), *maa://22500 (57.78)</t>
+          <t>maa://22676 (92.44), *maa://22583 (74.24), *maa://22500 (57.78)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>maa://30764 (88.68)</t>
+          <t>maa://30764 (88.89)</t>
         </is>
       </c>
       <c r="E14" s="1" t="n"/>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="AB14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (97.01)</t>
+          <t>maa://22764 (97.06)</t>
         </is>
       </c>
       <c r="AC14" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (87.86), maa://21478 (91.67)</t>
+          <t>maa://24304 (87.92), maa://21478 (91.67)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2439,7 +2439,7 @@
       </c>
       <c r="X15" s="2" t="inlineStr">
         <is>
-          <t>*maa://38786 (80.0)</t>
+          <t>maa://38786 (83.33)</t>
         </is>
       </c>
       <c r="Y15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.45), *maa://36666 (78.89), *maa://22766 (69.91)</t>
+          <t>maa://21364 (81.5), *maa://36666 (79.12), *maa://22766 (69.91)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.35), maa://36679 (93.62), maa://37650 (96.97)</t>
+          <t>maa://21441 (96.35), maa://36679 (93.62), maa://37650 (97.06)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.21)</t>
+          <t>maa://24570 (97.22)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (89.47)</t>
+          <t>maa://24421 (89.11)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (99.1)</t>
+          <t>maa://24386 (99.12)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (64.54), *maa://36668 (57.5)</t>
+          <t>*maa://30709 (64.62), *maa://36668 (57.5)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -2991,7 +2991,7 @@
       </c>
       <c r="AF19" s="2" t="inlineStr">
         <is>
-          <t>*maa://21663 (62.32)</t>
+          <t>*maa://21663 (62.86)</t>
         </is>
       </c>
       <c r="AG19" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (86.29)</t>
+          <t>maa://41331 (85.83)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (80.39), ***maa://23820 (29.31)</t>
+          <t>maa://21443 (80.44), ***maa://23820 (29.31)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.0), maa://39875 (93.94)</t>
+          <t>maa://39756 (95.05), maa://39875 (94.03)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.71), *maa://29748 (75.78), ***maa://29785 (16.42), *maa://37566 (71.88)</t>
+          <t>maa://30587 (91.71), *maa://29748 (75.78), ***maa://29785 (16.42), *maa://37566 (72.73)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="X23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (64.79)</t>
+          <t>*maa://28503 (65.28)</t>
         </is>
       </c>
       <c r="Y23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.11)</t>
+          <t>*maa://24368 (77.9)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (85.19), maa://23504 (93.09), **maa://22892 (40.14), *maa://25141 (76.74), *maa://36663 (77.78), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (85.37), maa://23504 (93.09), **maa://22892 (40.14), *maa://25141 (76.74), *maa://36663 (77.78), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.0)</t>
+          <t>maa://29753 (95.02)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (74.19), *maa://25311 (73.53), ***maa://22725 (4.84), **maa://45047 (50.0)</t>
+          <t>*maa://29063 (74.36), *maa://25311 (73.53), ***maa://22725 (4.84), **maa://45047 (50.0)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (94.25)</t>
+          <t>maa://42235 (94.38)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (77.19)</t>
+          <t>*maa://30624 (77.59)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.93), maa://25725 (83.72)</t>
+          <t>maa://24465 (90.96), maa://25725 (83.72)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>maa://23263 (95.1), *maa://29765 (62.96)</t>
+          <t>maa://23263 (95.15), *maa://29765 (62.96)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.68), maa://41749 (91.3), ***maa://39723 (14.29)</t>
+          <t>maa://39929 (90.73), maa://41749 (91.43), ***maa://39723 (14.29)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.38), *maa://36701 (65.52)</t>
+          <t>maa://36660 (92.42), *maa://36701 (65.52)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.95), maa://42865 (82.22), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.95), maa://42865 (80.43), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.21), maa://45045 (100.0), maa://45822 (100.0)</t>
+          <t>maa://42979 (96.3), maa://45045 (100.0), maa://45822 (100.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.48), maa://36258 (84.76), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.48), maa://36258 (84.91), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.45), maa://36667 (98.57), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.47), maa://36667 (98.59), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -5352,7 +5352,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.93)</t>
+          <t>maa://36697 (87.0)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (88.04), maa://25199 (84.82), maa://30434 (90.41), ***maa://25036 (16.0), *maa://45059 (66.67), *maa://44165 (66.67)</t>
+          <t>maa://36670 (88.04), maa://25199 (84.82), maa://30434 (90.54), ***maa://25036 (16.0), *maa://45059 (66.67), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5405,7 +5405,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (92.09)</t>
+          <t>maa://24709 (92.2)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>*maa://45788 (76.0), *maa://45790 (80.0)</t>
+          <t>*maa://45788 (78.12), maa://45790 (83.33)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5490,7 +5490,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.71), maa://21386 (95.74), maa://36664 (90.91), maa://45550 (100.0)</t>
+          <t>maa://23278 (95.74), maa://21386 (95.74), maa://36664 (90.91), maa://45550 (100.0)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5835,7 +5835,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.95), maa://30807 (95.52), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (86.67)</t>
+          <t>maa://21229 (84.95), maa://30807 (95.52), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (87.5)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5888,7 +5888,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.64), maa://43901 (92.86)</t>
+          <t>maa://35931 (92.64), maa://43901 (93.33)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6270,7 +6270,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.31)</t>
+          <t>maa://32532 (92.34)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6324,7 +6324,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (56.67)</t>
+          <t>*maa://37964 (54.84)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#148)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.43), maa://25390 (96.09), maa://36681 (87.34)</t>
+          <t>maa://24702 (94.43), maa://25390 (96.12), maa://36681 (87.34)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.6), *maa://30515 (69.9), *maa://34787 (72.97), ***maa://20792 (11.93), maa://39402 (90.57), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.88), *maa://30515 (69.9), *maa://34787 (72.97), ***maa://20792 (11.93), maa://39402 (90.74), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.41), maa://36684 (95.05), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.41), maa://36684 (95.1), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.52), ***maa://21730 (23.94), ***maa://39501 (21.74), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.66), ***maa://21730 (25.0), ***maa://39501 (20.83), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.26), maa://20276 (85.8), *maa://22749 (72.73)</t>
+          <t>*maa://22880 (65.26), maa://20276 (86.05), *maa://22749 (72.73)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.3), maa://26254 (96.3)</t>
+          <t>maa://21249 (94.32), maa://26254 (96.3)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.38), **maa://20790 (44.12), ***maa://37170 (17.19), maa://45854 (100.0)</t>
+          <t>maa://24617 (89.47), **maa://20790 (44.12), ***maa://37170 (17.19), maa://45854 (100.0)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.54), maa://27484 (96.36), maa://27480 (82.86)</t>
+          <t>maa://27396 (84.28), maa://27484 (96.43), maa://27480 (82.86)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (94.03)</t>
+          <t>maa://24390 (94.12)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.67), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.71), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.3), maa://27295 (85.07), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
+          <t>maa://32509 (97.32), maa://27295 (85.07), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.31), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (85.71)</t>
+          <t>**maa://32495 (48.51), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (85.71)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (62.5), ***maa://26209 (13.04), *maa://39394 (69.57)</t>
+          <t>*maa://30062 (63.27), ***maa://26209 (13.04), *maa://39394 (69.57)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.07), maa://22744 (84.0)</t>
+          <t>maa://21245 (84.14), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>maa://24370 (96.55)</t>
+          <t>maa://24370 (96.61)</t>
         </is>
       </c>
       <c r="I6" s="1" t="n"/>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>maa://24839 (98.96)</t>
+          <t>maa://24839 (98.97)</t>
         </is>
       </c>
       <c r="M6" s="1" t="n"/>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>*maa://22763 (64.52)</t>
+          <t>*maa://22763 (65.62)</t>
         </is>
       </c>
       <c r="I7" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (91.75), maa://24957 (97.73)</t>
+          <t>maa://28624 (92.0), maa://24957 (97.73)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="P7" s="2" t="inlineStr">
         <is>
-          <t>maa://22750 (91.3)</t>
+          <t>maa://22750 (91.49)</t>
         </is>
       </c>
       <c r="Q7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.01.27 13:17:55</t>
+          <t>更新日期：2025.01.28 13:17:19</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (83.49), *maa://21916 (61.9), maa://23252 (92.54), maa://37496 (96.67), **maa://22759 (45.45)</t>
+          <t>maa://32931 (83.04), *maa://21916 (60.94), maa://23252 (91.18), maa://37496 (96.77), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (96.06)</t>
+          <t>maa://21411 (96.08)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="AB8" s="2" t="inlineStr">
         <is>
-          <t>maa://25389 (87.88)</t>
+          <t>maa://25389 (88.57)</t>
         </is>
       </c>
       <c r="AC8" s="1" t="n"/>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>maa://22765 (92.31), *maa://21915 (69.23)</t>
+          <t>maa://22765 (92.39), *maa://21915 (69.23)</t>
         </is>
       </c>
       <c r="E9" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.67)</t>
+          <t>maa://26223 (97.69)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (86.49), ***maa://22740 (5.77), **maa://39938 (44.44), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (95.24)</t>
+          <t>maa://28711 (86.61), ***maa://22740 (5.77), **maa://39938 (42.86), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (95.24)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (90.18), *maa://22865 (51.92)</t>
+          <t>maa://26206 (90.43), *maa://22865 (51.92)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.02), **maa://32237 (40.91), ***maa://34206 (20.83), ***maa://39951 (15.56), ***maa://39243 (28.57), *maa://45271 (56.25)</t>
+          <t>***maa://25695 (18.82), **maa://32237 (41.3), ***maa://34206 (20.0), ***maa://39951 (15.22), ***maa://39243 (28.57), *maa://45271 (52.63)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.24), maa://22755 (87.72), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.32), maa://22755 (87.83), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.7), maa://22726 (100.0), maa://45828 (100.0)</t>
+          <t>maa://22301 (97.72), maa://22726 (100.0), maa://45828 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (54.65), *maa://22733 (60.61), maa://22761 (100.0)</t>
+          <t>*maa://25021 (53.41), *maa://22733 (60.0), **maa://22761 (50.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.86), maa://22501 (97.5), *maa://45521 (60.0)</t>
+          <t>maa://22747 (92.9), maa://22501 (97.56), *maa://45521 (60.0)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.85)</t>
+          <t>maa://36713 (97.87)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.23), *maa://21485 (76.81), maa://37962 (87.88)</t>
+          <t>maa://22753 (91.28), *maa://21485 (76.81), maa://37962 (87.88)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.44), maa://36677 (92.59), maa://39872 (90.91)</t>
+          <t>maa://23669 (95.47), maa://36677 (92.59), maa://39872 (90.91)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.1), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (78.26), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.82), maa://36673 (92.96), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.87), maa://36673 (92.96), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (75.0), **maa://22728 (47.73)</t>
+          <t>*maa://21248 (74.03), **maa://22728 (47.73)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (92.44), *maa://22583 (74.24), *maa://22500 (57.78)</t>
+          <t>maa://22676 (92.56), *maa://22583 (74.24), *maa://22500 (57.78)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (32.62), maa://39883 (91.94), *maa://39885 (55.56)</t>
+          <t>**maa://22737 (33.57), maa://39883 (91.94), *maa://39885 (55.56)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.58), maa://21288 (96.3), maa://39841 (95.65), maa://36682 (97.44)</t>
+          <t>maa://26245 (96.62), maa://21288 (96.3), maa://39841 (95.7), maa://36682 (97.44)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="T14" s="2" t="inlineStr">
         <is>
-          <t>maa://22521 (93.94), maa://42751 (100.0)</t>
+          <t>maa://22521 (94.0), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.39), maa://22734 (84.03), *maa://30808 (64.18), **maa://36048 (40.74), maa://45058 (100.0)</t>
+          <t>*maa://22743 (77.61), maa://22734 (84.03), *maa://30808 (64.18), **maa://36048 (42.86), maa://45058 (100.0)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (87.92), maa://21478 (91.67)</t>
+          <t>maa://24304 (88.04), maa://21478 (91.67)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (90.51), *maa://22727 (70.0)</t>
+          <t>maa://24762 (90.57), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.5), *maa://36666 (79.12), *maa://22766 (69.91)</t>
+          <t>maa://21364 (81.37), *maa://36666 (78.26), *maa://22766 (68.7)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.35), maa://36679 (93.62), maa://37650 (97.06)</t>
+          <t>maa://21441 (96.38), maa://36679 (93.62), maa://37650 (97.06)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.77), *maa://28648 (68.75), maa://36674 (82.22)</t>
+          <t>maa://22729 (94.81), *maa://28648 (68.75), maa://36674 (82.22)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (97.92), maa://28051 (96.0)</t>
+          <t>maa://28501 (97.96), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.7)</t>
+          <t>maa://26228 (95.79)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (65.38), maa://27755 (92.94)</t>
+          <t>*maa://23911 (64.76), maa://27755 (92.94)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.6), maa://39599 (84.44)</t>
+          <t>maa://22430 (88.66), maa://39599 (84.44)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.22)</t>
+          <t>maa://24570 (97.24)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (89.11)</t>
+          <t>maa://24421 (89.16)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (89.33), *maa://22732 (51.16)</t>
+          <t>maa://22466 (89.4), *maa://22732 (51.16)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2845,7 +2845,7 @@
       </c>
       <c r="AB18" s="2" t="inlineStr">
         <is>
-          <t>maa://24393 (97.67)</t>
+          <t>maa://24393 (97.78)</t>
         </is>
       </c>
       <c r="AC18" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (64.62), *maa://36668 (57.5)</t>
+          <t>*maa://30709 (64.71), *maa://36668 (57.5)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (89.68), maa://25198 (93.4), *maa://20795 (51.56), maa://36680 (93.75)</t>
+          <t>maa://21432 (89.87), maa://25198 (93.4), *maa://20795 (51.56), maa://36680 (93.75)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (89.61)</t>
+          <t>maa://22864 (89.74)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.83)</t>
+          <t>maa://41331 (86.36)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3155,7 +3155,7 @@
       </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>maa://24372 (96.84)</t>
+          <t>maa://24372 (96.88)</t>
         </is>
       </c>
       <c r="I21" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (80.44), ***maa://23820 (29.31)</t>
+          <t>maa://21443 (80.6), ***maa://23820 (29.31)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.29), *maa://22432 (78.46)</t>
+          <t>maa://22524 (94.31), *maa://22432 (78.46)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>maa://25236 (96.47), **maa://21678 (48.94), **maa://22735 (42.86)</t>
+          <t>maa://25236 (96.59), **maa://21678 (48.94), **maa://22735 (42.86)</t>
         </is>
       </c>
       <c r="I22" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (82.14), *maa://22751 (71.64)</t>
+          <t>maa://27127 (82.3), *maa://22751 (71.64)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.54), *maa://37649 (67.86)</t>
+          <t>maa://21282 (98.55), *maa://37649 (67.86)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.05), maa://39875 (94.03)</t>
+          <t>maa://39756 (95.11), maa://39875 (94.12)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.71), *maa://29748 (75.78), ***maa://29785 (16.42), *maa://37566 (72.73)</t>
+          <t>maa://30587 (91.75), *maa://29748 (75.78), ***maa://29785 (16.42), *maa://37566 (73.53)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (85.37), maa://23504 (93.09), **maa://22892 (40.14), *maa://25141 (76.74), *maa://36663 (77.78), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (85.02), maa://23504 (93.14), **maa://22892 (40.14), *maa://25141 (76.74), *maa://36663 (78.08), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.71), maa://36672 (80.36), maa://29910 (92.86), **maa://21440 (34.55), maa://45831 (100.0)</t>
+          <t>maa://22523 (85.79), maa://36672 (80.36), maa://29910 (92.86), **maa://21440 (34.55), maa://45831 (100.0)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.02)</t>
+          <t>maa://29753 (95.04)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (74.36), *maa://25311 (73.53), ***maa://22725 (4.84), **maa://45047 (50.0)</t>
+          <t>*maa://29063 (74.52), *maa://25311 (73.53), ***maa://22725 (4.84), **maa://45047 (50.0)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.27), maa://24621 (96.69), maa://36676 (96.88), maa://22771 (85.71), **maa://37772 (50.0)</t>
+          <t>maa://20108 (96.3), maa://24621 (96.72), maa://36676 (96.88), maa://22771 (85.71), **maa://37772 (50.0)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (91.67)</t>
+          <t>maa://24913 (91.76)</t>
         </is>
       </c>
       <c r="I26" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (94.38)</t>
+          <t>maa://42235 (94.44)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (48.0), *maa://39601 (76.47), maa://34494 (97.06), **maa://36665 (44.44)</t>
+          <t>**maa://21283 (47.37), *maa://39601 (76.47), maa://34494 (97.14), **maa://36665 (44.44)</t>
         </is>
       </c>
       <c r="I27" s="1" t="n"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (77.59)</t>
+          <t>*maa://30624 (77.97)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4031,7 +4031,7 @@
       </c>
       <c r="AF27" s="2" t="inlineStr">
         <is>
-          <t>maa://24023 (97.1)</t>
+          <t>maa://24023 (97.18)</t>
         </is>
       </c>
       <c r="AG27" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.96), maa://25725 (83.72)</t>
+          <t>maa://24465 (90.98), maa://25725 (83.72)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.73), maa://41749 (91.43), ***maa://39723 (14.29)</t>
+          <t>maa://39929 (90.53), maa://41749 (91.89), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.42), *maa://36701 (65.52)</t>
+          <t>maa://36660 (92.47), *maa://36701 (65.52)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4179,7 +4179,7 @@
       </c>
       <c r="D29" s="2" t="inlineStr">
         <is>
-          <t>maa://31694 (98.08)</t>
+          <t>maa://31694 (98.11)</t>
         </is>
       </c>
       <c r="E29" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.17), *maa://28440 (78.85), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.19), *maa://28440 (79.05), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.95), maa://42865 (80.43), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.77), maa://42865 (81.25), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.3), maa://45045 (100.0), maa://45822 (100.0)</t>
+          <t>maa://42979 (96.32), maa://45045 (100.0), maa://45822 (100.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.48), maa://36258 (84.91), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.5), maa://36258 (85.19), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.47), maa://36667 (98.59), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.49), maa://36667 (98.59), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4601,7 +4601,7 @@
       </c>
       <c r="L32" s="2" t="inlineStr">
         <is>
-          <t>maa://28065 (95.0)</t>
+          <t>maa://28065 (95.12)</t>
         </is>
       </c>
       <c r="M32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.0), maa://41108 (88.0), maa://41238 (96.88), maa://45523 (100.0)</t>
+          <t>maa://42859 (96.08), maa://41108 (88.0), maa://41238 (96.97), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4747,7 +4747,7 @@
       </c>
       <c r="P33" s="2" t="inlineStr">
         <is>
-          <t>maa://21956 (80.28), *maa://22730 (79.31)</t>
+          <t>maa://21956 (80.56), *maa://22730 (79.31)</t>
         </is>
       </c>
       <c r="Q33" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (95.77)</t>
+          <t>maa://41296 (95.83)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5203,7 +5203,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.0), *maa://21239 (66.67)</t>
+          <t>maa://21280 (89.1), *maa://21239 (66.67)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5219,7 +5219,7 @@
       </c>
       <c r="T37" s="2" t="inlineStr">
         <is>
-          <t>**maa://39354 (33.33)</t>
+          <t>**maa://39354 (40.0)</t>
         </is>
       </c>
       <c r="U37" s="1" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="P38" s="2" t="inlineStr">
         <is>
-          <t>*maa://24383 (69.0)</t>
+          <t>*maa://24383 (69.31)</t>
         </is>
       </c>
       <c r="Q38" s="1" t="n"/>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (88.04), maa://25199 (84.82), maa://30434 (90.54), ***maa://25036 (16.0), *maa://45059 (66.67), *maa://44165 (66.67)</t>
+          <t>maa://36670 (88.04), maa://25199 (84.82), maa://30434 (90.79), ***maa://25036 (16.0), *maa://45059 (72.73), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5405,7 +5405,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (92.2)</t>
+          <t>maa://24709 (92.31)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>*maa://45788 (78.12), maa://45790 (83.33)</t>
+          <t>*maa://45788 (77.78), maa://45790 (87.5)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5490,7 +5490,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.74), maa://21386 (95.74), maa://36664 (90.91), maa://45550 (100.0)</t>
+          <t>maa://23278 (95.75), maa://21386 (95.74), maa://36664 (90.91), maa://45550 (100.0)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5713,7 +5713,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (92.81), maa://21284 (85.11)</t>
+          <t>maa://22525 (92.91), maa://21284 (85.11)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5782,7 +5782,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.92), maa://27728 (96.0)</t>
+          <t>maa://29768 (97.93), maa://27728 (96.04)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5835,7 +5835,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.95), maa://30807 (95.52), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (87.5)</t>
+          <t>maa://21229 (84.49), maa://30807 (95.52), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (84.21)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5888,7 +5888,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.64), maa://43901 (93.33)</t>
+          <t>maa://35931 (92.72), maa://43901 (93.75)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5941,7 +5941,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.35), maa://29661 (97.24), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.37), maa://29661 (97.24), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6063,7 +6063,7 @@
       </c>
       <c r="P49" s="2" t="inlineStr">
         <is>
-          <t>*maa://39643 (68.0)</t>
+          <t>*maa://39643 (65.38)</t>
         </is>
       </c>
       <c r="Q49" s="1" t="n"/>
@@ -6234,7 +6234,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.01), **maa://32434 (34.78)</t>
+          <t>maa://32534 (93.73), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6270,7 +6270,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.34)</t>
+          <t>maa://32532 (92.39)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6342,7 +6342,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (82.57), maa://31270 (95.16)</t>
+          <t>maa://27746 (82.57), maa://31270 (95.2)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6360,7 +6360,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (65.38)</t>
+          <t>*maa://40438 (66.67)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#149)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.66), ***maa://21730 (25.0), ***maa://39501 (20.83), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.79), ***maa://21730 (25.0), ***maa://39501 (20.83), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.32), maa://26254 (96.3)</t>
+          <t>maa://21249 (94.32), maa://26254 (96.43)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.47), **maa://20790 (44.12), ***maa://37170 (17.19), maa://45854 (100.0)</t>
+          <t>maa://24617 (89.57), **maa://20790 (44.12), ***maa://37170 (17.19), maa://45854 (100.0)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.71), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.75), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.51), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (85.71)</t>
+          <t>**maa://32495 (48.51), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (86.05)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="P5" s="2" t="inlineStr">
         <is>
-          <t>maa://21919 (96.3), *maa://21281 (80.0)</t>
+          <t>maa://21919 (96.36), *maa://21281 (80.0)</t>
         </is>
       </c>
       <c r="Q5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (95.12)</t>
+          <t>maa://42407 (95.24)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="P6" s="2" t="inlineStr">
         <is>
-          <t>maa://31836 (92.31), maa://30381 (92.31)</t>
+          <t>maa://31836 (92.59), maa://30381 (92.31)</t>
         </is>
       </c>
       <c r="Q6" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.3), *maa://22758 (75.38)</t>
+          <t>maa://22399 (95.3), *maa://22758 (75.76)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (68.67), *maa://36671 (68.0), *maa://42530 (60.0), maa://45272 (100.0)</t>
+          <t>*maa://26191 (68.67), *maa://36671 (68.0), *maa://42530 (62.5), maa://45272 (100.0)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.01.28 13:17:19</t>
+          <t>更新日期：2025.01.30 13:18:46</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (83.04), *maa://21916 (60.94), maa://23252 (91.18), maa://37496 (96.77), **maa://22759 (45.45)</t>
+          <t>maa://32931 (83.33), *maa://21916 (60.94), maa://23252 (91.18), maa://37496 (96.77), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>maa://22765 (92.39), *maa://21915 (69.23)</t>
+          <t>maa://22765 (92.39), *maa://21915 (70.37)</t>
         </is>
       </c>
       <c r="E9" s="1" t="n"/>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (82.29)</t>
+          <t>maa://22736 (82.47)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.69)</t>
+          <t>maa://26223 (97.71)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.82), **maa://32237 (41.3), ***maa://34206 (20.0), ***maa://39951 (15.22), ***maa://39243 (28.57), *maa://45271 (52.63)</t>
+          <t>***maa://25695 (18.82), **maa://32237 (41.3), ***maa://34206 (20.0), ***maa://39951 (15.22), ***maa://39243 (28.57), *maa://45271 (55.0)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (90.36), maa://36669 (87.8), *maa://23264 (61.82)</t>
+          <t>maa://28977 (90.36), maa://36669 (88.1), *maa://23264 (61.82)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.72), maa://22726 (100.0), maa://45828 (100.0)</t>
+          <t>maa://22301 (97.74), maa://22726 (100.0), maa://45828 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.9), maa://22501 (97.56), *maa://45521 (60.0)</t>
+          <t>maa://22747 (92.9), maa://22501 (97.59), *maa://45521 (66.67)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.28), *maa://21485 (76.81), maa://37962 (87.88)</t>
+          <t>maa://22753 (91.28), *maa://21485 (76.26), maa://37962 (88.57)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.87), maa://36673 (92.96), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.89), maa://36673 (92.96), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (74.03), **maa://22728 (47.73)</t>
+          <t>*maa://21248 (73.71), **maa://22728 (47.73)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (92.56), *maa://22583 (74.24), *maa://22500 (57.78)</t>
+          <t>maa://22676 (92.62), *maa://22583 (74.24), *maa://22500 (58.7)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (33.57), maa://39883 (91.94), *maa://39885 (55.56)</t>
+          <t>**maa://22737 (33.57), maa://39883 (92.19), *maa://39885 (57.14)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.68), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.69), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="AB14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (97.06)</t>
+          <t>maa://22764 (97.1)</t>
         </is>
       </c>
       <c r="AC14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.61), maa://22734 (84.03), *maa://30808 (64.18), **maa://36048 (42.86), maa://45058 (100.0)</t>
+          <t>*maa://22743 (77.83), maa://22734 (84.03), *maa://30808 (64.18), **maa://36048 (42.86), maa://45058 (100.0)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.04), maa://21478 (91.67)</t>
+          <t>maa://24304 (88.1), maa://21478 (91.67)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.37), *maa://36666 (78.26), *maa://22766 (68.7)</t>
+          <t>maa://21364 (81.37), *maa://36666 (78.12), *maa://22766 (68.7)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.38), maa://36679 (93.62), maa://37650 (97.06)</t>
+          <t>maa://21441 (96.4), maa://36679 (93.75), maa://37650 (97.06)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.81), *maa://28648 (68.75), maa://36674 (82.22)</t>
+          <t>maa://22729 (94.81), *maa://28648 (68.75), maa://36674 (80.43)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (97.96), maa://28051 (96.0)</t>
+          <t>maa://28501 (97.98), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.79)</t>
+          <t>maa://26228 (95.83)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (64.76), maa://27755 (92.94)</t>
+          <t>*maa://23911 (64.76), maa://27755 (93.1)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.66), maa://39599 (84.44)</t>
+          <t>maa://22430 (88.66), maa://39599 (85.11)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (89.16)</t>
+          <t>maa://24421 (89.2)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (89.4), *maa://22732 (51.16)</t>
+          <t>maa://22466 (89.47), *maa://22732 (51.16)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2813,7 +2813,7 @@
       </c>
       <c r="T18" s="2" t="inlineStr">
         <is>
-          <t>maa://24385 (97.14)</t>
+          <t>maa://24385 (97.22)</t>
         </is>
       </c>
       <c r="U18" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (89.87), maa://25198 (93.4), *maa://20795 (51.56), maa://36680 (93.75)</t>
+          <t>maa://21432 (89.94), maa://25198 (93.4), *maa://20795 (51.56), maa://36680 (93.75)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (89.74)</t>
+          <t>maa://22864 (89.81)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (86.36)</t>
+          <t>maa://41331 (85.07)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (80.6), ***maa://23820 (29.31)</t>
+          <t>maa://21443 (80.71), ***maa://23820 (29.31)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.31), *maa://22432 (78.46)</t>
+          <t>maa://22524 (94.37), *maa://22432 (78.46)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (82.3), *maa://22751 (71.64)</t>
+          <t>maa://27127 (81.58), *maa://22751 (72.06)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.55), *maa://37649 (67.86)</t>
+          <t>maa://21282 (98.57), *maa://37649 (67.86)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.57), *maa://41753 (53.85)</t>
+          <t>***maa://28036 (28.57), *maa://41753 (57.14)</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.11), maa://39875 (94.12)</t>
+          <t>maa://39756 (95.19), maa://39875 (94.12)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (77.9)</t>
+          <t>*maa://24368 (77.96)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (85.02), maa://23504 (93.14), **maa://22892 (40.14), *maa://25141 (76.74), *maa://36663 (78.08), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (85.02), maa://23504 (93.15), **maa://22892 (40.14), *maa://25141 (76.74), *maa://36663 (78.08), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.79), maa://36672 (80.36), maa://29910 (92.86), **maa://21440 (34.55), maa://45831 (100.0)</t>
+          <t>maa://22523 (85.86), maa://36672 (80.36), maa://29910 (92.86), **maa://21440 (34.55), maa://45831 (100.0)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.04)</t>
+          <t>maa://29753 (95.06)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (74.52), *maa://25311 (73.53), ***maa://22725 (4.84), **maa://45047 (50.0)</t>
+          <t>*maa://29063 (74.52), *maa://25311 (73.53), ***maa://22725 (4.84), *maa://45047 (66.67)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3723,7 +3723,7 @@
       </c>
       <c r="T25" s="2" t="inlineStr">
         <is>
-          <t>maa://20109 (92.44), maa://22545 (100.0), maa://42915 (100.0)</t>
+          <t>maa://20109 (92.49), maa://22545 (100.0), maa://42915 (100.0)</t>
         </is>
       </c>
       <c r="U25" s="1" t="n"/>
@@ -3739,7 +3739,7 @@
       </c>
       <c r="X25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29890 (77.78)</t>
+          <t>*maa://29890 (78.26)</t>
         </is>
       </c>
       <c r="Y25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (86.92), *maa://24516 (80.0), maa://26001 (87.5)</t>
+          <t>maa://31215 (87.16), *maa://24516 (80.0), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.3), maa://24621 (96.72), maa://36676 (96.88), maa://22771 (85.71), **maa://37772 (50.0)</t>
+          <t>maa://20108 (96.3), maa://24621 (96.75), maa://36676 (96.88), maa://22771 (85.71), *maa://37772 (66.67)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (91.76)</t>
+          <t>maa://24913 (91.86)</t>
         </is>
       </c>
       <c r="I26" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (94.44)</t>
+          <t>maa://42235 (94.51)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>maa://23263 (95.15), *maa://29765 (62.96)</t>
+          <t>maa://23263 (95.19), *maa://29765 (63.41)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.53), maa://41749 (91.89), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.41), maa://41749 (91.89), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.47), *maa://36701 (65.52)</t>
+          <t>maa://36660 (92.51), *maa://36701 (65.52)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>*maa://25175 (66.0)</t>
+          <t>*maa://25175 (66.67)</t>
         </is>
       </c>
       <c r="I29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.77), maa://42865 (81.25), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.77), maa://42865 (82.0), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.32), maa://45045 (100.0), maa://45822 (100.0)</t>
+          <t>maa://42979 (96.43), maa://45822 (100.0), maa://45045 (100.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.5), maa://36258 (85.19), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.53), maa://36258 (85.32), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4601,7 +4601,7 @@
       </c>
       <c r="L32" s="2" t="inlineStr">
         <is>
-          <t>maa://28065 (95.12)</t>
+          <t>maa://28065 (95.24)</t>
         </is>
       </c>
       <c r="M32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.08), maa://41108 (88.0), maa://41238 (96.97), maa://45523 (100.0)</t>
+          <t>maa://42859 (96.12), maa://41108 (88.0), maa://41238 (96.97), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (93.65)</t>
+          <t>maa://24526 (93.28)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (95.83)</t>
+          <t>maa://41296 (95.92)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5203,7 +5203,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.1), *maa://21239 (66.67)</t>
+          <t>maa://21280 (89.2), *maa://21239 (66.67)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5219,7 +5219,7 @@
       </c>
       <c r="T37" s="2" t="inlineStr">
         <is>
-          <t>**maa://39354 (40.0)</t>
+          <t>**maa://39354 (45.45)</t>
         </is>
       </c>
       <c r="U37" s="1" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="P38" s="2" t="inlineStr">
         <is>
-          <t>*maa://24383 (69.31)</t>
+          <t>*maa://24383 (69.61)</t>
         </is>
       </c>
       <c r="Q38" s="1" t="n"/>
@@ -5352,7 +5352,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (87.0)</t>
+          <t>maa://36697 (87.06)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (88.04), maa://25199 (84.82), maa://30434 (90.79), ***maa://25036 (16.0), *maa://45059 (72.73), *maa://44165 (66.67)</t>
+          <t>maa://36670 (88.17), maa://25199 (84.82), maa://30434 (90.79), ***maa://25036 (16.0), *maa://45059 (75.0), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>*maa://45788 (77.78), maa://45790 (87.5)</t>
+          <t>maa://45788 (80.85), maa://45790 (88.89)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5490,7 +5490,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.75), maa://21386 (95.74), maa://36664 (90.91), maa://45550 (100.0)</t>
+          <t>maa://23278 (95.77), maa://21386 (95.74), maa://36664 (90.91), maa://45550 (100.0)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5782,7 +5782,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.93), maa://27728 (96.04)</t>
+          <t>maa://29768 (97.94), maa://27728 (96.04)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5835,7 +5835,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.49), maa://30807 (95.52), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (84.21)</t>
+          <t>maa://21229 (84.49), maa://30807 (95.59), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (84.21)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5888,7 +5888,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.72), maa://43901 (93.75)</t>
+          <t>maa://35931 (92.41), maa://43901 (88.24)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6234,7 +6234,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.73), **maa://32434 (33.33)</t>
+          <t>maa://32534 (93.75), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6270,7 +6270,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.39)</t>
+          <t>maa://32532 (92.45)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6360,7 +6360,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (66.67)</t>
+          <t>*maa://40438 (67.27)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>
@@ -6396,7 +6396,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (97.14), maa://43903 (100.0)</t>
+          <t>maa://42981 (97.22), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#150)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.36), *maa://20791 (63.01)</t>
+          <t>maa://22742 (91.41), *maa://20791 (63.01)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.57), **maa://20790 (44.12), ***maa://37170 (17.19), maa://45854 (100.0)</t>
+          <t>maa://24617 (89.57), **maa://20790 (43.48), ***maa://37170 (17.19), maa://45854 (100.0)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.28), maa://27484 (96.43), maa://27480 (82.86)</t>
+          <t>maa://27396 (84.28), maa://27484 (96.46), maa://27480 (82.86)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (94.12)</t>
+          <t>maa://24390 (94.2)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.51), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (86.05)</t>
+          <t>**maa://32495 (48.51), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (86.67)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (95.24)</t>
+          <t>maa://42407 (95.35)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="AF6" s="2" t="inlineStr">
         <is>
-          <t>*maa://33152 (60.87), ***maa://22770 (26.09)</t>
+          <t>*maa://33152 (59.57), ***maa://22770 (26.09)</t>
         </is>
       </c>
       <c r="AG6" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (68.67), *maa://36671 (68.0), *maa://42530 (62.5), maa://45272 (100.0)</t>
+          <t>*maa://26191 (69.05), *maa://36671 (68.0), *maa://42530 (62.5), maa://45272 (100.0)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.01.30 13:18:46</t>
+          <t>更新日期：2025.01.31 13:17:43</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1579,7 +1579,7 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>maa://22765 (92.39), *maa://21915 (70.37)</t>
+          <t>maa://22765 (92.47), *maa://21915 (70.37)</t>
         </is>
       </c>
       <c r="E9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (86.61), ***maa://22740 (5.77), **maa://39938 (42.86), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (95.24)</t>
+          <t>maa://28711 (86.61), ***maa://22740 (5.77), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (95.24)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.82), **maa://32237 (41.3), ***maa://34206 (20.0), ***maa://39951 (15.22), ***maa://39243 (28.57), *maa://45271 (55.0)</t>
+          <t>***maa://25695 (18.82), **maa://32237 (41.3), ***maa://34206 (20.0), ***maa://39951 (14.89), ***maa://39243 (28.57), *maa://45271 (52.38)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.9), maa://22501 (97.59), *maa://45521 (66.67)</t>
+          <t>maa://22747 (92.9), maa://22501 (97.59), *maa://45521 (71.43)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.87)</t>
+          <t>maa://36713 (97.88)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1951,7 +1951,7 @@
       </c>
       <c r="AF11" s="2" t="inlineStr">
         <is>
-          <t>maa://31203 (95.83)</t>
+          <t>maa://31203 (96.0)</t>
         </is>
       </c>
       <c r="AG11" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.89), maa://36673 (92.96), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.9), maa://36673 (92.96), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.71), **maa://22728 (47.73)</t>
+          <t>*maa://21248 (73.39), **maa://22728 (47.73)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (92.62), *maa://22583 (74.24), *maa://22500 (58.7)</t>
+          <t>maa://22676 (92.62), *maa://22583 (74.63), *maa://22500 (58.7)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="T14" s="2" t="inlineStr">
         <is>
-          <t>maa://22521 (94.0), maa://42751 (100.0)</t>
+          <t>maa://22521 (94.06), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.83), maa://22734 (84.03), *maa://30808 (64.18), **maa://36048 (42.86), maa://45058 (100.0)</t>
+          <t>*maa://22743 (77.45), maa://22734 (84.03), *maa://30808 (64.18), **maa://36048 (42.11), maa://45058 (100.0)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (90.57), *maa://22727 (70.0)</t>
+          <t>maa://24762 (90.62), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.4), maa://36679 (93.75), maa://37650 (97.06)</t>
+          <t>maa://21441 (96.4), maa://36679 (93.88), maa://37650 (97.06)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.81), *maa://28648 (68.75), maa://36674 (80.43)</t>
+          <t>maa://22729 (94.84), *maa://28648 (69.23), maa://36674 (80.43)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.66), maa://39599 (85.11)</t>
+          <t>maa://22430 (88.66), maa://39599 (85.42)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2667,7 +2667,7 @@
       </c>
       <c r="P17" s="2" t="inlineStr">
         <is>
-          <t>maa://23890 (81.0), *maa://24940 (67.86)</t>
+          <t>maa://23890 (81.19), *maa://24940 (67.86)</t>
         </is>
       </c>
       <c r="Q17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.24)</t>
+          <t>maa://24570 (97.25)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (89.47), *maa://22732 (51.16)</t>
+          <t>maa://22466 (89.54), *maa://22732 (51.16)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (58.39), **maa://29784 (44.44)</t>
+          <t>*maa://24313 (58.64), **maa://29784 (44.44)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (64.71), *maa://36668 (57.5)</t>
+          <t>*maa://30709 (64.79), *maa://36668 (57.5)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -2991,7 +2991,7 @@
       </c>
       <c r="AF19" s="2" t="inlineStr">
         <is>
-          <t>*maa://21663 (62.86)</t>
+          <t>*maa://21663 (63.38)</t>
         </is>
       </c>
       <c r="AG19" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.07)</t>
+          <t>maa://41331 (85.29)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (80.71), ***maa://23820 (29.31)</t>
+          <t>maa://21443 (80.76), ***maa://23820 (29.31)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.37), *maa://22432 (78.46)</t>
+          <t>maa://22524 (94.39), *maa://22432 (77.61)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.57), *maa://37649 (67.86)</t>
+          <t>maa://21282 (98.58), *maa://37649 (67.86)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="AF22" s="2" t="inlineStr">
         <is>
-          <t>maa://29658 (93.48)</t>
+          <t>maa://29658 (93.62)</t>
         </is>
       </c>
       <c r="AG22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.19), maa://39875 (94.12)</t>
+          <t>maa://39756 (95.25), maa://39875 (94.12)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.75), *maa://29748 (75.78), ***maa://29785 (16.42), *maa://37566 (73.53)</t>
+          <t>maa://30587 (91.79), *maa://29748 (75.78), ***maa://29785 (16.42), *maa://37566 (74.29)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (85.02), maa://23504 (93.15), **maa://22892 (40.14), *maa://25141 (76.74), *maa://36663 (78.08), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (85.08), maa://23504 (93.19), **maa://22892 (40.14), *maa://25141 (76.74), *maa://36663 (78.08), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.3), maa://24621 (96.75), maa://36676 (96.88), maa://22771 (85.71), *maa://37772 (66.67)</t>
+          <t>maa://20108 (96.3), maa://24621 (96.75), maa://36676 (96.97), maa://22771 (85.71), *maa://37772 (66.67)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>maa://41802 (92.86)</t>
+          <t>maa://41802 (93.33)</t>
         </is>
       </c>
       <c r="E26" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (94.51)</t>
+          <t>maa://42235 (94.57)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.98), maa://25725 (83.72)</t>
+          <t>maa://24465 (90.99), maa://25725 (83.72)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.41), maa://41749 (91.89), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.44), maa://41749 (92.0), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.19), *maa://28440 (79.05), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.21), *maa://28440 (79.05), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4227,7 +4227,7 @@
       </c>
       <c r="P29" s="2" t="inlineStr">
         <is>
-          <t>*maa://23168 (56.9), *maa://30050 (51.61)</t>
+          <t>*maa://23168 (57.63), *maa://30050 (51.61)</t>
         </is>
       </c>
       <c r="Q29" s="1" t="n"/>
@@ -4389,7 +4389,7 @@
       </c>
       <c r="X30" s="2" t="inlineStr">
         <is>
-          <t>maa://39477 (87.5)</t>
+          <t>maa://39477 (88.24)</t>
         </is>
       </c>
       <c r="Y30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.53), maa://36258 (85.32), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.55), maa://36258 (85.32), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.12), maa://41108 (88.0), maa://41238 (96.97), maa://45523 (100.0)</t>
+          <t>maa://42859 (96.12), maa://41108 (88.0), maa://41238 (97.0), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (95.92)</t>
+          <t>maa://41296 (95.97)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (80.85), maa://45790 (88.89)</t>
+          <t>maa://45788 (82.35), maa://45790 (88.89)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5575,7 +5575,7 @@
       </c>
       <c r="P41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (38.24), maa://43177 (87.5)</t>
+          <t>**maa://35616 (38.24), maa://43177 (88.89)</t>
         </is>
       </c>
       <c r="Q41" s="1" t="n"/>
@@ -5814,7 +5814,7 @@
       </c>
       <c r="T44" s="2" t="inlineStr">
         <is>
-          <t>maa://39366 (87.88)</t>
+          <t>maa://39366 (88.24)</t>
         </is>
       </c>
       <c r="U44" s="1" t="n"/>
@@ -5941,7 +5941,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.37), maa://29661 (97.24), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.38), maa://29661 (97.24), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6234,7 +6234,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.75), **maa://32434 (33.33)</t>
+          <t>maa://32534 (93.77), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6270,7 +6270,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.45)</t>
+          <t>maa://32532 (92.14)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6342,7 +6342,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (82.57), maa://31270 (95.2)</t>
+          <t>maa://27746 (82.73), maa://31270 (95.2)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6360,7 +6360,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (67.27)</t>
+          <t>*maa://40438 (67.86)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>
@@ -6396,7 +6396,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (97.22), maa://43903 (100.0)</t>
+          <t>maa://42981 (97.3), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#151)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.41), maa://36684 (95.1), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.41), maa://36684 (95.19), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.79), ***maa://21730 (25.0), ***maa://39501 (20.83), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.79), ***maa://21730 (24.66), ***maa://39501 (20.83), *maa://36675 (60.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.26), maa://20276 (86.05), *maa://22749 (72.73)</t>
+          <t>*maa://22880 (65.26), maa://20276 (86.13), *maa://22749 (72.73)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.32), maa://26254 (96.43)</t>
+          <t>maa://21249 (94.37), maa://26254 (96.43)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.28), maa://27484 (96.46), maa://27480 (82.86)</t>
+          <t>maa://27396 (84.28), maa://27484 (96.49), maa://27480 (82.86)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.75), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.79), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.51), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (86.67)</t>
+          <t>**maa://32495 (48.51), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (87.23)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (63.27), ***maa://26209 (13.04), *maa://39394 (69.57)</t>
+          <t>*maa://30062 (63.27), ***maa://26209 (13.04), *maa://39394 (66.67)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.14), maa://22744 (84.0)</t>
+          <t>maa://21245 (84.21), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.01.31 13:17:43</t>
+          <t>更新日期：2025.02.01 13:16:44</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>*maa://21476 (73.08), **maa://39431 (50.0), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (73.08), *maa://39431 (53.85), *maa://37551 (57.14)</t>
         </is>
       </c>
       <c r="E8" s="1" t="n"/>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24371 (54.93)</t>
+          <t>*maa://24371 (54.17)</t>
         </is>
       </c>
       <c r="I8" s="1" t="n"/>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>maa://22765 (92.47), *maa://21915 (70.37)</t>
+          <t>maa://22765 (92.55), *maa://21915 (70.37)</t>
         </is>
       </c>
       <c r="E9" s="1" t="n"/>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>maa://22762 (92.05), maa://39552 (90.0)</t>
+          <t>maa://22762 (92.13), maa://39552 (81.82)</t>
         </is>
       </c>
       <c r="M9" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.71)</t>
+          <t>maa://26223 (97.74)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (86.61), ***maa://22740 (5.77), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (95.24)</t>
+          <t>maa://28711 (86.73), ***maa://22740 (5.77), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (95.45)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (90.43), *maa://22865 (51.92)</t>
+          <t>maa://26206 (90.43), *maa://22865 (50.94)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.82), **maa://32237 (41.3), ***maa://34206 (20.0), ***maa://39951 (14.89), ***maa://39243 (28.57), *maa://45271 (52.38)</t>
+          <t>***maa://25695 (18.82), **maa://32237 (41.3), ***maa://34206 (20.0), ***maa://39951 (14.89), ***maa://39243 (28.57), *maa://45271 (54.55)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.32), maa://22755 (87.83), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.34), maa://22755 (87.83), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.45)</t>
+          <t>maa://36707 (99.46)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.9), maa://22501 (97.59), *maa://45521 (71.43)</t>
+          <t>maa://22747 (92.9), maa://22501 (97.59), *maa://45521 (75.0)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1935,7 +1935,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://29912 (100.0), maa://22516 (88.37), *maa://20794 (52.24)</t>
+          <t>maa://29912 (98.48), maa://22516 (88.37), *maa://20794 (52.24)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.28), *maa://21485 (76.26), maa://37962 (88.57)</t>
+          <t>maa://22753 (91.33), *maa://21485 (76.26), maa://37962 (88.89)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.47), maa://36677 (92.59), maa://39872 (90.91)</t>
+          <t>maa://23669 (95.47), maa://36677 (92.73), maa://39872 (90.91)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.26), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (78.57), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.9), maa://36673 (92.96), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.9), maa://36673 (93.15), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="T14" s="2" t="inlineStr">
         <is>
-          <t>maa://22521 (94.06), maa://42751 (100.0)</t>
+          <t>maa://22521 (94.12), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.45), maa://22734 (84.03), *maa://30808 (64.18), **maa://36048 (42.11), maa://45058 (100.0)</t>
+          <t>*maa://22743 (77.56), maa://22734 (84.03), *maa://30808 (64.18), **maa://36048 (42.11), maa://45058 (100.0)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="T15" s="2" t="inlineStr">
         <is>
-          <t>maa://23892 (97.4)</t>
+          <t>maa://23892 (97.44)</t>
         </is>
       </c>
       <c r="U15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.37), *maa://36666 (78.12), *maa://22766 (68.7)</t>
+          <t>maa://21364 (81.37), *maa://36666 (78.57), *maa://22766 (68.97)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (89.2)</t>
+          <t>maa://24421 (89.24)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (89.54), *maa://22732 (51.16)</t>
+          <t>maa://22466 (89.61), *maa://22732 (51.16)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="X18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (96.77), maa://22741 (85.71)</t>
+          <t>maa://21917 (96.81), maa://22741 (85.71)</t>
         </is>
       </c>
       <c r="Y18" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (89.94), maa://25198 (93.4), *maa://20795 (51.56), maa://36680 (93.75)</t>
+          <t>maa://21432 (90.0), maa://25198 (93.4), *maa://20795 (51.56), maa://36680 (93.75)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (81.58), *maa://22751 (72.06)</t>
+          <t>maa://27127 (80.87), *maa://22751 (72.06)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.57), *maa://41753 (57.14)</t>
+          <t>***maa://28036 (28.57), *maa://41753 (53.33)</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.25), maa://39875 (94.12)</t>
+          <t>maa://39756 (95.3), maa://39875 (94.12)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="X23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (65.28)</t>
+          <t>*maa://28503 (65.75)</t>
         </is>
       </c>
       <c r="Y23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (77.96)</t>
+          <t>*maa://24368 (77.81)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (85.08), maa://23504 (93.19), **maa://22892 (40.14), *maa://25141 (76.74), *maa://36663 (78.08), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (84.74), maa://23504 (93.19), **maa://22892 (40.14), *maa://25141 (76.74), *maa://36663 (78.08), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (74.52), *maa://25311 (73.53), ***maa://22725 (4.84), *maa://45047 (66.67)</t>
+          <t>*maa://29063 (74.05), *maa://25311 (73.53), ***maa://22725 (4.84), *maa://45047 (71.43)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (87.16), *maa://24516 (80.0), maa://26001 (87.5)</t>
+          <t>maa://31215 (87.27), *maa://24516 (80.0), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (94.57)</t>
+          <t>maa://42235 (94.62)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.51), *maa://36701 (65.52)</t>
+          <t>maa://36660 (92.56), *maa://36701 (65.52)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.21), *maa://28440 (79.05), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.25), *maa://28440 (79.05), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.77), maa://42865 (82.0), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.77), maa://42865 (82.35), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.43), maa://45822 (100.0), maa://45045 (100.0)</t>
+          <t>maa://42979 (96.48), maa://45822 (100.0), maa://45045 (100.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.55), maa://36258 (85.32), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.57), maa://36258 (85.32), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.49), maa://36667 (98.59), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.49), maa://36667 (98.61), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4601,7 +4601,7 @@
       </c>
       <c r="L32" s="2" t="inlineStr">
         <is>
-          <t>maa://28065 (95.24)</t>
+          <t>maa://28065 (95.35)</t>
         </is>
       </c>
       <c r="M32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.12), maa://41108 (88.0), maa://41238 (97.0), maa://45523 (100.0)</t>
+          <t>maa://42859 (96.19), maa://41108 (88.0), maa://41238 (97.0), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4747,7 +4747,7 @@
       </c>
       <c r="P33" s="2" t="inlineStr">
         <is>
-          <t>maa://21956 (80.56), *maa://22730 (79.31)</t>
+          <t>maa://21956 (80.69), *maa://22730 (79.31)</t>
         </is>
       </c>
       <c r="Q33" s="1" t="n"/>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (88.17), maa://25199 (84.82), maa://30434 (90.79), ***maa://25036 (16.0), *maa://45059 (75.0), *maa://44165 (66.67)</t>
+          <t>maa://36670 (88.3), maa://25199 (84.82), maa://30434 (90.79), ***maa://25036 (16.0), *maa://45059 (75.0), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5405,7 +5405,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (92.31)</t>
+          <t>maa://24709 (91.67)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (82.35), maa://45790 (88.89)</t>
+          <t>maa://45788 (83.33), maa://45790 (88.89)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5575,7 +5575,7 @@
       </c>
       <c r="P41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (38.24), maa://43177 (88.89)</t>
+          <t>**maa://35616 (38.24), maa://43177 (89.47)</t>
         </is>
       </c>
       <c r="Q41" s="1" t="n"/>
@@ -5713,7 +5713,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (92.91), maa://21284 (85.11)</t>
+          <t>maa://22525 (92.31), maa://21284 (85.11)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5782,7 +5782,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.94), maa://27728 (96.04)</t>
+          <t>maa://29768 (97.95), maa://27728 (96.04)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5835,7 +5835,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.49), maa://30807 (95.59), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (84.21)</t>
+          <t>maa://21229 (84.49), maa://30807 (95.65), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (84.21)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5888,7 +5888,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.41), maa://43901 (88.24)</t>
+          <t>maa://35931 (92.43), maa://43901 (88.24)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6270,7 +6270,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.14)</t>
+          <t>maa://32532 (92.2)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6342,7 +6342,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (82.73), maa://31270 (95.2)</t>
+          <t>maa://27746 (82.88), maa://31270 (95.2)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6360,7 +6360,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (67.86)</t>
+          <t>*maa://40438 (68.42)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>
@@ -6432,7 +6432,7 @@
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>maa://44405 (88.0)</t>
+          <t>maa://44405 (88.46)</t>
         </is>
       </c>
       <c r="I64" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#152)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.88), *maa://30515 (69.9), *maa://34787 (72.97), ***maa://20792 (11.93), maa://39402 (90.74), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.88), *maa://30515 (69.9), *maa://34787 (72.97), ***maa://20792 (11.93), maa://39402 (90.91), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.5), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.51), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.26), maa://20276 (86.13), *maa://22749 (72.73)</t>
+          <t>*maa://22880 (65.62), maa://20276 (86.13), *maa://22749 (72.73)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (94.2)</t>
+          <t>maa://24390 (94.29)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.32), maa://27295 (85.07), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
+          <t>maa://32509 (97.35), maa://27295 (85.07), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.51), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (87.23)</t>
+          <t>**maa://32495 (48.51), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (87.5)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.21), maa://22744 (84.0)</t>
+          <t>maa://21245 (84.28), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (95.35)</t>
+          <t>maa://42407 (95.45)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>maa://21955 (94.44)</t>
+          <t>maa://21955 (94.59)</t>
         </is>
       </c>
       <c r="E7" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (92.0), maa://24957 (97.73)</t>
+          <t>maa://28624 (92.31), maa://24957 (97.73)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.3), *maa://22758 (75.76)</t>
+          <t>maa://22399 (95.33), *maa://22758 (75.76)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.02.01 13:16:44</t>
+          <t>更新日期：2025.02.02 13:17:29</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1627,7 +1627,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (82.47)</t>
+          <t>maa://22736 (82.83)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.74)</t>
+          <t>maa://26223 (97.79)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (86.73), ***maa://22740 (5.77), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (95.45)</t>
+          <t>maa://28711 (86.84), ***maa://22740 (5.77), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (95.45)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (90.43), *maa://22865 (50.94)</t>
+          <t>maa://26206 (89.66), *maa://22865 (50.94)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.34), maa://22755 (87.83), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.35), maa://22755 (87.83), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.88)</t>
+          <t>maa://36713 (97.69)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1935,7 +1935,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://29912 (98.48), maa://22516 (88.37), *maa://20794 (52.24)</t>
+          <t>maa://29912 (98.51), maa://22516 (88.37), *maa://20794 (52.24)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.33), *maa://21485 (76.26), maa://37962 (88.89)</t>
+          <t>maa://22753 (91.33), *maa://21485 (76.26), maa://37962 (89.19)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.47), maa://36677 (92.73), maa://39872 (90.91)</t>
+          <t>maa://23669 (95.47), maa://36677 (92.98), maa://39872 (90.91)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.57), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (78.87), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.9), maa://36673 (93.15), maa://25001 (85.51)</t>
+          <t>maa://24999 (91.91), maa://36673 (93.15), maa://25001 (85.51)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>maa://34957 (81.43), *maa://22768 (51.61)</t>
+          <t>maa://34957 (81.69), *maa://22768 (51.61)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (33.57), maa://39883 (92.19), *maa://39885 (57.14)</t>
+          <t>**maa://22737 (33.57), maa://39883 (92.42), *maa://39885 (57.14)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.62), maa://21288 (96.3), maa://39841 (95.7), maa://36682 (97.44)</t>
+          <t>maa://26245 (96.64), maa://21288 (96.3), maa://39841 (95.79), maa://36682 (97.44)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.69), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.7), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.56), maa://22734 (84.03), *maa://30808 (64.18), **maa://36048 (42.11), maa://45058 (100.0)</t>
+          <t>*maa://22743 (77.67), maa://22734 (84.03), *maa://30808 (64.18), **maa://36048 (42.11), maa://45058 (100.0)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.1), maa://21478 (91.67)</t>
+          <t>maa://24304 (88.15), maa://21478 (91.67)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (90.62), *maa://22727 (70.0)</t>
+          <t>maa://24762 (90.18), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="T15" s="2" t="inlineStr">
         <is>
-          <t>maa://23892 (97.44)</t>
+          <t>maa://23892 (96.2)</t>
         </is>
       </c>
       <c r="U15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.37), *maa://36666 (78.57), *maa://22766 (68.97)</t>
+          <t>maa://21364 (81.37), *maa://36666 (78.79), *maa://22766 (68.97)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.4), maa://36679 (93.88), maa://37650 (97.06)</t>
+          <t>maa://21441 (96.4), maa://36679 (94.0), maa://37650 (97.06)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.84), *maa://28648 (69.23), maa://36674 (80.43)</t>
+          <t>maa://22729 (94.84), *maa://28648 (69.7), maa://36674 (80.43)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>maa://21624 (83.78)</t>
+          <t>maa://21624 (84.21)</t>
         </is>
       </c>
       <c r="E17" s="1" t="n"/>
@@ -2667,7 +2667,7 @@
       </c>
       <c r="P17" s="2" t="inlineStr">
         <is>
-          <t>maa://23890 (81.19), *maa://24940 (67.86)</t>
+          <t>maa://23890 (81.37), *maa://24940 (67.86)</t>
         </is>
       </c>
       <c r="Q17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.25)</t>
+          <t>maa://24570 (97.26)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (89.61), *maa://22732 (51.16)</t>
+          <t>maa://22466 (89.68), *maa://22732 (51.16)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="X18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (96.81), maa://22741 (85.71)</t>
+          <t>maa://21917 (96.84), maa://22741 (85.71)</t>
         </is>
       </c>
       <c r="Y18" s="1" t="n"/>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (58.64), **maa://29784 (44.44)</t>
+          <t>*maa://24313 (58.9), **maa://29784 (44.44)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (64.79), *maa://36668 (57.5)</t>
+          <t>*maa://30709 (64.87), *maa://36668 (57.5)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.0), maa://25198 (93.4), *maa://20795 (51.56), maa://36680 (93.75)</t>
+          <t>maa://21432 (90.06), maa://25198 (93.4), *maa://20795 (51.56), maa://36680 (93.75)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.29)</t>
+          <t>maa://41331 (85.51)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (80.76), ***maa://23820 (29.31)</t>
+          <t>maa://21443 (80.81), ***maa://23820 (29.31)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.3), maa://39875 (94.12)</t>
+          <t>maa://39756 (95.34), maa://39875 (94.2)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="X23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (65.75)</t>
+          <t>*maa://28503 (66.22)</t>
         </is>
       </c>
       <c r="Y23" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.3), maa://24621 (96.75), maa://36676 (96.97), maa://22771 (85.71), *maa://37772 (66.67)</t>
+          <t>maa://20108 (96.32), maa://24621 (96.77), maa://36676 (96.97), maa://22771 (85.71), *maa://37772 (66.67)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3951,7 +3951,7 @@
       </c>
       <c r="L27" s="2" t="inlineStr">
         <is>
-          <t>maa://28071 (89.47)</t>
+          <t>maa://28071 (90.0)</t>
         </is>
       </c>
       <c r="M27" s="1" t="n"/>
@@ -4031,7 +4031,7 @@
       </c>
       <c r="AF27" s="2" t="inlineStr">
         <is>
-          <t>maa://24023 (97.18)</t>
+          <t>maa://24023 (97.22)</t>
         </is>
       </c>
       <c r="AG27" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.99), maa://25725 (83.72)</t>
+          <t>maa://24465 (91.01), maa://25725 (83.72)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4081,7 +4081,7 @@
       </c>
       <c r="L28" s="2" t="inlineStr">
         <is>
-          <t>maa://30770 (80.43)</t>
+          <t>maa://30770 (80.85)</t>
         </is>
       </c>
       <c r="M28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.44), maa://41749 (92.0), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.24), maa://41749 (92.0), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.56), *maa://36701 (65.52)</t>
+          <t>maa://36660 (92.31), *maa://36701 (65.52)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>*maa://25175 (66.67)</t>
+          <t>*maa://25175 (65.38)</t>
         </is>
       </c>
       <c r="I29" s="1" t="n"/>
@@ -4227,7 +4227,7 @@
       </c>
       <c r="P29" s="2" t="inlineStr">
         <is>
-          <t>*maa://23168 (57.63), *maa://30050 (51.61)</t>
+          <t>*maa://23168 (57.38), *maa://30050 (51.61)</t>
         </is>
       </c>
       <c r="Q29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.77), maa://42865 (82.35), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.77), maa://42865 (82.69), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4341,7 +4341,7 @@
       </c>
       <c r="L30" s="2" t="inlineStr">
         <is>
-          <t>maa://30442 (95.0)</t>
+          <t>maa://30442 (95.08)</t>
         </is>
       </c>
       <c r="M30" s="1" t="n"/>
@@ -4389,7 +4389,7 @@
       </c>
       <c r="X30" s="2" t="inlineStr">
         <is>
-          <t>maa://39477 (88.24)</t>
+          <t>maa://39477 (88.89)</t>
         </is>
       </c>
       <c r="Y30" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.48), maa://45822 (100.0), maa://45045 (100.0)</t>
+          <t>maa://42979 (96.58), maa://45822 (100.0), maa://45045 (100.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.57), maa://36258 (85.32), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.26), maa://36258 (84.55), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.49), maa://36667 (98.61), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.5), maa://36667 (98.61), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.19), maa://41108 (88.0), maa://41238 (97.0), maa://45523 (100.0)</t>
+          <t>maa://42859 (96.26), maa://41108 (88.0), maa://41238 (97.0), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (93.28)</t>
+          <t>maa://24526 (93.31)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (95.97)</t>
+          <t>maa://41296 (96.0)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (88.3), maa://25199 (84.82), maa://30434 (90.79), ***maa://25036 (16.0), *maa://45059 (75.0), *maa://44165 (66.67)</t>
+          <t>maa://36670 (87.37), maa://25199 (84.82), maa://30434 (90.91), ***maa://25036 (16.0), *maa://45059 (75.0), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5405,7 +5405,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.67)</t>
+          <t>maa://24709 (91.72)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (83.33), maa://45790 (88.89)</t>
+          <t>maa://45788 (83.05), maa://45790 (88.89)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5490,7 +5490,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.77), maa://21386 (95.74), maa://36664 (90.91), maa://45550 (100.0)</t>
+          <t>maa://23278 (95.78), maa://21386 (95.74), maa://36664 (90.91), maa://45550 (100.0)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5543,7 +5543,7 @@
       </c>
       <c r="H41" s="2" t="inlineStr">
         <is>
-          <t>maa://24466 (93.33)</t>
+          <t>maa://24466 (93.48)</t>
         </is>
       </c>
       <c r="I41" s="1" t="n"/>
@@ -5713,7 +5713,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (92.31), maa://21284 (85.11)</t>
+          <t>maa://22525 (92.36), maa://21284 (85.11)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5782,7 +5782,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.95), maa://27728 (96.04)</t>
+          <t>maa://29768 (97.97), maa://27728 (96.08)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5888,7 +5888,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.43), maa://43901 (88.24)</t>
+          <t>maa://35931 (92.48), maa://43901 (88.89)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6234,7 +6234,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.77), **maa://32434 (33.33)</t>
+          <t>maa://32534 (93.79), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6270,7 +6270,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.2)</t>
+          <t>maa://32532 (91.96)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6342,7 +6342,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (82.88), maa://31270 (95.2)</t>
+          <t>maa://27746 (82.88), maa://31270 (95.24)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#153)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.43), maa://25390 (96.12), maa://36681 (87.34)</t>
+          <t>maa://24702 (94.46), maa://25390 (96.14), maa://36681 (87.34)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.88), *maa://30515 (69.9), *maa://34787 (72.97), ***maa://20792 (11.93), maa://39402 (90.91), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.88), *maa://30515 (69.9), *maa://34787 (72.97), ***maa://20792 (11.93), maa://39402 (91.23), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.41), *maa://20791 (63.01)</t>
+          <t>maa://22742 (91.57), *maa://20791 (62.16)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.41), maa://36684 (95.19), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.41), maa://36684 (95.41), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.79), ***maa://21730 (24.66), ***maa://39501 (20.83), *maa://36675 (60.0)</t>
+          <t>maa://25251 (92.17), ***maa://21730 (25.68), ***maa://39501 (17.24), **maa://36675 (50.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://36987 (95.92), maa://40192 (100.0), maa://39849 (88.89)</t>
+          <t>maa://36987 (96.0), maa://40192 (100.0), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.51), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.53), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.62), maa://20276 (86.13), *maa://22749 (72.73)</t>
+          <t>*maa://22880 (66.15), maa://20276 (86.36), *maa://22749 (72.73)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.37), maa://26254 (96.43)</t>
+          <t>maa://21249 (94.42), maa://26254 (96.43)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.57), **maa://20790 (43.48), ***maa://37170 (17.19), maa://45854 (100.0)</t>
+          <t>maa://24617 (89.66), **maa://20790 (43.48), ***maa://37170 (16.92), maa://45854 (100.0)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.28), maa://27484 (96.49), maa://27480 (82.86)</t>
+          <t>maa://27396 (84.38), maa://27484 (96.55), maa://27480 (82.86)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (94.29)</t>
+          <t>maa://24390 (94.52)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -901,7 +901,7 @@
       </c>
       <c r="AF3" s="2" t="inlineStr">
         <is>
-          <t>*maa://21289 (72.73)</t>
+          <t>*maa://21289 (73.91)</t>
         </is>
       </c>
       <c r="AG3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.79), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.94), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (97.35), maa://27295 (85.07), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
+          <t>maa://32509 (96.49), maa://27295 (85.71), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.51), ***maa://31785 (22.22), ***maa://36683 (28.26), maa://43217 (87.5)</t>
+          <t>**maa://32495 (48.51), ***maa://31785 (22.22), maa://43217 (88.24), ***maa://36683 (28.26)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (63.27), ***maa://26209 (13.04), *maa://39394 (66.67)</t>
+          <t>*maa://30062 (64.0), ***maa://26209 (13.04), *maa://39394 (66.67)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.28), maa://22744 (84.0)</t>
+          <t>maa://21245 (84.62), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="P5" s="2" t="inlineStr">
         <is>
-          <t>maa://21919 (96.36), *maa://21281 (80.0)</t>
+          <t>maa://21919 (96.55), *maa://21281 (80.0)</t>
         </is>
       </c>
       <c r="Q5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (95.45)</t>
+          <t>maa://42407 (95.83)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>maa://24370 (96.61)</t>
+          <t>maa://24370 (96.67)</t>
         </is>
       </c>
       <c r="I6" s="1" t="n"/>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>maa://24839 (98.97)</t>
+          <t>maa://24839 (98.99)</t>
         </is>
       </c>
       <c r="M6" s="1" t="n"/>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="P6" s="2" t="inlineStr">
         <is>
-          <t>maa://31836 (92.59), maa://30381 (92.31)</t>
+          <t>maa://31836 (92.59), maa://30381 (92.86)</t>
         </is>
       </c>
       <c r="Q6" s="1" t="n"/>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="AF6" s="2" t="inlineStr">
         <is>
-          <t>*maa://33152 (59.57), ***maa://22770 (26.09)</t>
+          <t>*maa://33152 (62.0), ***maa://22770 (26.09)</t>
         </is>
       </c>
       <c r="AG6" s="1" t="n"/>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>maa://21955 (94.59)</t>
+          <t>maa://21955 (94.74)</t>
         </is>
       </c>
       <c r="E7" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (92.31), maa://24957 (97.73)</t>
+          <t>maa://28624 (92.45), maa://24957 (97.73)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.33), *maa://22758 (75.76)</t>
+          <t>maa://22399 (95.33), *maa://22758 (75.36)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (69.05), *maa://36671 (68.0), *maa://42530 (62.5), maa://45272 (100.0)</t>
+          <t>*maa://26191 (68.24), *maa://36671 (68.0), *maa://42530 (62.5), maa://45272 (100.0)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.02.02 13:17:29</t>
+          <t>更新日期：2025.02.08 13:16:19</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24371 (54.17)</t>
+          <t>*maa://24371 (55.41)</t>
         </is>
       </c>
       <c r="I8" s="1" t="n"/>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (83.33), *maa://21916 (60.94), maa://23252 (91.18), maa://37496 (96.77), **maa://22759 (45.45)</t>
+          <t>maa://32931 (83.48), *maa://21916 (61.54), maa://23252 (91.18), maa://37496 (96.77), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (96.08)</t>
+          <t>maa://21411 (95.84)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>maa://22762 (92.13), maa://39552 (81.82)</t>
+          <t>maa://22762 (92.22), maa://39552 (81.82)</t>
         </is>
       </c>
       <c r="M9" s="1" t="n"/>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (82.83)</t>
+          <t>maa://22736 (83.0)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1643,7 +1643,7 @@
       </c>
       <c r="T9" s="2" t="inlineStr">
         <is>
-          <t>**maa://22866 (30.19), maa://26222 (97.92)</t>
+          <t>**maa://22866 (30.19), maa://26222 (98.0)</t>
         </is>
       </c>
       <c r="U9" s="1" t="n"/>
@@ -1670,12 +1670,12 @@
       </c>
       <c r="AA9" s="1" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (86.84), ***maa://22740 (5.77), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (95.45)</t>
+          <t>maa://28711 (87.18), ***maa://22740 (5.66), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (95.83), *maa://45044 (66.67)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (89.66), *maa://22865 (50.94)</t>
+          <t>maa://26206 (89.17), *maa://22865 (50.94)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1704,12 +1704,12 @@
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.82), **maa://32237 (41.3), ***maa://34206 (20.0), ***maa://39951 (14.89), ***maa://39243 (28.57), *maa://45271 (54.55)</t>
+          <t>***maa://25695 (18.82), ***maa://34206 (20.0), ***maa://39951 (14.29), ***maa://39243 (28.57), *maa://45271 (56.0)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1741,7 +1741,7 @@
       </c>
       <c r="L10" s="2" t="inlineStr">
         <is>
-          <t>**maa://24395 (41.38)</t>
+          <t>**maa://24395 (41.94)</t>
         </is>
       </c>
       <c r="M10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.35), maa://22755 (87.83), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.46), maa://22755 (87.83), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (53.41), *maa://22733 (60.0), **maa://22761 (50.0)</t>
+          <t>*maa://25021 (53.33), *maa://22733 (60.0), **maa://22761 (50.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.46)</t>
+          <t>maa://36707 (99.47)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (88.78)</t>
+          <t>maa://21287 (88.89)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="P11" s="2" t="inlineStr">
         <is>
-          <t>maa://45557 (100.0)</t>
+          <t>maa://45557 (87.5)</t>
         </is>
       </c>
       <c r="Q11" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.9), maa://22501 (97.59), *maa://45521 (75.0)</t>
+          <t>maa://22747 (93.04), maa://22501 (97.65), maa://45521 (81.82)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.69)</t>
+          <t>maa://36713 (97.73)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1935,7 +1935,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://29912 (98.51), maa://22516 (88.37), *maa://20794 (52.24)</t>
+          <t>maa://29912 (98.53), maa://22516 (88.37), *maa://20794 (52.24)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>maa://30766 (89.29), *maa://36678 (60.0)</t>
+          <t>maa://30766 (89.29), *maa://36678 (66.67)</t>
         </is>
       </c>
       <c r="E12" s="1" t="n"/>
@@ -1980,12 +1980,12 @@
       </c>
       <c r="G12" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (89.88)</t>
+          <t>maa://21867 (89.88), **maa://45826 (33.33)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.33), *maa://21485 (76.26), maa://37962 (89.19)</t>
+          <t>maa://22753 (90.91), *maa://21485 (76.26), maa://37962 (90.0)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.47), maa://36677 (92.98), maa://39872 (90.91)</t>
+          <t>maa://23669 (95.47), maa://36677 (93.1), maa://39872 (91.3)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.87), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (78.32), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (91.91), maa://36673 (93.15), maa://25001 (85.51)</t>
+          <t>maa://24999 (92.01), maa://36673 (93.15), maa://25001 (85.71)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.39), **maa://22728 (47.73)</t>
+          <t>*maa://21248 (73.08), **maa://22728 (47.73)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (92.62), *maa://22583 (74.63), *maa://22500 (58.7)</t>
+          <t>maa://22676 (92.68), *maa://22583 (74.63), *maa://22500 (58.7)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>maa://34957 (81.69), *maa://22768 (51.61)</t>
+          <t>maa://34957 (82.19), *maa://22768 (51.61)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (33.57), maa://39883 (92.42), *maa://39885 (57.14)</t>
+          <t>**maa://22737 (33.57), maa://39883 (92.54), *maa://39885 (57.14)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.64), maa://21288 (96.3), maa://39841 (95.79), maa://36682 (97.44)</t>
+          <t>maa://26245 (96.67), maa://21288 (96.3), maa://39841 (95.96), maa://36682 (97.44)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.7), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.73), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="T14" s="2" t="inlineStr">
         <is>
-          <t>maa://22521 (94.12), maa://42751 (100.0)</t>
+          <t>maa://22521 (94.23), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="1" t="n"/>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="AB14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (97.1)</t>
+          <t>maa://22764 (97.14)</t>
         </is>
       </c>
       <c r="AC14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.67), maa://22734 (84.03), *maa://30808 (64.18), **maa://36048 (42.11), maa://45058 (100.0)</t>
+          <t>*maa://22743 (77.51), maa://22734 (84.03), *maa://30808 (64.18), **maa://36048 (44.07), maa://45058 (88.89)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.15), maa://21478 (91.67)</t>
+          <t>maa://24304 (87.85), maa://21478 (89.19)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2391,7 +2391,7 @@
       </c>
       <c r="L15" s="2" t="inlineStr">
         <is>
-          <t>*maa://21334 (53.57)</t>
+          <t>*maa://21334 (55.17)</t>
         </is>
       </c>
       <c r="M15" s="1" t="n"/>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (90.18), *maa://22727 (70.0)</t>
+          <t>maa://24762 (90.24), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.37), *maa://36666 (78.79), *maa://22766 (68.97)</t>
+          <t>maa://21364 (81.17), *maa://36666 (79.05), *maa://22766 (68.97)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.4), maa://36679 (94.0), maa://37650 (97.06)</t>
+          <t>maa://21441 (96.4), maa://36679 (94.12), maa://37650 (97.06)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2537,7 +2537,7 @@
       </c>
       <c r="P16" s="2" t="inlineStr">
         <is>
-          <t>maa://28504 (90.91)</t>
+          <t>maa://28504 (91.23)</t>
         </is>
       </c>
       <c r="Q16" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.84), *maa://28648 (69.7), maa://36674 (80.43)</t>
+          <t>maa://22729 (94.87), *maa://28648 (69.12), maa://36674 (80.85)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (97.98), maa://28051 (96.0)</t>
+          <t>maa://28501 (98.0), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.83)</t>
+          <t>maa://26228 (95.88)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (64.76), maa://27755 (93.1)</t>
+          <t>*maa://23911 (64.76), maa://27755 (93.48)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>**maa://42324 (48.15)</t>
+          <t>**maa://42324 (50.0)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.26)</t>
+          <t>maa://24570 (97.29)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (89.24)</t>
+          <t>maa://24421 (89.33)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (89.68), *maa://22732 (51.16)</t>
+          <t>maa://22466 (89.94), *maa://22732 (51.16)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2813,7 +2813,7 @@
       </c>
       <c r="T18" s="2" t="inlineStr">
         <is>
-          <t>maa://24385 (97.22)</t>
+          <t>maa://24385 (97.3)</t>
         </is>
       </c>
       <c r="U18" s="1" t="n"/>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="X18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (96.84), maa://22741 (85.71)</t>
+          <t>maa://21917 (96.88), maa://22741 (85.71)</t>
         </is>
       </c>
       <c r="Y18" s="1" t="n"/>
@@ -2845,7 +2845,7 @@
       </c>
       <c r="AB18" s="2" t="inlineStr">
         <is>
-          <t>maa://24393 (97.78)</t>
+          <t>maa://24393 (97.92)</t>
         </is>
       </c>
       <c r="AC18" s="1" t="n"/>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (58.9), **maa://29784 (44.44)</t>
+          <t>*maa://24313 (59.39), **maa://29784 (46.43)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (99.12)</t>
+          <t>maa://24386 (99.14)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (64.87), *maa://36668 (57.5)</t>
+          <t>*maa://30709 (65.2), *maa://36668 (57.5)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.06), maa://25198 (93.4), *maa://20795 (51.56), maa://36680 (93.75)</t>
+          <t>maa://21432 (90.24), maa://25198 (93.4), *maa://20795 (51.16), maa://36680 (93.75)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (89.81)</t>
+          <t>maa://22864 (89.87)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.51)</t>
+          <t>maa://41331 (85.0)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="P20" s="2" t="inlineStr">
         <is>
-          <t>maa://37442 (94.87)</t>
+          <t>maa://37442 (95.0)</t>
         </is>
       </c>
       <c r="Q20" s="1" t="n"/>
@@ -3171,7 +3171,7 @@
       </c>
       <c r="L21" s="2" t="inlineStr">
         <is>
-          <t>maa://31731 (95.92)</t>
+          <t>maa://31731 (96.08)</t>
         </is>
       </c>
       <c r="M21" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (80.81), ***maa://23820 (29.31)</t>
+          <t>maa://21443 (80.91), ***maa://23820 (29.31)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.39), *maa://22432 (77.61)</t>
+          <t>maa://22524 (94.47), *maa://22432 (77.14)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>maa://25236 (96.59), **maa://21678 (48.94), **maa://22735 (42.86)</t>
+          <t>maa://25236 (96.63), **maa://21678 (48.94), **maa://22735 (42.86)</t>
         </is>
       </c>
       <c r="I22" s="1" t="n"/>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="T22" s="2" t="inlineStr">
         <is>
-          <t>maa://38495 (85.71)</t>
+          <t>maa://38495 (86.67)</t>
         </is>
       </c>
       <c r="U22" s="1" t="n"/>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="AF22" s="2" t="inlineStr">
         <is>
-          <t>maa://29658 (93.62)</t>
+          <t>maa://29658 (93.75)</t>
         </is>
       </c>
       <c r="AG22" s="1" t="n"/>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.57), *maa://41753 (53.33)</t>
+          <t>***maa://28036 (29.17), *maa://41753 (53.33)</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.34), maa://39875 (94.2)</t>
+          <t>maa://39756 (95.47), maa://39875 (94.37)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.79), *maa://29748 (75.78), ***maa://29785 (16.42), *maa://37566 (74.29)</t>
+          <t>maa://30587 (91.84), *maa://29748 (75.78), ***maa://29785 (16.42), *maa://37566 (76.32)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="T23" s="2" t="inlineStr">
         <is>
-          <t>maa://24387 (81.58), maa://31212 (93.33)</t>
+          <t>maa://24387 (82.05), maa://31212 (93.55)</t>
         </is>
       </c>
       <c r="U23" s="1" t="n"/>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="X23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (66.22)</t>
+          <t>*maa://28503 (67.95)</t>
         </is>
       </c>
       <c r="Y23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (77.81)</t>
+          <t>*maa://24368 (78.04)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (84.74), maa://23504 (93.19), **maa://22892 (40.14), *maa://25141 (76.74), *maa://36663 (78.08), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (84.74), maa://23504 (93.29), **maa://22892 (40.14), *maa://25141 (76.92), *maa://36663 (78.38), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.86), maa://36672 (80.36), maa://29910 (92.86), **maa://21440 (34.55), maa://45831 (100.0)</t>
+          <t>maa://22523 (85.86), maa://36672 (80.36), maa://29910 (92.98), **maa://21440 (35.71), *maa://45831 (75.0)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.06)</t>
+          <t>maa://29753 (95.08)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (74.05), *maa://25311 (73.53), ***maa://22725 (4.84), *maa://45047 (71.43)</t>
+          <t>*maa://29063 (74.05), *maa://25311 (73.53), ***maa://22725 (4.84), *maa://45047 (62.5)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3707,7 +3707,7 @@
       </c>
       <c r="P25" s="2" t="inlineStr">
         <is>
-          <t>maa://24382 (93.33)</t>
+          <t>maa://24382 (93.55)</t>
         </is>
       </c>
       <c r="Q25" s="1" t="n"/>
@@ -3723,7 +3723,7 @@
       </c>
       <c r="T25" s="2" t="inlineStr">
         <is>
-          <t>maa://20109 (92.49), maa://22545 (100.0), maa://42915 (100.0)</t>
+          <t>maa://20109 (92.05), maa://22545 (100.0), *maa://42915 (75.0)</t>
         </is>
       </c>
       <c r="U25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (87.27), *maa://24516 (80.0), maa://26001 (87.5)</t>
+          <t>maa://31215 (87.5), maa://24516 (80.22), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.32), maa://24621 (96.77), maa://36676 (96.97), maa://22771 (85.71), *maa://37772 (66.67)</t>
+          <t>maa://20108 (96.32), maa://24621 (96.85), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (91.86)</t>
+          <t>maa://24913 (92.05)</t>
         </is>
       </c>
       <c r="I26" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (94.62)</t>
+          <t>maa://42235 (94.68)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (47.37), *maa://39601 (76.47), maa://34494 (97.14), **maa://36665 (44.44)</t>
+          <t>**maa://21283 (47.37), *maa://39601 (77.78), maa://34494 (97.14), **maa://36665 (50.0)</t>
         </is>
       </c>
       <c r="I27" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (91.01), maa://25725 (83.72)</t>
+          <t>maa://24465 (91.07), maa://25725 (83.72)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.24), maa://41749 (92.0), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.48), maa://41749 (90.0), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.31), *maa://36701 (65.52)</t>
+          <t>maa://36660 (92.11), *maa://36701 (65.52)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.25), *maa://28440 (79.05), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.39), *maa://28440 (79.25), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4227,7 +4227,7 @@
       </c>
       <c r="P29" s="2" t="inlineStr">
         <is>
-          <t>*maa://23168 (57.38), *maa://30050 (51.61)</t>
+          <t>*maa://23168 (58.06), *maa://30050 (53.12)</t>
         </is>
       </c>
       <c r="Q29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.77), maa://42865 (82.69), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.77), maa://42865 (81.82), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4341,7 +4341,7 @@
       </c>
       <c r="L30" s="2" t="inlineStr">
         <is>
-          <t>maa://30442 (95.08)</t>
+          <t>maa://30442 (95.16)</t>
         </is>
       </c>
       <c r="M30" s="1" t="n"/>
@@ -4357,7 +4357,7 @@
       </c>
       <c r="P30" s="2" t="inlineStr">
         <is>
-          <t>maa://21442 (99.54)</t>
+          <t>maa://21442 (99.55)</t>
         </is>
       </c>
       <c r="Q30" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.58), maa://45822 (100.0), maa://45045 (100.0)</t>
+          <t>maa://42979 (96.67), maa://45822 (100.0), *maa://45045 (80.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.26), maa://36258 (84.55), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.33), maa://36258 (84.82), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.5), maa://36667 (98.61), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.5), maa://36667 (98.67), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.26), maa://41108 (88.0), maa://41238 (97.0), maa://45523 (100.0)</t>
+          <t>maa://42859 (96.43), maa://41108 (88.0), maa://41238 (97.06), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4747,7 +4747,7 @@
       </c>
       <c r="P33" s="2" t="inlineStr">
         <is>
-          <t>maa://21956 (80.69), *maa://22730 (79.31)</t>
+          <t>maa://21956 (81.08), *maa://22730 (79.31)</t>
         </is>
       </c>
       <c r="Q33" s="1" t="n"/>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (93.31)</t>
+          <t>maa://24526 (93.36)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.0)</t>
+          <t>maa://41296 (96.05)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5039,7 +5039,7 @@
       </c>
       <c r="AF35" s="2" t="inlineStr">
         <is>
-          <t>maa://39479 (93.75)</t>
+          <t>maa://39479 (94.12)</t>
         </is>
       </c>
       <c r="AG35" s="1" t="n"/>
@@ -5187,7 +5187,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (100.0), maa://45789 (100.0)</t>
+          <t>maa://45718 (99.01), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5203,7 +5203,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.2), *maa://21239 (66.67)</t>
+          <t>maa://21280 (89.3), *maa://21239 (66.67)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5352,7 +5352,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (87.06)</t>
+          <t>maa://36697 (86.76)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (87.37), maa://25199 (84.82), maa://30434 (90.91), ***maa://25036 (16.0), *maa://45059 (75.0), *maa://44165 (66.67)</t>
+          <t>maa://36670 (88.66), maa://25199 (84.82), maa://30434 (91.03), ***maa://25036 (16.0), *maa://45059 (78.57), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5405,7 +5405,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.72)</t>
+          <t>maa://24709 (91.22)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (83.05), maa://45790 (88.89)</t>
+          <t>maa://45788 (80.95), maa://45790 (81.82)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5490,7 +5490,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.78), maa://21386 (95.74), maa://36664 (90.91), maa://45550 (100.0)</t>
+          <t>maa://23278 (95.51), maa://21386 (95.77), maa://36664 (90.91), maa://45550 (100.0)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5575,7 +5575,7 @@
       </c>
       <c r="P41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (38.24), maa://43177 (89.47)</t>
+          <t>**maa://35616 (40.0), maa://43177 (90.48)</t>
         </is>
       </c>
       <c r="Q41" s="1" t="n"/>
@@ -5713,7 +5713,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (92.36), maa://21284 (85.11)</t>
+          <t>maa://22525 (92.36), maa://21284 (85.42)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5740,12 +5740,12 @@
       </c>
       <c r="S43" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="T43" s="2" t="inlineStr">
         <is>
-          <t>maa://43198 (100.0)</t>
+          <t>maa://43198 (100.0), maa://46286 (100.0)</t>
         </is>
       </c>
       <c r="U43" s="1" t="n"/>
@@ -5782,7 +5782,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.97), maa://27728 (96.08)</t>
+          <t>maa://29768 (97.99), maa://27728 (96.08)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5835,7 +5835,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.49), maa://30807 (95.65), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (84.21)</t>
+          <t>maa://21229 (84.57), maa://30807 (95.65), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (84.21)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5867,7 +5867,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (38.46)</t>
+          <t>**maa://39364 (37.93)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -5888,7 +5888,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.48), maa://43901 (88.89)</t>
+          <t>maa://35931 (92.53), maa://43901 (90.48)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5941,7 +5941,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.38), maa://29661 (97.24), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.41), maa://29661 (97.28), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6063,7 +6063,7 @@
       </c>
       <c r="P49" s="2" t="inlineStr">
         <is>
-          <t>*maa://39643 (65.38)</t>
+          <t>*maa://39643 (66.67)</t>
         </is>
       </c>
       <c r="Q49" s="1" t="n"/>
@@ -6234,7 +6234,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.79), **maa://32434 (33.33)</t>
+          <t>maa://32534 (93.87), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6270,7 +6270,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (91.96)</t>
+          <t>maa://32532 (92.07)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6306,7 +6306,7 @@
       </c>
       <c r="H57" s="2" t="inlineStr">
         <is>
-          <t>maa://25176 (98.31)</t>
+          <t>maa://25176 (98.36)</t>
         </is>
       </c>
       <c r="I57" s="1" t="n"/>
@@ -6324,7 +6324,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (54.84)</t>
+          <t>*maa://37964 (60.0)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>
@@ -6342,7 +6342,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (82.88), maa://31270 (95.24)</t>
+          <t>maa://27746 (83.04), maa://31270 (95.28)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6360,7 +6360,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (68.42)</t>
+          <t>*maa://40438 (67.24)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>
@@ -6396,7 +6396,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (97.3), maa://43903 (100.0)</t>
+          <t>maa://42981 (94.74), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#154)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.88), *maa://30515 (69.9), *maa://34787 (72.97), ***maa://20792 (11.93), maa://39402 (91.23), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.52), *maa://30515 (69.9), *maa://34787 (72.97), ***maa://20792 (11.93), maa://39402 (91.23), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.17), ***maa://21730 (25.68), ***maa://39501 (17.24), **maa://36675 (50.0)</t>
+          <t>maa://25251 (92.17), ***maa://21730 (25.33), ***maa://39501 (17.24), **maa://36675 (50.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.53), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.54), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.51), ***maa://31785 (22.22), maa://43217 (88.24), ***maa://36683 (28.26)</t>
+          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (88.24), ***maa://36683 (28.26)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.02.08 13:16:19</t>
+          <t>更新日期：2025.02.09 13:17:45</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.84)</t>
+          <t>maa://21411 (95.86)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.82), ***maa://34206 (20.0), ***maa://39951 (14.29), ***maa://39243 (28.57), *maa://45271 (56.0)</t>
+          <t>***maa://25695 (18.82), ***maa://34206 (20.0), ***maa://39951 (14.0), ***maa://39243 (28.57), *maa://45271 (56.0)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.01), maa://36673 (93.15), maa://25001 (85.71)</t>
+          <t>maa://24999 (92.02), maa://36673 (93.15), maa://25001 (85.71)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (33.57), maa://39883 (92.54), *maa://39885 (57.14)</t>
+          <t>**maa://22737 (33.33), maa://39883 (91.18), *maa://39885 (55.17)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.51), maa://22734 (84.03), *maa://30808 (64.18), **maa://36048 (44.07), maa://45058 (88.89)</t>
+          <t>*maa://22743 (77.51), maa://22734 (84.03), *maa://30808 (64.18), **maa://36048 (44.07), maa://45058 (90.0)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.17), *maa://36666 (79.05), *maa://22766 (68.97)</t>
+          <t>maa://21364 (81.17), *maa://36666 (79.25), *maa://22766 (68.38)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.4), maa://36679 (94.12), maa://37650 (97.06)</t>
+          <t>maa://21441 (96.4), maa://36679 (94.12), maa://37650 (97.14)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.87), *maa://28648 (69.12), maa://36674 (80.85)</t>
+          <t>maa://22729 (94.9), *maa://28648 (69.12), maa://36674 (80.85)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (64.76), maa://27755 (93.48)</t>
+          <t>*maa://23911 (65.09), maa://27755 (93.48)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.24), maa://25198 (93.4), *maa://20795 (51.16), maa://36680 (93.75)</t>
+          <t>maa://21432 (90.24), maa://25198 (93.46), *maa://20795 (51.16), maa://36680 (93.75)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.0)</t>
+          <t>maa://41331 (85.21)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="P20" s="2" t="inlineStr">
         <is>
-          <t>maa://37442 (95.0)</t>
+          <t>maa://37442 (95.12)</t>
         </is>
       </c>
       <c r="Q20" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.47), *maa://22432 (77.14)</t>
+          <t>maa://22524 (94.5), *maa://22432 (77.14)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (80.87), *maa://22751 (72.06)</t>
+          <t>maa://27127 (80.87), *maa://22751 (71.01)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3524,12 +3524,12 @@
       </c>
       <c r="C24" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.04)</t>
+          <t>*maa://24368 (78.04), **maa://46650 (50.0)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (84.74), maa://23504 (93.29), **maa://22892 (40.14), *maa://25141 (76.92), *maa://36663 (78.38), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (84.74), maa://23504 (93.29), **maa://22892 (40.14), *maa://25141 (76.92), *maa://36663 (78.67), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -4031,7 +4031,7 @@
       </c>
       <c r="AF27" s="2" t="inlineStr">
         <is>
-          <t>maa://24023 (97.22)</t>
+          <t>maa://24023 (97.26)</t>
         </is>
       </c>
       <c r="AG27" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.48), maa://41749 (90.0), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.5), maa://41749 (90.12), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.11), *maa://36701 (65.52)</t>
+          <t>maa://36660 (92.13), *maa://36701 (65.52)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4227,7 +4227,7 @@
       </c>
       <c r="P29" s="2" t="inlineStr">
         <is>
-          <t>*maa://23168 (58.06), *maa://30050 (53.12)</t>
+          <t>*maa://23168 (58.06), *maa://30050 (51.52)</t>
         </is>
       </c>
       <c r="Q29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.67), maa://45822 (100.0), *maa://45045 (80.0)</t>
+          <t>maa://42979 (96.71), maa://45822 (100.0), *maa://45045 (80.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.43), maa://41108 (88.0), maa://41238 (97.06), maa://45523 (100.0)</t>
+          <t>maa://42859 (96.49), maa://41108 (88.0), maa://41238 (97.09), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.05)</t>
+          <t>maa://41296 (96.13)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5187,7 +5187,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (99.01), maa://45789 (100.0)</t>
+          <t>maa://45718 (99.04), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5352,7 +5352,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.76)</t>
+          <t>maa://36697 (86.41)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (88.66), maa://25199 (84.82), maa://30434 (91.03), ***maa://25036 (16.0), *maa://45059 (78.57), *maa://44165 (66.67)</t>
+          <t>maa://36670 (88.66), maa://25199 (84.82), maa://30434 (91.03), ***maa://25036 (16.0), *maa://45059 (80.0), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (80.95), maa://45790 (81.82)</t>
+          <t>maa://45788 (81.4), maa://45790 (81.82)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5888,7 +5888,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.53), maa://43901 (90.48)</t>
+          <t>maa://35931 (92.56), maa://43901 (90.48)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5941,7 +5941,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.41), maa://29661 (97.28), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.42), maa://29661 (97.28), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6270,7 +6270,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.07)</t>
+          <t>maa://32532 (92.15)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6342,7 +6342,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (83.04), maa://31270 (95.28)</t>
+          <t>maa://27746 (82.3), maa://31270 (95.28)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#155)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.46), maa://25390 (96.14), maa://36681 (87.34)</t>
+          <t>maa://24702 (94.48), maa://25390 (96.14), maa://36681 (87.34)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.52), *maa://30515 (69.9), *maa://34787 (72.97), ***maa://20792 (11.93), maa://39402 (91.23), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.52), *maa://30515 (69.9), *maa://34787 (72.97), maa://39402 (91.23), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://36987 (96.0), maa://40192 (100.0), maa://39849 (88.89)</t>
+          <t>maa://36987 (96.08), maa://40192 (100.0), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.66), **maa://20790 (43.48), ***maa://37170 (16.92), maa://45854 (100.0)</t>
+          <t>maa://24617 (89.74), **maa://20790 (43.48), ***maa://37170 (16.92), maa://45854 (100.0)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -901,7 +901,7 @@
       </c>
       <c r="AF3" s="2" t="inlineStr">
         <is>
-          <t>*maa://21289 (73.91)</t>
+          <t>*maa://21289 (75.0)</t>
         </is>
       </c>
       <c r="AG3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.94), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (94.01), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (96.49), maa://27295 (85.71), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
+          <t>maa://32509 (96.52), maa://27295 (85.71), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (88.24), ***maa://36683 (28.26)</t>
+          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (88.68), ***maa://36683 (28.26)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.62), maa://22744 (84.0)</t>
+          <t>maa://21245 (84.68), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>maa://21955 (94.74)</t>
+          <t>maa://21955 (94.87)</t>
         </is>
       </c>
       <c r="E7" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (92.45), maa://24957 (97.73)</t>
+          <t>maa://28624 (92.52), maa://24957 (97.73)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.33), *maa://22758 (75.36)</t>
+          <t>maa://22399 (95.33), *maa://22758 (74.29)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.02.09 13:17:45</t>
+          <t>更新日期：2025.02.12 13:18:17</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>*maa://21476 (73.08), *maa://39431 (53.85), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (73.08), *maa://39431 (57.14), *maa://37551 (57.14)</t>
         </is>
       </c>
       <c r="E8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.86)</t>
+          <t>maa://21411 (95.88)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>maa://22762 (92.22), maa://39552 (81.82)</t>
+          <t>maa://22762 (92.22), *maa://39552 (75.0)</t>
         </is>
       </c>
       <c r="M9" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.79)</t>
+          <t>maa://26223 (97.83)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.18), ***maa://22740 (5.66), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (95.83), *maa://45044 (66.67)</t>
+          <t>maa://28711 (87.18), ***maa://22740 (5.66), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (96.0), *maa://45044 (66.67)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.82), ***maa://34206 (20.0), ***maa://39951 (14.0), ***maa://39243 (28.57), *maa://45271 (56.0)</t>
+          <t>***maa://25695 (18.82), ***maa://34206 (20.0), ***maa://39951 (15.69), ***maa://39243 (28.57), *maa://45271 (57.69)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (53.33), *maa://22733 (60.0), **maa://22761 (50.0)</t>
+          <t>*maa://25021 (53.85), *maa://22733 (60.0), **maa://22761 (50.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (93.04), maa://22501 (97.65), maa://45521 (81.82)</t>
+          <t>maa://22747 (93.08), maa://22501 (97.67), *maa://45521 (76.92)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.73)</t>
+          <t>maa://36713 (97.74)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (89.88), **maa://45826 (33.33)</t>
+          <t>maa://21867 (89.88), ***maa://45826 (25.0)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (90.91), *maa://21485 (76.26), maa://37962 (90.0)</t>
+          <t>maa://22753 (90.91), *maa://21485 (76.43), maa://37962 (90.24)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.47), maa://36677 (93.1), maa://39872 (91.3)</t>
+          <t>maa://23669 (95.49), maa://36677 (93.1), maa://39872 (91.3)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.32), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (77.93), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.02), maa://36673 (93.15), maa://25001 (85.71)</t>
+          <t>maa://24999 (92.03), maa://36673 (93.15), maa://25001 (85.71)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.08), **maa://22728 (47.73)</t>
+          <t>*maa://21248 (73.19), **maa://22728 (47.73)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (33.33), maa://39883 (91.18), *maa://39885 (55.17)</t>
+          <t>**maa://22737 (33.33), maa://39883 (91.18), *maa://39885 (53.33)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="T14" s="2" t="inlineStr">
         <is>
-          <t>maa://22521 (94.23), maa://42751 (100.0)</t>
+          <t>maa://22521 (94.29), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="1" t="n"/>
@@ -2309,7 +2309,7 @@
       </c>
       <c r="X14" s="2" t="inlineStr">
         <is>
-          <t>maa://37468 (90.48)</t>
+          <t>maa://37468 (90.91)</t>
         </is>
       </c>
       <c r="Y14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.51), maa://22734 (84.03), *maa://30808 (64.18), **maa://36048 (44.07), maa://45058 (90.0)</t>
+          <t>*maa://22743 (77.62), maa://22734 (84.17), *maa://30808 (64.18), **maa://36048 (44.07), maa://45058 (91.67)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2439,7 +2439,7 @@
       </c>
       <c r="X15" s="2" t="inlineStr">
         <is>
-          <t>maa://38786 (83.33)</t>
+          <t>maa://38786 (85.71)</t>
         </is>
       </c>
       <c r="Y15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.17), *maa://36666 (79.25), *maa://22766 (68.38)</t>
+          <t>maa://21364 (81.23), *maa://36666 (79.25), *maa://22766 (68.64)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.4), maa://36679 (94.12), maa://37650 (97.14)</t>
+          <t>maa://21441 (96.4), maa://36679 (94.23), maa://37650 (97.14)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.9), *maa://28648 (69.12), maa://36674 (80.85)</t>
+          <t>maa://22729 (94.94), *maa://28648 (69.12), maa://36674 (81.25)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.66), maa://39599 (85.42)</t>
+          <t>maa://22430 (88.66), maa://39599 (85.71)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.29)</t>
+          <t>maa://24570 (97.3)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (89.94), *maa://22732 (51.16)</t>
+          <t>maa://22466 (89.94), *maa://22732 (51.14)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.24), maa://25198 (93.46), *maa://20795 (51.16), maa://36680 (93.75)</t>
+          <t>maa://21432 (90.42), maa://25198 (93.58), *maa://20795 (51.16), maa://36680 (93.75)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.21)</t>
+          <t>maa://41331 (85.52)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3139,7 +3139,7 @@
       </c>
       <c r="D21" s="2" t="inlineStr">
         <is>
-          <t>maa://21261 (97.44)</t>
+          <t>maa://21261 (97.5)</t>
         </is>
       </c>
       <c r="E21" s="1" t="n"/>
@@ -3155,7 +3155,7 @@
       </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>maa://24372 (96.88)</t>
+          <t>maa://24372 (96.94)</t>
         </is>
       </c>
       <c r="I21" s="1" t="n"/>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="X21" s="2" t="inlineStr">
         <is>
-          <t>maa://20110 (86.76), maa://34946 (92.86)</t>
+          <t>maa://20110 (86.76), maa://34946 (93.02)</t>
         </is>
       </c>
       <c r="Y21" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (80.91), ***maa://23820 (29.31)</t>
+          <t>maa://21443 (80.97), ***maa://23820 (30.0)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.5), *maa://22432 (77.14)</t>
+          <t>maa://22524 (94.5), *maa://22432 (77.78)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.58), *maa://37649 (67.86)</t>
+          <t>maa://21282 (98.59), *maa://37649 (65.52)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.47), maa://39875 (94.37)</t>
+          <t>maa://39756 (95.51), maa://39875 (94.37)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="X23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (67.95)</t>
+          <t>*maa://28503 (68.35)</t>
         </is>
       </c>
       <c r="Y23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.04), **maa://46650 (50.0)</t>
+          <t>*maa://24368 (78.16), **maa://46650 (50.0)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (84.74), maa://23504 (93.29), **maa://22892 (40.14), *maa://25141 (76.92), *maa://36663 (78.67), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (84.92), maa://23504 (93.08), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (77.63), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.86), maa://36672 (80.36), maa://29910 (92.98), **maa://21440 (35.71), *maa://45831 (75.0)</t>
+          <t>maa://22523 (85.93), maa://36672 (80.36), maa://29910 (92.98), **maa://21440 (35.71), *maa://45831 (75.0)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.08)</t>
+          <t>maa://29753 (95.09)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (74.05), *maa://25311 (73.53), ***maa://22725 (4.84), *maa://45047 (62.5)</t>
+          <t>*maa://29063 (74.21), *maa://25311 (73.53), ***maa://22725 (4.84), *maa://45047 (62.5)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (94.68)</t>
+          <t>maa://42235 (94.74)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (47.37), *maa://39601 (77.78), maa://34494 (97.14), **maa://36665 (50.0)</t>
+          <t>**maa://21283 (47.37), *maa://39601 (78.95), maa://34494 (97.14), **maa://36665 (50.0)</t>
         </is>
       </c>
       <c r="I27" s="1" t="n"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (77.97)</t>
+          <t>*maa://30624 (78.33)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (91.07), maa://25725 (83.72)</t>
+          <t>maa://24465 (91.1), maa://25725 (83.72)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.5), maa://41749 (90.12), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.53), maa://41749 (90.36), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.39), *maa://28440 (79.25), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.39), *maa://28440 (79.44), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.77), maa://42865 (81.82), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.77), maa://42865 (81.03), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4341,7 +4341,7 @@
       </c>
       <c r="L30" s="2" t="inlineStr">
         <is>
-          <t>maa://30442 (95.16)</t>
+          <t>maa://30442 (95.24)</t>
         </is>
       </c>
       <c r="M30" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.71), maa://45822 (100.0), *maa://45045 (80.0)</t>
+          <t>maa://42979 (96.77), maa://45822 (100.0), *maa://45045 (80.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.33), maa://36258 (84.82), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.36), maa://36258 (84.96), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.5), maa://36667 (98.67), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.5), maa://36667 (98.72), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.49), maa://41108 (88.0), maa://41238 (97.09), maa://45523 (100.0)</t>
+          <t>maa://42859 (96.52), maa://41108 (88.0), maa://41238 (97.09), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -5187,7 +5187,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (99.04), maa://45789 (100.0)</t>
+          <t>maa://45718 (99.11), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5352,7 +5352,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.41)</t>
+          <t>maa://36697 (86.06)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (88.66), maa://25199 (84.82), maa://30434 (91.03), ***maa://25036 (16.0), *maa://45059 (80.0), *maa://44165 (66.67)</t>
+          <t>maa://36670 (88.89), maa://25199 (84.82), maa://30434 (91.14), ***maa://25036 (16.0), maa://45059 (81.25), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5405,7 +5405,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.22)</t>
+          <t>maa://24709 (91.33)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (81.4), maa://45790 (81.82)</t>
+          <t>maa://45788 (82.02), maa://45790 (81.82)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5490,7 +5490,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.51), maa://21386 (95.77), maa://36664 (90.91), maa://45550 (100.0)</t>
+          <t>maa://23278 (95.53), maa://21386 (95.77), maa://36664 (89.29), maa://45550 (100.0)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5835,7 +5835,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.57), maa://30807 (95.65), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (84.21)</t>
+          <t>maa://21229 (84.66), maa://30807 (95.65), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (84.21)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5867,7 +5867,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (37.93)</t>
+          <t>**maa://39364 (36.67)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -5888,7 +5888,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.56), maa://43901 (90.48)</t>
+          <t>maa://35931 (92.63), maa://43901 (91.67)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5941,7 +5941,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.42), maa://29661 (97.28), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.43), maa://29661 (97.3), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6234,7 +6234,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.87), **maa://32434 (33.33)</t>
+          <t>maa://32534 (93.9), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6270,7 +6270,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.15)</t>
+          <t>maa://32532 (92.23)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6342,7 +6342,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://27746 (82.3), maa://31270 (95.28)</t>
+          <t>maa://31270 (95.28), maa://27746 (82.3)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6360,7 +6360,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (67.24)</t>
+          <t>*maa://40438 (67.8)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>
@@ -6396,7 +6396,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (94.74), maa://43903 (100.0)</t>
+          <t>maa://42981 (94.87), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#156)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.48), maa://25390 (96.14), maa://36681 (87.34)</t>
+          <t>maa://24702 (94.48), maa://25390 (96.15), maa://36681 (87.34)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.52), *maa://30515 (69.9), *maa://34787 (72.97), maa://39402 (91.23), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.52), *maa://30515 (69.9), *maa://34787 (73.33), maa://39402 (91.53), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.41), maa://36684 (95.41), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.41), maa://36684 (95.5), ***maa://22731 (6.67)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.54), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.55), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (66.15), maa://20276 (86.36), *maa://22749 (72.73)</t>
+          <t>*maa://22880 (65.82), maa://20276 (86.44), *maa://22749 (72.73)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.42), maa://26254 (96.43)</t>
+          <t>maa://21249 (94.42), maa://26254 (96.55)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.38), maa://27484 (96.55), maa://27480 (82.86)</t>
+          <t>maa://27396 (84.16), maa://27484 (96.55), maa://27480 (83.33)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (94.01), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (94.08), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (96.52), maa://27295 (85.71), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
+          <t>maa://32509 (96.55), maa://27295 (85.71), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (88.68), ***maa://36683 (28.26)</t>
+          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (89.09), ***maa://36683 (28.26)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.68), maa://22744 (84.0)</t>
+          <t>maa://21245 (84.81), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (92.52), maa://24957 (97.73)</t>
+          <t>maa://28624 (92.59), maa://24957 (97.73)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (68.24), *maa://36671 (68.0), *maa://42530 (62.5), maa://45272 (100.0)</t>
+          <t>*maa://26191 (68.24), *maa://36671 (68.0), maa://45272 (100.0), *maa://42530 (62.5)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.02.12 13:18:17</t>
+          <t>更新日期：2025.02.14 13:17:46</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (83.48), *maa://21916 (61.54), maa://23252 (91.18), maa://37496 (96.77), **maa://22759 (45.45)</t>
+          <t>maa://32931 (83.62), *maa://21916 (61.54), maa://23252 (91.18), maa://37496 (96.77), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.88)</t>
+          <t>maa://21411 (95.91)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="AF8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24479 (77.91), *maa://21990 (51.85)</t>
+          <t>*maa://24479 (78.16), *maa://21990 (51.85)</t>
         </is>
       </c>
       <c r="AG8" s="1" t="n"/>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>maa://22762 (92.22), *maa://39552 (75.0)</t>
+          <t>maa://22762 (92.31), *maa://39552 (75.0)</t>
         </is>
       </c>
       <c r="M9" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.83)</t>
+          <t>maa://26223 (97.84)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.82), ***maa://34206 (20.0), ***maa://39951 (15.69), ***maa://39243 (28.57), *maa://45271 (57.69)</t>
+          <t>***maa://25695 (18.82), ***maa://34206 (20.0), ***maa://39951 (15.69), ***maa://39243 (28.57), *maa://45271 (57.14)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="H10" s="2" t="inlineStr">
         <is>
-          <t>maa://32651 (93.75)</t>
+          <t>maa://32651 (94.12)</t>
         </is>
       </c>
       <c r="I10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.74), maa://22726 (100.0), maa://45828 (100.0)</t>
+          <t>maa://22301 (97.75), maa://22726 (100.0), maa://45828 (88.89)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1935,7 +1935,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://29912 (98.53), maa://22516 (88.37), *maa://20794 (52.24)</t>
+          <t>maa://29912 (97.14), maa://22516 (88.37), *maa://20794 (52.24)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>maa://30766 (89.29), *maa://36678 (66.67)</t>
+          <t>maa://30766 (89.29), *maa://36678 (71.43)</t>
         </is>
       </c>
       <c r="E12" s="1" t="n"/>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (89.88), ***maa://45826 (25.0)</t>
+          <t>maa://21867 (89.88), ***maa://45826 (20.0)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.49), maa://36677 (93.1), maa://39872 (91.3)</t>
+          <t>maa://23669 (95.5), maa://36677 (93.1), maa://39872 (91.67)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (77.93), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (77.4), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.03), maa://36673 (93.15), maa://25001 (85.71)</t>
+          <t>maa://24999 (92.04), maa://36673 (93.24), maa://25001 (85.71)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (33.33), maa://39883 (91.18), *maa://39885 (53.33)</t>
+          <t>**maa://22737 (33.33), maa://39883 (91.3), *maa://39885 (53.33)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.62), maa://22734 (84.17), *maa://30808 (64.18), **maa://36048 (44.07), maa://45058 (91.67)</t>
+          <t>*maa://22743 (77.62), maa://22734 (84.17), *maa://30808 (64.18), **maa://36048 (45.0), maa://45058 (91.67)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (87.85), maa://21478 (89.19)</t>
+          <t>maa://24304 (87.91), maa://21478 (89.19)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.23), *maa://36666 (79.25), *maa://22766 (68.64)</t>
+          <t>maa://21364 (81.1), *maa://36666 (78.5), *maa://22766 (68.64)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.94), *maa://28648 (69.12), maa://36674 (81.25)</t>
+          <t>maa://22729 (94.94), *maa://28648 (69.12), maa://36674 (82.35)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.66), maa://39599 (85.71)</t>
+          <t>maa://22430 (88.66), maa://39599 (86.0)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.3)</t>
+          <t>maa://24570 (97.31)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (89.33)</t>
+          <t>maa://24421 (88.98)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (89.94), *maa://22732 (51.14)</t>
+          <t>maa://22466 (90.0), *maa://22732 (51.14)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="X18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (96.88), maa://22741 (85.71)</t>
+          <t>maa://21917 (96.91), maa://22741 (85.71)</t>
         </is>
       </c>
       <c r="Y18" s="1" t="n"/>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (59.39), **maa://29784 (46.43)</t>
+          <t>*maa://24313 (59.64), **maa://29784 (46.43)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (65.2), *maa://36668 (57.5)</t>
+          <t>*maa://30709 (65.28), *maa://36668 (57.5)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.52)</t>
+          <t>maa://41331 (85.62)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.59), *maa://37649 (65.52)</t>
+          <t>maa://21282 (98.6), *maa://37649 (65.52)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.51), maa://39875 (94.37)</t>
+          <t>maa://39756 (95.54), maa://39875 (94.37)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.09)</t>
+          <t>maa://29753 (95.11)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (74.21), *maa://25311 (73.53), ***maa://22725 (4.84), *maa://45047 (62.5)</t>
+          <t>*maa://29063 (73.75), *maa://25311 (73.53), ***maa://22725 (4.84), *maa://45047 (62.5)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3869,7 +3869,7 @@
       </c>
       <c r="X26" s="2" t="inlineStr">
         <is>
-          <t>maa://24389 (96.43)</t>
+          <t>maa://24389 (96.55)</t>
         </is>
       </c>
       <c r="Y26" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>maa://23263 (95.19), *maa://29765 (63.41)</t>
+          <t>maa://23263 (95.24), *maa://29765 (63.41)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.53), maa://41749 (90.36), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.55), maa://41749 (90.36), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.13), *maa://36701 (65.52)</t>
+          <t>maa://36660 (92.15), *maa://36701 (65.52)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.39), *maa://28440 (79.44), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.41), *maa://28440 (79.44), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.77), maa://42865 (81.03), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.85), maa://42865 (81.03), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.36), maa://36258 (84.96), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.38), maa://36258 (84.96), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.5), maa://36667 (98.72), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.5), maa://36667 (98.73), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -5187,7 +5187,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (99.11), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.32), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5352,7 +5352,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.06)</t>
+          <t>maa://36697 (86.12)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (82.02), maa://45790 (81.82)</t>
+          <t>maa://45788 (82.42), maa://45790 (81.82)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5490,7 +5490,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.53), maa://21386 (95.77), maa://36664 (89.29), maa://45550 (100.0)</t>
+          <t>maa://23278 (95.54), maa://21386 (95.77), maa://36664 (89.29), maa://45550 (100.0)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -6270,7 +6270,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.23)</t>
+          <t>maa://32532 (92.26)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6324,7 +6324,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (60.0)</t>
+          <t>*maa://37964 (61.11)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>
@@ -6342,7 +6342,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://31270 (95.28), maa://27746 (82.3)</t>
+          <t>maa://31270 (95.31), maa://27746 (82.3)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#157)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -467,7 +467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG73"/>
+  <dimension ref="A1:AG74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.48), maa://25390 (96.15), maa://36681 (87.34)</t>
+          <t>maa://24702 (94.48), maa://25390 (96.17), maa://36681 (87.34)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.52), *maa://30515 (69.9), *maa://34787 (73.33), maa://39402 (91.53), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.52), *maa://30515 (69.9), *maa://34787 (73.33), maa://39402 (91.67), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.17), ***maa://21730 (25.33), ***maa://39501 (17.24), **maa://36675 (50.0)</t>
+          <t>maa://25251 (92.24), ***maa://21730 (25.33), ***maa://39501 (17.24), **maa://36675 (50.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.74), **maa://20790 (43.48), ***maa://37170 (16.92), maa://45854 (100.0)</t>
+          <t>maa://24617 (89.74), **maa://20790 (43.48), ***maa://37170 (16.92), maa://45854 (93.75)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -901,7 +901,7 @@
       </c>
       <c r="AF3" s="2" t="inlineStr">
         <is>
-          <t>*maa://21289 (75.0)</t>
+          <t>*maa://21289 (72.0)</t>
         </is>
       </c>
       <c r="AG3" s="1" t="n"/>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>maa://24839 (98.99)</t>
+          <t>maa://24839 (99.0)</t>
         </is>
       </c>
       <c r="M6" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.02.14 13:17:46</t>
+          <t>更新日期：2025.02.15 13:17:50</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.18), ***maa://22740 (5.66), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (96.0), *maa://45044 (66.67)</t>
+          <t>maa://28711 (87.39), ***maa://22740 (5.66), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (96.0), *maa://45044 (66.67)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.82), ***maa://34206 (20.0), ***maa://39951 (15.69), ***maa://39243 (28.57), *maa://45271 (57.14)</t>
+          <t>***maa://25695 (18.72), ***maa://34206 (20.0), ***maa://39951 (15.69), ***maa://39243 (28.57), *maa://45271 (57.14)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.75), maa://22726 (100.0), maa://45828 (88.89)</t>
+          <t>maa://22301 (97.75), maa://45828 (88.89), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (53.85), *maa://22733 (60.0), **maa://22761 (50.0)</t>
+          <t>*maa://25021 (54.35), *maa://22733 (60.0), **maa://22761 (50.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (93.08), maa://22501 (97.67), *maa://45521 (76.92)</t>
+          <t>maa://22747 (93.08), maa://22501 (97.67), *maa://45521 (78.57)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.04), maa://36673 (93.24), maa://25001 (85.71)</t>
+          <t>maa://24999 (92.05), maa://36673 (93.24), maa://25001 (85.71)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (33.33), maa://39883 (91.3), *maa://39885 (53.33)</t>
+          <t>**maa://22737 (33.33), maa://39883 (91.43), *maa://39885 (53.33)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.67), maa://21288 (96.3), maa://39841 (95.96), maa://36682 (97.44)</t>
+          <t>maa://26245 (96.69), maa://21288 (96.3), maa://39841 (96.0), maa://36682 (97.44)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (65.28), *maa://36668 (57.5)</t>
+          <t>*maa://30709 (65.36), *maa://36668 (57.5)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.42), maa://25198 (93.58), *maa://20795 (51.16), maa://36680 (93.75)</t>
+          <t>maa://21432 (90.48), maa://25198 (93.58), *maa://20795 (51.16), maa://36680 (93.94)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.5), *maa://22432 (77.78)</t>
+          <t>maa://22524 (94.5), *maa://22432 (76.71)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>maa://25236 (96.63), **maa://21678 (48.94), **maa://22735 (42.86)</t>
+          <t>maa://25236 (96.67), **maa://21678 (48.94), **maa://22735 (42.86)</t>
         </is>
       </c>
       <c r="I22" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (84.92), maa://23504 (93.08), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (77.63), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (84.92), maa://23504 (93.1), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (77.63), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (94.74)</t>
+          <t>maa://42235 (94.79)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>maa://23263 (95.24), *maa://29765 (63.41)</t>
+          <t>maa://23263 (95.28), *maa://29765 (63.41)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.55), maa://41749 (90.36), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.55), maa://41749 (90.48), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.41), *maa://28440 (79.44), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.43), *maa://28440 (79.63), maa://31400 (100.0), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4389,7 +4389,7 @@
       </c>
       <c r="X30" s="2" t="inlineStr">
         <is>
-          <t>maa://39477 (88.89)</t>
+          <t>maa://39477 (90.0)</t>
         </is>
       </c>
       <c r="Y30" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.5), maa://36667 (98.73), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.5), maa://36667 (97.53), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4897,6 +4897,22 @@
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
+      <c r="V34" s="1" t="inlineStr">
+        <is>
+          <t>诺威尔</t>
+        </is>
+      </c>
+      <c r="W34" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X34" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y34" s="1" t="n"/>
       <c r="Z34" s="1" t="inlineStr">
         <is>
           <t>海霓</t>
@@ -5187,7 +5203,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (98.32), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.33), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5352,7 +5368,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.12)</t>
+          <t>maa://36697 (86.19)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5373,7 +5389,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (88.89), maa://25199 (84.82), maa://30434 (91.14), ***maa://25036 (16.0), maa://45059 (81.25), *maa://44165 (66.67)</t>
+          <t>maa://36670 (88.89), maa://25199 (84.82), maa://30434 (91.25), ***maa://25036 (16.0), maa://45059 (81.25), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5405,7 +5421,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.33)</t>
+          <t>maa://24709 (91.39)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5421,7 +5437,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (82.42), maa://45790 (81.82)</t>
+          <t>maa://45788 (82.61), maa://45790 (81.82)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5782,7 +5798,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (97.99), maa://27728 (96.08)</t>
+          <t>maa://29768 (98.0), maa://27728 (96.08)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5835,7 +5851,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.66), maa://30807 (95.65), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (84.21)</t>
+          <t>maa://21229 (84.74), maa://30807 (95.65), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (84.21)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -6234,7 +6250,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.9), **maa://32434 (33.33)</t>
+          <t>maa://32534 (93.92), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6270,7 +6286,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.26)</t>
+          <t>maa://32532 (92.28)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6396,7 +6412,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (94.87), maa://43903 (100.0)</t>
+          <t>maa://42981 (95.0), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>
@@ -6598,6 +6614,24 @@
         </is>
       </c>
       <c r="I73" s="1" t="n"/>
+    </row>
+    <row r="74">
+      <c r="F74" s="1" t="inlineStr">
+        <is>
+          <t>隐德来希</t>
+        </is>
+      </c>
+      <c r="G74" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H74" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I74" s="1" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
CI: Auto Update Data (#158)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.41), maa://36684 (95.5), ***maa://22731 (6.67)</t>
+          <t>maa://21246 (91.41), maa://36684 (95.5), ***maa://22731 (6.25)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.24), ***maa://21730 (25.33), ***maa://39501 (17.24), **maa://36675 (50.0)</t>
+          <t>maa://25251 (92.31), ***maa://21730 (25.33), ***maa://39501 (16.67), **maa://36675 (50.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.42), maa://26254 (96.55)</t>
+          <t>maa://21249 (94.44), maa://26254 (96.55)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.74), **maa://20790 (43.48), ***maa://37170 (16.92), maa://45854 (93.75)</t>
+          <t>maa://24617 (89.74), **maa://20790 (43.48), ***maa://37170 (16.92), maa://45854 (88.24)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (94.52)</t>
+          <t>maa://24390 (94.59)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (89.09), ***maa://36683 (28.26)</t>
+          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (89.29), ***maa://36683 (28.26)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (64.0), ***maa://26209 (13.04), *maa://39394 (66.67)</t>
+          <t>*maa://30062 (64.0), ***maa://26209 (13.04), *maa://39394 (64.0)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="AB5" s="2" t="inlineStr">
         <is>
-          <t>*maa://29863 (66.67), ***maa://22752 (12.5), **maa://26013 (37.5)</t>
+          <t>*maa://29863 (64.86), ***maa://22752 (12.5), **maa://26013 (37.5)</t>
         </is>
       </c>
       <c r="AC5" s="1" t="n"/>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="P7" s="2" t="inlineStr">
         <is>
-          <t>maa://22750 (91.49)</t>
+          <t>maa://22750 (91.67)</t>
         </is>
       </c>
       <c r="Q7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.02.15 13:17:50</t>
+          <t>更新日期：2025.02.15 19:34:59</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.91)</t>
+          <t>maa://21411 (95.92)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.84)</t>
+          <t>maa://26223 (97.87)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (89.17), *maa://22865 (50.94)</t>
+          <t>maa://26206 (88.43), *maa://22865 (50.94)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.72), ***maa://34206 (20.0), ***maa://39951 (15.69), ***maa://39243 (28.57), *maa://45271 (57.14)</t>
+          <t>***maa://25695 (18.72), ***maa://34206 (20.0), ***maa://39951 (15.69), ***maa://39243 (25.0), *maa://45271 (55.17)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.75), maa://45828 (88.89), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.75), maa://45828 (90.0), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.5), maa://36677 (93.1), maa://39872 (91.67)</t>
+          <t>maa://23669 (95.5), maa://36677 (93.22), maa://39872 (91.67)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>maa://34957 (82.19), *maa://22768 (51.61)</t>
+          <t>maa://34957 (82.43), *maa://22768 (51.61)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.4), maa://36679 (94.23), maa://37650 (97.14)</t>
+          <t>maa://21441 (96.4), maa://36679 (94.34), maa://37650 (97.14)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.94), *maa://28648 (69.12), maa://36674 (82.35)</t>
+          <t>maa://22729 (94.97), *maa://28648 (69.12), maa://36674 (82.69)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (98.0), maa://28051 (96.0)</t>
+          <t>maa://28501 (98.02), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.88)</t>
+          <t>maa://26228 (95.92)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (65.09), maa://27755 (93.48)</t>
+          <t>*maa://23911 (65.09), maa://27755 (93.55)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.31)</t>
+          <t>maa://24570 (97.32)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (90.0), *maa://22732 (51.14)</t>
+          <t>maa://22466 (90.06), *maa://22732 (51.14)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.48), maa://25198 (93.58), *maa://20795 (51.16), maa://36680 (93.94)</t>
+          <t>maa://21432 (89.94), maa://25198 (93.58), *maa://20795 (50.77), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.62)</t>
+          <t>maa://41331 (85.71)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3139,7 +3139,7 @@
       </c>
       <c r="D21" s="2" t="inlineStr">
         <is>
-          <t>maa://21261 (97.5)</t>
+          <t>maa://21261 (97.56)</t>
         </is>
       </c>
       <c r="E21" s="1" t="n"/>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (29.17), *maa://41753 (53.33)</t>
+          <t>***maa://28036 (28.77), *maa://41753 (56.25)</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.54), maa://39875 (94.37)</t>
+          <t>maa://39756 (95.55), maa://39875 (94.37)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (84.92), maa://23504 (93.1), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (77.63), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (84.58), maa://23504 (93.1), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (77.63), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (87.5), maa://24516 (80.22), maa://26001 (87.5)</t>
+          <t>maa://31215 (87.61), maa://24516 (80.22), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>maa://41802 (93.33)</t>
+          <t>maa://41802 (93.75)</t>
         </is>
       </c>
       <c r="E26" s="1" t="n"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (92.05)</t>
+          <t>maa://24913 (92.13)</t>
         </is>
       </c>
       <c r="I26" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (94.79)</t>
+          <t>maa://42235 (94.85)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (47.37), *maa://39601 (78.95), maa://34494 (97.14), **maa://36665 (50.0)</t>
+          <t>**maa://21283 (47.37), *maa://39601 (80.0), maa://34494 (97.14), **maa://36665 (50.0)</t>
         </is>
       </c>
       <c r="I27" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.55), maa://41749 (90.48), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.6), maa://41749 (90.48), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4179,7 +4179,7 @@
       </c>
       <c r="D29" s="2" t="inlineStr">
         <is>
-          <t>maa://31694 (98.11)</t>
+          <t>maa://31694 (98.15)</t>
         </is>
       </c>
       <c r="E29" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.43), *maa://28440 (79.63), maa://31400 (100.0), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.43), *maa://28440 (79.63), maa://31400 (98.81), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.52), maa://41108 (88.0), maa://41238 (97.09), maa://45523 (100.0)</t>
+          <t>maa://42859 (95.69), maa://41108 (88.0), maa://41238 (97.09), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4991,7 +4991,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.13)</t>
+          <t>maa://41296 (96.18)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5203,7 +5203,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (98.33), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.35), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.39)</t>
+          <t>maa://24709 (91.45)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5432,12 +5432,12 @@
       </c>
       <c r="S39" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (82.61), maa://45790 (81.82)</t>
+          <t>maa://45788 (82.8), *maa://45790 (75.0), **maa://47079 (50.0)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5798,7 +5798,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (98.0), maa://27728 (96.08)</t>
+          <t>maa://29768 (98.01), maa://27728 (96.08)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5904,7 +5904,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.63), maa://43901 (91.67)</t>
+          <t>maa://35931 (92.63), maa://43901 (92.0)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5957,7 +5957,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.43), maa://29661 (97.3), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.44), maa://29661 (97.3), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6412,7 +6412,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (95.0), maa://43903 (100.0)</t>
+          <t>maa://42981 (95.12), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#159)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.48), maa://25390 (96.17), maa://36681 (87.34)</t>
+          <t>maa://24702 (94.48), maa://25390 (96.18), maa://36681 (87.34)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.52), *maa://30515 (69.9), *maa://34787 (73.33), maa://39402 (91.67), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.52), *maa://30515 (69.9), *maa://34787 (73.33), maa://39402 (91.8), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.55), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.56), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.44), maa://26254 (96.55)</t>
+          <t>maa://21249 (94.47), maa://26254 (96.55)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (89.29), ***maa://36683 (28.26)</t>
+          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (89.47), ***maa://36683 (28.26)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (95.83)</t>
+          <t>maa://42407 (95.92)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1280,7 +1280,7 @@
       </c>
       <c r="AB6" s="2" t="inlineStr">
         <is>
-          <t>maa://22739 (92.98)</t>
+          <t>maa://22739 (91.38)</t>
         </is>
       </c>
       <c r="AC6" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.33), *maa://22758 (74.29)</t>
+          <t>maa://22399 (95.36), *maa://22758 (74.29)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.02.15 19:34:59</t>
+          <t>更新日期：2025.02.16 13:17:39</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.92)</t>
+          <t>maa://21411 (95.93)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>maa://22765 (92.55), *maa://21915 (70.37)</t>
+          <t>maa://22765 (91.58), *maa://21915 (67.86)</t>
         </is>
       </c>
       <c r="E9" s="1" t="n"/>
@@ -1643,7 +1643,7 @@
       </c>
       <c r="T9" s="2" t="inlineStr">
         <is>
-          <t>**maa://22866 (30.19), maa://26222 (98.0)</t>
+          <t>**maa://22866 (30.19), maa://26222 (98.04)</t>
         </is>
       </c>
       <c r="U9" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.87)</t>
+          <t>maa://26223 (97.89)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.72), ***maa://34206 (20.0), ***maa://39951 (15.69), ***maa://39243 (25.0), *maa://45271 (55.17)</t>
+          <t>***maa://25695 (18.72), ***maa://39951 (15.69), ***maa://34206 (20.0), ***maa://39243 (25.0), *maa://45271 (55.17)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (90.36), maa://36669 (88.1), *maa://23264 (61.82)</t>
+          <t>maa://28977 (90.48), maa://36669 (86.36), *maa://23264 (61.82)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (54.35), *maa://22733 (60.0), **maa://22761 (50.0)</t>
+          <t>*maa://25021 (53.76), *maa://22733 (60.0), **maa://22761 (50.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.47)</t>
+          <t>maa://36707 (99.48)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (88.89)</t>
+          <t>maa://21287 (89.11)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.74)</t>
+          <t>maa://36713 (97.75)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.05), maa://36673 (93.24), maa://25001 (85.71)</t>
+          <t>maa://24999 (92.08), maa://36673 (93.24), maa://25001 (85.71)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>maa://34957 (82.43), *maa://22768 (51.61)</t>
+          <t>maa://34957 (81.33), *maa://22768 (51.61)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.69), maa://21288 (96.3), maa://39841 (96.0), maa://36682 (97.44)</t>
+          <t>maa://26245 (96.71), maa://21288 (96.3), maa://39841 (95.05), maa://36682 (97.44)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.73), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.74), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.62), maa://22734 (84.17), *maa://30808 (64.18), **maa://36048 (45.0), maa://45058 (91.67)</t>
+          <t>*maa://22743 (77.73), maa://22734 (84.17), *maa://30808 (64.18), **maa://36048 (45.0), maa://45058 (91.67)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2667,7 +2667,7 @@
       </c>
       <c r="P17" s="2" t="inlineStr">
         <is>
-          <t>maa://23890 (81.37), *maa://24940 (67.86)</t>
+          <t>maa://23890 (80.58), *maa://24940 (67.86)</t>
         </is>
       </c>
       <c r="Q17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.32)</t>
+          <t>maa://24570 (97.33)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (59.64), **maa://29784 (46.43)</t>
+          <t>*maa://24313 (59.28), **maa://29784 (46.43)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (65.36), *maa://36668 (57.5)</t>
+          <t>*maa://30709 (65.52), *maa://36668 (57.5)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (89.94), maa://25198 (93.58), *maa://20795 (50.77), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.0), maa://25198 (93.58), *maa://20795 (50.77), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.71)</t>
+          <t>maa://41331 (85.23)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3187,7 +3187,7 @@
       </c>
       <c r="P21" s="2" t="inlineStr">
         <is>
-          <t>maa://24381 (88.89)</t>
+          <t>maa://24381 (84.21)</t>
         </is>
       </c>
       <c r="Q21" s="1" t="n"/>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="X21" s="2" t="inlineStr">
         <is>
-          <t>maa://20110 (86.76), maa://34946 (93.02)</t>
+          <t>maa://20110 (86.76), maa://34946 (90.91)</t>
         </is>
       </c>
       <c r="Y21" s="1" t="n"/>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>maa://25236 (96.67), **maa://21678 (48.94), **maa://22735 (42.86)</t>
+          <t>maa://25236 (95.6), **maa://21678 (48.94), **maa://22735 (42.86)</t>
         </is>
       </c>
       <c r="I22" s="1" t="n"/>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.77), *maa://41753 (56.25)</t>
+          <t>***maa://28036 (28.77), *maa://41753 (58.82)</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.55), maa://39875 (94.37)</t>
+          <t>maa://39756 (95.56), maa://39875 (94.37)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.84), *maa://29748 (75.78), ***maa://29785 (16.42), *maa://37566 (76.32)</t>
+          <t>maa://30587 (91.84), *maa://29748 (75.97), ***maa://29785 (16.18), *maa://37566 (76.32)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (84.58), maa://23504 (93.1), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (77.63), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (84.58), maa://23504 (93.11), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (77.63), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.11)</t>
+          <t>maa://29753 (95.13)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3723,7 +3723,7 @@
       </c>
       <c r="T25" s="2" t="inlineStr">
         <is>
-          <t>maa://20109 (92.05), maa://22545 (100.0), *maa://42915 (75.0)</t>
+          <t>maa://20109 (92.09), maa://22545 (100.0), *maa://42915 (75.0)</t>
         </is>
       </c>
       <c r="U25" s="1" t="n"/>
@@ -3739,7 +3739,7 @@
       </c>
       <c r="X25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29890 (78.26)</t>
+          <t>*maa://29890 (78.72)</t>
         </is>
       </c>
       <c r="Y25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (87.61), maa://24516 (80.22), maa://26001 (87.5)</t>
+          <t>maa://31215 (87.72), maa://24516 (80.22), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (94.85)</t>
+          <t>maa://42235 (93.94)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (91.1), maa://25725 (83.72)</t>
+          <t>maa://24465 (90.98), maa://25725 (83.72)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.6), maa://41749 (90.48), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.62), maa://41749 (90.59), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.15), *maa://36701 (65.52)</t>
+          <t>maa://36660 (92.15), *maa://36701 (66.67)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.85), maa://42865 (81.03), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.85), maa://42865 (81.67), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.77), maa://45822 (100.0), *maa://45045 (80.0)</t>
+          <t>maa://42979 (96.84), maa://45822 (100.0), *maa://45045 (80.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.38), maa://36258 (84.96), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.43), maa://36258 (84.96), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.5), maa://36667 (97.53), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.5), maa://36667 (97.56), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (95.69), maa://41108 (88.0), maa://41238 (97.09), maa://45523 (100.0)</t>
+          <t>maa://42859 (95.76), maa://41108 (88.0), maa://41238 (97.09), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4763,7 +4763,7 @@
       </c>
       <c r="T33" s="2" t="inlineStr">
         <is>
-          <t>maa://45558 (100.0)</t>
+          <t>maa://45558 (87.5)</t>
         </is>
       </c>
       <c r="U33" s="1" t="n"/>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (93.36)</t>
+          <t>maa://24526 (93.02)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4991,7 +4991,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.18)</t>
+          <t>maa://41296 (96.2)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5198,12 +5198,12 @@
       </c>
       <c r="K37" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (98.35), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.35), maa://45789 (100.0), maa://47069 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5368,7 +5368,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.19)</t>
+          <t>maa://36697 (86.26)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5389,7 +5389,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (88.89), maa://25199 (84.82), maa://30434 (91.25), ***maa://25036 (16.0), maa://45059 (81.25), *maa://44165 (66.67)</t>
+          <t>maa://36670 (88.89), maa://25199 (84.82), maa://30434 (91.36), ***maa://25036 (16.0), maa://45059 (81.25), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5416,12 +5416,12 @@
       </c>
       <c r="O39" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.45)</t>
+          <t>maa://24709 (91.5), maa://47093 (100.0)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5437,7 +5437,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (82.8), *maa://45790 (75.0), **maa://47079 (50.0)</t>
+          <t>maa://45788 (81.91), *maa://45790 (75.0), *maa://47079 (75.0)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5591,7 +5591,7 @@
       </c>
       <c r="P41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (40.0), maa://43177 (90.48)</t>
+          <t>**maa://35616 (40.0), maa://43177 (90.91)</t>
         </is>
       </c>
       <c r="Q41" s="1" t="n"/>
@@ -5830,7 +5830,7 @@
       </c>
       <c r="T44" s="2" t="inlineStr">
         <is>
-          <t>maa://39366 (88.24)</t>
+          <t>maa://39366 (88.57)</t>
         </is>
       </c>
       <c r="U44" s="1" t="n"/>
@@ -5904,7 +5904,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.63), maa://43901 (92.0)</t>
+          <t>maa://35931 (92.09), maa://43901 (92.31)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6250,7 +6250,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.92), **maa://32434 (33.33)</t>
+          <t>maa://32534 (93.96), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6286,7 +6286,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.28)</t>
+          <t>maa://32532 (92.0)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6322,7 +6322,7 @@
       </c>
       <c r="H57" s="2" t="inlineStr">
         <is>
-          <t>maa://25176 (98.36)</t>
+          <t>maa://25176 (98.39)</t>
         </is>
       </c>
       <c r="I57" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#160)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.48), maa://25390 (96.18), maa://36681 (87.34)</t>
+          <t>maa://24702 (94.5), maa://25390 (96.2), maa://36681 (87.34)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.52), *maa://30515 (69.9), *maa://34787 (73.33), maa://39402 (91.8), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.17), *maa://30515 (69.9), *maa://34787 (73.33), maa://39402 (92.19), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.57), *maa://20791 (62.16)</t>
+          <t>maa://22742 (91.62), *maa://20791 (62.16)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.41), maa://36684 (95.5), ***maa://22731 (6.25)</t>
+          <t>maa://21246 (91.41), maa://36684 (95.54), ***maa://22731 (6.25)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (92.31), ***maa://21730 (25.33), ***maa://39501 (16.67), **maa://36675 (50.0)</t>
+          <t>maa://25251 (91.53), ***maa://21730 (25.33), ***maa://39501 (16.13), **maa://36675 (50.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://36987 (96.08), maa://40192 (100.0), maa://39849 (88.89)</t>
+          <t>maa://36987 (96.08), maa://40192 (98.11), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.56), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.57), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.82), maa://20276 (86.44), *maa://22749 (72.73)</t>
+          <t>*maa://22880 (65.15), maa://20276 (86.52), *maa://22749 (72.73)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.47), maa://26254 (96.55)</t>
+          <t>maa://21249 (94.49), maa://26254 (96.55)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.74), **maa://20790 (43.48), ***maa://37170 (16.92), maa://45854 (88.24)</t>
+          <t>maa://24617 (89.74), **maa://20790 (43.48), ***maa://37170 (16.67), maa://45854 (85.71)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.16), maa://27484 (96.55), maa://27480 (83.33)</t>
+          <t>maa://27396 (84.31), maa://27484 (96.55), maa://27480 (83.33)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (94.59)</t>
+          <t>maa://24390 (94.67)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -901,7 +901,7 @@
       </c>
       <c r="AF3" s="2" t="inlineStr">
         <is>
-          <t>*maa://21289 (72.0)</t>
+          <t>*maa://21289 (73.08)</t>
         </is>
       </c>
       <c r="AG3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (94.08), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (94.12), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (96.55), maa://27295 (85.71), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
+          <t>maa://32509 (96.58), maa://27295 (85.92), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (89.47), ***maa://36683 (28.26)</t>
+          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (90.32), ***maa://36683 (28.26)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.81), maa://22744 (84.0)</t>
+          <t>maa://21245 (84.94), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>*maa://22757 (77.14)</t>
+          <t>*maa://22757 (77.78)</t>
         </is>
       </c>
       <c r="M5" s="1" t="n"/>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="AB5" s="2" t="inlineStr">
         <is>
-          <t>*maa://29863 (64.86), ***maa://22752 (12.5), **maa://26013 (37.5)</t>
+          <t>*maa://29863 (65.79), ***maa://22752 (12.5), **maa://26013 (37.5)</t>
         </is>
       </c>
       <c r="AC5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (95.92)</t>
+          <t>maa://42407 (96.3)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>maa://24839 (99.0)</t>
+          <t>maa://24839 (99.01)</t>
         </is>
       </c>
       <c r="M6" s="1" t="n"/>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="P6" s="2" t="inlineStr">
         <is>
-          <t>maa://31836 (92.59), maa://30381 (92.86)</t>
+          <t>maa://31836 (93.1), maa://30381 (92.86)</t>
         </is>
       </c>
       <c r="Q6" s="1" t="n"/>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="AF6" s="2" t="inlineStr">
         <is>
-          <t>*maa://33152 (62.0), ***maa://22770 (26.09)</t>
+          <t>*maa://33152 (63.46), ***maa://22770 (26.09)</t>
         </is>
       </c>
       <c r="AG6" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (92.59), maa://24957 (97.73)</t>
+          <t>maa://28624 (92.73), maa://24957 (97.73)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.36), *maa://22758 (74.29)</t>
+          <t>maa://22399 (95.45), *maa://22758 (74.29)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.02.16 13:17:39</t>
+          <t>更新日期：2025.02.22 13:17:25</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (83.62), *maa://21916 (61.54), maa://23252 (91.18), maa://37496 (96.77), **maa://22759 (45.45)</t>
+          <t>maa://32931 (83.76), *maa://21916 (62.12), maa://23252 (91.18), maa://37496 (96.77), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.93)</t>
+          <t>maa://21411 (95.95)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="AB8" s="2" t="inlineStr">
         <is>
-          <t>maa://25389 (88.57)</t>
+          <t>maa://25389 (88.89)</t>
         </is>
       </c>
       <c r="AC8" s="1" t="n"/>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>maa://22765 (91.58), *maa://21915 (67.86)</t>
+          <t>maa://22765 (91.67), *maa://21915 (67.86)</t>
         </is>
       </c>
       <c r="E9" s="1" t="n"/>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>maa://22762 (92.31), *maa://39552 (75.0)</t>
+          <t>maa://22762 (92.31), *maa://39552 (80.0)</t>
         </is>
       </c>
       <c r="M9" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.89)</t>
+          <t>maa://26223 (97.9)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.39), ***maa://22740 (5.66), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (96.0), *maa://45044 (66.67)</t>
+          <t>maa://28711 (86.89), ***maa://22740 (5.66), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (96.15), *maa://45044 (66.67)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (88.43), *maa://22865 (50.94)</t>
+          <t>maa://26206 (87.7), *maa://22865 (51.85)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.72), ***maa://39951 (15.69), ***maa://34206 (20.0), ***maa://39243 (25.0), *maa://45271 (55.17)</t>
+          <t>***maa://25695 (18.72), ***maa://39951 (15.69), ***maa://34206 (20.0), ***maa://39243 (25.0), *maa://45271 (57.58)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1741,7 +1741,7 @@
       </c>
       <c r="L10" s="2" t="inlineStr">
         <is>
-          <t>**maa://24395 (41.94)</t>
+          <t>**maa://24395 (40.62)</t>
         </is>
       </c>
       <c r="M10" s="1" t="n"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (90.48), maa://36669 (86.36), *maa://23264 (61.82)</t>
+          <t>maa://28977 (89.41), maa://36669 (86.36), *maa://23264 (61.82)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.46), maa://22755 (87.83), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.48), maa://22755 (87.83), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.75), maa://45828 (90.0), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.75), maa://45828 (92.31), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (53.76), *maa://22733 (60.0), **maa://22761 (50.0)</t>
+          <t>*maa://25021 (54.26), *maa://22733 (60.0), **maa://22761 (50.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (89.11)</t>
+          <t>maa://21287 (89.22)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (93.08), maa://22501 (97.67), *maa://45521 (78.57)</t>
+          <t>maa://22747 (92.5), maa://22501 (97.7), maa://45521 (83.33)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.75)</t>
+          <t>maa://36713 (97.76)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>maa://30766 (89.29), *maa://36678 (71.43)</t>
+          <t>maa://30766 (89.29), *maa://36678 (75.0)</t>
         </is>
       </c>
       <c r="E12" s="1" t="n"/>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (89.88), ***maa://45826 (20.0)</t>
+          <t>maa://21867 (89.94), ***maa://45826 (20.0)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (90.91), *maa://21485 (76.43), maa://37962 (90.24)</t>
+          <t>maa://22753 (90.96), *maa://21485 (76.43), maa://37962 (90.24)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.5), maa://36677 (93.22), maa://39872 (91.67)</t>
+          <t>maa://23669 (95.5), maa://36677 (93.55), maa://39872 (91.67)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (77.4), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (77.55), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.08), maa://36673 (93.24), maa://25001 (85.71)</t>
+          <t>maa://24999 (92.1), maa://36673 (93.24), maa://25001 (85.71)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.19), **maa://22728 (47.73)</t>
+          <t>*maa://21248 (73.53), **maa://22728 (46.67)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (92.68), *maa://22583 (74.63), *maa://22500 (58.7)</t>
+          <t>maa://22676 (92.74), *maa://22583 (74.63), *maa://22500 (58.7)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>maa://34957 (81.33), *maa://22768 (51.61)</t>
+          <t>maa://34957 (81.82), *maa://22768 (51.61)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (33.33), maa://39883 (91.43), *maa://39885 (53.33)</t>
+          <t>**maa://22737 (34.25), maa://39883 (91.43), *maa://39885 (53.33)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.71), maa://21288 (96.3), maa://39841 (95.05), maa://36682 (97.44)</t>
+          <t>maa://26245 (96.71), maa://21288 (96.3), maa://39841 (95.24), maa://36682 (97.44)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2309,7 +2309,7 @@
       </c>
       <c r="X14" s="2" t="inlineStr">
         <is>
-          <t>maa://37468 (90.91)</t>
+          <t>maa://37468 (91.3)</t>
         </is>
       </c>
       <c r="Y14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.73), maa://22734 (84.17), *maa://30808 (64.18), **maa://36048 (45.0), maa://45058 (91.67)</t>
+          <t>*maa://22743 (77.93), maa://22734 (84.17), *maa://30808 (64.18), **maa://36048 (45.0), maa://45058 (92.86)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (87.91), maa://21478 (89.19)</t>
+          <t>maa://24304 (88.02), maa://21478 (89.19)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2391,7 +2391,7 @@
       </c>
       <c r="L15" s="2" t="inlineStr">
         <is>
-          <t>*maa://21334 (55.17)</t>
+          <t>*maa://21334 (53.33)</t>
         </is>
       </c>
       <c r="M15" s="1" t="n"/>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (90.24), *maa://22727 (70.0)</t>
+          <t>maa://24762 (90.3), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.1), *maa://36666 (78.5), *maa://22766 (68.64)</t>
+          <t>maa://21364 (81.02), *maa://36666 (78.5), *maa://22766 (68.64)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.97), *maa://28648 (69.12), maa://36674 (82.69)</t>
+          <t>maa://22729 (95.0), *maa://28648 (69.12), maa://36674 (82.69)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.66), maa://39599 (86.0)</t>
+          <t>maa://22430 (88.72), maa://39599 (86.27)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2667,7 +2667,7 @@
       </c>
       <c r="P17" s="2" t="inlineStr">
         <is>
-          <t>maa://23890 (80.58), *maa://24940 (67.86)</t>
+          <t>maa://23890 (80.77), *maa://24940 (67.86)</t>
         </is>
       </c>
       <c r="Q17" s="1" t="n"/>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>**maa://42324 (50.0)</t>
+          <t>**maa://42324 (48.28)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (90.06), *maa://22732 (51.14)</t>
+          <t>maa://22466 (90.3), *maa://22732 (51.11)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (65.52), *maa://36668 (57.5)</t>
+          <t>*maa://30709 (65.75), *maa://36668 (57.5)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.0), maa://25198 (93.58), *maa://20795 (50.77), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.12), maa://25198 (93.64), *maa://20795 (50.77), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.23)</t>
+          <t>maa://41331 (84.97)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3155,7 +3155,7 @@
       </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>maa://24372 (96.94)</t>
+          <t>maa://24372 (96.97)</t>
         </is>
       </c>
       <c r="I21" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (80.97), ***maa://23820 (30.0)</t>
+          <t>maa://21443 (81.07), ***maa://23820 (30.0)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.5), *maa://22432 (76.71)</t>
+          <t>maa://22524 (94.14), *maa://22432 (77.03)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (80.87), *maa://22751 (71.01)</t>
+          <t>maa://27127 (80.17), *maa://22751 (71.01)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.77), *maa://41753 (58.82)</t>
+          <t>***maa://28036 (28.77), *maa://41753 (57.89)</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.56), maa://39875 (94.37)</t>
+          <t>maa://39756 (95.64), maa://39875 (94.44)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.84), *maa://29748 (75.97), ***maa://29785 (16.18), *maa://37566 (76.32)</t>
+          <t>maa://30587 (91.92), *maa://29748 (75.97), ***maa://29785 (16.18), *maa://37566 (76.32)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3495,7 +3495,7 @@
       </c>
       <c r="AB23" s="2" t="inlineStr">
         <is>
-          <t>maa://29652 (97.62)</t>
+          <t>maa://29652 (97.67)</t>
         </is>
       </c>
       <c r="AC23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (84.58), maa://23504 (93.11), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (77.63), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (84.65), maa://23504 (93.14), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (77.92), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.93), maa://36672 (80.36), maa://29910 (92.98), **maa://21440 (35.71), *maa://45831 (75.0)</t>
+          <t>maa://22523 (86.0), maa://36672 (80.36), maa://29910 (93.1), **maa://21440 (35.71), *maa://45831 (75.0)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.13)</t>
+          <t>maa://29753 (95.15)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (73.75), *maa://25311 (73.53), ***maa://22725 (4.84), *maa://45047 (62.5)</t>
+          <t>*maa://29063 (73.46), *maa://25311 (73.79), ***maa://22725 (4.84), *maa://45047 (62.5)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3691,7 +3691,7 @@
       </c>
       <c r="L25" s="2" t="inlineStr">
         <is>
-          <t>maa://24378 (87.8)</t>
+          <t>maa://24378 (88.1)</t>
         </is>
       </c>
       <c r="M25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (87.72), maa://24516 (80.22), maa://26001 (87.5)</t>
+          <t>maa://31215 (87.83), maa://24516 (80.22), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.32), maa://24621 (96.85), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
+          <t>maa://20108 (96.35), maa://24621 (96.88), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (92.13)</t>
+          <t>maa://24913 (92.22)</t>
         </is>
       </c>
       <c r="I26" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (93.94)</t>
+          <t>maa://42235 (94.06)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3901,7 +3901,7 @@
       </c>
       <c r="AF26" s="2" t="inlineStr">
         <is>
-          <t>maa://30511 (82.5), *maa://29760 (64.29)</t>
+          <t>maa://30511 (82.5), *maa://29760 (60.0)</t>
         </is>
       </c>
       <c r="AG26" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.98), maa://25725 (83.72)</t>
+          <t>maa://24465 (91.04), maa://25725 (83.72)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>maa://23263 (95.28), *maa://29765 (63.41)</t>
+          <t>*maa://29765 (63.41), maa://23263 (95.28)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.62), maa://41749 (90.59), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.65), maa://41749 (90.7), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.15), *maa://36701 (66.67)</t>
+          <t>maa://36660 (92.2), *maa://36701 (66.67)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.43), *maa://28440 (79.63), maa://31400 (98.81), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.45), *maa://28440 (79.82), maa://31400 (98.81), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.85), maa://42865 (81.67), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.85), maa://42865 (80.65), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.84), maa://45822 (100.0), *maa://45045 (80.0)</t>
+          <t>maa://42979 (96.91), maa://45822 (100.0), *maa://45045 (80.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.43), maa://36258 (84.96), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.47), maa://36258 (85.34), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.5), maa://36667 (97.56), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.5), maa://36667 (97.62), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4601,7 +4601,7 @@
       </c>
       <c r="L32" s="2" t="inlineStr">
         <is>
-          <t>maa://28065 (95.35)</t>
+          <t>maa://28065 (95.45)</t>
         </is>
       </c>
       <c r="M32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (95.76), maa://41108 (88.0), maa://41238 (97.09), maa://45523 (100.0)</t>
+          <t>maa://42859 (95.83), maa://41108 (88.0), maa://41238 (97.12), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (93.02)</t>
+          <t>maa://24526 (93.05)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4991,7 +4991,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.2)</t>
+          <t>maa://41296 (96.25)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5203,7 +5203,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (98.35), maa://45789 (100.0), maa://47069 (100.0)</t>
+          <t>maa://45718 (98.5), *maa://47069 (75.0), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5219,7 +5219,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.3), *maa://21239 (66.67)</t>
+          <t>maa://21280 (89.35), *maa://21239 (66.67)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5336,7 +5336,7 @@
       </c>
       <c r="T38" s="2" t="inlineStr">
         <is>
-          <t>maa://30713 (96.77)</t>
+          <t>maa://30713 (96.88)</t>
         </is>
       </c>
       <c r="U38" s="1" t="n"/>
@@ -5368,7 +5368,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.26)</t>
+          <t>maa://36697 (86.32)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5389,7 +5389,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (88.89), maa://25199 (84.82), maa://30434 (91.36), ***maa://25036 (16.0), maa://45059 (81.25), *maa://44165 (66.67)</t>
+          <t>maa://36670 (89.11), maa://25199 (84.82), maa://30434 (91.36), ***maa://25036 (16.0), maa://45059 (81.25), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.5), maa://47093 (100.0)</t>
+          <t>maa://24709 (91.56), maa://47093 (100.0)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5437,7 +5437,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (81.91), *maa://45790 (75.0), *maa://47079 (75.0)</t>
+          <t>maa://45788 (81.25), *maa://45790 (75.0), maa://47079 (92.31)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5740,12 +5740,12 @@
       </c>
       <c r="O43" s="1" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P43" s="2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>maa://47403 (100.0)</t>
         </is>
       </c>
       <c r="Q43" s="1" t="n"/>
@@ -5798,7 +5798,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (98.01), maa://27728 (96.08)</t>
+          <t>maa://29768 (98.04), maa://27728 (96.12)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5830,7 +5830,7 @@
       </c>
       <c r="T44" s="2" t="inlineStr">
         <is>
-          <t>maa://39366 (88.57)</t>
+          <t>maa://39366 (88.89)</t>
         </is>
       </c>
       <c r="U44" s="1" t="n"/>
@@ -5867,7 +5867,7 @@
       </c>
       <c r="P45" s="2" t="inlineStr">
         <is>
-          <t>*maa://36237 (64.29)</t>
+          <t>*maa://36237 (68.75)</t>
         </is>
       </c>
       <c r="Q45" s="1" t="n"/>
@@ -5904,7 +5904,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.09), maa://43901 (92.31)</t>
+          <t>maa://35931 (91.93), maa://43901 (92.31)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5957,7 +5957,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.44), maa://29661 (97.3), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.47), maa://29661 (97.32), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6079,7 +6079,7 @@
       </c>
       <c r="P49" s="2" t="inlineStr">
         <is>
-          <t>*maa://39643 (66.67)</t>
+          <t>*maa://39643 (64.52)</t>
         </is>
       </c>
       <c r="Q49" s="1" t="n"/>
@@ -6166,7 +6166,7 @@
       </c>
       <c r="H51" s="2" t="inlineStr">
         <is>
-          <t>maa://30769 (81.25)</t>
+          <t>maa://30769 (82.35)</t>
         </is>
       </c>
       <c r="I51" s="1" t="n"/>
@@ -6250,7 +6250,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (93.96), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.07), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6286,7 +6286,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.0)</t>
+          <t>maa://32532 (92.16)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6340,7 +6340,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (61.11)</t>
+          <t>*maa://37964 (62.16)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>
@@ -6376,7 +6376,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (67.8)</t>
+          <t>*maa://40438 (68.33)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#161)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.41), maa://36684 (95.54), ***maa://22731 (6.25)</t>
+          <t>maa://21246 (91.41), maa://36684 (95.61), ***maa://22731 (6.25)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (91.53), ***maa://21730 (25.33), ***maa://39501 (16.13), **maa://36675 (50.0)</t>
+          <t>maa://25251 (91.53), ***maa://21730 (26.32), ***maa://39501 (15.62), **maa://36675 (50.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://36987 (96.08), maa://40192 (98.11), maa://39849 (88.89)</t>
+          <t>maa://36987 (96.08), maa://40192 (98.15), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.57), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.58), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.74), **maa://20790 (43.48), ***maa://37170 (16.67), maa://45854 (85.71)</t>
+          <t>maa://24617 (89.74), **maa://20790 (43.48), ***maa://37170 (16.67), maa://45854 (86.36)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (94.67)</t>
+          <t>maa://24390 (94.74)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (94.12), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (94.15), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (96.58), maa://27295 (85.92), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
+          <t>maa://32509 (95.76), maa://27295 (85.92), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>*maa://22757 (77.78)</t>
+          <t>*maa://22757 (78.38)</t>
         </is>
       </c>
       <c r="M5" s="1" t="n"/>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>*maa://22763 (65.62)</t>
+          <t>*maa://22763 (66.67)</t>
         </is>
       </c>
       <c r="I7" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (92.73), maa://24957 (97.73)</t>
+          <t>maa://28624 (92.79), maa://24957 (97.73)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.45), *maa://22758 (74.29)</t>
+          <t>maa://22399 (95.48), *maa://22758 (74.29)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.02.22 13:17:25</t>
+          <t>更新日期：2025.02.27 13:19:23</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (83.76), *maa://21916 (62.12), maa://23252 (91.18), maa://37496 (96.77), **maa://22759 (45.45)</t>
+          <t>maa://32931 (83.9), *maa://21916 (62.12), maa://23252 (91.18), maa://37496 (96.88), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>maa://22765 (91.67), *maa://21915 (67.86)</t>
+          <t>maa://22765 (91.67), *maa://21915 (68.97)</t>
         </is>
       </c>
       <c r="E9" s="1" t="n"/>
@@ -1593,11 +1593,7 @@
           <t>0</t>
         </is>
       </c>
-      <c r="H9" s="2" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="H9" s="2" t="inlineStr"/>
       <c r="I9" s="1" t="n"/>
       <c r="J9" s="1" t="inlineStr">
         <is>
@@ -1627,7 +1623,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (83.0)</t>
+          <t>maa://22736 (83.17)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1659,7 +1655,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.9)</t>
+          <t>maa://26223 (97.92)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1675,7 +1671,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (86.89), ***maa://22740 (5.66), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (96.15), *maa://45044 (66.67)</t>
+          <t>maa://28711 (86.99), ***maa://22740 (5.66), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (96.3), *maa://45044 (66.67)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1709,7 +1705,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.72), ***maa://39951 (15.69), ***maa://34206 (20.0), ***maa://39243 (25.0), *maa://45271 (57.58)</t>
+          <t>***maa://25695 (18.62), ***maa://39951 (14.81), ***maa://34206 (20.0), ***maa://39243 (25.0), *maa://45271 (58.33)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1821,7 +1817,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (54.26), *maa://22733 (60.0), **maa://22761 (50.0)</t>
+          <t>*maa://25021 (54.74), *maa://22733 (61.11), **maa://22761 (50.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1871,7 +1867,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (89.22)</t>
+          <t>maa://21287 (89.32)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1903,7 +1899,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.5), maa://22501 (97.7), maa://45521 (83.33)</t>
+          <t>maa://22747 (92.5), maa://22501 (97.73), maa://45521 (84.21)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1915,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.76)</t>
+          <t>maa://36713 (97.77)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1935,7 +1931,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://29912 (97.14), maa://22516 (88.37), *maa://20794 (52.24)</t>
+          <t>maa://29912 (97.18), maa://22516 (88.37), *maa://20794 (52.24)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -2049,7 +2045,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (90.96), *maa://21485 (76.43), maa://37962 (90.24)</t>
+          <t>maa://22753 (91.01), *maa://21485 (76.43), maa://37962 (90.24)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2061,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.5), maa://36677 (93.55), maa://39872 (91.67)</t>
+          <t>maa://23669 (95.5), maa://36677 (93.65), maa://39872 (91.67)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2099,7 +2095,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.1), maa://36673 (93.24), maa://25001 (85.71)</t>
+          <t>maa://24999 (92.12), maa://36673 (93.24), maa://25001 (85.71)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2147,7 +2143,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (92.74), *maa://22583 (74.63), *maa://22500 (58.7)</t>
+          <t>maa://22676 (92.74), *maa://22583 (75.0), *maa://22500 (58.7)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2211,7 +2207,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (34.25), maa://39883 (91.43), *maa://39885 (53.33)</t>
+          <t>**maa://22737 (34.25), maa://39883 (91.67), *maa://39885 (53.33)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2257,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.71), maa://21288 (96.3), maa://39841 (95.24), maa://36682 (97.44)</t>
+          <t>maa://26245 (96.73), maa://21288 (96.3), maa://39841 (95.28), maa://36682 (97.44)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2293,7 +2289,7 @@
       </c>
       <c r="T14" s="2" t="inlineStr">
         <is>
-          <t>maa://22521 (94.29), maa://42751 (100.0)</t>
+          <t>maa://22521 (94.34), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="1" t="n"/>
@@ -2359,7 +2355,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (77.93), maa://22734 (84.17), *maa://30808 (64.18), **maa://36048 (45.0), maa://45058 (92.86)</t>
+          <t>*maa://22743 (78.04), maa://22734 (84.17), *maa://30808 (64.18), **maa://36048 (45.0), maa://45058 (92.86)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2439,7 +2435,7 @@
       </c>
       <c r="X15" s="2" t="inlineStr">
         <is>
-          <t>maa://38786 (85.71)</t>
+          <t>*maa://38786 (75.0)</t>
         </is>
       </c>
       <c r="Y15" s="1" t="n"/>
@@ -2471,7 +2467,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.02), *maa://36666 (78.5), *maa://22766 (68.64)</t>
+          <t>maa://21364 (80.78), *maa://36666 (78.18), *maa://22766 (68.64)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2485,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.4), maa://36679 (94.34), maa://37650 (97.14)</t>
+          <t>maa://21441 (96.4), maa://36679 (94.34), maa://37650 (97.3)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2553,7 +2549,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (95.0), *maa://28648 (69.12), maa://36674 (82.69)</t>
+          <t>maa://22729 (95.03), *maa://28648 (69.12), maa://36674 (82.69)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2585,7 +2581,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.92)</t>
+          <t>maa://26228 (95.96)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2635,7 +2631,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.72), maa://39599 (86.27)</t>
+          <t>maa://22430 (88.78), maa://39599 (86.27)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2683,7 +2679,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>**maa://42324 (48.28)</t>
+          <t>**maa://42324 (50.0)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2749,7 +2745,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.33)</t>
+          <t>maa://24570 (97.35)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2781,7 +2777,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (90.3), *maa://22732 (51.11)</t>
+          <t>maa://22466 (90.36), *maa://22732 (50.55)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2975,7 +2971,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (65.75), *maa://36668 (57.5)</t>
+          <t>*maa://30709 (65.83), *maa://36668 (57.5)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3009,7 +3005,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.12), maa://25198 (93.64), *maa://20795 (50.77), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.17), maa://25198 (93.64), *maa://20795 (50.77), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3041,7 +3037,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (84.97)</t>
+          <t>maa://41331 (85.06)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3139,7 +3135,7 @@
       </c>
       <c r="D21" s="2" t="inlineStr">
         <is>
-          <t>maa://21261 (97.56)</t>
+          <t>maa://21261 (97.67)</t>
         </is>
       </c>
       <c r="E21" s="1" t="n"/>
@@ -3155,7 +3151,7 @@
       </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>maa://24372 (96.97)</t>
+          <t>maa://24372 (97.0)</t>
         </is>
       </c>
       <c r="I21" s="1" t="n"/>
@@ -3187,7 +3183,7 @@
       </c>
       <c r="P21" s="2" t="inlineStr">
         <is>
-          <t>maa://24381 (84.21)</t>
+          <t>maa://24381 (85.0)</t>
         </is>
       </c>
       <c r="Q21" s="1" t="n"/>
@@ -3235,7 +3231,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (81.07), ***maa://23820 (30.0)</t>
+          <t>maa://21443 (81.12), ***maa://23820 (30.0)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3247,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.14), *maa://22432 (77.03)</t>
+          <t>maa://22524 (94.17), *maa://22432 (77.03)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3301,7 +3297,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>maa://27127 (80.17), *maa://22751 (71.01)</t>
+          <t>*maa://27127 (79.66), *maa://22751 (71.01)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3431,7 +3427,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.64), maa://39875 (94.44)</t>
+          <t>maa://39756 (95.68), maa://39875 (94.44)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3479,7 +3475,7 @@
       </c>
       <c r="X23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (68.35)</t>
+          <t>*maa://28503 (68.75)</t>
         </is>
       </c>
       <c r="Y23" s="1" t="n"/>
@@ -3511,7 +3507,7 @@
       </c>
       <c r="AF23" s="2" t="inlineStr">
         <is>
-          <t>maa://31489 (93.75)</t>
+          <t>maa://31489 (94.12)</t>
         </is>
       </c>
       <c r="AG23" s="1" t="n"/>
@@ -3529,7 +3525,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.16), **maa://46650 (50.0)</t>
+          <t>*maa://24368 (78.27), *maa://46650 (60.0)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3605,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (84.65), maa://23504 (93.14), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (77.92), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (84.65), maa://23504 (93.18), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (78.21), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3637,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (86.0), maa://36672 (80.36), maa://29910 (93.1), **maa://21440 (35.71), *maa://45831 (75.0)</t>
+          <t>maa://22523 (86.0), maa://36672 (80.36), maa://29910 (93.22), **maa://21440 (35.71), *maa://45831 (75.0)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3659,7 +3655,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.15)</t>
+          <t>maa://29753 (95.17)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3723,7 +3719,7 @@
       </c>
       <c r="T25" s="2" t="inlineStr">
         <is>
-          <t>maa://20109 (92.09), maa://22545 (100.0), *maa://42915 (75.0)</t>
+          <t>maa://20109 (92.13), maa://22545 (100.0), *maa://42915 (75.0)</t>
         </is>
       </c>
       <c r="U25" s="1" t="n"/>
@@ -3755,7 +3751,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (87.83), maa://24516 (80.22), maa://26001 (87.5)</t>
+          <t>maa://31215 (87.93), maa://24516 (80.22), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3789,7 +3785,7 @@
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>maa://41802 (93.75)</t>
+          <t>maa://41802 (94.44)</t>
         </is>
       </c>
       <c r="E26" s="1" t="n"/>
@@ -3885,7 +3881,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (94.06)</t>
+          <t>maa://42235 (94.12)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3901,7 +3897,7 @@
       </c>
       <c r="AF26" s="2" t="inlineStr">
         <is>
-          <t>maa://30511 (82.5), *maa://29760 (60.0)</t>
+          <t>maa://30511 (80.49), *maa://29760 (60.0)</t>
         </is>
       </c>
       <c r="AG26" s="1" t="n"/>
@@ -4049,7 +4045,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (91.04), maa://25725 (83.72)</t>
+          <t>maa://24465 (90.93), maa://25725 (83.91)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4113,7 +4109,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>*maa://29765 (63.41), maa://23263 (95.28)</t>
+          <t>*maa://29765 (63.86), maa://23263 (95.28)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4125,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.65), maa://41749 (90.7), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.7), maa://41749 (90.7), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4157,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.2), *maa://36701 (66.67)</t>
+          <t>maa://36660 (92.24), *maa://36701 (66.67)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4211,7 +4207,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.45), *maa://28440 (79.82), maa://31400 (98.81), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.45), *maa://28440 (80.0), maa://31400 (98.81), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4291,7 +4287,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.85), maa://42865 (80.65), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.85), maa://42865 (80.95), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4405,7 +4401,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.91), maa://45822 (100.0), *maa://45045 (80.0)</t>
+          <t>maa://42979 (96.97), maa://45822 (100.0), *maa://45045 (80.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4467,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.47), maa://36258 (85.34), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.47), maa://36258 (85.47), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4581,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.5), maa://36667 (97.62), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.01), maa://36667 (97.62), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4629,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (95.83), maa://41108 (88.0), maa://41238 (97.12), maa://45523 (100.0)</t>
+          <t>maa://42859 (95.93), maa://41108 (88.0), maa://41238 (97.12), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4893,7 +4889,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (93.05)</t>
+          <t>maa://24526 (93.08)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4941,7 +4937,7 @@
       </c>
       <c r="AF34" s="2" t="inlineStr">
         <is>
-          <t>*maa://32650 (68.75)</t>
+          <t>*maa://32650 (72.22)</t>
         </is>
       </c>
       <c r="AG34" s="1" t="n"/>
@@ -5203,7 +5199,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (98.5), *maa://47069 (75.0), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.55), *maa://47069 (69.23), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5219,7 +5215,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.35), *maa://21239 (66.67)</t>
+          <t>maa://21280 (89.4), *maa://21239 (66.67)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5368,7 +5364,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.32)</t>
+          <t>maa://36697 (86.38)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5389,7 +5385,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (89.11), maa://25199 (84.82), maa://30434 (91.36), ***maa://25036 (16.0), maa://45059 (81.25), *maa://44165 (66.67)</t>
+          <t>maa://36670 (89.11), maa://25199 (84.82), maa://30434 (91.46), ***maa://25036 (16.0), maa://45059 (82.35), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5421,7 +5417,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.56), maa://47093 (100.0)</t>
+          <t>maa://24709 (91.61), maa://47093 (100.0)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5437,7 +5433,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (81.25), *maa://45790 (75.0), maa://47079 (92.31)</t>
+          <t>maa://45788 (81.25), *maa://45790 (75.0), maa://47079 (94.12)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5851,7 +5847,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.74), maa://30807 (95.65), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (84.21)</t>
+          <t>maa://21229 (84.82), maa://30807 (95.65), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (85.0)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5883,7 +5879,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (36.67)</t>
+          <t>**maa://39364 (38.71)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -5904,7 +5900,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (91.93), maa://43901 (92.31)</t>
+          <t>maa://35931 (91.95), maa://43901 (92.59)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6250,7 +6246,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.07), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.08), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6286,7 +6282,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.16)</t>
+          <t>maa://32532 (92.21)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6340,7 +6336,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (62.16)</t>
+          <t>*maa://37964 (60.53)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>
@@ -6358,7 +6354,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://31270 (95.31), maa://27746 (82.3)</t>
+          <t>maa://31270 (95.35), maa://27746 (82.3)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6376,7 +6372,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (68.33)</t>
+          <t>*maa://40438 (69.35)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#162)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://36987 (96.08), maa://40192 (98.15), maa://39849 (88.89)</t>
+          <t>maa://40192 (98.15), maa://36987 (96.08), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (90.32), ***maa://36683 (28.26)</t>
+          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (90.48), ***maa://36683 (28.26)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="AF6" s="2" t="inlineStr">
         <is>
-          <t>*maa://33152 (63.46), ***maa://22770 (26.09)</t>
+          <t>*maa://33152 (64.15), ***maa://22770 (26.09)</t>
         </is>
       </c>
       <c r="AG6" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.02.27 13:19:23</t>
+          <t>更新日期：2025.03.01 13:17:29</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (83.9), *maa://21916 (62.12), maa://23252 (91.18), maa://37496 (96.88), **maa://22759 (45.45)</t>
+          <t>maa://32931 (83.9), *maa://21916 (62.12), maa://23252 (91.18), maa://37496 (96.97), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.62), ***maa://39951 (14.81), ***maa://34206 (20.0), ***maa://39243 (25.0), *maa://45271 (58.33)</t>
+          <t>***maa://25695 (18.62), ***maa://39951 (14.81), ***maa://34206 (20.0), ***maa://39243 (25.0), *maa://45271 (57.89)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (54.74), *maa://22733 (61.11), **maa://22761 (50.0)</t>
+          <t>*maa://25021 (54.17), *maa://22733 (61.11), **maa://22761 (50.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -2045,7 +2045,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.01), *maa://21485 (76.43), maa://37962 (90.24)</t>
+          <t>maa://22753 (91.01), *maa://21485 (75.89), maa://37962 (90.24)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (77.55), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (77.7), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.12), maa://36673 (93.24), maa://25001 (85.71)</t>
+          <t>maa://24999 (92.13), maa://36673 (93.33), maa://25001 (85.71)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (92.74), *maa://22583 (75.0), *maa://22500 (58.7)</t>
+          <t>maa://22676 (92.8), *maa://22583 (75.0), *maa://22500 (58.7)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2225,7 +2225,7 @@
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>maa://30764 (88.89)</t>
+          <t>maa://30764 (89.09)</t>
         </is>
       </c>
       <c r="E14" s="1" t="n"/>
@@ -2257,7 +2257,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.73), maa://21288 (96.3), maa://39841 (95.28), maa://36682 (97.44)</t>
+          <t>maa://26245 (96.73), maa://21288 (96.3), maa://39841 (95.33), maa://36682 (97.44)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.78), *maa://36666 (78.18), *maa://22766 (68.64)</t>
+          <t>maa://21364 (80.78), *maa://36666 (77.48), *maa://22766 (68.64)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2485,7 +2485,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.4), maa://36679 (94.34), maa://37650 (97.3)</t>
+          <t>maa://21441 (96.41), maa://36679 (94.44), maa://37650 (97.3)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2745,7 +2745,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.35)</t>
+          <t>maa://24570 (97.36)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2777,7 +2777,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (90.36), *maa://22732 (50.55)</t>
+          <t>maa://22466 (90.42), *maa://22732 (50.55)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (99.14)</t>
+          <t>maa://24386 (99.15)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="AF19" s="2" t="inlineStr">
         <is>
-          <t>*maa://21663 (63.38)</t>
+          <t>*maa://21663 (63.89)</t>
         </is>
       </c>
       <c r="AG19" s="1" t="n"/>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.06)</t>
+          <t>maa://41331 (85.16)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3443,7 +3443,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.92), *maa://29748 (75.97), ***maa://29785 (16.18), *maa://37566 (76.32)</t>
+          <t>maa://30587 (91.92), *maa://29748 (75.97), ***maa://29785 (16.18), *maa://37566 (76.92)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3605,7 +3605,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (84.65), maa://23504 (93.18), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (78.21), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (84.31), maa://23504 (93.19), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (76.92), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3671,7 +3671,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (73.46), *maa://25311 (73.79), ***maa://22725 (4.84), *maa://45047 (62.5)</t>
+          <t>*maa://29063 (73.17), *maa://25311 (74.04), ***maa://22725 (4.84), *maa://45047 (62.5)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (94.12)</t>
+          <t>maa://42235 (94.17)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3897,7 +3897,7 @@
       </c>
       <c r="AF26" s="2" t="inlineStr">
         <is>
-          <t>maa://30511 (80.49), *maa://29760 (60.0)</t>
+          <t>maa://30511 (80.95), *maa://29760 (60.0)</t>
         </is>
       </c>
       <c r="AG26" s="1" t="n"/>
@@ -4027,7 +4027,7 @@
       </c>
       <c r="AF27" s="2" t="inlineStr">
         <is>
-          <t>maa://24023 (97.26)</t>
+          <t>maa://24023 (97.3)</t>
         </is>
       </c>
       <c r="AG27" s="1" t="n"/>
@@ -4045,7 +4045,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.93), maa://25725 (83.91)</t>
+          <t>maa://24465 (90.94), maa://25725 (83.91)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.7), maa://41749 (90.7), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.77), maa://41749 (90.7), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4157,7 +4157,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.24), *maa://36701 (66.67)</t>
+          <t>maa://36660 (92.31), *maa://36701 (66.67)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.45), *maa://28440 (80.0), maa://31400 (98.81), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.49), *maa://28440 (80.0), maa://31400 (98.81), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4287,7 +4287,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.85), maa://42865 (80.95), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.85), maa://42865 (81.25), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4353,7 +4353,7 @@
       </c>
       <c r="P30" s="2" t="inlineStr">
         <is>
-          <t>maa://21442 (99.55)</t>
+          <t>maa://21442 (99.11)</t>
         </is>
       </c>
       <c r="Q30" s="1" t="n"/>
@@ -4401,7 +4401,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.97), maa://45822 (100.0), *maa://45045 (80.0)</t>
+          <t>maa://42979 (97.01), maa://45822 (100.0), *maa://45045 (80.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4467,7 +4467,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.47), maa://36258 (85.47), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.49), maa://36258 (85.47), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4629,7 +4629,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (95.93), maa://41108 (88.0), maa://41238 (97.12), maa://45523 (100.0)</t>
+          <t>maa://42859 (95.97), maa://41108 (88.0), maa://41238 (97.12), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4987,7 +4987,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.25)</t>
+          <t>maa://41296 (96.27)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5199,7 +5199,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (98.55), *maa://47069 (69.23), maa://45789 (100.0)</t>
+          <t>maa://45718 (97.89), *maa://47069 (69.23), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5385,7 +5385,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (89.11), maa://25199 (84.82), maa://30434 (91.46), ***maa://25036 (16.0), maa://45059 (82.35), *maa://44165 (66.67)</t>
+          <t>maa://36670 (89.11), maa://25199 (84.82), maa://30434 (91.46), ***maa://25036 (16.0), maa://45059 (83.33), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (81.25), *maa://45790 (75.0), maa://47079 (94.12)</t>
+          <t>maa://45788 (81.44), maa://47079 (94.12), *maa://45790 (75.0)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5502,7 +5502,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.54), maa://21386 (95.77), maa://36664 (89.29), maa://45550 (100.0)</t>
+          <t>maa://23278 (95.56), maa://21386 (95.77), maa://36664 (89.29), maa://45550 (100.0)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5847,7 +5847,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.82), maa://30807 (95.65), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (85.0)</t>
+          <t>maa://21229 (84.82), maa://30807 (95.65), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (85.71)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -6246,7 +6246,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.08), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.1), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6282,7 +6282,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.21)</t>
+          <t>maa://32532 (91.91)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6336,7 +6336,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (60.53)</t>
+          <t>*maa://37964 (61.54)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#163)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.41), maa://36684 (95.61), ***maa://22731 (6.25)</t>
+          <t>maa://21246 (91.41), maa://36684 (95.65), ***maa://22731 (6.25)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.03.01 13:17:29</t>
+          <t>更新日期：2025.03.02 13:19:18</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1785,7 +1785,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.75), maa://45828 (92.31), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.75), maa://45828 (92.86), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -2257,7 +2257,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.73), maa://21288 (96.3), maa://39841 (95.33), maa://36682 (97.44)</t>
+          <t>maa://26245 (96.75), maa://21288 (96.3), maa://39841 (95.33), maa://36682 (97.44)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.02), maa://21478 (89.19)</t>
+          <t>maa://24304 (88.07), maa://21478 (89.19)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.78), *maa://36666 (77.48), *maa://22766 (68.64)</t>
+          <t>maa://21364 (80.78), *maa://36666 (77.68), *maa://22766 (68.64)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (95.03), *maa://28648 (69.12), maa://36674 (82.69)</t>
+          <t>maa://22729 (95.06), *maa://28648 (69.12), maa://36674 (82.69)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.68), maa://39875 (94.44)</t>
+          <t>maa://39756 (95.69), maa://39875 (94.44)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -4045,7 +4045,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.94), maa://25725 (83.91)</t>
+          <t>maa://24465 (90.96), maa://25725 (83.91)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4401,7 +4401,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.01), maa://45822 (100.0), *maa://45045 (80.0)</t>
+          <t>maa://42979 (97.02), maa://45822 (100.0), *maa://45045 (80.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -5199,7 +5199,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (97.89), *maa://47069 (69.23), maa://45789 (100.0)</t>
+          <t>maa://45718 (97.92), *maa://47069 (69.23), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (81.44), maa://47079 (94.12), *maa://45790 (75.0)</t>
+          <t>maa://45788 (81.63), maa://47079 (94.12), *maa://45790 (75.0)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5502,7 +5502,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.56), maa://21386 (95.77), maa://36664 (89.29), maa://45550 (100.0)</t>
+          <t>maa://23278 (95.57), maa://21386 (95.77), maa://36664 (89.29), maa://45550 (100.0)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5794,7 +5794,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (98.04), maa://27728 (96.12)</t>
+          <t>maa://29768 (98.05), maa://27728 (96.12)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5953,7 +5953,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.47), maa://29661 (97.32), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.48), maa://29661 (97.32), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6354,7 +6354,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://31270 (95.35), maa://27746 (82.3)</t>
+          <t>maa://31270 (95.38), maa://27746 (82.3)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#164)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.5), maa://25390 (96.2), maa://36681 (87.34)</t>
+          <t>maa://24702 (94.54), maa://25390 (96.2), maa://36681 (87.34)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://40192 (98.15), maa://36987 (96.08), maa://39849 (88.89)</t>
+          <t>maa://40192 (98.18), maa://36987 (96.08), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.58), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.6), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.15), maa://20276 (86.52), *maa://22749 (72.73)</t>
+          <t>*maa://22880 (65.33), maa://20276 (86.59), *maa://22749 (75.0)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.49), maa://26254 (96.55)</t>
+          <t>maa://21249 (94.54), maa://26254 (96.67)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.74), **maa://20790 (43.48), ***maa://37170 (16.67), maa://45854 (86.36)</t>
+          <t>maa://24617 (89.83), **maa://20790 (43.48), ***maa://37170 (16.67), maa://45854 (87.5)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.31), maa://27484 (96.55), maa://27480 (83.33)</t>
+          <t>maa://27396 (84.36), maa://27484 (96.58), maa://27480 (83.33)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (95.76), maa://27295 (85.92), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
+          <t>maa://32509 (95.76), maa://27295 (86.11), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (90.48), ***maa://36683 (28.26)</t>
+          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (90.62), ***maa://36683 (28.26)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.94), maa://22744 (84.0)</t>
+          <t>maa://21245 (84.58), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>*maa://22757 (78.38)</t>
+          <t>*maa://22757 (76.32)</t>
         </is>
       </c>
       <c r="M5" s="1" t="n"/>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="P6" s="2" t="inlineStr">
         <is>
-          <t>maa://31836 (93.1), maa://30381 (92.86)</t>
+          <t>maa://31836 (93.1), maa://30381 (93.33)</t>
         </is>
       </c>
       <c r="Q6" s="1" t="n"/>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="P7" s="2" t="inlineStr">
         <is>
-          <t>maa://22750 (91.67)</t>
+          <t>maa://22750 (91.84)</t>
         </is>
       </c>
       <c r="Q7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.48), *maa://22758 (74.29)</t>
+          <t>maa://22399 (95.51), *maa://22758 (74.29)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.03.02 13:19:18</t>
+          <t>更新日期：2025.03.06 13:18:49</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (83.9), *maa://21916 (62.12), maa://23252 (91.18), maa://37496 (96.97), **maa://22759 (45.45)</t>
+          <t>maa://32931 (84.03), *maa://21916 (62.12), maa://23252 (91.18), maa://37496 (96.97), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1623,7 +1623,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (83.17)</t>
+          <t>maa://22736 (83.33)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1655,7 +1655,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.92)</t>
+          <t>maa://26223 (97.93)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (86.99), ***maa://22740 (5.66), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (96.3), *maa://45044 (66.67)</t>
+          <t>maa://28711 (87.1), ***maa://22740 (5.66), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (96.3), *maa://45044 (66.67)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (87.7), *maa://22865 (51.85)</t>
+          <t>maa://26206 (87.8), *maa://22865 (51.85)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.62), ***maa://39951 (14.81), ***maa://34206 (20.0), ***maa://39243 (25.0), *maa://45271 (57.89)</t>
+          <t>***maa://25695 (18.62), ***maa://39951 (14.29), ***maa://34206 (19.23), ***maa://39243 (25.0), *maa://45271 (57.89)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (89.41), maa://36669 (86.36), *maa://23264 (61.82)</t>
+          <t>maa://28977 (89.41), maa://36669 (86.67), *maa://23264 (61.82)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1769,7 +1769,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.48), maa://22755 (87.83), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.5), maa://22755 (87.83), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1867,7 +1867,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (89.32)</t>
+          <t>maa://21287 (89.42)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1883,7 +1883,7 @@
       </c>
       <c r="P11" s="2" t="inlineStr">
         <is>
-          <t>maa://45557 (87.5)</t>
+          <t>maa://45557 (88.89)</t>
         </is>
       </c>
       <c r="Q11" s="1" t="n"/>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.5), maa://22501 (97.73), maa://45521 (84.21)</t>
+          <t>maa://22747 (92.5), maa://22501 (97.78), maa://45521 (85.0)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (89.94), ***maa://45826 (20.0)</t>
+          <t>maa://21867 (89.94), **maa://45826 (33.33)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2045,7 +2045,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.01), *maa://21485 (75.89), maa://37962 (90.24)</t>
+          <t>maa://22753 (91.06), *maa://21485 (75.35), maa://37962 (90.48)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.13), maa://36673 (93.33), maa://25001 (85.71)</t>
+          <t>maa://24999 (92.16), maa://36673 (93.33), maa://25001 (85.71)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2111,7 +2111,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.53), **maa://22728 (46.67)</t>
+          <t>*maa://21248 (73.33), **maa://22728 (46.67)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (92.8), *maa://22583 (75.0), *maa://22500 (58.7)</t>
+          <t>maa://22676 (92.86), *maa://22583 (75.0), *maa://22500 (58.7)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2225,7 +2225,7 @@
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>maa://30764 (89.09)</t>
+          <t>maa://30764 (87.5)</t>
         </is>
       </c>
       <c r="E14" s="1" t="n"/>
@@ -2257,7 +2257,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.75), maa://21288 (96.3), maa://39841 (95.33), maa://36682 (97.44)</t>
+          <t>maa://26245 (96.75), maa://21288 (96.3), maa://39841 (94.55), maa://36682 (97.44)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2355,7 +2355,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.04), maa://22734 (84.17), *maa://30808 (64.18), **maa://36048 (45.0), maa://45058 (92.86)</t>
+          <t>*maa://22743 (78.04), maa://22734 (84.17), *maa://30808 (64.18), **maa://36048 (46.77), maa://45058 (92.86)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.07), maa://21478 (89.19)</t>
+          <t>maa://24304 (88.13), maa://21478 (89.19)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2435,7 +2435,7 @@
       </c>
       <c r="X15" s="2" t="inlineStr">
         <is>
-          <t>*maa://38786 (75.0)</t>
+          <t>*maa://38786 (66.67)</t>
         </is>
       </c>
       <c r="Y15" s="1" t="n"/>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.78), *maa://36666 (77.68), *maa://22766 (68.64)</t>
+          <t>maa://21364 (80.84), *maa://36666 (77.68), *maa://22766 (68.64)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (95.06), *maa://28648 (69.12), maa://36674 (82.69)</t>
+          <t>maa://22729 (94.48), *maa://28648 (69.12), maa://36674 (82.69)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2615,7 +2615,7 @@
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>maa://21624 (84.21)</t>
+          <t>maa://21624 (84.62)</t>
         </is>
       </c>
       <c r="E17" s="1" t="n"/>
@@ -2631,7 +2631,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.78), maa://39599 (86.27)</t>
+          <t>maa://22430 (88.83), maa://39599 (86.27)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (88.98)</t>
+          <t>maa://24421 (89.02)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2777,7 +2777,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (90.42), *maa://22732 (50.55)</t>
+          <t>maa://22466 (90.53), *maa://22732 (50.55)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.17), maa://25198 (93.64), *maa://20795 (50.77), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.23), maa://25198 (93.64), *maa://20795 (50.77), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (89.87)</t>
+          <t>maa://22864 (89.94)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.16)</t>
+          <t>maa://41331 (85.26)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="L21" s="2" t="inlineStr">
         <is>
-          <t>maa://31731 (96.08)</t>
+          <t>maa://31731 (96.15)</t>
         </is>
       </c>
       <c r="M21" s="1" t="n"/>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.17), *maa://22432 (77.03)</t>
+          <t>maa://22524 (94.17), *maa://22432 (77.63)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>maa://25236 (95.6), **maa://21678 (48.94), **maa://22735 (42.86)</t>
+          <t>maa://25236 (95.7), **maa://21678 (48.94), **maa://22735 (42.86)</t>
         </is>
       </c>
       <c r="I22" s="1" t="n"/>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>*maa://27127 (79.66), *maa://22751 (71.01)</t>
+          <t>*maa://27127 (78.99), *maa://22751 (71.01)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.69), maa://39875 (94.44)</t>
+          <t>maa://39756 (95.74), maa://39875 (94.44)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3443,7 +3443,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.92), *maa://29748 (75.97), ***maa://29785 (16.18), *maa://37566 (76.92)</t>
+          <t>maa://30587 (92.0), *maa://29748 (75.97), ***maa://29785 (16.18), *maa://37566 (76.92)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.27), *maa://46650 (60.0)</t>
+          <t>*maa://24368 (78.27), **maa://46650 (50.0)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3605,7 +3605,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (84.31), maa://23504 (93.19), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (76.92), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (84.44), maa://23504 (93.21), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (76.92), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3637,7 +3637,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (86.0), maa://36672 (80.36), maa://29910 (93.22), **maa://21440 (35.71), *maa://45831 (75.0)</t>
+          <t>maa://22523 (85.57), maa://36672 (80.36), maa://29910 (93.22), **maa://21440 (35.71), *maa://45831 (80.0)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3671,7 +3671,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (73.17), *maa://25311 (74.04), ***maa://22725 (4.84), *maa://45047 (62.5)</t>
+          <t>*maa://29063 (73.33), *maa://25311 (74.29), ***maa://22725 (4.84), *maa://45047 (62.5)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3719,7 +3719,7 @@
       </c>
       <c r="T25" s="2" t="inlineStr">
         <is>
-          <t>maa://20109 (92.13), maa://22545 (100.0), *maa://42915 (75.0)</t>
+          <t>maa://20109 (92.18), maa://22545 (100.0), *maa://42915 (75.0)</t>
         </is>
       </c>
       <c r="U25" s="1" t="n"/>
@@ -3767,7 +3767,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.35), maa://24621 (96.88), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
+          <t>maa://20108 (96.35), maa://24621 (96.9), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (94.17)</t>
+          <t>maa://42235 (94.23)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4109,7 +4109,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>*maa://29765 (63.86), maa://23263 (95.28)</t>
+          <t>*maa://29765 (64.29), maa://23263 (95.28)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.77), maa://41749 (90.7), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.63), maa://41749 (90.91), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4157,7 +4157,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.31), *maa://36701 (66.67)</t>
+          <t>maa://36660 (92.35), *maa://36701 (66.67)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.49), *maa://28440 (80.0), maa://31400 (98.81), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.53), maa://28440 (80.18), maa://31400 (98.81), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4353,7 +4353,7 @@
       </c>
       <c r="P30" s="2" t="inlineStr">
         <is>
-          <t>maa://21442 (99.11)</t>
+          <t>maa://21442 (99.12)</t>
         </is>
       </c>
       <c r="Q30" s="1" t="n"/>
@@ -4467,7 +4467,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.49), maa://36258 (85.47), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.52), maa://36258 (85.47), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4581,7 +4581,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.01), maa://36667 (97.62), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.04), maa://36667 (97.62), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4629,7 +4629,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (95.97), maa://41108 (88.0), maa://41238 (97.12), maa://45523 (100.0)</t>
+          <t>maa://42859 (95.97), maa://41108 (88.0), maa://41238 (97.14), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4743,7 +4743,7 @@
       </c>
       <c r="P33" s="2" t="inlineStr">
         <is>
-          <t>maa://21956 (81.08), *maa://22730 (79.31)</t>
+          <t>maa://21956 (81.21), *maa://22730 (79.31)</t>
         </is>
       </c>
       <c r="Q33" s="1" t="n"/>
@@ -4889,7 +4889,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (93.08)</t>
+          <t>maa://24526 (93.1)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4987,7 +4987,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.27)</t>
+          <t>maa://41296 (96.3)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5051,7 +5051,7 @@
       </c>
       <c r="AF35" s="2" t="inlineStr">
         <is>
-          <t>maa://39479 (94.12)</t>
+          <t>maa://39479 (88.89)</t>
         </is>
       </c>
       <c r="AG35" s="1" t="n"/>
@@ -5183,7 +5183,7 @@
       </c>
       <c r="H37" s="2" t="inlineStr">
         <is>
-          <t>*maa://24374 (56.82)</t>
+          <t>*maa://24374 (55.56)</t>
         </is>
       </c>
       <c r="I37" s="1" t="n"/>
@@ -5199,7 +5199,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (97.92), *maa://47069 (69.23), maa://45789 (100.0)</t>
+          <t>maa://45718 (97.96), *maa://47069 (71.43), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5215,7 +5215,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.4), *maa://21239 (66.67)</t>
+          <t>maa://21280 (89.45), *maa://21239 (66.67)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5364,7 +5364,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.38)</t>
+          <t>maa://36697 (86.45)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5385,7 +5385,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (89.11), maa://25199 (84.82), maa://30434 (91.46), ***maa://25036 (16.0), maa://45059 (83.33), *maa://44165 (66.67)</t>
+          <t>maa://36670 (89.11), maa://25199 (84.82), maa://30434 (91.57), ***maa://25036 (16.0), maa://45059 (83.33), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (81.63), maa://47079 (94.12), *maa://45790 (75.0)</t>
+          <t>maa://45788 (82.0), maa://47079 (94.12), *maa://45790 (75.0)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5587,7 +5587,7 @@
       </c>
       <c r="P41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (40.0), maa://43177 (90.91)</t>
+          <t>**maa://35616 (40.0), maa://43177 (91.3)</t>
         </is>
       </c>
       <c r="Q41" s="1" t="n"/>
@@ -5725,7 +5725,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (92.36), maa://21284 (85.42)</t>
+          <t>maa://22525 (92.41), maa://21284 (85.42)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5847,7 +5847,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.82), maa://30807 (95.65), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (85.71)</t>
+          <t>maa://21229 (84.82), maa://30807 (95.65), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (86.36)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5879,7 +5879,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (38.71)</t>
+          <t>**maa://39364 (37.5)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -6282,7 +6282,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (91.91)</t>
+          <t>maa://32532 (91.94)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6336,7 +6336,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (61.54)</t>
+          <t>*maa://37964 (60.98)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#165)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.62), *maa://20791 (62.16)</t>
+          <t>maa://22742 (91.67), *maa://20791 (62.16)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.83), **maa://20790 (43.48), ***maa://37170 (16.67), maa://45854 (87.5)</t>
+          <t>maa://24617 (89.83), **maa://20790 (43.48), ***maa://37170 (16.67), maa://45854 (84.0)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (96.3)</t>
+          <t>maa://42407 (96.36)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.03.06 13:18:49</t>
+          <t>更新日期：2025.03.07 13:21:00</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.95)</t>
+          <t>maa://21411 (95.96)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1623,7 +1623,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (83.33)</t>
+          <t>maa://22736 (83.5)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1655,7 +1655,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.93)</t>
+          <t>maa://26223 (97.95)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.62), ***maa://39951 (14.29), ***maa://34206 (19.23), ***maa://39243 (25.0), *maa://45271 (57.89)</t>
+          <t>***maa://25695 (18.62), ***maa://39951 (14.04), ***maa://34206 (19.23), ***maa://39243 (25.0), *maa://45271 (58.97)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1769,7 +1769,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.5), maa://22755 (87.83), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.53), maa://22755 (87.83), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.5), maa://22501 (97.78), maa://45521 (85.0)</t>
+          <t>maa://22747 (92.55), maa://22501 (97.78), maa://45521 (85.0)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.77)</t>
+          <t>maa://36713 (97.78)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1931,7 +1931,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://29912 (97.18), maa://22516 (88.37), *maa://20794 (52.24)</t>
+          <t>maa://29912 (97.22), maa://22516 (88.37), *maa://20794 (52.24)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (89.94), **maa://45826 (33.33)</t>
+          <t>maa://21867 (90.0), **maa://45826 (33.33)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2045,7 +2045,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.06), *maa://21485 (75.35), maa://37962 (90.48)</t>
+          <t>maa://22753 (91.06), *maa://21485 (75.35), maa://37962 (90.7)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (92.86), *maa://22583 (75.0), *maa://22500 (58.7)</t>
+          <t>maa://22676 (92.97), *maa://22583 (75.0), *maa://22500 (58.7)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="AB14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (97.14)</t>
+          <t>maa://22764 (97.18)</t>
         </is>
       </c>
       <c r="AC14" s="1" t="n"/>
@@ -2355,7 +2355,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.04), maa://22734 (84.17), *maa://30808 (64.18), **maa://36048 (46.77), maa://45058 (92.86)</t>
+          <t>*maa://22743 (78.04), maa://22734 (84.17), *maa://30808 (64.18), **maa://36048 (46.77), maa://45058 (93.33)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2403,7 +2403,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (90.3), *maa://22727 (70.0)</t>
+          <t>maa://24762 (90.36), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.23), maa://25198 (93.64), *maa://20795 (50.77), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.29), maa://25198 (93.64), *maa://20795 (50.77), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>maa://25236 (95.7), **maa://21678 (48.94), **maa://22735 (42.86)</t>
+          <t>maa://25236 (95.74), **maa://21678 (48.94), **maa://22735 (42.86)</t>
         </is>
       </c>
       <c r="I22" s="1" t="n"/>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.6), *maa://37649 (65.52)</t>
+          <t>maa://21282 (98.61), *maa://37649 (65.52)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3395,7 +3395,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.77), *maa://41753 (57.89)</t>
+          <t>***maa://28036 (28.77), *maa://41753 (55.0)</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.74), maa://39875 (94.44)</t>
+          <t>maa://39756 (95.76), maa://39875 (94.44)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3475,7 +3475,7 @@
       </c>
       <c r="X23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (68.75)</t>
+          <t>*maa://28503 (69.14)</t>
         </is>
       </c>
       <c r="Y23" s="1" t="n"/>
@@ -3605,7 +3605,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (84.44), maa://23504 (93.21), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (76.92), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (84.11), maa://23504 (93.22), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (76.92), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3785,7 +3785,7 @@
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>maa://41802 (94.44)</t>
+          <t>maa://41802 (94.74)</t>
         </is>
       </c>
       <c r="E26" s="1" t="n"/>
@@ -4077,7 +4077,7 @@
       </c>
       <c r="L28" s="2" t="inlineStr">
         <is>
-          <t>maa://30770 (80.85)</t>
+          <t>maa://30770 (81.25)</t>
         </is>
       </c>
       <c r="M28" s="1" t="n"/>
@@ -4109,7 +4109,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>*maa://29765 (64.29), maa://23263 (95.28)</t>
+          <t>*maa://29765 (64.71), maa://23263 (95.28)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4305,7 +4305,7 @@
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>maa://45792 (100.0)</t>
+          <t>maa://45792 (93.33)</t>
         </is>
       </c>
       <c r="E30" s="1" t="n"/>
@@ -4467,7 +4467,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.52), maa://36258 (85.47), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.52), maa://36258 (84.75), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4581,7 +4581,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.04), maa://36667 (97.62), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.04), maa://36667 (97.65), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4868,12 +4868,12 @@
       </c>
       <c r="O34" s="1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0</t>
         </is>
       </c>
       <c r="P34" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>None</t>
         </is>
       </c>
       <c r="Q34" s="1" t="n"/>
@@ -5051,7 +5051,7 @@
       </c>
       <c r="AF35" s="2" t="inlineStr">
         <is>
-          <t>maa://39479 (88.89)</t>
+          <t>maa://39479 (89.47)</t>
         </is>
       </c>
       <c r="AG35" s="1" t="n"/>
@@ -5199,7 +5199,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (97.96), *maa://47069 (71.43), maa://45789 (100.0)</t>
+          <t>maa://45718 (97.96), *maa://47069 (73.33), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5215,7 +5215,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.45), *maa://21239 (66.67)</t>
+          <t>maa://21280 (89.5), *maa://21239 (66.67)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5316,7 +5316,7 @@
       </c>
       <c r="P38" s="2" t="inlineStr">
         <is>
-          <t>*maa://24383 (69.61)</t>
+          <t>*maa://24383 (68.93)</t>
         </is>
       </c>
       <c r="Q38" s="1" t="n"/>
@@ -5385,7 +5385,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (89.11), maa://25199 (84.82), maa://30434 (91.57), ***maa://25036 (16.0), maa://45059 (83.33), *maa://44165 (66.67)</t>
+          <t>maa://36670 (89.11), maa://25199 (84.82), maa://30434 (91.67), ***maa://25036 (16.0), maa://45059 (83.33), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5830,6 +5830,22 @@
         </is>
       </c>
       <c r="U44" s="1" t="n"/>
+      <c r="AD44" s="1" t="inlineStr">
+        <is>
+          <t>钼铅</t>
+        </is>
+      </c>
+      <c r="AE44" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF44" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG44" s="1" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="B45" s="3" t="n"/>
@@ -6232,6 +6248,22 @@
         </is>
       </c>
       <c r="Q52" s="1" t="n"/>
+      <c r="R52" s="1" t="inlineStr">
+        <is>
+          <t>死芒</t>
+        </is>
+      </c>
+      <c r="S52" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T52" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U52" s="1" t="n"/>
     </row>
     <row r="53">
       <c r="F53" s="1" t="inlineStr">
@@ -6250,6 +6282,22 @@
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
+      <c r="N53" s="1" t="inlineStr">
+        <is>
+          <t>水灯心</t>
+        </is>
+      </c>
+      <c r="O53" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P53" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q53" s="1" t="n"/>
     </row>
     <row r="54">
       <c r="F54" s="1" t="inlineStr">
@@ -6336,7 +6384,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (60.98)</t>
+          <t>*maa://37964 (59.52)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>
@@ -6372,7 +6420,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (69.35)</t>
+          <t>*maa://40438 (69.84)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#166)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.17), *maa://30515 (69.9), *maa://34787 (73.33), maa://39402 (92.19), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.17), *maa://30515 (69.9), *maa://34787 (73.68), maa://39402 (92.19), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.67), *maa://20791 (62.16)</t>
+          <t>maa://22742 (91.12), *maa://20791 (62.16)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.83), **maa://20790 (43.48), ***maa://37170 (16.67), maa://45854 (84.0)</t>
+          <t>maa://24617 (89.83), **maa://20790 (43.48), ***maa://37170 (16.42), maa://45854 (84.0)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (90.62), ***maa://36683 (28.26)</t>
+          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (90.91), ***maa://36683 (28.26)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (96.36)</t>
+          <t>maa://42407 (96.43)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="T7" s="2" t="inlineStr">
         <is>
-          <t>maa://21291 (84.78)</t>
+          <t>maa://21291 (85.11)</t>
         </is>
       </c>
       <c r="U7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.03.07 13:21:00</t>
+          <t>更新日期：2025.03.08 13:15:15</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1639,7 +1639,7 @@
       </c>
       <c r="T9" s="2" t="inlineStr">
         <is>
-          <t>**maa://22866 (30.19), maa://26222 (98.04)</t>
+          <t>**maa://22866 (30.19), maa://26222 (98.08)</t>
         </is>
       </c>
       <c r="U9" s="1" t="n"/>
@@ -1655,7 +1655,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.95)</t>
+          <t>maa://26223 (97.96)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1931,7 +1931,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://29912 (97.22), maa://22516 (88.37), *maa://20794 (52.24)</t>
+          <t>maa://29912 (97.26), maa://22516 (88.37), *maa://20794 (52.24)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (77.7), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (77.85), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.16), maa://36673 (93.33), maa://25001 (85.71)</t>
+          <t>maa://24999 (92.17), maa://36673 (93.33), maa://25001 (85.71)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2175,7 +2175,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>maa://34957 (81.82), *maa://22768 (51.61)</t>
+          <t>maa://34957 (82.05), **maa://22768 (50.0)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="AB14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (97.18)</t>
+          <t>maa://22764 (97.22)</t>
         </is>
       </c>
       <c r="AC14" s="1" t="n"/>
@@ -2485,7 +2485,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.41), maa://36679 (94.44), maa://37650 (97.3)</t>
+          <t>maa://21441 (96.41), maa://36679 (94.55), maa://37650 (97.3)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2777,7 +2777,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (90.53), *maa://22732 (50.55)</t>
+          <t>maa://22466 (90.53), *maa://22732 (51.09)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (99.15)</t>
+          <t>maa://24386 (99.17)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -2971,7 +2971,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (65.83), *maa://36668 (57.5)</t>
+          <t>*maa://30709 (65.91), *maa://36668 (57.5)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.29), maa://25198 (93.64), *maa://20795 (50.77), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.34), maa://25198 (93.64), *maa://20795 (50.77), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.26)</t>
+          <t>maa://41331 (85.44)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="P20" s="2" t="inlineStr">
         <is>
-          <t>maa://37442 (95.12)</t>
+          <t>maa://37442 (95.24)</t>
         </is>
       </c>
       <c r="Q20" s="1" t="n"/>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="L21" s="2" t="inlineStr">
         <is>
-          <t>maa://31731 (96.15)</t>
+          <t>maa://31731 (96.23)</t>
         </is>
       </c>
       <c r="M21" s="1" t="n"/>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.76), maa://39875 (94.44)</t>
+          <t>maa://39756 (95.81), maa://39875 (94.52)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3637,7 +3637,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.57), maa://36672 (80.36), maa://29910 (93.22), **maa://21440 (35.71), *maa://45831 (80.0)</t>
+          <t>maa://22523 (85.64), maa://36672 (80.7), maa://29910 (93.22), **maa://21440 (35.71), *maa://45831 (80.0)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3655,7 +3655,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.17)</t>
+          <t>maa://29753 (95.19)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3735,7 +3735,7 @@
       </c>
       <c r="X25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29890 (78.72)</t>
+          <t>*maa://29890 (79.17)</t>
         </is>
       </c>
       <c r="Y25" s="1" t="n"/>
@@ -3751,7 +3751,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (87.93), maa://24516 (80.22), maa://26001 (87.5)</t>
+          <t>maa://31215 (88.03), maa://24516 (80.22), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3785,7 +3785,7 @@
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>maa://41802 (94.74)</t>
+          <t>maa://41802 (95.0)</t>
         </is>
       </c>
       <c r="E26" s="1" t="n"/>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.63), maa://41749 (90.91), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.68), maa://41749 (90.91), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4157,7 +4157,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.35), *maa://36701 (66.67)</t>
+          <t>maa://36660 (92.37), *maa://36701 (66.67)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.53), maa://28440 (80.18), maa://31400 (98.81), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.55), maa://28440 (80.36), maa://31400 (98.82), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4401,7 +4401,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.02), maa://45822 (100.0), *maa://45045 (80.0)</t>
+          <t>maa://42979 (97.04), maa://45822 (100.0), *maa://45045 (80.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4629,7 +4629,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (95.97), maa://41108 (88.0), maa://41238 (97.14), maa://45523 (100.0)</t>
+          <t>maa://42859 (96.0), maa://41108 (88.0), maa://41238 (97.14), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4987,7 +4987,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.3)</t>
+          <t>maa://41296 (96.34)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5199,7 +5199,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (97.96), *maa://47069 (73.33), maa://45789 (100.0)</t>
+          <t>maa://45718 (97.99), *maa://47069 (73.33), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (82.0), maa://47079 (94.12), *maa://45790 (75.0)</t>
+          <t>maa://45788 (82.18), maa://47079 (94.12), *maa://45790 (76.92)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5725,7 +5725,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (92.41), maa://21284 (85.42)</t>
+          <t>maa://22525 (92.41), maa://21284 (85.71)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5826,7 +5826,7 @@
       </c>
       <c r="T44" s="2" t="inlineStr">
         <is>
-          <t>maa://39366 (88.89)</t>
+          <t>maa://39366 (89.19)</t>
         </is>
       </c>
       <c r="U44" s="1" t="n"/>
@@ -5895,7 +5895,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (37.5)</t>
+          <t>**maa://39364 (36.36)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -5916,7 +5916,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (91.95), maa://43901 (92.59)</t>
+          <t>maa://35931 (91.95), maa://43901 (93.1)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.1), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.12), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6330,7 +6330,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (91.94)</t>
+          <t>maa://32532 (91.96)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6402,7 +6402,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://31270 (95.38), maa://27746 (82.3)</t>
+          <t>maa://31270 (94.66), maa://27746 (82.3)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6420,7 +6420,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (69.84)</t>
+          <t>*maa://40438 (70.31)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#167)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.83), **maa://20790 (43.48), ***maa://37170 (16.42), maa://45854 (84.0)</t>
+          <t>maa://24617 (89.83), **maa://20790 (43.48), ***maa://37170 (16.42), maa://45854 (80.77)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (96.43)</t>
+          <t>maa://42407 (96.49)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.03.08 13:15:15</t>
+          <t>更新日期：2025.03.08 16:37:02</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1883,7 +1883,7 @@
       </c>
       <c r="P11" s="2" t="inlineStr">
         <is>
-          <t>maa://45557 (88.89)</t>
+          <t>maa://45557 (90.0)</t>
         </is>
       </c>
       <c r="Q11" s="1" t="n"/>
@@ -2241,7 +2241,7 @@
       </c>
       <c r="H14" s="2" t="inlineStr">
         <is>
-          <t>**maa://32656 (50.0)</t>
+          <t>**maa://32656 (40.0)</t>
         </is>
       </c>
       <c r="I14" s="1" t="n"/>
@@ -2273,7 +2273,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.74), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.75), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2745,7 +2745,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.36)</t>
+          <t>maa://24570 (96.93)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2777,7 +2777,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (90.53), *maa://22732 (51.09)</t>
+          <t>maa://22466 (90.53), *maa://22732 (50.54)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="AF19" s="2" t="inlineStr">
         <is>
-          <t>*maa://21663 (63.89)</t>
+          <t>*maa://21663 (63.01)</t>
         </is>
       </c>
       <c r="AG19" s="1" t="n"/>
@@ -3605,7 +3605,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (84.11), maa://23504 (93.22), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (76.92), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (84.11), maa://23504 (93.24), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (76.92), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="AF32" s="2" t="inlineStr">
         <is>
-          <t>*maa://42408 (80.0)</t>
+          <t>maa://42408 (81.82)</t>
         </is>
       </c>
       <c r="AG32" s="1" t="n"/>
@@ -4889,7 +4889,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (93.1)</t>
+          <t>maa://24526 (92.75)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -5199,7 +5199,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (97.99), *maa://47069 (73.33), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.01), *maa://47069 (73.33), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -6492,7 +6492,7 @@
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>maa://44405 (88.46)</t>
+          <t>maa://44405 (85.19)</t>
         </is>
       </c>
       <c r="I64" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#168)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.54), maa://25390 (96.2), maa://36681 (87.34)</t>
+          <t>maa://24702 (94.58), maa://25390 (96.2), maa://36681 (87.34)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.17), *maa://30515 (69.9), *maa://34787 (73.68), maa://39402 (92.19), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.17), *maa://30515 (70.19), maa://39402 (92.31), *maa://34787 (72.73), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.12), *maa://20791 (62.16)</t>
+          <t>maa://22742 (90.59), *maa://20791 (61.33)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.41), maa://36684 (95.65), ***maa://22731 (6.25)</t>
+          <t>maa://21246 (91.41), maa://36684 (95.8), ***maa://22731 (6.25)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (91.53), ***maa://21730 (26.32), ***maa://39501 (15.62), **maa://36675 (50.0)</t>
+          <t>maa://25251 (91.67), ***maa://21730 (26.32), ***maa://39501 (15.62), **maa://36675 (50.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://40192 (98.18), maa://36987 (96.08), maa://39849 (88.89)</t>
+          <t>maa://40192 (96.49), maa://36987 (96.15), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.33), maa://20276 (86.59), *maa://22749 (75.0)</t>
+          <t>*maa://22880 (65.0), maa://20276 (86.59), *maa://22749 (75.0)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.54), maa://26254 (96.67)</t>
+          <t>maa://21249 (94.58), maa://26254 (96.67)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.36), maa://27484 (96.58), maa://27480 (83.33)</t>
+          <t>maa://27396 (84.36), maa://27484 (96.61), maa://27480 (83.33)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (94.74)</t>
+          <t>maa://24390 (94.81)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -901,7 +901,7 @@
       </c>
       <c r="AF3" s="2" t="inlineStr">
         <is>
-          <t>*maa://21289 (73.08)</t>
+          <t>*maa://21289 (74.07)</t>
         </is>
       </c>
       <c r="AG3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (94.15), **maa://24303 (33.33), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.6), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (95.76), maa://27295 (86.11), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
+          <t>maa://32509 (95.76), maa://27295 (86.3), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (90.91), ***maa://36683 (28.26)</t>
+          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (91.55), ***maa://36683 (28.26)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1015,7 +1015,7 @@
       </c>
       <c r="AB4" s="2" t="inlineStr">
         <is>
-          <t>*maa://32658 (68.42)</t>
+          <t>*maa://32658 (70.0)</t>
         </is>
       </c>
       <c r="AC4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.58), maa://22744 (84.0)</t>
+          <t>maa://21245 (84.3), maa://22744 (84.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="P5" s="2" t="inlineStr">
         <is>
-          <t>maa://21919 (96.55), *maa://21281 (80.0)</t>
+          <t>maa://21919 (96.61), *maa://21281 (80.0)</t>
         </is>
       </c>
       <c r="Q5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (96.49)</t>
+          <t>maa://42407 (96.61)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>maa://24370 (96.67)</t>
+          <t>maa://24370 (96.72)</t>
         </is>
       </c>
       <c r="I6" s="1" t="n"/>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="P6" s="2" t="inlineStr">
         <is>
-          <t>maa://31836 (93.1), maa://30381 (93.33)</t>
+          <t>maa://31836 (93.1), maa://30381 (93.75)</t>
         </is>
       </c>
       <c r="Q6" s="1" t="n"/>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="AF6" s="2" t="inlineStr">
         <is>
-          <t>*maa://33152 (64.15), ***maa://22770 (26.09)</t>
+          <t>*maa://33152 (64.81), ***maa://22770 (26.09)</t>
         </is>
       </c>
       <c r="AG6" s="1" t="n"/>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>maa://21955 (94.87)</t>
+          <t>maa://21955 (95.0)</t>
         </is>
       </c>
       <c r="E7" s="1" t="n"/>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>*maa://22763 (66.67)</t>
+          <t>*maa://22763 (65.71)</t>
         </is>
       </c>
       <c r="I7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.51), *maa://22758 (74.29)</t>
+          <t>maa://22399 (95.57), *maa://22758 (74.29)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.03.08 16:37:02</t>
+          <t>更新日期：2025.03.15 13:17:29</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24371 (55.41)</t>
+          <t>*maa://24371 (56.0)</t>
         </is>
       </c>
       <c r="I8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.96)</t>
+          <t>maa://21411 (95.98)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="AB8" s="2" t="inlineStr">
         <is>
-          <t>maa://25389 (88.89)</t>
+          <t>maa://25389 (89.19)</t>
         </is>
       </c>
       <c r="AC8" s="1" t="n"/>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="AF8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24479 (78.16), *maa://21990 (51.85)</t>
+          <t>*maa://24479 (78.41), *maa://21990 (51.85)</t>
         </is>
       </c>
       <c r="AG8" s="1" t="n"/>
@@ -1607,7 +1607,7 @@
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>maa://22762 (92.31), *maa://39552 (80.0)</t>
+          <t>maa://22762 (92.39), *maa://39552 (80.0)</t>
         </is>
       </c>
       <c r="M9" s="1" t="n"/>
@@ -1623,7 +1623,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (83.5)</t>
+          <t>maa://22736 (82.69)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1639,7 +1639,7 @@
       </c>
       <c r="T9" s="2" t="inlineStr">
         <is>
-          <t>**maa://22866 (30.19), maa://26222 (98.08)</t>
+          <t>**maa://22866 (30.19), maa://26222 (98.11)</t>
         </is>
       </c>
       <c r="U9" s="1" t="n"/>
@@ -1655,7 +1655,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.96)</t>
+          <t>maa://26223 (97.99)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (87.8), *maa://22865 (51.85)</t>
+          <t>maa://26206 (87.9), *maa://22865 (51.85)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.62), ***maa://39951 (14.04), ***maa://34206 (19.23), ***maa://39243 (25.0), *maa://45271 (58.97)</t>
+          <t>***maa://25695 (18.52), ***maa://39951 (13.79), ***maa://34206 (19.23), ***maa://39243 (25.0), *maa://45271 (58.97)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="L10" s="2" t="inlineStr">
         <is>
-          <t>**maa://24395 (40.62)</t>
+          <t>**maa://24395 (39.39)</t>
         </is>
       </c>
       <c r="M10" s="1" t="n"/>
@@ -1769,7 +1769,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.53), maa://22755 (87.83), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.55), maa://22755 (87.83), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.75), maa://45828 (92.86), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.76), maa://45828 (92.86), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (54.17), *maa://22733 (61.11), **maa://22761 (50.0)</t>
+          <t>*maa://25021 (54.55), *maa://22733 (62.16), **maa://22761 (50.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1835,7 +1835,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.48)</t>
+          <t>maa://36707 (99.49)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -1883,7 +1883,7 @@
       </c>
       <c r="P11" s="2" t="inlineStr">
         <is>
-          <t>maa://45557 (90.0)</t>
+          <t>maa://45557 (90.91)</t>
         </is>
       </c>
       <c r="Q11" s="1" t="n"/>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.55), maa://22501 (97.78), maa://45521 (85.0)</t>
+          <t>maa://22747 (92.59), maa://22501 (97.8), maa://45521 (85.71)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.78)</t>
+          <t>maa://36713 (97.8)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1931,7 +1931,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://29912 (97.26), maa://22516 (88.37), *maa://20794 (52.24)</t>
+          <t>maa://29912 (97.3), maa://22516 (88.37), *maa://20794 (52.24)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (90.0), **maa://45826 (33.33)</t>
+          <t>maa://21867 (90.0), ***maa://45826 (28.57)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.5), maa://36677 (93.65), maa://39872 (91.67)</t>
+          <t>maa://23669 (95.5), maa://36677 (93.85), maa://39872 (92.0)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (77.85), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (78.0), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.17), maa://36673 (93.33), maa://25001 (85.71)</t>
+          <t>maa://24999 (92.21), maa://36673 (92.21), maa://25001 (85.71)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2111,7 +2111,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.33), **maa://22728 (46.67)</t>
+          <t>*maa://21248 (73.44), **maa://22728 (46.67)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (92.97), *maa://22583 (75.0), *maa://22500 (58.7)</t>
+          <t>maa://22676 (93.02), *maa://22583 (75.0), *maa://22500 (58.7)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2175,7 +2175,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>maa://34957 (82.05), **maa://22768 (50.0)</t>
+          <t>maa://34957 (82.5), **maa://22768 (50.0)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2225,7 +2225,7 @@
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>maa://30764 (87.5)</t>
+          <t>maa://30764 (88.14)</t>
         </is>
       </c>
       <c r="E14" s="1" t="n"/>
@@ -2257,7 +2257,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.75), maa://21288 (96.3), maa://39841 (94.55), maa://36682 (97.44)</t>
+          <t>maa://26245 (96.77), maa://21288 (96.3), maa://39841 (94.69), maa://36682 (97.44)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="AB14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (97.22)</t>
+          <t>maa://22764 (97.26)</t>
         </is>
       </c>
       <c r="AC14" s="1" t="n"/>
@@ -2355,7 +2355,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.04), maa://22734 (84.17), *maa://30808 (64.18), **maa://36048 (46.77), maa://45058 (93.33)</t>
+          <t>*maa://22743 (78.24), maa://22734 (84.17), *maa://30808 (64.18), **maa://36048 (50.0), maa://45058 (93.33)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.13), maa://21478 (89.19)</t>
+          <t>maa://24304 (88.18), maa://21478 (89.19)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2387,7 +2387,7 @@
       </c>
       <c r="L15" s="2" t="inlineStr">
         <is>
-          <t>*maa://21334 (53.33)</t>
+          <t>*maa://21334 (54.84)</t>
         </is>
       </c>
       <c r="M15" s="1" t="n"/>
@@ -2403,7 +2403,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (90.36), *maa://22727 (70.0)</t>
+          <t>maa://24762 (90.42), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="T15" s="2" t="inlineStr">
         <is>
-          <t>maa://23892 (96.2)</t>
+          <t>maa://23892 (96.25)</t>
         </is>
       </c>
       <c r="U15" s="1" t="n"/>
@@ -2435,7 +2435,7 @@
       </c>
       <c r="X15" s="2" t="inlineStr">
         <is>
-          <t>*maa://38786 (66.67)</t>
+          <t>*maa://38786 (70.0)</t>
         </is>
       </c>
       <c r="Y15" s="1" t="n"/>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.84), *maa://36666 (77.68), *maa://22766 (68.64)</t>
+          <t>maa://21364 (81.01), *maa://36666 (77.39), *maa://22766 (68.64)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2485,7 +2485,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.41), maa://36679 (94.55), maa://37650 (97.3)</t>
+          <t>maa://21441 (96.41), maa://36679 (94.55), maa://37650 (97.5)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2533,7 +2533,7 @@
       </c>
       <c r="P16" s="2" t="inlineStr">
         <is>
-          <t>maa://28504 (91.23)</t>
+          <t>maa://28504 (91.53)</t>
         </is>
       </c>
       <c r="Q16" s="1" t="n"/>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.48), *maa://28648 (69.12), maa://36674 (82.69)</t>
+          <t>maa://22729 (94.51), *maa://28648 (69.57), maa://36674 (82.69)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2565,7 +2565,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (98.02), maa://28051 (96.0)</t>
+          <t>maa://28501 (98.08), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2581,7 +2581,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.96)</t>
+          <t>maa://26228 (96.04)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (65.09), maa://27755 (93.55)</t>
+          <t>*maa://23911 (65.42), maa://27755 (93.62)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2631,7 +2631,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.83), maa://39599 (86.27)</t>
+          <t>maa://22430 (88.83), maa://39599 (86.54)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>**maa://42324 (50.0)</t>
+          <t>*maa://42324 (53.12)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2745,7 +2745,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.93)</t>
+          <t>maa://24570 (96.94)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2777,7 +2777,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (90.53), *maa://22732 (50.54)</t>
+          <t>maa://22466 (90.64), *maa://22732 (51.06)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2809,7 +2809,7 @@
       </c>
       <c r="T18" s="2" t="inlineStr">
         <is>
-          <t>maa://24385 (97.3)</t>
+          <t>maa://24385 (97.37)</t>
         </is>
       </c>
       <c r="U18" s="1" t="n"/>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="X18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (96.91), maa://22741 (85.71)</t>
+          <t>maa://21917 (96.94), maa://22741 (85.71)</t>
         </is>
       </c>
       <c r="Y18" s="1" t="n"/>
@@ -2841,7 +2841,7 @@
       </c>
       <c r="AB18" s="2" t="inlineStr">
         <is>
-          <t>maa://24393 (97.92)</t>
+          <t>maa://24393 (97.96)</t>
         </is>
       </c>
       <c r="AC18" s="1" t="n"/>
@@ -2852,12 +2852,12 @@
       </c>
       <c r="AE18" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (59.28), **maa://29784 (46.43)</t>
+          <t>*maa://24313 (59.28), **maa://29784 (46.43), maa://47854 (100.0)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -2971,7 +2971,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (65.91), *maa://36668 (57.5)</t>
+          <t>*maa://30709 (66.14), *maa://36668 (57.5)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="AF19" s="2" t="inlineStr">
         <is>
-          <t>*maa://21663 (63.01)</t>
+          <t>*maa://21663 (62.67)</t>
         </is>
       </c>
       <c r="AG19" s="1" t="n"/>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.34), maa://25198 (93.64), *maa://20795 (50.77), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.45), maa://25198 (93.69), *maa://20795 (50.77), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.44)</t>
+          <t>maa://41331 (85.19)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (81.12), ***maa://23820 (30.0)</t>
+          <t>maa://21443 (81.32), ***maa://23820 (30.0)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.17), *maa://22432 (77.63)</t>
+          <t>maa://22524 (94.22), *maa://22432 (77.92)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.61), *maa://37649 (65.52)</t>
+          <t>maa://21282 (98.62), *maa://37649 (65.52)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3377,7 +3377,7 @@
       </c>
       <c r="AF22" s="2" t="inlineStr">
         <is>
-          <t>maa://29658 (93.75)</t>
+          <t>maa://29658 (93.88)</t>
         </is>
       </c>
       <c r="AG22" s="1" t="n"/>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.81), maa://39875 (94.52)</t>
+          <t>maa://39756 (95.88), maa://39875 (94.52)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3443,7 +3443,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (92.0), *maa://29748 (75.97), ***maa://29785 (16.18), *maa://37566 (76.92)</t>
+          <t>maa://30587 (92.0), *maa://29748 (75.97), ***maa://29785 (16.18), *maa://37566 (77.5)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3475,7 +3475,7 @@
       </c>
       <c r="X23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (69.14)</t>
+          <t>*maa://28503 (68.29)</t>
         </is>
       </c>
       <c r="Y23" s="1" t="n"/>
@@ -3507,7 +3507,7 @@
       </c>
       <c r="AF23" s="2" t="inlineStr">
         <is>
-          <t>maa://31489 (94.12)</t>
+          <t>maa://31489 (94.44)</t>
         </is>
       </c>
       <c r="AG23" s="1" t="n"/>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.27), **maa://46650 (50.0)</t>
+          <t>*maa://24368 (78.39), *maa://46650 (57.14)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3605,7 +3605,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (84.11), maa://23504 (93.24), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (76.92), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (84.11), maa://23504 (93.32), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (77.22), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3637,7 +3637,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.64), maa://36672 (80.7), maa://29910 (93.22), **maa://21440 (35.71), *maa://45831 (80.0)</t>
+          <t>maa://22523 (85.64), maa://36672 (80.7), maa://29910 (93.22), **maa://21440 (35.71), maa://45831 (83.33)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3655,7 +3655,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.19)</t>
+          <t>maa://29753 (95.2)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3671,7 +3671,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (73.33), *maa://25311 (74.29), ***maa://22725 (4.84), *maa://45047 (62.5)</t>
+          <t>*maa://29063 (73.05), *maa://25311 (74.53), ***maa://22725 (4.84), *maa://45047 (62.5)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3735,7 +3735,7 @@
       </c>
       <c r="X25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29890 (79.17)</t>
+          <t>*maa://29890 (79.59)</t>
         </is>
       </c>
       <c r="Y25" s="1" t="n"/>
@@ -3751,7 +3751,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (88.03), maa://24516 (80.22), maa://26001 (87.5)</t>
+          <t>maa://31215 (88.14), maa://24516 (80.22), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3767,7 +3767,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.35), maa://24621 (96.9), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
+          <t>maa://20108 (96.35), maa://24621 (96.92), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3785,7 +3785,7 @@
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>maa://41802 (95.0)</t>
+          <t>maa://41802 (90.48)</t>
         </is>
       </c>
       <c r="E26" s="1" t="n"/>
@@ -3801,7 +3801,7 @@
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (92.22)</t>
+          <t>maa://24913 (91.21)</t>
         </is>
       </c>
       <c r="I26" s="1" t="n"/>
@@ -3865,7 +3865,7 @@
       </c>
       <c r="X26" s="2" t="inlineStr">
         <is>
-          <t>maa://24389 (96.55)</t>
+          <t>maa://24389 (96.67)</t>
         </is>
       </c>
       <c r="Y26" s="1" t="n"/>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (94.23)</t>
+          <t>maa://42235 (94.5)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3897,7 +3897,7 @@
       </c>
       <c r="AF26" s="2" t="inlineStr">
         <is>
-          <t>maa://30511 (80.95), *maa://29760 (60.0)</t>
+          <t>maa://30511 (81.82), *maa://29760 (56.25)</t>
         </is>
       </c>
       <c r="AG26" s="1" t="n"/>
@@ -3979,7 +3979,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (78.33)</t>
+          <t>*maa://30624 (77.05)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4045,7 +4045,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.96), maa://25725 (83.91)</t>
+          <t>maa://24465 (90.97), maa://25725 (84.27)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4077,7 +4077,7 @@
       </c>
       <c r="L28" s="2" t="inlineStr">
         <is>
-          <t>maa://30770 (81.25)</t>
+          <t>maa://30770 (81.63)</t>
         </is>
       </c>
       <c r="M28" s="1" t="n"/>
@@ -4109,7 +4109,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>*maa://29765 (64.71), maa://23263 (95.28)</t>
+          <t>*maa://29765 (63.95), maa://23263 (95.28)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.68), maa://41749 (90.91), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.77), maa://41749 (91.3), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4157,7 +4157,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.37), *maa://36701 (66.67)</t>
+          <t>maa://36660 (92.52), *maa://36701 (66.67)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.55), maa://28440 (80.36), maa://31400 (98.82), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.57), maa://28440 (80.53), maa://31400 (98.82), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4223,7 +4223,7 @@
       </c>
       <c r="P29" s="2" t="inlineStr">
         <is>
-          <t>*maa://23168 (58.06), *maa://30050 (51.52)</t>
+          <t>*maa://23168 (58.06), *maa://30050 (54.29)</t>
         </is>
       </c>
       <c r="Q29" s="1" t="n"/>
@@ -4287,7 +4287,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.85), maa://42865 (81.25), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.85), maa://42865 (81.54), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4337,7 +4337,7 @@
       </c>
       <c r="L30" s="2" t="inlineStr">
         <is>
-          <t>maa://30442 (95.24)</t>
+          <t>maa://30442 (95.31)</t>
         </is>
       </c>
       <c r="M30" s="1" t="n"/>
@@ -4385,7 +4385,7 @@
       </c>
       <c r="X30" s="2" t="inlineStr">
         <is>
-          <t>maa://39477 (90.0)</t>
+          <t>maa://39477 (90.48)</t>
         </is>
       </c>
       <c r="Y30" s="1" t="n"/>
@@ -4401,7 +4401,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.04), maa://45822 (100.0), *maa://45045 (80.0)</t>
+          <t>maa://42979 (97.11), maa://45822 (100.0), *maa://45045 (80.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4467,7 +4467,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.52), maa://36258 (84.75), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.33), maa://36258 (84.87), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4581,7 +4581,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.04), maa://36667 (97.65), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.06), maa://36667 (97.67), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4629,7 +4629,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.0), maa://41108 (88.0), maa://41238 (97.14), maa://45523 (100.0)</t>
+          <t>maa://42859 (96.09), maa://41108 (88.0), maa://41238 (97.2), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="AF32" s="2" t="inlineStr">
         <is>
-          <t>maa://42408 (81.82)</t>
+          <t>maa://42408 (83.33)</t>
         </is>
       </c>
       <c r="AG32" s="1" t="n"/>
@@ -4743,7 +4743,7 @@
       </c>
       <c r="P33" s="2" t="inlineStr">
         <is>
-          <t>maa://21956 (81.21), *maa://22730 (79.31)</t>
+          <t>maa://21956 (80.79), *maa://22730 (79.31)</t>
         </is>
       </c>
       <c r="Q33" s="1" t="n"/>
@@ -4759,7 +4759,7 @@
       </c>
       <c r="T33" s="2" t="inlineStr">
         <is>
-          <t>maa://45558 (87.5)</t>
+          <t>maa://45558 (88.89)</t>
         </is>
       </c>
       <c r="U33" s="1" t="n"/>
@@ -4937,7 +4937,7 @@
       </c>
       <c r="AF34" s="2" t="inlineStr">
         <is>
-          <t>*maa://32650 (72.22)</t>
+          <t>*maa://32650 (73.68)</t>
         </is>
       </c>
       <c r="AG34" s="1" t="n"/>
@@ -4987,7 +4987,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.34)</t>
+          <t>maa://41296 (96.43)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5085,7 +5085,7 @@
       </c>
       <c r="H36" s="2" t="inlineStr">
         <is>
-          <t>maa://24375 (92.68)</t>
+          <t>maa://24375 (90.48)</t>
         </is>
       </c>
       <c r="I36" s="1" t="n"/>
@@ -5199,7 +5199,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (98.01), *maa://47069 (73.33), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.16), *maa://47069 (73.33), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5215,7 +5215,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.5), *maa://21239 (66.67)</t>
+          <t>maa://21280 (89.55), *maa://21239 (69.23)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5332,7 +5332,7 @@
       </c>
       <c r="T38" s="2" t="inlineStr">
         <is>
-          <t>maa://30713 (96.88)</t>
+          <t>maa://30713 (96.97)</t>
         </is>
       </c>
       <c r="U38" s="1" t="n"/>
@@ -5364,7 +5364,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.45)</t>
+          <t>maa://36697 (86.7)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5385,7 +5385,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (89.11), maa://25199 (84.82), maa://30434 (91.67), ***maa://25036 (16.0), maa://45059 (83.33), *maa://44165 (66.67)</t>
+          <t>maa://36670 (89.11), maa://25199 (84.82), maa://30434 (91.86), ***maa://25036 (16.0), maa://45059 (85.0), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (82.18), maa://47079 (94.12), *maa://45790 (76.92)</t>
+          <t>maa://45788 (80.77), maa://47079 (91.3), *maa://45790 (71.43)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5502,7 +5502,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.57), maa://21386 (95.77), maa://36664 (89.29), maa://45550 (100.0)</t>
+          <t>maa://23278 (95.28), maa://21386 (95.77), maa://36664 (89.29), maa://45550 (100.0)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5555,7 +5555,7 @@
       </c>
       <c r="H41" s="2" t="inlineStr">
         <is>
-          <t>maa://24466 (93.48)</t>
+          <t>maa://24466 (93.75)</t>
         </is>
       </c>
       <c r="I41" s="1" t="n"/>
@@ -5794,7 +5794,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (98.05), maa://27728 (96.12)</t>
+          <t>maa://29768 (98.07), maa://27728 (96.12)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5863,7 +5863,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.82), maa://30807 (95.65), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (86.36)</t>
+          <t>maa://21229 (84.82), maa://30807 (95.65), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (86.96)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5895,7 +5895,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (36.36)</t>
+          <t>**maa://39364 (37.14)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -5916,7 +5916,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (91.95), maa://43901 (93.1)</t>
+          <t>maa://35931 (92.0), maa://43901 (93.33)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5969,7 +5969,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.48), maa://29661 (97.32), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.49), maa://29661 (97.32), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.12), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.17), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6330,7 +6330,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (91.96)</t>
+          <t>maa://32532 (92.01)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6402,7 +6402,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://31270 (94.66), maa://27746 (82.3)</t>
+          <t>maa://31270 (94.66), maa://27746 (82.46)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6456,7 +6456,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (95.12), maa://43903 (100.0)</t>
+          <t>maa://42981 (95.24), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>
@@ -6492,7 +6492,7 @@
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>maa://44405 (85.19)</t>
+          <t>maa://44405 (85.71)</t>
         </is>
       </c>
       <c r="I64" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#169)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.58), maa://25390 (96.2), maa://36681 (87.34)</t>
+          <t>maa://24702 (94.59), maa://25390 (96.2), maa://36681 (87.34)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (90.59), *maa://20791 (61.33)</t>
+          <t>maa://22742 (90.59), *maa://20791 (61.84)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.41), maa://36684 (95.8), ***maa://22731 (6.25)</t>
+          <t>maa://21246 (91.44), maa://36684 (95.8), ***maa://22731 (6.25)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.83), **maa://20790 (43.48), ***maa://37170 (16.42), maa://45854 (80.77)</t>
+          <t>maa://24617 (89.83), **maa://20790 (43.48), ***maa://37170 (16.42), maa://45854 (81.48)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (94.81)</t>
+          <t>maa://24390 (94.87)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.03.15 13:17:29</t>
+          <t>更新日期：2025.03.16 13:17:23</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1687,7 +1687,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (87.9), *maa://22865 (51.85)</t>
+          <t>maa://26206 (88.0), *maa://22865 (51.85)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.76), maa://45828 (92.86), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.77), maa://45828 (92.86), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.59), maa://22501 (97.8), maa://45521 (85.71)</t>
+          <t>maa://22747 (92.59), maa://22501 (97.83), maa://45521 (85.71)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -2111,7 +2111,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.44), **maa://22728 (46.67)</t>
+          <t>*maa://21248 (73.55), **maa://22728 (46.67)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.18), maa://21478 (89.19)</t>
+          <t>maa://24304 (88.24), maa://21478 (89.19)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.01), *maa://36666 (77.39), *maa://22766 (68.64)</t>
+          <t>maa://21364 (81.07), *maa://36666 (77.39), *maa://22766 (68.64)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2857,7 +2857,7 @@
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (59.28), **maa://29784 (46.43), maa://47854 (100.0)</t>
+          <t>*maa://24313 (59.28), **maa://29784 (48.28), maa://47854 (100.0)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (81.32), ***maa://23820 (30.0)</t>
+          <t>maa://21443 (81.36), ***maa://23820 (30.0)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.88), maa://39875 (94.52)</t>
+          <t>maa://39756 (95.89), maa://39875 (94.52)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3605,7 +3605,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (84.11), maa://23504 (93.32), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (77.22), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (84.11), maa://23504 (93.32), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (77.5), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3671,7 +3671,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (73.05), *maa://25311 (74.53), ***maa://22725 (4.84), *maa://45047 (62.5)</t>
+          <t>*maa://29063 (73.05), *maa://25311 (74.77), ***maa://22725 (4.76), *maa://45047 (62.5)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3767,7 +3767,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.35), maa://24621 (96.92), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
+          <t>maa://20108 (96.38), maa://24621 (96.92), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.77), maa://41749 (91.3), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.77), maa://41749 (91.4), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4581,7 +4581,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.06), maa://36667 (97.67), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.06), maa://36667 (97.7), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -5364,7 +5364,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.7)</t>
+          <t>maa://36697 (86.76)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.17), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.19), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6402,7 +6402,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://31270 (94.66), maa://27746 (82.46)</t>
+          <t>maa://31270 (94.7), maa://27746 (82.46)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#170)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.59), maa://25390 (96.2), maa://36681 (87.34)</t>
+          <t>maa://24702 (94.59), maa://25390 (96.21), maa://36681 (87.34)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.17), *maa://30515 (70.19), maa://39402 (92.31), *maa://34787 (72.73), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.17), *maa://30515 (70.48), maa://39402 (92.42), *maa://34787 (72.73), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.6), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.61), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.0), maa://20276 (86.59), *maa://22749 (75.0)</t>
+          <t>*maa://22880 (65.0), maa://20276 (86.59), *maa://22749 (76.92)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -832,12 +832,12 @@
       </c>
       <c r="O3" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.58), maa://26254 (96.67)</t>
+          <t>maa://21249 (94.58), maa://26254 (96.67), **maa://22738 (50.0)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.83), **maa://20790 (43.48), ***maa://37170 (16.42), maa://45854 (81.48)</t>
+          <t>maa://24617 (89.83), **maa://20790 (43.48), ***maa://37170 (16.42), maa://45854 (82.14)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (91.55), ***maa://36683 (28.26)</t>
+          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (91.78), ***maa://36683 (28.26)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (64.0), ***maa://26209 (13.04), *maa://39394 (64.0)</t>
+          <t>*maa://30062 (64.0), ***maa://26209 (13.04), *maa://39394 (65.38)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.3), maa://22744 (84.0)</t>
+          <t>maa://21245 (84.36), maa://22744 (84.62)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.57), *maa://22758 (74.29)</t>
+          <t>maa://22399 (95.57), *maa://22758 (75.0)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.03.16 13:17:23</t>
+          <t>更新日期：2025.03.19 13:19:27</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1607,7 +1607,7 @@
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>maa://22762 (92.39), *maa://39552 (80.0)</t>
+          <t>maa://22762 (92.39), maa://39552 (81.25)</t>
         </is>
       </c>
       <c r="M9" s="1" t="n"/>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.1), ***maa://22740 (5.66), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (96.3), *maa://45044 (66.67)</t>
+          <t>maa://28711 (87.1), ***maa://22740 (5.66), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), *maa://45044 (66.67), maa://40166 (96.3)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (88.0), *maa://22865 (51.85)</t>
+          <t>maa://26206 (88.1), *maa://22865 (51.85)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.52), ***maa://39951 (13.79), ***maa://34206 (19.23), ***maa://39243 (25.0), *maa://45271 (58.97)</t>
+          <t>***maa://25695 (18.52), ***maa://39951 (13.79), ***maa://34206 (19.23), ***maa://39243 (25.0), *maa://45271 (57.5)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.77), maa://45828 (92.86), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.77), maa://45828 (86.67), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1931,7 +1931,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://29912 (97.3), maa://22516 (88.37), *maa://20794 (52.24)</t>
+          <t>maa://29912 (97.33), maa://22516 (88.37), *maa://20794 (52.24)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (90.0), ***maa://45826 (28.57)</t>
+          <t>maa://21867 (90.0), ***maa://45826 (25.0)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.5), maa://36677 (93.85), maa://39872 (92.0)</t>
+          <t>maa://23669 (95.5), maa://36677 (93.94), maa://39872 (92.0)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.21), maa://36673 (92.21), maa://25001 (85.71)</t>
+          <t>maa://24999 (92.09), maa://36673 (92.21), maa://25001 (85.71)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2207,7 +2207,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (34.25), maa://39883 (91.67), *maa://39885 (53.33)</t>
+          <t>**maa://22737 (34.25), maa://39883 (91.78), *maa://39885 (53.33)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (88.24), maa://21478 (89.19)</t>
+          <t>maa://24304 (87.84), maa://21478 (89.19)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.51), *maa://28648 (69.57), maa://36674 (82.69)</t>
+          <t>maa://22729 (94.55), *maa://28648 (69.57), maa://36674 (81.13)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2581,7 +2581,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (96.04)</t>
+          <t>maa://26228 (95.1)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2663,7 +2663,7 @@
       </c>
       <c r="P17" s="2" t="inlineStr">
         <is>
-          <t>maa://23890 (80.77), *maa://24940 (67.86)</t>
+          <t>maa://23890 (80.95), *maa://24940 (67.86)</t>
         </is>
       </c>
       <c r="Q17" s="1" t="n"/>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="X18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (96.94), maa://22741 (85.71)</t>
+          <t>maa://21917 (96.94), maa://22741 (87.5)</t>
         </is>
       </c>
       <c r="Y18" s="1" t="n"/>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.19)</t>
+          <t>maa://41331 (84.85)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3215,7 +3215,7 @@
       </c>
       <c r="X21" s="2" t="inlineStr">
         <is>
-          <t>maa://20110 (86.76), maa://34946 (90.91)</t>
+          <t>maa://20110 (86.76), maa://34946 (91.11)</t>
         </is>
       </c>
       <c r="Y21" s="1" t="n"/>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.22), *maa://22432 (77.92)</t>
+          <t>maa://22524 (94.22), *maa://22432 (76.92)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3395,7 +3395,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.77), *maa://41753 (55.0)</t>
+          <t>***maa://28036 (28.77), *maa://41753 (52.38)</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.89), maa://39875 (94.52)</t>
+          <t>maa://39756 (95.9), maa://39875 (94.52)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3459,7 +3459,7 @@
       </c>
       <c r="T23" s="2" t="inlineStr">
         <is>
-          <t>maa://24387 (82.05), maa://31212 (93.55)</t>
+          <t>maa://24387 (82.05), maa://31212 (93.75)</t>
         </is>
       </c>
       <c r="U23" s="1" t="n"/>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.39), *maa://46650 (57.14)</t>
+          <t>*maa://24368 (78.44), *maa://46650 (57.14)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3605,7 +3605,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (84.11), maa://23504 (93.32), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (77.5), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (84.11), maa://23504 (93.33), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (77.5), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3655,7 +3655,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.2)</t>
+          <t>maa://29753 (95.22)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (94.5)</t>
+          <t>maa://42235 (94.59)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3947,7 +3947,7 @@
       </c>
       <c r="L27" s="2" t="inlineStr">
         <is>
-          <t>maa://28071 (90.0)</t>
+          <t>maa://28071 (90.48)</t>
         </is>
       </c>
       <c r="M27" s="1" t="n"/>
@@ -4109,7 +4109,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>*maa://29765 (63.95), maa://23263 (95.28)</t>
+          <t>*maa://29765 (64.37), maa://23263 (95.28)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.77), maa://41749 (91.4), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.82), maa://41749 (91.4), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4287,7 +4287,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.85), maa://42865 (81.54), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.85), maa://42865 (81.82), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4337,7 +4337,7 @@
       </c>
       <c r="L30" s="2" t="inlineStr">
         <is>
-          <t>maa://30442 (95.31)</t>
+          <t>maa://30442 (95.38)</t>
         </is>
       </c>
       <c r="M30" s="1" t="n"/>
@@ -4401,7 +4401,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.11), maa://45822 (100.0), *maa://45045 (80.0)</t>
+          <t>maa://42979 (97.13), maa://45822 (100.0), *maa://45045 (80.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4629,7 +4629,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.09), maa://41108 (88.0), maa://41238 (97.2), maa://45523 (100.0)</t>
+          <t>maa://42859 (96.12), maa://41108 (88.0), maa://41238 (97.2), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4743,7 +4743,7 @@
       </c>
       <c r="P33" s="2" t="inlineStr">
         <is>
-          <t>maa://21956 (80.79), *maa://22730 (79.31)</t>
+          <t>maa://21956 (80.79), *maa://22730 (76.67)</t>
         </is>
       </c>
       <c r="Q33" s="1" t="n"/>
@@ -4868,12 +4868,12 @@
       </c>
       <c r="O34" s="1" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P34" s="2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>maa://48817 (100.0)</t>
         </is>
       </c>
       <c r="Q34" s="1" t="n"/>
@@ -5199,7 +5199,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (98.16), *maa://47069 (73.33), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.17), *maa://47069 (73.33), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5385,7 +5385,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (89.11), maa://25199 (84.82), maa://30434 (91.86), ***maa://25036 (16.0), maa://45059 (85.0), *maa://44165 (66.67)</t>
+          <t>maa://36670 (89.22), maa://25199 (84.82), maa://30434 (91.86), maa://45059 (85.0), ***maa://25036 (16.0), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (80.77), maa://47079 (91.3), *maa://45790 (71.43)</t>
+          <t>maa://45788 (80.77), maa://47079 (92.0), *maa://45790 (73.33)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5587,7 +5587,7 @@
       </c>
       <c r="P41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (40.0), maa://43177 (91.3)</t>
+          <t>**maa://35616 (40.0), maa://43177 (91.67)</t>
         </is>
       </c>
       <c r="Q41" s="1" t="n"/>
@@ -5725,7 +5725,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (92.41), maa://21284 (85.71)</t>
+          <t>maa://22525 (92.47), maa://21284 (85.71)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5895,7 +5895,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (37.14)</t>
+          <t>**maa://39364 (38.89)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -6091,7 +6091,7 @@
       </c>
       <c r="P49" s="2" t="inlineStr">
         <is>
-          <t>*maa://39643 (64.52)</t>
+          <t>*maa://39643 (63.64)</t>
         </is>
       </c>
       <c r="Q49" s="1" t="n"/>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.19), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.2), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6456,7 +6456,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (95.24), maa://43903 (100.0)</t>
+          <t>maa://42981 (95.35), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#171)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (96.61)</t>
+          <t>maa://42407 (96.67)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>maa://21955 (95.0)</t>
+          <t>maa://21955 (95.12)</t>
         </is>
       </c>
       <c r="E7" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (92.79), maa://24957 (97.73)</t>
+          <t>maa://28624 (92.92), maa://24957 (97.73)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.03.19 13:19:27</t>
+          <t>更新日期：2025.03.20 13:18:45</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1561,7 +1561,7 @@
       </c>
       <c r="AF8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24479 (78.41), *maa://21990 (51.85)</t>
+          <t>*maa://24479 (78.65), *maa://21990 (51.85)</t>
         </is>
       </c>
       <c r="AG8" s="1" t="n"/>
@@ -2403,7 +2403,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (90.42), *maa://22727 (70.0)</t>
+          <t>maa://24762 (90.48), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2615,7 +2615,7 @@
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>maa://21624 (84.62)</t>
+          <t>maa://21624 (85.0)</t>
         </is>
       </c>
       <c r="E17" s="1" t="n"/>
@@ -2857,7 +2857,7 @@
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (59.28), **maa://29784 (48.28), maa://47854 (100.0)</t>
+          <t>*maa://24313 (59.52), **maa://29784 (48.28), maa://47854 (100.0)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -2971,7 +2971,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (66.14), *maa://36668 (57.5)</t>
+          <t>*maa://30709 (66.22), *maa://36668 (57.5)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (81.36), ***maa://23820 (30.0)</t>
+          <t>maa://21443 (81.41), ***maa://23820 (30.0)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3395,7 +3395,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.77), *maa://41753 (52.38)</t>
+          <t>***maa://28036 (28.38), *maa://41753 (52.38)</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.9), maa://39875 (94.52)</t>
+          <t>maa://39756 (95.91), maa://39875 (94.59)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.44), *maa://46650 (57.14)</t>
+          <t>*maa://24368 (78.44), *maa://46650 (62.5)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3605,7 +3605,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (84.11), maa://23504 (93.33), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (77.5), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (84.17), maa://23504 (93.33), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (77.5), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -4157,7 +4157,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.52), *maa://36701 (66.67)</t>
+          <t>maa://36660 (92.54), *maa://36701 (66.67)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4287,7 +4287,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.85), maa://42865 (81.82), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.85), maa://42865 (82.09), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4467,7 +4467,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.33), maa://36258 (84.87), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.36), maa://36258 (84.87), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4597,7 +4597,7 @@
       </c>
       <c r="L32" s="2" t="inlineStr">
         <is>
-          <t>maa://28065 (95.45)</t>
+          <t>maa://28065 (95.56)</t>
         </is>
       </c>
       <c r="M32" s="1" t="n"/>
@@ -4987,7 +4987,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.43)</t>
+          <t>maa://41296 (96.45)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5199,7 +5199,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (98.17), *maa://47069 (73.33), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.18), *maa://47069 (73.33), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5385,7 +5385,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (89.22), maa://25199 (84.82), maa://30434 (91.86), maa://45059 (85.0), ***maa://25036 (16.0), *maa://44165 (66.67)</t>
+          <t>maa://36670 (89.22), maa://25199 (84.82), maa://30434 (91.86), maa://45059 (80.95), ***maa://25036 (19.23), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (80.77), maa://47079 (92.0), *maa://45790 (73.33)</t>
+          <t>maa://45788 (80.77), maa://47079 (92.31), *maa://45790 (73.33)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -6091,7 +6091,7 @@
       </c>
       <c r="P49" s="2" t="inlineStr">
         <is>
-          <t>*maa://39643 (63.64)</t>
+          <t>*maa://39643 (64.71)</t>
         </is>
       </c>
       <c r="Q49" s="1" t="n"/>
@@ -6330,7 +6330,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.01)</t>
+          <t>maa://32532 (92.04)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6402,7 +6402,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://31270 (94.7), maa://27746 (82.46)</t>
+          <t>maa://31270 (94.74), maa://27746 (82.46)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#172)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (91.67), ***maa://21730 (26.32), ***maa://39501 (15.62), **maa://36675 (50.0)</t>
+          <t>maa://25251 (91.74), ***maa://21730 (26.32), ***maa://39501 (15.15), **maa://36675 (50.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://40192 (96.49), maa://36987 (96.15), maa://39849 (88.89)</t>
+          <t>maa://40192 (96.55), maa://36987 (96.15), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.61), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.62), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.0), maa://20276 (86.59), *maa://22749 (76.92)</t>
+          <t>*maa://22880 (64.68), maa://20276 (86.59), *maa://22749 (76.92)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.83), **maa://20790 (43.48), ***maa://37170 (16.42), maa://45854 (82.14)</t>
+          <t>maa://24617 (89.83), **maa://20790 (43.48), ***maa://37170 (16.18), maa://45854 (83.33)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.6), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.68), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -1015,7 +1015,7 @@
       </c>
       <c r="AB4" s="2" t="inlineStr">
         <is>
-          <t>*maa://32658 (70.0)</t>
+          <t>*maa://32658 (71.43)</t>
         </is>
       </c>
       <c r="AC4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.36), maa://22744 (84.62)</t>
+          <t>maa://21245 (84.43), maa://22744 (84.62)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>*maa://22757 (76.32)</t>
+          <t>*maa://22757 (76.92)</t>
         </is>
       </c>
       <c r="M5" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (92.92), maa://24957 (97.73)</t>
+          <t>maa://28624 (92.92), maa://24957 (97.78)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.03.20 13:18:45</t>
+          <t>更新日期：2025.03.23 13:17:41</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1655,7 +1655,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (97.99)</t>
+          <t>maa://26223 (98.0)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.1), ***maa://22740 (5.66), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), *maa://45044 (66.67), maa://40166 (96.3)</t>
+          <t>maa://28711 (87.2), ***maa://22740 (5.66), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), *maa://45044 (66.67), maa://40166 (96.3)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.52), ***maa://39951 (13.79), ***maa://34206 (19.23), ***maa://39243 (25.0), *maa://45271 (57.5)</t>
+          <t>***maa://25695 (18.52), ***maa://39951 (13.79), ***maa://34206 (19.23), ***maa://39243 (25.0), *maa://45271 (54.76)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1769,7 +1769,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.55), maa://22755 (87.83), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.57), maa://22755 (87.83), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1931,7 +1931,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://29912 (97.33), maa://22516 (88.37), *maa://20794 (52.24)</t>
+          <t>maa://29912 (97.37), maa://22516 (88.37), *maa://20794 (52.24)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.5), maa://36677 (93.94), maa://39872 (92.0)</t>
+          <t>maa://23669 (95.5), maa://36677 (94.03), maa://39872 (92.0)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.09), maa://36673 (92.21), maa://25001 (85.71)</t>
+          <t>maa://24999 (92.09), maa://36673 (92.31), maa://25001 (85.92)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2111,7 +2111,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.55), **maa://22728 (46.67)</t>
+          <t>*maa://21248 (73.88), **maa://22728 (46.67)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2138,12 +2138,12 @@
       </c>
       <c r="O13" s="1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (93.02), *maa://22583 (75.0), *maa://22500 (58.7)</t>
+          <t>maa://22676 (93.02), *maa://22583 (75.36), *maa://22500 (58.7), maa://48321 (100.0)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2207,7 +2207,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (34.25), maa://39883 (91.78), *maa://39885 (53.33)</t>
+          <t>**maa://22737 (34.25), maa://39883 (91.89), *maa://39885 (53.33)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2257,7 +2257,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.77), maa://21288 (96.3), maa://39841 (94.69), maa://36682 (97.44)</t>
+          <t>maa://26245 (96.77), maa://21288 (96.3), maa://39841 (93.91), maa://36682 (97.44)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="AB14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (97.26)</t>
+          <t>maa://22764 (97.3)</t>
         </is>
       </c>
       <c r="AC14" s="1" t="n"/>
@@ -2355,7 +2355,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.24), maa://22734 (84.17), *maa://30808 (64.18), **maa://36048 (50.0), maa://45058 (93.33)</t>
+          <t>*maa://22743 (78.24), maa://22734 (84.17), *maa://30808 (64.18), *maa://36048 (50.75), maa://45058 (93.33)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (87.84), maa://21478 (89.19)</t>
+          <t>maa://24304 (87.95), maa://21478 (89.19)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.07), *maa://36666 (77.39), *maa://22766 (68.64)</t>
+          <t>maa://21364 (81.12), *maa://36666 (77.59), *maa://22766 (68.07)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2565,7 +2565,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (98.08), maa://28051 (96.0)</t>
+          <t>maa://28501 (98.1), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2581,7 +2581,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.1)</t>
+          <t>maa://26228 (95.15)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2631,7 +2631,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.83), maa://39599 (86.54)</t>
+          <t>maa://22430 (88.83), maa://39599 (84.91)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>*maa://42324 (53.12)</t>
+          <t>*maa://42324 (51.52)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (89.02)</t>
+          <t>maa://24421 (88.67)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2777,7 +2777,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (90.64), *maa://22732 (51.06)</t>
+          <t>maa://22466 (90.64), *maa://22732 (51.58)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2857,7 +2857,7 @@
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (59.52), **maa://29784 (48.28), maa://47854 (100.0)</t>
+          <t>*maa://24313 (59.52), **maa://29784 (50.0), maa://47854 (100.0)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -2971,7 +2971,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (66.22), *maa://36668 (57.5)</t>
+          <t>*maa://30709 (66.29), *maa://36668 (57.5)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (84.85)</t>
+          <t>maa://41331 (84.94)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (94.22), *maa://22432 (76.92)</t>
+          <t>maa://22524 (93.39), *maa://22432 (76.92)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3475,7 +3475,7 @@
       </c>
       <c r="X23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (68.29)</t>
+          <t>*maa://28503 (68.67)</t>
         </is>
       </c>
       <c r="Y23" s="1" t="n"/>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.44), *maa://46650 (62.5)</t>
+          <t>*maa://24368 (78.5), *maa://46650 (62.5)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3605,7 +3605,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (84.17), maa://23504 (93.33), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (77.5), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (83.91), maa://23504 (93.33), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (77.5), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3655,7 +3655,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.22)</t>
+          <t>maa://29753 (95.24)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3671,7 +3671,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (73.05), *maa://25311 (74.77), ***maa://22725 (4.76), *maa://45047 (62.5)</t>
+          <t>*maa://29063 (72.62), *maa://25311 (74.77), ***maa://22725 (4.76), *maa://45047 (62.5)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (94.59)</t>
+          <t>maa://42235 (94.64)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4157,7 +4157,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.54), *maa://36701 (66.67)</t>
+          <t>maa://36660 (92.56), *maa://36701 (66.67)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4191,7 +4191,7 @@
       </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>*maa://25175 (65.38)</t>
+          <t>*maa://25175 (66.04)</t>
         </is>
       </c>
       <c r="I29" s="1" t="n"/>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.57), maa://28440 (80.53), maa://31400 (98.82), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.59), maa://28440 (80.53), maa://31400 (98.82), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4305,7 +4305,7 @@
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>maa://45792 (93.33)</t>
+          <t>maa://45792 (93.75)</t>
         </is>
       </c>
       <c r="E30" s="1" t="n"/>
@@ -4467,7 +4467,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.36), maa://36258 (84.87), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.38), maa://36258 (84.87), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4581,7 +4581,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.06), maa://36667 (97.7), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.06), maa://36667 (97.73), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="AF32" s="2" t="inlineStr">
         <is>
-          <t>maa://42408 (83.33)</t>
+          <t>maa://42408 (84.62)</t>
         </is>
       </c>
       <c r="AG32" s="1" t="n"/>
@@ -4889,7 +4889,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (92.75)</t>
+          <t>maa://24526 (92.78)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4937,7 +4937,7 @@
       </c>
       <c r="AF34" s="2" t="inlineStr">
         <is>
-          <t>*maa://32650 (73.68)</t>
+          <t>*maa://32650 (75.0)</t>
         </is>
       </c>
       <c r="AG34" s="1" t="n"/>
@@ -5385,7 +5385,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (89.22), maa://25199 (84.82), maa://30434 (91.86), maa://45059 (80.95), ***maa://25036 (19.23), *maa://44165 (66.67)</t>
+          <t>maa://36670 (89.22), maa://25199 (84.82), maa://30434 (91.95), maa://45059 (81.82), ***maa://25036 (19.23), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5417,7 +5417,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.61), maa://47093 (100.0)</t>
+          <t>maa://24709 (91.72), maa://47093 (100.0)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (80.77), maa://47079 (92.31), *maa://45790 (73.33)</t>
+          <t>maa://45788 (80.77), maa://47079 (92.59), *maa://45790 (73.33)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5502,7 +5502,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.28), maa://21386 (95.77), maa://36664 (89.29), maa://45550 (100.0)</t>
+          <t>maa://23278 (95.3), maa://21386 (95.77), maa://36664 (89.29), maa://45550 (100.0)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5895,7 +5895,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (38.89)</t>
+          <t>**maa://39364 (39.47)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -5969,7 +5969,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.49), maa://29661 (97.32), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.5), maa://29661 (97.33), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6330,7 +6330,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.04)</t>
+          <t>maa://32532 (92.09)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6366,7 +6366,7 @@
       </c>
       <c r="H57" s="2" t="inlineStr">
         <is>
-          <t>maa://25176 (98.39)</t>
+          <t>maa://25176 (98.41)</t>
         </is>
       </c>
       <c r="I57" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#173)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.59), maa://25390 (96.21), maa://36681 (87.34)</t>
+          <t>maa://24702 (94.59), maa://25390 (96.25), maa://36681 (87.34)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.17), *maa://30515 (70.48), maa://39402 (92.42), *maa://34787 (72.73), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.17), *maa://30515 (70.48), maa://39402 (92.75), *maa://34787 (72.73), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (90.59), *maa://20791 (61.84)</t>
+          <t>maa://22742 (90.7), *maa://20791 (62.34)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.44), maa://36684 (95.8), ***maa://22731 (6.25)</t>
+          <t>maa://21246 (91.44), maa://36684 (95.83), ***maa://22731 (6.25)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (91.74), ***maa://21730 (26.32), ***maa://39501 (15.15), **maa://36675 (50.0)</t>
+          <t>maa://25251 (91.74), ***maa://21730 (27.27), ***maa://39501 (15.15), **maa://36675 (50.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://40192 (96.55), maa://36987 (96.15), maa://39849 (88.89)</t>
+          <t>maa://40192 (96.67), maa://36987 (96.15), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (64.68), maa://20276 (86.59), *maa://22749 (76.92)</t>
+          <t>*maa://22880 (64.85), maa://20276 (86.67), *maa://22749 (76.92)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.58), maa://26254 (96.67), **maa://22738 (50.0)</t>
+          <t>maa://21249 (94.65), maa://26254 (96.67), **maa://22738 (50.0)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.83), **maa://20790 (43.48), ***maa://37170 (16.18), maa://45854 (83.33)</t>
+          <t>maa://24617 (89.83), **maa://20790 (43.48), ***maa://37170 (16.18), maa://45854 (84.85)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.36), maa://27484 (96.61), maa://27480 (83.33)</t>
+          <t>maa://27396 (84.36), maa://27484 (96.67), maa://27480 (83.33)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.68), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.71), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (95.76), maa://27295 (86.3), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
+          <t>maa://32509 (95.8), maa://27295 (86.49), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.7), ***maa://31785 (22.22), maa://43217 (91.78), ***maa://36683 (28.26)</t>
+          <t>**maa://32495 (48.89), ***maa://31785 (22.22), maa://43217 (92.0), ***maa://36683 (28.26)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.43), maa://22744 (84.62)</t>
+          <t>maa://21245 (84.49), maa://22744 (84.62)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (96.67)</t>
+          <t>maa://42407 (96.72)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="T6" s="2" t="inlineStr">
         <is>
-          <t>maa://37411 (87.5)</t>
+          <t>maa://37411 (88.24)</t>
         </is>
       </c>
       <c r="U6" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.57), *maa://22758 (75.0)</t>
+          <t>maa://22399 (95.62), *maa://22758 (75.0)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.03.23 13:17:41</t>
+          <t>更新日期：2025.03.28 13:20:26</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>*maa://21476 (73.08), *maa://39431 (57.14), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (73.58), *maa://39431 (60.0), *maa://37551 (57.14)</t>
         </is>
       </c>
       <c r="E8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.98)</t>
+          <t>maa://21411 (96.0)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1639,7 +1639,7 @@
       </c>
       <c r="T9" s="2" t="inlineStr">
         <is>
-          <t>**maa://22866 (30.19), maa://26222 (98.11)</t>
+          <t>**maa://22866 (30.19), maa://26222 (98.15)</t>
         </is>
       </c>
       <c r="U9" s="1" t="n"/>
@@ -1666,12 +1666,12 @@
       </c>
       <c r="AA9" s="1" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.2), ***maa://22740 (5.66), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), *maa://45044 (66.67), maa://40166 (96.3)</t>
+          <t>maa://28711 (87.2), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), *maa://45044 (66.67), maa://40166 (96.3)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (88.1), *maa://22865 (51.85)</t>
+          <t>maa://26206 (88.19), *maa://22865 (51.85)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.52), ***maa://39951 (13.79), ***maa://34206 (19.23), ***maa://39243 (25.0), *maa://45271 (54.76)</t>
+          <t>***maa://25695 (18.32), ***maa://39951 (13.56), ***maa://34206 (22.22), ***maa://39243 (25.0), *maa://45271 (53.49)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.77), maa://45828 (86.67), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.78), maa://45828 (87.5), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (54.55), *maa://22733 (62.16), **maa://22761 (50.0)</t>
+          <t>*maa://25021 (54.0), *maa://22733 (62.16), **maa://22761 (50.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.8)</t>
+          <t>maa://36713 (97.81)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (90.0), ***maa://45826 (25.0)</t>
+          <t>maa://21867 (90.06), ***maa://45826 (25.0)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.5), maa://36677 (94.03), maa://39872 (92.0)</t>
+          <t>maa://23669 (95.52), maa://36677 (94.12), maa://39872 (92.0)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.0), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (78.15), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.09), maa://36673 (92.31), maa://25001 (85.92)</t>
+          <t>maa://24999 (92.14), maa://36673 (92.41), maa://25001 (85.92)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2111,7 +2111,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.88), **maa://22728 (46.67)</t>
+          <t>*maa://21248 (74.09), **maa://22728 (46.67)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2175,7 +2175,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>maa://34957 (82.5), **maa://22768 (50.0)</t>
+          <t>maa://34957 (81.71), **maa://22768 (50.0)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2207,7 +2207,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (34.25), maa://39883 (91.89), *maa://39885 (53.33)</t>
+          <t>**maa://22737 (34.25), maa://39883 (90.79), *maa://39885 (53.33)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2257,7 +2257,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.77), maa://21288 (96.3), maa://39841 (93.91), maa://36682 (97.44)</t>
+          <t>maa://26245 (96.77), maa://21288 (96.3), maa://39841 (94.02), maa://36682 (97.44)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2273,7 +2273,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.75), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.76), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2289,7 +2289,7 @@
       </c>
       <c r="T14" s="2" t="inlineStr">
         <is>
-          <t>maa://22521 (94.34), maa://42751 (100.0)</t>
+          <t>maa://22521 (94.44), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="1" t="n"/>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (87.95), maa://21478 (89.19)</t>
+          <t>maa://24304 (87.95), maa://21478 (89.47)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2403,7 +2403,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (90.48), *maa://22727 (70.0)</t>
+          <t>maa://24762 (90.53), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="T15" s="2" t="inlineStr">
         <is>
-          <t>maa://23892 (96.25)</t>
+          <t>maa://23892 (96.3)</t>
         </is>
       </c>
       <c r="U15" s="1" t="n"/>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.12), *maa://36666 (77.59), *maa://22766 (68.07)</t>
+          <t>maa://21364 (81.18), *maa://36666 (77.59), *maa://22766 (68.33)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2485,7 +2485,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.41), maa://36679 (94.55), maa://37650 (97.5)</t>
+          <t>maa://21441 (96.43), maa://36679 (94.55), maa://37650 (97.67)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.55), *maa://28648 (69.57), maa://36674 (81.13)</t>
+          <t>maa://22729 (94.55), *maa://28648 (69.57), *maa://36674 (79.63)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2631,7 +2631,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.83), maa://39599 (84.91)</t>
+          <t>maa://22430 (88.83), maa://39599 (83.64)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2745,7 +2745,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.94)</t>
+          <t>maa://24570 (96.98)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2777,7 +2777,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (90.64), *maa://22732 (51.58)</t>
+          <t>maa://22466 (90.75), *maa://22732 (51.04)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="X18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (96.94), maa://22741 (87.5)</t>
+          <t>maa://21917 (96.97), maa://22741 (87.5)</t>
         </is>
       </c>
       <c r="Y18" s="1" t="n"/>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (99.17)</t>
+          <t>maa://24386 (99.18)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.45), maa://25198 (93.69), *maa://20795 (50.77), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.56), maa://25198 (93.69), *maa://20795 (50.77), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (89.94)</t>
+          <t>maa://22864 (90.0)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="P20" s="2" t="inlineStr">
         <is>
-          <t>maa://37442 (95.24)</t>
+          <t>maa://37442 (95.35)</t>
         </is>
       </c>
       <c r="Q20" s="1" t="n"/>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (93.39), *maa://22432 (76.92)</t>
+          <t>maa://22524 (93.39), *maa://22432 (78.31)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3329,7 +3329,7 @@
       </c>
       <c r="T22" s="2" t="inlineStr">
         <is>
-          <t>maa://38495 (86.67)</t>
+          <t>maa://38495 (87.5)</t>
         </is>
       </c>
       <c r="U22" s="1" t="n"/>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.62), *maa://37649 (65.52)</t>
+          <t>maa://21282 (98.63), *maa://37649 (65.52)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3443,7 +3443,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (92.0), *maa://29748 (75.97), ***maa://29785 (16.18), *maa://37566 (77.5)</t>
+          <t>maa://30587 (92.0), *maa://29748 (76.15), ***maa://29785 (16.18), *maa://37566 (77.5)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.5), *maa://46650 (62.5)</t>
+          <t>*maa://24368 (78.61), *maa://46650 (62.5)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3605,7 +3605,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (83.91), maa://23504 (93.33), **maa://22892 (40.14), *maa://25141 (77.1), *maa://36663 (77.5), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (83.97), maa://23504 (93.33), **maa://22892 (40.54), *maa://25141 (77.1), *maa://36663 (77.5), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3637,7 +3637,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (85.64), maa://36672 (80.7), maa://29910 (93.22), **maa://21440 (35.71), maa://45831 (83.33)</t>
+          <t>maa://22523 (85.22), *maa://36672 (79.31), maa://29910 (93.22), **maa://21440 (35.71), maa://45831 (85.71)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3671,7 +3671,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (72.62), *maa://25311 (74.77), ***maa://22725 (4.76), *maa://45047 (62.5)</t>
+          <t>*maa://29063 (72.62), *maa://25311 (74.77), ***maa://22725 (4.76), *maa://45047 (66.67)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3751,7 +3751,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (88.14), maa://24516 (80.22), maa://26001 (87.5)</t>
+          <t>maa://31215 (88.33), maa://24516 (80.22), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3785,7 +3785,7 @@
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>maa://41802 (90.48)</t>
+          <t>maa://41802 (90.91)</t>
         </is>
       </c>
       <c r="E26" s="1" t="n"/>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (94.64)</t>
+          <t>maa://42235 (94.69)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.82), maa://41749 (91.4), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.89), maa://41749 (91.4), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4157,7 +4157,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.56), *maa://36701 (66.67)</t>
+          <t>maa://36660 (92.58), *maa://36701 (66.67)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4191,7 +4191,7 @@
       </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>*maa://25175 (66.04)</t>
+          <t>*maa://25175 (66.67)</t>
         </is>
       </c>
       <c r="I29" s="1" t="n"/>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.59), maa://28440 (80.53), maa://31400 (98.82), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.59), maa://28440 (80.87), maa://31400 (98.82), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4223,7 +4223,7 @@
       </c>
       <c r="P29" s="2" t="inlineStr">
         <is>
-          <t>*maa://23168 (58.06), *maa://30050 (54.29)</t>
+          <t>*maa://23168 (58.06), *maa://30050 (55.56)</t>
         </is>
       </c>
       <c r="Q29" s="1" t="n"/>
@@ -4287,7 +4287,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.85), maa://42865 (82.09), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.93), maa://42865 (81.16), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4305,7 +4305,7 @@
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>maa://45792 (93.75)</t>
+          <t>maa://45792 (94.12)</t>
         </is>
       </c>
       <c r="E30" s="1" t="n"/>
@@ -4581,7 +4581,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.06), maa://36667 (97.73), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.07), maa://36667 (97.73), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4629,7 +4629,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.12), maa://41108 (88.0), maa://41238 (97.2), maa://45523 (100.0)</t>
+          <t>maa://42859 (96.15), maa://41108 (88.0), maa://41238 (97.2), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4873,7 +4873,7 @@
       </c>
       <c r="P34" s="2" t="inlineStr">
         <is>
-          <t>maa://48817 (100.0)</t>
+          <t>maa://48817 (90.91)</t>
         </is>
       </c>
       <c r="Q34" s="1" t="n"/>
@@ -4987,7 +4987,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.45)</t>
+          <t>maa://41296 (96.47)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5199,7 +5199,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (98.18), *maa://47069 (73.33), maa://45789 (100.0)</t>
+          <t>maa://45718 (97.6), *maa://47069 (73.33), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5385,7 +5385,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (89.22), maa://25199 (84.82), maa://30434 (91.95), maa://45059 (81.82), ***maa://25036 (19.23), *maa://44165 (66.67)</t>
+          <t>maa://36670 (89.22), maa://25199 (84.82), maa://30434 (92.05), maa://45059 (81.82), ***maa://25036 (19.23), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5502,7 +5502,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.3), maa://21386 (95.77), maa://36664 (89.29), maa://45550 (100.0)</t>
+          <t>maa://23278 (95.31), maa://21386 (95.79), maa://36664 (89.29), maa://45550 (87.5)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5555,7 +5555,7 @@
       </c>
       <c r="H41" s="2" t="inlineStr">
         <is>
-          <t>maa://24466 (93.75)</t>
+          <t>maa://24466 (93.88)</t>
         </is>
       </c>
       <c r="I41" s="1" t="n"/>
@@ -5794,7 +5794,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (98.07), maa://27728 (96.12)</t>
+          <t>maa://29768 (98.08), maa://27728 (96.12)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5916,7 +5916,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.0), maa://43901 (93.33)</t>
+          <t>maa://35931 (91.98), maa://43901 (93.33)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -5969,7 +5969,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.5), maa://29661 (97.33), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.5), maa://29661 (97.35), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.2), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.22), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6330,7 +6330,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.09)</t>
+          <t>maa://32532 (92.11)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6366,7 +6366,7 @@
       </c>
       <c r="H57" s="2" t="inlineStr">
         <is>
-          <t>maa://25176 (98.41)</t>
+          <t>maa://25176 (98.44)</t>
         </is>
       </c>
       <c r="I57" s="1" t="n"/>
@@ -6384,7 +6384,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (59.52)</t>
+          <t>*maa://37964 (58.14)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>
@@ -6402,7 +6402,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://31270 (94.74), maa://27746 (82.46)</t>
+          <t>maa://31270 (94.78), maa://27746 (82.46)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#174)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.59), maa://25390 (96.25), maa://36681 (87.34)</t>
+          <t>maa://24702 (94.59), maa://25390 (96.27), maa://36681 (87.34)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://40192 (96.67), maa://36987 (96.15), maa://39849 (88.89)</t>
+          <t>maa://40192 (96.72), maa://36987 (96.15), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (64.85), maa://20276 (86.67), *maa://22749 (76.92)</t>
+          <t>*maa://22880 (64.85), maa://20276 (86.74), *maa://22749 (76.92)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.89), ***maa://31785 (22.22), maa://43217 (92.0), ***maa://36683 (28.26)</t>
+          <t>**maa://32495 (48.89), ***maa://31785 (22.22), maa://43217 (92.11), ***maa://36683 (28.26)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>maa://24370 (96.72)</t>
+          <t>maa://24370 (96.77)</t>
         </is>
       </c>
       <c r="I6" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.03.28 13:20:26</t>
+          <t>更新日期：2025.03.30 13:18:18</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1687,7 +1687,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (88.19), *maa://22865 (51.85)</t>
+          <t>maa://26206 (88.28), *maa://22865 (51.85)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.59), maa://22501 (97.83), maa://45521 (85.71)</t>
+          <t>maa://22747 (92.59), maa://22501 (97.83), maa://45521 (86.36)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -2045,7 +2045,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.06), *maa://21485 (75.35), maa://37962 (90.7)</t>
+          <t>maa://22753 (91.11), *maa://21485 (75.35), maa://37962 (90.7)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.52), maa://36677 (94.12), maa://39872 (92.0)</t>
+          <t>maa://23669 (95.53), maa://36677 (94.12), maa://39872 (92.0)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.14), maa://36673 (92.41), maa://25001 (85.92)</t>
+          <t>maa://24999 (92.16), maa://36673 (92.41), maa://25001 (85.92)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2111,7 +2111,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (74.09), **maa://22728 (46.67)</t>
+          <t>*maa://21248 (74.19), **maa://22728 (46.67)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.18), *maa://36666 (77.59), *maa://22766 (68.33)</t>
+          <t>maa://21364 (81.18), *maa://36666 (77.78), *maa://22766 (68.33)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2745,7 +2745,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.98)</t>
+          <t>maa://24570 (97.0)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2777,7 +2777,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (90.75), *maa://22732 (51.04)</t>
+          <t>maa://22466 (90.8), *maa://22732 (51.55)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (81.41), ***maa://23820 (30.0)</t>
+          <t>maa://21443 (81.51), ***maa://23820 (30.0)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (93.39), *maa://22432 (78.31)</t>
+          <t>maa://22524 (93.42), *maa://22432 (78.31)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3491,7 +3491,7 @@
       </c>
       <c r="AB23" s="2" t="inlineStr">
         <is>
-          <t>maa://29652 (97.67)</t>
+          <t>maa://29652 (97.73)</t>
         </is>
       </c>
       <c r="AC23" s="1" t="n"/>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.61), *maa://46650 (62.5)</t>
+          <t>*maa://24368 (78.66), *maa://46650 (62.5)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3719,7 +3719,7 @@
       </c>
       <c r="T25" s="2" t="inlineStr">
         <is>
-          <t>maa://20109 (92.18), maa://22545 (100.0), *maa://42915 (75.0)</t>
+          <t>maa://20109 (92.22), maa://22545 (100.0), *maa://42915 (75.0)</t>
         </is>
       </c>
       <c r="U25" s="1" t="n"/>
@@ -4109,7 +4109,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>*maa://29765 (64.37), maa://23263 (95.28)</t>
+          <t>*maa://29765 (64.77), maa://23263 (95.28)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.89), maa://41749 (91.4), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.89), maa://41749 (91.58), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.59), maa://28440 (80.87), maa://31400 (98.82), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.59), maa://28440 (81.03), maa://31400 (98.82), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4597,7 +4597,7 @@
       </c>
       <c r="L32" s="2" t="inlineStr">
         <is>
-          <t>maa://28065 (95.56)</t>
+          <t>maa://28065 (95.65)</t>
         </is>
       </c>
       <c r="M32" s="1" t="n"/>
@@ -4759,7 +4759,7 @@
       </c>
       <c r="T33" s="2" t="inlineStr">
         <is>
-          <t>maa://45558 (88.89)</t>
+          <t>maa://45558 (90.0)</t>
         </is>
       </c>
       <c r="U33" s="1" t="n"/>
@@ -4873,7 +4873,7 @@
       </c>
       <c r="P34" s="2" t="inlineStr">
         <is>
-          <t>maa://48817 (90.91)</t>
+          <t>maa://48817 (84.62)</t>
         </is>
       </c>
       <c r="Q34" s="1" t="n"/>
@@ -5199,7 +5199,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (97.6), *maa://47069 (73.33), maa://45789 (100.0)</t>
+          <t>maa://45718 (97.6), *maa://47069 (75.0), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5364,7 +5364,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.76)</t>
+          <t>maa://36697 (86.82)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5385,7 +5385,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (89.22), maa://25199 (84.82), maa://30434 (92.05), maa://45059 (81.82), ***maa://25036 (19.23), *maa://44165 (66.67)</t>
+          <t>maa://36670 (89.22), maa://25199 (84.82), maa://30434 (92.31), maa://45059 (81.82), ***maa://25036 (19.23), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5417,7 +5417,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.72), maa://47093 (100.0)</t>
+          <t>maa://24709 (91.77), maa://47093 (100.0)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (80.77), maa://47079 (92.59), *maa://45790 (73.33)</t>
+          <t>maa://45788 (80.77), maa://47079 (93.1), *maa://45790 (73.33)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5502,7 +5502,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.31), maa://21386 (95.79), maa://36664 (89.29), maa://45550 (87.5)</t>
+          <t>maa://23278 (95.31), maa://21386 (95.79), maa://36664 (89.47), maa://45550 (87.5)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5969,7 +5969,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.5), maa://29661 (97.35), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.51), maa://29661 (97.35), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.22), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.24), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#175)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.59), maa://25390 (96.27), maa://36681 (87.34)</t>
+          <t>maa://24702 (94.61), maa://25390 (95.91), maa://36681 (87.34)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (90.7), *maa://20791 (62.34)</t>
+          <t>maa://22742 (90.7), *maa://20791 (62.82)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.44), maa://36684 (95.83), ***maa://22731 (6.25)</t>
+          <t>maa://21246 (91.47), maa://36684 (95.83), ***maa://22731 (6.25)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://40192 (96.72), maa://36987 (96.15), maa://39849 (88.89)</t>
+          <t>maa://40192 (96.77), maa://36987 (96.15), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.83), **maa://20790 (43.48), ***maa://37170 (16.18), maa://45854 (84.85)</t>
+          <t>maa://24617 (89.92), **maa://20790 (43.48), ***maa://37170 (16.18), maa://45854 (85.29)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.89), ***maa://31785 (22.22), maa://43217 (92.11), ***maa://36683 (28.26)</t>
+          <t>**maa://32495 (48.89), ***maa://31785 (22.22), maa://43217 (91.03), ***maa://36683 (28.26)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1026,12 +1026,12 @@
       </c>
       <c r="AE4" s="1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (64.0), ***maa://26209 (13.04), *maa://39394 (65.38)</t>
+          <t>*maa://30062 (64.0), ***maa://26209 (13.04), *maa://39394 (65.38), maa://48095 (100.0)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (96.72)</t>
+          <t>maa://42407 (95.16)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (92.92), maa://24957 (97.78)</t>
+          <t>maa://28624 (92.98), maa://24957 (97.78)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.62), *maa://22758 (75.0)</t>
+          <t>maa://22399 (95.68), *maa://22758 (75.34)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.03.30 13:18:18</t>
+          <t>更新日期：2025.04.03 13:19:19</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1607,7 +1607,7 @@
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>maa://22762 (92.39), maa://39552 (81.25)</t>
+          <t>maa://22762 (92.47), maa://39552 (81.25)</t>
         </is>
       </c>
       <c r="M9" s="1" t="n"/>
@@ -1769,7 +1769,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.57), maa://22755 (87.83), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.59), maa://22755 (87.83), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.78), maa://45828 (87.5), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.78), maa://45828 (88.24), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.16), maa://36673 (92.41), maa://25001 (85.92)</t>
+          <t>maa://24999 (92.18), maa://36673 (92.41), maa://25001 (85.92)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2111,7 +2111,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (74.19), **maa://22728 (46.67)</t>
+          <t>*maa://21248 (73.9), **maa://22728 (46.67)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2175,7 +2175,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>maa://34957 (81.71), **maa://22768 (50.0)</t>
+          <t>maa://34957 (81.93), **maa://22768 (50.0)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2207,7 +2207,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (34.25), maa://39883 (90.79), *maa://39885 (53.33)</t>
+          <t>**maa://22737 (34.25), maa://39883 (90.79), *maa://39885 (51.61)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2257,7 +2257,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://26245 (96.77), maa://21288 (96.3), maa://39841 (94.02), maa://36682 (97.44)</t>
+          <t>maa://26245 (96.82), maa://21288 (96.3), maa://39841 (94.17), maa://36682 (97.44)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="T15" s="2" t="inlineStr">
         <is>
-          <t>maa://23892 (96.3)</t>
+          <t>maa://23892 (96.34)</t>
         </is>
       </c>
       <c r="U15" s="1" t="n"/>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.18), *maa://36666 (77.78), *maa://22766 (68.33)</t>
+          <t>maa://21364 (80.94), *maa://36666 (77.12), *maa://22766 (68.33)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2631,7 +2631,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.83), maa://39599 (83.64)</t>
+          <t>maa://22430 (88.83), maa://39599 (84.21)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (88.67)</t>
+          <t>maa://24421 (88.33)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2777,7 +2777,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (90.8), *maa://22732 (51.55)</t>
+          <t>maa://22466 (90.91), *maa://22732 (51.55)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (99.18)</t>
+          <t>maa://24386 (99.19)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -2971,7 +2971,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (66.29), *maa://36668 (57.5)</t>
+          <t>*maa://30709 (66.22), *maa://36668 (57.5)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.56), maa://25198 (93.69), *maa://20795 (50.77), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.61), maa://25198 (93.75), *maa://20795 (50.77), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (84.94)</t>
+          <t>maa://41331 (85.03)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3183,7 +3183,7 @@
       </c>
       <c r="P21" s="2" t="inlineStr">
         <is>
-          <t>maa://24381 (85.0)</t>
+          <t>maa://24381 (80.95)</t>
         </is>
       </c>
       <c r="Q21" s="1" t="n"/>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (93.42), *maa://22432 (78.31)</t>
+          <t>maa://22524 (93.42), *maa://22432 (78.82)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.63), *maa://37649 (65.52)</t>
+          <t>maa://21282 (98.64), *maa://37649 (65.52)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3395,7 +3395,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.38), *maa://41753 (52.38)</t>
+          <t>***maa://28036 (28.0), *maa://41753 (52.38)</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.91), maa://39875 (94.59)</t>
+          <t>maa://39756 (95.92), maa://39875 (94.59)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3605,7 +3605,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (83.97), maa://23504 (93.33), **maa://22892 (40.54), *maa://25141 (77.1), *maa://36663 (77.5), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (83.71), maa://23504 (93.35), **maa://22892 (40.54), *maa://25141 (77.1), *maa://36663 (77.5), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3655,7 +3655,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.24)</t>
+          <t>maa://29753 (95.26)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3671,7 +3671,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (72.62), *maa://25311 (74.77), ***maa://22725 (4.76), *maa://45047 (66.67)</t>
+          <t>*maa://29063 (72.78), *maa://25311 (74.77), ***maa://22725 (4.76), *maa://45047 (66.67)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3735,7 +3735,7 @@
       </c>
       <c r="X25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29890 (79.59)</t>
+          <t>*maa://29890 (80.0)</t>
         </is>
       </c>
       <c r="Y25" s="1" t="n"/>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (94.69)</t>
+          <t>maa://42235 (94.78)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4045,7 +4045,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.97), maa://25725 (84.27)</t>
+          <t>maa://24465 (90.98), maa://25725 (84.27)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.89), maa://41749 (91.58), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.69), maa://41749 (91.67), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4191,7 +4191,7 @@
       </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>*maa://25175 (66.67)</t>
+          <t>*maa://25175 (65.45)</t>
         </is>
       </c>
       <c r="I29" s="1" t="n"/>
@@ -4287,7 +4287,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.93), maa://42865 (81.16), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.93), maa://42865 (81.43), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4305,7 +4305,7 @@
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>maa://45792 (94.12)</t>
+          <t>maa://45792 (94.44)</t>
         </is>
       </c>
       <c r="E30" s="1" t="n"/>
@@ -4401,7 +4401,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.13), maa://45822 (100.0), *maa://45045 (80.0)</t>
+          <t>maa://42979 (97.14), maa://45822 (100.0), *maa://45045 (80.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4467,7 +4467,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.38), maa://36258 (84.87), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.4), maa://36258 (85.12), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4581,7 +4581,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.07), maa://36667 (97.73), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.1), maa://36667 (97.73), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4597,7 +4597,7 @@
       </c>
       <c r="L32" s="2" t="inlineStr">
         <is>
-          <t>maa://28065 (95.65)</t>
+          <t>maa://28065 (95.74)</t>
         </is>
       </c>
       <c r="M32" s="1" t="n"/>
@@ -4873,7 +4873,7 @@
       </c>
       <c r="P34" s="2" t="inlineStr">
         <is>
-          <t>maa://48817 (84.62)</t>
+          <t>maa://48817 (87.5)</t>
         </is>
       </c>
       <c r="Q34" s="1" t="n"/>
@@ -4937,7 +4937,7 @@
       </c>
       <c r="AF34" s="2" t="inlineStr">
         <is>
-          <t>*maa://32650 (75.0)</t>
+          <t>*maa://32650 (76.19)</t>
         </is>
       </c>
       <c r="AG34" s="1" t="n"/>
@@ -4987,7 +4987,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.47)</t>
+          <t>maa://41296 (96.51)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5019,7 +5019,7 @@
       </c>
       <c r="T35" s="2" t="inlineStr">
         <is>
-          <t>maa://24842 (94.12)</t>
+          <t>maa://24842 (94.23)</t>
         </is>
       </c>
       <c r="U35" s="1" t="n"/>
@@ -5199,7 +5199,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (97.6), *maa://47069 (75.0), maa://45789 (100.0)</t>
+          <t>maa://45718 (97.66), *maa://47069 (75.0), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5364,7 +5364,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.82)</t>
+          <t>maa://36697 (86.94)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5385,7 +5385,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (89.22), maa://25199 (84.82), maa://30434 (92.31), maa://45059 (81.82), ***maa://25036 (19.23), *maa://44165 (66.67)</t>
+          <t>maa://36670 (89.22), maa://25199 (84.96), maa://30434 (91.3), *maa://45059 (78.26), ***maa://25036 (18.52), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://45788 (80.77), maa://47079 (93.1), *maa://45790 (73.33)</t>
+          <t>*maa://45788 (80.0), maa://47079 (93.33), *maa://45790 (73.33)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5916,7 +5916,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (91.98), maa://43901 (93.33)</t>
+          <t>maa://35931 (91.98), maa://43901 (93.75)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.24), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.25), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6330,7 +6330,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.11)</t>
+          <t>maa://32532 (92.14)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#176)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (90.7), *maa://20791 (62.82)</t>
+          <t>maa://22742 (90.75), *maa://20791 (62.82)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://40192 (96.77), maa://36987 (96.15), maa://39849 (88.89)</t>
+          <t>maa://40192 (96.83), maa://36987 (96.15), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (89.92), **maa://20790 (43.48), ***maa://37170 (16.18), maa://45854 (85.29)</t>
+          <t>maa://24617 (90.0), **maa://20790 (43.48), ***maa://37170 (16.18), maa://45854 (85.71)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (95.8), maa://27295 (86.49), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
+          <t>maa://32509 (95.8), maa://27295 (86.67), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.89), ***maa://31785 (22.22), maa://43217 (91.03), ***maa://36683 (28.26)</t>
+          <t>**maa://32495 (48.71), ***maa://31785 (22.22), maa://43217 (91.14), ***maa://36683 (28.26)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.49), maa://22744 (84.62)</t>
+          <t>maa://21245 (84.55), maa://22744 (84.62)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.04.03 13:19:19</t>
+          <t>更新日期：2025.04.04 13:19:56</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (84.03), *maa://21916 (62.12), maa://23252 (91.18), maa://37496 (96.97), **maa://22759 (45.45)</t>
+          <t>maa://32931 (84.17), *maa://21916 (62.12), maa://23252 (91.18), maa://37496 (96.97), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (96.0)</t>
+          <t>maa://21411 (96.01)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1769,7 +1769,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.59), maa://22755 (87.83), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.6), maa://22755 (87.83), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.59), maa://22501 (97.83), maa://45521 (86.36)</t>
+          <t>maa://22747 (92.64), maa://22501 (97.85), maa://45521 (86.36)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -2045,7 +2045,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.11), *maa://21485 (75.35), maa://37962 (90.7)</t>
+          <t>maa://22753 (91.16), *maa://21485 (75.35), maa://37962 (90.7)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.18), maa://36673 (92.41), maa://25001 (85.92)</t>
+          <t>maa://24999 (92.19), maa://36673 (92.41), maa://25001 (85.92)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2111,7 +2111,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.9), **maa://22728 (46.67)</t>
+          <t>*maa://21248 (73.6), **maa://22728 (46.67)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2355,7 +2355,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.24), maa://22734 (84.17), *maa://30808 (64.18), *maa://36048 (50.75), maa://45058 (93.33)</t>
+          <t>*maa://22743 (78.24), maa://22734 (84.17), *maa://30808 (64.18), *maa://36048 (51.47), maa://45058 (93.33)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.94), *maa://36666 (77.12), *maa://22766 (68.33)</t>
+          <t>maa://21364 (80.99), *maa://36666 (77.12), *maa://22766 (68.33)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2533,7 +2533,7 @@
       </c>
       <c r="P16" s="2" t="inlineStr">
         <is>
-          <t>maa://28504 (91.53)</t>
+          <t>maa://28504 (91.67)</t>
         </is>
       </c>
       <c r="Q16" s="1" t="n"/>
@@ -2581,7 +2581,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.15)</t>
+          <t>maa://26228 (95.19)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2777,7 +2777,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (90.91), *maa://22732 (51.55)</t>
+          <t>maa://22466 (90.96), *maa://22732 (51.55)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2971,7 +2971,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (66.22), *maa://36668 (57.5)</t>
+          <t>*maa://30709 (66.22), *maa://36668 (58.02)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.61), maa://25198 (93.75), *maa://20795 (50.77), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.66), maa://25198 (93.75), *maa://20795 (50.77), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3215,7 +3215,7 @@
       </c>
       <c r="X21" s="2" t="inlineStr">
         <is>
-          <t>maa://20110 (86.76), maa://34946 (91.11)</t>
+          <t>maa://20110 (86.76), maa://34946 (91.3)</t>
         </is>
       </c>
       <c r="Y21" s="1" t="n"/>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (81.51), ***maa://23820 (30.0)</t>
+          <t>maa://21443 (81.56), ***maa://23820 (30.0)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.92), maa://39875 (94.59)</t>
+          <t>maa://39756 (95.68), maa://39875 (94.59)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3605,7 +3605,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (83.71), maa://23504 (93.35), **maa://22892 (40.54), *maa://25141 (77.1), *maa://36663 (77.5), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (83.71), maa://23504 (93.39), **maa://22892 (40.54), *maa://25141 (77.1), *maa://36663 (77.5), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3671,7 +3671,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (72.78), *maa://25311 (74.77), ***maa://22725 (4.76), *maa://45047 (66.67)</t>
+          <t>*maa://29063 (72.94), *maa://25311 (74.77), ***maa://22725 (4.76), *maa://45047 (66.67)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3785,7 +3785,7 @@
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>maa://41802 (90.91)</t>
+          <t>maa://41802 (91.3)</t>
         </is>
       </c>
       <c r="E26" s="1" t="n"/>
@@ -4287,7 +4287,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (68.93), maa://42865 (81.43), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (68.93), maa://42865 (81.94), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4581,7 +4581,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.1), maa://36667 (97.73), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.12), maa://36667 (97.73), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4873,7 +4873,7 @@
       </c>
       <c r="P34" s="2" t="inlineStr">
         <is>
-          <t>maa://48817 (87.5)</t>
+          <t>maa://48817 (88.24)</t>
         </is>
       </c>
       <c r="Q34" s="1" t="n"/>
@@ -5199,7 +5199,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (97.66), *maa://47069 (75.0), maa://45789 (100.0)</t>
+          <t>maa://45718 (97.67), *maa://47069 (75.0), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.25), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.27), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6330,7 +6330,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.14)</t>
+          <t>maa://32532 (92.16)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6402,7 +6402,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://31270 (94.78), maa://27746 (82.46)</t>
+          <t>maa://31270 (94.81), maa://27746 (82.46)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6420,7 +6420,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (70.31)</t>
+          <t>*maa://40438 (70.77)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#177)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.65), maa://26254 (96.67), **maa://22738 (50.0)</t>
+          <t>maa://21249 (94.67), maa://26254 (96.67), **maa://22738 (50.0)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.36), maa://27484 (96.67), maa://27480 (83.33)</t>
+          <t>maa://27396 (84.36), maa://27484 (96.69), maa://27480 (83.33)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (95.8), maa://27295 (86.67), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
+          <t>maa://32509 (95.8), maa://27295 (86.84), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.55), maa://22744 (84.62)</t>
+          <t>maa://21245 (84.55), maa://22744 (81.48)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.04.04 13:19:56</t>
+          <t>更新日期：2025.04.05 17:12:18</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.32), ***maa://39951 (13.56), ***maa://34206 (22.22), ***maa://39243 (25.0), *maa://45271 (53.49)</t>
+          <t>***maa://25695 (18.32), ***maa://39951 (13.33), ***maa://34206 (22.22), ***maa://39243 (25.0), *maa://45271 (53.49)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.81)</t>
+          <t>maa://36713 (97.82)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (90.06), ***maa://45826 (25.0)</t>
+          <t>maa://21867 (90.06), **maa://45826 (33.33)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.19), maa://36673 (92.41), maa://25001 (85.92)</t>
+          <t>maa://24999 (92.2), maa://36673 (92.41), maa://25001 (85.92)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2111,7 +2111,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.6), **maa://22728 (46.67)</t>
+          <t>*maa://21248 (73.71), **maa://22728 (46.67)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (87.95), maa://21478 (89.47)</t>
+          <t>maa://24304 (87.95), maa://21478 (89.74)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.99), *maa://36666 (77.12), *maa://22766 (68.33)</t>
+          <t>maa://21364 (80.29), *maa://36666 (77.12), *maa://22766 (68.33)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2565,7 +2565,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (98.1), maa://28051 (96.0)</t>
+          <t>maa://28501 (98.11), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>*maa://42324 (51.52)</t>
+          <t>**maa://42324 (50.0)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2745,7 +2745,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.0)</t>
+          <t>maa://24570 (97.01)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (81.56), ***maa://23820 (30.0)</t>
+          <t>maa://21443 (81.61), ***maa://23820 (30.0)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.68), maa://39875 (94.59)</t>
+          <t>maa://39756 (95.69), maa://39875 (94.59)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3507,7 +3507,7 @@
       </c>
       <c r="AF23" s="2" t="inlineStr">
         <is>
-          <t>maa://31489 (94.44)</t>
+          <t>maa://31489 (94.74)</t>
         </is>
       </c>
       <c r="AG23" s="1" t="n"/>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.66), *maa://46650 (62.5)</t>
+          <t>*maa://24368 (78.66), *maa://46650 (66.67)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3979,7 +3979,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (77.05)</t>
+          <t>*maa://30624 (75.81)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.69), maa://41749 (91.67), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.69), maa://41749 (91.75), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4157,7 +4157,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.58), *maa://36701 (66.67)</t>
+          <t>maa://36660 (92.6), *maa://36701 (66.67)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4401,7 +4401,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.14), maa://45822 (100.0), *maa://45045 (80.0)</t>
+          <t>maa://42979 (97.16), maa://45822 (100.0), *maa://45045 (80.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4873,7 +4873,7 @@
       </c>
       <c r="P34" s="2" t="inlineStr">
         <is>
-          <t>maa://48817 (88.24)</t>
+          <t>maa://48817 (89.47)</t>
         </is>
       </c>
       <c r="Q34" s="1" t="n"/>
@@ -5316,7 +5316,7 @@
       </c>
       <c r="P38" s="2" t="inlineStr">
         <is>
-          <t>*maa://24383 (68.93)</t>
+          <t>*maa://24383 (69.23)</t>
         </is>
       </c>
       <c r="Q38" s="1" t="n"/>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>*maa://45788 (80.0), maa://47079 (93.33), *maa://45790 (73.33)</t>
+          <t>*maa://45788 (80.0), maa://47079 (93.55), *maa://45790 (75.0)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5916,7 +5916,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (91.98), maa://43901 (93.75)</t>
+          <t>maa://35931 (92.0), maa://43901 (93.75)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.27), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.29), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6330,7 +6330,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.16)</t>
+          <t>maa://32532 (92.19)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6492,7 +6492,7 @@
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>maa://44405 (85.71)</t>
+          <t>maa://44405 (86.21)</t>
         </is>
       </c>
       <c r="I64" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#178)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.04.05 17:12:18</t>
+          <t>更新日期：2025.04.05 17:33:18</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -2355,7 +2355,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.24), maa://22734 (84.17), *maa://30808 (64.18), *maa://36048 (51.47), maa://45058 (93.33)</t>
+          <t>*maa://22743 (78.24), maa://22734 (84.17), *maa://30808 (64.18), *maa://36048 (52.17), maa://45058 (93.33)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -4467,7 +4467,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.4), maa://36258 (85.12), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.4), maa://36258 (85.25), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.29), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.3), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>

</xml_diff>

<commit_message>
Revert "CI: Auto Update Data (#177)"
This reverts commit bdc6f5b7
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.67), maa://26254 (96.67), **maa://22738 (50.0)</t>
+          <t>maa://21249 (94.65), maa://26254 (96.67), **maa://22738 (50.0)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.36), maa://27484 (96.69), maa://27480 (83.33)</t>
+          <t>maa://27396 (84.36), maa://27484 (96.67), maa://27480 (83.33)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (95.8), maa://27295 (86.84), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
+          <t>maa://32509 (95.8), maa://27295 (86.67), maa://22754 (90.41), *maa://21746 (55.81), *maa://31008 (78.57)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.55), maa://22744 (81.48)</t>
+          <t>maa://21245 (84.55), maa://22744 (84.62)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.04.05 17:33:18</t>
+          <t>更新日期：2025.04.04 13:19:56</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.32), ***maa://39951 (13.33), ***maa://34206 (22.22), ***maa://39243 (25.0), *maa://45271 (53.49)</t>
+          <t>***maa://25695 (18.32), ***maa://39951 (13.56), ***maa://34206 (22.22), ***maa://39243 (25.0), *maa://45271 (53.49)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.82)</t>
+          <t>maa://36713 (97.81)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (90.06), **maa://45826 (33.33)</t>
+          <t>maa://21867 (90.06), ***maa://45826 (25.0)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.2), maa://36673 (92.41), maa://25001 (85.92)</t>
+          <t>maa://24999 (92.19), maa://36673 (92.41), maa://25001 (85.92)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2111,7 +2111,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.71), **maa://22728 (46.67)</t>
+          <t>*maa://21248 (73.6), **maa://22728 (46.67)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2355,7 +2355,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.24), maa://22734 (84.17), *maa://30808 (64.18), *maa://36048 (52.17), maa://45058 (93.33)</t>
+          <t>*maa://22743 (78.24), maa://22734 (84.17), *maa://30808 (64.18), *maa://36048 (51.47), maa://45058 (93.33)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (87.95), maa://21478 (89.74)</t>
+          <t>maa://24304 (87.95), maa://21478 (89.47)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.29), *maa://36666 (77.12), *maa://22766 (68.33)</t>
+          <t>maa://21364 (80.99), *maa://36666 (77.12), *maa://22766 (68.33)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2565,7 +2565,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (98.11), maa://28051 (96.0)</t>
+          <t>maa://28501 (98.1), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>**maa://42324 (50.0)</t>
+          <t>*maa://42324 (51.52)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2745,7 +2745,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.01)</t>
+          <t>maa://24570 (97.0)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (81.61), ***maa://23820 (30.0)</t>
+          <t>maa://21443 (81.56), ***maa://23820 (30.0)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.69), maa://39875 (94.59)</t>
+          <t>maa://39756 (95.68), maa://39875 (94.59)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3507,7 +3507,7 @@
       </c>
       <c r="AF23" s="2" t="inlineStr">
         <is>
-          <t>maa://31489 (94.74)</t>
+          <t>maa://31489 (94.44)</t>
         </is>
       </c>
       <c r="AG23" s="1" t="n"/>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.66), *maa://46650 (66.67)</t>
+          <t>*maa://24368 (78.66), *maa://46650 (62.5)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3979,7 +3979,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (75.81)</t>
+          <t>*maa://30624 (77.05)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.69), maa://41749 (91.75), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.69), maa://41749 (91.67), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4157,7 +4157,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.6), *maa://36701 (66.67)</t>
+          <t>maa://36660 (92.58), *maa://36701 (66.67)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4401,7 +4401,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.16), maa://45822 (100.0), *maa://45045 (80.0)</t>
+          <t>maa://42979 (97.14), maa://45822 (100.0), *maa://45045 (80.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4467,7 +4467,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.4), maa://36258 (85.25), *maa://43904 (72.73)</t>
+          <t>maa://35926 (93.4), maa://36258 (85.12), *maa://43904 (72.73)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4873,7 +4873,7 @@
       </c>
       <c r="P34" s="2" t="inlineStr">
         <is>
-          <t>maa://48817 (89.47)</t>
+          <t>maa://48817 (88.24)</t>
         </is>
       </c>
       <c r="Q34" s="1" t="n"/>
@@ -5316,7 +5316,7 @@
       </c>
       <c r="P38" s="2" t="inlineStr">
         <is>
-          <t>*maa://24383 (69.23)</t>
+          <t>*maa://24383 (68.93)</t>
         </is>
       </c>
       <c r="Q38" s="1" t="n"/>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>*maa://45788 (80.0), maa://47079 (93.55), *maa://45790 (75.0)</t>
+          <t>*maa://45788 (80.0), maa://47079 (93.33), *maa://45790 (73.33)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5916,7 +5916,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.0), maa://43901 (93.75)</t>
+          <t>maa://35931 (91.98), maa://43901 (93.75)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.3), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.27), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6330,7 +6330,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.19)</t>
+          <t>maa://32532 (92.16)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6492,7 +6492,7 @@
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>maa://44405 (86.21)</t>
+          <t>maa://44405 (85.71)</t>
         </is>
       </c>
       <c r="I64" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#180)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1260" yWindow="3000" windowWidth="23925" windowHeight="16665" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.17), *maa://30515 (70.48), maa://39402 (93.06), *maa://34787 (73.42), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.17), *maa://30515 (70.48), maa://39402 (93.15), *maa://34787 (73.42), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.47), maa://36684 (95.2), ***maa://22731 (6.25)</t>
+          <t>maa://21246 (91.47), maa://36684 (95.24), ***maa://22731 (6.25)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (83.89), maa://27484 (96.75), maa://27480 (83.33)</t>
+          <t>maa://27396 (83.94), maa://27484 (96.75), maa://27480 (83.33)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (94.94)</t>
+          <t>maa://24390 (95.0)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (95.83), maa://27295 (87.18), maa://22754 (90.41), *maa://31008 (78.57), *maa://21746 (55.81)</t>
+          <t>maa://32509 (95.87), maa://27295 (87.18), maa://22754 (90.41), *maa://31008 (78.57), *maa://21746 (55.81)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.72), ***maa://31785 (22.22), maa://43217 (90.48), ***maa://36683 (29.79)</t>
+          <t>**maa://32495 (48.54), ***maa://31785 (22.22), maa://43217 (90.59), ***maa://36683 (29.79)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (95.31)</t>
+          <t>maa://42407 (95.38)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.04.13 00:29:41</t>
+          <t>更新日期：2025.04.13 13:23:50</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1671,7 +1671,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.2), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), *maa://45044 (66.67), maa://40166 (96.67)</t>
+          <t>maa://28711 (87.3), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), *maa://45044 (66.67), maa://40166 (96.67)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.65), ***maa://39951 (12.7), ***maa://34206 (22.22), ***maa://39243 (25.0), *maa://45271 (53.19)</t>
+          <t>***maa://25695 (18.65), ***maa://39951 (12.7), ***maa://34206 (22.22), ***maa://39243 (25.0), *maa://45271 (54.17)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.68), maa://22501 (97.92), maa://45521 (88.0)</t>
+          <t>maa://22747 (92.73), maa://22501 (97.92), maa://45521 (88.0)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1931,7 +1931,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://29912 (97.37), maa://22516 (88.37), *maa://20794 (52.24)</t>
+          <t>maa://29912 (97.4), maa://22516 (88.37), *maa://20794 (52.24)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -1965,7 +1965,7 @@
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>maa://30766 (89.29), *maa://36678 (75.0)</t>
+          <t>maa://30766 (89.29), *maa://36678 (77.78)</t>
         </is>
       </c>
       <c r="E12" s="1" t="n"/>
@@ -2225,7 +2225,7 @@
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>maa://30764 (88.14)</t>
+          <t>maa://30764 (88.33)</t>
         </is>
       </c>
       <c r="E14" s="1" t="n"/>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="T15" s="2" t="inlineStr">
         <is>
-          <t>maa://23892 (96.34)</t>
+          <t>maa://23892 (96.39)</t>
         </is>
       </c>
       <c r="U15" s="1" t="n"/>
@@ -2533,7 +2533,7 @@
       </c>
       <c r="P16" s="2" t="inlineStr">
         <is>
-          <t>maa://28504 (91.8)</t>
+          <t>maa://28504 (91.94)</t>
         </is>
       </c>
       <c r="Q16" s="1" t="n"/>
@@ -2565,7 +2565,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (98.15), maa://28051 (96.0)</t>
+          <t>maa://28501 (98.17), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2615,7 +2615,7 @@
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>maa://21624 (85.0)</t>
+          <t>maa://21624 (85.37)</t>
         </is>
       </c>
       <c r="E17" s="1" t="n"/>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>**maa://42324 (50.0)</t>
+          <t>*maa://42324 (51.22)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2777,7 +2777,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (91.21), *maa://22732 (52.04)</t>
+          <t>maa://22466 (91.3), *maa://22732 (52.04)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2841,7 +2841,7 @@
       </c>
       <c r="AB18" s="2" t="inlineStr">
         <is>
-          <t>maa://24393 (97.96)</t>
+          <t>maa://24393 (98.0)</t>
         </is>
       </c>
       <c r="AC18" s="1" t="n"/>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.76), maa://25198 (93.81), *maa://20795 (50.77), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.81), maa://25198 (93.81), *maa://20795 (50.77), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (86.03)</t>
+          <t>maa://41331 (86.11)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="P20" s="2" t="inlineStr">
         <is>
-          <t>maa://37442 (95.65)</t>
+          <t>maa://37442 (95.74)</t>
         </is>
       </c>
       <c r="Q20" s="1" t="n"/>
@@ -3085,7 +3085,7 @@
       </c>
       <c r="X20" s="2" t="inlineStr">
         <is>
-          <t>maa://49976 (90.91), maa://50085 (100.0)</t>
+          <t>maa://49976 (91.3), maa://50085 (100.0)</t>
         </is>
       </c>
       <c r="Y20" s="1" t="n"/>
@@ -3377,7 +3377,7 @@
       </c>
       <c r="AF22" s="2" t="inlineStr">
         <is>
-          <t>maa://29658 (93.88)</t>
+          <t>maa://29658 (94.0)</t>
         </is>
       </c>
       <c r="AG22" s="1" t="n"/>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.85), maa://39875 (94.59)</t>
+          <t>maa://39756 (95.87), maa://39875 (94.59)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3475,7 +3475,7 @@
       </c>
       <c r="X23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (69.41)</t>
+          <t>*maa://28503 (69.77)</t>
         </is>
       </c>
       <c r="Y23" s="1" t="n"/>
@@ -3491,7 +3491,7 @@
       </c>
       <c r="AB23" s="2" t="inlineStr">
         <is>
-          <t>maa://29652 (97.73)</t>
+          <t>maa://29652 (97.78)</t>
         </is>
       </c>
       <c r="AC23" s="1" t="n"/>
@@ -3605,7 +3605,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (83.4), maa://23504 (93.45), **maa://22892 (40.27), *maa://25141 (77.27), *maa://36663 (78.31), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (83.4), maa://23504 (93.48), **maa://22892 (40.27), *maa://25141 (77.27), *maa://36663 (78.31), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3655,7 +3655,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.31)</t>
+          <t>maa://29753 (95.32)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3703,7 +3703,7 @@
       </c>
       <c r="P25" s="2" t="inlineStr">
         <is>
-          <t>maa://24382 (93.55)</t>
+          <t>maa://24382 (93.75)</t>
         </is>
       </c>
       <c r="Q25" s="1" t="n"/>
@@ -3751,7 +3751,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (88.52), maa://24516 (80.22), maa://26001 (87.5)</t>
+          <t>maa://31215 (88.62), maa://24516 (80.22), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3767,7 +3767,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.4), maa://24621 (96.95), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
+          <t>maa://20108 (96.4), maa://24621 (96.97), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3785,7 +3785,7 @@
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>maa://41802 (91.67)</t>
+          <t>maa://41802 (92.0)</t>
         </is>
       </c>
       <c r="E26" s="1" t="n"/>
@@ -3865,7 +3865,7 @@
       </c>
       <c r="X26" s="2" t="inlineStr">
         <is>
-          <t>maa://24389 (96.67)</t>
+          <t>maa://24389 (96.77)</t>
         </is>
       </c>
       <c r="Y26" s="1" t="n"/>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (95.0)</t>
+          <t>maa://42235 (95.04)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3897,7 +3897,7 @@
       </c>
       <c r="AF26" s="2" t="inlineStr">
         <is>
-          <t>maa://30511 (81.82), *maa://29760 (56.25)</t>
+          <t>maa://30511 (82.22), *maa://29760 (56.25)</t>
         </is>
       </c>
       <c r="AG26" s="1" t="n"/>
@@ -3947,7 +3947,7 @@
       </c>
       <c r="L27" s="2" t="inlineStr">
         <is>
-          <t>maa://28071 (90.48)</t>
+          <t>maa://28071 (90.91)</t>
         </is>
       </c>
       <c r="M27" s="1" t="n"/>
@@ -4157,7 +4157,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.47), *maa://36701 (66.67)</t>
+          <t>maa://36660 (92.49), *maa://36701 (66.67)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4175,7 +4175,7 @@
       </c>
       <c r="D29" s="2" t="inlineStr">
         <is>
-          <t>maa://31694 (98.15)</t>
+          <t>maa://31694 (98.18)</t>
         </is>
       </c>
       <c r="E29" s="1" t="n"/>
@@ -4305,7 +4305,7 @@
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>maa://45792 (90.48)</t>
+          <t>maa://45792 (90.91)</t>
         </is>
       </c>
       <c r="E30" s="1" t="n"/>
@@ -4467,7 +4467,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.46), maa://36258 (85.16), *maa://43904 (75.0)</t>
+          <t>maa://35926 (93.49), maa://36258 (85.16), *maa://43904 (75.0)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4499,7 +4499,7 @@
       </c>
       <c r="T31" s="2" t="inlineStr">
         <is>
-          <t>maa://30711 (96.61), maa://30768 (100.0)</t>
+          <t>maa://30711 (96.67), maa://30768 (100.0)</t>
         </is>
       </c>
       <c r="U31" s="1" t="n"/>
@@ -4597,7 +4597,7 @@
       </c>
       <c r="L32" s="2" t="inlineStr">
         <is>
-          <t>maa://28065 (95.74)</t>
+          <t>maa://28065 (95.83)</t>
         </is>
       </c>
       <c r="M32" s="1" t="n"/>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="AF32" s="2" t="inlineStr">
         <is>
-          <t>maa://42408 (84.62)</t>
+          <t>maa://42408 (85.71)</t>
         </is>
       </c>
       <c r="AG32" s="1" t="n"/>
@@ -4873,7 +4873,7 @@
       </c>
       <c r="P34" s="2" t="inlineStr">
         <is>
-          <t>maa://48817 (92.31)</t>
+          <t>maa://48817 (92.59)</t>
         </is>
       </c>
       <c r="Q34" s="1" t="n"/>
@@ -4937,7 +4937,7 @@
       </c>
       <c r="AF34" s="2" t="inlineStr">
         <is>
-          <t>*maa://32650 (76.19)</t>
+          <t>*maa://32650 (77.27)</t>
         </is>
       </c>
       <c r="AG34" s="1" t="n"/>
@@ -4987,7 +4987,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.72)</t>
+          <t>maa://41296 (96.74)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5067,7 +5067,7 @@
       </c>
       <c r="AF35" s="2" t="inlineStr">
         <is>
-          <t>maa://39479 (90.0)</t>
+          <t>maa://39479 (90.48)</t>
         </is>
       </c>
       <c r="AG35" s="1" t="n"/>
@@ -5231,7 +5231,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.64), *maa://21239 (69.23)</t>
+          <t>maa://21280 (89.69), *maa://21239 (69.23)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5348,7 +5348,7 @@
       </c>
       <c r="T38" s="2" t="inlineStr">
         <is>
-          <t>maa://30713 (96.97)</t>
+          <t>maa://30713 (97.06)</t>
         </is>
       </c>
       <c r="U38" s="1" t="n"/>
@@ -5619,7 +5619,7 @@
       </c>
       <c r="P41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (40.0), maa://43177 (91.67)</t>
+          <t>**maa://35616 (40.0), maa://43177 (92.0)</t>
         </is>
       </c>
       <c r="Q41" s="1" t="n"/>
@@ -5858,7 +5858,7 @@
       </c>
       <c r="T44" s="2" t="inlineStr">
         <is>
-          <t>maa://39366 (89.19)</t>
+          <t>maa://39366 (89.47)</t>
         </is>
       </c>
       <c r="U44" s="1" t="n"/>
@@ -5911,7 +5911,7 @@
       </c>
       <c r="P45" s="2" t="inlineStr">
         <is>
-          <t>*maa://36237 (70.59)</t>
+          <t>*maa://36237 (72.22)</t>
         </is>
       </c>
       <c r="Q45" s="1" t="n"/>
@@ -5948,7 +5948,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.12), maa://43901 (94.12)</t>
+          <t>maa://35931 (92.12), maa://43901 (94.29)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6123,7 +6123,7 @@
       </c>
       <c r="P49" s="2" t="inlineStr">
         <is>
-          <t>*maa://39643 (64.71)</t>
+          <t>*maa://39643 (65.71)</t>
         </is>
       </c>
       <c r="Q49" s="1" t="n"/>
@@ -6416,7 +6416,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (56.82)</t>
+          <t>*maa://37964 (57.78)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>
@@ -6452,7 +6452,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (71.64)</t>
+          <t>*maa://40438 (72.06)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>
@@ -6729,9 +6729,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="A5:A7"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A5:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#181)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.17), *maa://30515 (70.48), maa://39402 (93.15), *maa://34787 (73.42), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.17), *maa://30515 (70.48), maa://39402 (93.42), *maa://34787 (72.5), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (90.91), *maa://20791 (62.03)</t>
+          <t>maa://22742 (91.01), *maa://20791 (62.03)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.47), maa://36684 (95.24), ***maa://22731 (6.25)</t>
+          <t>maa://21246 (91.53), maa://36684 (94.57), ***maa://22731 (6.25)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (91.2), ***maa://21730 (27.27), ***maa://39501 (13.89), **maa://36675 (50.0)</t>
+          <t>maa://25251 (91.27), ***maa://21730 (27.27), ***maa://39501 (13.89), **maa://36675 (50.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://40192 (97.01), maa://36987 (96.15), maa://39849 (88.89)</t>
+          <t>maa://40192 (97.06), maa://36987 (96.15), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.63), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.65), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (63.77), maa://20276 (86.81), *maa://22749 (80.0)</t>
+          <t>*maa://22880 (63.94), maa://20276 (86.96), *maa://22749 (80.0)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.44), maa://26254 (96.77), **maa://22738 (50.0)</t>
+          <t>maa://21249 (94.51), maa://26254 (96.77), **maa://22738 (50.0)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (90.16), **maa://20790 (43.48), ***maa://37170 (16.18), maa://45854 (87.5)</t>
+          <t>maa://24617 (90.16), **maa://20790 (43.48), ***maa://37170 (15.94), maa://45854 (87.8)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (83.94), maa://27484 (96.75), maa://27480 (83.33)</t>
+          <t>maa://27396 (83.99), maa://27484 (96.75), maa://27480 (83.33)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (95.0)</t>
+          <t>maa://24390 (95.06)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -901,7 +901,7 @@
       </c>
       <c r="AF3" s="2" t="inlineStr">
         <is>
-          <t>*maa://21289 (75.0)</t>
+          <t>*maa://21289 (72.41)</t>
         </is>
       </c>
       <c r="AG3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.85), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.89), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -962,12 +962,12 @@
       </c>
       <c r="O4" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="P4" s="2" t="inlineStr">
         <is>
-          <t>maa://49983 (91.67)</t>
+          <t>maa://49983 (94.44), maa://50121 (100.0)</t>
         </is>
       </c>
       <c r="Q4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (95.87), maa://27295 (87.18), maa://22754 (90.41), *maa://31008 (78.57), *maa://21746 (55.81)</t>
+          <t>maa://32509 (95.87), maa://27295 (87.18), maa://22754 (90.41), *maa://31008 (79.07), *maa://21746 (55.81)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.54), ***maa://31785 (22.22), maa://43217 (90.59), ***maa://36683 (29.79)</t>
+          <t>**maa://32495 (48.54), ***maa://31785 (22.22), maa://43217 (90.8), ***maa://36683 (29.79)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.74), maa://22744 (81.48)</t>
+          <t>maa://21245 (84.92), maa://22744 (81.48)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>*maa://22757 (76.92)</t>
+          <t>*maa://22757 (77.5)</t>
         </is>
       </c>
       <c r="M5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (95.38)</t>
+          <t>maa://42407 (95.52)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>maa://24839 (99.03)</t>
+          <t>maa://24839 (99.04)</t>
         </is>
       </c>
       <c r="M6" s="1" t="n"/>
@@ -1259,12 +1259,12 @@
       </c>
       <c r="W6" s="1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0</t>
         </is>
       </c>
       <c r="X6" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>None</t>
         </is>
       </c>
       <c r="Y6" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (92.44), maa://24957 (97.78)</t>
+          <t>maa://28624 (92.62), maa://24957 (97.78)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="T7" s="2" t="inlineStr">
         <is>
-          <t>maa://21291 (85.42)</t>
+          <t>maa://21291 (86.54)</t>
         </is>
       </c>
       <c r="U7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.81), *maa://22758 (76.32)</t>
+          <t>maa://22399 (95.83), *maa://22758 (76.32)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1405,12 +1405,12 @@
       </c>
       <c r="AA7" s="1" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AB7" s="2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>maa://50141 (100.0)</t>
         </is>
       </c>
       <c r="AC7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (68.6), *maa://36671 (68.0), maa://45272 (94.74), *maa://42530 (62.5)</t>
+          <t>*maa://26191 (68.6), *maa://36671 (68.0), maa://45272 (95.0), *maa://42530 (62.5)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.04.13 13:23:50</t>
+          <t>更新日期：2025.04.17 13:19:49</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>*maa://21476 (73.58), *maa://39431 (60.0), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (74.07), *maa://39431 (60.0), *maa://37551 (57.14)</t>
         </is>
       </c>
       <c r="E8" s="1" t="n"/>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (84.17), *maa://21916 (62.12), maa://23252 (91.18), maa://37496 (96.97), **maa://22759 (45.45)</t>
+          <t>maa://32931 (83.61), *maa://21916 (62.12), maa://23252 (91.18), maa://37496 (96.97), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (96.05)</t>
+          <t>maa://21411 (96.11)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1607,7 +1607,7 @@
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>maa://22762 (92.47), maa://39552 (82.35)</t>
+          <t>maa://22762 (92.55), maa://39552 (83.33)</t>
         </is>
       </c>
       <c r="M9" s="1" t="n"/>
@@ -1623,7 +1623,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (83.02)</t>
+          <t>maa://22736 (83.18)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (87.79), *maa://22865 (51.85)</t>
+          <t>maa://26206 (87.88), *maa://22865 (51.85)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.65), ***maa://39951 (12.7), ***maa://34206 (22.22), ***maa://39243 (25.0), *maa://45271 (54.17)</t>
+          <t>***maa://25695 (18.65), ***maa://39951 (12.7), ***maa://34206 (22.22), *maa://45271 (54.17), ***maa://39243 (25.0)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1721,7 +1721,7 @@
       </c>
       <c r="H10" s="2" t="inlineStr">
         <is>
-          <t>maa://32651 (94.12)</t>
+          <t>maa://32651 (94.44)</t>
         </is>
       </c>
       <c r="I10" s="1" t="n"/>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (89.41), maa://36669 (85.11), *maa://23264 (61.82)</t>
+          <t>maa://28977 (89.41), maa://36669 (83.33), *maa://23264 (61.82)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1769,7 +1769,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.68), maa://22755 (87.93), **maa://22756 (40.91), ***maa://21737 (10.61)</t>
+          <t>maa://27395 (96.24), maa://22755 (88.03), **maa://22756 (40.91), ***maa://21737 (10.45)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.79), maa://45828 (90.91), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.8), maa://45828 (92.0), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1867,7 +1867,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (89.62)</t>
+          <t>maa://21287 (88.79)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.73), maa://22501 (97.92), maa://45521 (88.0)</t>
+          <t>maa://22747 (92.73), maa://22501 (97.96), maa://45521 (88.0)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.86)</t>
+          <t>maa://36713 (97.88)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1931,7 +1931,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://29912 (97.4), maa://22516 (88.37), *maa://20794 (52.24)</t>
+          <t>maa://29912 (97.4), maa://22516 (88.37), *maa://20794 (51.47)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -1965,7 +1965,7 @@
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>maa://30766 (89.29), *maa://36678 (77.78)</t>
+          <t>maa://30766 (89.29), *maa://36678 (80.0)</t>
         </is>
       </c>
       <c r="E12" s="1" t="n"/>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (90.12), **maa://45826 (33.33)</t>
+          <t>maa://21867 (90.17), **maa://45826 (33.33)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2045,7 +2045,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.26), *maa://21485 (74.83), maa://37962 (91.49)</t>
+          <t>maa://22753 (90.86), *maa://21485 (74.83), maa://37962 (91.84)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.43), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (78.21), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.29), maa://36673 (92.59), maa://25001 (85.92)</t>
+          <t>maa://24999 (92.33), maa://36673 (92.68), maa://25001 (85.92)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2111,7 +2111,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.41), **maa://22728 (46.67)</t>
+          <t>*maa://21248 (73.33), **maa://22728 (46.67)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (93.23), *maa://22583 (75.36), *maa://22500 (59.57), maa://48321 (100.0)</t>
+          <t>maa://22676 (93.23), *maa://22583 (75.71), *maa://22500 (59.57), maa://48321 (100.0)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2175,7 +2175,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>maa://34957 (81.18), **maa://22768 (50.0)</t>
+          <t>maa://34957 (81.4), **maa://22768 (50.0)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2207,7 +2207,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (34.25), maa://39883 (90.36), *maa://39885 (53.12)</t>
+          <t>**maa://22737 (34.69), maa://39883 (90.36), *maa://39885 (53.12)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2225,7 +2225,7 @@
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>maa://30764 (88.33)</t>
+          <t>maa://30764 (88.52)</t>
         </is>
       </c>
       <c r="E14" s="1" t="n"/>
@@ -2257,7 +2257,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://39841 (94.44), maa://26245 (96.82), maa://21288 (96.3), maa://36682 (97.5)</t>
+          <t>maa://39841 (94.49), maa://26245 (96.89), maa://21288 (96.3), maa://36682 (97.5)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="AB14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (96.05)</t>
+          <t>maa://22764 (96.1)</t>
         </is>
       </c>
       <c r="AC14" s="1" t="n"/>
@@ -2355,7 +2355,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.64), maa://22734 (84.17), *maa://30808 (64.18), *maa://36048 (56.0), maa://45058 (93.75)</t>
+          <t>*maa://22743 (78.73), maa://22734 (84.17), *maa://30808 (64.18), *maa://36048 (56.0), maa://45058 (93.75)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (87.61), maa://21478 (89.74)</t>
+          <t>maa://24304 (87.67), maa://21478 (89.74)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2403,7 +2403,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (90.7), *maa://22727 (70.0)</t>
+          <t>maa://24762 (90.75), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.4), *maa://36666 (77.5), *maa://22766 (68.33)</t>
+          <t>maa://21364 (80.52), *maa://36666 (78.05), *maa://22766 (68.33)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2485,7 +2485,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.46), maa://36679 (94.55), maa://37650 (97.67)</t>
+          <t>maa://21441 (96.48), maa://36679 (94.55), maa://37650 (97.73)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2533,7 +2533,7 @@
       </c>
       <c r="P16" s="2" t="inlineStr">
         <is>
-          <t>maa://28504 (91.94)</t>
+          <t>maa://28504 (92.06)</t>
         </is>
       </c>
       <c r="Q16" s="1" t="n"/>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.05), *maa://28648 (70.0), *maa://36674 (80.0)</t>
+          <t>maa://22729 (94.08), *maa://28648 (71.23), *maa://36674 (80.0)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2565,7 +2565,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (98.17), maa://28051 (96.0)</t>
+          <t>maa://28501 (98.18), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (65.74), maa://27755 (93.68)</t>
+          <t>*maa://23911 (66.06), maa://27755 (93.68)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2631,7 +2631,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.89), maa://39599 (83.33)</t>
+          <t>maa://22430 (88.89), maa://39599 (83.87)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2663,7 +2663,7 @@
       </c>
       <c r="P17" s="2" t="inlineStr">
         <is>
-          <t>maa://23890 (80.95), *maa://24940 (67.86)</t>
+          <t>maa://23890 (81.13), *maa://24940 (67.86)</t>
         </is>
       </c>
       <c r="Q17" s="1" t="n"/>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>*maa://42324 (51.22)</t>
+          <t>*maa://42324 (52.27)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2722,12 +2722,12 @@
       </c>
       <c r="AE17" s="1" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF17" s="2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>maa://50136 (100.0)</t>
         </is>
       </c>
       <c r="AG17" s="1" t="n"/>
@@ -2745,7 +2745,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (97.06)</t>
+          <t>maa://24570 (96.67)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (88.08)</t>
+          <t>maa://24421 (88.12)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2777,7 +2777,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (91.3), *maa://22732 (52.04)</t>
+          <t>maa://22466 (91.4), *maa://22732 (51.52)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2857,7 +2857,7 @@
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (59.52), **maa://29784 (50.0), *maa://47854 (71.43)</t>
+          <t>*maa://24313 (59.76), **maa://29784 (50.0), *maa://47854 (75.0)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -2971,7 +2971,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (66.44), *maa://36668 (58.02)</t>
+          <t>*maa://30709 (66.37), *maa://36668 (58.02)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.81), maa://25198 (93.81), *maa://20795 (50.77), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.86), maa://25198 (93.86), *maa://20795 (50.77), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3016,12 +3016,12 @@
       </c>
       <c r="G20" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (90.12)</t>
+          <t>maa://22864 (89.57), ***maa://43283 (25.0)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (86.11)</t>
+          <t>maa://41331 (85.71)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="P20" s="2" t="inlineStr">
         <is>
-          <t>maa://37442 (95.74)</t>
+          <t>maa://37442 (95.83)</t>
         </is>
       </c>
       <c r="Q20" s="1" t="n"/>
@@ -3085,7 +3085,7 @@
       </c>
       <c r="X20" s="2" t="inlineStr">
         <is>
-          <t>maa://49976 (91.3), maa://50085 (100.0)</t>
+          <t>*maa://49976 (80.0), maa://50085 (83.33)</t>
         </is>
       </c>
       <c r="Y20" s="1" t="n"/>
@@ -3151,7 +3151,7 @@
       </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>maa://24372 (97.03)</t>
+          <t>maa://24372 (97.06)</t>
         </is>
       </c>
       <c r="I21" s="1" t="n"/>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (81.75), ***maa://23820 (30.0)</t>
+          <t>maa://21443 (81.79), ***maa://23820 (30.0)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (93.04), *maa://22432 (79.55)</t>
+          <t>maa://22524 (92.64), *maa://22432 (77.78)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>*maa://27127 (77.24), *maa://22751 (71.01)</t>
+          <t>*maa://27127 (77.42), *maa://22751 (71.01)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.67), *maa://37649 (65.52)</t>
+          <t>maa://21282 (98.68), *maa://37649 (66.67)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3377,7 +3377,7 @@
       </c>
       <c r="AF22" s="2" t="inlineStr">
         <is>
-          <t>maa://29658 (94.0)</t>
+          <t>maa://29658 (94.23)</t>
         </is>
       </c>
       <c r="AG22" s="1" t="n"/>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.87), maa://39875 (94.59)</t>
+          <t>maa://39756 (95.9), maa://39875 (94.59)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3475,7 +3475,7 @@
       </c>
       <c r="X23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (69.77)</t>
+          <t>*maa://28503 (70.11)</t>
         </is>
       </c>
       <c r="Y23" s="1" t="n"/>
@@ -3491,7 +3491,7 @@
       </c>
       <c r="AB23" s="2" t="inlineStr">
         <is>
-          <t>maa://29652 (97.78)</t>
+          <t>maa://29652 (97.87)</t>
         </is>
       </c>
       <c r="AC23" s="1" t="n"/>
@@ -3605,7 +3605,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (83.4), maa://23504 (93.48), **maa://22892 (40.27), *maa://25141 (77.27), *maa://36663 (78.31), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (83.46), maa://23504 (93.51), **maa://22892 (40.67), *maa://25141 (77.27), *maa://36663 (78.31), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3621,7 +3621,7 @@
       </c>
       <c r="AB24" s="2" t="inlineStr">
         <is>
-          <t>maa://39349 (100.0)</t>
+          <t>maa://39349 (85.71)</t>
         </is>
       </c>
       <c r="AC24" s="1" t="n"/>
@@ -3637,7 +3637,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (84.8), *maa://36672 (79.31), maa://29910 (93.44), **maa://21440 (35.71), maa://45831 (85.71)</t>
+          <t>maa://22523 (84.8), *maa://36672 (79.31), maa://29910 (93.44), **maa://21440 (35.71), maa://45831 (87.5)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3655,7 +3655,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.32)</t>
+          <t>maa://29753 (95.34)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3719,7 +3719,7 @@
       </c>
       <c r="T25" s="2" t="inlineStr">
         <is>
-          <t>maa://20109 (92.27), maa://22545 (100.0), *maa://42915 (75.0)</t>
+          <t>maa://20109 (92.31), maa://22545 (100.0), *maa://42915 (75.0)</t>
         </is>
       </c>
       <c r="U25" s="1" t="n"/>
@@ -3735,7 +3735,7 @@
       </c>
       <c r="X25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29890 (80.0)</t>
+          <t>maa://29890 (80.39)</t>
         </is>
       </c>
       <c r="Y25" s="1" t="n"/>
@@ -4027,7 +4027,7 @@
       </c>
       <c r="AF27" s="2" t="inlineStr">
         <is>
-          <t>maa://24023 (96.0)</t>
+          <t>maa://24023 (96.05)</t>
         </is>
       </c>
       <c r="AG27" s="1" t="n"/>
@@ -4045,7 +4045,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (91.02), maa://25725 (84.62)</t>
+          <t>maa://24465 (91.03), maa://25725 (84.62)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4109,7 +4109,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>*maa://29765 (64.77), maa://23263 (95.28)</t>
+          <t>*maa://29765 (65.17), maa://23263 (95.33)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.82), maa://41749 (91.26), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (90.93), maa://41749 (91.26), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4157,7 +4157,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.49), *maa://36701 (66.67)</t>
+          <t>maa://36660 (92.27), *maa://36701 (66.67)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4175,7 +4175,7 @@
       </c>
       <c r="D29" s="2" t="inlineStr">
         <is>
-          <t>maa://31694 (98.18)</t>
+          <t>maa://31694 (98.21)</t>
         </is>
       </c>
       <c r="E29" s="1" t="n"/>
@@ -4191,7 +4191,7 @@
       </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>*maa://25175 (65.45)</t>
+          <t>*maa://25175 (66.07)</t>
         </is>
       </c>
       <c r="I29" s="1" t="n"/>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.62), maa://28440 (81.36), maa://31400 (98.84), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.66), maa://28440 (81.36), maa://31400 (98.84), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4353,7 +4353,7 @@
       </c>
       <c r="P30" s="2" t="inlineStr">
         <is>
-          <t>maa://21442 (99.12)</t>
+          <t>maa://21442 (99.13)</t>
         </is>
       </c>
       <c r="Q30" s="1" t="n"/>
@@ -4401,7 +4401,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.25), maa://45822 (100.0), *maa://45045 (80.0)</t>
+          <t>maa://42979 (97.28), maa://45822 (100.0), *maa://45045 (80.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4467,7 +4467,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.49), maa://36258 (85.16), *maa://43904 (75.0)</t>
+          <t>maa://35926 (93.51), maa://36258 (85.27), *maa://43904 (76.92)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4499,7 +4499,7 @@
       </c>
       <c r="T31" s="2" t="inlineStr">
         <is>
-          <t>maa://30711 (96.67), maa://30768 (100.0)</t>
+          <t>maa://30711 (96.72), maa://30768 (100.0)</t>
         </is>
       </c>
       <c r="U31" s="1" t="n"/>
@@ -4581,7 +4581,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.17), maa://36667 (97.83), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.21), maa://36667 (97.83), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4629,7 +4629,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.45), maa://41108 (88.0), maa://41238 (97.3), maa://45523 (100.0)</t>
+          <t>maa://42859 (96.5), maa://41108 (88.0), maa://41238 (97.35), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4873,7 +4873,7 @@
       </c>
       <c r="P34" s="2" t="inlineStr">
         <is>
-          <t>maa://48817 (92.59)</t>
+          <t>maa://48817 (93.1)</t>
         </is>
       </c>
       <c r="Q34" s="1" t="n"/>
@@ -4889,7 +4889,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (92.8)</t>
+          <t>maa://24526 (92.45)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4937,7 +4937,7 @@
       </c>
       <c r="AF34" s="2" t="inlineStr">
         <is>
-          <t>*maa://32650 (77.27)</t>
+          <t>*maa://32650 (78.26)</t>
         </is>
       </c>
       <c r="AG34" s="1" t="n"/>
@@ -5215,7 +5215,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (97.79), *maa://47069 (75.0), maa://45789 (100.0)</t>
+          <t>maa://45718 (97.8), *maa://47069 (76.47), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5348,7 +5348,7 @@
       </c>
       <c r="T38" s="2" t="inlineStr">
         <is>
-          <t>maa://30713 (97.06)</t>
+          <t>maa://30713 (97.14)</t>
         </is>
       </c>
       <c r="U38" s="1" t="n"/>
@@ -5380,7 +5380,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.73)</t>
+          <t>maa://36697 (86.84)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5401,7 +5401,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (89.22), maa://25199 (85.09), maa://30434 (91.49), *maa://45059 (80.0), ***maa://25036 (18.52), *maa://44165 (66.67)</t>
+          <t>maa://36670 (89.22), maa://25199 (85.09), maa://30434 (91.67), maa://45059 (80.77), ***maa://25036 (18.52), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.82), maa://47093 (100.0)</t>
+          <t>maa://24709 (91.88), maa://47093 (100.0)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5449,7 +5449,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>*maa://45788 (79.25), maa://47079 (92.31), *maa://45790 (75.0)</t>
+          <t>*maa://45788 (78.5), maa://47079 (92.68), *maa://45790 (70.59)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5534,7 +5534,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.33), maa://21386 (95.79), maa://36664 (89.47), maa://45550 (87.5)</t>
+          <t>maa://23278 (95.03), maa://21386 (95.79), maa://36664 (89.47), maa://45550 (87.5)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5826,7 +5826,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (98.09), maa://27728 (96.12)</t>
+          <t>maa://29768 (98.11), maa://27728 (96.12)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5895,7 +5895,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.82), maa://30807 (95.71), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (88.46)</t>
+          <t>maa://21229 (84.9), maa://30807 (95.71), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (88.89)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5948,7 +5948,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.12), maa://43901 (94.29)</t>
+          <t>maa://35931 (92.15), maa://43901 (94.29)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6001,7 +6001,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.57), maa://29661 (97.37), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.58), maa://29661 (97.37), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6123,7 +6123,7 @@
       </c>
       <c r="P49" s="2" t="inlineStr">
         <is>
-          <t>*maa://39643 (65.71)</t>
+          <t>*maa://39643 (62.16)</t>
         </is>
       </c>
       <c r="Q49" s="1" t="n"/>
@@ -6310,7 +6310,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.38), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.4), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6362,7 +6362,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.35)</t>
+          <t>maa://32532 (92.42)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6434,7 +6434,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://31270 (94.81), maa://27746 (82.46)</t>
+          <t>maa://31270 (94.12), maa://27746 (82.61)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6524,7 +6524,7 @@
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>maa://44405 (84.38)</t>
+          <t>maa://44405 (84.85)</t>
         </is>
       </c>
       <c r="I64" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#182)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.65), maa://25390 (95.96), maa://36681 (87.5)</t>
+          <t>maa://24702 (94.65), maa://25390 (96.0), maa://36681 (87.5)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.17), *maa://30515 (70.48), maa://39402 (93.42), *maa://34787 (72.5), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.17), *maa://30515 (70.48), maa://39402 (93.67), *maa://34787 (72.5), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.53), maa://36684 (94.57), ***maa://22731 (6.25)</t>
+          <t>maa://21246 (91.25), maa://36684 (93.23), ***maa://22731 (6.25)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (91.27), ***maa://21730 (27.27), ***maa://39501 (13.89), **maa://36675 (50.0)</t>
+          <t>maa://25251 (91.34), ***maa://21730 (26.92), ***maa://39501 (13.16), **maa://36675 (50.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://40192 (97.06), maa://36987 (96.15), maa://39849 (88.89)</t>
+          <t>maa://40192 (97.3), maa://36987 (96.15), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.65), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.25), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (63.94), maa://20276 (86.96), *maa://22749 (80.0)</t>
+          <t>*maa://22880 (63.94), maa://20276 (87.03), *maa://22749 (80.0)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.51), maa://26254 (96.77), **maa://22738 (50.0)</t>
+          <t>maa://21249 (94.19), maa://26254 (96.97), **maa://22738 (50.0)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (90.16), **maa://20790 (43.48), ***maa://37170 (15.94), maa://45854 (87.8)</t>
+          <t>maa://24617 (90.24), **maa://20790 (43.48), maa://45854 (88.89), ***maa://37170 (17.14)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (83.99), maa://27484 (96.75), maa://27480 (83.33)</t>
+          <t>maa://27396 (84.04), maa://27484 (96.0), maa://27480 (83.33)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.89), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.96), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -967,7 +967,7 @@
       </c>
       <c r="P4" s="2" t="inlineStr">
         <is>
-          <t>maa://49983 (94.44), maa://50121 (100.0)</t>
+          <t>maa://49983 (91.67), *maa://50121 (80.0)</t>
         </is>
       </c>
       <c r="Q4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (95.87), maa://27295 (87.18), maa://22754 (90.41), *maa://31008 (79.07), *maa://21746 (55.81)</t>
+          <t>maa://32509 (95.87), maa://27295 (87.18), maa://22754 (90.41), *maa://31008 (79.07), *maa://21746 (54.55)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.54), ***maa://31785 (22.22), maa://43217 (90.8), ***maa://36683 (29.79)</t>
+          <t>**maa://32495 (48.73), ***maa://31785 (22.22), maa://43217 (90.91), ***maa://36683 (29.79)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1026,12 +1026,12 @@
       </c>
       <c r="AE4" s="1" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (64.71), *maa://39394 (65.38), ***maa://26209 (13.04), maa://48095 (100.0)</t>
+          <t>*maa://30062 (65.38), *maa://39394 (65.38), ***maa://26209 (13.04)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.92), maa://22744 (81.48)</t>
+          <t>maa://21245 (85.04), maa://22744 (81.48)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="P5" s="2" t="inlineStr">
         <is>
-          <t>maa://21919 (96.61), *maa://21281 (80.0)</t>
+          <t>maa://21919 (96.72), *maa://21281 (80.0)</t>
         </is>
       </c>
       <c r="Q5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (95.52)</t>
+          <t>maa://42407 (94.12)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="P6" s="2" t="inlineStr">
         <is>
-          <t>maa://31836 (93.33), maa://30381 (93.75)</t>
+          <t>maa://31836 (93.33), maa://30381 (94.12)</t>
         </is>
       </c>
       <c r="Q6" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (92.62), maa://24957 (97.78)</t>
+          <t>maa://28624 (92.68), maa://24957 (97.78)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.83), *maa://22758 (76.32)</t>
+          <t>maa://22399 (95.86), *maa://22758 (76.62)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.04.17 13:19:49</t>
+          <t>更新日期：2025.04.24 13:20:31</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (83.61), *maa://21916 (62.12), maa://23252 (91.18), maa://37496 (96.97), **maa://22759 (45.45)</t>
+          <t>maa://32931 (83.74), *maa://21916 (62.12), maa://23252 (91.18), maa://37496 (97.06), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (96.11)</t>
+          <t>maa://21411 (96.18)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>maa://22765 (91.67), *maa://21915 (68.97)</t>
+          <t>maa://22765 (90.72), *maa://21915 (70.97)</t>
         </is>
       </c>
       <c r="E9" s="1" t="n"/>
@@ -1607,7 +1607,7 @@
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>maa://22762 (92.55), maa://39552 (83.33)</t>
+          <t>maa://22762 (92.63), maa://39552 (83.33)</t>
         </is>
       </c>
       <c r="M9" s="1" t="n"/>
@@ -1655,7 +1655,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (98.01)</t>
+          <t>maa://26223 (98.05)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.3), **maa://39938 (46.67), **maa://27377 (42.86), ***maa://25174 (19.05), *maa://45044 (66.67), maa://40166 (96.67)</t>
+          <t>maa://28711 (87.4), **maa://39938 (46.88), **maa://27377 (42.86), *maa://45044 (66.67), ***maa://25174 (19.05), maa://40166 (96.97)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (87.88), *maa://22865 (51.85)</t>
+          <t>maa://26206 (88.32), *maa://22865 (51.85)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.65), ***maa://39951 (12.7), ***maa://34206 (22.22), *maa://45271 (54.17), ***maa://39243 (25.0)</t>
+          <t>***maa://25695 (18.65), ***maa://39951 (12.5), ***maa://34206 (22.22), *maa://45271 (56.86), ***maa://39243 (25.0)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1721,7 +1721,7 @@
       </c>
       <c r="H10" s="2" t="inlineStr">
         <is>
-          <t>maa://32651 (94.44)</t>
+          <t>maa://32651 (94.74)</t>
         </is>
       </c>
       <c r="I10" s="1" t="n"/>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (89.41), maa://36669 (83.33), *maa://23264 (61.82)</t>
+          <t>maa://28977 (89.53), maa://36669 (83.33), *maa://23264 (60.71)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1769,7 +1769,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.24), maa://22755 (88.03), **maa://22756 (40.91), ***maa://21737 (10.45)</t>
+          <t>maa://27395 (96.26), maa://22755 (88.33), **maa://22756 (40.91), ***maa://21737 (10.45)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.8), maa://45828 (92.0), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.8), maa://45828 (92.86), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (54.0), *maa://22733 (62.16), **maa://22761 (50.0)</t>
+          <t>*maa://25021 (53.47), *maa://22733 (62.16), **maa://22761 (50.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1835,7 +1835,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.26)</t>
+          <t>maa://36707 (99.28)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -1867,7 +1867,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (88.79)</t>
+          <t>maa://21287 (88.89)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.73), maa://22501 (97.96), maa://45521 (88.0)</t>
+          <t>maa://22747 (92.77), maa://22501 (98.0), maa://45521 (88.46)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.88)</t>
+          <t>maa://36713 (97.91)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1931,7 +1931,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://29912 (97.4), maa://22516 (88.37), *maa://20794 (51.47)</t>
+          <t>maa://29912 (97.44), maa://22516 (87.36), *maa://20794 (52.86)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (90.17), **maa://45826 (33.33)</t>
+          <t>maa://21867 (90.29), **maa://45826 (33.33)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2045,7 +2045,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (90.86), *maa://21485 (74.83), maa://37962 (91.84)</t>
+          <t>maa://22753 (91.1), *maa://21485 (75.0), maa://37962 (92.31)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.56), maa://36677 (94.2), maa://39872 (92.31)</t>
+          <t>maa://23669 (95.58), maa://36677 (94.44), maa://39872 (92.31)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.21), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (78.48), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.33), maa://36673 (92.68), maa://25001 (85.92)</t>
+          <t>maa://24999 (92.41), maa://36673 (92.77), maa://25001 (85.92)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2111,7 +2111,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.33), **maa://22728 (46.67)</t>
+          <t>*maa://21248 (73.56), **maa://22728 (46.67)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2207,7 +2207,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (34.69), maa://39883 (90.36), *maa://39885 (53.12)</t>
+          <t>**maa://22737 (35.57), maa://39883 (90.0), *maa://39885 (51.52)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2257,7 +2257,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://39841 (94.49), maa://26245 (96.89), maa://21288 (96.3), maa://36682 (97.5)</t>
+          <t>maa://39841 (94.74), maa://26245 (96.89), maa://21288 (96.3), maa://36682 (97.56)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2273,7 +2273,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.77), maa://20107 (87.1), maa://22772 (100.0), **maa://22745 (50.0)</t>
+          <t>maa://23250 (98.77), maa://20107 (87.1), maa://22772 (100.0), *maa://22745 (66.67)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2289,7 +2289,7 @@
       </c>
       <c r="T14" s="2" t="inlineStr">
         <is>
-          <t>maa://22521 (94.55), maa://42751 (100.0)</t>
+          <t>maa://22521 (94.64), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="1" t="n"/>
@@ -2355,7 +2355,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.73), maa://22734 (84.17), *maa://30808 (64.18), *maa://36048 (56.0), maa://45058 (93.75)</t>
+          <t>*maa://22743 (78.83), maa://22734 (84.3), *maa://30808 (64.18), *maa://36048 (59.26), maa://45058 (93.75)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (87.67), maa://21478 (89.74)</t>
+          <t>maa://24304 (87.72), maa://21478 (89.74)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2403,7 +2403,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (90.75), *maa://22727 (70.0)</t>
+          <t>maa://24762 (90.8), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.52), *maa://36666 (78.05), *maa://22766 (68.33)</t>
+          <t>maa://21364 (80.52), *maa://36666 (78.74), *maa://22766 (68.33)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2485,7 +2485,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.48), maa://36679 (94.55), maa://37650 (97.73)</t>
+          <t>maa://21441 (96.49), maa://37650 (97.78), maa://36679 (94.55)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2533,7 +2533,7 @@
       </c>
       <c r="P16" s="2" t="inlineStr">
         <is>
-          <t>maa://28504 (92.06)</t>
+          <t>maa://28504 (92.19)</t>
         </is>
       </c>
       <c r="Q16" s="1" t="n"/>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.08), *maa://28648 (71.23), *maa://36674 (80.0)</t>
+          <t>maa://22729 (94.19), *maa://28648 (71.23), maa://36674 (80.36)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2581,7 +2581,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.24)</t>
+          <t>maa://26228 (95.33)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (66.06), maa://27755 (93.68)</t>
+          <t>*maa://23911 (66.36), maa://27755 (93.68)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2631,7 +2631,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (88.89), maa://39599 (83.87)</t>
+          <t>maa://22430 (89.16), maa://39599 (84.62)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2663,7 +2663,7 @@
       </c>
       <c r="P17" s="2" t="inlineStr">
         <is>
-          <t>maa://23890 (81.13), *maa://24940 (67.86)</t>
+          <t>maa://23890 (81.31), *maa://24940 (67.86)</t>
         </is>
       </c>
       <c r="Q17" s="1" t="n"/>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (88.12)</t>
+          <t>maa://24421 (87.79)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2777,7 +2777,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (91.4), *maa://22732 (51.52)</t>
+          <t>maa://22466 (91.58), *maa://22732 (51.0)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="X18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (96.97), maa://22741 (87.5)</t>
+          <t>maa://21917 (97.0), maa://22741 (87.5)</t>
         </is>
       </c>
       <c r="Y18" s="1" t="n"/>
@@ -2857,7 +2857,7 @@
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (59.76), **maa://29784 (50.0), *maa://47854 (75.0)</t>
+          <t>*maa://24313 (60.0), **maa://29784 (50.0), *maa://47854 (80.0)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -2907,7 +2907,7 @@
       </c>
       <c r="L19" s="2" t="inlineStr">
         <is>
-          <t>maa://39347 (93.33)</t>
+          <t>maa://39347 (93.75)</t>
         </is>
       </c>
       <c r="M19" s="1" t="n"/>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (99.22)</t>
+          <t>maa://24386 (99.24)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -2971,7 +2971,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (66.37), *maa://36668 (58.02)</t>
+          <t>*maa://30709 (66.67), *maa://36668 (58.02)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.86), maa://25198 (93.86), *maa://20795 (50.77), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.96), maa://25198 (93.91), *maa://20795 (50.77), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (89.57), ***maa://43283 (25.0)</t>
+          <t>maa://22864 (89.88), ***maa://43283 (25.0)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.71)</t>
+          <t>maa://41331 (85.64)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3085,7 +3085,7 @@
       </c>
       <c r="X20" s="2" t="inlineStr">
         <is>
-          <t>*maa://49976 (80.0), maa://50085 (83.33)</t>
+          <t>maa://49976 (84.09), maa://50085 (92.86)</t>
         </is>
       </c>
       <c r="Y20" s="1" t="n"/>
@@ -3215,7 +3215,7 @@
       </c>
       <c r="X21" s="2" t="inlineStr">
         <is>
-          <t>maa://20110 (86.76), maa://34946 (91.67)</t>
+          <t>maa://20110 (86.76), maa://34946 (92.0)</t>
         </is>
       </c>
       <c r="Y21" s="1" t="n"/>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (81.79), ***maa://23820 (30.0)</t>
+          <t>maa://21443 (82.03), ***maa://23820 (30.0)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (92.64), *maa://22432 (77.78)</t>
+          <t>maa://22524 (92.67), *maa://22432 (78.49)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>maa://25236 (95.79), **maa://21678 (48.94), **maa://22735 (42.86)</t>
+          <t>maa://25236 (95.88), **maa://21678 (48.94), **maa://22735 (42.86)</t>
         </is>
       </c>
       <c r="I22" s="1" t="n"/>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>*maa://27127 (77.42), *maa://22751 (71.01)</t>
+          <t>*maa://27127 (77.6), *maa://22751 (71.43)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.68), *maa://37649 (66.67)</t>
+          <t>maa://21282 (98.68), *maa://37649 (67.74)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3395,7 +3395,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.0), **maa://41753 (50.0)</t>
+          <t>***maa://28036 (27.63), **maa://41753 (50.0)</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.9), maa://39875 (94.59)</t>
+          <t>maa://39756 (95.58), maa://39875 (94.67)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3443,7 +3443,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (92.08), *maa://29748 (76.52), ***maa://29785 (17.39), *maa://37566 (77.5)</t>
+          <t>maa://30587 (91.67), *maa://29748 (76.12), ***maa://29785 (17.39), *maa://37566 (78.05)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3459,7 +3459,7 @@
       </c>
       <c r="T23" s="2" t="inlineStr">
         <is>
-          <t>maa://24387 (82.05), maa://31212 (93.94)</t>
+          <t>maa://31212 (93.94), maa://24387 (82.05)</t>
         </is>
       </c>
       <c r="U23" s="1" t="n"/>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.52), *maa://46650 (58.33)</t>
+          <t>*maa://24368 (78.48), *maa://46650 (57.14)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3605,7 +3605,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (83.46), maa://23504 (93.51), **maa://22892 (40.67), *maa://25141 (77.27), *maa://36663 (78.31), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (83.27), maa://23504 (93.35), **maa://22892 (40.79), *maa://25141 (76.69), *maa://36663 (78.16), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3637,7 +3637,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (84.8), *maa://36672 (79.31), maa://29910 (93.44), **maa://21440 (35.71), maa://45831 (87.5)</t>
+          <t>maa://22523 (84.47), *maa://36672 (79.31), maa://29910 (93.55), **maa://21440 (35.71), maa://45831 (90.91)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3655,7 +3655,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.34)</t>
+          <t>maa://29753 (95.42)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3671,7 +3671,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (72.25), *maa://25311 (74.31), ***maa://22725 (4.76), *maa://45047 (66.67)</t>
+          <t>*maa://29063 (72.57), *maa://25311 (74.31), ***maa://22725 (4.76), *maa://45047 (66.67)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3719,7 +3719,7 @@
       </c>
       <c r="T25" s="2" t="inlineStr">
         <is>
-          <t>maa://20109 (92.31), maa://22545 (100.0), *maa://42915 (75.0)</t>
+          <t>maa://20109 (92.35), maa://22545 (100.0), *maa://42915 (75.0)</t>
         </is>
       </c>
       <c r="U25" s="1" t="n"/>
@@ -3735,7 +3735,7 @@
       </c>
       <c r="X25" s="2" t="inlineStr">
         <is>
-          <t>maa://29890 (80.39)</t>
+          <t>maa://29890 (80.77)</t>
         </is>
       </c>
       <c r="Y25" s="1" t="n"/>
@@ -3751,7 +3751,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (88.62), maa://24516 (80.22), maa://26001 (87.5)</t>
+          <t>maa://31215 (88.71), maa://24516 (80.22), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3767,7 +3767,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.4), maa://24621 (96.97), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
+          <t>maa://20108 (96.43), maa://24621 (96.97), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3833,7 +3833,7 @@
       </c>
       <c r="P26" s="2" t="inlineStr">
         <is>
-          <t>*maa://30968 (65.0), maa://39870 (90.91)</t>
+          <t>*maa://30968 (65.0), maa://39870 (91.67)</t>
         </is>
       </c>
       <c r="Q26" s="1" t="n"/>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (95.04)</t>
+          <t>maa://42235 (95.16)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3897,7 +3897,7 @@
       </c>
       <c r="AF26" s="2" t="inlineStr">
         <is>
-          <t>maa://30511 (82.22), *maa://29760 (56.25)</t>
+          <t>*maa://30511 (78.72), *maa://29760 (56.25)</t>
         </is>
       </c>
       <c r="AG26" s="1" t="n"/>
@@ -3931,7 +3931,7 @@
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (47.37), *maa://39601 (80.0), maa://34494 (97.14), **maa://36665 (50.0)</t>
+          <t>**maa://21283 (47.37), *maa://39601 (76.19), maa://34494 (97.14), **maa://36665 (50.0)</t>
         </is>
       </c>
       <c r="I27" s="1" t="n"/>
@@ -4045,7 +4045,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (91.03), maa://25725 (84.62)</t>
+          <t>maa://24465 (90.92), maa://25725 (84.62)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (90.93), maa://41749 (91.26), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (91.08), maa://41749 (91.43), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4157,7 +4157,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.27), *maa://36701 (66.67)</t>
+          <t>maa://36660 (92.41), *maa://36701 (67.74)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4175,7 +4175,7 @@
       </c>
       <c r="D29" s="2" t="inlineStr">
         <is>
-          <t>maa://31694 (98.21)</t>
+          <t>maa://31694 (98.25)</t>
         </is>
       </c>
       <c r="E29" s="1" t="n"/>
@@ -4191,7 +4191,7 @@
       </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>*maa://25175 (66.07)</t>
+          <t>*maa://25175 (64.91)</t>
         </is>
       </c>
       <c r="I29" s="1" t="n"/>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.66), maa://28440 (81.36), maa://31400 (98.84), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.71), maa://28440 (81.82), maa://31400 (98.84), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4223,7 +4223,7 @@
       </c>
       <c r="P29" s="2" t="inlineStr">
         <is>
-          <t>*maa://23168 (58.06), *maa://30050 (56.76)</t>
+          <t>*maa://23168 (58.73), *maa://30050 (53.85)</t>
         </is>
       </c>
       <c r="Q29" s="1" t="n"/>
@@ -4287,7 +4287,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.01), maa://42865 (81.08), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (69.01), maa://42865 (82.05), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4305,7 +4305,7 @@
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>maa://45792 (90.91)</t>
+          <t>maa://45792 (91.3)</t>
         </is>
       </c>
       <c r="E30" s="1" t="n"/>
@@ -4353,7 +4353,7 @@
       </c>
       <c r="P30" s="2" t="inlineStr">
         <is>
-          <t>maa://21442 (99.13)</t>
+          <t>maa://21442 (98.71)</t>
         </is>
       </c>
       <c r="Q30" s="1" t="n"/>
@@ -4401,7 +4401,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.28), maa://45822 (100.0), *maa://45045 (80.0)</t>
+          <t>maa://42979 (97.35), maa://45822 (100.0), *maa://45045 (80.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4467,7 +4467,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.51), maa://36258 (85.27), *maa://43904 (76.92)</t>
+          <t>maa://35926 (93.55), maa://36258 (85.71), *maa://43904 (76.92)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4581,7 +4581,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.21), maa://36667 (97.83), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.27), maa://36667 (97.92), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4629,7 +4629,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.5), maa://41108 (88.0), maa://41238 (97.35), maa://45523 (100.0)</t>
+          <t>maa://42859 (96.69), maa://41108 (88.0), maa://41238 (97.44), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4711,7 +4711,7 @@
       </c>
       <c r="H33" s="2" t="inlineStr">
         <is>
-          <t>**maa://39351 (33.33)</t>
+          <t>**maa://39351 (42.86)</t>
         </is>
       </c>
       <c r="I33" s="1" t="n"/>
@@ -4743,7 +4743,7 @@
       </c>
       <c r="P33" s="2" t="inlineStr">
         <is>
-          <t>maa://21956 (80.92), *maa://22730 (76.67)</t>
+          <t>maa://21956 (81.17), *maa://22730 (76.67)</t>
         </is>
       </c>
       <c r="Q33" s="1" t="n"/>
@@ -4759,7 +4759,7 @@
       </c>
       <c r="T33" s="2" t="inlineStr">
         <is>
-          <t>maa://45558 (90.91)</t>
+          <t>maa://45558 (91.67)</t>
         </is>
       </c>
       <c r="U33" s="1" t="n"/>
@@ -4873,7 +4873,7 @@
       </c>
       <c r="P34" s="2" t="inlineStr">
         <is>
-          <t>maa://48817 (93.1)</t>
+          <t>maa://48817 (93.94)</t>
         </is>
       </c>
       <c r="Q34" s="1" t="n"/>
@@ -4889,7 +4889,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (92.45)</t>
+          <t>maa://24526 (92.16)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4987,7 +4987,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.74)</t>
+          <t>maa://41296 (96.83)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5019,7 +5019,7 @@
       </c>
       <c r="T35" s="2" t="inlineStr">
         <is>
-          <t>maa://24842 (94.34)</t>
+          <t>maa://24842 (94.44)</t>
         </is>
       </c>
       <c r="U35" s="1" t="n"/>
@@ -5215,7 +5215,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (97.8), *maa://47069 (76.47), maa://45789 (100.0)</t>
+          <t>maa://45718 (97.91), *maa://47069 (76.47), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5231,7 +5231,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.69), *maa://21239 (69.23)</t>
+          <t>maa://21280 (89.73), *maa://21239 (69.23)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5380,7 +5380,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (86.84)</t>
+          <t>maa://36697 (87.23)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5401,7 +5401,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (89.22), maa://25199 (85.09), maa://30434 (91.67), maa://45059 (80.77), ***maa://25036 (18.52), *maa://44165 (66.67)</t>
+          <t>maa://36670 (89.32), maa://25199 (85.22), maa://30434 (92.08), maa://45059 (81.48), ***maa://25036 (18.52), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.88), maa://47093 (100.0)</t>
+          <t>maa://24709 (91.93), maa://47093 (100.0)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5449,7 +5449,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>*maa://45788 (78.5), maa://47079 (92.68), *maa://45790 (70.59)</t>
+          <t>*maa://45788 (78.5), maa://47079 (93.48), *maa://45790 (70.59)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5534,7 +5534,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.03), maa://21386 (95.79), maa://36664 (89.47), maa://45550 (87.5)</t>
+          <t>maa://23278 (95.06), maa://21386 (95.79), maa://36664 (89.47), maa://45550 (87.5)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5757,7 +5757,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (91.84), maa://21284 (86.0)</t>
+          <t>maa://22525 (91.28), maa://21284 (86.0)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5826,7 +5826,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (98.11), maa://27728 (96.12)</t>
+          <t>maa://29768 (98.12), maa://27728 (96.12)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5895,7 +5895,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.9), maa://30807 (95.71), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (88.89)</t>
+          <t>maa://21229 (84.9), maa://30807 (95.77), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (89.29)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5911,7 +5911,7 @@
       </c>
       <c r="P45" s="2" t="inlineStr">
         <is>
-          <t>*maa://36237 (72.22)</t>
+          <t>*maa://36237 (73.68)</t>
         </is>
       </c>
       <c r="Q45" s="1" t="n"/>
@@ -5927,7 +5927,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (38.46)</t>
+          <t>**maa://39364 (37.5)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -5948,7 +5948,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.15), maa://43901 (94.29)</t>
+          <t>maa://35931 (92.24), maa://43901 (94.74)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6001,7 +6001,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.58), maa://29661 (97.37), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.65), maa://29661 (97.44), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6123,7 +6123,7 @@
       </c>
       <c r="P49" s="2" t="inlineStr">
         <is>
-          <t>*maa://39643 (62.16)</t>
+          <t>*maa://39643 (63.16)</t>
         </is>
       </c>
       <c r="Q49" s="1" t="n"/>
@@ -6310,7 +6310,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.4), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.48), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6362,7 +6362,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.42)</t>
+          <t>maa://32532 (92.58)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6416,7 +6416,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (57.78)</t>
+          <t>*maa://37964 (56.52)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>
@@ -6434,7 +6434,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://31270 (94.12), maa://27746 (82.61)</t>
+          <t>maa://31270 (94.16), maa://27746 (82.76)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#183)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.65), maa://25390 (96.0), maa://36681 (87.5)</t>
+          <t>maa://24702 (94.68), maa://25390 (96.0), maa://36681 (86.42)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.17), *maa://30515 (70.48), maa://39402 (93.67), *maa://34787 (72.5), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.17), *maa://30515 (70.48), maa://39402 (93.98), *maa://34787 (72.84), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.01), *maa://20791 (62.03)</t>
+          <t>maa://22742 (91.11), *maa://20791 (62.03)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.25), maa://36684 (93.23), ***maa://22731 (6.25)</t>
+          <t>maa://21246 (91.36), maa://36684 (93.28), ***maa://22731 (6.25)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (91.34), ***maa://21730 (26.92), ***maa://39501 (13.16), **maa://36675 (50.0)</t>
+          <t>maa://25251 (91.41), ***maa://21730 (27.85), ***maa://39501 (12.5), **maa://36675 (50.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://40192 (97.3), maa://36987 (96.15), maa://39849 (88.89)</t>
+          <t>maa://40192 (96.0), maa://36987 (96.15), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.25), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.27), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (63.94), maa://20276 (87.03), *maa://22749 (80.0)</t>
+          <t>*maa://22880 (63.64), maa://20276 (87.3), *maa://22749 (80.0)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.19), maa://26254 (96.97), **maa://22738 (50.0)</t>
+          <t>maa://21249 (94.27), maa://26254 (96.97), **maa://22738 (50.0)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (90.24), **maa://20790 (43.48), maa://45854 (88.89), ***maa://37170 (17.14)</t>
+          <t>maa://24617 (90.32), **maa://20790 (43.48), maa://45854 (88.24), ***maa://37170 (17.14)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.04), maa://27484 (96.0), maa://27480 (83.33)</t>
+          <t>maa://27396 (84.13), maa://27484 (96.03), maa://27480 (83.33)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (95.06)</t>
+          <t>maa://24390 (95.18)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -901,7 +901,7 @@
       </c>
       <c r="AF3" s="2" t="inlineStr">
         <is>
-          <t>*maa://21289 (72.41)</t>
+          <t>*maa://21289 (74.19)</t>
         </is>
       </c>
       <c r="AG3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.96), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.51), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -967,7 +967,7 @@
       </c>
       <c r="P4" s="2" t="inlineStr">
         <is>
-          <t>maa://49983 (91.67), *maa://50121 (80.0)</t>
+          <t>maa://49983 (92.86), maa://50121 (86.67)</t>
         </is>
       </c>
       <c r="Q4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (95.87), maa://27295 (87.18), maa://22754 (90.41), *maa://31008 (79.07), *maa://21746 (54.55)</t>
+          <t>maa://32509 (95.12), maa://27295 (87.5), maa://22754 (89.19), *maa://31008 (79.07), *maa://21746 (54.55)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.73), ***maa://31785 (22.22), maa://43217 (90.91), ***maa://36683 (29.79)</t>
+          <t>**maa://32495 (48.73), ***maa://31785 (22.22), maa://43217 (91.11), ***maa://36683 (29.79)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (85.04), maa://22744 (81.48)</t>
+          <t>maa://21245 (84.82), maa://22744 (81.48)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="AB5" s="2" t="inlineStr">
         <is>
-          <t>*maa://29863 (66.67), ***maa://22752 (12.5), **maa://26013 (37.5)</t>
+          <t>*maa://29863 (65.0), ***maa://22752 (12.5), **maa://26013 (37.5)</t>
         </is>
       </c>
       <c r="AC5" s="1" t="n"/>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>maa://24839 (99.04)</t>
+          <t>maa://24839 (99.05)</t>
         </is>
       </c>
       <c r="M6" s="1" t="n"/>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="P6" s="2" t="inlineStr">
         <is>
-          <t>maa://31836 (93.33), maa://30381 (94.12)</t>
+          <t>maa://31836 (93.55), maa://30381 (94.12)</t>
         </is>
       </c>
       <c r="Q6" s="1" t="n"/>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="T6" s="2" t="inlineStr">
         <is>
-          <t>maa://37411 (88.24)</t>
+          <t>maa://37411 (89.47)</t>
         </is>
       </c>
       <c r="U6" s="1" t="n"/>
@@ -1280,7 +1280,7 @@
       </c>
       <c r="AB6" s="2" t="inlineStr">
         <is>
-          <t>maa://22739 (91.38)</t>
+          <t>maa://22739 (91.53)</t>
         </is>
       </c>
       <c r="AC6" s="1" t="n"/>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="T7" s="2" t="inlineStr">
         <is>
-          <t>maa://21291 (86.54)</t>
+          <t>maa://21291 (84.91)</t>
         </is>
       </c>
       <c r="U7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.86), *maa://22758 (76.62)</t>
+          <t>maa://22399 (95.88), *maa://22758 (76.92)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.04.24 13:20:31</t>
+          <t>更新日期：2025.05.01 13:20:46</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>*maa://21476 (74.07), *maa://39431 (60.0), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (74.55), *maa://39431 (60.0), *maa://37551 (57.14)</t>
         </is>
       </c>
       <c r="E8" s="1" t="n"/>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24371 (56.0)</t>
+          <t>*maa://24371 (56.58)</t>
         </is>
       </c>
       <c r="I8" s="1" t="n"/>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (83.74), *maa://21916 (62.12), maa://23252 (91.18), maa://37496 (97.06), **maa://22759 (45.45)</t>
+          <t>maa://32931 (83.87), *maa://21916 (62.12), maa://23252 (91.18), maa://37496 (97.06), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (96.18)</t>
+          <t>maa://21411 (96.23)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="AF8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24479 (78.89), *maa://21990 (51.85)</t>
+          <t>*maa://24479 (79.12), *maa://21990 (51.85)</t>
         </is>
       </c>
       <c r="AG8" s="1" t="n"/>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>maa://22765 (90.72), *maa://21915 (70.97)</t>
+          <t>maa://22765 (90.82), *maa://21915 (70.97)</t>
         </is>
       </c>
       <c r="E9" s="1" t="n"/>
@@ -1590,10 +1590,14 @@
       </c>
       <c r="G9" s="1" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H9" s="2" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H9" s="2" t="inlineStr">
+        <is>
+          <t>**maa://47450 (33.33)</t>
+        </is>
+      </c>
       <c r="I9" s="1" t="n"/>
       <c r="J9" s="1" t="inlineStr">
         <is>
@@ -1607,7 +1611,7 @@
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>maa://22762 (92.63), maa://39552 (83.33)</t>
+          <t>maa://22762 (92.71), maa://39552 (83.33)</t>
         </is>
       </c>
       <c r="M9" s="1" t="n"/>
@@ -1623,7 +1627,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (83.18)</t>
+          <t>maa://22736 (83.33)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1639,7 +1643,7 @@
       </c>
       <c r="T9" s="2" t="inlineStr">
         <is>
-          <t>**maa://22866 (30.19), maa://26222 (98.15)</t>
+          <t>**maa://22866 (30.19), maa://26222 (98.18)</t>
         </is>
       </c>
       <c r="U9" s="1" t="n"/>
@@ -1671,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.4), **maa://39938 (46.88), **maa://27377 (42.86), *maa://45044 (66.67), ***maa://25174 (19.05), maa://40166 (96.97)</t>
+          <t>maa://28711 (87.4), **maa://39938 (46.88), *maa://45044 (66.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (96.97)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1687,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (88.32), *maa://22865 (51.85)</t>
+          <t>maa://26206 (88.89), *maa://22865 (51.85)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1705,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.65), ***maa://39951 (12.5), ***maa://34206 (22.22), *maa://45271 (56.86), ***maa://39243 (25.0)</t>
+          <t>***maa://25695 (18.56), ***maa://39951 (11.94), ***maa://34206 (22.22), *maa://45271 (59.65), ***maa://39243 (25.0)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1753,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (89.53), maa://36669 (83.33), *maa://23264 (60.71)</t>
+          <t>maa://28977 (89.53), maa://36669 (83.67), *maa://23264 (60.71)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1769,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.26), maa://22755 (88.33), **maa://22756 (40.91), ***maa://21737 (10.45)</t>
+          <t>maa://27395 (96.28), maa://22755 (88.43), **maa://22756 (40.91), ***maa://21737 (10.45)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1835,7 +1839,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.28)</t>
+          <t>maa://36707 (99.3)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -1867,7 +1871,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (88.89)</t>
+          <t>maa://21287 (88.99)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1899,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.77), maa://22501 (98.0), maa://45521 (88.46)</t>
+          <t>maa://22747 (92.86), maa://22501 (98.0), maa://45521 (88.46)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1915,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.91)</t>
+          <t>maa://36713 (97.94)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1931,7 +1935,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://29912 (97.44), maa://22516 (87.36), *maa://20794 (52.86)</t>
+          <t>maa://29912 (97.47), maa://22516 (87.36), *maa://20794 (53.52)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -1947,7 +1951,7 @@
       </c>
       <c r="AF11" s="2" t="inlineStr">
         <is>
-          <t>maa://31203 (96.0)</t>
+          <t>maa://31203 (96.15)</t>
         </is>
       </c>
       <c r="AG11" s="1" t="n"/>
@@ -1981,7 +1985,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (90.29), **maa://45826 (33.33)</t>
+          <t>maa://21867 (90.29), ***maa://45826 (30.0)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2045,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.1), *maa://21485 (75.0), maa://37962 (92.31)</t>
+          <t>maa://22753 (91.33), *maa://21485 (75.17), maa://37962 (92.45)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2061,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.58), maa://36677 (94.44), maa://39872 (92.31)</t>
+          <t>maa://23669 (95.61), maa://36677 (94.59), maa://39872 (92.31)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2077,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.48), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (78.62), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2095,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.41), maa://36673 (92.77), maa://25001 (85.92)</t>
+          <t>maa://24999 (92.48), maa://36673 (92.86), maa://25001 (85.92)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2143,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (93.23), *maa://22583 (75.71), *maa://22500 (59.57), maa://48321 (100.0)</t>
+          <t>maa://22676 (93.28), *maa://22583 (76.06), *maa://22500 (59.57), maa://48321 (100.0)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2175,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>maa://34957 (81.4), **maa://22768 (50.0)</t>
+          <t>maa://34957 (82.02), **maa://22768 (50.0)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2207,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (35.57), maa://39883 (90.0), *maa://39885 (51.52)</t>
+          <t>**maa://22737 (37.66), maa://39883 (90.43), *maa://39885 (51.52)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2257,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://39841 (94.74), maa://26245 (96.89), maa://21288 (96.3), maa://36682 (97.56)</t>
+          <t>maa://39841 (94.81), maa://26245 (96.97), maa://21288 (96.3), maa://36682 (97.56)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2289,7 +2293,7 @@
       </c>
       <c r="T14" s="2" t="inlineStr">
         <is>
-          <t>maa://22521 (94.64), maa://42751 (100.0)</t>
+          <t>maa://22521 (94.74), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="1" t="n"/>
@@ -2355,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.83), maa://22734 (84.3), *maa://30808 (64.18), *maa://36048 (59.26), maa://45058 (93.75)</t>
+          <t>*maa://22743 (78.57), maa://22734 (84.43), *maa://30808 (64.18), *maa://36048 (60.71), maa://45058 (94.12)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2371,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (87.72), maa://21478 (89.74)</t>
+          <t>maa://24304 (87.34), maa://21478 (89.74)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2467,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.52), *maa://36666 (78.74), *maa://22766 (68.33)</t>
+          <t>maa://21364 (80.68), *maa://36666 (78.91), *maa://22766 (68.33)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2485,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.49), maa://37650 (97.78), maa://36679 (94.55)</t>
+          <t>maa://21441 (96.49), maa://37650 (97.87), maa://36679 (94.55)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2533,7 +2537,7 @@
       </c>
       <c r="P16" s="2" t="inlineStr">
         <is>
-          <t>maa://28504 (92.19)</t>
+          <t>maa://28504 (92.42)</t>
         </is>
       </c>
       <c r="Q16" s="1" t="n"/>
@@ -2549,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.19), *maa://28648 (71.23), maa://36674 (80.36)</t>
+          <t>maa://22729 (94.29), *maa://28648 (71.62), maa://36674 (80.7)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2597,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (66.36), maa://27755 (93.68)</t>
+          <t>*maa://23911 (66.67), maa://27755 (93.68)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2679,7 +2683,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>*maa://42324 (52.27)</t>
+          <t>*maa://42324 (53.33)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2727,7 +2731,7 @@
       </c>
       <c r="AF17" s="2" t="inlineStr">
         <is>
-          <t>maa://50136 (100.0)</t>
+          <t>maa://50136 (90.0)</t>
         </is>
       </c>
       <c r="AG17" s="1" t="n"/>
@@ -2745,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.67)</t>
+          <t>maa://24570 (96.68)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2761,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (87.79)</t>
+          <t>maa://24421 (87.55)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2777,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (91.58), *maa://22732 (51.0)</t>
+          <t>maa://22466 (91.62), *maa://22732 (50.5)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2971,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (66.67), *maa://36668 (58.02)</t>
+          <t>*maa://30709 (66.81), *maa://36668 (58.02)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3005,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.96), maa://25198 (93.91), *maa://20795 (50.77), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.53), maa://25198 (94.07), *maa://20795 (50.77), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3021,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (89.88), ***maa://43283 (25.0)</t>
+          <t>maa://22864 (90.06), ***maa://43283 (25.0)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3037,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.64)</t>
+          <t>maa://41331 (85.49)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3053,7 +3057,7 @@
       </c>
       <c r="P20" s="2" t="inlineStr">
         <is>
-          <t>maa://37442 (95.83)</t>
+          <t>maa://37442 (95.92)</t>
         </is>
       </c>
       <c r="Q20" s="1" t="n"/>
@@ -3085,7 +3089,7 @@
       </c>
       <c r="X20" s="2" t="inlineStr">
         <is>
-          <t>maa://49976 (84.09), maa://50085 (92.86)</t>
+          <t>maa://49976 (84.21), maa://50085 (88.57)</t>
         </is>
       </c>
       <c r="Y20" s="1" t="n"/>
@@ -3231,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (82.03), ***maa://23820 (30.0)</t>
+          <t>maa://21443 (82.16), ***maa://23820 (30.0)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3247,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (92.67), *maa://22432 (78.49)</t>
+          <t>maa://22524 (92.34), *maa://22432 (79.59)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3297,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>*maa://27127 (77.6), *maa://22751 (71.43)</t>
+          <t>*maa://27127 (78.12), *maa://22751 (71.43)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3427,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.58), maa://39875 (94.67)</t>
+          <t>maa://39756 (95.67), maa://39875 (94.67)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3443,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.67), *maa://29748 (76.12), ***maa://29785 (17.39), *maa://37566 (78.05)</t>
+          <t>maa://30587 (91.71), *maa://29748 (76.12), ***maa://29785 (17.39), *maa://37566 (76.19)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3525,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.48), *maa://46650 (57.14)</t>
+          <t>*maa://24368 (78.64), *maa://46650 (53.33)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3605,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (83.27), maa://23504 (93.35), **maa://22892 (40.79), *maa://25141 (76.69), *maa://36663 (78.16), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (83.7), maa://23504 (93.39), **maa://22892 (40.79), *maa://25141 (76.87), *maa://36663 (78.41), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3637,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (84.47), *maa://36672 (79.31), maa://29910 (93.55), **maa://21440 (35.71), maa://45831 (90.91)</t>
+          <t>maa://22523 (84.47), *maa://36672 (79.31), maa://29910 (93.55), **maa://21440 (35.71), maa://45831 (91.67)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3655,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.42)</t>
+          <t>maa://29753 (95.1)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3671,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (72.57), *maa://25311 (74.31), ***maa://22725 (4.76), *maa://45047 (66.67)</t>
+          <t>*maa://29063 (72.88), *maa://25311 (74.31), ***maa://22725 (4.76), *maa://45047 (66.67)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3703,7 +3707,7 @@
       </c>
       <c r="P25" s="2" t="inlineStr">
         <is>
-          <t>maa://24382 (93.75)</t>
+          <t>maa://24382 (93.94)</t>
         </is>
       </c>
       <c r="Q25" s="1" t="n"/>
@@ -3719,7 +3723,7 @@
       </c>
       <c r="T25" s="2" t="inlineStr">
         <is>
-          <t>maa://20109 (92.35), maa://22545 (100.0), *maa://42915 (75.0)</t>
+          <t>maa://20109 (92.39), maa://22545 (100.0), *maa://42915 (75.0)</t>
         </is>
       </c>
       <c r="U25" s="1" t="n"/>
@@ -3735,7 +3739,7 @@
       </c>
       <c r="X25" s="2" t="inlineStr">
         <is>
-          <t>maa://29890 (80.77)</t>
+          <t>maa://29890 (81.13)</t>
         </is>
       </c>
       <c r="Y25" s="1" t="n"/>
@@ -3751,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (88.71), maa://24516 (80.22), maa://26001 (87.5)</t>
+          <t>maa://31215 (88.89), maa://24516 (80.22), maa://26001 (87.5)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3767,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.43), maa://24621 (96.97), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
+          <t>maa://20108 (96.48), maa://24621 (96.97), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3881,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (95.16)</t>
+          <t>maa://42235 (95.24)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3897,7 +3901,7 @@
       </c>
       <c r="AF26" s="2" t="inlineStr">
         <is>
-          <t>*maa://30511 (78.72), *maa://29760 (56.25)</t>
+          <t>*maa://30511 (77.08), *maa://29760 (56.25)</t>
         </is>
       </c>
       <c r="AG26" s="1" t="n"/>
@@ -4027,7 +4031,7 @@
       </c>
       <c r="AF27" s="2" t="inlineStr">
         <is>
-          <t>maa://24023 (96.05)</t>
+          <t>maa://24023 (96.1)</t>
         </is>
       </c>
       <c r="AG27" s="1" t="n"/>
@@ -4045,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.92), maa://25725 (84.62)</t>
+          <t>maa://24465 (90.96), maa://25725 (84.62)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4125,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (91.08), maa://41749 (91.43), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (91.2), maa://41749 (92.04), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4157,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.41), *maa://36701 (67.74)</t>
+          <t>maa://36660 (92.47), *maa://36701 (67.74)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4207,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.71), maa://28440 (81.82), maa://31400 (98.84), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.77), maa://28440 (82.4), maa://31400 (98.84), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4223,7 +4227,7 @@
       </c>
       <c r="P29" s="2" t="inlineStr">
         <is>
-          <t>*maa://23168 (58.73), *maa://30050 (53.85)</t>
+          <t>*maa://23168 (57.81), *maa://30050 (53.85)</t>
         </is>
       </c>
       <c r="Q29" s="1" t="n"/>
@@ -4287,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.01), maa://42865 (82.05), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (69.01), maa://42865 (82.28), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4305,7 +4309,7 @@
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>maa://45792 (91.3)</t>
+          <t>maa://45792 (87.5)</t>
         </is>
       </c>
       <c r="E30" s="1" t="n"/>
@@ -4401,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.35), maa://45822 (100.0), *maa://45045 (80.0)</t>
+          <t>maa://42979 (97.38), maa://45822 (100.0), *maa://45045 (80.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4467,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.55), maa://36258 (85.71), *maa://43904 (76.92)</t>
+          <t>maa://35926 (93.59), maa://36258 (86.23), *maa://43904 (76.92)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4499,7 +4503,7 @@
       </c>
       <c r="T31" s="2" t="inlineStr">
         <is>
-          <t>maa://30711 (96.72), maa://30768 (100.0)</t>
+          <t>maa://30711 (96.83), maa://30768 (100.0)</t>
         </is>
       </c>
       <c r="U31" s="1" t="n"/>
@@ -4529,11 +4533,7 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AB31" s="2" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="AB31" s="2" t="inlineStr"/>
       <c r="AC31" s="1" t="n"/>
       <c r="AD31" s="1" t="inlineStr">
         <is>
@@ -4581,7 +4581,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.27), maa://36667 (97.92), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.33), maa://36667 (97.92), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4629,7 +4629,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.69), maa://41108 (88.0), maa://41238 (97.44), maa://45523 (100.0)</t>
+          <t>maa://42859 (96.82), maa://41108 (88.0), maa://41238 (97.54), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4759,7 +4759,7 @@
       </c>
       <c r="T33" s="2" t="inlineStr">
         <is>
-          <t>maa://45558 (91.67)</t>
+          <t>maa://45558 (84.62)</t>
         </is>
       </c>
       <c r="U33" s="1" t="n"/>
@@ -4873,7 +4873,7 @@
       </c>
       <c r="P34" s="2" t="inlineStr">
         <is>
-          <t>maa://48817 (93.94)</t>
+          <t>maa://48817 (94.12)</t>
         </is>
       </c>
       <c r="Q34" s="1" t="n"/>
@@ -4889,7 +4889,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (92.16)</t>
+          <t>maa://24526 (92.19)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4987,7 +4987,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.83)</t>
+          <t>maa://41296 (96.86)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5149,7 +5149,7 @@
       </c>
       <c r="T36" s="2" t="inlineStr">
         <is>
-          <t>maa://27613 (99.07)</t>
+          <t>maa://27613 (99.08)</t>
         </is>
       </c>
       <c r="U36" s="1" t="n"/>
@@ -5215,7 +5215,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (97.91), *maa://47069 (76.47), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.02), *maa://47069 (77.78), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5231,7 +5231,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.73), *maa://21239 (69.23)</t>
+          <t>maa://21280 (89.78), *maa://21239 (69.23)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5348,7 +5348,7 @@
       </c>
       <c r="T38" s="2" t="inlineStr">
         <is>
-          <t>maa://30713 (97.14)</t>
+          <t>maa://30713 (97.22)</t>
         </is>
       </c>
       <c r="U38" s="1" t="n"/>
@@ -5380,7 +5380,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (87.23)</t>
+          <t>maa://36697 (87.76)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5401,7 +5401,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (89.32), maa://25199 (85.22), maa://30434 (92.08), maa://45059 (81.48), ***maa://25036 (18.52), *maa://44165 (66.67)</t>
+          <t>maa://36670 (88.57), maa://25199 (85.22), maa://30434 (91.51), maa://45059 (81.48), ***maa://25036 (18.52), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5449,7 +5449,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>*maa://45788 (78.5), maa://47079 (93.48), *maa://45790 (70.59)</t>
+          <t>*maa://45788 (77.48), maa://47079 (94.34), *maa://45790 (72.22)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5757,7 +5757,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (91.28), maa://21284 (86.0)</t>
+          <t>maa://22525 (90.07), maa://21284 (86.27)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5826,7 +5826,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (98.12), maa://27728 (96.12)</t>
+          <t>maa://29768 (98.13), maa://27728 (96.12)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5895,7 +5895,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.9), maa://30807 (95.77), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (89.29)</t>
+          <t>maa://21229 (84.9), maa://30807 (95.77), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (89.66)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5927,7 +5927,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (37.5)</t>
+          <t>**maa://39364 (40.48)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -5948,7 +5948,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.24), maa://43901 (94.74)</t>
+          <t>maa://35931 (92.38), maa://43901 (95.24)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6001,7 +6001,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.65), maa://29661 (97.44), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.69), maa://29661 (97.44), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6310,7 +6310,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.48), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.54), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6362,7 +6362,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.58)</t>
+          <t>maa://32532 (92.73)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6416,7 +6416,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (56.52)</t>
+          <t>*maa://37964 (55.1)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>
@@ -6434,7 +6434,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://31270 (94.16), maa://27746 (82.76)</t>
+          <t>maa://31270 (94.2), maa://27746 (82.76)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6488,7 +6488,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (95.65), maa://43903 (100.0)</t>
+          <t>maa://42981 (95.83), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#184)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -467,7 +467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG75"/>
+  <dimension ref="A1:AG76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.68), maa://25390 (96.0), maa://36681 (86.42)</t>
+          <t>maa://24702 (94.7), maa://25390 (96.0), maa://36681 (86.42)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.17), *maa://30515 (70.48), maa://39402 (93.98), *maa://34787 (72.84), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.44), maa://39402 (94.19), *maa://30515 (70.48), *maa://34787 (72.84), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.11), *maa://20791 (62.03)</t>
+          <t>maa://22742 (91.16), *maa://20791 (62.03)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.36), maa://36684 (93.28), ***maa://22731 (6.25)</t>
+          <t>maa://21246 (91.36), maa://36684 (93.38), ***maa://22731 (6.25)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://40192 (96.0), maa://36987 (96.15), maa://39849 (88.89)</t>
+          <t>maa://40192 (96.05), maa://36987 (96.15), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (63.64), maa://20276 (87.3), *maa://22749 (80.0)</t>
+          <t>*maa://22880 (63.85), maa://20276 (87.3), *maa://22749 (80.0)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.27), maa://26254 (96.97), **maa://22738 (50.0)</t>
+          <t>maa://21249 (94.32), maa://26254 (96.97), **maa://22738 (50.0)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (90.32), **maa://20790 (43.48), maa://45854 (88.24), ***maa://37170 (17.14)</t>
+          <t>maa://24617 (90.32), maa://45854 (88.68), **maa://20790 (43.48), ***maa://37170 (17.14)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.13), maa://27484 (96.03), maa://27480 (83.33)</t>
+          <t>maa://27396 (84.23), maa://27484 (96.03), maa://27480 (83.33)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (95.18)</t>
+          <t>maa://24390 (95.24)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.51), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.55), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -967,7 +967,7 @@
       </c>
       <c r="P4" s="2" t="inlineStr">
         <is>
-          <t>maa://49983 (92.86), maa://50121 (86.67)</t>
+          <t>maa://49983 (94.44), maa://50121 (87.5)</t>
         </is>
       </c>
       <c r="Q4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (95.12), maa://27295 (87.5), maa://22754 (89.19), *maa://31008 (79.07), *maa://21746 (54.55)</t>
+          <t>maa://32509 (95.16), maa://27295 (87.5), maa://22754 (89.19), *maa://31008 (79.07), *maa://21746 (54.55)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.73), ***maa://31785 (22.22), maa://43217 (91.11), ***maa://36683 (29.79)</t>
+          <t>**maa://32495 (48.74), ***maa://31785 (22.22), maa://43217 (91.58), ***maa://36683 (29.79)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.82), maa://22744 (81.48)</t>
+          <t>maa://21245 (84.88), maa://22744 (81.48)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>*maa://22757 (77.5)</t>
+          <t>*maa://22757 (78.05)</t>
         </is>
       </c>
       <c r="M5" s="1" t="n"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="P5" s="2" t="inlineStr">
         <is>
-          <t>maa://21919 (96.72), *maa://21281 (80.0)</t>
+          <t>maa://21919 (96.83), *maa://21281 (80.0)</t>
         </is>
       </c>
       <c r="Q5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (94.12)</t>
+          <t>maa://42407 (94.29)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>maa://21955 (95.24)</t>
+          <t>maa://21955 (95.45)</t>
         </is>
       </c>
       <c r="E7" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (92.68), maa://24957 (97.78)</t>
+          <t>maa://28624 (92.86), maa://24957 (97.78)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (68.6), *maa://36671 (68.0), maa://45272 (95.0), *maa://42530 (62.5)</t>
+          <t>*maa://26191 (68.6), *maa://36671 (68.0), maa://45272 (95.24), *maa://42530 (62.5)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.05.01 13:20:46</t>
+          <t>更新日期：2025.05.02 13:20:57</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1545,7 +1545,7 @@
       </c>
       <c r="AB8" s="2" t="inlineStr">
         <is>
-          <t>maa://25389 (89.47)</t>
+          <t>maa://25389 (89.74)</t>
         </is>
       </c>
       <c r="AC8" s="1" t="n"/>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="AF8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24479 (79.12), *maa://21990 (51.85)</t>
+          <t>*maa://24479 (79.35), *maa://21990 (51.85)</t>
         </is>
       </c>
       <c r="AG8" s="1" t="n"/>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>maa://22765 (90.82), *maa://21915 (70.97)</t>
+          <t>maa://22765 (89.9), *maa://21915 (71.88)</t>
         </is>
       </c>
       <c r="E9" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (98.05)</t>
+          <t>maa://26223 (98.06)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.4), **maa://39938 (46.88), *maa://45044 (66.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (96.97)</t>
+          <t>maa://28711 (87.5), **maa://39938 (48.48), *maa://45044 (66.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (96.97)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.56), ***maa://39951 (11.94), ***maa://34206 (22.22), *maa://45271 (59.65), ***maa://39243 (25.0)</t>
+          <t>***maa://25695 (18.56), ***maa://39951 (11.94), ***maa://34206 (22.22), *maa://45271 (61.67), ***maa://39243 (25.0)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (89.53), maa://36669 (83.67), *maa://23264 (60.71)</t>
+          <t>maa://28977 (88.51), maa://36669 (84.0), *maa://23264 (60.71)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.28), maa://22755 (88.43), **maa://22756 (40.91), ***maa://21737 (10.45)</t>
+          <t>maa://27395 (96.31), maa://22755 (88.52), **maa://22756 (40.91), ***maa://21737 (11.76)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.8), maa://45828 (92.86), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.8), maa://45828 (93.1), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.3)</t>
+          <t>maa://36707 (99.31)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (88.99)</t>
+          <t>maa://21287 (89.09)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.86), maa://22501 (98.0), maa://45521 (88.46)</t>
+          <t>maa://22747 (92.86), maa://22501 (98.0), maa://45521 (89.29)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.94)</t>
+          <t>maa://36713 (97.96)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>maa://30766 (89.29), *maa://36678 (80.0)</t>
+          <t>maa://30766 (89.66), maa://36678 (81.82)</t>
         </is>
       </c>
       <c r="E12" s="1" t="n"/>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (90.29), ***maa://45826 (30.0)</t>
+          <t>maa://21867 (90.34), **maa://45826 (36.36)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.33), *maa://21485 (75.17), maa://37962 (92.45)</t>
+          <t>maa://22753 (91.33), *maa://21485 (75.17), maa://37962 (92.59)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.62), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (78.75), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.48), maa://36673 (92.86), maa://25001 (85.92)</t>
+          <t>maa://24999 (92.52), maa://36673 (92.86), maa://25001 (85.92)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>maa://34957 (82.02), **maa://22768 (50.0)</t>
+          <t>maa://34957 (82.42), **maa://22768 (50.0)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (37.66), maa://39883 (90.43), *maa://39885 (51.52)</t>
+          <t>**maa://22737 (37.66), maa://39883 (90.62), *maa://39885 (51.52)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>maa://30764 (88.52)</t>
+          <t>maa://30764 (88.71)</t>
         </is>
       </c>
       <c r="E14" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://39841 (94.81), maa://26245 (96.97), maa://21288 (96.3), maa://36682 (97.56)</t>
+          <t>maa://39841 (94.89), maa://26245 (96.99), maa://21288 (96.3), maa://36682 (97.56)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.77), maa://20107 (87.1), maa://22772 (100.0), *maa://22745 (66.67)</t>
+          <t>maa://23250 (98.78), maa://20107 (87.1), maa://22772 (100.0), *maa://22745 (66.67)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="T14" s="2" t="inlineStr">
         <is>
-          <t>maa://22521 (94.74), maa://42751 (100.0)</t>
+          <t>maa://22521 (94.78), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.57), maa://22734 (84.43), *maa://30808 (64.18), *maa://36048 (60.71), maa://45058 (94.12)</t>
+          <t>*maa://22743 (78.57), maa://22734 (84.43), *maa://30808 (64.18), *maa://36048 (60.71), maa://45058 (88.89)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (87.34), maa://21478 (89.74)</t>
+          <t>maa://24304 (86.96), maa://21478 (89.74)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="T15" s="2" t="inlineStr">
         <is>
-          <t>maa://23892 (96.39)</t>
+          <t>maa://23892 (96.43)</t>
         </is>
       </c>
       <c r="U15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.68), *maa://36666 (78.91), *maa://22766 (68.33)</t>
+          <t>maa://21364 (80.68), *maa://36666 (79.39), *maa://22766 (68.6)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.49), maa://37650 (97.87), maa://36679 (94.55)</t>
+          <t>maa://21441 (96.49), maa://37650 (97.96), maa://36679 (94.55)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.29), *maa://28648 (71.62), maa://36674 (80.7)</t>
+          <t>maa://22729 (94.35), *maa://28648 (71.62), maa://36674 (80.7)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.33)</t>
+          <t>maa://26228 (95.41)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (66.67), maa://27755 (93.68)</t>
+          <t>*maa://23911 (66.96), maa://27755 (93.68)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>maa://21624 (85.37)</t>
+          <t>maa://21624 (85.71)</t>
         </is>
       </c>
       <c r="E17" s="1" t="n"/>
@@ -2667,7 +2667,7 @@
       </c>
       <c r="P17" s="2" t="inlineStr">
         <is>
-          <t>maa://23890 (81.31), *maa://24940 (67.86)</t>
+          <t>maa://23890 (80.56), *maa://24940 (67.86)</t>
         </is>
       </c>
       <c r="Q17" s="1" t="n"/>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>*maa://42324 (53.33)</t>
+          <t>*maa://42324 (55.32)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2731,7 +2731,7 @@
       </c>
       <c r="AF17" s="2" t="inlineStr">
         <is>
-          <t>maa://50136 (90.0)</t>
+          <t>maa://50136 (91.67)</t>
         </is>
       </c>
       <c r="AG17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.68)</t>
+          <t>maa://24570 (96.76)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (87.55)</t>
+          <t>maa://24421 (87.59)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (91.62), *maa://22732 (50.5)</t>
+          <t>maa://22466 (91.62), **maa://22732 (49.52)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (60.0), **maa://29784 (50.0), *maa://47854 (80.0)</t>
+          <t>*maa://24313 (60.0), **maa://29784 (50.0), *maa://47854 (75.0)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (99.24)</t>
+          <t>maa://24386 (99.25)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (66.81), *maa://36668 (58.02)</t>
+          <t>*maa://30709 (66.96), *maa://36668 (58.02)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.53), maa://25198 (94.07), *maa://20795 (50.77), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.53), maa://25198 (94.12), *maa://20795 (50.77), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (90.06), ***maa://43283 (25.0)</t>
+          <t>maa://22864 (90.12), ***maa://43283 (25.0)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.49)</t>
+          <t>maa://41331 (84.85)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="P20" s="2" t="inlineStr">
         <is>
-          <t>maa://37442 (95.92)</t>
+          <t>maa://37442 (96.0)</t>
         </is>
       </c>
       <c r="Q20" s="1" t="n"/>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="T20" s="2" t="inlineStr">
         <is>
-          <t>maa://29113 (86.21)</t>
+          <t>maa://29113 (87.1)</t>
         </is>
       </c>
       <c r="U20" s="1" t="n"/>
@@ -3089,7 +3089,7 @@
       </c>
       <c r="X20" s="2" t="inlineStr">
         <is>
-          <t>maa://49976 (84.21), maa://50085 (88.57)</t>
+          <t>maa://49976 (84.13), maa://50085 (88.37)</t>
         </is>
       </c>
       <c r="Y20" s="1" t="n"/>
@@ -3171,7 +3171,7 @@
       </c>
       <c r="L21" s="2" t="inlineStr">
         <is>
-          <t>maa://31731 (96.23)</t>
+          <t>maa://31731 (96.3)</t>
         </is>
       </c>
       <c r="M21" s="1" t="n"/>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="X21" s="2" t="inlineStr">
         <is>
-          <t>maa://20110 (86.76), maa://34946 (92.0)</t>
+          <t>maa://20110 (86.76), maa://34946 (92.16)</t>
         </is>
       </c>
       <c r="Y21" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (82.16), ***maa://23820 (30.0)</t>
+          <t>maa://21443 (82.21), ***maa://23820 (30.0)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.68), *maa://37649 (67.74)</t>
+          <t>maa://21282 (98.68), *maa://37649 (65.62)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.67), maa://39875 (94.67)</t>
+          <t>maa://39756 (95.26), maa://39875 (94.67)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.71), *maa://29748 (76.12), ***maa://29785 (17.39), *maa://37566 (76.19)</t>
+          <t>maa://30587 (91.71), *maa://29748 (76.12), ***maa://29785 (17.39), *maa://37566 (76.74)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3495,7 +3495,7 @@
       </c>
       <c r="AB23" s="2" t="inlineStr">
         <is>
-          <t>maa://29652 (97.87)</t>
+          <t>maa://29652 (97.96)</t>
         </is>
       </c>
       <c r="AC23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.64), *maa://46650 (53.33)</t>
+          <t>*maa://24368 (78.7), *maa://46650 (58.82)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (83.7), maa://23504 (93.39), **maa://22892 (40.79), *maa://25141 (76.87), *maa://36663 (78.41), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (83.81), maa://23504 (93.42), **maa://22892 (41.18), *maa://25141 (76.87), *maa://36663 (78.89), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (84.47), *maa://36672 (79.31), maa://29910 (93.55), **maa://21440 (35.71), maa://45831 (91.67)</t>
+          <t>maa://22523 (84.54), *maa://36672 (79.66), maa://29910 (93.55), **maa://21440 (35.71), maa://45831 (91.67)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3739,7 +3739,7 @@
       </c>
       <c r="X25" s="2" t="inlineStr">
         <is>
-          <t>maa://29890 (81.13)</t>
+          <t>maa://29890 (81.48)</t>
         </is>
       </c>
       <c r="Y25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (88.89), maa://24516 (80.22), maa://26001 (87.5)</t>
+          <t>maa://31215 (89.06), maa://24516 (80.22), maa://26001 (85.96)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.48), maa://24621 (96.97), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
+          <t>maa://20108 (96.48), maa://24621 (96.99), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3837,7 +3837,7 @@
       </c>
       <c r="P26" s="2" t="inlineStr">
         <is>
-          <t>*maa://30968 (65.0), maa://39870 (91.67)</t>
+          <t>*maa://30968 (65.0), maa://39870 (92.31)</t>
         </is>
       </c>
       <c r="Q26" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (95.24)</t>
+          <t>maa://42235 (95.31)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (76.56)</t>
+          <t>*maa://30624 (76.92)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4031,7 +4031,7 @@
       </c>
       <c r="AF27" s="2" t="inlineStr">
         <is>
-          <t>maa://24023 (96.1)</t>
+          <t>maa://24023 (96.15)</t>
         </is>
       </c>
       <c r="AG27" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.96), maa://25725 (84.62)</t>
+          <t>maa://24465 (90.85), maa://25725 (84.78)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>*maa://29765 (65.17), maa://23263 (95.33)</t>
+          <t>*maa://29765 (64.44), maa://23263 (95.33)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (91.2), maa://41749 (92.04), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (91.32), maa://41749 (92.17), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.47), *maa://36701 (67.74)</t>
+          <t>maa://36660 (92.51), *maa://36701 (67.74)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.77), maa://28440 (82.4), maa://31400 (98.84), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.8), maa://28440 (82.54), maa://31400 (98.84), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.01), maa://42865 (82.28), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (69.09), maa://42865 (82.95), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4309,7 +4309,7 @@
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>maa://45792 (87.5)</t>
+          <t>maa://45792 (88.0)</t>
         </is>
       </c>
       <c r="E30" s="1" t="n"/>
@@ -4341,7 +4341,7 @@
       </c>
       <c r="L30" s="2" t="inlineStr">
         <is>
-          <t>maa://30442 (95.52)</t>
+          <t>maa://30442 (95.59)</t>
         </is>
       </c>
       <c r="M30" s="1" t="n"/>
@@ -4357,7 +4357,7 @@
       </c>
       <c r="P30" s="2" t="inlineStr">
         <is>
-          <t>maa://21442 (98.71)</t>
+          <t>maa://21442 (98.72)</t>
         </is>
       </c>
       <c r="Q30" s="1" t="n"/>
@@ -4373,7 +4373,7 @@
       </c>
       <c r="T30" s="2" t="inlineStr">
         <is>
-          <t>*maa://32940 (66.67), maa://24388 (94.44)</t>
+          <t>*maa://32940 (66.67), maa://24388 (94.74)</t>
         </is>
       </c>
       <c r="U30" s="1" t="n"/>
@@ -4389,7 +4389,7 @@
       </c>
       <c r="X30" s="2" t="inlineStr">
         <is>
-          <t>maa://39477 (90.91)</t>
+          <t>maa://39477 (91.3)</t>
         </is>
       </c>
       <c r="Y30" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.38), maa://45822 (100.0), *maa://45045 (80.0)</t>
+          <t>maa://42979 (97.42), maa://45822 (100.0), *maa://45045 (80.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.59), maa://36258 (86.23), *maa://43904 (76.92)</t>
+          <t>maa://35926 (93.63), maa://36258 (86.43), *maa://43904 (76.92)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4530,10 +4530,14 @@
       </c>
       <c r="AA31" s="1" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AB31" s="2" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AB31" s="2" t="inlineStr">
+        <is>
+          <t>**maa://51420 (50.0)</t>
+        </is>
+      </c>
       <c r="AC31" s="1" t="n"/>
       <c r="AD31" s="1" t="inlineStr">
         <is>
@@ -4581,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.33), maa://36667 (97.92), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.35), maa://36667 (97.94), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4597,7 +4601,7 @@
       </c>
       <c r="L32" s="2" t="inlineStr">
         <is>
-          <t>maa://28065 (95.83)</t>
+          <t>maa://28065 (95.92)</t>
         </is>
       </c>
       <c r="M32" s="1" t="n"/>
@@ -4629,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.82), maa://41108 (88.0), maa://41238 (97.54), maa://45523 (100.0)</t>
+          <t>maa://42859 (96.91), maa://41108 (88.0), maa://41238 (97.58), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4677,7 +4681,7 @@
       </c>
       <c r="AF32" s="2" t="inlineStr">
         <is>
-          <t>maa://42408 (85.71)</t>
+          <t>maa://42408 (86.67)</t>
         </is>
       </c>
       <c r="AG32" s="1" t="n"/>
@@ -4836,12 +4840,12 @@
       </c>
       <c r="G34" s="1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H34" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>None</t>
         </is>
       </c>
       <c r="I34" s="1" t="n"/>
@@ -4873,7 +4877,7 @@
       </c>
       <c r="P34" s="2" t="inlineStr">
         <is>
-          <t>maa://48817 (94.12)</t>
+          <t>maa://48817 (94.44)</t>
         </is>
       </c>
       <c r="Q34" s="1" t="n"/>
@@ -4900,12 +4904,12 @@
       </c>
       <c r="W34" s="1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0</t>
         </is>
       </c>
       <c r="X34" s="1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>None</t>
         </is>
       </c>
       <c r="Y34" s="1" t="n"/>
@@ -4987,7 +4991,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.86)</t>
+          <t>maa://41296 (96.91)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5067,7 +5071,7 @@
       </c>
       <c r="AF35" s="2" t="inlineStr">
         <is>
-          <t>maa://39479 (90.48)</t>
+          <t>maa://39479 (90.91)</t>
         </is>
       </c>
       <c r="AG35" s="1" t="n"/>
@@ -5149,7 +5153,7 @@
       </c>
       <c r="T36" s="2" t="inlineStr">
         <is>
-          <t>maa://27613 (99.08)</t>
+          <t>maa://27613 (99.09)</t>
         </is>
       </c>
       <c r="U36" s="1" t="n"/>
@@ -5187,6 +5191,22 @@
       <c r="AG36" s="1" t="n"/>
     </row>
     <row r="37">
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>CONFESS-47</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D37" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E37" s="1" t="n"/>
       <c r="F37" s="1" t="inlineStr">
         <is>
           <t>杰克</t>
@@ -5215,7 +5235,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (98.02), *maa://47069 (77.78), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.09), *maa://47069 (77.78), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5247,7 +5267,7 @@
       </c>
       <c r="T37" s="2" t="inlineStr">
         <is>
-          <t>**maa://39354 (45.45)</t>
+          <t>**maa://39354 (41.67)</t>
         </is>
       </c>
       <c r="U37" s="1" t="n"/>
@@ -5332,7 +5352,7 @@
       </c>
       <c r="P38" s="2" t="inlineStr">
         <is>
-          <t>*maa://24383 (69.52)</t>
+          <t>*maa://24383 (69.81)</t>
         </is>
       </c>
       <c r="Q38" s="1" t="n"/>
@@ -5380,7 +5400,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (87.76)</t>
+          <t>maa://36697 (88.05)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5401,7 +5421,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (88.57), maa://25199 (85.22), maa://30434 (91.51), maa://45059 (81.48), ***maa://25036 (18.52), *maa://44165 (66.67)</t>
+          <t>maa://36670 (88.57), maa://25199 (85.22), maa://30434 (91.59), maa://45059 (81.48), ***maa://25036 (18.52), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5449,7 +5469,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>*maa://45788 (77.48), maa://47079 (94.34), *maa://45790 (72.22)</t>
+          <t>*maa://45788 (76.79), maa://47079 (94.83), *maa://45790 (72.22)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5534,7 +5554,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.06), maa://21386 (95.79), maa://36664 (89.47), maa://45550 (87.5)</t>
+          <t>maa://23278 (95.08), maa://21386 (95.79), maa://36664 (89.66), maa://45550 (87.5)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5619,7 +5639,7 @@
       </c>
       <c r="P41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (40.0), maa://43177 (92.0)</t>
+          <t>**maa://35616 (40.0), maa://43177 (92.31)</t>
         </is>
       </c>
       <c r="Q41" s="1" t="n"/>
@@ -5757,10 +5777,26 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (90.07), maa://21284 (86.27)</t>
+          <t>maa://22525 (89.47), maa://21284 (86.27)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
+      <c r="J43" s="1" t="inlineStr">
+        <is>
+          <t>信仰搅拌机</t>
+        </is>
+      </c>
+      <c r="K43" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L43" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M43" s="1" t="n"/>
       <c r="N43" s="1" t="inlineStr">
         <is>
           <t>截云</t>
@@ -5773,7 +5809,7 @@
       </c>
       <c r="P43" s="2" t="inlineStr">
         <is>
-          <t>maa://47403 (100.0)</t>
+          <t>maa://47403 (85.71)</t>
         </is>
       </c>
       <c r="Q43" s="1" t="n"/>
@@ -5826,7 +5862,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (98.13), maa://27728 (96.12)</t>
+          <t>maa://29768 (98.14), maa://27728 (96.12)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5895,7 +5931,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.9), maa://30807 (95.77), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (89.66)</t>
+          <t>maa://21229 (84.46), maa://30807 (95.77), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (90.0)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5927,10 +5963,26 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (40.48)</t>
+          <t>**maa://39364 (40.0)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
+      <c r="AD45" s="1" t="inlineStr">
+        <is>
+          <t>新约能天使</t>
+        </is>
+      </c>
+      <c r="AE45" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF45" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG45" s="1" t="n"/>
     </row>
     <row r="46">
       <c r="B46" s="3" t="n"/>
@@ -5948,7 +6000,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.38), maa://43901 (95.24)</t>
+          <t>maa://35931 (92.4), maa://43901 (95.35)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6001,7 +6053,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.69), maa://29661 (97.44), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.7), maa://29661 (97.45), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6260,7 +6312,7 @@
       </c>
       <c r="H52" s="2" t="inlineStr">
         <is>
-          <t>maa://24376 (96.67)</t>
+          <t>maa://24376 (96.77)</t>
         </is>
       </c>
       <c r="I52" s="1" t="n"/>
@@ -6310,7 +6362,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.54), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.55), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6348,6 +6400,22 @@
         </is>
       </c>
       <c r="I54" s="1" t="n"/>
+      <c r="N54" s="1" t="inlineStr">
+        <is>
+          <t>蕾缪安</t>
+        </is>
+      </c>
+      <c r="O54" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P54" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q54" s="1" t="n"/>
     </row>
     <row r="55">
       <c r="F55" s="1" t="inlineStr">
@@ -6416,7 +6484,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (55.1)</t>
+          <t>*maa://37964 (56.86)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>
@@ -6452,7 +6520,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (72.06)</t>
+          <t>*maa://40438 (72.46)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>
@@ -6488,7 +6556,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (95.83), maa://43903 (100.0)</t>
+          <t>maa://42981 (96.0), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>
@@ -6524,7 +6592,7 @@
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>maa://44405 (84.85)</t>
+          <t>maa://44405 (85.29)</t>
         </is>
       </c>
       <c r="I64" s="1" t="n"/>
@@ -6726,6 +6794,24 @@
         </is>
       </c>
       <c r="I75" s="1" t="n"/>
+    </row>
+    <row r="76">
+      <c r="F76" s="1" t="inlineStr">
+        <is>
+          <t>聆音</t>
+        </is>
+      </c>
+      <c r="G76" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H76" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I76" s="1" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
CI: Auto Update Data (#185)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.7), maa://25390 (96.0), maa://36681 (86.42)</t>
+          <t>maa://24702 (94.72), maa://25390 (96.04), maa://36681 (86.42)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.44), maa://39402 (94.19), *maa://30515 (70.48), *maa://34787 (72.84), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
+          <t>*maa://24633 (56.44), maa://39402 (94.44), *maa://30515 (69.81), *maa://34787 (72.62), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.16), *maa://20791 (62.03)</t>
+          <t>maa://22742 (91.35), *maa://20791 (62.5)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.36), maa://36684 (93.38), ***maa://22731 (6.25)</t>
+          <t>maa://21246 (91.39), maa://36684 (93.38), ***maa://22731 (6.25)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (91.41), ***maa://21730 (27.85), ***maa://39501 (12.5), **maa://36675 (50.0)</t>
+          <t>maa://25251 (91.47), ***maa://21730 (27.85), ***maa://39501 (12.5), **maa://36675 (50.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://40192 (96.05), maa://36987 (96.15), maa://39849 (88.89)</t>
+          <t>maa://40192 (96.1), maa://36987 (96.15), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.27), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.29), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (63.85), maa://20276 (87.3), *maa://22749 (80.0)</t>
+          <t>*maa://22880 (64.68), maa://20276 (87.43), *maa://22749 (80.0)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.32), maa://26254 (96.97), **maa://22738 (50.0)</t>
+          <t>maa://21249 (94.36), maa://26254 (96.97), **maa://22738 (50.0)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (90.32), maa://45854 (88.68), **maa://20790 (43.48), ***maa://37170 (17.14)</t>
+          <t>maa://24617 (90.32), maa://45854 (89.09), **maa://20790 (43.48), ***maa://37170 (17.14)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.23), maa://27484 (96.03), maa://27480 (83.33)</t>
+          <t>maa://27396 (84.32), maa://27484 (96.06), maa://27480 (83.33)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (95.24)</t>
+          <t>maa://24390 (95.29)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.55), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.68), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -967,7 +967,7 @@
       </c>
       <c r="P4" s="2" t="inlineStr">
         <is>
-          <t>maa://49983 (94.44), maa://50121 (87.5)</t>
+          <t>maa://49983 (94.59), maa://50121 (90.48)</t>
         </is>
       </c>
       <c r="Q4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (95.16), maa://27295 (87.5), maa://22754 (89.19), *maa://31008 (79.07), *maa://21746 (54.55)</t>
+          <t>maa://32509 (95.2), maa://27295 (87.5), maa://22754 (89.19), *maa://31008 (79.07), *maa://21746 (54.55)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.74), ***maa://31785 (22.22), maa://43217 (91.58), ***maa://36683 (29.79)</t>
+          <t>**maa://32495 (48.74), ***maa://31785 (22.22), maa://43217 (91.92), ***maa://36683 (29.79)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (65.38), *maa://39394 (65.38), ***maa://26209 (13.04)</t>
+          <t>*maa://30062 (65.38), *maa://39394 (66.67), ***maa://26209 (13.04)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.88), maa://22744 (81.48)</t>
+          <t>maa://21245 (84.73), maa://22744 (81.48)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>*maa://22757 (78.05)</t>
+          <t>*maa://22757 (78.57)</t>
         </is>
       </c>
       <c r="M5" s="1" t="n"/>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="AB5" s="2" t="inlineStr">
         <is>
-          <t>*maa://29863 (65.0), ***maa://22752 (12.5), **maa://26013 (37.5)</t>
+          <t>*maa://29863 (63.41), ***maa://22752 (12.5), **maa://26013 (37.5)</t>
         </is>
       </c>
       <c r="AC5" s="1" t="n"/>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>maa://24839 (99.05)</t>
+          <t>maa://24839 (98.76)</t>
         </is>
       </c>
       <c r="M6" s="1" t="n"/>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="AF6" s="2" t="inlineStr">
         <is>
-          <t>*maa://33152 (64.81), ***maa://22770 (26.09)</t>
+          <t>*maa://33152 (65.45), ***maa://22770 (26.09)</t>
         </is>
       </c>
       <c r="AG6" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (92.86), maa://24957 (97.78)</t>
+          <t>maa://28624 (93.02), maa://24957 (97.78)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.88), *maa://22758 (76.92)</t>
+          <t>maa://22399 (95.95), *maa://22758 (76.92)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (68.6), *maa://36671 (68.0), maa://45272 (95.24), *maa://42530 (62.5)</t>
+          <t>*maa://26191 (68.6), *maa://36671 (68.0), maa://45272 (95.83), *maa://42530 (62.5)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.05.02 13:20:57</t>
+          <t>更新日期：2025.05.03 13:20:53</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>*maa://21476 (74.55), *maa://39431 (60.0), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (74.55), *maa://39431 (56.25), *maa://37551 (57.14)</t>
         </is>
       </c>
       <c r="E8" s="1" t="n"/>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (83.87), *maa://21916 (62.12), maa://23252 (91.18), maa://37496 (97.06), **maa://22759 (45.45)</t>
+          <t>maa://32931 (84.0), *maa://21916 (62.12), maa://23252 (91.18), maa://37496 (97.14), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (96.23)</t>
+          <t>maa://21411 (96.01)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="AB8" s="2" t="inlineStr">
         <is>
-          <t>maa://25389 (89.74)</t>
+          <t>maa://25389 (90.24)</t>
         </is>
       </c>
       <c r="AC8" s="1" t="n"/>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>maa://22765 (89.9), *maa://21915 (71.88)</t>
+          <t>maa://22765 (90.0), *maa://21915 (71.88)</t>
         </is>
       </c>
       <c r="E9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.5), **maa://39938 (48.48), *maa://45044 (66.67), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (96.97)</t>
+          <t>maa://28711 (86.82), **maa://39938 (47.06), **maa://45044 (50.0), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (96.97)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (88.89), *maa://22865 (51.85)</t>
+          <t>maa://26206 (88.51), *maa://22865 (51.85)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.56), ***maa://39951 (11.94), ***maa://34206 (22.22), *maa://45271 (61.67), ***maa://39243 (25.0)</t>
+          <t>***maa://25695 (18.88), ***maa://39951 (11.94), ***maa://34206 (22.22), *maa://45271 (60.66), ***maa://39243 (25.0)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (88.51), maa://36669 (84.0), *maa://23264 (60.71)</t>
+          <t>maa://28977 (88.64), maa://36669 (84.0), *maa://23264 (60.71)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.31), maa://22755 (88.52), **maa://22756 (40.91), ***maa://21737 (11.76)</t>
+          <t>maa://27395 (96.38), maa://22755 (88.52), **maa://22756 (40.91), ***maa://21737 (11.76)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.8), maa://45828 (93.1), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.8), maa://45828 (93.33), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (53.47), *maa://22733 (62.16), **maa://22761 (50.0)</t>
+          <t>*maa://25021 (53.92), *maa://22733 (62.16), **maa://22761 (50.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.31)</t>
+          <t>maa://36707 (99.32)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (89.09)</t>
+          <t>maa://21287 (89.19)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (92.86), maa://22501 (98.0), maa://45521 (89.29)</t>
+          <t>maa://22747 (91.23), maa://22501 (98.0), maa://45521 (89.66)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.96)</t>
+          <t>maa://36713 (97.97)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1935,7 +1935,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://29912 (97.47), maa://22516 (87.36), *maa://20794 (53.52)</t>
+          <t>maa://29912 (97.5), maa://22516 (87.36), *maa://20794 (54.17)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -1951,7 +1951,7 @@
       </c>
       <c r="AF11" s="2" t="inlineStr">
         <is>
-          <t>maa://31203 (96.15)</t>
+          <t>maa://31203 (96.3)</t>
         </is>
       </c>
       <c r="AG11" s="1" t="n"/>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (90.34), **maa://45826 (36.36)</t>
+          <t>maa://21867 (90.4), **maa://45826 (36.36)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.61), maa://36677 (94.59), maa://39872 (92.31)</t>
+          <t>maa://23669 (95.61), maa://36677 (94.67), maa://39872 (92.59)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.75), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (79.14), *maa://20106 (63.96), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.52), maa://36673 (92.86), maa://25001 (85.92)</t>
+          <t>maa://24999 (92.57), maa://36673 (92.86), maa://25001 (85.92)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.56), **maa://22728 (46.67)</t>
+          <t>*maa://21248 (73.48), **maa://22728 (46.67)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (93.28), *maa://22583 (76.06), *maa://22500 (59.57), maa://48321 (100.0)</t>
+          <t>maa://22676 (93.28), *maa://22583 (76.39), *maa://22500 (59.57), maa://48321 (100.0)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>maa://34957 (82.42), **maa://22768 (50.0)</t>
+          <t>maa://34957 (80.65), **maa://22768 (50.0)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (37.66), maa://39883 (90.62), *maa://39885 (51.52)</t>
+          <t>**maa://22737 (37.42), maa://39883 (90.82), *maa://39885 (51.52)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://39841 (94.89), maa://26245 (96.99), maa://21288 (96.3), maa://36682 (97.56)</t>
+          <t>maa://39841 (94.93), maa://26245 (96.41), maa://21288 (96.3), maa://36682 (97.67)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.78), maa://20107 (87.1), maa://22772 (100.0), *maa://22745 (66.67)</t>
+          <t>maa://23250 (98.79), maa://20107 (87.1), maa://22772 (100.0), *maa://22745 (66.67)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.57), maa://22734 (84.43), *maa://30808 (64.18), *maa://36048 (60.71), maa://45058 (88.89)</t>
+          <t>*maa://22743 (78.76), maa://22734 (84.43), *maa://30808 (64.18), *maa://36048 (62.07), maa://45058 (88.89)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (86.96), maa://21478 (89.74)</t>
+          <t>maa://24304 (86.64), maa://21478 (90.0)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (90.8), *maa://22727 (70.0)</t>
+          <t>maa://24762 (90.91), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.68), *maa://36666 (79.39), *maa://22766 (68.6)</t>
+          <t>maa://21364 (80.79), maa://36666 (80.15), *maa://22766 (68.6)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.49), maa://37650 (97.96), maa://36679 (94.55)</t>
+          <t>maa://21441 (96.49), maa://37650 (98.0), maa://36679 (94.55)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.35), *maa://28648 (71.62), maa://36674 (80.7)</t>
+          <t>maa://22729 (94.38), *maa://28648 (71.62), *maa://36674 (79.31)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (98.18), maa://28051 (96.0)</t>
+          <t>maa://28501 (98.2), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="AB16" s="2" t="inlineStr">
         <is>
-          <t>maa://26228 (95.41)</t>
+          <t>maa://26228 (95.45)</t>
         </is>
       </c>
       <c r="AC16" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (66.96), maa://27755 (93.68)</t>
+          <t>*maa://23911 (66.96), maa://27755 (93.75)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>*maa://42324 (55.32)</t>
+          <t>*maa://42324 (56.25)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2731,7 +2731,7 @@
       </c>
       <c r="AF17" s="2" t="inlineStr">
         <is>
-          <t>maa://50136 (91.67)</t>
+          <t>maa://50136 (92.86)</t>
         </is>
       </c>
       <c r="AG17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.76)</t>
+          <t>maa://24570 (96.79)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (91.62), **maa://22732 (49.52)</t>
+          <t>maa://22466 (91.67), *maa://22732 (50.47)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (60.0), **maa://29784 (50.0), *maa://47854 (75.0)</t>
+          <t>*maa://24313 (60.23), **maa://29784 (50.0), *maa://47854 (75.0)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (99.25)</t>
+          <t>maa://24386 (98.53)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (66.96), *maa://36668 (58.02)</t>
+          <t>*maa://30709 (67.17), *maa://36668 (57.32)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -2991,7 +2991,7 @@
       </c>
       <c r="AF19" s="2" t="inlineStr">
         <is>
-          <t>*maa://21663 (62.67)</t>
+          <t>*maa://21663 (63.64)</t>
         </is>
       </c>
       <c r="AG19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.53), maa://25198 (94.12), *maa://20795 (50.77), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.62), maa://25198 (94.31), *maa://20795 (50.77), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (90.12), ***maa://43283 (25.0)</t>
+          <t>maa://22864 (90.17), ***maa://43283 (25.0)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (84.85)</t>
+          <t>maa://41331 (84.65)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3089,7 +3089,7 @@
       </c>
       <c r="X20" s="2" t="inlineStr">
         <is>
-          <t>maa://49976 (84.13), maa://50085 (88.37)</t>
+          <t>maa://49976 (85.92), maa://50085 (88.46)</t>
         </is>
       </c>
       <c r="Y20" s="1" t="n"/>
@@ -3155,7 +3155,7 @@
       </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>maa://24372 (97.06)</t>
+          <t>maa://24372 (97.12)</t>
         </is>
       </c>
       <c r="I21" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (82.21), ***maa://23820 (30.0)</t>
+          <t>maa://21443 (82.29), ***maa://23820 (30.0)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (92.34), *maa://22432 (79.59)</t>
+          <t>maa://22524 (91.56), maa://22432 (80.2)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>maa://25236 (95.88), **maa://21678 (48.94), **maa://22735 (42.86)</t>
+          <t>maa://25236 (95.92), **maa://21678 (48.94), **maa://22735 (42.86)</t>
         </is>
       </c>
       <c r="I22" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>*maa://27127 (78.12), *maa://22751 (71.43)</t>
+          <t>*maa://27127 (78.12), *maa://22751 (71.83)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="AF22" s="2" t="inlineStr">
         <is>
-          <t>maa://29658 (94.23)</t>
+          <t>maa://29658 (94.34)</t>
         </is>
       </c>
       <c r="AG22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.26), maa://39875 (94.67)</t>
+          <t>maa://39756 (95.14), maa://39875 (94.67)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.71), *maa://29748 (76.12), ***maa://29785 (17.39), *maa://37566 (76.74)</t>
+          <t>maa://30587 (91.79), *maa://29748 (76.12), ***maa://29785 (17.39), *maa://37566 (76.74)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="X23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (70.11)</t>
+          <t>*maa://28503 (69.32)</t>
         </is>
       </c>
       <c r="Y23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.7), *maa://46650 (58.82)</t>
+          <t>*maa://24368 (78.8), *maa://46650 (57.89)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (83.81), maa://23504 (93.42), **maa://22892 (41.18), *maa://25141 (76.87), *maa://36663 (78.89), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (83.81), maa://23504 (93.46), **maa://22892 (41.56), *maa://25141 (77.04), *maa://36663 (79.12), ***maa://22815 (23.08)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (84.54), *maa://36672 (79.66), maa://29910 (93.55), **maa://21440 (35.71), maa://45831 (91.67)</t>
+          <t>maa://22523 (84.54), *maa://36672 (78.33), maa://29910 (93.55), **maa://21440 (35.71), maa://45831 (91.67)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.1)</t>
+          <t>maa://29753 (95.12)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (72.88), *maa://25311 (74.31), ***maa://22725 (4.76), *maa://45047 (66.67)</t>
+          <t>*maa://29063 (73.03), *maa://25311 (73.64), ***maa://22725 (4.76), *maa://45047 (66.67)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3723,7 +3723,7 @@
       </c>
       <c r="T25" s="2" t="inlineStr">
         <is>
-          <t>maa://20109 (92.39), maa://22545 (100.0), *maa://42915 (75.0)</t>
+          <t>maa://20109 (92.47), maa://22545 (100.0), *maa://42915 (75.0)</t>
         </is>
       </c>
       <c r="U25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (89.06), maa://24516 (80.22), maa://26001 (85.96)</t>
+          <t>maa://31215 (89.15), maa://24516 (80.22), maa://26001 (85.96)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.48), maa://24621 (96.99), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
+          <t>maa://20108 (96.48), maa://24621 (97.04), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (95.31)</t>
+          <t>maa://42235 (95.45)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.85), maa://25725 (84.78)</t>
+          <t>maa://24465 (90.89), maa://25725 (84.95)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>*maa://29765 (64.44), maa://23263 (95.33)</t>
+          <t>*maa://29765 (65.59), maa://23263 (95.33)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (91.32), maa://41749 (92.17), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (91.44), maa://41749 (92.44), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.51), *maa://36701 (67.74)</t>
+          <t>maa://36660 (92.6), *maa://36701 (67.74)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4179,7 +4179,7 @@
       </c>
       <c r="D29" s="2" t="inlineStr">
         <is>
-          <t>maa://31694 (98.25)</t>
+          <t>maa://31694 (98.28)</t>
         </is>
       </c>
       <c r="E29" s="1" t="n"/>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>*maa://25175 (64.91)</t>
+          <t>*maa://25175 (63.79)</t>
         </is>
       </c>
       <c r="I29" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.8), maa://28440 (82.54), maa://31400 (98.84), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.87), maa://28440 (82.54), maa://31400 (98.84), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.09), maa://42865 (82.95), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (69.09), maa://42865 (83.33), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4389,7 +4389,7 @@
       </c>
       <c r="X30" s="2" t="inlineStr">
         <is>
-          <t>maa://39477 (91.3)</t>
+          <t>maa://39477 (91.67)</t>
         </is>
       </c>
       <c r="Y30" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.42), maa://45822 (100.0), *maa://45045 (80.0)</t>
+          <t>maa://42979 (97.46), maa://45822 (100.0), *maa://45045 (80.0)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.63), maa://36258 (86.43), *maa://43904 (76.92)</t>
+          <t>maa://35926 (93.69), maa://36258 (86.43), *maa://43904 (76.92)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.35), maa://36667 (97.94), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.37), maa://36667 (97.94), **maa://20793 (38.78), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (96.91), maa://41108 (88.0), maa://41238 (97.58), maa://45523 (100.0)</t>
+          <t>maa://42859 (97.04), maa://41108 (88.0), maa://41238 (97.64), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4763,7 +4763,7 @@
       </c>
       <c r="T33" s="2" t="inlineStr">
         <is>
-          <t>maa://45558 (84.62)</t>
+          <t>maa://45558 (85.71)</t>
         </is>
       </c>
       <c r="U33" s="1" t="n"/>
@@ -4877,7 +4877,7 @@
       </c>
       <c r="P34" s="2" t="inlineStr">
         <is>
-          <t>maa://48817 (94.44)</t>
+          <t>maa://48817 (95.24)</t>
         </is>
       </c>
       <c r="Q34" s="1" t="n"/>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="T34" s="2" t="inlineStr">
         <is>
-          <t>maa://24526 (92.19)</t>
+          <t>maa://24526 (92.22)</t>
         </is>
       </c>
       <c r="U34" s="1" t="n"/>
@@ -4991,7 +4991,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.91)</t>
+          <t>maa://41296 (96.97)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5235,7 +5235,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (98.09), *maa://47069 (77.78), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.17), *maa://47069 (77.78), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5352,7 +5352,7 @@
       </c>
       <c r="P38" s="2" t="inlineStr">
         <is>
-          <t>*maa://24383 (69.81)</t>
+          <t>*maa://24383 (70.09)</t>
         </is>
       </c>
       <c r="Q38" s="1" t="n"/>
@@ -5400,7 +5400,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (88.05)</t>
+          <t>maa://36697 (88.12)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (88.57), maa://25199 (85.22), maa://30434 (91.59), maa://45059 (81.48), ***maa://25036 (18.52), *maa://44165 (66.67)</t>
+          <t>maa://36670 (88.68), maa://25199 (85.22), maa://30434 (91.96), maa://45059 (82.14), ***maa://25036 (18.52), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5453,7 +5453,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (91.93), maa://47093 (100.0)</t>
+          <t>maa://24709 (92.02), maa://47093 (100.0)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5469,7 +5469,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>*maa://45788 (76.79), maa://47079 (94.83), *maa://45790 (72.22)</t>
+          <t>*maa://45788 (76.32), maa://47079 (95.31), *maa://45790 (75.0)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5554,7 +5554,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.08), maa://21386 (95.79), maa://36664 (89.66), maa://45550 (87.5)</t>
+          <t>maa://23278 (95.11), maa://21386 (95.79), maa://36664 (89.66), maa://45550 (87.5)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5809,7 +5809,7 @@
       </c>
       <c r="P43" s="2" t="inlineStr">
         <is>
-          <t>maa://47403 (85.71)</t>
+          <t>maa://47403 (87.5)</t>
         </is>
       </c>
       <c r="Q43" s="1" t="n"/>
@@ -5862,7 +5862,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (98.14), maa://27728 (96.12)</t>
+          <t>maa://29768 (98.15), maa://27728 (96.12)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5931,7 +5931,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.46), maa://30807 (95.77), *maa://22767 (55.0), ***maa://20796 (13.79), maa://42459 (90.0)</t>
+          <t>maa://21229 (84.46), maa://30807 (95.83), *maa://22767 (55.0), maa://42459 (90.32), ***maa://20796 (13.79)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -6000,7 +6000,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.4), maa://43901 (95.35)</t>
+          <t>maa://35931 (92.53), maa://43901 (95.45)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6053,7 +6053,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.7), maa://29661 (97.45), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.73), maa://29661 (97.45), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6175,7 +6175,7 @@
       </c>
       <c r="P49" s="2" t="inlineStr">
         <is>
-          <t>*maa://39643 (63.16)</t>
+          <t>*maa://39643 (61.54)</t>
         </is>
       </c>
       <c r="Q49" s="1" t="n"/>
@@ -6362,7 +6362,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.55), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.58), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6430,7 +6430,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.73)</t>
+          <t>maa://32532 (92.77)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6466,7 +6466,7 @@
       </c>
       <c r="H57" s="2" t="inlineStr">
         <is>
-          <t>maa://25176 (98.44)</t>
+          <t>maa://25176 (98.46)</t>
         </is>
       </c>
       <c r="I57" s="1" t="n"/>
@@ -6502,7 +6502,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://31270 (94.2), maa://27746 (82.76)</t>
+          <t>maa://31270 (94.24), maa://27746 (82.91)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6520,7 +6520,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (72.46)</t>
+          <t>*maa://40438 (72.86)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#186)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://24702 (94.72), maa://25390 (96.04), maa://36681 (86.42)</t>
+          <t>maa://25390 (95.33), maa://24702 (94.74), maa://36681 (86.42)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>*maa://24633 (56.44), maa://39402 (94.44), *maa://30515 (69.81), *maa://34787 (72.62), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
+          <t>maa://39402 (94.23), *maa://24633 (56.1), *maa://30515 (70.09), *maa://34787 (73.26), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.35), *maa://20791 (62.5)</t>
+          <t>maa://22742 (91.28), *maa://20791 (62.2)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.39), maa://36684 (93.38), ***maa://22731 (6.25)</t>
+          <t>maa://21246 (91.42), maa://36684 (93.2), ***maa://22731 (6.25)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (91.47), ***maa://21730 (27.85), ***maa://39501 (12.5), **maa://36675 (50.0)</t>
+          <t>maa://25251 (91.67), **maa://21730 (30.49), ***maa://39501 (11.36), **maa://36675 (50.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://40192 (96.1), maa://36987 (96.15), maa://39849 (88.89)</t>
+          <t>maa://40192 (96.63), maa://36987 (96.15), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.29), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.36), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (64.68), maa://20276 (87.43), *maa://22749 (80.0)</t>
+          <t>*maa://22880 (65.16), maa://20276 (87.82), *maa://22749 (75.0)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.36), maa://26254 (96.97), **maa://22738 (50.0)</t>
+          <t>maa://21249 (94.42), maa://26254 (97.14), **maa://22738 (50.0)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (90.32), maa://45854 (89.09), **maa://20790 (43.48), ***maa://37170 (17.14)</t>
+          <t>maa://24617 (90.48), maa://45854 (84.85), **maa://20790 (43.48), ***maa://37170 (17.14)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.32), maa://27484 (96.06), maa://27480 (83.33)</t>
+          <t>maa://27396 (84.35), maa://27484 (96.15), maa://27480 (83.78)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -880,12 +880,12 @@
       </c>
       <c r="AA3" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (95.29)</t>
+          <t>maa://24390 (95.4), maa://52241 (100.0)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -901,7 +901,7 @@
       </c>
       <c r="AF3" s="2" t="inlineStr">
         <is>
-          <t>*maa://21289 (74.19)</t>
+          <t>*maa://21289 (75.76)</t>
         </is>
       </c>
       <c r="AG3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.68), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.75), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -967,7 +967,7 @@
       </c>
       <c r="P4" s="2" t="inlineStr">
         <is>
-          <t>maa://49983 (94.59), maa://50121 (90.48)</t>
+          <t>maa://49983 (94.12), maa://50121 (92.0)</t>
         </is>
       </c>
       <c r="Q4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (95.2), maa://27295 (87.5), maa://22754 (89.19), *maa://31008 (79.07), *maa://21746 (54.55)</t>
+          <t>maa://32509 (94.49), maa://27295 (88.1), maa://22754 (89.19), *maa://31008 (79.07), *maa://21746 (54.55)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.74), ***maa://31785 (22.22), maa://43217 (91.92), ***maa://36683 (29.79)</t>
+          <t>**maa://32495 (48.57), maa://43217 (92.92), ***maa://31785 (22.22), ***maa://36683 (29.79)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (65.38), *maa://39394 (66.67), ***maa://26209 (13.04)</t>
+          <t>*maa://30062 (66.04), *maa://39394 (65.52), ***maa://26209 (13.04)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.73), maa://22744 (81.48)</t>
+          <t>maa://21245 (85.13), maa://22744 (81.48)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>*maa://22757 (78.57)</t>
+          <t>*maa://22757 (79.55)</t>
         </is>
       </c>
       <c r="M5" s="1" t="n"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="P5" s="2" t="inlineStr">
         <is>
-          <t>maa://21919 (96.83), *maa://21281 (80.0)</t>
+          <t>maa://21919 (96.92), *maa://21281 (80.0)</t>
         </is>
       </c>
       <c r="Q5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (94.29)</t>
+          <t>maa://42407 (94.74)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>maa://24370 (96.77)</t>
+          <t>maa://24370 (96.88)</t>
         </is>
       </c>
       <c r="I6" s="1" t="n"/>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>maa://24839 (98.76)</t>
+          <t>maa://24839 (98.79)</t>
         </is>
       </c>
       <c r="M6" s="1" t="n"/>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="P6" s="2" t="inlineStr">
         <is>
-          <t>maa://31836 (93.55), maa://30381 (94.12)</t>
+          <t>maa://31836 (93.94), maa://30381 (94.44)</t>
         </is>
       </c>
       <c r="Q6" s="1" t="n"/>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="T6" s="2" t="inlineStr">
         <is>
-          <t>maa://37411 (89.47)</t>
+          <t>maa://37411 (90.0)</t>
         </is>
       </c>
       <c r="U6" s="1" t="n"/>
@@ -1259,12 +1259,12 @@
       </c>
       <c r="W6" s="1" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X6" s="2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>maa://52754 (100.0)</t>
         </is>
       </c>
       <c r="Y6" s="1" t="n"/>
@@ -1280,7 +1280,7 @@
       </c>
       <c r="AB6" s="2" t="inlineStr">
         <is>
-          <t>maa://22739 (91.53)</t>
+          <t>maa://22739 (91.8)</t>
         </is>
       </c>
       <c r="AC6" s="1" t="n"/>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="AF6" s="2" t="inlineStr">
         <is>
-          <t>*maa://33152 (65.45), ***maa://22770 (26.09)</t>
+          <t>*maa://33152 (64.91), ***maa://22770 (26.09)</t>
         </is>
       </c>
       <c r="AG6" s="1" t="n"/>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>maa://21955 (95.45)</t>
+          <t>maa://21955 (93.62)</t>
         </is>
       </c>
       <c r="E7" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (93.02), maa://24957 (97.78)</t>
+          <t>maa://28624 (93.43), maa://24957 (97.78)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="P7" s="2" t="inlineStr">
         <is>
-          <t>maa://22750 (91.84)</t>
+          <t>maa://22750 (92.31)</t>
         </is>
       </c>
       <c r="Q7" s="1" t="n"/>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="T7" s="2" t="inlineStr">
         <is>
-          <t>maa://21291 (84.91)</t>
+          <t>maa://21291 (85.19)</t>
         </is>
       </c>
       <c r="U7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (95.95), *maa://22758 (76.92)</t>
+          <t>maa://22399 (96.07), *maa://22758 (77.22)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (68.6), *maa://36671 (68.0), maa://45272 (95.83), *maa://42530 (62.5)</t>
+          <t>*maa://26191 (67.82), *maa://36671 (68.63), maa://45272 (96.67), *maa://42530 (62.5)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.05.03 13:20:53</t>
+          <t>更新日期：2025.05.10 13:19:34</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>*maa://21476 (74.55), *maa://39431 (56.25), *maa://37551 (57.14)</t>
+          <t>*maa://21476 (75.44), *maa://39431 (56.25), **maa://37551 (50.0)</t>
         </is>
       </c>
       <c r="E8" s="1" t="n"/>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24371 (56.58)</t>
+          <t>*maa://24371 (55.84)</t>
         </is>
       </c>
       <c r="I8" s="1" t="n"/>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (84.0), *maa://21916 (62.12), maa://23252 (91.18), maa://37496 (97.14), **maa://22759 (45.45)</t>
+          <t>maa://32931 (84.73), *maa://21916 (62.69), maa://23252 (91.55), maa://37496 (97.22), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (96.01)</t>
+          <t>maa://21411 (96.13)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="AF8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24479 (79.35), *maa://21990 (51.85)</t>
+          <t>*maa://24479 (79.79), *maa://21990 (51.85)</t>
         </is>
       </c>
       <c r="AG8" s="1" t="n"/>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>maa://22765 (90.0), *maa://21915 (71.88)</t>
+          <t>maa://22765 (90.1), *maa://21915 (71.88)</t>
         </is>
       </c>
       <c r="E9" s="1" t="n"/>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="L9" s="2" t="inlineStr">
         <is>
-          <t>maa://22762 (92.71), maa://39552 (83.33)</t>
+          <t>maa://22762 (92.78), maa://39552 (83.33)</t>
         </is>
       </c>
       <c r="M9" s="1" t="n"/>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (83.33)</t>
+          <t>maa://22736 (83.64)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1643,7 +1643,7 @@
       </c>
       <c r="T9" s="2" t="inlineStr">
         <is>
-          <t>**maa://22866 (30.19), maa://26222 (98.18)</t>
+          <t>**maa://22866 (30.19), maa://26222 (98.25)</t>
         </is>
       </c>
       <c r="U9" s="1" t="n"/>
@@ -1654,12 +1654,12 @@
       </c>
       <c r="W9" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (98.06)</t>
+          <t>maa://26223 (98.09), maa://52237 (100.0)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (86.82), **maa://39938 (47.06), **maa://45044 (50.0), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (96.97)</t>
+          <t>maa://28711 (86.76), **maa://39938 (47.37), **maa://45044 (40.0), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (97.06)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (88.51), *maa://22865 (51.85)</t>
+          <t>maa://26206 (88.34), *maa://22865 (51.85)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.88), ***maa://39951 (11.94), ***maa://34206 (22.22), *maa://45271 (60.66), ***maa://39243 (25.0)</t>
+          <t>***maa://25695 (19.1), ***maa://39951 (12.86), ***maa://34206 (22.22), *maa://45271 (59.09), ***maa://39243 (25.0)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="H10" s="2" t="inlineStr">
         <is>
-          <t>maa://32651 (94.74)</t>
+          <t>maa://32651 (95.0)</t>
         </is>
       </c>
       <c r="I10" s="1" t="n"/>
@@ -1741,7 +1741,7 @@
       </c>
       <c r="L10" s="2" t="inlineStr">
         <is>
-          <t>**maa://24395 (39.39)</t>
+          <t>**maa://24395 (40.0)</t>
         </is>
       </c>
       <c r="M10" s="1" t="n"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (88.64), maa://36669 (84.0), *maa://23264 (60.71)</t>
+          <t>maa://28977 (88.42), maa://36669 (82.35), *maa://23264 (60.71)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.38), maa://22755 (88.52), **maa://22756 (40.91), ***maa://21737 (11.76)</t>
+          <t>maa://27395 (96.49), maa://22755 (88.62), **maa://22756 (40.91), ***maa://21737 (11.76)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.8), maa://45828 (93.33), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.85), maa://45828 (92.5), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (53.92), *maa://22733 (62.16), **maa://22761 (50.0)</t>
+          <t>*maa://25021 (53.85), *maa://22733 (64.1), **maa://22761 (50.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.32)</t>
+          <t>maa://36707 (99.35)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (89.19)</t>
+          <t>maa://21287 (88.39)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="P11" s="2" t="inlineStr">
         <is>
-          <t>maa://45557 (90.91)</t>
+          <t>maa://45557 (91.67)</t>
         </is>
       </c>
       <c r="Q11" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (91.23), maa://22501 (98.0), maa://45521 (89.66)</t>
+          <t>maa://22747 (90.8), maa://22501 (98.08), maa://45521 (90.91)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (97.97)</t>
+          <t>maa://36713 (98.05)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1935,7 +1935,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://29912 (97.5), maa://22516 (87.36), *maa://20794 (54.17)</t>
+          <t>maa://29912 (97.7), maa://22516 (87.36), *maa://20794 (54.67)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (90.4), **maa://45826 (36.36)</t>
+          <t>maa://21867 (90.81), **maa://45826 (36.36)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.33), *maa://21485 (75.17), maa://37962 (92.59)</t>
+          <t>maa://22753 (91.67), *maa://21485 (75.51), maa://37962 (91.53)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.61), maa://36677 (94.67), maa://39872 (92.59)</t>
+          <t>maa://23669 (95.64), maa://36677 (95.06), maa://39872 (92.86)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (79.14), *maa://20106 (63.96), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (79.29), *maa://20106 (64.29), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.57), maa://36673 (92.86), maa://25001 (85.92)</t>
+          <t>maa://24999 (92.67), maa://36673 (92.86), maa://25001 (86.3)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.48), **maa://22728 (46.67)</t>
+          <t>*maa://21248 (73.9), **maa://22728 (45.65)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (93.28), *maa://22583 (76.39), *maa://22500 (59.57), maa://48321 (100.0)</t>
+          <t>maa://22676 (93.53), *maa://22583 (77.33), *maa://22500 (59.57), maa://48321 (100.0)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>maa://34957 (80.65), **maa://22768 (50.0)</t>
+          <t>maa://34957 (82.0), **maa://22768 (50.0)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (37.42), maa://39883 (90.82), *maa://39885 (51.52)</t>
+          <t>**maa://22737 (38.22), maa://39883 (88.39), *maa://39885 (52.63)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>maa://30764 (88.71)</t>
+          <t>maa://30764 (89.55)</t>
         </is>
       </c>
       <c r="E14" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://39841 (94.93), maa://26245 (96.41), maa://21288 (96.3), maa://36682 (97.67)</t>
+          <t>maa://39841 (94.56), maa://26245 (96.53), maa://21288 (96.3), maa://36682 (95.56)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.79), maa://20107 (87.1), maa://22772 (100.0), *maa://22745 (66.67)</t>
+          <t>maa://23250 (98.8), maa://20107 (87.1), maa://22772 (100.0), *maa://22745 (66.67)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="T14" s="2" t="inlineStr">
         <is>
-          <t>maa://22521 (94.78), maa://42751 (100.0)</t>
+          <t>maa://22521 (94.83), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="1" t="n"/>
@@ -2309,7 +2309,7 @@
       </c>
       <c r="X14" s="2" t="inlineStr">
         <is>
-          <t>maa://37468 (91.3)</t>
+          <t>maa://37468 (91.67)</t>
         </is>
       </c>
       <c r="Y14" s="1" t="n"/>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="AB14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (96.1)</t>
+          <t>maa://22764 (96.2)</t>
         </is>
       </c>
       <c r="AC14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.76), maa://22734 (84.43), *maa://30808 (64.18), *maa://36048 (62.07), maa://45058 (88.89)</t>
+          <t>*maa://22743 (79.06), maa://22734 (84.43), *maa://30808 (64.71), *maa://36048 (63.83), maa://45058 (88.89)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (86.64), maa://21478 (90.0)</t>
+          <t>maa://24304 (86.61), maa://21478 (90.0)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2391,7 +2391,7 @@
       </c>
       <c r="L15" s="2" t="inlineStr">
         <is>
-          <t>*maa://21334 (54.84)</t>
+          <t>*maa://21334 (56.25)</t>
         </is>
       </c>
       <c r="M15" s="1" t="n"/>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (90.91), *maa://22727 (70.0)</t>
+          <t>maa://24762 (91.06), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="T15" s="2" t="inlineStr">
         <is>
-          <t>maa://23892 (96.43)</t>
+          <t>maa://23892 (96.47)</t>
         </is>
       </c>
       <c r="U15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (80.79), maa://36666 (80.15), *maa://22766 (68.6)</t>
+          <t>maa://21364 (81.22), maa://36666 (80.85), *maa://22766 (68.6)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.49), maa://37650 (98.0), maa://36679 (94.55)</t>
+          <t>maa://21441 (96.52), maa://37650 (96.23), maa://36679 (94.55)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2537,7 +2537,7 @@
       </c>
       <c r="P16" s="2" t="inlineStr">
         <is>
-          <t>maa://28504 (92.42)</t>
+          <t>maa://28504 (92.54)</t>
         </is>
       </c>
       <c r="Q16" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.38), *maa://28648 (71.62), *maa://36674 (79.31)</t>
+          <t>maa://22729 (94.44), *maa://28648 (72.0), *maa://36674 (79.31)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (98.2), maa://28051 (96.0)</t>
+          <t>maa://28501 (98.23), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (66.96), maa://27755 (93.75)</t>
+          <t>*maa://23911 (67.83), maa://27755 (93.88)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (89.16), maa://39599 (84.62)</t>
+          <t>maa://22430 (89.37), maa://39599 (86.3)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2651,7 +2651,7 @@
       </c>
       <c r="L17" s="2" t="inlineStr">
         <is>
-          <t>*maa://21679 (76.92)</t>
+          <t>*maa://21679 (77.78)</t>
         </is>
       </c>
       <c r="M17" s="1" t="n"/>
@@ -2667,7 +2667,7 @@
       </c>
       <c r="P17" s="2" t="inlineStr">
         <is>
-          <t>maa://23890 (80.56), *maa://24940 (67.86)</t>
+          <t>maa://23890 (80.91), *maa://24940 (67.86)</t>
         </is>
       </c>
       <c r="Q17" s="1" t="n"/>
@@ -2731,7 +2731,7 @@
       </c>
       <c r="AF17" s="2" t="inlineStr">
         <is>
-          <t>maa://50136 (92.86)</t>
+          <t>maa://50136 (94.12)</t>
         </is>
       </c>
       <c r="AG17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.79)</t>
+          <t>maa://24570 (96.9)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (87.59)</t>
+          <t>maa://24421 (87.78)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2776,12 +2776,12 @@
       </c>
       <c r="K18" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (91.67), *maa://22732 (50.47)</t>
+          <t>maa://22466 (92.08), *maa://22732 (50.93), maa://52226 (100.0)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="X18" s="2" t="inlineStr">
         <is>
-          <t>maa://21917 (97.0), maa://22741 (87.5)</t>
+          <t>maa://21917 (97.09), maa://22741 (87.5)</t>
         </is>
       </c>
       <c r="Y18" s="1" t="n"/>
@@ -2845,7 +2845,7 @@
       </c>
       <c r="AB18" s="2" t="inlineStr">
         <is>
-          <t>maa://24393 (98.0)</t>
+          <t>maa://24393 (98.04)</t>
         </is>
       </c>
       <c r="AC18" s="1" t="n"/>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (60.23), **maa://29784 (50.0), *maa://47854 (75.0)</t>
+          <t>*maa://24313 (60.23), **maa://29784 (50.0), *maa://47854 (80.0)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -2911,7 +2911,7 @@
       </c>
       <c r="L19" s="2" t="inlineStr">
         <is>
-          <t>maa://39347 (93.75)</t>
+          <t>maa://39347 (94.44)</t>
         </is>
       </c>
       <c r="M19" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (98.53)</t>
+          <t>maa://24386 (98.6)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (67.17), *maa://36668 (57.32)</t>
+          <t>*maa://30709 (67.52), *maa://36668 (57.32)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.62), maa://25198 (94.31), *maa://20795 (50.77), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.77), maa://25198 (94.4), *maa://20795 (50.76), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (90.17), ***maa://43283 (25.0)</t>
+          <t>maa://22864 (90.5), ***maa://43283 (25.0)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (84.65)</t>
+          <t>maa://41331 (85.65)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="T20" s="2" t="inlineStr">
         <is>
-          <t>maa://29113 (87.1)</t>
+          <t>maa://29113 (87.5)</t>
         </is>
       </c>
       <c r="U20" s="1" t="n"/>
@@ -3089,7 +3089,7 @@
       </c>
       <c r="X20" s="2" t="inlineStr">
         <is>
-          <t>maa://49976 (85.92), maa://50085 (88.46)</t>
+          <t>maa://50085 (89.16), maa://49976 (85.71)</t>
         </is>
       </c>
       <c r="Y20" s="1" t="n"/>
@@ -3139,7 +3139,7 @@
       </c>
       <c r="D21" s="2" t="inlineStr">
         <is>
-          <t>maa://21261 (97.78)</t>
+          <t>maa://21261 (97.92)</t>
         </is>
       </c>
       <c r="E21" s="1" t="n"/>
@@ -3171,7 +3171,7 @@
       </c>
       <c r="L21" s="2" t="inlineStr">
         <is>
-          <t>maa://31731 (96.3)</t>
+          <t>maa://31731 (96.43)</t>
         </is>
       </c>
       <c r="M21" s="1" t="n"/>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="X21" s="2" t="inlineStr">
         <is>
-          <t>maa://20110 (86.76), maa://34946 (92.16)</t>
+          <t>maa://20110 (86.76), maa://34946 (92.98)</t>
         </is>
       </c>
       <c r="Y21" s="1" t="n"/>
@@ -3230,12 +3230,12 @@
       </c>
       <c r="AA21" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (82.29), ***maa://23820 (30.0)</t>
+          <t>maa://21443 (82.51), ***maa://23820 (30.0), **maa://52223 (44.44)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (91.56), maa://22432 (80.2)</t>
+          <t>maa://22524 (91.7), maa://22432 (81.82)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>maa://25236 (95.92), **maa://21678 (48.94), **maa://22735 (42.86)</t>
+          <t>maa://25236 (96.08), **maa://21678 (48.94), **maa://22735 (42.86)</t>
         </is>
       </c>
       <c r="I22" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>*maa://27127 (78.12), *maa://22751 (71.83)</t>
+          <t>*maa://27127 (78.46), *maa://22751 (70.83)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.68), *maa://37649 (65.62)</t>
+          <t>maa://21282 (98.7), *maa://37649 (68.57)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="AF22" s="2" t="inlineStr">
         <is>
-          <t>maa://29658 (94.34)</t>
+          <t>maa://29658 (94.44)</t>
         </is>
       </c>
       <c r="AG22" s="1" t="n"/>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (27.63), **maa://41753 (50.0)</t>
+          <t>***maa://28036 (26.92), **maa://41753 (50.0)</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.14), maa://39875 (94.67)</t>
+          <t>maa://39756 (95.38), maa://39875 (94.67)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.79), *maa://29748 (76.12), ***maa://29785 (17.39), *maa://37566 (76.74)</t>
+          <t>maa://30587 (91.87), *maa://29748 (76.3), ***maa://29785 (17.39), *maa://37566 (78.26)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="T23" s="2" t="inlineStr">
         <is>
-          <t>maa://31212 (93.94), maa://24387 (82.05)</t>
+          <t>maa://31212 (91.43), maa://24387 (82.5)</t>
         </is>
       </c>
       <c r="U23" s="1" t="n"/>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="X23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (69.32)</t>
+          <t>*maa://28503 (68.13)</t>
         </is>
       </c>
       <c r="Y23" s="1" t="n"/>
@@ -3511,7 +3511,7 @@
       </c>
       <c r="AF23" s="2" t="inlineStr">
         <is>
-          <t>maa://31489 (94.74)</t>
+          <t>maa://31489 (95.0)</t>
         </is>
       </c>
       <c r="AG23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.8), *maa://46650 (57.89)</t>
+          <t>*maa://24368 (78.96), *maa://46650 (66.67)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3604,12 +3604,12 @@
       </c>
       <c r="W24" s="1" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (83.81), maa://23504 (93.46), **maa://22892 (41.56), *maa://25141 (77.04), *maa://36663 (79.12), ***maa://22815 (23.08)</t>
+          <t>maa://29988 (84.1), maa://23504 (93.52), **maa://22892 (41.29), *maa://25141 (77.37), *maa://36663 (77.78), ***maa://22815 (23.08), maa://52227 (100.0)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (84.54), *maa://36672 (78.33), maa://29910 (93.55), **maa://21440 (35.71), maa://45831 (91.67)</t>
+          <t>maa://22523 (83.49), *maa://36672 (77.42), maa://29910 (93.65), **maa://21440 (35.71), maa://45831 (84.62)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.12)</t>
+          <t>maa://29753 (95.29)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (73.03), *maa://25311 (73.64), ***maa://22725 (4.76), *maa://45047 (66.67)</t>
+          <t>*maa://29063 (73.37), *maa://25311 (74.11), ***maa://22725 (4.76), *maa://45047 (72.73)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3691,7 +3691,7 @@
       </c>
       <c r="L25" s="2" t="inlineStr">
         <is>
-          <t>maa://24378 (88.37)</t>
+          <t>maa://24378 (88.64)</t>
         </is>
       </c>
       <c r="M25" s="1" t="n"/>
@@ -3707,7 +3707,7 @@
       </c>
       <c r="P25" s="2" t="inlineStr">
         <is>
-          <t>maa://24382 (93.94)</t>
+          <t>maa://24382 (94.12)</t>
         </is>
       </c>
       <c r="Q25" s="1" t="n"/>
@@ -3723,7 +3723,7 @@
       </c>
       <c r="T25" s="2" t="inlineStr">
         <is>
-          <t>maa://20109 (92.47), maa://22545 (100.0), *maa://42915 (75.0)</t>
+          <t>maa://20109 (92.51), maa://22545 (100.0), *maa://42915 (75.0)</t>
         </is>
       </c>
       <c r="U25" s="1" t="n"/>
@@ -3739,7 +3739,7 @@
       </c>
       <c r="X25" s="2" t="inlineStr">
         <is>
-          <t>maa://29890 (81.48)</t>
+          <t>maa://29890 (82.46)</t>
         </is>
       </c>
       <c r="Y25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (89.15), maa://24516 (80.22), maa://26001 (85.96)</t>
+          <t>maa://31215 (89.39), maa://24516 (80.22), maa://26001 (84.48)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.48), maa://24621 (97.04), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
+          <t>maa://20108 (96.48), maa://24621 (97.14), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>maa://41802 (92.0)</t>
+          <t>maa://41802 (93.1)</t>
         </is>
       </c>
       <c r="E26" s="1" t="n"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (91.49)</t>
+          <t>maa://24913 (91.67)</t>
         </is>
       </c>
       <c r="I26" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (95.45)</t>
+          <t>maa://42235 (95.59)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (47.37), *maa://39601 (76.19), maa://34494 (97.14), **maa://36665 (50.0)</t>
+          <t>**maa://21283 (47.37), *maa://39601 (78.26), maa://34494 (97.14), **maa://36665 (50.0)</t>
         </is>
       </c>
       <c r="I27" s="1" t="n"/>
@@ -3951,7 +3951,7 @@
       </c>
       <c r="L27" s="2" t="inlineStr">
         <is>
-          <t>maa://28071 (90.91)</t>
+          <t>maa://28071 (91.3)</t>
         </is>
       </c>
       <c r="M27" s="1" t="n"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (76.92)</t>
+          <t>*maa://30624 (76.47)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.89), maa://25725 (84.95)</t>
+          <t>maa://24465 (90.61), maa://25725 (85.11)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>*maa://29765 (65.59), maa://23263 (95.33)</t>
+          <t>*maa://29765 (65.96), maa://23263 (95.41)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (91.44), maa://41749 (92.44), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (91.72), maa://41749 (91.6), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.6), *maa://36701 (67.74)</t>
+          <t>maa://36660 (92.63), *maa://36701 (66.67)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4179,7 +4179,7 @@
       </c>
       <c r="D29" s="2" t="inlineStr">
         <is>
-          <t>maa://31694 (98.28)</t>
+          <t>maa://31694 (98.31)</t>
         </is>
       </c>
       <c r="E29" s="1" t="n"/>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>*maa://25175 (63.79)</t>
+          <t>*maa://25175 (61.67)</t>
         </is>
       </c>
       <c r="I29" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.87), maa://28440 (82.54), maa://31400 (98.84), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.92), maa://28440 (83.33), maa://31400 (98.88), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.09), maa://42865 (83.33), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (69.17), maa://42865 (81.63), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4309,7 +4309,7 @@
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>maa://45792 (88.0)</t>
+          <t>maa://45792 (88.46)</t>
         </is>
       </c>
       <c r="E30" s="1" t="n"/>
@@ -4341,7 +4341,7 @@
       </c>
       <c r="L30" s="2" t="inlineStr">
         <is>
-          <t>maa://30442 (95.59)</t>
+          <t>maa://30442 (95.65)</t>
         </is>
       </c>
       <c r="M30" s="1" t="n"/>
@@ -4357,7 +4357,7 @@
       </c>
       <c r="P30" s="2" t="inlineStr">
         <is>
-          <t>maa://21442 (98.72)</t>
+          <t>maa://21442 (98.74)</t>
         </is>
       </c>
       <c r="Q30" s="1" t="n"/>
@@ -4373,7 +4373,7 @@
       </c>
       <c r="T30" s="2" t="inlineStr">
         <is>
-          <t>*maa://32940 (66.67), maa://24388 (94.74)</t>
+          <t>*maa://32940 (70.0), maa://24388 (94.74)</t>
         </is>
       </c>
       <c r="U30" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (97.46), maa://45822 (100.0), *maa://45045 (80.0)</t>
+          <t>maa://42979 (96.73), maa://45822 (100.0), maa://45045 (83.33)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.69), maa://36258 (86.43), *maa://43904 (76.92)</t>
+          <t>maa://35926 (93.83), maa://36258 (86.75), *maa://43904 (71.43)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4535,7 +4535,7 @@
       </c>
       <c r="AB31" s="2" t="inlineStr">
         <is>
-          <t>**maa://51420 (50.0)</t>
+          <t>**maa://51420 (33.33)</t>
         </is>
       </c>
       <c r="AC31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.37), maa://36667 (97.94), **maa://20793 (38.78), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.49), maa://36667 (98.0), **maa://20793 (38.0), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4601,7 +4601,7 @@
       </c>
       <c r="L32" s="2" t="inlineStr">
         <is>
-          <t>maa://28065 (95.92)</t>
+          <t>maa://28065 (96.0)</t>
         </is>
       </c>
       <c r="M32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (97.04), maa://41108 (88.0), maa://41238 (97.64), maa://45523 (100.0)</t>
+          <t>maa://42859 (97.22), maa://41108 (88.0), maa://41238 (97.81), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4681,7 +4681,7 @@
       </c>
       <c r="AF32" s="2" t="inlineStr">
         <is>
-          <t>maa://42408 (86.67)</t>
+          <t>maa://42408 (87.5)</t>
         </is>
       </c>
       <c r="AG32" s="1" t="n"/>
@@ -4747,7 +4747,7 @@
       </c>
       <c r="P33" s="2" t="inlineStr">
         <is>
-          <t>maa://21956 (81.17), *maa://22730 (76.67)</t>
+          <t>maa://21956 (81.65), *maa://22730 (74.19)</t>
         </is>
       </c>
       <c r="Q33" s="1" t="n"/>
@@ -4877,7 +4877,7 @@
       </c>
       <c r="P34" s="2" t="inlineStr">
         <is>
-          <t>maa://48817 (95.24)</t>
+          <t>maa://48817 (95.92)</t>
         </is>
       </c>
       <c r="Q34" s="1" t="n"/>
@@ -4991,7 +4991,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (96.97)</t>
+          <t>maa://41296 (97.12)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5023,7 +5023,7 @@
       </c>
       <c r="T35" s="2" t="inlineStr">
         <is>
-          <t>maa://24842 (94.44)</t>
+          <t>maa://24842 (94.64)</t>
         </is>
       </c>
       <c r="U35" s="1" t="n"/>
@@ -5071,7 +5071,7 @@
       </c>
       <c r="AF35" s="2" t="inlineStr">
         <is>
-          <t>maa://39479 (90.91)</t>
+          <t>maa://39479 (91.3)</t>
         </is>
       </c>
       <c r="AG35" s="1" t="n"/>
@@ -5219,7 +5219,7 @@
       </c>
       <c r="H37" s="2" t="inlineStr">
         <is>
-          <t>*maa://24374 (55.32)</t>
+          <t>*maa://24374 (56.25)</t>
         </is>
       </c>
       <c r="I37" s="1" t="n"/>
@@ -5235,7 +5235,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (98.17), *maa://47069 (77.78), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.28), *maa://47069 (78.95), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5251,7 +5251,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.78), *maa://21239 (69.23)</t>
+          <t>maa://21280 (89.96), *maa://21239 (69.23)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5352,7 +5352,7 @@
       </c>
       <c r="P38" s="2" t="inlineStr">
         <is>
-          <t>*maa://24383 (70.09)</t>
+          <t>*maa://24383 (69.44)</t>
         </is>
       </c>
       <c r="Q38" s="1" t="n"/>
@@ -5400,7 +5400,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (88.12)</t>
+          <t>maa://36697 (88.73)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (88.68), maa://25199 (85.22), maa://30434 (91.96), maa://45059 (82.14), ***maa://25036 (18.52), *maa://44165 (66.67)</t>
+          <t>maa://36670 (88.89), maa://25199 (85.22), maa://30434 (92.44), maa://45059 (80.65), ***maa://25036 (18.52), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5453,7 +5453,7 @@
       </c>
       <c r="P39" s="2" t="inlineStr">
         <is>
-          <t>maa://24709 (92.02), maa://47093 (100.0)</t>
+          <t>maa://24709 (91.62), maa://47093 (100.0)</t>
         </is>
       </c>
       <c r="Q39" s="1" t="n"/>
@@ -5469,7 +5469,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>*maa://45788 (76.32), maa://47079 (95.31), *maa://45790 (75.0)</t>
+          <t>maa://47079 (94.81), *maa://45788 (76.32), *maa://45790 (79.17)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5554,7 +5554,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.11), maa://21386 (95.79), maa://36664 (89.66), maa://45550 (87.5)</t>
+          <t>maa://23278 (95.17), maa://21386 (95.79), maa://36664 (89.66), maa://45550 (87.5)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5639,7 +5639,7 @@
       </c>
       <c r="P41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (40.0), maa://43177 (92.31)</t>
+          <t>**maa://35616 (40.0), maa://43177 (93.1)</t>
         </is>
       </c>
       <c r="Q41" s="1" t="n"/>
@@ -5777,7 +5777,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (89.47), maa://21284 (86.27)</t>
+          <t>maa://22525 (88.96), maa://21284 (87.04)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5809,7 +5809,7 @@
       </c>
       <c r="P43" s="2" t="inlineStr">
         <is>
-          <t>maa://47403 (87.5)</t>
+          <t>*maa://47403 (80.0)</t>
         </is>
       </c>
       <c r="Q43" s="1" t="n"/>
@@ -5862,7 +5862,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (98.15), maa://27728 (96.12)</t>
+          <t>maa://29768 (98.21), maa://27728 (96.15)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5931,7 +5931,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.46), maa://30807 (95.83), *maa://22767 (55.0), maa://42459 (90.32), ***maa://20796 (13.79)</t>
+          <t>maa://21229 (84.54), maa://30807 (94.59), *maa://22767 (55.0), maa://42459 (91.43), ***maa://20796 (13.79)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5963,7 +5963,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (40.0)</t>
+          <t>**maa://39364 (46.0)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -6000,7 +6000,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.53), maa://43901 (95.45)</t>
+          <t>maa://35931 (92.46), maa://43901 (95.92)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6053,7 +6053,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.73), maa://29661 (97.45), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.81), maa://29661 (97.52), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6175,7 +6175,7 @@
       </c>
       <c r="P49" s="2" t="inlineStr">
         <is>
-          <t>*maa://39643 (61.54)</t>
+          <t>*maa://39643 (57.14)</t>
         </is>
       </c>
       <c r="Q49" s="1" t="n"/>
@@ -6312,7 +6312,7 @@
       </c>
       <c r="H52" s="2" t="inlineStr">
         <is>
-          <t>maa://24376 (96.77)</t>
+          <t>maa://24376 (96.88)</t>
         </is>
       </c>
       <c r="I52" s="1" t="n"/>
@@ -6362,7 +6362,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.58), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.75), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6430,7 +6430,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.77)</t>
+          <t>maa://32532 (92.9)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6466,7 +6466,7 @@
       </c>
       <c r="H57" s="2" t="inlineStr">
         <is>
-          <t>maa://25176 (98.46)</t>
+          <t>maa://25176 (98.51)</t>
         </is>
       </c>
       <c r="I57" s="1" t="n"/>
@@ -6484,7 +6484,7 @@
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>*maa://37964 (56.86)</t>
+          <t>*maa://37964 (54.72)</t>
         </is>
       </c>
       <c r="I58" s="1" t="n"/>
@@ -6502,7 +6502,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://31270 (94.24), maa://27746 (82.91)</t>
+          <t>maa://31270 (94.41), maa://27746 (82.91)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6520,7 +6520,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (72.86)</t>
+          <t>*maa://40438 (72.6)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>
@@ -6556,7 +6556,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (96.0), maa://43903 (100.0)</t>
+          <t>maa://42981 (96.23), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>
@@ -6592,7 +6592,7 @@
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>maa://44405 (85.29)</t>
+          <t>maa://44405 (85.71)</t>
         </is>
       </c>
       <c r="I64" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#187)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://25390 (95.33), maa://24702 (94.74), maa://36681 (86.42)</t>
+          <t>maa://25390 (95.35), maa://24702 (94.77), maa://36681 (86.42)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>maa://39402 (94.23), *maa://24633 (56.1), *maa://30515 (70.09), *maa://34787 (73.26), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
+          <t>maa://39402 (94.23), *maa://24633 (56.1), *maa://30515 (70.09), *maa://34787 (73.56), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.28), *maa://20791 (62.2)</t>
+          <t>maa://22742 (91.33), *maa://20791 (62.2)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.42), maa://36684 (93.2), ***maa://22731 (6.25)</t>
+          <t>maa://21246 (91.42), maa://36684 (93.29), ***maa://22731 (6.25)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (91.67), **maa://21730 (30.49), ***maa://39501 (11.36), **maa://36675 (50.0)</t>
+          <t>maa://25251 (91.79), **maa://21730 (30.49), ***maa://39501 (11.36), **maa://36675 (50.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.36), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.37), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.16), maa://20276 (87.82), *maa://22749 (75.0)</t>
+          <t>*maa://22880 (65.02), maa://20276 (88.0), *maa://22749 (75.0)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.42), maa://26254 (97.14), **maa://22738 (50.0)</t>
+          <t>maa://21249 (94.51), maa://26254 (97.14), **maa://22738 (50.0)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (90.48), maa://45854 (84.85), **maa://20790 (43.48), ***maa://37170 (17.14)</t>
+          <t>maa://24617 (90.55), maa://45854 (85.29), **maa://20790 (43.48), ***maa://37170 (16.67)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.35), maa://27484 (96.15), maa://27480 (83.78)</t>
+          <t>maa://27396 (84.35), maa://27484 (96.21), maa://27480 (83.78)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -967,7 +967,7 @@
       </c>
       <c r="P4" s="2" t="inlineStr">
         <is>
-          <t>maa://49983 (94.12), maa://50121 (92.0)</t>
+          <t>maa://49983 (94.34), maa://50121 (92.0)</t>
         </is>
       </c>
       <c r="Q4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (94.49), maa://27295 (88.1), maa://22754 (89.19), *maa://31008 (79.07), *maa://21746 (54.55)</t>
+          <t>maa://32509 (94.53), maa://27295 (88.24), maa://22754 (89.19), *maa://31008 (79.07), *maa://21746 (54.55)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.57), maa://43217 (92.92), ***maa://31785 (22.22), ***maa://36683 (29.79)</t>
+          <t>**maa://32495 (48.4), maa://43217 (92.92), ***maa://31785 (22.22), ***maa://36683 (29.79)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (66.04), *maa://39394 (65.52), ***maa://26209 (13.04)</t>
+          <t>*maa://30062 (65.45), *maa://39394 (65.52), ***maa://26209 (13.04)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (85.13), maa://22744 (81.48)</t>
+          <t>maa://21245 (84.93), maa://22744 (81.48)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (94.74)</t>
+          <t>maa://42407 (94.81)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>maa://24839 (98.79)</t>
+          <t>maa://24839 (98.8)</t>
         </is>
       </c>
       <c r="M6" s="1" t="n"/>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="AF6" s="2" t="inlineStr">
         <is>
-          <t>*maa://33152 (64.91), ***maa://22770 (26.09)</t>
+          <t>*maa://33152 (63.79), ***maa://22770 (26.09)</t>
         </is>
       </c>
       <c r="AG6" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (93.43), maa://24957 (97.78)</t>
+          <t>maa://28624 (93.53), maa://24957 (97.78)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (67.82), *maa://36671 (68.63), maa://45272 (96.67), *maa://42530 (62.5)</t>
+          <t>*maa://26191 (67.82), *maa://36671 (69.23), maa://45272 (96.67), *maa://42530 (62.5)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.05.10 13:19:34</t>
+          <t>更新日期：2025.05.11 13:19:54</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (84.73), *maa://21916 (62.69), maa://23252 (91.55), maa://37496 (97.22), **maa://22759 (45.45)</t>
+          <t>maa://32931 (84.09), *maa://21916 (62.69), maa://23252 (91.55), maa://37496 (97.22), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (83.64)</t>
+          <t>maa://22736 (82.88)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1643,7 +1643,7 @@
       </c>
       <c r="T9" s="2" t="inlineStr">
         <is>
-          <t>**maa://22866 (30.19), maa://26222 (98.25)</t>
+          <t>**maa://22866 (30.19), maa://26222 (98.28)</t>
         </is>
       </c>
       <c r="U9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (86.76), **maa://39938 (47.37), **maa://45044 (40.0), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (97.06)</t>
+          <t>maa://28711 (86.76), **maa://39938 (45.0), **maa://45044 (40.0), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (97.06)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1741,7 +1741,7 @@
       </c>
       <c r="L10" s="2" t="inlineStr">
         <is>
-          <t>**maa://24395 (40.0)</t>
+          <t>**maa://24395 (38.89)</t>
         </is>
       </c>
       <c r="M10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.49), maa://22755 (88.62), **maa://22756 (40.91), ***maa://21737 (11.76)</t>
+          <t>maa://27395 (96.52), maa://22755 (88.62), **maa://22756 (40.91), ***maa://21737 (11.76)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.85), maa://45828 (92.5), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.85), maa://45828 (92.68), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.67), *maa://21485 (75.51), maa://37962 (91.53)</t>
+          <t>maa://22753 (91.67), *maa://21485 (75.51), maa://37962 (91.67)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.64), maa://36677 (95.06), maa://39872 (92.86)</t>
+          <t>maa://23669 (95.64), maa://36677 (95.12), maa://39872 (92.86)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (79.29), *maa://20106 (64.29), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (79.53), *maa://20106 (64.29), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.67), maa://36673 (92.86), maa://25001 (86.3)</t>
+          <t>maa://24999 (92.57), maa://36673 (92.94), maa://25001 (86.3)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (93.53), *maa://22583 (77.33), *maa://22500 (59.57), maa://48321 (100.0)</t>
+          <t>maa://22676 (93.53), *maa://22583 (77.63), *maa://22500 (59.57), maa://48321 (100.0)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (38.22), maa://39883 (88.39), *maa://39885 (52.63)</t>
+          <t>**maa://22737 (38.22), maa://39883 (87.72), *maa://39885 (52.63)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://39841 (94.56), maa://26245 (96.53), maa://21288 (96.3), maa://36682 (95.56)</t>
+          <t>maa://39841 (94.59), maa://26245 (96.53), maa://21288 (96.3), maa://36682 (95.56)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.8), maa://20107 (87.1), maa://22772 (100.0), *maa://22745 (66.67)</t>
+          <t>maa://23250 (98.81), maa://20107 (87.1), maa://22772 (100.0), *maa://22745 (66.67)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="AB14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (96.2)</t>
+          <t>maa://22764 (96.25)</t>
         </is>
       </c>
       <c r="AC14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (79.06), maa://22734 (84.43), *maa://30808 (64.71), *maa://36048 (63.83), maa://45058 (88.89)</t>
+          <t>*maa://22743 (79.06), maa://22734 (84.43), *maa://30808 (65.22), *maa://36048 (64.58), maa://45058 (84.21)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (86.61), maa://21478 (90.0)</t>
+          <t>maa://24304 (86.67), maa://21478 (90.0)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.22), maa://36666 (80.85), *maa://22766 (68.6)</t>
+          <t>maa://21364 (81.27), maa://36666 (81.12), *maa://22766 (68.03)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (67.83), maa://27755 (93.88)</t>
+          <t>*maa://23911 (68.1), maa://27755 (93.88)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (89.37), maa://39599 (86.3)</t>
+          <t>maa://22430 (89.42), maa://39599 (85.14)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2731,7 +2731,7 @@
       </c>
       <c r="AF17" s="2" t="inlineStr">
         <is>
-          <t>maa://50136 (94.12)</t>
+          <t>maa://50136 (94.44)</t>
         </is>
       </c>
       <c r="AG17" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (87.78)</t>
+          <t>maa://24421 (87.82)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (92.08), *maa://22732 (50.93), maa://52226 (100.0)</t>
+          <t>maa://22466 (92.08), *maa://22732 (51.38), maa://52226 (100.0)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.77), maa://25198 (94.4), *maa://20795 (50.76), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.82), maa://25198 (94.4), *maa://20795 (50.76), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3020,12 +3020,12 @@
       </c>
       <c r="G20" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (90.5), ***maa://43283 (25.0)</t>
+          <t>maa://22864 (90.5), ***maa://43283 (25.0), maa://53361 (100.0)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.65)</t>
+          <t>maa://41331 (85.71)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3089,7 +3089,7 @@
       </c>
       <c r="X20" s="2" t="inlineStr">
         <is>
-          <t>maa://50085 (89.16), maa://49976 (85.71)</t>
+          <t>maa://50085 (88.64), maa://49976 (85.71)</t>
         </is>
       </c>
       <c r="Y20" s="1" t="n"/>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="X21" s="2" t="inlineStr">
         <is>
-          <t>maa://20110 (86.76), maa://34946 (92.98)</t>
+          <t>maa://20110 (86.76), maa://34946 (93.1)</t>
         </is>
       </c>
       <c r="Y21" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (82.51), ***maa://23820 (30.0), **maa://52223 (44.44)</t>
+          <t>maa://21443 (82.56), ***maa://23820 (30.0), **maa://52223 (38.46)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (91.7), maa://22432 (81.82)</t>
+          <t>maa://22524 (90.95), maa://22432 (81.98)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L22" s="2" t="inlineStr">
         <is>
-          <t>*maa://27127 (78.46), *maa://22751 (70.83)</t>
+          <t>*maa://27127 (78.46), *maa://22751 (71.23)</t>
         </is>
       </c>
       <c r="M22" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.7), *maa://37649 (68.57)</t>
+          <t>maa://21282 (98.7), *maa://37649 (69.44)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.38), maa://39875 (94.67)</t>
+          <t>maa://39756 (95.41), maa://39875 (94.67)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (84.1), maa://23504 (93.52), **maa://22892 (41.29), *maa://25141 (77.37), *maa://36663 (77.78), ***maa://22815 (23.08), maa://52227 (100.0)</t>
+          <t>maa://29988 (84.1), maa://23504 (93.53), **maa://22892 (41.29), *maa://25141 (77.37), *maa://36663 (77.78), ***maa://22815 (23.08), maa://52227 (100.0)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (83.49), *maa://36672 (77.42), maa://29910 (93.65), **maa://21440 (35.71), maa://45831 (84.62)</t>
+          <t>maa://22523 (82.71), *maa://36672 (76.19), maa://29910 (93.75), **maa://21440 (35.71), maa://45831 (84.62)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.29)</t>
+          <t>maa://29753 (95.3)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (89.39), maa://24516 (80.22), maa://26001 (84.48)</t>
+          <t>maa://31215 (89.47), maa://24516 (80.22), maa://26001 (84.48)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="AF25" s="2" t="inlineStr">
         <is>
-          <t>maa://20108 (96.48), maa://24621 (97.14), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
+          <t>maa://20108 (95.8), maa://24621 (97.14), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (66.67)</t>
         </is>
       </c>
       <c r="AG25" s="1" t="n"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (91.67)</t>
+          <t>maa://24913 (91.75)</t>
         </is>
       </c>
       <c r="I26" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (95.59)</t>
+          <t>maa://42235 (95.62)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (91.72), maa://41749 (91.6), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (91.79), maa://41749 (91.67), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.63), *maa://36701 (66.67)</t>
+          <t>maa://36660 (92.65), *maa://36701 (66.67)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>*maa://25175 (61.67)</t>
+          <t>*maa://25175 (60.66)</t>
         </is>
       </c>
       <c r="I29" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.92), maa://28440 (83.33), maa://31400 (98.88), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.92), maa://28440 (83.46), maa://31400 (98.88), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.17), maa://42865 (81.63), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (69.17), maa://42865 (81.0), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4309,7 +4309,7 @@
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>maa://45792 (88.46)</t>
+          <t>maa://45792 (88.89)</t>
         </is>
       </c>
       <c r="E30" s="1" t="n"/>
@@ -4357,7 +4357,7 @@
       </c>
       <c r="P30" s="2" t="inlineStr">
         <is>
-          <t>maa://21442 (98.74)</t>
+          <t>maa://21442 (98.76)</t>
         </is>
       </c>
       <c r="Q30" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.73), maa://45822 (100.0), maa://45045 (83.33)</t>
+          <t>maa://42979 (96.76), maa://45822 (100.0), maa://45045 (83.33)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.83), maa://36258 (86.75), *maa://43904 (71.43)</t>
+          <t>maa://35926 (93.85), maa://36258 (86.75), *maa://43904 (71.43)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.49), maa://36667 (98.0), **maa://20793 (38.0), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.51), maa://36667 (98.0), **maa://20793 (38.0), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4877,7 +4877,7 @@
       </c>
       <c r="P34" s="2" t="inlineStr">
         <is>
-          <t>maa://48817 (95.92)</t>
+          <t>maa://48817 (96.08)</t>
         </is>
       </c>
       <c r="Q34" s="1" t="n"/>
@@ -5400,7 +5400,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (88.73)</t>
+          <t>maa://36697 (88.77)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (88.89), maa://25199 (85.22), maa://30434 (92.44), maa://45059 (80.65), ***maa://25036 (18.52), *maa://44165 (66.67)</t>
+          <t>maa://36670 (88.89), maa://25199 (85.22), maa://30434 (92.56), maa://45059 (80.65), ***maa://25036 (18.52), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5469,7 +5469,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://47079 (94.81), *maa://45788 (76.32), *maa://45790 (79.17)</t>
+          <t>maa://47079 (94.87), *maa://45788 (76.32), *maa://45790 (79.17)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5639,7 +5639,7 @@
       </c>
       <c r="P41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (40.0), maa://43177 (93.1)</t>
+          <t>**maa://35616 (40.0), maa://43177 (93.33)</t>
         </is>
       </c>
       <c r="Q41" s="1" t="n"/>
@@ -5777,7 +5777,7 @@
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>maa://22525 (88.96), maa://21284 (87.04)</t>
+          <t>maa://22525 (88.39), maa://21284 (87.04)</t>
         </is>
       </c>
       <c r="I43" s="1" t="n"/>
@@ -5862,7 +5862,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (98.21), maa://27728 (96.15)</t>
+          <t>maa://29768 (98.22), maa://27728 (96.15)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -6000,7 +6000,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.46), maa://43901 (95.92)</t>
+          <t>maa://35931 (92.48), maa://43901 (94.0)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6053,7 +6053,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.81), maa://29661 (97.52), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.82), maa://29661 (97.52), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6362,7 +6362,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.75), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.78), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6430,7 +6430,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.9)</t>
+          <t>maa://32532 (92.92)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6556,7 +6556,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (96.23), maa://43903 (100.0)</t>
+          <t>maa://42981 (96.3), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#188)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://25390 (95.35), maa://24702 (94.77), maa://36681 (86.42)</t>
+          <t>maa://25390 (95.11), maa://24702 (94.79), maa://36681 (86.42)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>maa://39402 (94.23), *maa://24633 (56.1), *maa://30515 (70.09), *maa://34787 (73.56), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
+          <t>maa://39402 (94.34), *maa://24633 (56.36), *maa://30515 (70.09), *maa://34787 (73.56), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.33), *maa://20791 (62.2)</t>
+          <t>maa://22742 (91.37), *maa://20791 (62.2)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.42), maa://36684 (93.29), ***maa://22731 (6.25)</t>
+          <t>maa://21246 (91.42), maa://36684 (93.33), ***maa://22731 (6.25)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (91.79), **maa://21730 (30.49), ***maa://39501 (11.36), **maa://36675 (50.0)</t>
+          <t>maa://25251 (91.79), **maa://21730 (30.12), ***maa://39501 (10.87), **maa://36675 (50.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://40192 (96.63), maa://36987 (96.15), maa://39849 (88.89)</t>
+          <t>maa://40192 (96.77), maa://36987 (96.15), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.37), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.39), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.02), maa://20276 (88.0), *maa://22749 (75.0)</t>
+          <t>*maa://22880 (65.33), maa://20276 (88.18), *maa://22749 (75.0)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.51), maa://26254 (97.14), **maa://22738 (50.0)</t>
+          <t>maa://21249 (94.57), maa://26254 (97.14), **maa://22738 (50.0)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (90.55), maa://45854 (85.29), **maa://20790 (43.48), ***maa://37170 (16.67)</t>
+          <t>maa://24617 (90.62), maa://45854 (84.72), **maa://20790 (43.48), ***maa://37170 (16.67)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.35), maa://27484 (96.21), maa://27480 (83.78)</t>
+          <t>maa://27396 (84.1), maa://27484 (96.21), maa://27480 (83.78)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.75), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.81), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -967,7 +967,7 @@
       </c>
       <c r="P4" s="2" t="inlineStr">
         <is>
-          <t>maa://49983 (94.34), maa://50121 (92.0)</t>
+          <t>maa://49983 (94.74), maa://50121 (92.31)</t>
         </is>
       </c>
       <c r="Q4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (94.53), maa://27295 (88.24), maa://22754 (89.19), *maa://31008 (79.07), *maa://21746 (54.55)</t>
+          <t>maa://32509 (94.53), maa://27295 (88.51), maa://22754 (89.19), *maa://31008 (79.07), *maa://21746 (54.55)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.4), maa://43217 (92.92), ***maa://31785 (22.22), ***maa://36683 (29.79)</t>
+          <t>**maa://32495 (48.4), maa://43217 (92.98), ***maa://31785 (22.22), ***maa://36683 (29.79)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (65.45), *maa://39394 (65.52), ***maa://26209 (13.04)</t>
+          <t>*maa://30062 (66.07), *maa://39394 (65.52), ***maa://26209 (13.04)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.93), maa://22744 (81.48)</t>
+          <t>maa://21245 (84.78), maa://22744 (81.48)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="P5" s="2" t="inlineStr">
         <is>
-          <t>maa://21919 (96.92), *maa://21281 (80.0)</t>
+          <t>maa://21919 (96.97), *maa://21281 (80.0)</t>
         </is>
       </c>
       <c r="Q5" s="1" t="n"/>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="AB5" s="2" t="inlineStr">
         <is>
-          <t>*maa://29863 (63.41), ***maa://22752 (12.5), **maa://26013 (37.5)</t>
+          <t>*maa://29863 (63.41), ***maa://22752 (12.5), **maa://26013 (44.44)</t>
         </is>
       </c>
       <c r="AC5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (94.81)</t>
+          <t>maa://42407 (94.87)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1264,7 +1264,7 @@
       </c>
       <c r="X6" s="2" t="inlineStr">
         <is>
-          <t>maa://52754 (100.0)</t>
+          <t>maa://52754 (83.33)</t>
         </is>
       </c>
       <c r="Y6" s="1" t="n"/>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="AF6" s="2" t="inlineStr">
         <is>
-          <t>*maa://33152 (63.79), ***maa://22770 (26.09)</t>
+          <t>*maa://33152 (62.71), ***maa://22770 (26.09)</t>
         </is>
       </c>
       <c r="AG6" s="1" t="n"/>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="P7" s="2" t="inlineStr">
         <is>
-          <t>maa://22750 (92.31)</t>
+          <t>maa://22750 (92.59)</t>
         </is>
       </c>
       <c r="Q7" s="1" t="n"/>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="T7" s="2" t="inlineStr">
         <is>
-          <t>maa://21291 (85.19)</t>
+          <t>maa://21291 (85.71)</t>
         </is>
       </c>
       <c r="U7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (96.07), *maa://22758 (77.22)</t>
+          <t>maa://22399 (96.09), *maa://22758 (77.22)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (67.82), *maa://36671 (69.23), maa://45272 (96.67), *maa://42530 (62.5)</t>
+          <t>*maa://26191 (67.82), maa://45272 (96.77), *maa://36671 (69.23), *maa://42530 (62.5)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.05.11 13:19:54</t>
+          <t>更新日期：2025.05.13 13:20:58</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (84.09), *maa://21916 (62.69), maa://23252 (91.55), maa://37496 (97.22), **maa://22759 (45.45)</t>
+          <t>maa://32931 (84.33), *maa://21916 (62.69), maa://23252 (91.55), maa://37496 (97.3), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (96.13)</t>
+          <t>maa://21411 (96.14)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="P9" s="2" t="inlineStr">
         <is>
-          <t>maa://22736 (82.88)</t>
+          <t>maa://22736 (83.04)</t>
         </is>
       </c>
       <c r="Q9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (86.76), **maa://39938 (45.0), **maa://45044 (40.0), **maa://27377 (42.86), ***maa://25174 (19.05), maa://40166 (97.06)</t>
+          <t>maa://28711 (86.96), **maa://39938 (46.34), **maa://45044 (40.0), **maa://27377 (42.86), maa://40166 (97.14), ***maa://25174 (19.05)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (88.34), *maa://22865 (51.85)</t>
+          <t>maa://26206 (88.41), *maa://22865 (51.85)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1704,12 +1704,12 @@
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.1), ***maa://39951 (12.86), ***maa://34206 (22.22), *maa://45271 (59.09), ***maa://39243 (25.0)</t>
+          <t>***maa://25695 (19.0), ***maa://39951 (12.5), ***maa://34206 (22.22), *maa://45271 (59.09), ***maa://39243 (25.0), maa://54000 (100.0)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.52), maa://22755 (88.62), **maa://22756 (40.91), ***maa://21737 (11.76)</t>
+          <t>maa://27395 (96.54), maa://22755 (88.89), **maa://22756 (40.91), ***maa://21737 (11.76)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.85), maa://45828 (92.68), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.86), maa://45828 (92.86), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (88.39)</t>
+          <t>maa://21287 (88.6)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (90.8), maa://22501 (98.08), maa://45521 (90.91)</t>
+          <t>maa://22747 (90.8), maa://22501 (98.11), maa://45521 (90.91)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (98.05)</t>
+          <t>maa://36713 (98.06)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1935,7 +1935,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://29912 (97.7), maa://22516 (87.36), *maa://20794 (54.67)</t>
+          <t>maa://29912 (97.7), maa://22516 (87.36), *maa://20794 (55.26)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.64), maa://36677 (95.12), maa://39872 (92.86)</t>
+          <t>maa://23669 (95.64), maa://36677 (95.12), maa://39872 (93.1)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.57), maa://36673 (92.94), maa://25001 (86.3)</t>
+          <t>maa://24999 (92.58), maa://36673 (92.94), maa://25001 (86.3)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>maa://34957 (82.0), **maa://22768 (50.0)</t>
+          <t>maa://34957 (82.35), **maa://22768 (50.0)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (38.22), maa://39883 (87.72), *maa://39885 (52.63)</t>
+          <t>**maa://22737 (38.22), maa://39883 (87.07), *maa://39885 (51.28)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://39841 (94.59), maa://26245 (96.53), maa://21288 (96.3), maa://36682 (95.56)</t>
+          <t>maa://39841 (94.0), maa://26245 (96.57), maa://21288 (96.3), maa://36682 (95.74)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (79.06), maa://22734 (84.43), *maa://30808 (65.22), *maa://36048 (64.58), maa://45058 (84.21)</t>
+          <t>*maa://22743 (79.06), maa://22734 (84.43), *maa://30808 (65.22), *maa://36048 (65.66), maa://45058 (84.21)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (86.67), maa://21478 (90.0)</t>
+          <t>maa://24304 (86.83), maa://21478 (90.0)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.27), maa://36666 (81.12), *maa://22766 (68.03)</t>
+          <t>maa://21364 (81.27), maa://36666 (81.25), *maa://22766 (68.29)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.44), *maa://28648 (72.0), *maa://36674 (79.31)</t>
+          <t>maa://22729 (94.44), *maa://28648 (72.73), *maa://36674 (79.31)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (68.1), maa://27755 (93.88)</t>
+          <t>*maa://23911 (68.38), maa://27755 (93.88)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (89.42), maa://39599 (85.14)</t>
+          <t>maa://22430 (89.47), maa://39599 (85.33)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.9)</t>
+          <t>maa://24570 (96.93)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (87.82)</t>
+          <t>maa://24421 (87.5)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2845,7 +2845,7 @@
       </c>
       <c r="AB18" s="2" t="inlineStr">
         <is>
-          <t>maa://24393 (98.04)</t>
+          <t>maa://24393 (98.11)</t>
         </is>
       </c>
       <c r="AC18" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (98.6)</t>
+          <t>maa://24386 (98.61)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (67.52), *maa://36668 (57.32)</t>
+          <t>*maa://30709 (67.59), *maa://36668 (57.32)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.82), maa://25198 (94.4), *maa://20795 (50.76), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.86), maa://25198 (94.44), *maa://20795 (50.76), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.71)</t>
+          <t>maa://41331 (85.97)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3089,7 +3089,7 @@
       </c>
       <c r="X20" s="2" t="inlineStr">
         <is>
-          <t>maa://50085 (88.64), maa://49976 (85.71)</t>
+          <t>maa://50085 (87.23), maa://49976 (85.9)</t>
         </is>
       </c>
       <c r="Y20" s="1" t="n"/>
@@ -3171,7 +3171,7 @@
       </c>
       <c r="L21" s="2" t="inlineStr">
         <is>
-          <t>maa://31731 (96.43)</t>
+          <t>maa://31731 (96.49)</t>
         </is>
       </c>
       <c r="M21" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (82.56), ***maa://23820 (30.0), **maa://52223 (38.46)</t>
+          <t>maa://21443 (82.56), ***maa://23820 (30.0), **maa://52223 (46.67)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (90.95), maa://22432 (81.98)</t>
+          <t>maa://22524 (90.57), maa://22432 (82.3)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>maa://25236 (96.08), **maa://21678 (48.94), **maa://22735 (42.86)</t>
+          <t>maa://25236 (96.12), **maa://21678 (48.94), **maa://22735 (42.86)</t>
         </is>
       </c>
       <c r="I22" s="1" t="n"/>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (26.92), **maa://41753 (50.0)</t>
+          <t>***maa://28036 (26.92), **maa://41753 (48.0)</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.41), maa://39875 (94.67)</t>
+          <t>maa://39756 (95.44), maa://39875 (94.67)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P23" s="2" t="inlineStr">
         <is>
-          <t>maa://30587 (91.87), *maa://29748 (76.3), ***maa://29785 (17.39), *maa://37566 (78.26)</t>
+          <t>maa://30587 (91.9), *maa://29748 (76.3), ***maa://29785 (17.39), *maa://37566 (78.26)</t>
         </is>
       </c>
       <c r="Q23" s="1" t="n"/>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="T23" s="2" t="inlineStr">
         <is>
-          <t>maa://31212 (91.43), maa://24387 (82.5)</t>
+          <t>maa://31212 (91.67), maa://24387 (82.5)</t>
         </is>
       </c>
       <c r="U23" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (84.1), maa://23504 (93.53), **maa://22892 (41.29), *maa://25141 (77.37), *maa://36663 (77.78), ***maa://22815 (23.08), maa://52227 (100.0)</t>
+          <t>maa://29988 (84.15), maa://23504 (93.56), **maa://22892 (41.29), *maa://25141 (77.37), *maa://36663 (77.78), ***maa://22815 (23.08), maa://52227 (100.0)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="AF24" s="2" t="inlineStr">
         <is>
-          <t>maa://22523 (82.71), *maa://36672 (76.19), maa://29910 (93.75), **maa://21440 (35.71), maa://45831 (84.62)</t>
+          <t>maa://22523 (82.33), *maa://36672 (76.19), maa://29910 (93.75), **maa://21440 (35.71), maa://45831 (84.62)</t>
         </is>
       </c>
       <c r="AG24" s="1" t="n"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>maa://29753 (95.3)</t>
+          <t>maa://29753 (95.32)</t>
         </is>
       </c>
       <c r="E25" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (73.37), *maa://25311 (74.11), ***maa://22725 (4.76), *maa://45047 (72.73)</t>
+          <t>*maa://29063 (73.12), *maa://25311 (74.11), ***maa://22725 (4.76), *maa://45047 (72.73)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3739,7 +3739,7 @@
       </c>
       <c r="X25" s="2" t="inlineStr">
         <is>
-          <t>maa://29890 (82.46)</t>
+          <t>maa://29890 (82.76)</t>
         </is>
       </c>
       <c r="Y25" s="1" t="n"/>
@@ -3837,7 +3837,7 @@
       </c>
       <c r="P26" s="2" t="inlineStr">
         <is>
-          <t>*maa://30968 (65.0), maa://39870 (92.31)</t>
+          <t>*maa://30968 (65.0), maa://39870 (92.86)</t>
         </is>
       </c>
       <c r="Q26" s="1" t="n"/>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>**maa://21283 (47.37), *maa://39601 (78.26), maa://34494 (97.14), **maa://36665 (50.0)</t>
+          <t>*maa://39601 (78.26), **maa://21283 (47.37), maa://34494 (97.14), **maa://36665 (50.0)</t>
         </is>
       </c>
       <c r="I27" s="1" t="n"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (76.47)</t>
+          <t>*maa://30624 (77.14)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.61), maa://25725 (85.11)</t>
+          <t>maa://24465 (90.61), maa://25725 (84.21)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>*maa://29765 (65.96), maa://23263 (95.41)</t>
+          <t>*maa://29765 (66.32), maa://23263 (95.41)</t>
         </is>
       </c>
       <c r="U28" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (91.79), maa://41749 (91.67), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (91.82), maa://41749 (91.67), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.65), *maa://36701 (66.67)</t>
+          <t>maa://36660 (92.68), *maa://36701 (66.67)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>*maa://25175 (60.66)</t>
+          <t>*maa://25175 (59.68)</t>
         </is>
       </c>
       <c r="I29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.17), maa://42865 (81.0), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (69.17), maa://42865 (81.19), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.76), maa://45822 (100.0), maa://45045 (83.33)</t>
+          <t>maa://42979 (96.79), maa://45822 (100.0), maa://45045 (83.33)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.85), maa://36258 (86.75), *maa://43904 (71.43)</t>
+          <t>maa://35926 (93.85), maa://36258 (86.93), *maa://43904 (71.43)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4535,7 +4535,7 @@
       </c>
       <c r="AB31" s="2" t="inlineStr">
         <is>
-          <t>**maa://51420 (33.33)</t>
+          <t>***maa://51420 (25.0)</t>
         </is>
       </c>
       <c r="AC31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.51), maa://36667 (98.0), **maa://20793 (38.0), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.53), maa://36667 (98.02), **maa://20793 (38.0), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (97.22), maa://41108 (88.0), maa://41238 (97.81), maa://45523 (100.0)</t>
+          <t>maa://42859 (97.22), maa://41108 (88.0), maa://41238 (97.86), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4877,7 +4877,7 @@
       </c>
       <c r="P34" s="2" t="inlineStr">
         <is>
-          <t>maa://48817 (96.08)</t>
+          <t>maa://48817 (96.23)</t>
         </is>
       </c>
       <c r="Q34" s="1" t="n"/>
@@ -4991,7 +4991,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (97.12)</t>
+          <t>maa://41296 (97.13)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5235,7 +5235,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (98.28), *maa://47069 (78.95), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.3), *maa://47069 (78.95), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (88.89), maa://25199 (85.22), maa://30434 (92.56), maa://45059 (80.65), ***maa://25036 (18.52), *maa://44165 (66.67)</t>
+          <t>maa://36670 (89.09), maa://25199 (85.22), maa://30434 (92.68), maa://45059 (80.65), ***maa://25036 (18.52), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5469,7 +5469,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://47079 (94.87), *maa://45788 (76.32), *maa://45790 (79.17)</t>
+          <t>maa://47079 (95.0), *maa://45788 (75.65), *maa://45790 (79.17)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5554,7 +5554,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.17), maa://21386 (95.79), maa://36664 (89.66), maa://45550 (87.5)</t>
+          <t>maa://23278 (95.18), maa://21386 (95.79), maa://36664 (89.66), maa://45550 (87.5)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5862,7 +5862,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (98.22), maa://27728 (96.15)</t>
+          <t>maa://29768 (98.23), maa://27728 (96.15)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5931,7 +5931,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.54), maa://30807 (94.59), *maa://22767 (55.0), maa://42459 (91.43), ***maa://20796 (13.79)</t>
+          <t>maa://21229 (84.54), maa://30807 (94.67), *maa://22767 (55.0), maa://42459 (91.43), ***maa://20796 (13.79)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -5947,7 +5947,7 @@
       </c>
       <c r="P45" s="2" t="inlineStr">
         <is>
-          <t>*maa://36237 (73.68)</t>
+          <t>*maa://36237 (75.0)</t>
         </is>
       </c>
       <c r="Q45" s="1" t="n"/>
@@ -6000,7 +6000,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.48), maa://43901 (94.0)</t>
+          <t>maa://35931 (92.29), maa://43901 (94.12)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6053,7 +6053,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.82), maa://29661 (97.52), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.83), maa://29661 (97.55), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6362,7 +6362,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.78), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.81), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6430,7 +6430,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (92.92)</t>
+          <t>maa://32532 (93.0)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#189)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://25390 (95.11), maa://24702 (94.79), maa://36681 (86.42)</t>
+          <t>maa://25390 (95.19), maa://24702 (94.79), maa://36681 (86.42)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>maa://39402 (94.34), *maa://24633 (56.36), *maa://30515 (70.09), *maa://34787 (73.56), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
+          <t>maa://39402 (94.44), *maa://24633 (56.36), *maa://30515 (70.09), *maa://34787 (73.56), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.37), *maa://20791 (62.2)</t>
+          <t>maa://22742 (91.41), *maa://20791 (62.2)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.42), maa://36684 (93.33), ***maa://22731 (6.25)</t>
+          <t>maa://21246 (91.45), maa://36684 (93.42), ***maa://22731 (6.25)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://40192 (96.77), maa://36987 (96.15), maa://39849 (88.89)</t>
+          <t>maa://40192 (96.84), maa://36987 (96.15), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.39), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.41), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.33), maa://20276 (88.18), *maa://22749 (75.0)</t>
+          <t>*maa://22880 (65.33), maa://20276 (88.24), *maa://22749 (75.0)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.57), maa://26254 (97.14), **maa://22738 (50.0)</t>
+          <t>maa://21249 (94.58), maa://26254 (97.14), **maa://22738 (50.0)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (90.62), maa://45854 (84.72), **maa://20790 (43.48), ***maa://37170 (16.67)</t>
+          <t>maa://24617 (90.62), maa://45854 (85.14), **maa://20790 (43.48), ***maa://37170 (16.67)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.1), maa://27484 (96.21), maa://27480 (83.78)</t>
+          <t>maa://27396 (84.15), maa://27484 (96.21), maa://27480 (83.78)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -967,7 +967,7 @@
       </c>
       <c r="P4" s="2" t="inlineStr">
         <is>
-          <t>maa://49983 (94.74), maa://50121 (92.31)</t>
+          <t>maa://49983 (94.83), maa://50121 (92.31)</t>
         </is>
       </c>
       <c r="Q4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (94.53), maa://27295 (88.51), maa://22754 (89.19), *maa://31008 (79.07), *maa://21746 (54.55)</t>
+          <t>maa://32509 (94.53), maa://27295 (87.5), maa://22754 (89.19), *maa://31008 (79.55), *maa://21746 (54.55)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.4), maa://43217 (92.98), ***maa://31785 (22.22), ***maa://36683 (29.79)</t>
+          <t>**maa://32495 (48.4), maa://43217 (93.04), ***maa://31785 (22.22), ***maa://36683 (29.79)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1015,7 +1015,7 @@
       </c>
       <c r="AB4" s="2" t="inlineStr">
         <is>
-          <t>*maa://32658 (72.73)</t>
+          <t>*maa://32658 (76.0)</t>
         </is>
       </c>
       <c r="AC4" s="1" t="n"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AF4" s="2" t="inlineStr">
         <is>
-          <t>*maa://30062 (66.07), *maa://39394 (65.52), ***maa://26209 (13.04)</t>
+          <t>*maa://30062 (66.07), *maa://39394 (66.67), ***maa://26209 (13.04)</t>
         </is>
       </c>
       <c r="AG4" s="1" t="n"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.78), maa://22744 (81.48)</t>
+          <t>maa://21245 (84.95), maa://22744 (81.48)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="P6" s="2" t="inlineStr">
         <is>
-          <t>maa://31836 (93.94), maa://30381 (94.44)</t>
+          <t>maa://31836 (94.12), maa://30381 (94.44)</t>
         </is>
       </c>
       <c r="Q6" s="1" t="n"/>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="T6" s="2" t="inlineStr">
         <is>
-          <t>maa://37411 (90.0)</t>
+          <t>maa://37411 (90.48)</t>
         </is>
       </c>
       <c r="U6" s="1" t="n"/>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>maa://21955 (93.62)</t>
+          <t>maa://21955 (93.75)</t>
         </is>
       </c>
       <c r="E7" s="1" t="n"/>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="P7" s="2" t="inlineStr">
         <is>
-          <t>maa://22750 (92.59)</t>
+          <t>maa://22750 (92.73)</t>
         </is>
       </c>
       <c r="Q7" s="1" t="n"/>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="T7" s="2" t="inlineStr">
         <is>
-          <t>maa://21291 (85.71)</t>
+          <t>maa://21291 (85.96)</t>
         </is>
       </c>
       <c r="U7" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (96.09), *maa://22758 (77.22)</t>
+          <t>maa://22399 (96.11), *maa://22758 (77.22)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.05.13 13:20:58</t>
+          <t>更新日期：2025.05.14 13:20:50</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24371 (55.84)</t>
+          <t>*maa://24371 (55.13)</t>
         </is>
       </c>
       <c r="I8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (96.14)</t>
+          <t>maa://21411 (95.93)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1643,7 +1643,7 @@
       </c>
       <c r="T9" s="2" t="inlineStr">
         <is>
-          <t>**maa://22866 (30.19), maa://26222 (98.28)</t>
+          <t>maa://26222 (98.28), **maa://22866 (30.19)</t>
         </is>
       </c>
       <c r="U9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (86.96), **maa://39938 (46.34), **maa://45044 (40.0), **maa://27377 (42.86), maa://40166 (97.14), ***maa://25174 (19.05)</t>
+          <t>maa://28711 (86.96), **maa://39938 (46.34), **maa://45044 (40.0), **maa://27377 (42.86), maa://40166 (94.59), ***maa://25174 (19.05)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (88.41), *maa://22865 (51.85)</t>
+          <t>maa://26206 (88.55), *maa://22865 (51.85)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.0), ***maa://39951 (12.5), ***maa://34206 (22.22), *maa://45271 (59.09), ***maa://39243 (25.0), maa://54000 (100.0)</t>
+          <t>***maa://25695 (19.0), ***maa://39951 (12.5), ***maa://34206 (22.22), *maa://45271 (59.7), ***maa://39243 (25.0), maa://54000 (100.0)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.54), maa://22755 (88.89), **maa://22756 (40.91), ***maa://21737 (11.76)</t>
+          <t>maa://27395 (96.57), maa://22755 (88.89), **maa://22756 (40.91), ***maa://21737 (11.76)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.86), maa://45828 (92.86), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.87), maa://45828 (93.02), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.35)</t>
+          <t>maa://36707 (99.36)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (90.8), maa://22501 (98.11), maa://45521 (90.91)</t>
+          <t>maa://22747 (90.8), maa://22501 (98.13), maa://45521 (90.91)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1935,7 +1935,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://29912 (97.7), maa://22516 (87.36), *maa://20794 (55.26)</t>
+          <t>maa://29912 (97.73), maa://22516 (87.36), *maa://20794 (55.26)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (90.81), **maa://45826 (36.36)</t>
+          <t>maa://21867 (90.81), **maa://45826 (33.33)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.67), *maa://21485 (75.51), maa://37962 (91.67)</t>
+          <t>maa://22753 (91.71), *maa://21485 (75.68), maa://37962 (91.67)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.58), maa://36673 (92.94), maa://25001 (86.3)</t>
+          <t>maa://24999 (92.62), maa://36673 (92.94), maa://25001 (86.3)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>maa://34957 (82.35), **maa://22768 (50.0)</t>
+          <t>maa://34957 (82.69), **maa://22768 (50.0)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (38.22), maa://39883 (87.07), *maa://39885 (51.28)</t>
+          <t>**maa://22737 (38.22), maa://39883 (87.39), *maa://39885 (51.28)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://39841 (94.0), maa://26245 (96.57), maa://21288 (96.3), maa://36682 (95.74)</t>
+          <t>maa://39841 (94.04), maa://26245 (96.57), maa://21288 (96.3), maa://36682 (95.74)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.81), maa://20107 (87.1), maa://22772 (100.0), *maa://22745 (66.67)</t>
+          <t>maa://23250 (98.82), maa://20107 (87.1), maa://22772 (100.0), *maa://22745 (66.67)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="AB14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (96.25)</t>
+          <t>maa://22764 (96.3)</t>
         </is>
       </c>
       <c r="AC14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (79.06), maa://22734 (84.43), *maa://30808 (65.22), *maa://36048 (65.66), maa://45058 (84.21)</t>
+          <t>*maa://22743 (79.06), maa://22734 (84.43), *maa://30808 (65.22), *maa://36048 (66.0), maa://45058 (84.21)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2391,7 +2391,7 @@
       </c>
       <c r="L15" s="2" t="inlineStr">
         <is>
-          <t>*maa://21334 (56.25)</t>
+          <t>*maa://21334 (54.55)</t>
         </is>
       </c>
       <c r="M15" s="1" t="n"/>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (91.06), *maa://22727 (70.0)</t>
+          <t>maa://24762 (91.11), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="T15" s="2" t="inlineStr">
         <is>
-          <t>maa://23892 (96.47)</t>
+          <t>maa://23892 (96.51)</t>
         </is>
       </c>
       <c r="U15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.27), maa://36666 (81.25), *maa://22766 (68.29)</t>
+          <t>maa://21364 (81.27), maa://36666 (81.38), *maa://22766 (68.29)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.44), *maa://28648 (72.73), *maa://36674 (79.31)</t>
+          <t>maa://22729 (94.44), *maa://28648 (72.73), *maa://36674 (79.66)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (68.38), maa://27755 (93.88)</t>
+          <t>*maa://23911 (68.38), maa://27755 (93.94)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="T17" s="2" t="inlineStr">
         <is>
-          <t>*maa://42324 (56.25)</t>
+          <t>*maa://42324 (57.14)</t>
         </is>
       </c>
       <c r="U17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.93)</t>
+          <t>maa://24570 (96.95)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (87.5)</t>
+          <t>maa://24421 (87.64)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t>maa://22466 (92.08), *maa://22732 (51.38), maa://52226 (100.0)</t>
+          <t>maa://22466 (92.08), *maa://22732 (51.38), maa://52226 (92.86)</t>
         </is>
       </c>
       <c r="M18" s="1" t="n"/>
@@ -2792,12 +2792,12 @@
       </c>
       <c r="O18" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="P18" s="2" t="inlineStr">
         <is>
-          <t>maa://24379 (100.0), maa://24380 (100.0)</t>
+          <t>maa://24379 (100.0), maa://24380 (100.0), maa://54153 (100.0)</t>
         </is>
       </c>
       <c r="Q18" s="1" t="n"/>
@@ -2845,7 +2845,7 @@
       </c>
       <c r="AB18" s="2" t="inlineStr">
         <is>
-          <t>maa://24393 (98.11)</t>
+          <t>maa://24393 (98.15)</t>
         </is>
       </c>
       <c r="AC18" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.86), maa://25198 (94.44), *maa://20795 (50.76), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.91), maa://25198 (94.44), *maa://20795 (50.76), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (85.97)</t>
+          <t>maa://41331 (86.1)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="T20" s="2" t="inlineStr">
         <is>
-          <t>maa://29113 (87.5)</t>
+          <t>maa://29113 (87.88)</t>
         </is>
       </c>
       <c r="U20" s="1" t="n"/>
@@ -3089,7 +3089,7 @@
       </c>
       <c r="X20" s="2" t="inlineStr">
         <is>
-          <t>maa://50085 (87.23), maa://49976 (85.9)</t>
+          <t>maa://50085 (86.73), maa://49976 (86.25)</t>
         </is>
       </c>
       <c r="Y20" s="1" t="n"/>
@@ -3171,7 +3171,7 @@
       </c>
       <c r="L21" s="2" t="inlineStr">
         <is>
-          <t>maa://31731 (96.49)</t>
+          <t>maa://31731 (96.55)</t>
         </is>
       </c>
       <c r="M21" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (82.56), ***maa://23820 (30.0), **maa://52223 (46.67)</t>
+          <t>maa://21443 (82.56), ***maa://23820 (30.0), **maa://52223 (41.18)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (90.57), maa://22432 (82.3)</t>
+          <t>maa://22524 (90.2), maa://22432 (81.9)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.7), *maa://37649 (69.44)</t>
+          <t>maa://21282 (98.7), *maa://37649 (71.05)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.44), maa://39875 (94.67)</t>
+          <t>maa://39756 (95.45), maa://39875 (94.67)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="X23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (68.13)</t>
+          <t>*maa://28503 (67.39)</t>
         </is>
       </c>
       <c r="Y23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (78.96), *maa://46650 (66.67)</t>
+          <t>*maa://24368 (79.01), *maa://46650 (66.67)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (84.15), maa://23504 (93.56), **maa://22892 (41.29), *maa://25141 (77.37), *maa://36663 (77.78), ***maa://22815 (23.08), maa://52227 (100.0)</t>
+          <t>maa://29988 (84.32), maa://23504 (93.58), **maa://22892 (41.29), *maa://25141 (77.37), *maa://36663 (77.78), ***maa://22815 (23.08), maa://52227 (100.0)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (73.12), *maa://25311 (74.11), ***maa://22725 (4.76), *maa://45047 (72.73)</t>
+          <t>*maa://29063 (73.12), *maa://25311 (74.11), ***maa://22725 (4.76), *maa://45047 (66.67)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3707,7 +3707,7 @@
       </c>
       <c r="P25" s="2" t="inlineStr">
         <is>
-          <t>maa://24382 (94.12)</t>
+          <t>maa://24382 (94.29)</t>
         </is>
       </c>
       <c r="Q25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (89.47), maa://24516 (80.22), maa://26001 (84.48)</t>
+          <t>maa://31215 (88.81), *maa://24516 (79.35), maa://26001 (84.48)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (91.75)</t>
+          <t>maa://24913 (91.84)</t>
         </is>
       </c>
       <c r="I26" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (95.62)</t>
+          <t>maa://42235 (95.68)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>*maa://30624 (77.14)</t>
+          <t>*maa://30624 (76.06)</t>
         </is>
       </c>
       <c r="U27" s="1" t="n"/>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="X28" s="2" t="inlineStr">
         <is>
-          <t>maa://39929 (91.82), maa://41749 (91.67), ***maa://39723 (13.89)</t>
+          <t>maa://39929 (91.88), maa://41749 (91.73), ***maa://39723 (13.89)</t>
         </is>
       </c>
       <c r="Y28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.68), *maa://36701 (66.67)</t>
+          <t>maa://36660 (92.48), *maa://36701 (64.71)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>*maa://25175 (59.68)</t>
+          <t>*maa://25175 (60.32)</t>
         </is>
       </c>
       <c r="I29" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.92), maa://28440 (83.46), maa://31400 (98.88), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.94), maa://28440 (83.46), maa://31400 (98.88), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4222,12 +4222,12 @@
       </c>
       <c r="O29" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="P29" s="2" t="inlineStr">
         <is>
-          <t>*maa://23168 (57.81), *maa://30050 (53.85)</t>
+          <t>*maa://23168 (56.72), *maa://30050 (51.22), maa://54169 (100.0)</t>
         </is>
       </c>
       <c r="Q29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.17), maa://42865 (81.19), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (69.17), maa://42865 (81.55), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4373,7 +4373,7 @@
       </c>
       <c r="T30" s="2" t="inlineStr">
         <is>
-          <t>*maa://32940 (70.0), maa://24388 (94.74)</t>
+          <t>*maa://32940 (72.73), maa://24388 (94.74)</t>
         </is>
       </c>
       <c r="U30" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.79), maa://45822 (100.0), maa://45045 (83.33)</t>
+          <t>maa://42979 (96.8), maa://45822 (100.0), maa://45045 (83.33)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.53), maa://36667 (98.02), **maa://20793 (38.0), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.54), maa://36667 (98.02), **maa://20793 (38.0), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (97.22), maa://41108 (88.0), maa://41238 (97.86), maa://45523 (100.0)</t>
+          <t>maa://42859 (97.22), maa://41108 (88.0), maa://41238 (97.87), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4991,7 +4991,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (97.13)</t>
+          <t>maa://41296 (97.14)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5219,7 +5219,7 @@
       </c>
       <c r="H37" s="2" t="inlineStr">
         <is>
-          <t>*maa://24374 (56.25)</t>
+          <t>*maa://24374 (57.14)</t>
         </is>
       </c>
       <c r="I37" s="1" t="n"/>
@@ -5235,7 +5235,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (98.3), *maa://47069 (78.95), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.31), *maa://47069 (80.0), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5352,7 +5352,7 @@
       </c>
       <c r="P38" s="2" t="inlineStr">
         <is>
-          <t>*maa://24383 (69.44)</t>
+          <t>*maa://24383 (69.72)</t>
         </is>
       </c>
       <c r="Q38" s="1" t="n"/>
@@ -5368,7 +5368,7 @@
       </c>
       <c r="T38" s="2" t="inlineStr">
         <is>
-          <t>maa://30713 (97.22)</t>
+          <t>maa://30713 (97.3)</t>
         </is>
       </c>
       <c r="U38" s="1" t="n"/>
@@ -5400,7 +5400,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (88.77)</t>
+          <t>maa://36697 (88.85)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5639,7 +5639,7 @@
       </c>
       <c r="P41" s="2" t="inlineStr">
         <is>
-          <t>**maa://35616 (40.0), maa://43177 (93.33)</t>
+          <t>**maa://35616 (40.0), maa://43177 (90.32)</t>
         </is>
       </c>
       <c r="Q41" s="1" t="n"/>
@@ -5809,7 +5809,7 @@
       </c>
       <c r="P43" s="2" t="inlineStr">
         <is>
-          <t>*maa://47403 (80.0)</t>
+          <t>*maa://47403 (72.73)</t>
         </is>
       </c>
       <c r="Q43" s="1" t="n"/>
@@ -5963,7 +5963,7 @@
       </c>
       <c r="T45" s="2" t="inlineStr">
         <is>
-          <t>**maa://39364 (46.0)</t>
+          <t>**maa://39364 (45.28)</t>
         </is>
       </c>
       <c r="U45" s="1" t="n"/>
@@ -6000,7 +6000,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.29), maa://43901 (94.12)</t>
+          <t>maa://35931 (92.33), maa://43901 (94.34)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6053,7 +6053,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.83), maa://29661 (97.55), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.84), maa://29661 (97.56), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6312,7 +6312,7 @@
       </c>
       <c r="H52" s="2" t="inlineStr">
         <is>
-          <t>maa://24376 (96.88)</t>
+          <t>maa://24376 (96.97)</t>
         </is>
       </c>
       <c r="I52" s="1" t="n"/>
@@ -6362,7 +6362,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.81), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.83), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6502,7 +6502,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://31270 (94.41), maa://27746 (82.91)</t>
+          <t>maa://31270 (94.44), maa://27746 (82.91)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6520,7 +6520,7 @@
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>*maa://40438 (72.6)</t>
+          <t>*maa://40438 (72.97)</t>
         </is>
       </c>
       <c r="I60" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#190)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://25390 (95.19), maa://24702 (94.79), maa://36681 (86.42)</t>
+          <t>maa://25390 (95.25), maa://24702 (94.79), maa://36681 (86.42)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -686,12 +686,12 @@
       </c>
       <c r="K2" s="1" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>maa://39402 (94.44), *maa://24633 (56.36), *maa://30515 (70.09), *maa://34787 (73.56), ***maa://20792 (11.93), ***maa://29083 (27.78)</t>
+          <t>maa://39402 (94.44), *maa://24633 (56.36), *maa://30515 (70.09), *maa://34787 (72.73), ***maa://20792 (11.93), ***maa://29083 (27.78), maa://54304 (100.0)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.41), *maa://20791 (62.2)</t>
+          <t>maa://22742 (91.41), *maa://20791 (62.65)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.45), maa://36684 (93.42), ***maa://22731 (6.25)</t>
+          <t>maa://21246 (91.45), maa://36684 (93.46), ***maa://22731 (6.25)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://40192 (96.84), maa://36987 (96.15), maa://39849 (88.89)</t>
+          <t>maa://40192 (96.88), maa://36987 (96.15), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.33), maa://20276 (88.24), *maa://22749 (75.0)</t>
+          <t>*maa://22880 (65.49), maa://20276 (88.24), *maa://22749 (75.0)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.58), maa://26254 (97.14), **maa://22738 (50.0)</t>
+          <t>maa://21249 (94.6), maa://26254 (97.22), **maa://22738 (50.0)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (90.62), maa://45854 (85.14), **maa://20790 (43.48), ***maa://37170 (16.67)</t>
+          <t>maa://24617 (90.62), maa://45854 (85.33), **maa://20790 (43.48), ***maa://37170 (16.67)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.15), maa://27484 (96.21), maa://27480 (83.78)</t>
+          <t>maa://27396 (84.24), maa://27484 (96.21), maa://27480 (83.78)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (95.4), maa://52241 (100.0)</t>
+          <t>maa://24390 (95.45), maa://52241 (100.0)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.81), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.85), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -967,7 +967,7 @@
       </c>
       <c r="P4" s="2" t="inlineStr">
         <is>
-          <t>maa://49983 (94.83), maa://50121 (92.31)</t>
+          <t>maa://49983 (95.16), maa://50121 (92.86)</t>
         </is>
       </c>
       <c r="Q4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (94.53), maa://27295 (87.5), maa://22754 (89.19), *maa://31008 (79.55), *maa://21746 (54.55)</t>
+          <t>maa://32509 (94.62), maa://27295 (87.78), maa://22754 (89.19), *maa://31008 (79.55), *maa://21746 (54.55)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.4), maa://43217 (93.04), ***maa://31785 (22.22), ***maa://36683 (29.79)</t>
+          <t>**maa://32495 (48.58), maa://43217 (93.22), ***maa://31785 (22.22), ***maa://36683 (29.79)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (94.87)</t>
+          <t>maa://42407 (94.94)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="P6" s="2" t="inlineStr">
         <is>
-          <t>maa://31836 (94.12), maa://30381 (94.44)</t>
+          <t>maa://31836 (94.29), maa://30381 (94.44)</t>
         </is>
       </c>
       <c r="Q6" s="1" t="n"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="X7" s="2" t="inlineStr">
         <is>
-          <t>maa://22399 (96.11), *maa://22758 (77.22)</t>
+          <t>maa://22399 (96.13), *maa://22758 (77.22)</t>
         </is>
       </c>
       <c r="Y7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (67.82), maa://45272 (96.77), *maa://36671 (69.23), *maa://42530 (62.5)</t>
+          <t>*maa://26191 (67.82), maa://45272 (96.88), *maa://36671 (69.23), *maa://42530 (62.5)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.05.14 13:20:50</t>
+          <t>更新日期：2025.05.17 13:19:59</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (84.33), *maa://21916 (62.69), maa://23252 (91.55), maa://37496 (97.3), **maa://22759 (45.45)</t>
+          <t>maa://32931 (84.67), *maa://21916 (62.69), maa://23252 (91.55), maa://37496 (97.37), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="AF8" s="2" t="inlineStr">
         <is>
-          <t>*maa://24479 (79.79), *maa://21990 (51.85)</t>
+          <t>*maa://24479 (78.12), *maa://21990 (51.85)</t>
         </is>
       </c>
       <c r="AG8" s="1" t="n"/>
@@ -1643,7 +1643,7 @@
       </c>
       <c r="T9" s="2" t="inlineStr">
         <is>
-          <t>maa://26222 (98.28), **maa://22866 (30.19)</t>
+          <t>maa://26222 (98.31), **maa://22866 (30.19)</t>
         </is>
       </c>
       <c r="U9" s="1" t="n"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="X9" s="2" t="inlineStr">
         <is>
-          <t>maa://26223 (98.09), maa://52237 (100.0)</t>
+          <t>maa://26223 (98.11), maa://52237 (100.0)</t>
         </is>
       </c>
       <c r="Y9" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (86.96), **maa://39938 (46.34), **maa://45044 (40.0), **maa://27377 (42.86), maa://40166 (94.59), ***maa://25174 (19.05)</t>
+          <t>maa://28711 (87.05), **maa://39938 (46.34), **maa://45044 (40.0), **maa://27377 (42.86), maa://40166 (94.59), ***maa://25174 (19.05)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (88.55), *maa://22865 (51.85)</t>
+          <t>maa://26206 (88.62), *maa://22865 (51.85)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (19.0), ***maa://39951 (12.5), ***maa://34206 (22.22), *maa://45271 (59.7), ***maa://39243 (25.0), maa://54000 (100.0)</t>
+          <t>***maa://25695 (18.91), ***maa://39951 (12.5), ***maa://34206 (22.22), *maa://45271 (59.7), ***maa://39243 (25.0), maa://54000 (100.0)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.57), maa://22755 (88.89), **maa://22756 (40.91), ***maa://21737 (11.76)</t>
+          <t>maa://27395 (96.6), maa://22755 (88.89), **maa://22756 (40.91), ***maa://21737 (11.76)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.87), maa://45828 (93.02), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.89), maa://45828 (93.02), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="AF10" s="2" t="inlineStr">
         <is>
-          <t>*maa://25021 (53.85), *maa://22733 (64.1), **maa://22761 (50.0)</t>
+          <t>*maa://25021 (53.85), *maa://22733 (65.0), **maa://22761 (50.0)</t>
         </is>
       </c>
       <c r="AG10" s="1" t="n"/>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (88.6)</t>
+          <t>maa://21287 (88.7)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="T11" s="2" t="inlineStr">
         <is>
-          <t>maa://22747 (90.8), maa://22501 (98.13), maa://45521 (90.91)</t>
+          <t>maa://22747 (90.8), maa://22501 (98.15), maa://45521 (91.43)</t>
         </is>
       </c>
       <c r="U11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (98.06)</t>
+          <t>maa://36713 (98.07)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1935,7 +1935,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://29912 (97.73), maa://22516 (87.36), *maa://20794 (55.26)</t>
+          <t>maa://29912 (97.73), maa://22516 (87.36), *maa://20794 (55.84)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.71), *maa://21485 (75.68), maa://37962 (91.67)</t>
+          <t>maa://22753 (91.79), *maa://21485 (75.84), maa://37962 (91.67)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AF12" s="2" t="inlineStr">
         <is>
-          <t>*maa://28932 (79.53), *maa://20106 (64.29), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (79.19), *maa://20106 (64.29), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.62), maa://36673 (92.94), maa://25001 (86.3)</t>
+          <t>maa://24999 (92.65), maa://36673 (92.94), maa://25001 (86.49)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.9), **maa://22728 (45.65)</t>
+          <t>*maa://21248 (73.72), **maa://22728 (45.65)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (93.53), *maa://22583 (77.63), *maa://22500 (59.57), maa://48321 (100.0)</t>
+          <t>maa://22676 (93.53), *maa://22583 (77.22), *maa://22500 (59.57), maa://48321 (100.0)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>maa://30764 (89.55)</t>
+          <t>maa://30764 (89.71)</t>
         </is>
       </c>
       <c r="E14" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://39841 (94.04), maa://26245 (96.57), maa://21288 (96.3), maa://36682 (95.74)</t>
+          <t>maa://39841 (94.12), maa://26245 (96.57), maa://21288 (96.3), maa://36682 (95.83)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="AB14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (96.3)</t>
+          <t>maa://22764 (96.34)</t>
         </is>
       </c>
       <c r="AC14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (79.06), maa://22734 (84.43), *maa://30808 (65.22), *maa://36048 (66.0), maa://45058 (84.21)</t>
+          <t>*maa://22743 (79.15), maa://22734 (84.43), *maa://30808 (65.71), *maa://36048 (66.67), maa://45058 (84.21)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (86.83), maa://21478 (90.0)</t>
+          <t>maa://24304 (86.94), maa://21478 (90.0)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (91.11), *maa://22727 (70.0)</t>
+          <t>maa://24762 (91.16), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="T15" s="2" t="inlineStr">
         <is>
-          <t>maa://23892 (96.51)</t>
+          <t>maa://23892 (96.55)</t>
         </is>
       </c>
       <c r="U15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.27), maa://36666 (81.38), *maa://22766 (68.29)</t>
+          <t>maa://21364 (81.04), maa://36666 (81.51), *maa://22766 (68.29)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.52), maa://37650 (96.23), maa://36679 (94.55)</t>
+          <t>maa://21441 (96.54), maa://37650 (96.23), maa://36679 (94.55)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.44), *maa://28648 (72.73), *maa://36674 (79.66)</t>
+          <t>maa://22729 (94.44), *maa://28648 (73.42), *maa://36674 (80.0)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="AF16" s="2" t="inlineStr">
         <is>
-          <t>*maa://23911 (68.38), maa://27755 (93.94)</t>
+          <t>*maa://23911 (69.17), maa://27755 (94.0)</t>
         </is>
       </c>
       <c r="AG16" s="1" t="n"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>maa://22430 (89.47), maa://39599 (85.33)</t>
+          <t>maa://22430 (89.52), maa://39599 (85.33)</t>
         </is>
       </c>
       <c r="I17" s="1" t="n"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>maa://24570 (96.95)</t>
+          <t>maa://24570 (96.97)</t>
         </is>
       </c>
       <c r="E18" s="1" t="n"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>maa://24421 (87.64)</t>
+          <t>maa://24421 (87.73)</t>
         </is>
       </c>
       <c r="I18" s="1" t="n"/>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="AF18" s="2" t="inlineStr">
         <is>
-          <t>*maa://24313 (60.23), **maa://29784 (50.0), *maa://47854 (80.0)</t>
+          <t>*maa://24313 (60.23), **maa://29784 (50.0), maa://47854 (81.25)</t>
         </is>
       </c>
       <c r="AG18" s="1" t="n"/>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="T19" s="2" t="inlineStr">
         <is>
-          <t>maa://24386 (98.61)</t>
+          <t>maa://24386 (98.63)</t>
         </is>
       </c>
       <c r="U19" s="1" t="n"/>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="AB19" s="2" t="inlineStr">
         <is>
-          <t>*maa://30709 (67.59), *maa://36668 (57.32)</t>
+          <t>*maa://30709 (67.8), *maa://36668 (57.32)</t>
         </is>
       </c>
       <c r="AC19" s="1" t="n"/>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>maa://21432 (90.91), maa://25198 (94.44), *maa://20795 (50.76), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.95), maa://25198 (94.53), *maa://20795 (50.76), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="1" t="n"/>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>maa://22864 (90.5), ***maa://43283 (25.0), maa://53361 (100.0)</t>
+          <t>maa://22864 (90.61), ***maa://43283 (25.0), maa://53361 (100.0)</t>
         </is>
       </c>
       <c r="I20" s="1" t="n"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t>maa://41331 (86.1)</t>
+          <t>maa://41331 (85.78)</t>
         </is>
       </c>
       <c r="M20" s="1" t="n"/>
@@ -3089,7 +3089,7 @@
       </c>
       <c r="X20" s="2" t="inlineStr">
         <is>
-          <t>maa://50085 (86.73), maa://49976 (86.25)</t>
+          <t>maa://50085 (86.27), maa://49976 (86.25)</t>
         </is>
       </c>
       <c r="Y20" s="1" t="n"/>
@@ -3139,7 +3139,7 @@
       </c>
       <c r="D21" s="2" t="inlineStr">
         <is>
-          <t>maa://21261 (97.92)</t>
+          <t>maa://21261 (97.96)</t>
         </is>
       </c>
       <c r="E21" s="1" t="n"/>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="X21" s="2" t="inlineStr">
         <is>
-          <t>maa://20110 (86.76), maa://34946 (93.1)</t>
+          <t>maa://20110 (86.76), maa://34946 (93.22)</t>
         </is>
       </c>
       <c r="Y21" s="1" t="n"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="AB21" s="2" t="inlineStr">
         <is>
-          <t>maa://21443 (82.56), ***maa://23820 (30.0), **maa://52223 (41.18)</t>
+          <t>maa://21443 (82.6), ***maa://23820 (30.0), **maa://52223 (41.18)</t>
         </is>
       </c>
       <c r="AC21" s="1" t="n"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="AF21" s="2" t="inlineStr">
         <is>
-          <t>maa://22524 (90.2), maa://22432 (81.9)</t>
+          <t>maa://22524 (90.2), maa://22432 (81.36)</t>
         </is>
       </c>
       <c r="AG21" s="1" t="n"/>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>maa://25236 (96.12), **maa://21678 (48.94), **maa://22735 (42.86)</t>
+          <t>maa://25236 (96.15), **maa://21678 (48.94), **maa://22735 (42.86)</t>
         </is>
       </c>
       <c r="I22" s="1" t="n"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="X22" s="2" t="inlineStr">
         <is>
-          <t>maa://21282 (98.7), *maa://37649 (71.05)</t>
+          <t>maa://21282 (98.71), *maa://37649 (71.79)</t>
         </is>
       </c>
       <c r="Y22" s="1" t="n"/>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>***maa://28036 (26.92), **maa://41753 (48.0)</t>
+          <t>***maa://28036 (26.92), **maa://41753 (50.0)</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L23" s="2" t="inlineStr">
         <is>
-          <t>maa://39756 (95.45), maa://39875 (94.67)</t>
+          <t>maa://39756 (95.55), maa://39875 (94.67)</t>
         </is>
       </c>
       <c r="M23" s="1" t="n"/>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="X23" s="2" t="inlineStr">
         <is>
-          <t>*maa://28503 (67.39)</t>
+          <t>*maa://28503 (66.67)</t>
         </is>
       </c>
       <c r="Y23" s="1" t="n"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>*maa://24368 (79.01), *maa://46650 (66.67)</t>
+          <t>*maa://24368 (79.01), *maa://46650 (64.29)</t>
         </is>
       </c>
       <c r="E24" s="1" t="n"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="X24" s="2" t="inlineStr">
         <is>
-          <t>maa://29988 (84.32), maa://23504 (93.58), **maa://22892 (41.29), *maa://25141 (77.37), *maa://36663 (77.78), ***maa://22815 (23.08), maa://52227 (100.0)</t>
+          <t>maa://29988 (84.48), maa://23504 (93.6), **maa://22892 (41.29), *maa://25141 (77.37), *maa://36663 (77.78), ***maa://22815 (23.08), maa://52227 (100.0)</t>
         </is>
       </c>
       <c r="Y24" s="1" t="n"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>*maa://29063 (73.12), *maa://25311 (74.11), ***maa://22725 (4.76), *maa://45047 (66.67)</t>
+          <t>*maa://29063 (73.26), *maa://25311 (74.11), ***maa://22725 (4.76), *maa://45047 (66.67)</t>
         </is>
       </c>
       <c r="I25" s="1" t="n"/>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="AB25" s="2" t="inlineStr">
         <is>
-          <t>maa://31215 (88.81), *maa://24516 (79.35), maa://26001 (84.48)</t>
+          <t>maa://31215 (88.97), *maa://24516 (79.35), maa://26001 (84.48)</t>
         </is>
       </c>
       <c r="AC25" s="1" t="n"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>maa://24913 (91.84)</t>
+          <t>maa://24913 (91.92)</t>
         </is>
       </c>
       <c r="I26" s="1" t="n"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="AB26" s="2" t="inlineStr">
         <is>
-          <t>maa://42235 (95.68)</t>
+          <t>maa://42235 (95.71)</t>
         </is>
       </c>
       <c r="AC26" s="1" t="n"/>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>*maa://39601 (78.26), **maa://21283 (47.37), maa://34494 (97.14), **maa://36665 (50.0)</t>
+          <t>*maa://39601 (79.17), **maa://21283 (47.37), maa://34494 (97.22), **maa://36665 (50.0)</t>
         </is>
       </c>
       <c r="I27" s="1" t="n"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>maa://24465 (90.61), maa://25725 (84.21)</t>
+          <t>maa://24465 (90.62), maa://25725 (84.21)</t>
         </is>
       </c>
       <c r="E28" s="1" t="n"/>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="AF28" s="2" t="inlineStr">
         <is>
-          <t>maa://36660 (92.48), *maa://36701 (64.71)</t>
+          <t>maa://36660 (92.51), *maa://36701 (64.71)</t>
         </is>
       </c>
       <c r="AG28" s="1" t="n"/>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>*maa://25175 (60.32)</t>
+          <t>*maa://25175 (58.46)</t>
         </is>
       </c>
       <c r="I29" s="1" t="n"/>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>maa://28432 (93.94), maa://28440 (83.46), maa://31400 (98.88), *maa://28650 (71.43)</t>
+          <t>maa://28432 (93.96), maa://31400 (98.88), maa://28440 (83.58), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="1" t="n"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="AF29" s="2" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.17), maa://42865 (81.55), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (69.17), maa://42865 (80.77), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="1" t="n"/>
@@ -4357,7 +4357,7 @@
       </c>
       <c r="P30" s="2" t="inlineStr">
         <is>
-          <t>maa://21442 (98.76)</t>
+          <t>maa://21442 (98.77)</t>
         </is>
       </c>
       <c r="Q30" s="1" t="n"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="AB30" s="2" t="inlineStr">
         <is>
-          <t>maa://42979 (96.8), maa://45822 (100.0), maa://45045 (83.33)</t>
+          <t>maa://42979 (96.85), maa://45822 (100.0), maa://45045 (83.33)</t>
         </is>
       </c>
       <c r="AC30" s="1" t="n"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>maa://35926 (93.85), maa://36258 (86.93), *maa://43904 (71.43)</t>
+          <t>maa://35926 (93.9), maa://36258 (87.01), *maa://43904 (71.43)</t>
         </is>
       </c>
       <c r="M31" s="1" t="n"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>maa://21895 (97.54), maa://36667 (98.02), **maa://20793 (38.0), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.54), maa://36667 (97.14), **maa://20793 (38.0), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="1" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T32" s="2" t="inlineStr">
         <is>
-          <t>maa://42859 (97.22), maa://41108 (88.0), maa://41238 (97.87), maa://45523 (100.0)</t>
+          <t>maa://42859 (97.25), maa://41108 (88.0), maa://41238 (97.9), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="1" t="n"/>
@@ -4991,7 +4991,7 @@
       </c>
       <c r="L35" s="2" t="inlineStr">
         <is>
-          <t>maa://41296 (97.14)</t>
+          <t>maa://41296 (97.2)</t>
         </is>
       </c>
       <c r="M35" s="1" t="n"/>
@@ -5153,7 +5153,7 @@
       </c>
       <c r="T36" s="2" t="inlineStr">
         <is>
-          <t>maa://27613 (99.09)</t>
+          <t>maa://27613 (99.11)</t>
         </is>
       </c>
       <c r="U36" s="1" t="n"/>
@@ -5235,7 +5235,7 @@
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>maa://45718 (98.31), *maa://47069 (80.0), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.33), *maa://47069 (80.0), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="1" t="n"/>
@@ -5251,7 +5251,7 @@
       </c>
       <c r="P37" s="2" t="inlineStr">
         <is>
-          <t>maa://21280 (89.96), *maa://21239 (69.23)</t>
+          <t>maa://21280 (90.0), *maa://21239 (71.43)</t>
         </is>
       </c>
       <c r="Q37" s="1" t="n"/>
@@ -5352,7 +5352,7 @@
       </c>
       <c r="P38" s="2" t="inlineStr">
         <is>
-          <t>*maa://24383 (69.72)</t>
+          <t>*maa://24383 (70.0)</t>
         </is>
       </c>
       <c r="Q38" s="1" t="n"/>
@@ -5400,7 +5400,7 @@
       </c>
       <c r="AF38" s="2" t="inlineStr">
         <is>
-          <t>maa://36697 (88.85)</t>
+          <t>maa://36697 (88.93)</t>
         </is>
       </c>
       <c r="AG38" s="1" t="n"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>maa://36670 (89.09), maa://25199 (85.22), maa://30434 (92.68), maa://45059 (80.65), ***maa://25036 (18.52), *maa://44165 (66.67)</t>
+          <t>maa://36670 (89.09), maa://25199 (85.22), maa://30434 (92.68), maa://45059 (81.25), ***maa://25036 (18.52), *maa://44165 (66.67)</t>
         </is>
       </c>
       <c r="I39" s="1" t="n"/>
@@ -5469,7 +5469,7 @@
       </c>
       <c r="T39" s="2" t="inlineStr">
         <is>
-          <t>maa://47079 (95.0), *maa://45788 (75.65), *maa://45790 (79.17)</t>
+          <t>maa://47079 (95.12), *maa://45788 (75.65), *maa://45790 (79.17)</t>
         </is>
       </c>
       <c r="U39" s="1" t="n"/>
@@ -5554,7 +5554,7 @@
       </c>
       <c r="P40" s="2" t="inlineStr">
         <is>
-          <t>maa://23278 (95.18), maa://21386 (95.79), maa://36664 (89.66), maa://45550 (87.5)</t>
+          <t>maa://23278 (95.2), maa://21386 (95.79), maa://36664 (89.83), maa://45550 (87.5)</t>
         </is>
       </c>
       <c r="Q40" s="1" t="n"/>
@@ -5862,7 +5862,7 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>maa://29768 (98.23), maa://27728 (96.15)</t>
+          <t>maa://29768 (98.24), maa://27728 (96.15)</t>
         </is>
       </c>
       <c r="I44" s="1" t="n"/>
@@ -5931,7 +5931,7 @@
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>maa://21229 (84.54), maa://30807 (94.67), *maa://22767 (55.0), maa://42459 (91.43), ***maa://20796 (13.79)</t>
+          <t>maa://21229 (84.69), maa://30807 (94.67), *maa://22767 (55.0), maa://42459 (91.89), ***maa://20796 (13.79)</t>
         </is>
       </c>
       <c r="I45" s="1" t="n"/>
@@ -6000,7 +6000,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>maa://35931 (92.33), maa://43901 (94.34)</t>
+          <t>maa://35931 (92.39), maa://43901 (94.34)</t>
         </is>
       </c>
       <c r="I46" s="1" t="n"/>
@@ -6053,7 +6053,7 @@
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>maa://27410 (96.84), maa://29661 (97.56), maa://28038 (84.62)</t>
+          <t>maa://27410 (96.84), maa://29661 (97.6), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="1" t="n"/>
@@ -6362,7 +6362,7 @@
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>maa://32534 (94.83), **maa://32434 (33.33)</t>
+          <t>maa://32534 (94.86), **maa://32434 (33.33)</t>
         </is>
       </c>
       <c r="I53" s="1" t="n"/>
@@ -6430,7 +6430,7 @@
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>maa://32532 (93.0)</t>
+          <t>maa://32532 (93.04)</t>
         </is>
       </c>
       <c r="I55" s="1" t="n"/>
@@ -6466,7 +6466,7 @@
       </c>
       <c r="H57" s="2" t="inlineStr">
         <is>
-          <t>maa://25176 (98.51)</t>
+          <t>maa://25176 (98.53)</t>
         </is>
       </c>
       <c r="I57" s="1" t="n"/>
@@ -6502,7 +6502,7 @@
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>maa://31270 (94.44), maa://27746 (82.91)</t>
+          <t>maa://31270 (94.48), maa://27746 (82.91)</t>
         </is>
       </c>
       <c r="I59" s="1" t="n"/>
@@ -6556,7 +6556,7 @@
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>maa://42981 (96.3), maa://43903 (100.0)</t>
+          <t>maa://42981 (96.36), maa://43903 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="1" t="n"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#191)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论模拟干员名单作者版.xlsx
+++ b/Excel/悖论模拟干员名单作者版.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>maa://25390 (95.25), maa://24702 (94.79), maa://36681 (86.42)</t>
+          <t>maa://25390 (95.33), maa://24702 (94.81), maa://36681 (86.42)</t>
         </is>
       </c>
       <c r="E2" s="1" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>maa://39402 (94.44), *maa://24633 (56.36), *maa://30515 (70.09), *maa://34787 (72.73), ***maa://20792 (11.93), ***maa://29083 (27.78), maa://54304 (100.0)</t>
+          <t>maa://39402 (94.59), *maa://24633 (56.02), *maa://30515 (70.37), *maa://34787 (73.33), ***maa://20792 (11.93), ***maa://29083 (27.78), **maa://54304 (50.0)</t>
         </is>
       </c>
       <c r="M2" s="1" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>maa://22742 (91.41), *maa://20791 (62.65)</t>
+          <t>maa://22742 (91.04), *maa://20791 (62.65)</t>
         </is>
       </c>
       <c r="U2" s="1" t="n"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>maa://21246 (91.45), maa://36684 (93.46), ***maa://22731 (6.25)</t>
+          <t>maa://21246 (91.45), maa://36684 (93.59), ***maa://22731 (6.25)</t>
         </is>
       </c>
       <c r="AC2" s="1" t="n"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="AF2" s="2" t="inlineStr">
         <is>
-          <t>maa://25251 (91.79), **maa://21730 (30.12), ***maa://39501 (10.87), **maa://36675 (50.0)</t>
+          <t>maa://25251 (91.79), **maa://21730 (31.76), ***maa://39501 (10.87), **maa://36675 (50.0)</t>
         </is>
       </c>
       <c r="AG2" s="1" t="n"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>maa://40192 (96.88), maa://36987 (96.15), maa://39849 (88.89)</t>
+          <t>maa://40192 (96.97), maa://36987 (96.15), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="1" t="n"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>maa://21247 (98.41), *maa://22748 (60.0)</t>
+          <t>maa://21247 (98.42), *maa://22748 (60.0)</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.49), maa://20276 (88.24), *maa://22749 (75.0)</t>
+          <t>*maa://22880 (65.79), maa://20276 (88.29), *maa://22749 (75.0)</t>
         </is>
       </c>
       <c r="M3" s="1" t="n"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>maa://21249 (94.6), maa://26254 (97.22), **maa://22738 (50.0)</t>
+          <t>maa://21249 (94.62), maa://26254 (97.22), **maa://22738 (50.0)</t>
         </is>
       </c>
       <c r="Q3" s="1" t="n"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
-          <t>maa://24617 (90.62), maa://45854 (85.33), **maa://20790 (43.48), ***maa://37170 (16.67)</t>
+          <t>maa://24617 (90.84), maa://45854 (83.54), **maa://20790 (42.86), ***maa://37170 (16.44)</t>
         </is>
       </c>
       <c r="U3" s="1" t="n"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="X3" s="2" t="inlineStr">
         <is>
-          <t>maa://27396 (84.24), maa://27484 (96.21), maa://27480 (83.78)</t>
+          <t>maa://27396 (84.18), maa://27484 (96.27), maa://27480 (84.21)</t>
         </is>
       </c>
       <c r="Y3" s="1" t="n"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>maa://24390 (95.45), maa://52241 (100.0)</t>
+          <t>maa://24390 (95.51), maa://52241 (100.0)</t>
         </is>
       </c>
       <c r="AC3" s="1" t="n"/>
@@ -919,7 +919,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>maa://24632 (93.85), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.94), **maa://24303 (38.46), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="1" t="n"/>
@@ -967,7 +967,7 @@
       </c>
       <c r="P4" s="2" t="inlineStr">
         <is>
-          <t>maa://49983 (95.16), maa://50121 (92.86)</t>
+          <t>maa://49983 (95.38), maa://50121 (93.75)</t>
         </is>
       </c>
       <c r="Q4" s="1" t="n"/>
@@ -983,7 +983,7 @@
       </c>
       <c r="T4" s="2" t="inlineStr">
         <is>
-          <t>maa://32509 (94.62), maa://27295 (87.78), maa://22754 (89.19), *maa://31008 (79.55), *maa://21746 (54.55)</t>
+          <t>maa://32509 (94.66), maa://27295 (87.91), maa://22754 (89.19), *maa://31008 (79.55), *maa://21746 (54.55)</t>
         </is>
       </c>
       <c r="U4" s="1" t="n"/>
@@ -999,7 +999,7 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
-          <t>**maa://32495 (48.58), maa://43217 (93.22), ***maa://31785 (22.22), ***maa://36683 (29.79)</t>
+          <t>**maa://32495 (48.76), maa://43217 (93.39), ***maa://31785 (22.22), ***maa://36683 (29.79)</t>
         </is>
       </c>
       <c r="Y4" s="1" t="n"/>
@@ -1049,12 +1049,12 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>maa://21245 (84.95), maa://22744 (81.48)</t>
+          <t>maa://21245 (84.7), maa://22744 (81.48), maa://54105 (100.0)</t>
         </is>
       </c>
       <c r="E5" s="1" t="n"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="P5" s="2" t="inlineStr">
         <is>
-          <t>maa://21919 (96.97), *maa://21281 (80.0)</t>
+          <t>maa://21919 (97.01), *maa://21281 (80.0)</t>
         </is>
       </c>
       <c r="Q5" s="1" t="n"/>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="AB5" s="2" t="inlineStr">
         <is>
-          <t>*maa://29863 (63.41), ***maa://22752 (12.5), **maa://26013 (44.44)</t>
+          <t>*maa://29863 (62.79), ***maa://22752 (12.5), **maa://26013 (44.44)</t>
         </is>
       </c>
       <c r="AC5" s="1" t="n"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>maa://42407 (94.94)</t>
+          <t>maa://42407 (95.0)</t>
         </is>
       </c>
       <c r="E6" s="1" t="n"/>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>maa://24839 (98.8)</t>
+          <t>maa://24839 (98.81)</t>
         </is>
       </c>
       <c r="M6" s="1" t="n"/>
@@ -1264,7 +1264,7 @@
       </c>
       <c r="X6" s="2" t="inlineStr">
         <is>
-          <t>maa://52754 (83.33)</t>
+          <t>maa://52754 (88.89)</t>
         </is>
       </c>
       <c r="Y6" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>maa://28624 (93.53), maa://24957 (97.78)</t>
+          <t>maa://28624 (93.62), maa://24957 (97.78)</t>
         </is>
       </c>
       <c r="M7" s="1" t="n"/>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="T7" s="2" t="inlineStr">
         <is>
-          <t>maa://21291 (85.96)</t>
+          <t>maa://21291 (86.21)</t>
         </is>
       </c>
       <c r="U7" s="1" t="n"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="AF7" s="2" t="inlineStr">
         <is>
-          <t>*maa://26191 (67.82), maa://45272 (96.88), *maa://36671 (69.23), *maa://42530 (62.5)</t>
+          <t>*maa://26191 (67.42), maa://45272 (96.88), *maa://36671 (69.23), *maa://42530 (62.5)</t>
         </is>
       </c>
       <c r="AG7" s="1" t="n"/>
@@ -1434,7 +1434,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2025.05.17 13:19:59</t>
+          <t>更新日期：2025.05.24 13:19:10</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="P8" s="2" t="inlineStr">
         <is>
-          <t>maa://32931 (84.67), *maa://21916 (62.69), maa://23252 (91.55), maa://37496 (97.37), **maa://22759 (45.45)</t>
+          <t>maa://32931 (84.17), *maa://21916 (63.24), maa://23252 (91.55), maa://37496 (97.44), **maa://22759 (45.45)</t>
         </is>
       </c>
       <c r="Q8" s="1" t="n"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="X8" s="2" t="inlineStr">
         <is>
-          <t>maa://21411 (95.93)</t>
+          <t>maa://21411 (95.96)</t>
         </is>
       </c>
       <c r="Y8" s="1" t="n"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="AB9" s="2" t="inlineStr">
         <is>
-          <t>maa://28711 (87.05), **maa://39938 (46.34), **maa://45044 (40.0), **maa://27377 (42.86), maa://40166 (94.59), ***maa://25174 (19.05)</t>
+          <t>maa://28711 (87.14), **maa://39938 (45.24), **maa://45044 (40.0), maa://40166 (94.74), **maa://27377 (42.86), ***maa://25174 (19.05)</t>
         </is>
       </c>
       <c r="AC9" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="AF9" s="2" t="inlineStr">
         <is>
-          <t>maa://26206 (88.62), *maa://22865 (51.85)</t>
+          <t>maa://26206 (88.89), *maa://22865 (51.85)</t>
         </is>
       </c>
       <c r="AG9" s="1" t="n"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.91), ***maa://39951 (12.5), ***maa://34206 (22.22), *maa://45271 (59.7), ***maa://39243 (25.0), maa://54000 (100.0)</t>
+          <t>***maa://25695 (18.81), ***maa://39951 (12.33), ***maa://34206 (22.22), *maa://45271 (60.0), ***maa://39243 (25.0), maa://54000 (100.0)</t>
         </is>
       </c>
       <c r="E10" s="1" t="n"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="P10" s="2" t="inlineStr">
         <is>
-          <t>maa://28977 (88.42), maa://36669 (82.35), *maa://23264 (60.71)</t>
+          <t>maa://28977 (88.42), maa://36669 (82.35), *maa://23264 (61.4)</t>
         </is>
       </c>
       <c r="Q10" s="1" t="n"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="T10" s="2" t="inlineStr">
         <is>
-          <t>maa://27395 (96.6), maa://22755 (88.89), **maa://22756 (40.91), ***maa://21737 (11.76)</t>
+          <t>maa://27395 (96.64), maa://22755 (88.89), **maa://22756 (40.91), ***maa://21737 (11.76)</t>
         </is>
       </c>
       <c r="U10" s="1" t="n"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="X10" s="2" t="inlineStr">
         <is>
-          <t>maa://22301 (97.89), maa://45828 (93.02), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.89), maa://45828 (93.18), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="1" t="n"/>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>maa://36707 (99.36)</t>
+          <t>maa://36707 (99.37)</t>
         </is>
       </c>
       <c r="E11" s="1" t="n"/>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="L11" s="2" t="inlineStr">
         <is>
-          <t>maa://21287 (88.7)</t>
+          <t>maa://21287 (88.79)</t>
         </is>
       </c>
       <c r="M11" s="1" t="n"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X11" s="2" t="inlineStr">
         <is>
-          <t>maa://36713 (98.07)</t>
+          <t>maa://36713 (98.1)</t>
         </is>
       </c>
       <c r="Y11" s="1" t="n"/>
@@ -1935,7 +1935,7 @@
       </c>
       <c r="AB11" s="2" t="inlineStr">
         <is>
-          <t>maa://29912 (97.73), maa://22516 (87.36), *maa://20794 (55.84)</t>
+          <t>maa://29912 (97.78), maa://22516 (87.36), *maa://20794 (55.84)</t>
         </is>
       </c>
       <c r="AC11" s="1" t="n"/>
@@ -1980,12 +1980,12 @@
       </c>
       <c r="G12" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>maa://21867 (90.81), **maa://45826 (33.33)</t>
+          <t>maa://21867 (90.81), **maa://45826 (33.33), maa://54294 (100.0)</t>
         </is>
       </c>
       <c r="I12" s="1" t="n"/>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="X12" s="2" t="inlineStr">
         <is>
-          <t>maa://22753 (91.79), *maa://21485 (75.84), maa://37962 (91.67)</t>
+          <t>maa://22753 (91.83), *maa://21485 (75.84), maa://37962 (91.8)</t>
         </is>
       </c>
       <c r="Y12" s="1" t="n"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="AB12" s="2" t="inlineStr">
         <is>
-          <t>maa://23669 (95.64), maa://36677 (95.12), maa://39872 (93.1)</t>
+          <t>maa://23669 (95.64), maa://36677 (95.18), maa://39872 (93.1)</t>
         </is>
       </c>
       <c r="AC12" s="1" t="n"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>maa://24999 (92.65), maa://36673 (92.94), maa://25001 (86.49)</t>
+          <t>maa://24999 (92.7), maa://36673 (91.86), maa://25001 (86.49)</t>
         </is>
       </c>
       <c r="E13" s="1" t="n"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.72), **maa://22728 (45.65)</t>
+          <t>*maa://21248 (73.45), **maa://22728 (45.65)</t>
         </is>
       </c>
       <c r="I13" s="1" t="n"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="P13" s="2" t="inlineStr">
         <is>
-          <t>maa://22676 (93.53), *maa://22583 (77.22), *maa://22500 (59.57), maa://48321 (100.0)</t>
+          <t>maa://22676 (93.57), *maa://22583 (77.22), *maa://22500 (59.57), maa://48321 (100.0)</t>
         </is>
       </c>
       <c r="Q13" s="1" t="n"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="X13" s="2" t="inlineStr">
         <is>
-          <t>maa://34957 (82.69), **maa://22768 (50.0)</t>
+          <t>maa://34957 (83.02), **maa://22768 (50.0)</t>
         </is>
       </c>
       <c r="Y13" s="1" t="n"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="AF13" s="2" t="inlineStr">
         <is>
-          <t>**maa://22737 (38.22), maa://39883 (87.39), *maa://39885 (51.28)</t>
+          <t>**maa://22737 (38.22), maa://39883 (87.6), **maa://39885 (50.0)</t>
         </is>
       </c>
       <c r="AG13" s="1" t="n"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>maa://39841 (94.12), maa://26245 (96.57), maa://21288 (96.3), maa://36682 (95.83)</t>
+          <t>maa://39841 (94.16), maa://26245 (96.59), maa://21288 (96.3), maa://36682 (95.83)</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="P14" s="2" t="inlineStr">
         <is>
-          <t>maa://23250 (98.82), maa://20107 (87.1), maa://22772 (100.0), *maa://22745 (66.67)</t>
+          <t>maa://23250 (98.84), maa://20107 (87.1), maa://22772 (100.0), *maa://22745 (66.67)</t>
         </is>
       </c>
       <c r="Q14" s="1" t="n"/>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="T14" s="2" t="inlineStr">
         <is>
-          <t>maa://22521 (94.83), maa://42751 (100.0)</t>
+          <t>maa://22521 (94.87), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="1" t="n"/>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="AB14" s="2" t="inlineStr">
         <is>
-          <t>maa://22764 (96.34)</t>
+          <t>maa://22764 (96.39)</t>
         </is>
       </c>
       <c r="AC14" s="1" t="n"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>*maa://22743 (79.15), maa://22734 (84.43), *maa://30808 (65.71), *maa://36048 (66.67), maa://45058 (84.21)</t>
+          <t>*maa://22743 (79.08), maa://22734 (84.55), *maa://30808 (65.71), *maa://36048 (67.31), maa://45058 (84.21)</t>
         </is>
       </c>
       <c r="E15" s="1" t="n"/>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>maa://24304 (86.94), maa://21478 (90.0)</t>
+          <t>maa://24304 (87.1), maa://21478 (90.0)</t>
         </is>
       </c>
       <c r="I15" s="1" t="n"/>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P15" s="2" t="inlineStr">
         <is>
-          <t>maa://24762 (91.16), *maa://22727 (70.0)</t>
+          <t>maa://24762 (91.21), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="1" t="n"/>
@@ -2434,12 +2434,12 @@
       </c>
       <c r="W15" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="X15" s="2" t="inlineStr">
         <is>
-          <t>*maa://38786 (70.0)</t>
+          <t>*maa://38786 (70.0), maa://56102 (100.0)</t>
         </is>
       </c>
       <c r="Y15" s="1" t="n"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AF15" s="2" t="inlineStr">
         <is>
-          <t>maa://21364 (81.04), maa://36666 (81.51), *maa://22766 (68.29)</t>
+          <t>maa://21364 (81.1), maa://36666 (81.46), *maa://22766 (68.29)</t>
         </is>
       </c>
       <c r="AG15" s="1" t="n"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>maa://21441 (96.54), maa://37650 (96.23), maa://36679 (94.55)</t>
+          <t>maa://21441 (96.54), maa://37650 (96.3), maa://36679 (94.55)</t>
         </is>
       </c>
       <c r="E16" s="1" t="n"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="T16" s="2" t="inlineStr">
         <is>
-          <t>maa://22729 (94.44), *maa://28648 (73.42), *maa://36674 (80.0)</t>
+          <t>maa://22729 (94.44), *maa://28648 (73.75), *maa://36674 (80.0)</t>
         </is>
       </c>
       <c r="U16" s="1" t="n"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="X16" s="2" t="inlineStr">
         <is>
-          <t>maa://28501 (98.23), maa://28051 (96.0)</t>
+          <t>maa://28501 (98.26), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="1" t="n"/>
@@ -2601,7 +2601,7